<commit_message>
added new solar capacity
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -15,26 +15,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BusDemand">Sheet2!#REF!</definedName>
-    <definedName name="CH4_total">Sheet2!$B$36</definedName>
-    <definedName name="CO2_total">Sheet2!$B$35</definedName>
-    <definedName name="Gen">Sheet2!$B$3:$AA$22</definedName>
-    <definedName name="LineCapacity">Sheet2!#REF!</definedName>
-    <definedName name="LineFlow">Sheet2!$B$26:$AA$28</definedName>
-    <definedName name="LineFromBus">Sheet2!#REF!</definedName>
-    <definedName name="LineReactance">Sheet2!#REF!</definedName>
-    <definedName name="LineToBus">Sheet2!#REF!</definedName>
-    <definedName name="MarginalC">Sheet2!#REF!</definedName>
-    <definedName name="MaxGen">Sheet2!#REF!</definedName>
-    <definedName name="MinGen">Sheet2!#REF!</definedName>
-    <definedName name="N2O_total">Sheet2!$B$37</definedName>
-    <definedName name="NOx_total">Sheet2!$B$33</definedName>
-    <definedName name="NumBuses">Sheet2!#REF!</definedName>
-    <definedName name="NumLines">Sheet2!#REF!</definedName>
-    <definedName name="NumUnits">Sheet2!#REF!</definedName>
-    <definedName name="SO2_total">Sheet2!$B$34</definedName>
-    <definedName name="TotalCost">Sheet2!$B$30</definedName>
-    <definedName name="UnitsByBus">Sheet2!#REF!</definedName>
+    <definedName name="CH4_total">Sheet2!$B$56</definedName>
+    <definedName name="CO2_total">Sheet2!$B$55</definedName>
+    <definedName name="Gen">Sheet2!$B$3:$AA$42</definedName>
+    <definedName name="LineFlow">Sheet2!$B$46:$AA$48</definedName>
+    <definedName name="N2O_total">Sheet2!$B$57</definedName>
+    <definedName name="NOx_total">Sheet2!$B$53</definedName>
+    <definedName name="SO2_total">Sheet2!$B$54</definedName>
+    <definedName name="TotalCost">Sheet2!$B$50</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -569,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA37"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,10 +854,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="11">
-        <v>0</v>
+        <v>20.483750609269187</v>
       </c>
       <c r="K5" s="11">
-        <v>0</v>
+        <v>38.555504364752068</v>
       </c>
       <c r="L5" s="11">
         <v>0</v>
@@ -1008,25 +996,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="10">
-        <v>339.19999999999982</v>
+        <v>197.39999999999978</v>
       </c>
       <c r="C7" s="11">
-        <v>392.08500000099912</v>
+        <v>240.28499999999914</v>
       </c>
       <c r="D7" s="11">
-        <v>435.35596500099882</v>
+        <v>283.55596499999888</v>
       </c>
       <c r="E7" s="11">
-        <v>464</v>
+        <v>327.21636868499832</v>
       </c>
       <c r="F7" s="11">
-        <v>464</v>
+        <v>371.26971600316318</v>
       </c>
       <c r="G7" s="11">
-        <v>464</v>
+        <v>415.7195434471916</v>
       </c>
       <c r="H7" s="11">
-        <v>464</v>
+        <v>460.56941933821616</v>
       </c>
       <c r="I7" s="11">
         <v>464</v>
@@ -1038,13 +1026,13 @@
         <v>464</v>
       </c>
       <c r="L7" s="11">
-        <v>464</v>
+        <v>367.04190390503413</v>
       </c>
       <c r="M7" s="11">
-        <v>464</v>
+        <v>413.94668104017018</v>
       </c>
       <c r="N7" s="11">
-        <v>464</v>
+        <v>461.27360116952258</v>
       </c>
       <c r="O7" s="11">
         <v>464</v>
@@ -1450,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="11">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="L12" s="11">
         <v>0</v>
@@ -1672,82 +1660,82 @@
         <v>13</v>
       </c>
       <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
+      <c r="J15" s="11">
+        <v>0</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0</v>
+      </c>
+      <c r="L15" s="11">
+        <v>276.99999999900001</v>
+      </c>
+      <c r="M15" s="11">
+        <v>276.99999999900001</v>
+      </c>
+      <c r="N15" s="11">
+        <v>276.99999999900001</v>
+      </c>
+      <c r="O15" s="11">
         <v>277</v>
       </c>
-      <c r="C15" s="11">
-        <v>276.99999999900001</v>
-      </c>
-      <c r="D15" s="11">
-        <v>276.99999999900001</v>
-      </c>
-      <c r="E15" s="11">
-        <v>277</v>
-      </c>
-      <c r="F15" s="11">
-        <v>277</v>
-      </c>
-      <c r="G15" s="11">
-        <v>313.51954344719161</v>
-      </c>
-      <c r="H15" s="11">
-        <v>358.36941933821618</v>
-      </c>
-      <c r="I15" s="11">
-        <v>403.62294411225957</v>
-      </c>
-      <c r="J15" s="11">
-        <v>449.28375060926919</v>
-      </c>
-      <c r="K15" s="11">
-        <v>495.35550436475205</v>
-      </c>
-      <c r="L15" s="11">
-        <v>541.84190390403455</v>
-      </c>
-      <c r="M15" s="11">
-        <v>588.74668103917065</v>
-      </c>
-      <c r="N15" s="11">
-        <v>636.07360116852306</v>
-      </c>
-      <c r="O15" s="11">
-        <v>683.82646357903923</v>
-      </c>
       <c r="P15" s="11">
-        <v>732.00910175125045</v>
+        <v>303.20910175125044</v>
       </c>
       <c r="Q15" s="11">
-        <v>780.62538366701028</v>
+        <v>351.82538366701033</v>
       </c>
       <c r="R15" s="11">
-        <v>829.67921212001329</v>
+        <v>400.87921212001322</v>
       </c>
       <c r="S15" s="11">
-        <v>879.17452502909282</v>
+        <v>450.37452502909287</v>
       </c>
       <c r="T15" s="11">
-        <v>929.11529575435407</v>
+        <v>500.315295754354</v>
       </c>
       <c r="U15" s="11">
-        <v>979.50553341614295</v>
+        <v>550.705533416143</v>
       </c>
       <c r="V15" s="11">
-        <v>1030.3492832168872</v>
+        <v>601.54928321688715</v>
       </c>
       <c r="W15" s="11">
-        <v>1081.6506267658383</v>
+        <v>652.85062676583823</v>
       </c>
       <c r="X15" s="11">
-        <v>1133.4136824067305</v>
+        <v>704.61368240673039</v>
       </c>
       <c r="Y15" s="11">
-        <v>1185.6426055483903</v>
+        <v>756.84260554839022</v>
       </c>
       <c r="Z15" s="11">
-        <v>1238.3415889983248</v>
+        <v>809.54158899832498</v>
       </c>
       <c r="AA15" s="12">
-        <v>1291.5148632993091</v>
+        <v>862.71486329930906</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
@@ -1921,7 +1909,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C18" s="11">
         <v>0</v>
@@ -1930,19 +1918,19 @@
         <v>0</v>
       </c>
       <c r="E18" s="11">
-        <v>15.016368684998724</v>
+        <v>0</v>
       </c>
       <c r="F18" s="11">
-        <v>59.069716003163649</v>
+        <v>0</v>
       </c>
       <c r="G18" s="11">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="H18" s="11">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="I18" s="11">
-        <v>67</v>
+        <v>41.822944112259563</v>
       </c>
       <c r="J18" s="11">
         <v>67</v>
@@ -1951,16 +1939,16 @@
         <v>67</v>
       </c>
       <c r="L18" s="11">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="M18" s="11">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="N18" s="11">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="O18" s="11">
-        <v>67</v>
+        <v>45.026463579039273</v>
       </c>
       <c r="P18" s="11">
         <v>67</v>
@@ -2252,395 +2240,2055 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="13">
-        <v>0</v>
-      </c>
-      <c r="C22" s="14">
-        <v>0</v>
-      </c>
-      <c r="D22" s="14">
-        <v>0</v>
-      </c>
-      <c r="E22" s="14">
-        <v>0</v>
-      </c>
-      <c r="F22" s="14">
-        <v>0</v>
-      </c>
-      <c r="G22" s="14">
-        <v>0</v>
-      </c>
-      <c r="H22" s="14">
-        <v>0</v>
-      </c>
-      <c r="I22" s="14">
-        <v>0</v>
-      </c>
-      <c r="J22" s="14">
-        <v>0</v>
-      </c>
-      <c r="K22" s="14">
-        <v>0</v>
-      </c>
-      <c r="L22" s="14">
-        <v>0</v>
-      </c>
-      <c r="M22" s="14">
-        <v>0</v>
-      </c>
-      <c r="N22" s="14">
-        <v>0</v>
-      </c>
-      <c r="O22" s="14">
-        <v>0</v>
-      </c>
-      <c r="P22" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="14">
-        <v>0</v>
-      </c>
-      <c r="R22" s="14">
-        <v>0</v>
-      </c>
-      <c r="S22" s="14">
-        <v>0</v>
-      </c>
-      <c r="T22" s="14">
-        <v>0</v>
-      </c>
-      <c r="U22" s="14">
-        <v>0</v>
-      </c>
-      <c r="V22" s="14">
-        <v>0</v>
-      </c>
-      <c r="W22" s="14">
-        <v>0</v>
-      </c>
-      <c r="X22" s="14">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="15">
-        <v>0</v>
+      <c r="B22" s="10">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0</v>
+      </c>
+      <c r="G22" s="11">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>0</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0</v>
+      </c>
+      <c r="J22" s="11">
+        <v>0</v>
+      </c>
+      <c r="K22" s="11">
+        <v>0</v>
+      </c>
+      <c r="L22" s="11">
+        <v>0</v>
+      </c>
+      <c r="M22" s="11">
+        <v>0</v>
+      </c>
+      <c r="N22" s="11">
+        <v>0</v>
+      </c>
+      <c r="O22" s="11">
+        <v>0</v>
+      </c>
+      <c r="P22" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>0</v>
+      </c>
+      <c r="R22" s="11">
+        <v>0</v>
+      </c>
+      <c r="S22" s="11">
+        <v>0</v>
+      </c>
+      <c r="T22" s="11">
+        <v>0</v>
+      </c>
+      <c r="U22" s="11">
+        <v>0</v>
+      </c>
+      <c r="V22" s="11">
+        <v>0</v>
+      </c>
+      <c r="W22" s="11">
+        <v>0</v>
+      </c>
+      <c r="X22" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10">
+        <v>28.1</v>
+      </c>
+      <c r="C23" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="D23" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="E23" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="F23" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="G23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="H23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="I23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="J23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="K23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="L23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="M23" s="11">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="N23" s="11">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="O23" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="P23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="R23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="S23" s="11">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="T23" s="11">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="U23" s="11">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="V23" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="W23" s="11">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="X23" s="11">
+        <v>28.1</v>
+      </c>
+      <c r="Y23" s="11">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="Z23" s="11">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="AA23" s="12">
+        <v>28.1</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10">
+        <v>25</v>
+      </c>
+      <c r="C24" s="11">
+        <v>25</v>
+      </c>
+      <c r="D24" s="11">
+        <v>25</v>
+      </c>
+      <c r="E24" s="11">
+        <v>25</v>
+      </c>
+      <c r="F24" s="11">
+        <v>25</v>
+      </c>
+      <c r="G24" s="11">
+        <v>25</v>
+      </c>
+      <c r="H24" s="11">
+        <v>25</v>
+      </c>
+      <c r="I24" s="11">
+        <v>25</v>
+      </c>
+      <c r="J24" s="11">
+        <v>25</v>
+      </c>
+      <c r="K24" s="11">
+        <v>25</v>
+      </c>
+      <c r="L24" s="11">
+        <v>25</v>
+      </c>
+      <c r="M24" s="11">
+        <v>25</v>
+      </c>
+      <c r="N24" s="11">
+        <v>25</v>
+      </c>
+      <c r="O24" s="11">
+        <v>25</v>
+      </c>
+      <c r="P24" s="11">
+        <v>25</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>25</v>
+      </c>
+      <c r="R24" s="11">
+        <v>25</v>
+      </c>
+      <c r="S24" s="11">
+        <v>25</v>
+      </c>
+      <c r="T24" s="11">
+        <v>25</v>
+      </c>
+      <c r="U24" s="11">
+        <v>25</v>
+      </c>
+      <c r="V24" s="11">
+        <v>25</v>
+      </c>
+      <c r="W24" s="11">
+        <v>25</v>
+      </c>
+      <c r="X24" s="11">
+        <v>25</v>
+      </c>
+      <c r="Y24" s="11">
+        <v>25</v>
+      </c>
+      <c r="Z24" s="11">
+        <v>25</v>
+      </c>
+      <c r="AA24" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10">
+        <v>70</v>
+      </c>
+      <c r="C25" s="11">
+        <v>70</v>
+      </c>
+      <c r="D25" s="11">
+        <v>70</v>
+      </c>
+      <c r="E25" s="11">
+        <v>70</v>
+      </c>
+      <c r="F25" s="11">
+        <v>70</v>
+      </c>
+      <c r="G25" s="11">
+        <v>70</v>
+      </c>
+      <c r="H25" s="11">
+        <v>70</v>
+      </c>
+      <c r="I25" s="11">
+        <v>70</v>
+      </c>
+      <c r="J25" s="11">
+        <v>70</v>
+      </c>
+      <c r="K25" s="11">
+        <v>70</v>
+      </c>
+      <c r="L25" s="11">
+        <v>70</v>
+      </c>
+      <c r="M25" s="11">
+        <v>70</v>
+      </c>
+      <c r="N25" s="11">
+        <v>70</v>
+      </c>
+      <c r="O25" s="11">
+        <v>70</v>
+      </c>
+      <c r="P25" s="11">
+        <v>70</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>70</v>
+      </c>
+      <c r="R25" s="11">
+        <v>70</v>
+      </c>
+      <c r="S25" s="11">
+        <v>70</v>
+      </c>
+      <c r="T25" s="11">
+        <v>70</v>
+      </c>
+      <c r="U25" s="11">
+        <v>70</v>
+      </c>
+      <c r="V25" s="11">
+        <v>70</v>
+      </c>
+      <c r="W25" s="11">
+        <v>70</v>
+      </c>
+      <c r="X25" s="11">
+        <v>70</v>
+      </c>
+      <c r="Y25" s="11">
+        <v>70</v>
+      </c>
+      <c r="Z25" s="11">
+        <v>70</v>
+      </c>
+      <c r="AA25" s="12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="10">
+        <v>30.6</v>
+      </c>
+      <c r="C26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="D26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="E26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="F26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="G26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="H26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="I26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="J26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="K26" s="11">
+        <v>30.599999999999998</v>
+      </c>
+      <c r="L26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="M26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="N26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="O26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="P26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="Q26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="R26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="S26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="T26" s="11">
+        <v>30.599999999999998</v>
+      </c>
+      <c r="U26" s="11">
+        <v>30.599999999999998</v>
+      </c>
+      <c r="V26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="W26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="X26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="Y26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="Z26" s="11">
+        <v>30.6</v>
+      </c>
+      <c r="AA26" s="12">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="10">
+        <v>10.000000000000014</v>
+      </c>
+      <c r="C27" s="11">
+        <v>10</v>
+      </c>
+      <c r="D27" s="11">
+        <v>10</v>
+      </c>
+      <c r="E27" s="11">
+        <v>10</v>
+      </c>
+      <c r="F27" s="11">
+        <v>10</v>
+      </c>
+      <c r="G27" s="11">
+        <v>10</v>
+      </c>
+      <c r="H27" s="11">
+        <v>10</v>
+      </c>
+      <c r="I27" s="11">
+        <v>10</v>
+      </c>
+      <c r="J27" s="11">
+        <v>10</v>
+      </c>
+      <c r="K27" s="11">
+        <v>10</v>
+      </c>
+      <c r="L27" s="11">
+        <v>10</v>
+      </c>
+      <c r="M27" s="11">
+        <v>10</v>
+      </c>
+      <c r="N27" s="11">
+        <v>10</v>
+      </c>
+      <c r="O27" s="11">
+        <v>10</v>
+      </c>
+      <c r="P27" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q27" s="11">
+        <v>10</v>
+      </c>
+      <c r="R27" s="11">
+        <v>10</v>
+      </c>
+      <c r="S27" s="11">
+        <v>10</v>
+      </c>
+      <c r="T27" s="11">
+        <v>10</v>
+      </c>
+      <c r="U27" s="11">
+        <v>10</v>
+      </c>
+      <c r="V27" s="11">
+        <v>10</v>
+      </c>
+      <c r="W27" s="11">
+        <v>10</v>
+      </c>
+      <c r="X27" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y27" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z27" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA27" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" s="10">
+        <v>10</v>
+      </c>
+      <c r="C28" s="11">
+        <v>10</v>
+      </c>
+      <c r="D28" s="11">
+        <v>10</v>
+      </c>
+      <c r="E28" s="11">
+        <v>10</v>
+      </c>
+      <c r="F28" s="11">
+        <v>10</v>
+      </c>
+      <c r="G28" s="11">
+        <v>10</v>
+      </c>
+      <c r="H28" s="11">
+        <v>10</v>
+      </c>
+      <c r="I28" s="11">
+        <v>10</v>
+      </c>
+      <c r="J28" s="11">
+        <v>10</v>
+      </c>
+      <c r="K28" s="11">
+        <v>10</v>
+      </c>
+      <c r="L28" s="11">
+        <v>10</v>
+      </c>
+      <c r="M28" s="11">
+        <v>10</v>
+      </c>
+      <c r="N28" s="11">
+        <v>10</v>
+      </c>
+      <c r="O28" s="11">
+        <v>10</v>
+      </c>
+      <c r="P28" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="11">
+        <v>10</v>
+      </c>
+      <c r="R28" s="11">
+        <v>10</v>
+      </c>
+      <c r="S28" s="11">
+        <v>10</v>
+      </c>
+      <c r="T28" s="11">
+        <v>10</v>
+      </c>
+      <c r="U28" s="11">
+        <v>10</v>
+      </c>
+      <c r="V28" s="11">
+        <v>10</v>
+      </c>
+      <c r="W28" s="11">
+        <v>10</v>
+      </c>
+      <c r="X28" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y28" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z28" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA28" s="12">
+        <v>9.9999999999999929</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" s="10">
+        <v>10</v>
+      </c>
+      <c r="C29" s="11">
+        <v>10</v>
+      </c>
+      <c r="D29" s="11">
+        <v>10</v>
+      </c>
+      <c r="E29" s="11">
+        <v>10</v>
+      </c>
+      <c r="F29" s="11">
+        <v>10</v>
+      </c>
+      <c r="G29" s="11">
+        <v>10</v>
+      </c>
+      <c r="H29" s="11">
+        <v>10</v>
+      </c>
+      <c r="I29" s="11">
+        <v>10</v>
+      </c>
+      <c r="J29" s="11">
+        <v>10</v>
+      </c>
+      <c r="K29" s="11">
+        <v>10</v>
+      </c>
+      <c r="L29" s="11">
+        <v>10</v>
+      </c>
+      <c r="M29" s="11">
+        <v>10</v>
+      </c>
+      <c r="N29" s="11">
+        <v>10</v>
+      </c>
+      <c r="O29" s="11">
+        <v>10</v>
+      </c>
+      <c r="P29" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="11">
+        <v>10</v>
+      </c>
+      <c r="R29" s="11">
+        <v>10</v>
+      </c>
+      <c r="S29" s="11">
+        <v>10</v>
+      </c>
+      <c r="T29" s="11">
+        <v>10</v>
+      </c>
+      <c r="U29" s="11">
+        <v>10</v>
+      </c>
+      <c r="V29" s="11">
+        <v>10</v>
+      </c>
+      <c r="W29" s="11">
+        <v>10</v>
+      </c>
+      <c r="X29" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y29" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z29" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA29" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" s="10">
+        <v>52.2</v>
+      </c>
+      <c r="C30" s="11">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="D30" s="11">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="E30" s="11">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="F30" s="11">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="G30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="H30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="I30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="J30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="K30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="L30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="M30" s="11">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="N30" s="11">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="O30" s="11">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="P30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="Q30" s="11">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="R30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="S30" s="11">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="T30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="U30" s="11">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="V30" s="11">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="W30" s="11">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="X30" s="11">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="Y30" s="11">
+        <v>52.2</v>
+      </c>
+      <c r="Z30" s="11">
+        <v>52.199999999999989</v>
+      </c>
+      <c r="AA30" s="12">
+        <v>52.200000000000017</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" s="10">
+        <v>10</v>
+      </c>
+      <c r="C31" s="11">
+        <v>10</v>
+      </c>
+      <c r="D31" s="11">
+        <v>10</v>
+      </c>
+      <c r="E31" s="11">
+        <v>10</v>
+      </c>
+      <c r="F31" s="11">
+        <v>10</v>
+      </c>
+      <c r="G31" s="11">
+        <v>10</v>
+      </c>
+      <c r="H31" s="11">
+        <v>10</v>
+      </c>
+      <c r="I31" s="11">
+        <v>10</v>
+      </c>
+      <c r="J31" s="11">
+        <v>10</v>
+      </c>
+      <c r="K31" s="11">
+        <v>10</v>
+      </c>
+      <c r="L31" s="11">
+        <v>10</v>
+      </c>
+      <c r="M31" s="11">
+        <v>10</v>
+      </c>
+      <c r="N31" s="11">
+        <v>10</v>
+      </c>
+      <c r="O31" s="11">
+        <v>10</v>
+      </c>
+      <c r="P31" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="11">
+        <v>10</v>
+      </c>
+      <c r="R31" s="11">
+        <v>10</v>
+      </c>
+      <c r="S31" s="11">
+        <v>10</v>
+      </c>
+      <c r="T31" s="11">
+        <v>10</v>
+      </c>
+      <c r="U31" s="11">
+        <v>10</v>
+      </c>
+      <c r="V31" s="11">
+        <v>10</v>
+      </c>
+      <c r="W31" s="11">
+        <v>10</v>
+      </c>
+      <c r="X31" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y31" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z31" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA31" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" s="10">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="C32" s="11">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="D32" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="E32" s="11">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="F32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="G32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="H32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="I32" s="11">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="J32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="K32" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="L32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="M32" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="N32" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="O32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="P32" s="11">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="Q32" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="R32" s="11">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="S32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="T32" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="U32" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="V32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="W32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="X32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="Y32" s="11">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="Z32" s="11">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="AA32" s="12">
+        <v>20.199999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" s="10">
+        <v>70</v>
+      </c>
+      <c r="C33" s="11">
+        <v>70</v>
+      </c>
+      <c r="D33" s="11">
+        <v>70</v>
+      </c>
+      <c r="E33" s="11">
+        <v>70</v>
+      </c>
+      <c r="F33" s="11">
+        <v>70</v>
+      </c>
+      <c r="G33" s="11">
+        <v>70</v>
+      </c>
+      <c r="H33" s="11">
+        <v>70</v>
+      </c>
+      <c r="I33" s="11">
+        <v>70</v>
+      </c>
+      <c r="J33" s="11">
+        <v>70</v>
+      </c>
+      <c r="K33" s="11">
+        <v>70</v>
+      </c>
+      <c r="L33" s="11">
+        <v>70</v>
+      </c>
+      <c r="M33" s="11">
+        <v>70</v>
+      </c>
+      <c r="N33" s="11">
+        <v>70</v>
+      </c>
+      <c r="O33" s="11">
+        <v>70</v>
+      </c>
+      <c r="P33" s="11">
+        <v>70</v>
+      </c>
+      <c r="Q33" s="11">
+        <v>70</v>
+      </c>
+      <c r="R33" s="11">
+        <v>70</v>
+      </c>
+      <c r="S33" s="11">
+        <v>70</v>
+      </c>
+      <c r="T33" s="11">
+        <v>70</v>
+      </c>
+      <c r="U33" s="11">
+        <v>70</v>
+      </c>
+      <c r="V33" s="11">
+        <v>70</v>
+      </c>
+      <c r="W33" s="11">
+        <v>70</v>
+      </c>
+      <c r="X33" s="11">
+        <v>70</v>
+      </c>
+      <c r="Y33" s="11">
+        <v>70</v>
+      </c>
+      <c r="Z33" s="11">
+        <v>70</v>
+      </c>
+      <c r="AA33" s="12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" s="10">
+        <v>10.5</v>
+      </c>
+      <c r="C34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="D34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="E34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="F34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="G34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="H34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="I34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="J34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="K34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="L34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="M34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="N34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="O34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="P34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="Q34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="R34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="S34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="T34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="U34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="V34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="W34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="X34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="Y34" s="11">
+        <v>10.499999999999986</v>
+      </c>
+      <c r="Z34" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="AA34" s="12">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" s="10">
+        <v>9.9999999999999929</v>
+      </c>
+      <c r="C35" s="11">
+        <v>10</v>
+      </c>
+      <c r="D35" s="11">
+        <v>10</v>
+      </c>
+      <c r="E35" s="11">
+        <v>10</v>
+      </c>
+      <c r="F35" s="11">
+        <v>10</v>
+      </c>
+      <c r="G35" s="11">
+        <v>10</v>
+      </c>
+      <c r="H35" s="11">
+        <v>10</v>
+      </c>
+      <c r="I35" s="11">
+        <v>10</v>
+      </c>
+      <c r="J35" s="11">
+        <v>10</v>
+      </c>
+      <c r="K35" s="11">
+        <v>10</v>
+      </c>
+      <c r="L35" s="11">
+        <v>10</v>
+      </c>
+      <c r="M35" s="11">
+        <v>10</v>
+      </c>
+      <c r="N35" s="11">
+        <v>10</v>
+      </c>
+      <c r="O35" s="11">
+        <v>10</v>
+      </c>
+      <c r="P35" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q35" s="11">
+        <v>10</v>
+      </c>
+      <c r="R35" s="11">
+        <v>10</v>
+      </c>
+      <c r="S35" s="11">
+        <v>10</v>
+      </c>
+      <c r="T35" s="11">
+        <v>10</v>
+      </c>
+      <c r="U35" s="11">
+        <v>10</v>
+      </c>
+      <c r="V35" s="11">
+        <v>10</v>
+      </c>
+      <c r="W35" s="11">
+        <v>10</v>
+      </c>
+      <c r="X35" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y35" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z35" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA35" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" s="10">
+        <v>10</v>
+      </c>
+      <c r="C36" s="11">
+        <v>10</v>
+      </c>
+      <c r="D36" s="11">
+        <v>10</v>
+      </c>
+      <c r="E36" s="11">
+        <v>10</v>
+      </c>
+      <c r="F36" s="11">
+        <v>10</v>
+      </c>
+      <c r="G36" s="11">
+        <v>10</v>
+      </c>
+      <c r="H36" s="11">
+        <v>10</v>
+      </c>
+      <c r="I36" s="11">
+        <v>10</v>
+      </c>
+      <c r="J36" s="11">
+        <v>10</v>
+      </c>
+      <c r="K36" s="11">
+        <v>10</v>
+      </c>
+      <c r="L36" s="11">
+        <v>10</v>
+      </c>
+      <c r="M36" s="11">
+        <v>10</v>
+      </c>
+      <c r="N36" s="11">
+        <v>10</v>
+      </c>
+      <c r="O36" s="11">
+        <v>10</v>
+      </c>
+      <c r="P36" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q36" s="11">
+        <v>10</v>
+      </c>
+      <c r="R36" s="11">
+        <v>10</v>
+      </c>
+      <c r="S36" s="11">
+        <v>10</v>
+      </c>
+      <c r="T36" s="11">
+        <v>10</v>
+      </c>
+      <c r="U36" s="11">
+        <v>10</v>
+      </c>
+      <c r="V36" s="11">
+        <v>10</v>
+      </c>
+      <c r="W36" s="11">
+        <v>10</v>
+      </c>
+      <c r="X36" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y36" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z36" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA36" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" s="10">
+        <v>10</v>
+      </c>
+      <c r="C37" s="11">
+        <v>10</v>
+      </c>
+      <c r="D37" s="11">
+        <v>10</v>
+      </c>
+      <c r="E37" s="11">
+        <v>10</v>
+      </c>
+      <c r="F37" s="11">
+        <v>10</v>
+      </c>
+      <c r="G37" s="11">
+        <v>10</v>
+      </c>
+      <c r="H37" s="11">
+        <v>10</v>
+      </c>
+      <c r="I37" s="11">
+        <v>10</v>
+      </c>
+      <c r="J37" s="11">
+        <v>10</v>
+      </c>
+      <c r="K37" s="11">
+        <v>10</v>
+      </c>
+      <c r="L37" s="11">
+        <v>10</v>
+      </c>
+      <c r="M37" s="11">
+        <v>10</v>
+      </c>
+      <c r="N37" s="11">
+        <v>10</v>
+      </c>
+      <c r="O37" s="11">
+        <v>10</v>
+      </c>
+      <c r="P37" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q37" s="11">
+        <v>10</v>
+      </c>
+      <c r="R37" s="11">
+        <v>10</v>
+      </c>
+      <c r="S37" s="11">
+        <v>10</v>
+      </c>
+      <c r="T37" s="11">
+        <v>10</v>
+      </c>
+      <c r="U37" s="11">
+        <v>10.000000000000002</v>
+      </c>
+      <c r="V37" s="11">
+        <v>10</v>
+      </c>
+      <c r="W37" s="11">
+        <v>10</v>
+      </c>
+      <c r="X37" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y37" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z37" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA37" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" s="10">
+        <v>10</v>
+      </c>
+      <c r="C38" s="11">
+        <v>10</v>
+      </c>
+      <c r="D38" s="11">
+        <v>10</v>
+      </c>
+      <c r="E38" s="11">
+        <v>10</v>
+      </c>
+      <c r="F38" s="11">
+        <v>10</v>
+      </c>
+      <c r="G38" s="11">
+        <v>10</v>
+      </c>
+      <c r="H38" s="11">
+        <v>10</v>
+      </c>
+      <c r="I38" s="11">
+        <v>10</v>
+      </c>
+      <c r="J38" s="11">
+        <v>10</v>
+      </c>
+      <c r="K38" s="11">
+        <v>10</v>
+      </c>
+      <c r="L38" s="11">
+        <v>10</v>
+      </c>
+      <c r="M38" s="11">
+        <v>10</v>
+      </c>
+      <c r="N38" s="11">
+        <v>9.9999999999999929</v>
+      </c>
+      <c r="O38" s="11">
+        <v>10</v>
+      </c>
+      <c r="P38" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q38" s="11">
+        <v>10</v>
+      </c>
+      <c r="R38" s="11">
+        <v>10</v>
+      </c>
+      <c r="S38" s="11">
+        <v>10</v>
+      </c>
+      <c r="T38" s="11">
+        <v>10</v>
+      </c>
+      <c r="U38" s="11">
+        <v>10</v>
+      </c>
+      <c r="V38" s="11">
+        <v>10</v>
+      </c>
+      <c r="W38" s="11">
+        <v>10</v>
+      </c>
+      <c r="X38" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y38" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z38" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA38" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" s="10">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="C39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="D39" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="E39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="F39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="G39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="H39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="I39" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="J39" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="K39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="L39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="M39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="N39" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="O39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="P39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="Q39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="R39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="S39" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="T39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="U39" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="V39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="W39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="X39" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="Y39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="Z39" s="11">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="AA39" s="12">
+        <v>10.099999999999994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="C40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="D40" s="11">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="E40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="F40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="G40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="H40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="I40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="J40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="K40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="L40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="M40" s="11">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="N40" s="11">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="O40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="P40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="Q40" s="11">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="R40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="S40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="T40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="U40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="V40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="W40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="X40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="Y40" s="11">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="Z40" s="11">
+        <v>10.1</v>
+      </c>
+      <c r="AA40" s="12">
+        <v>10.100000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" s="10">
+        <v>10</v>
+      </c>
+      <c r="C41" s="11">
+        <v>10</v>
+      </c>
+      <c r="D41" s="11">
+        <v>10</v>
+      </c>
+      <c r="E41" s="11">
+        <v>10</v>
+      </c>
+      <c r="F41" s="11">
+        <v>10</v>
+      </c>
+      <c r="G41" s="11">
+        <v>10</v>
+      </c>
+      <c r="H41" s="11">
+        <v>10</v>
+      </c>
+      <c r="I41" s="11">
+        <v>10</v>
+      </c>
+      <c r="J41" s="11">
+        <v>10</v>
+      </c>
+      <c r="K41" s="11">
+        <v>10</v>
+      </c>
+      <c r="L41" s="11">
+        <v>10</v>
+      </c>
+      <c r="M41" s="11">
+        <v>10</v>
+      </c>
+      <c r="N41" s="11">
+        <v>10</v>
+      </c>
+      <c r="O41" s="11">
+        <v>10</v>
+      </c>
+      <c r="P41" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q41" s="11">
+        <v>10</v>
+      </c>
+      <c r="R41" s="11">
+        <v>10</v>
+      </c>
+      <c r="S41" s="11">
+        <v>10</v>
+      </c>
+      <c r="T41" s="11">
+        <v>10</v>
+      </c>
+      <c r="U41" s="11">
+        <v>10</v>
+      </c>
+      <c r="V41" s="11">
+        <v>10</v>
+      </c>
+      <c r="W41" s="11">
+        <v>10</v>
+      </c>
+      <c r="X41" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y41" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z41" s="11">
+        <v>10</v>
+      </c>
+      <c r="AA41" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" s="13">
+        <v>12</v>
+      </c>
+      <c r="C42" s="14">
+        <v>12</v>
+      </c>
+      <c r="D42" s="14">
+        <v>12</v>
+      </c>
+      <c r="E42" s="14">
+        <v>12</v>
+      </c>
+      <c r="F42" s="14">
+        <v>12</v>
+      </c>
+      <c r="G42" s="14">
+        <v>12</v>
+      </c>
+      <c r="H42" s="14">
+        <v>12</v>
+      </c>
+      <c r="I42" s="14">
+        <v>12</v>
+      </c>
+      <c r="J42" s="14">
+        <v>12</v>
+      </c>
+      <c r="K42" s="14">
+        <v>12</v>
+      </c>
+      <c r="L42" s="14">
+        <v>12</v>
+      </c>
+      <c r="M42" s="14">
+        <v>12</v>
+      </c>
+      <c r="N42" s="14">
+        <v>12</v>
+      </c>
+      <c r="O42" s="14">
+        <v>12</v>
+      </c>
+      <c r="P42" s="14">
+        <v>12</v>
+      </c>
+      <c r="Q42" s="14">
+        <v>12</v>
+      </c>
+      <c r="R42" s="14">
+        <v>12</v>
+      </c>
+      <c r="S42" s="14">
+        <v>12</v>
+      </c>
+      <c r="T42" s="14">
+        <v>12</v>
+      </c>
+      <c r="U42" s="14">
+        <v>12</v>
+      </c>
+      <c r="V42" s="14">
+        <v>12</v>
+      </c>
+      <c r="W42" s="14">
+        <v>12</v>
+      </c>
+      <c r="X42" s="14">
+        <v>12</v>
+      </c>
+      <c r="Y42" s="14">
+        <v>12</v>
+      </c>
+      <c r="Z42" s="14">
+        <v>12</v>
+      </c>
+      <c r="AA42" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="7">
-        <v>680.71666666666647</v>
-      </c>
-      <c r="C26" s="8">
-        <v>703.34825000066633</v>
-      </c>
-      <c r="D26" s="8">
-        <v>722.82018425066622</v>
-      </c>
-      <c r="E26" s="8">
-        <v>737.4619096799164</v>
-      </c>
-      <c r="F26" s="8">
-        <v>742.6014668670357</v>
-      </c>
-      <c r="G26" s="8">
-        <v>735.61409891977507</v>
-      </c>
-      <c r="H26" s="8">
-        <v>725.89662581005314</v>
-      </c>
-      <c r="I26" s="8">
-        <v>716.09169544234373</v>
-      </c>
-      <c r="J26" s="8">
-        <v>706.19852070132504</v>
-      </c>
-      <c r="K26" s="8">
-        <v>696.21630738763702</v>
-      </c>
-      <c r="L26" s="8">
-        <v>686.14425415412586</v>
-      </c>
-      <c r="M26" s="8">
-        <v>675.98155244151303</v>
-      </c>
-      <c r="N26" s="8">
-        <v>665.72738641348667</v>
-      </c>
-      <c r="O26" s="8">
-        <v>655.38093289120809</v>
-      </c>
-      <c r="P26" s="8">
-        <v>644.94136128722903</v>
-      </c>
-      <c r="Q26" s="8">
-        <v>634.40783353881454</v>
-      </c>
-      <c r="R26" s="8">
-        <v>623.77950404066382</v>
-      </c>
-      <c r="S26" s="8">
-        <v>613.05551957702994</v>
-      </c>
-      <c r="T26" s="8">
-        <v>602.23501925322341</v>
-      </c>
-      <c r="U26" s="8">
-        <v>591.31713442650243</v>
-      </c>
-      <c r="V26" s="8">
-        <v>580.30098863634123</v>
-      </c>
-      <c r="W26" s="8">
-        <v>569.18569753406848</v>
-      </c>
-      <c r="X26" s="8">
-        <v>557.97036881187523</v>
-      </c>
-      <c r="Y26" s="8">
-        <v>546.65410213118219</v>
-      </c>
-      <c r="Z26" s="8">
-        <v>535.23598905036306</v>
-      </c>
-      <c r="AA26" s="9">
-        <v>523.71511295181665</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="B46" s="7">
+        <v>739.88333333333321</v>
+      </c>
+      <c r="C46" s="8">
+        <v>759.18158333333292</v>
+      </c>
+      <c r="D46" s="8">
+        <v>778.65351758333293</v>
+      </c>
+      <c r="E46" s="8">
+        <v>798.30069924158261</v>
+      </c>
+      <c r="F46" s="8">
+        <v>818.12470553475669</v>
+      </c>
+      <c r="G46" s="8">
+        <v>838.12712788456952</v>
+      </c>
+      <c r="H46" s="8">
+        <v>858.30957203553066</v>
+      </c>
+      <c r="I46" s="8">
+        <v>864.73267681309699</v>
+      </c>
+      <c r="J46" s="8">
+        <v>876.88768777417124</v>
+      </c>
+      <c r="K46" s="8">
+        <v>878.95331029747183</v>
+      </c>
+      <c r="L46" s="8">
+        <v>756.20552342414862</v>
+      </c>
+      <c r="M46" s="8">
+        <v>777.31267313495971</v>
+      </c>
+      <c r="N46" s="8">
+        <v>798.60978719316847</v>
+      </c>
+      <c r="O46" s="8">
+        <v>805.08975408422134</v>
+      </c>
+      <c r="P46" s="8">
+        <v>801.97469462056245</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>791.44116687214762</v>
+      </c>
+      <c r="R46" s="8">
+        <v>780.81283737399713</v>
+      </c>
+      <c r="S46" s="8">
+        <v>770.08885291036313</v>
+      </c>
+      <c r="T46" s="8">
+        <v>759.26835258655649</v>
+      </c>
+      <c r="U46" s="8">
+        <v>748.35046775983562</v>
+      </c>
+      <c r="V46" s="8">
+        <v>737.33432196967442</v>
+      </c>
+      <c r="W46" s="8">
+        <v>726.21903086740167</v>
+      </c>
+      <c r="X46" s="8">
+        <v>715.00370214520831</v>
+      </c>
+      <c r="Y46" s="8">
+        <v>703.68743546451526</v>
+      </c>
+      <c r="Z46" s="8">
+        <v>692.26932238369625</v>
+      </c>
+      <c r="AA46" s="9">
+        <v>680.74844628514961</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="10">
-        <v>-774.7833333333333</v>
-      </c>
-      <c r="C27" s="11">
-        <v>-773.59425000033332</v>
-      </c>
-      <c r="D27" s="11">
-        <v>-775.75779825033328</v>
-      </c>
-      <c r="E27" s="11">
-        <v>-782.94627466258282</v>
-      </c>
-      <c r="F27" s="11">
-        <v>-799.83339113454599</v>
-      </c>
-      <c r="G27" s="11">
-        <v>-792.52612935662921</v>
-      </c>
-      <c r="H27" s="11">
-        <v>-779.81866452083887</v>
-      </c>
-      <c r="I27" s="11">
-        <v>-766.99683250152657</v>
-      </c>
-      <c r="J27" s="11">
-        <v>-754.05960399404046</v>
-      </c>
-      <c r="K27" s="11">
-        <v>-741.00594042998705</v>
-      </c>
-      <c r="L27" s="11">
-        <v>-727.83479389385695</v>
-      </c>
-      <c r="M27" s="11">
-        <v>-714.54510703890173</v>
-      </c>
-      <c r="N27" s="11">
-        <v>-701.13581300225189</v>
-      </c>
-      <c r="O27" s="11">
-        <v>-687.60583531927239</v>
-      </c>
-      <c r="P27" s="11">
-        <v>-673.95408783714583</v>
-      </c>
-      <c r="Q27" s="11">
-        <v>-660.17947462768086</v>
-      </c>
-      <c r="R27" s="11">
-        <v>-646.28088989932962</v>
-      </c>
-      <c r="S27" s="11">
-        <v>-632.25721790842397</v>
-      </c>
-      <c r="T27" s="11">
-        <v>-618.10733286959987</v>
-      </c>
-      <c r="U27" s="11">
-        <v>-603.83009886542641</v>
-      </c>
-      <c r="V27" s="11">
-        <v>-589.42436975521548</v>
-      </c>
-      <c r="W27" s="11">
-        <v>-574.88898908301269</v>
-      </c>
-      <c r="X27" s="11">
-        <v>-560.22278998475986</v>
-      </c>
-      <c r="Y27" s="11">
-        <v>-545.42459509462299</v>
-      </c>
-      <c r="Z27" s="11">
-        <v>-530.49321645047485</v>
-      </c>
-      <c r="AA27" s="12">
-        <v>-515.42745539852899</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="B47" s="10">
+        <v>-829.81666666666661</v>
+      </c>
+      <c r="C47" s="11">
+        <v>-831.96091666666655</v>
+      </c>
+      <c r="D47" s="11">
+        <v>-834.12446491666651</v>
+      </c>
+      <c r="E47" s="11">
+        <v>-836.30748510091655</v>
+      </c>
+      <c r="F47" s="11">
+        <v>-838.51015246682482</v>
+      </c>
+      <c r="G47" s="11">
+        <v>-840.73264383902608</v>
+      </c>
+      <c r="H47" s="11">
+        <v>-842.97513763357745</v>
+      </c>
+      <c r="I47" s="11">
+        <v>-859.17879524303282</v>
+      </c>
+      <c r="J47" s="11">
+        <v>-869.85418753046338</v>
+      </c>
+      <c r="K47" s="11">
+        <v>-862.82444188490433</v>
+      </c>
+      <c r="L47" s="11">
+        <v>-759.81542852886821</v>
+      </c>
+      <c r="M47" s="11">
+        <v>-762.16066738562506</v>
+      </c>
+      <c r="N47" s="11">
+        <v>-764.52701339209261</v>
+      </c>
+      <c r="O47" s="11">
+        <v>-781.92347770529841</v>
+      </c>
+      <c r="P47" s="11">
+        <v>-782.92075450381242</v>
+      </c>
+      <c r="Q47" s="11">
+        <v>-769.14614129434688</v>
+      </c>
+      <c r="R47" s="11">
+        <v>-755.24755656599632</v>
+      </c>
+      <c r="S47" s="11">
+        <v>-741.22388457509032</v>
+      </c>
+      <c r="T47" s="11">
+        <v>-727.07399953626634</v>
+      </c>
+      <c r="U47" s="11">
+        <v>-712.79676553209265</v>
+      </c>
+      <c r="V47" s="11">
+        <v>-698.39103642188184</v>
+      </c>
+      <c r="W47" s="11">
+        <v>-683.85565574967893</v>
+      </c>
+      <c r="X47" s="11">
+        <v>-669.18945665142633</v>
+      </c>
+      <c r="Y47" s="11">
+        <v>-654.39126176128912</v>
+      </c>
+      <c r="Z47" s="11">
+        <v>-639.4598831171412</v>
+      </c>
+      <c r="AA47" s="12">
+        <v>-624.39412206519546</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="13">
-        <v>94.066666666666649</v>
-      </c>
-      <c r="C28" s="14">
-        <v>70.245999999666992</v>
-      </c>
-      <c r="D28" s="14">
-        <v>52.937613999667178</v>
-      </c>
-      <c r="E28" s="14">
-        <v>45.484364982666079</v>
-      </c>
-      <c r="F28" s="14">
-        <v>57.23192426751018</v>
-      </c>
-      <c r="G28" s="14">
-        <v>56.912030436853797</v>
-      </c>
-      <c r="H28" s="14">
-        <v>53.9220387107855</v>
-      </c>
-      <c r="I28" s="14">
-        <v>50.905137059182607</v>
-      </c>
-      <c r="J28" s="14">
-        <v>47.861083292715421</v>
-      </c>
-      <c r="K28" s="14">
-        <v>44.789633042349806</v>
-      </c>
-      <c r="L28" s="14">
-        <v>41.69053973973098</v>
-      </c>
-      <c r="M28" s="14">
-        <v>38.563554597388588</v>
-      </c>
-      <c r="N28" s="14">
-        <v>35.40842658876511</v>
-      </c>
-      <c r="O28" s="14">
-        <v>32.224902428063956</v>
-      </c>
-      <c r="P28" s="14">
-        <v>29.012726549916579</v>
-      </c>
-      <c r="Q28" s="14">
-        <v>25.771641088866204</v>
-      </c>
-      <c r="R28" s="14">
-        <v>22.501385858665799</v>
-      </c>
-      <c r="S28" s="14">
-        <v>19.201698331393914</v>
-      </c>
-      <c r="T28" s="14">
-        <v>15.872313616376573</v>
-      </c>
-      <c r="U28" s="14">
-        <v>12.512964438923859</v>
-      </c>
-      <c r="V28" s="14">
-        <v>9.123381118874363</v>
-      </c>
-      <c r="W28" s="14">
-        <v>5.7032915489442075</v>
-      </c>
-      <c r="X28" s="14">
-        <v>2.2524211728848513</v>
-      </c>
-      <c r="Y28" s="14">
-        <v>-1.2295070365591982</v>
-      </c>
-      <c r="Z28" s="14">
-        <v>-4.7427725998882124</v>
-      </c>
-      <c r="AA28" s="15">
-        <v>-8.2876575532876018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="B48" s="13">
+        <v>89.933333333333337</v>
+      </c>
+      <c r="C48" s="14">
+        <v>72.779333333333653</v>
+      </c>
+      <c r="D48" s="14">
+        <v>55.470947333333761</v>
+      </c>
+      <c r="E48" s="14">
+        <v>38.006785859334016</v>
+      </c>
+      <c r="F48" s="14">
+        <v>20.385446932068067</v>
+      </c>
+      <c r="G48" s="14">
+        <v>2.6055159544566679</v>
+      </c>
+      <c r="H48" s="14">
+        <v>-15.33443440195313</v>
+      </c>
+      <c r="I48" s="14">
+        <v>-5.553881570064191</v>
+      </c>
+      <c r="J48" s="14">
+        <v>-7.0335002437076826</v>
+      </c>
+      <c r="K48" s="14">
+        <v>-16.128868412567478</v>
+      </c>
+      <c r="L48" s="14">
+        <v>3.6099051047196911</v>
+      </c>
+      <c r="M48" s="14">
+        <v>-15.152005749334828</v>
+      </c>
+      <c r="N48" s="14">
+        <v>-34.082773801075675</v>
+      </c>
+      <c r="O48" s="14">
+        <v>-23.166276378922863</v>
+      </c>
+      <c r="P48" s="14">
+        <v>-19.053940116749999</v>
+      </c>
+      <c r="Q48" s="14">
+        <v>-22.29502557780075</v>
+      </c>
+      <c r="R48" s="14">
+        <v>-25.565280808000871</v>
+      </c>
+      <c r="S48" s="14">
+        <v>-28.864968335272888</v>
+      </c>
+      <c r="T48" s="14">
+        <v>-32.194353050290324</v>
+      </c>
+      <c r="U48" s="14">
+        <v>-35.553702227743003</v>
+      </c>
+      <c r="V48" s="14">
+        <v>-38.943285547792499</v>
+      </c>
+      <c r="W48" s="14">
+        <v>-42.363375117722669</v>
+      </c>
+      <c r="X48" s="14">
+        <v>-45.814245493782046</v>
+      </c>
+      <c r="Y48" s="14">
+        <v>-49.296173703226145</v>
+      </c>
+      <c r="Z48" s="14">
+        <v>-52.809439266555053</v>
+      </c>
+      <c r="AA48" s="15">
+        <v>-56.35432421995408</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="3">
-        <v>3274802.0340343202</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+      <c r="B50" s="3">
+        <v>2984434.2658852255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="4">
-        <v>159356.40751318654</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="4">
+        <v>133480.4640845384</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="5">
-        <v>42675.177221961967</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="B54" s="5">
+        <v>37397.35954357584</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="5">
-        <v>242162106.74134582</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+      <c r="B55" s="5">
+        <v>215741460.0598028</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="5">
-        <v>20736.701973587995</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="B56" s="5">
+        <v>18005.859222547522</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="6">
-        <v>2964.9311146407326</v>
+      <c r="B57" s="6">
+        <v>2566.7184018013213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new binary logical constraints
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -734,55 +734,55 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>476.58096263724519</v>
+        <v>495.91917837746996</v>
       </c>
       <c r="H3" s="4">
-        <v>377.70348649883817</v>
+        <v>396.80584595544178</v>
       </c>
       <c r="I3" s="4">
-        <v>403.6033688231114</v>
+        <v>421.675301164948</v>
       </c>
       <c r="J3" s="4">
-        <v>389.91049839802554</v>
+        <v>407.00758733670227</v>
       </c>
       <c r="K3" s="4">
-        <v>498.05101802736908</v>
+        <v>514.22584895567979</v>
       </c>
       <c r="L3" s="4">
-        <v>411.81888815108755</v>
+        <v>427.12120987952767</v>
       </c>
       <c r="M3" s="4">
-        <v>451.5761073350717</v>
+        <v>466.05298510390912</v>
       </c>
       <c r="N3" s="4">
-        <v>460.06517014815483</v>
+        <v>473.7611303856429</v>
       </c>
       <c r="O3" s="4">
-        <v>439.09701579602279</v>
+        <v>452.05418306798219</v>
       </c>
       <c r="P3" s="4">
-        <v>390.38601541551793</v>
+        <v>402.64424198762845</v>
       </c>
       <c r="Q3" s="4">
-        <v>474.72572062991969</v>
+        <v>486.3227090409838</v>
       </c>
       <c r="R3" s="4">
-        <v>375.31168377619906</v>
+        <v>386.28310279959442</v>
       </c>
       <c r="S3" s="4">
-        <v>435.13960772483927</v>
+        <v>419.45037015797629</v>
       </c>
       <c r="T3" s="4">
-        <v>243.27367851252768</v>
+        <v>129.0329188223846</v>
       </c>
       <c r="U3" s="4">
-        <v>78.059328724965241</v>
+        <v>117.86808104206557</v>
       </c>
       <c r="V3" s="4">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="W3" s="4">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="X3" s="4">
         <v>0</v>
@@ -805,10 +805,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>149.65758779768657</v>
+        <v>130.26735234473381</v>
       </c>
       <c r="D4" s="7">
-        <v>606.04188169902409</v>
+        <v>641.05189162051852</v>
       </c>
       <c r="E4" s="7">
         <v>665.6</v>
@@ -936,7 +936,7 @@
         <v>46.5</v>
       </c>
       <c r="S5" s="7">
-        <v>26.78797256508085</v>
+        <v>42.477210131940573</v>
       </c>
       <c r="T5" s="7">
         <v>46.5</v>
@@ -951,7 +951,7 @@
         <v>46.5</v>
       </c>
       <c r="X5" s="7">
-        <v>43.188165168928066</v>
+        <v>46.5</v>
       </c>
       <c r="Y5" s="7">
         <v>46.5</v>
@@ -1051,7 +1051,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>183.18806320475795</v>
+        <v>192.67035526309945</v>
       </c>
       <c r="C7" s="7">
         <v>464</v>
@@ -1197,7 +1197,7 @@
         <v>101.5</v>
       </c>
       <c r="W8" s="7">
-        <v>38.087889959494504</v>
+        <v>101.5</v>
       </c>
       <c r="X8" s="7">
         <v>0</v>
@@ -1369,10 +1369,10 @@
         <v>88</v>
       </c>
       <c r="Y10" s="7">
-        <v>85.513755621299993</v>
+        <v>85.513755621296582</v>
       </c>
       <c r="Z10" s="7">
-        <v>16.480629421891308</v>
+        <v>0</v>
       </c>
       <c r="AA10" s="8">
         <v>0</v>
@@ -1609,13 +1609,13 @@
         <v>154</v>
       </c>
       <c r="V13" s="7">
-        <v>126.02157994995193</v>
+        <v>90.066924690421729</v>
       </c>
       <c r="W13" s="7">
-        <v>0</v>
+        <v>44.93222638095358</v>
       </c>
       <c r="X13" s="7">
-        <v>121.59457918513726</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="7">
         <v>0</v>
@@ -1638,7 +1638,7 @@
         <v>150</v>
       </c>
       <c r="D14" s="7">
-        <v>120.52511830097376</v>
+        <v>85.515108379479386</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -1704,7 +1704,7 @@
         <v>150</v>
       </c>
       <c r="Z14" s="7">
-        <v>150</v>
+        <v>132.96125884377764</v>
       </c>
       <c r="AA14" s="8">
         <v>0</v>
@@ -1724,10 +1724,10 @@
         <v>1848</v>
       </c>
       <c r="E15" s="7">
-        <v>1267.9555255442774</v>
+        <v>1254.6797472637281</v>
       </c>
       <c r="F15" s="7">
-        <v>621.3425041496921</v>
+        <v>607.83770948546044</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -1748,10 +1748,10 @@
         <v>0</v>
       </c>
       <c r="M15" s="7">
-        <v>-1.2050804798491299E-11</v>
+        <v>0</v>
       </c>
       <c r="N15" s="7">
-        <v>-7.9580786405131221E-12</v>
+        <v>0</v>
       </c>
       <c r="O15" s="7">
         <v>0</v>
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>591.6505774557188</v>
+        <v>604.92635573626785</v>
       </c>
       <c r="F16" s="7">
         <v>656.1</v>
@@ -1873,7 +1873,7 @@
         <v>656.1</v>
       </c>
       <c r="AA16" s="8">
-        <v>651.55241017337903</v>
+        <v>651.55241017337175</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
@@ -1893,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="7">
-        <v>10.579953777303217</v>
+        <v>24.084748441534884</v>
       </c>
       <c r="G17" s="7">
         <v>50.3</v>
@@ -1932,7 +1932,7 @@
         <v>50.3</v>
       </c>
       <c r="S17" s="7">
-        <v>28.366370434876508</v>
+        <v>28.366370434874398</v>
       </c>
       <c r="T17" s="7">
         <v>50.3</v>
@@ -2062,7 +2062,7 @@
         <v>257</v>
       </c>
       <c r="G19" s="7">
-        <v>171.84029741109225</v>
+        <v>152.50208167086748</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
@@ -2080,13 +2080,13 @@
         <v>0</v>
       </c>
       <c r="M19" s="7">
-        <v>7.2759576141834259E-12</v>
+        <v>0</v>
       </c>
       <c r="N19" s="7">
-        <v>-4.3655745685100555E-11</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7">
-        <v>3.0240698833949864E-11</v>
+        <v>0</v>
       </c>
       <c r="P19" s="7">
         <v>0</v>
@@ -2101,28 +2101,28 @@
         <v>257</v>
       </c>
       <c r="T19" s="7">
-        <v>169.0855177687904</v>
+        <v>243.3262774589266</v>
       </c>
       <c r="U19" s="7">
-        <v>158.32540032288483</v>
+        <v>128.51664800577811</v>
       </c>
       <c r="V19" s="7">
-        <v>61.054911659327445</v>
+        <v>135.00956691885096</v>
       </c>
       <c r="W19" s="7">
-        <v>75.852590074266118</v>
+        <v>55.50825365280177</v>
       </c>
       <c r="X19" s="7">
-        <v>0</v>
+        <v>79.064458690961146</v>
       </c>
       <c r="Y19" s="7">
-        <v>42.858822277240506</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="7">
-        <v>0</v>
+        <v>42.671387508931296</v>
       </c>
       <c r="AA19" s="8">
-        <v>48.222203806046309</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
@@ -2148,37 +2148,37 @@
         <v>2269.6</v>
       </c>
       <c r="H20" s="7">
-        <v>2256.2042648899333</v>
+        <v>2237.1019054333301</v>
       </c>
       <c r="I20" s="7">
-        <v>1996.7838523281605</v>
+        <v>1978.7119199863209</v>
       </c>
       <c r="J20" s="7">
-        <v>1777.5545077436095</v>
+        <v>1760.4574188049276</v>
       </c>
       <c r="K20" s="7">
-        <v>1487.0954731695394</v>
+        <v>1470.920642241224</v>
       </c>
       <c r="L20" s="7">
-        <v>1341.618221466593</v>
+        <v>1326.3158997381474</v>
       </c>
       <c r="M20" s="7">
-        <v>1120.7662362691731</v>
+        <v>1106.2893585003244</v>
       </c>
       <c r="N20" s="7">
-        <v>931.80255454857161</v>
+        <v>918.10659431102636</v>
       </c>
       <c r="O20" s="7">
-        <v>772.92181842289301</v>
+        <v>759.96465115095816</v>
       </c>
       <c r="P20" s="7">
-        <v>642.41528831139897</v>
+        <v>630.15706173928265</v>
       </c>
       <c r="Q20" s="7">
-        <v>429.4950948305368</v>
+        <v>417.89810641946679</v>
       </c>
       <c r="R20" s="7">
-        <v>350.97141902340167</v>
+        <v>340</v>
       </c>
       <c r="S20" s="7">
         <v>0</v>
@@ -2187,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="7">
-        <v>0</v>
+        <v>-1.9895196601282805E-13</v>
       </c>
       <c r="V20" s="7">
         <v>0</v>
@@ -2213,7 +2213,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>25.311936795242218</v>
+        <v>15.829644736899297</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2249,7 +2249,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="7">
-        <v>-1.7053025658242404E-12</v>
+        <v>0</v>
       </c>
       <c r="O21" s="7">
         <v>0</v>
@@ -2362,16 +2362,16 @@
         <v>398.3</v>
       </c>
       <c r="X22" s="7">
-        <v>398.3</v>
+        <v>397.51828566309814</v>
       </c>
       <c r="Y22" s="7">
-        <v>302.93681115470872</v>
+        <v>355.79563343194695</v>
       </c>
       <c r="Z22" s="7">
-        <v>292.24594413283558</v>
+        <v>243.09392720201456</v>
       </c>
       <c r="AA22" s="8">
-        <v>243.16589873729515</v>
+        <v>301.38810254334294</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
@@ -2382,16 +2382,16 @@
         <v>0</v>
       </c>
       <c r="C23" s="7">
-        <v>28.1</v>
+        <v>21.232647655264202</v>
       </c>
       <c r="D23" s="7">
         <v>28.100000000000009</v>
       </c>
       <c r="E23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="F23" s="7">
         <v>28.100000000000009</v>
-      </c>
-      <c r="F23" s="7">
-        <v>28.099999999999994</v>
       </c>
       <c r="G23" s="7">
         <v>28.1</v>
@@ -2400,7 +2400,7 @@
         <v>28.099999999999994</v>
       </c>
       <c r="I23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="J23" s="7">
         <v>28.099999999999994</v>
@@ -2409,28 +2409,28 @@
         <v>28.1</v>
       </c>
       <c r="L23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="M23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="N23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="O23" s="7">
-        <v>28.1</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="P23" s="7">
-        <v>28.1</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="Q23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="R23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="S23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="T23" s="7">
         <v>28.100000000000009</v>
@@ -2448,13 +2448,13 @@
         <v>28.1</v>
       </c>
       <c r="Y23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="Z23" s="7">
         <v>28.1</v>
       </c>
       <c r="AA23" s="8">
-        <v>28.1</v>
+        <v>28.099999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
@@ -2646,10 +2646,10 @@
         <v>30.599999999999998</v>
       </c>
       <c r="H26" s="7">
+        <v>30.599999999999998</v>
+      </c>
+      <c r="I26" s="7">
         <v>30.6</v>
-      </c>
-      <c r="I26" s="7">
-        <v>30.599999999999998</v>
       </c>
       <c r="J26" s="7">
         <v>30.6</v>
@@ -2658,7 +2658,7 @@
         <v>30.599999999999998</v>
       </c>
       <c r="L26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="M26" s="7">
         <v>30.6</v>
@@ -2703,7 +2703,7 @@
         <v>30.6</v>
       </c>
       <c r="AA26" s="8">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
@@ -2732,7 +2732,7 @@
         <v>10</v>
       </c>
       <c r="I27" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="J27" s="7">
         <v>10</v>
@@ -2771,10 +2771,10 @@
         <v>10</v>
       </c>
       <c r="V27" s="7">
+        <v>10</v>
+      </c>
+      <c r="W27" s="7">
         <v>9.9999999999999929</v>
-      </c>
-      <c r="W27" s="7">
-        <v>10</v>
       </c>
       <c r="X27" s="7">
         <v>10</v>
@@ -2797,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D28" s="7">
         <v>10</v>
@@ -2880,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="7">
-        <v>5.7424122023118684</v>
+        <v>10</v>
       </c>
       <c r="D29" s="7">
         <v>10</v>
@@ -2913,7 +2913,7 @@
         <v>10</v>
       </c>
       <c r="N29" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="O29" s="7">
         <v>10</v>
@@ -2928,7 +2928,7 @@
         <v>10</v>
       </c>
       <c r="S29" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="T29" s="7">
         <v>10</v>
@@ -2963,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="D30" s="7">
         <v>52.2</v>
@@ -2975,7 +2975,7 @@
         <v>52.2</v>
       </c>
       <c r="G30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="H30" s="7">
         <v>52.200000000000017</v>
@@ -2987,40 +2987,40 @@
         <v>52.200000000000017</v>
       </c>
       <c r="K30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="L30" s="7">
         <v>52.2</v>
       </c>
       <c r="M30" s="7">
-        <v>52.20000000000001</v>
+        <v>52.2</v>
       </c>
       <c r="N30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="O30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="P30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="Q30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="R30" s="7">
-        <v>52.20000000000001</v>
+        <v>52.2</v>
       </c>
       <c r="S30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="T30" s="7">
         <v>52.2</v>
       </c>
       <c r="U30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.20000000000001</v>
       </c>
       <c r="V30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="W30" s="7">
         <v>52.200000000000017</v>
@@ -3029,13 +3029,13 @@
         <v>52.200000000000017</v>
       </c>
       <c r="Y30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="Z30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.20000000000001</v>
       </c>
       <c r="AA30" s="8">
-        <v>52.20000000000001</v>
+        <v>52.2</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.35">
@@ -3046,20 +3046,20 @@
         <v>0</v>
       </c>
       <c r="C31" s="7">
+        <v>10</v>
+      </c>
+      <c r="D31" s="7">
+        <v>10</v>
+      </c>
+      <c r="E31" s="7">
+        <v>9.9999999999999858</v>
+      </c>
+      <c r="F31" s="7">
+        <v>10</v>
+      </c>
+      <c r="G31" s="7">
         <v>9.9999999999999929</v>
       </c>
-      <c r="D31" s="7">
-        <v>10</v>
-      </c>
-      <c r="E31" s="7">
-        <v>10</v>
-      </c>
-      <c r="F31" s="7">
-        <v>10</v>
-      </c>
-      <c r="G31" s="7">
-        <v>10</v>
-      </c>
       <c r="H31" s="7">
         <v>10</v>
       </c>
@@ -3070,10 +3070,10 @@
         <v>10</v>
       </c>
       <c r="K31" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="L31" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="M31" s="7">
         <v>10</v>
@@ -3082,7 +3082,7 @@
         <v>10</v>
       </c>
       <c r="O31" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="P31" s="7">
         <v>10</v>
@@ -3100,10 +3100,10 @@
         <v>10</v>
       </c>
       <c r="U31" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="V31" s="7">
-        <v>10</v>
+        <v>10.000000000000014</v>
       </c>
       <c r="W31" s="7">
         <v>10</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="Z31" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="AA31" s="8">
         <v>10</v>
@@ -3132,13 +3132,13 @@
         <v>0</v>
       </c>
       <c r="D32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="E32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="F32" s="7">
         <v>20.200000000000003</v>
-      </c>
-      <c r="E32" s="7">
-        <v>20.200000000000003</v>
-      </c>
-      <c r="F32" s="7">
-        <v>20.2</v>
       </c>
       <c r="G32" s="7">
         <v>20.2</v>
@@ -3147,10 +3147,10 @@
         <v>20.2</v>
       </c>
       <c r="I32" s="7">
-        <v>20.2</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="J32" s="7">
-        <v>20.2</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="K32" s="7">
         <v>20.2</v>
@@ -3159,49 +3159,49 @@
         <v>20.2</v>
       </c>
       <c r="M32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="N32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="O32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="P32" s="7">
         <v>20.200000000000003</v>
-      </c>
-      <c r="N32" s="7">
-        <v>20.200000000000003</v>
-      </c>
-      <c r="O32" s="7">
-        <v>20.200000000000003</v>
-      </c>
-      <c r="P32" s="7">
-        <v>20.2</v>
       </c>
       <c r="Q32" s="7">
         <v>20.200000000000003</v>
       </c>
       <c r="R32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="S32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="T32" s="7">
-        <v>20.2</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="U32" s="7">
         <v>20.2</v>
       </c>
       <c r="V32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="W32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="X32" s="7">
         <v>20.2</v>
-      </c>
-      <c r="X32" s="7">
-        <v>20.200000000000003</v>
       </c>
       <c r="Y32" s="7">
         <v>20.200000000000003</v>
       </c>
       <c r="Z32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="AA32" s="8">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.35">
@@ -3307,7 +3307,7 @@
         <v>10.5</v>
       </c>
       <c r="G34" s="7">
-        <v>10.499999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="H34" s="7">
         <v>10.5</v>
@@ -3331,10 +3331,10 @@
         <v>10.5</v>
       </c>
       <c r="O34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="P34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="Q34" s="7">
         <v>10.5</v>
@@ -3355,7 +3355,7 @@
         <v>10.5</v>
       </c>
       <c r="W34" s="7">
-        <v>10.499999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="X34" s="7">
         <v>10.499999999999993</v>
@@ -3367,7 +3367,7 @@
         <v>10.5</v>
       </c>
       <c r="AA34" s="8">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.35">
@@ -3387,10 +3387,10 @@
         <v>10</v>
       </c>
       <c r="F35" s="7">
-        <v>10.000000000000014</v>
+        <v>10</v>
       </c>
       <c r="G35" s="7">
-        <v>10.000000000000014</v>
+        <v>10</v>
       </c>
       <c r="H35" s="7">
         <v>10</v>
@@ -3402,10 +3402,10 @@
         <v>10</v>
       </c>
       <c r="K35" s="7">
-        <v>10.000000000000014</v>
+        <v>10</v>
       </c>
       <c r="L35" s="7">
-        <v>10.000000000000014</v>
+        <v>10</v>
       </c>
       <c r="M35" s="7">
         <v>10</v>
@@ -3417,25 +3417,25 @@
         <v>10</v>
       </c>
       <c r="P35" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>10</v>
+      </c>
+      <c r="R35" s="7">
+        <v>10</v>
+      </c>
+      <c r="S35" s="7">
+        <v>10</v>
+      </c>
+      <c r="T35" s="7">
+        <v>10</v>
+      </c>
+      <c r="U35" s="7">
+        <v>10</v>
+      </c>
+      <c r="V35" s="7">
         <v>9.9999999999999929</v>
-      </c>
-      <c r="Q35" s="7">
-        <v>10</v>
-      </c>
-      <c r="R35" s="7">
-        <v>10</v>
-      </c>
-      <c r="S35" s="7">
-        <v>10</v>
-      </c>
-      <c r="T35" s="7">
-        <v>10</v>
-      </c>
-      <c r="U35" s="7">
-        <v>10</v>
-      </c>
-      <c r="V35" s="7">
-        <v>10</v>
       </c>
       <c r="W35" s="7">
         <v>10</v>
@@ -3464,10 +3464,10 @@
         <v>0</v>
       </c>
       <c r="D36" s="7">
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="E36" s="7">
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="F36" s="7">
         <v>10</v>
@@ -3491,7 +3491,7 @@
         <v>10</v>
       </c>
       <c r="M36" s="7">
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="N36" s="7">
         <v>10</v>
@@ -3506,7 +3506,7 @@
         <v>10</v>
       </c>
       <c r="R36" s="7">
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="S36" s="7">
         <v>10</v>
@@ -3530,7 +3530,7 @@
         <v>10</v>
       </c>
       <c r="Z36" s="7">
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="AA36" s="8">
         <v>10</v>
@@ -3693,7 +3693,7 @@
         <v>10</v>
       </c>
       <c r="Y38" s="7">
-        <v>10</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="Z38" s="7">
         <v>10</v>
@@ -3716,37 +3716,37 @@
         <v>10.1</v>
       </c>
       <c r="E39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="F39" s="7">
         <v>10.1</v>
       </c>
-      <c r="F39" s="7">
+      <c r="G39" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="G39" s="7">
+      <c r="H39" s="7">
         <v>10.099999999999994</v>
-      </c>
-      <c r="H39" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="I39" s="7">
         <v>10.1</v>
       </c>
       <c r="J39" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="K39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="L39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="M39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="N39" s="7">
         <v>10.1</v>
       </c>
-      <c r="M39" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="N39" s="7">
-        <v>10.099999999999994</v>
-      </c>
       <c r="O39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="P39" s="7">
         <v>10.099999999999994</v>
@@ -3755,16 +3755,16 @@
         <v>10.099999999999994</v>
       </c>
       <c r="R39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="S39" s="7">
         <v>10.1</v>
       </c>
-      <c r="S39" s="7">
-        <v>10.099999999999994</v>
-      </c>
       <c r="T39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="U39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="V39" s="7">
         <v>10.099999999999994</v>
@@ -3776,13 +3776,13 @@
         <v>10.099999999999994</v>
       </c>
       <c r="Y39" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="Z39" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="AA39" s="8">
         <v>10.099999999999994</v>
-      </c>
-      <c r="Z39" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="AA39" s="8">
-        <v>10.1</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.35">
@@ -3796,55 +3796,55 @@
         <v>0</v>
       </c>
       <c r="D40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="E40" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="E40" s="7">
-        <v>10.1</v>
-      </c>
       <c r="F40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="G40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="H40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="I40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="J40" s="7">
         <v>10.100000000000001</v>
-      </c>
-      <c r="J40" s="7">
-        <v>10.099999999999998</v>
       </c>
       <c r="K40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="L40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="M40" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="M40" s="7">
+      <c r="N40" s="7">
         <v>10.1</v>
       </c>
-      <c r="N40" s="7">
+      <c r="O40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="P40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="R40" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="O40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="P40" s="7">
-        <v>10.099999999999998</v>
-      </c>
-      <c r="Q40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="R40" s="7">
+      <c r="S40" s="7">
         <v>10.1</v>
       </c>
-      <c r="S40" s="7">
-        <v>10.100000000000001</v>
-      </c>
       <c r="T40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.1</v>
       </c>
       <c r="U40" s="7">
         <v>10.100000000000001</v>
@@ -3853,16 +3853,16 @@
         <v>10.100000000000001</v>
       </c>
       <c r="W40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="X40" s="7">
         <v>10.099999999999998</v>
-      </c>
-      <c r="X40" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="Y40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="Z40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="AA40" s="8">
         <v>10.100000000000001</v>
@@ -3876,7 +3876,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="D41" s="7">
         <v>10</v>
@@ -3959,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="7">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D42" s="7">
         <v>12</v>
@@ -3983,7 +3983,7 @@
         <v>12</v>
       </c>
       <c r="K42" s="7">
-        <v>11.999999999999993</v>
+        <v>12</v>
       </c>
       <c r="L42" s="7">
         <v>12</v>
@@ -4001,7 +4001,7 @@
         <v>12</v>
       </c>
       <c r="Q42" s="7">
-        <v>11.999999999999993</v>
+        <v>12</v>
       </c>
       <c r="R42" s="7">
         <v>12</v>
@@ -4025,7 +4025,7 @@
         <v>12</v>
       </c>
       <c r="Y42" s="7">
-        <v>11.999999999999993</v>
+        <v>12</v>
       </c>
       <c r="Z42" s="7">
         <v>12</v>
@@ -4060,61 +4060,61 @@
         <v>350</v>
       </c>
       <c r="I43" s="7">
-        <v>649.99999999999523</v>
+        <v>650</v>
       </c>
       <c r="J43" s="7">
-        <v>949.99999999999272</v>
+        <v>950</v>
       </c>
       <c r="K43" s="7">
-        <v>1199.9999999999927</v>
+        <v>1200</v>
       </c>
       <c r="L43" s="7">
-        <v>1499.9999999999927</v>
+        <v>1500</v>
       </c>
       <c r="M43" s="7">
-        <v>1749.9999999999927</v>
+        <v>1750</v>
       </c>
       <c r="N43" s="7">
-        <v>1999.9999999999959</v>
+        <v>2000</v>
       </c>
       <c r="O43" s="7">
-        <v>2249.9999999999927</v>
+        <v>2250</v>
       </c>
       <c r="P43" s="7">
-        <v>2499.9999999999927</v>
+        <v>2500</v>
       </c>
       <c r="Q43" s="7">
-        <v>2699.9999999999927</v>
+        <v>2700</v>
       </c>
       <c r="R43" s="7">
-        <v>2949.9999999999927</v>
+        <v>2950</v>
       </c>
       <c r="S43" s="7">
-        <v>3199.9999999999927</v>
+        <v>3200</v>
       </c>
       <c r="T43" s="7">
-        <v>3399.9999999999923</v>
+        <v>3450</v>
       </c>
       <c r="U43" s="7">
-        <v>3649.9999999999927</v>
+        <v>3650</v>
       </c>
       <c r="V43" s="7">
-        <v>3849.9999999999927</v>
+        <v>3900</v>
       </c>
       <c r="W43" s="7">
-        <v>4099.9999999999927</v>
+        <v>4100</v>
       </c>
       <c r="X43" s="7">
-        <v>4299.9999999999927</v>
+        <v>4350</v>
       </c>
       <c r="Y43" s="7">
-        <v>4549.9999999999927</v>
+        <v>4550</v>
       </c>
       <c r="Z43" s="7">
-        <v>4749.9999999999927</v>
+        <v>4800</v>
       </c>
       <c r="AA43" s="8">
-        <v>4999.9999999999927</v>
+        <v>5000</v>
       </c>
       <c r="AB43" t="s">
         <v>17</v>
@@ -4146,61 +4146,61 @@
         <v>0</v>
       </c>
       <c r="I44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="J44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="K44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="L44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="M44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="N44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="O44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="P44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="R44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="S44" s="7">
-        <v>1.5276668818842154E-12</v>
+        <v>0</v>
       </c>
       <c r="T44" s="7">
-        <v>10.000000000001364</v>
+        <v>0</v>
       </c>
       <c r="U44" s="7">
-        <v>10.000000000001528</v>
+        <v>0</v>
       </c>
       <c r="V44" s="7">
-        <v>10.000000000001528</v>
+        <v>0</v>
       </c>
       <c r="W44" s="7">
-        <v>10.000000000001528</v>
+        <v>0</v>
       </c>
       <c r="X44" s="7">
-        <v>10.000000000001528</v>
+        <v>0</v>
       </c>
       <c r="Y44" s="7">
-        <v>10.000000000001528</v>
+        <v>0</v>
       </c>
       <c r="Z44" s="7">
-        <v>10.000000000002728</v>
+        <v>0</v>
       </c>
       <c r="AA44" s="8">
-        <v>10.000000000001528</v>
+        <v>0</v>
       </c>
       <c r="AB44" t="s">
         <v>18</v>
@@ -4307,79 +4307,79 @@
         <v>1</v>
       </c>
       <c r="B49" s="3">
-        <v>131.42935440158607</v>
+        <v>134.59011842103354</v>
       </c>
       <c r="C49" s="4">
-        <v>230.78839186512482</v>
+        <v>217.86156822982312</v>
       </c>
       <c r="D49" s="4">
-        <v>366.23840446601673</v>
+        <v>389.57841108034609</v>
       </c>
       <c r="E49" s="4">
-        <v>445.3803443500006</v>
+        <v>445.38034435000162</v>
       </c>
       <c r="F49" s="4">
-        <v>626.31845204158526</v>
+        <v>630.82005026299578</v>
       </c>
       <c r="G49" s="4">
-        <v>982.41113455138793</v>
+        <v>988.85720646479581</v>
       </c>
       <c r="H49" s="4">
-        <v>840.47206649496934</v>
+        <v>846.83951964717062</v>
       </c>
       <c r="I49" s="4">
-        <v>756.86129874202049</v>
+        <v>762.88527618929709</v>
       </c>
       <c r="J49" s="4">
-        <v>660.12275018253536</v>
+        <v>665.82177982875828</v>
       </c>
       <c r="K49" s="4">
-        <v>620.73242998209787</v>
+        <v>626.12404029153174</v>
       </c>
       <c r="L49" s="4">
-        <v>499.95562550576074</v>
+        <v>505.05639941523867</v>
       </c>
       <c r="M49" s="4">
-        <v>437.91364253219143</v>
+        <v>442.73926845513012</v>
       </c>
       <c r="N49" s="4">
-        <v>365.52129126400126</v>
+        <v>370.08661134316026</v>
       </c>
       <c r="O49" s="4">
-        <v>283.38286925755358</v>
+        <v>287.70192501487048</v>
       </c>
       <c r="P49" s="4">
-        <v>192.07049057331494</v>
+        <v>196.15656609734955</v>
       </c>
       <c r="Q49" s="4">
-        <v>161.84933534702861</v>
+        <v>165.71499815071411</v>
       </c>
       <c r="R49" s="4">
-        <v>53.785256585355228</v>
+        <v>57.442396259818224</v>
       </c>
       <c r="S49" s="4">
-        <v>-41.526512318798495</v>
+        <v>-41.526512318802133</v>
       </c>
       <c r="T49" s="4">
-        <v>-123.18520092966764</v>
+        <v>-177.93212082638502</v>
       </c>
       <c r="U49" s="4">
-        <v>-252.95367203609396</v>
+        <v>-239.68408793039606</v>
       </c>
       <c r="V49" s="4">
-        <v>-301.59993596223268</v>
+        <v>-332.28171754239145</v>
       </c>
       <c r="W49" s="4">
-        <v>-355.27098067622768</v>
+        <v>-375.11101945637927</v>
       </c>
       <c r="X49" s="4">
-        <v>-493.39748449742729</v>
+        <v>-468.42867982535995</v>
       </c>
       <c r="Y49" s="4">
-        <v>-526.97265273668495</v>
+        <v>-526.97265273668859</v>
       </c>
       <c r="Z49" s="4">
-        <v>-607.61835661131522</v>
+        <v>-624.09898603320767</v>
       </c>
       <c r="AA49" s="5">
         <v>-635.81607690750707</v>
@@ -4390,79 +4390,79 @@
         <v>2</v>
       </c>
       <c r="B50" s="6">
-        <v>-374.47064559841419</v>
+        <v>-371.30988157896644</v>
       </c>
       <c r="C50" s="7">
-        <v>-176.16919593256281</v>
+        <v>-169.70578411491221</v>
       </c>
       <c r="D50" s="7">
-        <v>-229.71997723300865</v>
+        <v>-241.38998054017338</v>
       </c>
       <c r="E50" s="7">
-        <v>-291.56660415000079</v>
+        <v>-291.56660415000135</v>
       </c>
       <c r="F50" s="7">
-        <v>-575.15027277221986</v>
+        <v>-584.15346921504101</v>
       </c>
       <c r="G50" s="7">
-        <v>-719.0494954727817</v>
+        <v>-712.60342355937246</v>
       </c>
       <c r="H50" s="7">
-        <v>-543.93180919941642</v>
+        <v>-537.56435604721537</v>
       </c>
       <c r="I50" s="7">
-        <v>-360.7823118336201</v>
+        <v>-354.75833438633686</v>
       </c>
       <c r="J50" s="7">
-        <v>-191.05975288828813</v>
+        <v>-185.3607232420577</v>
       </c>
       <c r="K50" s="7">
-        <v>-14.290815616362408</v>
+        <v>-8.8992053069193844</v>
       </c>
       <c r="L50" s="7">
-        <v>130.78707069691475</v>
+        <v>135.88784460639994</v>
       </c>
       <c r="M50" s="7">
-        <v>284.29247073005416</v>
+        <v>289.11809665301365</v>
       </c>
       <c r="N50" s="7">
-        <v>427.13742891565283</v>
+        <v>431.70274899482411</v>
       </c>
       <c r="O50" s="7">
-        <v>559.92345214807517</v>
+        <v>564.24250790540009</v>
       </c>
       <c r="P50" s="7">
-        <v>683.2198387098515</v>
+        <v>687.30591423389353</v>
       </c>
       <c r="Q50" s="7">
-        <v>817.28892761679458</v>
+        <v>821.15459042048769</v>
       </c>
       <c r="R50" s="7">
-        <v>923.19370518555002</v>
+        <v>926.85084486002006</v>
       </c>
       <c r="S50" s="7">
-        <v>1041.5265123187985</v>
+        <v>1041.5265123188021</v>
       </c>
       <c r="T50" s="7">
-        <v>1123.1852009296676</v>
+        <v>1118.4382810329578</v>
       </c>
       <c r="U50" s="7">
-        <v>1206.4039634399765</v>
+        <v>1219.673547545681</v>
       </c>
       <c r="V50" s="7">
-        <v>1292.4333981830744</v>
+        <v>1275.7969613433931</v>
       </c>
       <c r="W50" s="7">
-        <v>1325.0587793068864</v>
+        <v>1350.1509669076961</v>
       </c>
       <c r="X50" s="7">
-        <v>1470.5057225106732</v>
+        <v>1423.879947997611</v>
       </c>
       <c r="Y50" s="7">
-        <v>1526.9726527366849</v>
+        <v>1526.9726527366886</v>
       </c>
       <c r="Z50" s="7">
-        <v>1607.6183566113152</v>
+        <v>1624.0989860332077</v>
       </c>
       <c r="AA50" s="8">
         <v>1635.8160769075071</v>
@@ -4473,73 +4473,73 @@
         <v>3</v>
       </c>
       <c r="B51" s="9">
-        <v>243.0412911968281</v>
+        <v>236.7197631579329</v>
       </c>
       <c r="C51" s="10">
-        <v>-54.619195932561979</v>
+        <v>-48.155784114910915</v>
       </c>
       <c r="D51" s="10">
-        <v>-136.51842723300805</v>
+        <v>-148.1884305401727</v>
       </c>
       <c r="E51" s="10">
-        <v>-153.81374019999981</v>
+        <v>-153.81374020000032</v>
       </c>
       <c r="F51" s="10">
-        <v>-51.168179269365396</v>
+        <v>-46.666581047954878</v>
       </c>
       <c r="G51" s="10">
-        <v>-263.36163907860646</v>
+        <v>-276.25378290542335</v>
       </c>
       <c r="H51" s="10">
-        <v>-296.54025729555292</v>
+        <v>-309.27516359995525</v>
       </c>
       <c r="I51" s="10">
-        <v>-396.07898690840022</v>
+        <v>-408.12694180296023</v>
       </c>
       <c r="J51" s="10">
-        <v>-469.06299729424722</v>
+        <v>-480.46105658670058</v>
       </c>
       <c r="K51" s="10">
-        <v>-606.44161436573552</v>
+        <v>-617.22483498461236</v>
       </c>
       <c r="L51" s="10">
-        <v>-630.74269620267546</v>
+        <v>-640.94424402163861</v>
       </c>
       <c r="M51" s="10">
-        <v>-722.20611326224559</v>
+        <v>-731.85736510814377</v>
       </c>
       <c r="N51" s="10">
-        <v>-792.6587201796541</v>
+        <v>-801.78936033798436</v>
       </c>
       <c r="O51" s="10">
-        <v>-843.30632140562898</v>
+        <v>-851.94443292027063</v>
       </c>
       <c r="P51" s="10">
-        <v>-875.29032928316622</v>
+        <v>-883.46248033124311</v>
       </c>
       <c r="Q51" s="10">
-        <v>-979.13826296382319</v>
+        <v>-986.8695885712018</v>
       </c>
       <c r="R51" s="10">
-        <v>-976.97896177090524</v>
+        <v>-984.29324111983806</v>
       </c>
       <c r="S51" s="10">
         <v>-1000</v>
       </c>
       <c r="T51" s="10">
-        <v>-1000</v>
+        <v>-940.50616020657276</v>
       </c>
       <c r="U51" s="10">
-        <v>-953.45029140388249</v>
+        <v>-979.98945961528489</v>
       </c>
       <c r="V51" s="10">
-        <v>-990.83346222084174</v>
+        <v>-943.5152438010017</v>
       </c>
       <c r="W51" s="10">
-        <v>-969.7877986306587</v>
+        <v>-975.03994745131683</v>
       </c>
       <c r="X51" s="10">
-        <v>-977.10823801324636</v>
+        <v>-955.45126817225093</v>
       </c>
       <c r="Y51" s="10">
         <v>-1000</v>
@@ -4639,86 +4639,86 @@
         <v>8</v>
       </c>
       <c r="B54" s="15">
-        <v>187067.81092078245</v>
+        <v>185343.2957730343</v>
       </c>
       <c r="C54" s="16">
-        <v>150732.88932861568</v>
+        <v>150354.42590554856</v>
       </c>
       <c r="D54" s="16">
-        <v>123175.51953414564</v>
+        <v>122850.98857876577</v>
       </c>
       <c r="E54" s="16">
-        <v>115689.69506787832</v>
+        <v>115767.04458876407</v>
       </c>
       <c r="F54" s="16">
-        <v>110744.52859723844</v>
+        <v>110839.76863109934</v>
       </c>
       <c r="G54" s="16">
-        <v>107424.10359766634</v>
+        <v>107601.0888445216</v>
       </c>
       <c r="H54" s="16">
-        <v>3661670.1339732334</v>
+        <v>4801787.6002829252</v>
       </c>
       <c r="I54" s="16">
-        <v>6106867.0528585901</v>
+        <v>7143329.7763654375</v>
       </c>
       <c r="J54" s="16">
-        <v>8076957.997792678</v>
+        <v>9019190.2145876419</v>
       </c>
       <c r="K54" s="16">
-        <v>9256611.1456463076</v>
+        <v>10113180.192269597</v>
       </c>
       <c r="L54" s="16">
-        <v>10501696.110261483</v>
+        <v>11280390.344767999</v>
       </c>
       <c r="M54" s="16">
-        <v>11128410.409977544</v>
+        <v>11836310.046315253</v>
       </c>
       <c r="N54" s="16">
-        <v>11554244.936863484</v>
+        <v>12197786.437222462</v>
       </c>
       <c r="O54" s="16">
-        <v>11810564.306614228</v>
+        <v>12395598.917741014</v>
       </c>
       <c r="P54" s="16">
-        <v>11924687.711666334</v>
+        <v>12456534.677815856</v>
       </c>
       <c r="Q54" s="16">
-        <v>11704993.803017179</v>
+        <v>12188488.739747677</v>
       </c>
       <c r="R54" s="16">
-        <v>11622410.792931966</v>
+        <v>12061949.661892131</v>
       </c>
       <c r="S54" s="16">
-        <v>11458222.771363657</v>
+        <v>11857739.354170015</v>
       </c>
       <c r="T54" s="16">
-        <v>11136757.908128934</v>
+        <v>11590726.403390428</v>
       </c>
       <c r="U54" s="16">
-        <v>10861596.891806329</v>
+        <v>11127184.463038474</v>
       </c>
       <c r="V54" s="16">
-        <v>10410656.179152189</v>
+        <v>10785840.636510139</v>
       </c>
       <c r="W54" s="16">
-        <v>10073525.415561445</v>
+        <v>10292985.498904472</v>
       </c>
       <c r="X54" s="16">
-        <v>9601097.70867154</v>
+        <v>9911160.63153263</v>
       </c>
       <c r="Y54" s="16">
-        <v>9231791.2591375373</v>
+        <v>9413197.9445184693</v>
       </c>
       <c r="Z54" s="16">
-        <v>8758907.2165259589</v>
+        <v>9015230.6338730641</v>
       </c>
       <c r="AA54" s="17">
-        <v>8378810.8095743293</v>
+        <v>8528739.7553199679</v>
       </c>
       <c r="AB54" s="18">
         <f>SUM(TotalCost)</f>
-        <v>198055315.10857129</v>
+        <v>208810108.5425874</v>
       </c>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.35">
@@ -4812,86 +4812,86 @@
         <v>10</v>
       </c>
       <c r="B57" s="3">
-        <v>13546.179193698952</v>
+        <v>13395.809006237749</v>
       </c>
       <c r="C57" s="4">
-        <v>10789.085021802086</v>
+        <v>10788.134900264893</v>
       </c>
       <c r="D57" s="4">
-        <v>9571.5136009432536</v>
+        <v>9558.8049673417518</v>
       </c>
       <c r="E57" s="4">
-        <v>9343.2363146215939</v>
+        <v>9312.0249598840237</v>
       </c>
       <c r="F57" s="4">
-        <v>8651.2475016100889</v>
+        <v>8666.7645106792916</v>
       </c>
       <c r="G57" s="4">
-        <v>8038.2165093081167</v>
+        <v>7992.7910405343282</v>
       </c>
       <c r="H57" s="4">
-        <v>7228.5430222441555</v>
+        <v>7231.7522186328661</v>
       </c>
       <c r="I57" s="4">
-        <v>6936.5566496032461</v>
+        <v>6939.5927342366713</v>
       </c>
       <c r="J57" s="4">
-        <v>6638.6779565246034</v>
+        <v>6641.5502674662948</v>
       </c>
       <c r="K57" s="4">
-        <v>6425.4833683574752</v>
+        <v>6428.200739953425</v>
       </c>
       <c r="L57" s="4">
-        <v>6116.9571653142193</v>
+        <v>6119.5279553645905</v>
       </c>
       <c r="M57" s="4">
-        <v>5893.8271200660729</v>
+        <v>5896.259235531229</v>
       </c>
       <c r="N57" s="4">
-        <v>5666.2309912248211</v>
+        <v>5668.5319125448614</v>
       </c>
       <c r="O57" s="4">
-        <v>5434.4800992776509</v>
+        <v>5436.6569033792557</v>
       </c>
       <c r="P57" s="4">
-        <v>5198.8696050192648</v>
+        <v>5200.9289870833718</v>
       </c>
       <c r="Q57" s="4">
-        <v>5049.8700358851456</v>
+        <v>5051.8183299381972</v>
       </c>
       <c r="R57" s="4">
-        <v>4807.3655203270955</v>
+        <v>4809.2087187230172</v>
       </c>
       <c r="S57" s="4">
-        <v>4732.4965182340493</v>
+        <v>5099.216757121816</v>
       </c>
       <c r="T57" s="4">
-        <v>4812.4019462951419</v>
+        <v>4929.3134908072625</v>
       </c>
       <c r="U57" s="4">
-        <v>4534.2511210002167</v>
+        <v>4478.6003618073237</v>
       </c>
       <c r="V57" s="4">
-        <v>4082.6080390532206</v>
+        <v>4143.4773551581548</v>
       </c>
       <c r="W57" s="4">
-        <v>3692.1905943356433</v>
+        <v>3708.119386265606</v>
       </c>
       <c r="X57" s="4">
-        <v>3334.3163282404275</v>
+        <v>3352.1940770678111</v>
       </c>
       <c r="Y57" s="4">
-        <v>3013.074674252141</v>
+        <v>2961.9204175372593</v>
       </c>
       <c r="Z57" s="4">
-        <v>2738.5268734451006</v>
+        <v>2768.3019467310851</v>
       </c>
       <c r="AA57" s="5">
-        <v>2732.9195703129299</v>
+        <v>2672.733379103548</v>
       </c>
       <c r="AB57" s="12">
         <f>SUM(B57:AA57)</f>
-        <v>159009.12534099666</v>
+        <v>159252.2345593957</v>
       </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.35">
@@ -4899,86 +4899,86 @@
         <v>11</v>
       </c>
       <c r="B58" s="6">
-        <v>2499.3386430939754</v>
+        <v>2413.9885322768305</v>
       </c>
       <c r="C58" s="7">
-        <v>2265.7857151755957</v>
+        <v>2265.7469347046895</v>
       </c>
       <c r="D58" s="7">
-        <v>2260.7715595915051</v>
+        <v>2260.5965095418974</v>
       </c>
       <c r="E58" s="7">
-        <v>1956.7083491572898</v>
+        <v>1949.7252897817209</v>
       </c>
       <c r="F58" s="7">
-        <v>1617.4694729091009</v>
+        <v>1610.7981043449702</v>
       </c>
       <c r="G58" s="7">
-        <v>1176.644653667239</v>
+        <v>1150.402694907754</v>
       </c>
       <c r="H58" s="7">
-        <v>935.89314664263384</v>
+        <v>928.34771465727567</v>
       </c>
       <c r="I58" s="7">
-        <v>831.55391943883365</v>
+        <v>824.41550616380698</v>
       </c>
       <c r="J58" s="7">
-        <v>743.09495060785889</v>
+        <v>736.3416004770794</v>
       </c>
       <c r="K58" s="7">
-        <v>626.90508383154338</v>
+        <v>620.51602561485879</v>
       </c>
       <c r="L58" s="7">
-        <v>567.58789435624578</v>
+        <v>561.54347727350978</v>
       </c>
       <c r="M58" s="7">
-        <v>478.90260207516081</v>
+        <v>473.18423535646207</v>
       </c>
       <c r="N58" s="7">
-        <v>402.81815084418042</v>
+        <v>397.40824655042883</v>
       </c>
       <c r="O58" s="7">
-        <v>338.62146895083538</v>
+        <v>333.50338787838001</v>
       </c>
       <c r="P58" s="7">
-        <v>285.63764931281798</v>
+        <v>280.795649816832</v>
       </c>
       <c r="Q58" s="7">
-        <v>200.50552898174573</v>
+        <v>195.92471855937299</v>
       </c>
       <c r="R58" s="7">
-        <v>168.06517533664049</v>
+        <v>163.73146482239679</v>
       </c>
       <c r="S58" s="7">
-        <v>376.48025651314629</v>
+        <v>376.80973050205012</v>
       </c>
       <c r="T58" s="7">
-        <v>256.3691211824991</v>
+        <v>356.79383208201386</v>
       </c>
       <c r="U58" s="7">
-        <v>240.35984607053751</v>
+        <v>199.98936917622353</v>
       </c>
       <c r="V58" s="7">
-        <v>107.36132705458158</v>
+        <v>207.39779424175492</v>
       </c>
       <c r="W58" s="7">
-        <v>126.55198545137324</v>
+        <v>98.517424047122049</v>
       </c>
       <c r="X58" s="7">
-        <v>21.304213423380013</v>
+        <v>128.34501411280365</v>
       </c>
       <c r="Y58" s="7">
-        <v>78.242360131486649</v>
+        <v>20.110079478994006</v>
       </c>
       <c r="Z58" s="7">
-        <v>19.112966644304979</v>
+        <v>76.764230252011771</v>
       </c>
       <c r="AA58" s="8">
-        <v>83.379036357627911</v>
+        <v>17.963283589017003</v>
       </c>
       <c r="AB58" s="13">
         <f t="shared" ref="AB58:AB61" si="0">SUM(B58:AA58)</f>
-        <v>18665.465076802142</v>
+        <v>18649.660850210254</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.35">
@@ -4986,86 +4986,86 @@
         <v>12</v>
       </c>
       <c r="B59" s="6">
-        <v>14036617.048186619</v>
+        <v>14017815.711210009</v>
       </c>
       <c r="C59" s="7">
-        <v>13279448.236726513</v>
+        <v>13261661.088989634</v>
       </c>
       <c r="D59" s="7">
-        <v>12563122.928161718</v>
+        <v>12546295.261862919</v>
       </c>
       <c r="E59" s="7">
-        <v>11885437.925921649</v>
+        <v>11869517.984329404</v>
       </c>
       <c r="F59" s="7">
-        <v>11244308.879146414</v>
+        <v>11229247.697411515</v>
       </c>
       <c r="G59" s="7">
-        <v>10637763.871863946</v>
+        <v>10623515.126418665</v>
       </c>
       <c r="H59" s="7">
-        <v>10063937.357982313</v>
+        <v>10050457.224063339</v>
       </c>
       <c r="I59" s="7">
-        <v>9521064.4234430883</v>
+        <v>9508311.4403000269</v>
       </c>
       <c r="J59" s="7">
-        <v>9007475.3578879535</v>
+        <v>8995410.3012627866</v>
       </c>
       <c r="K59" s="7">
-        <v>8521590.5191426184</v>
+        <v>8510176.2806279492</v>
       </c>
       <c r="L59" s="7">
-        <v>8061915.4747228203</v>
+        <v>8051116.9476278042</v>
       </c>
       <c r="M59" s="7">
-        <v>7627036.4054191327</v>
+        <v>7616820.3767920863</v>
       </c>
       <c r="N59" s="7">
-        <v>7215615.7568234513</v>
+        <v>7205950.8052990176</v>
       </c>
       <c r="O59" s="7">
-        <v>6826388.1254225783</v>
+        <v>6817244.5245792558</v>
       </c>
       <c r="P59" s="7">
-        <v>6458156.3666057838</v>
+        <v>6449505.9935365925</v>
       </c>
       <c r="Q59" s="7">
-        <v>6109787.9126157882</v>
+        <v>6101604.1614308441</v>
       </c>
       <c r="R59" s="7">
-        <v>5780211.289118303</v>
+        <v>5772468.9891132778</v>
       </c>
       <c r="S59" s="7">
-        <v>5468412.8196761673</v>
+        <v>5461088.1579149337</v>
       </c>
       <c r="T59" s="7">
-        <v>5173433.5079920683</v>
+        <v>5166503.9560654238</v>
       </c>
       <c r="U59" s="7">
-        <v>4894366.0883305576</v>
+        <v>4887810.3330657603</v>
       </c>
       <c r="V59" s="7">
-        <v>4630352.2350473953</v>
+        <v>4624150.1129553942</v>
       </c>
       <c r="W59" s="7">
-        <v>4380579.9226435749</v>
+        <v>4374712.3579023099</v>
       </c>
       <c r="X59" s="7">
-        <v>4140395.2704786304</v>
+        <v>4138729.8740074006</v>
       </c>
       <c r="Y59" s="7">
-        <v>3917052.4126403639</v>
+        <v>3895260.8637902341</v>
       </c>
       <c r="Z59" s="7">
-        <v>3705757.2045767521</v>
+        <v>3685141.1441713162</v>
       </c>
       <c r="AA59" s="8">
-        <v>3505859.7671445911</v>
+        <v>3479546.1153387381</v>
       </c>
       <c r="AB59" s="13">
         <f t="shared" si="0"/>
-        <v>198656087.10772076</v>
+        <v>198340062.83006662</v>
       </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.35">
@@ -5073,86 +5073,86 @@
         <v>13</v>
       </c>
       <c r="B60" s="6">
-        <v>1143.9782175531147</v>
+        <v>1143.0110237631638</v>
       </c>
       <c r="C60" s="7">
-        <v>1129.7721214047631</v>
+        <v>1129.461877637516</v>
       </c>
       <c r="D60" s="7">
-        <v>1120.5957231830098</v>
+        <v>1120.245623083795</v>
       </c>
       <c r="E60" s="7">
-        <v>976.93472901298071</v>
+        <v>973.64233599940439</v>
       </c>
       <c r="F60" s="7">
-        <v>818.75420488900284</v>
+        <v>815.41852060693759</v>
       </c>
       <c r="G60" s="7">
-        <v>646.96597715865585</v>
+        <v>642.61487861710532</v>
       </c>
       <c r="H60" s="7">
-        <v>598.81743474642724</v>
+        <v>595.01606521456324</v>
       </c>
       <c r="I60" s="7">
-        <v>541.5882799209345</v>
+        <v>537.99196538490833</v>
       </c>
       <c r="J60" s="7">
-        <v>492.37150718837751</v>
+        <v>488.96918648957967</v>
       </c>
       <c r="K60" s="7">
-        <v>430.19451494946418</v>
+        <v>426.97572359472923</v>
       </c>
       <c r="L60" s="7">
-        <v>395.68351670267634</v>
+        <v>392.63835467871553</v>
       </c>
       <c r="M60" s="7">
-        <v>347.38769726406582</v>
+        <v>344.50679858806615</v>
       </c>
       <c r="N60" s="7">
-        <v>305.45253374787387</v>
+        <v>302.72703766061431</v>
       </c>
       <c r="O60" s="7">
-        <v>269.51889388741722</v>
+        <v>266.94041760029523</v>
       </c>
       <c r="P60" s="7">
-        <v>239.24687366341439</v>
+        <v>236.8074865755631</v>
       </c>
       <c r="Q60" s="7">
-        <v>193.78982344232776</v>
+        <v>191.48202274852468</v>
       </c>
       <c r="R60" s="7">
-        <v>173.89310685284732</v>
+        <v>171.70979446719025</v>
       </c>
       <c r="S60" s="7">
-        <v>157.22690203843942</v>
+        <v>157.16414508817184</v>
       </c>
       <c r="T60" s="7">
-        <v>134.55986220872947</v>
+        <v>150.30403313900993</v>
       </c>
       <c r="U60" s="7">
-        <v>127.91544856979749</v>
+        <v>121.44847929844828</v>
       </c>
       <c r="V60" s="7">
-        <v>102.91027724177117</v>
+        <v>118.44625605412568</v>
       </c>
       <c r="W60" s="7">
-        <v>101.29075584735811</v>
+        <v>97.386657498214333</v>
       </c>
       <c r="X60" s="7">
-        <v>81.445311520562399</v>
+        <v>97.772843926952973</v>
       </c>
       <c r="Y60" s="7">
-        <v>86.13681204998511</v>
+        <v>76.892153504437573</v>
       </c>
       <c r="Z60" s="7">
-        <v>73.312417485977619</v>
+        <v>81.722504254116501</v>
       </c>
       <c r="AA60" s="8">
-        <v>79.531370678120368</v>
+        <v>69.096041433177916</v>
       </c>
       <c r="AB60" s="13">
         <f t="shared" si="0"/>
-        <v>10769.274313208094</v>
+        <v>10750.392226907325</v>
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.35">
@@ -5160,86 +5160,86 @@
         <v>14</v>
       </c>
       <c r="B61" s="9">
-        <v>163.39106260949535</v>
+        <v>163.18245218421177</v>
       </c>
       <c r="C61" s="10">
-        <v>161.60491517559535</v>
+        <v>161.56613470468946</v>
       </c>
       <c r="D61" s="10">
-        <v>161.04865911830098</v>
+        <v>161.01364910837947</v>
       </c>
       <c r="E61" s="10">
-        <v>139.60637275413825</v>
+        <v>139.11516895775793</v>
       </c>
       <c r="F61" s="10">
-        <v>115.8758400273196</v>
+        <v>115.37616262474303</v>
       </c>
       <c r="G61" s="10">
-        <v>89.795212632073813</v>
+        <v>89.137713296906171</v>
       </c>
       <c r="H61" s="10">
-        <v>82.982543449475557</v>
+        <v>82.409472665777457</v>
       </c>
       <c r="I61" s="10">
-        <v>74.732890012147365</v>
+        <v>74.190732041892176</v>
       </c>
       <c r="J61" s="10">
-        <v>67.690165244591554</v>
+        <v>67.177252576431087</v>
       </c>
       <c r="K61" s="10">
-        <v>58.611757177479994</v>
+        <v>58.12651224963053</v>
       </c>
       <c r="L61" s="10">
-        <v>53.784020863233145</v>
+        <v>53.324951211379776</v>
       </c>
       <c r="M61" s="10">
-        <v>46.796271775283458</v>
+        <v>46.361965442218199</v>
       </c>
       <c r="N61" s="10">
-        <v>40.766412085848664</v>
+        <v>40.355533278724131</v>
       </c>
       <c r="O61" s="10">
-        <v>35.640292221125712</v>
+        <v>35.251577202966622</v>
       </c>
       <c r="P61" s="10">
-        <v>31.366661256795805</v>
+        <v>30.998914459632303</v>
       </c>
       <c r="Q61" s="10">
-        <v>24.721894475837018</v>
+        <v>24.373984823504905</v>
       </c>
       <c r="R61" s="10">
-        <v>22.010308776301255</v>
+        <v>21.681166205599194</v>
       </c>
       <c r="S61" s="10">
-        <v>19.741154271884469</v>
+        <v>19.741154271884458</v>
       </c>
       <c r="T61" s="10">
-        <v>16.60222599670151</v>
+        <v>19.046411826166125</v>
       </c>
       <c r="U61" s="10">
-        <v>15.884433069073784</v>
+        <v>14.890935490292136</v>
       </c>
       <c r="V61" s="10">
-        <v>12.298641559585645</v>
+        <v>14.6971451831499</v>
       </c>
       <c r="W61" s="10">
-        <v>12.263056912552065</v>
+        <v>11.699693810643726</v>
       </c>
       <c r="X61" s="10">
-        <v>9.4693600678932679</v>
+        <v>11.955175369863897</v>
       </c>
       <c r="Y61" s="10">
-        <v>10.360569302308685</v>
+        <v>8.9762281671597304</v>
       </c>
       <c r="Z61" s="10">
-        <v>8.5784797206641805</v>
+        <v>9.8666355084589021</v>
       </c>
       <c r="AA61" s="11">
-        <v>9.6541542637496889</v>
+        <v>8.0928215381501456</v>
       </c>
       <c r="AB61" s="14">
         <f t="shared" si="0"/>
-        <v>1485.2773548194559</v>
+        <v>1482.6095442002131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed new solar/wind constraint again
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -734,49 +734,49 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>495.91917837745905</v>
+        <v>495.9191783774736</v>
       </c>
       <c r="H3" s="4">
-        <v>396.80584595542996</v>
+        <v>396.80584595544178</v>
       </c>
       <c r="I3" s="4">
-        <v>421.67530116494368</v>
+        <v>421.67530116495027</v>
       </c>
       <c r="J3" s="4">
-        <v>407.00758733669591</v>
+        <v>407.00758733670591</v>
       </c>
       <c r="K3" s="4">
-        <v>514.22584895567445</v>
+        <v>514.22584895567707</v>
       </c>
       <c r="L3" s="4">
-        <v>427.12120987952449</v>
+        <v>427.12120987953153</v>
       </c>
       <c r="M3" s="4">
-        <v>466.05298510390321</v>
+        <v>466.05298510391117</v>
       </c>
       <c r="N3" s="4">
-        <v>473.76113038564222</v>
+        <v>473.76113038564449</v>
       </c>
       <c r="O3" s="4">
-        <v>452.05418306797833</v>
+        <v>452.05418306798612</v>
       </c>
       <c r="P3" s="4">
-        <v>402.64424198762526</v>
+        <v>402.64424198762902</v>
       </c>
       <c r="Q3" s="4">
-        <v>486.32270904100915</v>
+        <v>486.3227090409855</v>
       </c>
       <c r="R3" s="4">
-        <v>386.28310279959442</v>
+        <v>386.28310279959396</v>
       </c>
       <c r="S3" s="4">
-        <v>419.45037015797897</v>
+        <v>419.45037015797811</v>
       </c>
       <c r="T3" s="4">
-        <v>129.03291882238841</v>
+        <v>129.03291882239137</v>
       </c>
       <c r="U3" s="4">
-        <v>117.86808104206888</v>
+        <v>117.86808104206641</v>
       </c>
       <c r="V3" s="4">
         <v>0</v>
@@ -805,10 +805,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>130.26735234474739</v>
+        <v>130.26735234473745</v>
       </c>
       <c r="D4" s="7">
-        <v>641.05189162049885</v>
+        <v>641.0518916205184</v>
       </c>
       <c r="E4" s="7">
         <v>665.6</v>
@@ -936,7 +936,7 @@
         <v>46.5</v>
       </c>
       <c r="S5" s="7">
-        <v>42.477210131936829</v>
+        <v>42.477210131937454</v>
       </c>
       <c r="T5" s="7">
         <v>46.5</v>
@@ -1051,7 +1051,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>192.67035526309442</v>
+        <v>192.67035526309974</v>
       </c>
       <c r="C7" s="7">
         <v>464</v>
@@ -1369,7 +1369,7 @@
         <v>88</v>
       </c>
       <c r="Y10" s="7">
-        <v>85.51375562129715</v>
+        <v>85.513755621295331</v>
       </c>
       <c r="Z10" s="7">
         <v>0</v>
@@ -1606,13 +1606,13 @@
         <v>154</v>
       </c>
       <c r="U13" s="7">
-        <v>153.99999999999935</v>
+        <v>154</v>
       </c>
       <c r="V13" s="7">
-        <v>90.066924690423036</v>
+        <v>90.066924690421729</v>
       </c>
       <c r="W13" s="7">
-        <v>44.932226380952073</v>
+        <v>44.932226380950823</v>
       </c>
       <c r="X13" s="7">
         <v>0</v>
@@ -1638,7 +1638,7 @@
         <v>150</v>
       </c>
       <c r="D14" s="7">
-        <v>85.515108379499111</v>
+        <v>85.515108379479443</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -1704,7 +1704,7 @@
         <v>150</v>
       </c>
       <c r="Z14" s="7">
-        <v>132.96125884377807</v>
+        <v>132.9612588437767</v>
       </c>
       <c r="AA14" s="8">
         <v>0</v>
@@ -1724,10 +1724,10 @@
         <v>1848</v>
       </c>
       <c r="E15" s="7">
-        <v>1254.6797472637363</v>
+        <v>1254.6797472637277</v>
       </c>
       <c r="F15" s="7">
-        <v>607.83770948546908</v>
+        <v>607.83770948545941</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>604.92635573625989</v>
+        <v>604.92635573626876</v>
       </c>
       <c r="F16" s="7">
         <v>656.1</v>
@@ -1873,7 +1873,7 @@
         <v>656.1</v>
       </c>
       <c r="AA16" s="8">
-        <v>651.55241017337175</v>
+        <v>651.55241017337084</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
@@ -1893,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="7">
-        <v>24.084748441526244</v>
+        <v>24.084748441537158</v>
       </c>
       <c r="G17" s="7">
         <v>50.3</v>
@@ -1932,7 +1932,7 @@
         <v>50.3</v>
       </c>
       <c r="S17" s="7">
-        <v>28.366370434874398</v>
+        <v>28.36637043487417</v>
       </c>
       <c r="T17" s="7">
         <v>50.3</v>
@@ -2062,7 +2062,7 @@
         <v>257</v>
       </c>
       <c r="G19" s="7">
-        <v>152.5020816708784</v>
+        <v>152.50208167086572</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
@@ -2083,13 +2083,13 @@
         <v>0</v>
       </c>
       <c r="N19" s="7">
-        <v>0</v>
+        <v>-5.2295945351943374E-12</v>
       </c>
       <c r="O19" s="7">
-        <v>0</v>
+        <v>-1.3642420526593924E-11</v>
       </c>
       <c r="P19" s="7">
-        <v>0</v>
+        <v>-7.1622707764618099E-12</v>
       </c>
       <c r="Q19" s="7">
         <v>0</v>
@@ -2101,16 +2101,16 @@
         <v>257</v>
       </c>
       <c r="T19" s="7">
-        <v>243.3262774589241</v>
+        <v>243.32627745892165</v>
       </c>
       <c r="U19" s="7">
-        <v>128.51664800577601</v>
+        <v>128.51664800577859</v>
       </c>
       <c r="V19" s="7">
-        <v>135.00956691885</v>
+        <v>135.00956691885051</v>
       </c>
       <c r="W19" s="7">
-        <v>55.50825365280312</v>
+        <v>55.508253652803432</v>
       </c>
       <c r="X19" s="7">
         <v>79.06445869096126</v>
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="Z19" s="7">
-        <v>42.671387508933805</v>
+        <v>42.67138750893254</v>
       </c>
       <c r="AA19" s="8">
         <v>0</v>
@@ -2148,34 +2148,34 @@
         <v>2269.6</v>
       </c>
       <c r="H20" s="7">
-        <v>2237.1019054333419</v>
+        <v>2237.1019054333301</v>
       </c>
       <c r="I20" s="7">
-        <v>1978.7119199863257</v>
+        <v>1978.7119199863191</v>
       </c>
       <c r="J20" s="7">
-        <v>1760.4574188049342</v>
+        <v>1760.4574188049241</v>
       </c>
       <c r="K20" s="7">
-        <v>1470.9206422412299</v>
+        <v>1470.9206422412265</v>
       </c>
       <c r="L20" s="7">
-        <v>1326.3158997381511</v>
+        <v>1326.3158997381433</v>
       </c>
       <c r="M20" s="7">
-        <v>1106.2893585003299</v>
+        <v>1106.2893585003221</v>
       </c>
       <c r="N20" s="7">
-        <v>918.10659431102772</v>
+        <v>918.10659431102954</v>
       </c>
       <c r="O20" s="7">
-        <v>759.96465115096203</v>
+        <v>759.96465115096896</v>
       </c>
       <c r="P20" s="7">
-        <v>630.15706173928584</v>
+        <v>630.15706173928947</v>
       </c>
       <c r="Q20" s="7">
-        <v>417.89810641941591</v>
+        <v>417.89810641946508</v>
       </c>
       <c r="R20" s="7">
         <v>340</v>
@@ -2187,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="7">
-        <v>-6.8212102632969618E-13</v>
+        <v>-1.7621459846850485E-12</v>
       </c>
       <c r="V20" s="7">
         <v>0</v>
@@ -2213,7 +2213,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>15.829644736905736</v>
+        <v>15.829644736900207</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2258,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="7">
-        <v>2.6275825063407099E-11</v>
+        <v>0</v>
       </c>
       <c r="R21" s="7">
         <v>0</v>
@@ -2362,13 +2362,13 @@
         <v>398.3</v>
       </c>
       <c r="X22" s="7">
-        <v>397.51828566309803</v>
+        <v>397.51828566309723</v>
       </c>
       <c r="Y22" s="7">
-        <v>355.79563343194741</v>
+        <v>355.79563343194718</v>
       </c>
       <c r="Z22" s="7">
-        <v>243.0939272020116</v>
+        <v>243.09392720201333</v>
       </c>
       <c r="AA22" s="8">
         <v>301.38810254334294</v>
@@ -2385,22 +2385,22 @@
         <v>0</v>
       </c>
       <c r="D23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="E23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="G23" s="7">
         <v>28.100000000000009</v>
       </c>
-      <c r="E23" s="7">
-        <v>28.099999999999994</v>
-      </c>
-      <c r="F23" s="7">
+      <c r="H23" s="7">
         <v>28.100000000000009</v>
       </c>
-      <c r="G23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="H23" s="7">
-        <v>28.099999999999994</v>
-      </c>
       <c r="I23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="J23" s="7">
         <v>28.099999999999994</v>
@@ -2412,7 +2412,7 @@
         <v>28.100000000000009</v>
       </c>
       <c r="M23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="N23" s="7">
         <v>28.100000000000009</v>
@@ -2430,13 +2430,13 @@
         <v>28.100000000000009</v>
       </c>
       <c r="S23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="T23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="U23" s="7">
-        <v>28.1</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="V23" s="7">
         <v>28.1</v>
@@ -2445,13 +2445,13 @@
         <v>28.1</v>
       </c>
       <c r="X23" s="7">
-        <v>28.1</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="Y23" s="7">
         <v>28.099999999999994</v>
       </c>
       <c r="Z23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="AA23" s="8">
         <v>28.1</v>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="7">
-        <v>0</v>
+        <v>5.9326476552607801</v>
       </c>
       <c r="D24" s="7">
         <v>25</v>
@@ -2548,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="7">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D25" s="7">
         <v>70</v>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="7">
-        <v>30.599999999999998</v>
+        <v>0</v>
       </c>
       <c r="D26" s="7">
         <v>30.6</v>
@@ -2643,10 +2643,10 @@
         <v>30.6</v>
       </c>
       <c r="G26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="H26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="I26" s="7">
         <v>30.6</v>
@@ -2655,7 +2655,7 @@
         <v>30.6</v>
       </c>
       <c r="K26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="L26" s="7">
         <v>30.6</v>
@@ -2697,13 +2697,13 @@
         <v>30.6</v>
       </c>
       <c r="Y26" s="7">
+        <v>30.599999999999998</v>
+      </c>
+      <c r="Z26" s="7">
         <v>30.6</v>
       </c>
-      <c r="Z26" s="7">
-        <v>30.599999999999998</v>
-      </c>
       <c r="AA26" s="8">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D27" s="7">
         <v>10</v>
@@ -2732,7 +2732,7 @@
         <v>10</v>
       </c>
       <c r="I27" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="J27" s="7">
         <v>10</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="W27" s="7">
-        <v>9.9999999999999929</v>
+        <v>10.000000000000014</v>
       </c>
       <c r="X27" s="7">
         <v>10</v>
@@ -2786,7 +2786,7 @@
         <v>10</v>
       </c>
       <c r="AA27" s="8">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.35">
@@ -2797,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D28" s="7">
         <v>10</v>
@@ -2880,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="7">
-        <v>0.83264765525105133</v>
+        <v>0</v>
       </c>
       <c r="D29" s="7">
         <v>10</v>
@@ -2889,7 +2889,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="G29" s="7">
         <v>10</v>
@@ -2916,10 +2916,10 @@
         <v>10</v>
       </c>
       <c r="O29" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="P29" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="Q29" s="7">
         <v>10</v>
@@ -2931,7 +2931,7 @@
         <v>10</v>
       </c>
       <c r="T29" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="U29" s="7">
         <v>10</v>
@@ -2963,22 +2963,22 @@
         <v>0</v>
       </c>
       <c r="C30" s="7">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="E30" s="7">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="F30" s="7">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="G30" s="7">
         <v>52.2</v>
       </c>
-      <c r="D30" s="7">
+      <c r="H30" s="7">
         <v>52.2</v>
-      </c>
-      <c r="E30" s="7">
-        <v>52.2</v>
-      </c>
-      <c r="F30" s="7">
-        <v>52.2</v>
-      </c>
-      <c r="G30" s="7">
-        <v>52.200000000000017</v>
-      </c>
-      <c r="H30" s="7">
-        <v>52.200000000000017</v>
       </c>
       <c r="I30" s="7">
         <v>52.2</v>
@@ -2987,13 +2987,13 @@
         <v>52.200000000000017</v>
       </c>
       <c r="K30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.20000000000001</v>
       </c>
       <c r="L30" s="7">
         <v>52.2</v>
       </c>
       <c r="M30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="N30" s="7">
         <v>52.2</v>
@@ -3017,19 +3017,19 @@
         <v>52.2</v>
       </c>
       <c r="U30" s="7">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="V30" s="7">
         <v>52.20000000000001</v>
       </c>
-      <c r="V30" s="7">
+      <c r="W30" s="7">
         <v>52.2</v>
-      </c>
-      <c r="W30" s="7">
-        <v>52.200000000000017</v>
       </c>
       <c r="X30" s="7">
         <v>52.200000000000017</v>
       </c>
       <c r="Y30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="Z30" s="7">
         <v>52.2</v>
@@ -3046,79 +3046,79 @@
         <v>0</v>
       </c>
       <c r="C31" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D31" s="7">
         <v>10</v>
       </c>
       <c r="E31" s="7">
-        <v>9.9999999999999858</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="F31" s="7">
         <v>10</v>
       </c>
       <c r="G31" s="7">
+        <v>10</v>
+      </c>
+      <c r="H31" s="7">
+        <v>10</v>
+      </c>
+      <c r="I31" s="7">
+        <v>10</v>
+      </c>
+      <c r="J31" s="7">
+        <v>10</v>
+      </c>
+      <c r="K31" s="7">
+        <v>10</v>
+      </c>
+      <c r="L31" s="7">
+        <v>10</v>
+      </c>
+      <c r="M31" s="7">
+        <v>10</v>
+      </c>
+      <c r="N31" s="7">
+        <v>10</v>
+      </c>
+      <c r="O31" s="7">
+        <v>10</v>
+      </c>
+      <c r="P31" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>10</v>
+      </c>
+      <c r="R31" s="7">
+        <v>10</v>
+      </c>
+      <c r="S31" s="7">
+        <v>10</v>
+      </c>
+      <c r="T31" s="7">
+        <v>10</v>
+      </c>
+      <c r="U31" s="7">
+        <v>10</v>
+      </c>
+      <c r="V31" s="7">
+        <v>10</v>
+      </c>
+      <c r="W31" s="7">
+        <v>10</v>
+      </c>
+      <c r="X31" s="7">
+        <v>10</v>
+      </c>
+      <c r="Y31" s="7">
+        <v>10</v>
+      </c>
+      <c r="Z31" s="7">
+        <v>10</v>
+      </c>
+      <c r="AA31" s="8">
         <v>9.9999999999999929</v>
-      </c>
-      <c r="H31" s="7">
-        <v>10</v>
-      </c>
-      <c r="I31" s="7">
-        <v>10</v>
-      </c>
-      <c r="J31" s="7">
-        <v>10</v>
-      </c>
-      <c r="K31" s="7">
-        <v>9.9999999999999929</v>
-      </c>
-      <c r="L31" s="7">
-        <v>10</v>
-      </c>
-      <c r="M31" s="7">
-        <v>10</v>
-      </c>
-      <c r="N31" s="7">
-        <v>10</v>
-      </c>
-      <c r="O31" s="7">
-        <v>10</v>
-      </c>
-      <c r="P31" s="7">
-        <v>10</v>
-      </c>
-      <c r="Q31" s="7">
-        <v>10</v>
-      </c>
-      <c r="R31" s="7">
-        <v>10</v>
-      </c>
-      <c r="S31" s="7">
-        <v>10</v>
-      </c>
-      <c r="T31" s="7">
-        <v>10</v>
-      </c>
-      <c r="U31" s="7">
-        <v>10</v>
-      </c>
-      <c r="V31" s="7">
-        <v>10.000000000000014</v>
-      </c>
-      <c r="W31" s="7">
-        <v>10</v>
-      </c>
-      <c r="X31" s="7">
-        <v>10</v>
-      </c>
-      <c r="Y31" s="7">
-        <v>9.9999999999999858</v>
-      </c>
-      <c r="Z31" s="7">
-        <v>10</v>
-      </c>
-      <c r="AA31" s="8">
-        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
@@ -3129,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="7">
-        <v>20.2</v>
+        <v>0</v>
       </c>
       <c r="D32" s="7">
         <v>20.199999999999996</v>
@@ -3138,31 +3138,31 @@
         <v>20.199999999999996</v>
       </c>
       <c r="F32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="G32" s="7">
         <v>20.200000000000003</v>
       </c>
-      <c r="G32" s="7">
+      <c r="H32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="I32" s="7">
         <v>20.2</v>
-      </c>
-      <c r="H32" s="7">
-        <v>20.2</v>
-      </c>
-      <c r="I32" s="7">
-        <v>20.199999999999996</v>
       </c>
       <c r="J32" s="7">
         <v>20.200000000000003</v>
       </c>
       <c r="K32" s="7">
-        <v>20.2</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="L32" s="7">
-        <v>20.2</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="M32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="N32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="O32" s="7">
         <v>20.2</v>
@@ -3180,28 +3180,28 @@
         <v>20.199999999999996</v>
       </c>
       <c r="T32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
       <c r="U32" s="7">
         <v>20.2</v>
       </c>
       <c r="V32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="W32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="X32" s="7">
         <v>20.199999999999996</v>
       </c>
-      <c r="W32" s="7">
+      <c r="Y32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="Z32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="AA32" s="8">
         <v>20.199999999999996</v>
-      </c>
-      <c r="X32" s="7">
-        <v>20.2</v>
-      </c>
-      <c r="Y32" s="7">
-        <v>20.199999999999996</v>
-      </c>
-      <c r="Z32" s="7">
-        <v>20.2</v>
-      </c>
-      <c r="AA32" s="8">
-        <v>20.2</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.35">
@@ -3212,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="7">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D33" s="7">
         <v>70</v>
@@ -3331,10 +3331,10 @@
         <v>10.5</v>
       </c>
       <c r="O34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="P34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="Q34" s="7">
         <v>10.5</v>
@@ -3343,7 +3343,7 @@
         <v>10.5</v>
       </c>
       <c r="S34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="T34" s="7">
         <v>10.5</v>
@@ -3358,7 +3358,7 @@
         <v>10.5</v>
       </c>
       <c r="X34" s="7">
-        <v>10.499999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="Y34" s="7">
         <v>10.5</v>
@@ -3435,7 +3435,7 @@
         <v>10</v>
       </c>
       <c r="V35" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="W35" s="7">
         <v>10</v>
@@ -3476,7 +3476,7 @@
         <v>10</v>
       </c>
       <c r="H36" s="7">
-        <v>10</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="I36" s="7">
         <v>10</v>
@@ -3515,7 +3515,7 @@
         <v>10</v>
       </c>
       <c r="U36" s="7">
-        <v>10</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="V36" s="7">
         <v>10</v>
@@ -3627,7 +3627,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D38" s="7">
         <v>10</v>
@@ -3713,22 +3713,22 @@
         <v>0</v>
       </c>
       <c r="D39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="E39" s="7">
         <v>10.1</v>
       </c>
-      <c r="E39" s="7">
+      <c r="F39" s="7">
         <v>10.099999999999994</v>
       </c>
-      <c r="F39" s="7">
+      <c r="G39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="H39" s="7">
         <v>10.1</v>
       </c>
-      <c r="G39" s="7">
+      <c r="I39" s="7">
         <v>10.100000000000001</v>
-      </c>
-      <c r="H39" s="7">
-        <v>10.099999999999994</v>
-      </c>
-      <c r="I39" s="7">
-        <v>10.1</v>
       </c>
       <c r="J39" s="7">
         <v>10.099999999999994</v>
@@ -3743,10 +3743,10 @@
         <v>10.099999999999994</v>
       </c>
       <c r="N39" s="7">
-        <v>10.1</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="O39" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="P39" s="7">
         <v>10.099999999999994</v>
@@ -3761,13 +3761,13 @@
         <v>10.1</v>
       </c>
       <c r="T39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="U39" s="7">
         <v>10.1</v>
       </c>
-      <c r="U39" s="7">
-        <v>10.100000000000001</v>
-      </c>
       <c r="V39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="W39" s="7">
         <v>10.099999999999994</v>
@@ -3793,13 +3793,13 @@
         <v>0</v>
       </c>
       <c r="C40" s="7">
-        <v>10.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="D40" s="7">
         <v>10.1</v>
       </c>
       <c r="E40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="F40" s="7">
         <v>10.100000000000001</v>
@@ -3811,16 +3811,16 @@
         <v>10.100000000000001</v>
       </c>
       <c r="I40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="J40" s="7">
         <v>10.1</v>
       </c>
-      <c r="J40" s="7">
-        <v>10.100000000000001</v>
-      </c>
       <c r="K40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="L40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.1</v>
       </c>
       <c r="M40" s="7">
         <v>10.100000000000001</v>
@@ -3844,25 +3844,25 @@
         <v>10.1</v>
       </c>
       <c r="T40" s="7">
-        <v>10.1</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="U40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="V40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="W40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="X40" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="W40" s="7">
+      <c r="Y40" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="X40" s="7">
-        <v>10.099999999999998</v>
-      </c>
-      <c r="Y40" s="7">
+      <c r="Z40" s="7">
         <v>10.1</v>
-      </c>
-      <c r="Z40" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="AA40" s="8">
         <v>10.100000000000001</v>
@@ -3936,7 +3936,7 @@
         <v>10</v>
       </c>
       <c r="W41" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="X41" s="7">
         <v>10</v>
@@ -3945,7 +3945,7 @@
         <v>10</v>
       </c>
       <c r="Z41" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="AA41" s="8">
         <v>10</v>
@@ -3959,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="7">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D42" s="7">
         <v>12</v>
@@ -4066,55 +4066,55 @@
         <v>950</v>
       </c>
       <c r="K43" s="7">
-        <v>1200</v>
+        <v>1200.0000000000007</v>
       </c>
       <c r="L43" s="7">
-        <v>1500</v>
+        <v>1500.0000000000007</v>
       </c>
       <c r="M43" s="7">
-        <v>1750</v>
+        <v>1749.9999999999998</v>
       </c>
       <c r="N43" s="7">
-        <v>2000</v>
+        <v>2000.0000000000005</v>
       </c>
       <c r="O43" s="7">
-        <v>2250</v>
+        <v>2249.9999999999995</v>
       </c>
       <c r="P43" s="7">
-        <v>2500</v>
+        <v>2500.0000000000005</v>
       </c>
       <c r="Q43" s="7">
-        <v>2700</v>
+        <v>2700.0000000000009</v>
       </c>
       <c r="R43" s="7">
-        <v>2950</v>
+        <v>2950.0000000000005</v>
       </c>
       <c r="S43" s="7">
-        <v>3200</v>
+        <v>3200.0000000000005</v>
       </c>
       <c r="T43" s="7">
-        <v>3450</v>
+        <v>3450.0000000000005</v>
       </c>
       <c r="U43" s="7">
-        <v>3650</v>
+        <v>3650.0000000000005</v>
       </c>
       <c r="V43" s="7">
-        <v>3900</v>
+        <v>3900.0000000000009</v>
       </c>
       <c r="W43" s="7">
-        <v>4100</v>
+        <v>4100.0000000000009</v>
       </c>
       <c r="X43" s="7">
-        <v>4350</v>
+        <v>4350.0000000000009</v>
       </c>
       <c r="Y43" s="7">
         <v>4550</v>
       </c>
       <c r="Z43" s="7">
-        <v>4800</v>
+        <v>4800.0000000000009</v>
       </c>
       <c r="AA43" s="8">
-        <v>5000</v>
+        <v>5000.0000000000009</v>
       </c>
       <c r="AB43" t="s">
         <v>17</v>
@@ -4307,79 +4307,79 @@
         <v>1</v>
       </c>
       <c r="B49" s="3">
-        <v>134.59011842103158</v>
+        <v>134.59011842103328</v>
       </c>
       <c r="C49" s="4">
-        <v>238.16156822983203</v>
+        <v>321.81666666666598</v>
       </c>
       <c r="D49" s="4">
-        <v>389.57841108033307</v>
+        <v>389.57841108034597</v>
       </c>
       <c r="E49" s="4">
-        <v>445.38034435000094</v>
+        <v>445.38034435000066</v>
       </c>
       <c r="F49" s="4">
-        <v>630.82005026299339</v>
+        <v>630.82005026299657</v>
       </c>
       <c r="G49" s="4">
-        <v>988.85720646479319</v>
+        <v>988.85720646479751</v>
       </c>
       <c r="H49" s="4">
-        <v>846.83951964716664</v>
+        <v>846.83951964717062</v>
       </c>
       <c r="I49" s="4">
-        <v>762.88527618929629</v>
+        <v>762.88527618929811</v>
       </c>
       <c r="J49" s="4">
-        <v>665.82177982875533</v>
+        <v>665.82177982875953</v>
       </c>
       <c r="K49" s="4">
-        <v>626.12404029153095</v>
+        <v>626.12404029153163</v>
       </c>
       <c r="L49" s="4">
-        <v>505.05639941523725</v>
+        <v>505.05639941523896</v>
       </c>
       <c r="M49" s="4">
-        <v>442.73926845512926</v>
+        <v>442.73926845513068</v>
       </c>
       <c r="N49" s="4">
-        <v>370.0866113431598</v>
+        <v>370.08661134315912</v>
       </c>
       <c r="O49" s="4">
-        <v>287.7019250148694</v>
+        <v>287.70192501487213</v>
       </c>
       <c r="P49" s="4">
-        <v>196.1565660973481</v>
+        <v>196.15656609734944</v>
       </c>
       <c r="Q49" s="4">
-        <v>165.71499815072264</v>
+        <v>165.71499815071456</v>
       </c>
       <c r="R49" s="4">
-        <v>57.442396259817713</v>
+        <v>57.44239625981777</v>
       </c>
       <c r="S49" s="4">
-        <v>-41.526512318802133</v>
+        <v>-41.526512318802361</v>
       </c>
       <c r="T49" s="4">
-        <v>-177.93212082638382</v>
+        <v>-177.9321208263826</v>
       </c>
       <c r="U49" s="4">
-        <v>-239.68408793039487</v>
+        <v>-239.68408793039612</v>
       </c>
       <c r="V49" s="4">
-        <v>-332.28171754239202</v>
+        <v>-332.28171754239207</v>
       </c>
       <c r="W49" s="4">
-        <v>-375.11101945637904</v>
+        <v>-375.11101945637893</v>
       </c>
       <c r="X49" s="4">
-        <v>-468.42867982535927</v>
+        <v>-468.42867982536023</v>
       </c>
       <c r="Y49" s="4">
-        <v>-526.97265273668881</v>
+        <v>-526.97265273668859</v>
       </c>
       <c r="Z49" s="4">
-        <v>-624.09898603320789</v>
+        <v>-624.09898603320767</v>
       </c>
       <c r="AA49" s="5">
         <v>-635.81607690750707</v>
@@ -4390,79 +4390,79 @@
         <v>2</v>
       </c>
       <c r="B50" s="6">
-        <v>-371.30988157896866</v>
+        <v>-371.30988157896684</v>
       </c>
       <c r="C50" s="7">
-        <v>-210.30578411491643</v>
+        <v>-221.68333333333354</v>
       </c>
       <c r="D50" s="7">
-        <v>-241.38998054016702</v>
+        <v>-241.38998054017327</v>
       </c>
       <c r="E50" s="7">
-        <v>-291.56660415000147</v>
+        <v>-291.5666041500009</v>
       </c>
       <c r="F50" s="7">
-        <v>-584.15346921503601</v>
+        <v>-584.15346921504249</v>
       </c>
       <c r="G50" s="7">
-        <v>-712.60342355937644</v>
+        <v>-712.60342355937212</v>
       </c>
       <c r="H50" s="7">
-        <v>-537.56435604721923</v>
+        <v>-537.56435604721537</v>
       </c>
       <c r="I50" s="7">
-        <v>-354.75833438633958</v>
+        <v>-354.7583343863364</v>
       </c>
       <c r="J50" s="7">
-        <v>-185.36072324205941</v>
+        <v>-185.36072324205668</v>
       </c>
       <c r="K50" s="7">
-        <v>-8.8992053069221129</v>
+        <v>-8.8992053069208055</v>
       </c>
       <c r="L50" s="7">
-        <v>135.88784460639855</v>
+        <v>135.88784460640204</v>
       </c>
       <c r="M50" s="7">
-        <v>289.11809665301132</v>
+        <v>289.1180966530145</v>
       </c>
       <c r="N50" s="7">
-        <v>431.70274899482342</v>
+        <v>431.70274899482547</v>
       </c>
       <c r="O50" s="7">
-        <v>564.24250790539827</v>
+        <v>564.24250790540077</v>
       </c>
       <c r="P50" s="7">
-        <v>687.30591423389239</v>
+        <v>687.30591423389342</v>
       </c>
       <c r="Q50" s="7">
-        <v>821.15459042049599</v>
+        <v>821.1545904204886</v>
       </c>
       <c r="R50" s="7">
-        <v>926.85084486001972</v>
+        <v>926.85084486002029</v>
       </c>
       <c r="S50" s="7">
-        <v>1041.5265123188021</v>
+        <v>1041.5265123188024</v>
       </c>
       <c r="T50" s="7">
-        <v>1118.4382810329591</v>
+        <v>1118.4382810329603</v>
       </c>
       <c r="U50" s="7">
         <v>1219.6735475456819</v>
       </c>
       <c r="V50" s="7">
-        <v>1275.7969613433938</v>
+        <v>1275.7969613433931</v>
       </c>
       <c r="W50" s="7">
-        <v>1350.1509669076947</v>
+        <v>1350.1509669076945</v>
       </c>
       <c r="X50" s="7">
-        <v>1423.8799479976105</v>
+        <v>1423.8799479976115</v>
       </c>
       <c r="Y50" s="7">
-        <v>1526.9726527366884</v>
+        <v>1526.9726527366886</v>
       </c>
       <c r="Z50" s="7">
-        <v>1624.0989860332079</v>
+        <v>1624.0989860332077</v>
       </c>
       <c r="AA50" s="8">
         <v>1635.8160769075071</v>
@@ -4473,73 +4473,73 @@
         <v>3</v>
       </c>
       <c r="B51" s="9">
-        <v>236.71976315793711</v>
+        <v>236.71976315793358</v>
       </c>
       <c r="C51" s="10">
-        <v>-27.855784114915593</v>
+        <v>-100.13333333333244</v>
       </c>
       <c r="D51" s="10">
-        <v>-148.18843054016605</v>
+        <v>-148.1884305401727</v>
       </c>
       <c r="E51" s="10">
-        <v>-153.81374019999947</v>
+        <v>-153.81374019999976</v>
       </c>
       <c r="F51" s="10">
-        <v>-46.666581047957266</v>
+        <v>-46.666581047954082</v>
       </c>
       <c r="G51" s="10">
-        <v>-276.25378290541647</v>
+        <v>-276.2537829054254</v>
       </c>
       <c r="H51" s="10">
-        <v>-309.27516359994735</v>
+        <v>-309.27516359995525</v>
       </c>
       <c r="I51" s="10">
-        <v>-408.12694180295694</v>
+        <v>-408.12694180296171</v>
       </c>
       <c r="J51" s="10">
-        <v>-480.46105658669592</v>
+        <v>-480.46105658670285</v>
       </c>
       <c r="K51" s="10">
-        <v>-617.22483498460883</v>
+        <v>-617.22483498461077</v>
       </c>
       <c r="L51" s="10">
-        <v>-640.94424402163565</v>
+        <v>-640.944244021641</v>
       </c>
       <c r="M51" s="10">
-        <v>-731.85736510814058</v>
+        <v>-731.85736510814525</v>
       </c>
       <c r="N51" s="10">
-        <v>-801.78936033798323</v>
+        <v>-801.78936033798459</v>
       </c>
       <c r="O51" s="10">
-        <v>-851.94443292026767</v>
+        <v>-851.9444329202729</v>
       </c>
       <c r="P51" s="10">
-        <v>-883.4624803312405</v>
+        <v>-883.46248033124289</v>
       </c>
       <c r="Q51" s="10">
-        <v>-986.86958857121863</v>
+        <v>-986.86958857120317</v>
       </c>
       <c r="R51" s="10">
-        <v>-984.29324111983738</v>
+        <v>-984.29324111983783</v>
       </c>
       <c r="S51" s="10">
         <v>-1000</v>
       </c>
       <c r="T51" s="10">
-        <v>-940.50616020657537</v>
+        <v>-940.50616020657753</v>
       </c>
       <c r="U51" s="10">
-        <v>-979.98945961528705</v>
+        <v>-979.9894596152858</v>
       </c>
       <c r="V51" s="10">
-        <v>-943.51524380100182</v>
+        <v>-943.51524380100113</v>
       </c>
       <c r="W51" s="10">
-        <v>-975.03994745131558</v>
+        <v>-975.03994745131547</v>
       </c>
       <c r="X51" s="10">
-        <v>-955.45126817225139</v>
+        <v>-955.45126817225128</v>
       </c>
       <c r="Y51" s="10">
         <v>-1000</v>
@@ -4639,22 +4639,22 @@
         <v>8</v>
       </c>
       <c r="B54" s="15">
-        <v>185343.2957730355</v>
+        <v>185343.29577303451</v>
       </c>
       <c r="C54" s="16">
-        <v>150354.42590554882</v>
+        <v>150354.42590554862</v>
       </c>
       <c r="D54" s="16">
-        <v>122850.98857876594</v>
+        <v>122850.98857876577</v>
       </c>
       <c r="E54" s="16">
-        <v>115767.04458876402</v>
+        <v>115767.04458876408</v>
       </c>
       <c r="F54" s="16">
-        <v>110839.76863109929</v>
+        <v>110839.76863109937</v>
       </c>
       <c r="G54" s="16">
-        <v>107601.0888445215</v>
+        <v>107601.08884452166</v>
       </c>
       <c r="H54" s="16">
         <v>11641550.231811121</v>
@@ -4666,34 +4666,34 @@
         <v>13729770.539331574</v>
       </c>
       <c r="K54" s="16">
-        <v>13539056.792083366</v>
+        <v>13539056.792083383</v>
       </c>
       <c r="L54" s="16">
-        <v>15173431.935465464</v>
+        <v>15173431.935465468</v>
       </c>
       <c r="M54" s="16">
-        <v>14667613.021367956</v>
+        <v>14667613.021367941</v>
       </c>
       <c r="N54" s="16">
-        <v>14771698.232724916</v>
+        <v>14771698.232724929</v>
       </c>
       <c r="O54" s="16">
-        <v>14735518.731834156</v>
+        <v>14735518.731834147</v>
       </c>
       <c r="P54" s="16">
-        <v>14583734.508809622</v>
+        <v>14583734.508809632</v>
       </c>
       <c r="Q54" s="16">
         <v>13638852.260879792</v>
       </c>
       <c r="R54" s="16">
-        <v>13819966.051143175</v>
+        <v>13819966.051143177</v>
       </c>
       <c r="S54" s="16">
-        <v>13455936.071670964</v>
+        <v>13455936.071670968</v>
       </c>
       <c r="T54" s="16">
-        <v>13043632.510209475</v>
+        <v>13043632.510209477</v>
       </c>
       <c r="U54" s="16">
         <v>12117802.26314237</v>
@@ -4812,86 +4812,86 @@
         <v>10</v>
       </c>
       <c r="B57" s="3">
-        <v>13395.809006237852</v>
+        <v>13395.809006237763</v>
       </c>
       <c r="C57" s="4">
         <v>10788.134900264893</v>
       </c>
       <c r="D57" s="4">
-        <v>9558.804967341759</v>
+        <v>9558.8049673417518</v>
       </c>
       <c r="E57" s="4">
-        <v>9312.0249598840437</v>
+        <v>9312.0249598840237</v>
       </c>
       <c r="F57" s="4">
-        <v>8666.7645106792806</v>
+        <v>8666.764510679297</v>
       </c>
       <c r="G57" s="4">
-        <v>7992.7910405343537</v>
+        <v>7992.7910405343282</v>
       </c>
       <c r="H57" s="4">
-        <v>7231.7522186328642</v>
+        <v>7231.7522186328661</v>
       </c>
       <c r="I57" s="4">
-        <v>6939.5927342366704</v>
+        <v>6939.5927342366722</v>
       </c>
       <c r="J57" s="4">
-        <v>6641.5502674662939</v>
+        <v>6641.5502674662948</v>
       </c>
       <c r="K57" s="4">
-        <v>6428.200739953425</v>
+        <v>6428.2007399534241</v>
       </c>
       <c r="L57" s="4">
         <v>6119.5279553645905</v>
       </c>
       <c r="M57" s="4">
-        <v>5896.2592355312281</v>
+        <v>5896.259235531229</v>
       </c>
       <c r="N57" s="4">
-        <v>5668.5319125448623</v>
+        <v>5668.5319125448477</v>
       </c>
       <c r="O57" s="4">
-        <v>5436.6569033792557</v>
+        <v>5436.6569033792239</v>
       </c>
       <c r="P57" s="4">
-        <v>5200.9289870833718</v>
+        <v>5200.9289870833545</v>
       </c>
       <c r="Q57" s="4">
-        <v>5051.8183299385892</v>
+        <v>5051.8183299381972</v>
       </c>
       <c r="R57" s="4">
-        <v>4809.2087187230172</v>
+        <v>4809.2087187230163</v>
       </c>
       <c r="S57" s="4">
-        <v>5099.2167571217269</v>
+        <v>5099.2167571217396</v>
       </c>
       <c r="T57" s="4">
-        <v>4929.3134908072589</v>
+        <v>4929.3134908072534</v>
       </c>
       <c r="U57" s="4">
-        <v>4478.6003618073182</v>
+        <v>4478.6003618073246</v>
       </c>
       <c r="V57" s="4">
-        <v>4143.4773551581557</v>
+        <v>4143.4773551581529</v>
       </c>
       <c r="W57" s="4">
-        <v>3708.1193862656064</v>
+        <v>3708.1193862656041</v>
       </c>
       <c r="X57" s="4">
-        <v>3352.1940770678111</v>
+        <v>3352.1940770678093</v>
       </c>
       <c r="Y57" s="4">
-        <v>2961.9204175372606</v>
+        <v>2961.9204175372579</v>
       </c>
       <c r="Z57" s="4">
-        <v>2768.3019467310883</v>
+        <v>2768.3019467310864</v>
       </c>
       <c r="AA57" s="5">
         <v>2672.733379103548</v>
       </c>
       <c r="AB57" s="12">
         <f>SUM(B57:AA57)</f>
-        <v>159252.23455939617</v>
+        <v>159252.23455939555</v>
       </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.35">
@@ -4899,7 +4899,7 @@
         <v>11</v>
       </c>
       <c r="B58" s="6">
-        <v>2413.9885322768887</v>
+        <v>2413.9885322768387</v>
       </c>
       <c r="C58" s="7">
         <v>2265.7469347046895</v>
@@ -4908,43 +4908,43 @@
         <v>2260.5965095418974</v>
       </c>
       <c r="E58" s="7">
-        <v>1949.7252897817255</v>
+        <v>1949.7252897817209</v>
       </c>
       <c r="F58" s="7">
-        <v>1610.7981043449747</v>
+        <v>1610.7981043449699</v>
       </c>
       <c r="G58" s="7">
-        <v>1150.4026949077688</v>
+        <v>1150.4026949077515</v>
       </c>
       <c r="H58" s="7">
-        <v>928.34771465728033</v>
+        <v>928.34771465727567</v>
       </c>
       <c r="I58" s="7">
-        <v>824.41550616380891</v>
+        <v>824.4155061638063</v>
       </c>
       <c r="J58" s="7">
-        <v>736.34160047708212</v>
+        <v>736.34160047707815</v>
       </c>
       <c r="K58" s="7">
-        <v>620.51602561486106</v>
+        <v>620.5160256148597</v>
       </c>
       <c r="L58" s="7">
-        <v>561.54347727351114</v>
+        <v>561.54347727350807</v>
       </c>
       <c r="M58" s="7">
-        <v>473.18423535646423</v>
+        <v>473.18423535646116</v>
       </c>
       <c r="N58" s="7">
-        <v>397.40824655042934</v>
+        <v>397.40824655042297</v>
       </c>
       <c r="O58" s="7">
-        <v>333.50338787838155</v>
+        <v>333.5033878783658</v>
       </c>
       <c r="P58" s="7">
-        <v>280.79564981683325</v>
+        <v>280.79564981682495</v>
       </c>
       <c r="Q58" s="7">
-        <v>195.92471855958934</v>
+        <v>195.92471855937231</v>
       </c>
       <c r="R58" s="7">
         <v>163.73146482239679</v>
@@ -4953,32 +4953,32 @@
         <v>376.80973050205012</v>
       </c>
       <c r="T58" s="7">
-        <v>356.79383208201045</v>
+        <v>356.79383208200716</v>
       </c>
       <c r="U58" s="7">
-        <v>199.98936917622052</v>
+        <v>199.98936917622359</v>
       </c>
       <c r="V58" s="7">
-        <v>207.39779424175362</v>
+        <v>207.3977942417543</v>
       </c>
       <c r="W58" s="7">
-        <v>98.517424047123882</v>
+        <v>98.517424047124294</v>
       </c>
       <c r="X58" s="7">
         <v>128.3450141128038</v>
       </c>
       <c r="Y58" s="7">
-        <v>20.11007947899401</v>
+        <v>20.110079478993992</v>
       </c>
       <c r="Z58" s="7">
-        <v>76.764230252015167</v>
+        <v>76.764230252013448</v>
       </c>
       <c r="AA58" s="8">
-        <v>17.963283589017003</v>
+        <v>17.963283589016996</v>
       </c>
       <c r="AB58" s="13">
         <f t="shared" ref="AB58:AB61" si="0">SUM(B58:AA58)</f>
-        <v>18649.660850210566</v>
+        <v>18649.660850210232</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.35">
@@ -4986,86 +4986,86 @@
         <v>12</v>
       </c>
       <c r="B59" s="6">
-        <v>14017815.71121002</v>
+        <v>14017815.711210009</v>
       </c>
       <c r="C59" s="7">
-        <v>13261661.088989645</v>
+        <v>13261661.088989636</v>
       </c>
       <c r="D59" s="7">
-        <v>12546295.26186293</v>
+        <v>12546295.261862921</v>
       </c>
       <c r="E59" s="7">
-        <v>11869517.984329415</v>
+        <v>11869517.984329406</v>
       </c>
       <c r="F59" s="7">
-        <v>11229247.697411524</v>
+        <v>11229247.697411515</v>
       </c>
       <c r="G59" s="7">
-        <v>10623515.126418673</v>
+        <v>10623515.126418665</v>
       </c>
       <c r="H59" s="7">
-        <v>10050457.224063346</v>
+        <v>10050457.224063339</v>
       </c>
       <c r="I59" s="7">
-        <v>9508311.4403000306</v>
+        <v>9508311.440300025</v>
       </c>
       <c r="J59" s="7">
-        <v>8995410.3012627903</v>
+        <v>8995410.3012627847</v>
       </c>
       <c r="K59" s="7">
-        <v>8510176.2806279529</v>
+        <v>8510176.2806279473</v>
       </c>
       <c r="L59" s="7">
-        <v>8051116.947627808</v>
+        <v>8051116.9476278024</v>
       </c>
       <c r="M59" s="7">
-        <v>7616820.3767920891</v>
+        <v>7616820.3767920844</v>
       </c>
       <c r="N59" s="7">
-        <v>7205950.8052990194</v>
+        <v>7205950.8052990157</v>
       </c>
       <c r="O59" s="7">
-        <v>6817244.5245792577</v>
+        <v>6817244.524579254</v>
       </c>
       <c r="P59" s="7">
-        <v>6449505.9935365934</v>
+        <v>6449505.9935365906</v>
       </c>
       <c r="Q59" s="7">
-        <v>6101604.161430845</v>
+        <v>6101604.1614308432</v>
       </c>
       <c r="R59" s="7">
-        <v>5772468.9891132778</v>
+        <v>5772468.9891132768</v>
       </c>
       <c r="S59" s="7">
-        <v>5461088.1579149337</v>
+        <v>5461088.1579149328</v>
       </c>
       <c r="T59" s="7">
-        <v>5166503.9560654238</v>
+        <v>5166503.9560654229</v>
       </c>
       <c r="U59" s="7">
-        <v>4887810.3330657603</v>
+        <v>4887810.3330657594</v>
       </c>
       <c r="V59" s="7">
-        <v>4624150.1129553942</v>
+        <v>4624150.1129553933</v>
       </c>
       <c r="W59" s="7">
-        <v>4374712.3579023099</v>
+        <v>4374712.3579023089</v>
       </c>
       <c r="X59" s="7">
-        <v>4138729.8740074006</v>
+        <v>4138729.8740073997</v>
       </c>
       <c r="Y59" s="7">
-        <v>3895260.8637902355</v>
+        <v>3895260.8637902332</v>
       </c>
       <c r="Z59" s="7">
-        <v>3685141.1441713171</v>
+        <v>3685141.1441713148</v>
       </c>
       <c r="AA59" s="8">
-        <v>3479546.1153387381</v>
+        <v>3479546.1153387371</v>
       </c>
       <c r="AB59" s="13">
         <f t="shared" si="0"/>
-        <v>198340062.83006674</v>
+        <v>198340062.83006662</v>
       </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.35">
@@ -5073,86 +5073,86 @@
         <v>13</v>
       </c>
       <c r="B60" s="6">
-        <v>1143.0110237631643</v>
+        <v>1143.0110237631638</v>
       </c>
       <c r="C60" s="7">
         <v>1129.461877637516</v>
       </c>
       <c r="D60" s="7">
-        <v>1120.2456230837952</v>
+        <v>1120.245623083795</v>
       </c>
       <c r="E60" s="7">
-        <v>973.64233599940644</v>
+        <v>973.64233599940439</v>
       </c>
       <c r="F60" s="7">
-        <v>815.41852060693975</v>
+        <v>815.41852060693736</v>
       </c>
       <c r="G60" s="7">
-        <v>642.61487861710771</v>
+        <v>642.61487861710486</v>
       </c>
       <c r="H60" s="7">
-        <v>595.01606521456551</v>
+        <v>595.01606521456324</v>
       </c>
       <c r="I60" s="7">
-        <v>537.99196538490924</v>
+        <v>537.99196538490799</v>
       </c>
       <c r="J60" s="7">
-        <v>488.96918648958103</v>
+        <v>488.96918648957904</v>
       </c>
       <c r="K60" s="7">
-        <v>426.97572359473043</v>
+        <v>426.97572359472974</v>
       </c>
       <c r="L60" s="7">
-        <v>392.63835467871627</v>
+        <v>392.63835467871473</v>
       </c>
       <c r="M60" s="7">
-        <v>344.50679858806723</v>
+        <v>344.50679858806569</v>
       </c>
       <c r="N60" s="7">
-        <v>302.7270376606146</v>
+        <v>302.72703766061375</v>
       </c>
       <c r="O60" s="7">
-        <v>266.94041760029597</v>
+        <v>266.94041760029432</v>
       </c>
       <c r="P60" s="7">
-        <v>236.80748657556373</v>
+        <v>236.80748657556288</v>
       </c>
       <c r="Q60" s="7">
-        <v>191.48202274851704</v>
+        <v>191.48202274852434</v>
       </c>
       <c r="R60" s="7">
         <v>171.70979446719025</v>
       </c>
       <c r="S60" s="7">
-        <v>157.16414508817184</v>
+        <v>157.16414508817181</v>
       </c>
       <c r="T60" s="7">
-        <v>150.30403313900942</v>
+        <v>150.30403313900888</v>
       </c>
       <c r="U60" s="7">
-        <v>121.44847929844768</v>
+        <v>121.44847929844805</v>
       </c>
       <c r="V60" s="7">
-        <v>118.44625605412547</v>
+        <v>118.44625605412557</v>
       </c>
       <c r="W60" s="7">
-        <v>97.386657498214618</v>
+        <v>97.38665749821466</v>
       </c>
       <c r="X60" s="7">
-        <v>97.772843926953001</v>
+        <v>97.772843926952973</v>
       </c>
       <c r="Y60" s="7">
-        <v>76.892153504437616</v>
+        <v>76.892153504437545</v>
       </c>
       <c r="Z60" s="7">
-        <v>81.722504254117055</v>
+        <v>81.722504254116757</v>
       </c>
       <c r="AA60" s="8">
-        <v>69.096041433177916</v>
+        <v>69.096041433177902</v>
       </c>
       <c r="AB60" s="13">
         <f t="shared" si="0"/>
-        <v>10750.392226907335</v>
+        <v>10750.392226907323</v>
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.35">
@@ -5160,86 +5160,86 @@
         <v>14</v>
       </c>
       <c r="B61" s="9">
-        <v>163.18245218421194</v>
+        <v>163.1824521842118</v>
       </c>
       <c r="C61" s="10">
-        <v>161.56613470468949</v>
+        <v>161.56613470468946</v>
       </c>
       <c r="D61" s="10">
         <v>161.01364910837947</v>
       </c>
       <c r="E61" s="10">
-        <v>139.11516895775821</v>
+        <v>139.11516895775793</v>
       </c>
       <c r="F61" s="10">
-        <v>115.37616262474334</v>
+        <v>115.37616262474299</v>
       </c>
       <c r="G61" s="10">
-        <v>89.13771329690654</v>
+        <v>89.137713296906114</v>
       </c>
       <c r="H61" s="10">
-        <v>82.409472665777812</v>
+        <v>82.409472665777457</v>
       </c>
       <c r="I61" s="10">
-        <v>74.190732041892318</v>
+        <v>74.190732041892119</v>
       </c>
       <c r="J61" s="10">
-        <v>67.177252576431286</v>
+        <v>67.177252576430988</v>
       </c>
       <c r="K61" s="10">
-        <v>58.126512249630707</v>
+        <v>58.126512249630601</v>
       </c>
       <c r="L61" s="10">
-        <v>53.324951211379876</v>
+        <v>53.324951211379648</v>
       </c>
       <c r="M61" s="10">
-        <v>46.361965442218363</v>
+        <v>46.361965442218128</v>
       </c>
       <c r="N61" s="10">
-        <v>40.355533278724167</v>
+        <v>40.355533278724046</v>
       </c>
       <c r="O61" s="10">
-        <v>35.251577202966736</v>
+        <v>35.251577202966487</v>
       </c>
       <c r="P61" s="10">
-        <v>30.998914459632399</v>
+        <v>30.998914459632267</v>
       </c>
       <c r="Q61" s="10">
-        <v>24.373984823503964</v>
+        <v>24.373984823504852</v>
       </c>
       <c r="R61" s="10">
-        <v>21.681166205599194</v>
+        <v>21.68116620559919</v>
       </c>
       <c r="S61" s="10">
-        <v>19.741154271884454</v>
+        <v>19.741154271884451</v>
       </c>
       <c r="T61" s="10">
-        <v>19.046411826166047</v>
+        <v>19.046411826165961</v>
       </c>
       <c r="U61" s="10">
-        <v>14.890935490292053</v>
+        <v>14.890935490292108</v>
       </c>
       <c r="V61" s="10">
-        <v>14.697145183149871</v>
+        <v>14.697145183149884</v>
       </c>
       <c r="W61" s="10">
-        <v>11.699693810643769</v>
+        <v>11.699693810643776</v>
       </c>
       <c r="X61" s="10">
-        <v>11.955175369863898</v>
+        <v>11.955175369863897</v>
       </c>
       <c r="Y61" s="10">
-        <v>8.9762281671597339</v>
+        <v>8.9762281671597286</v>
       </c>
       <c r="Z61" s="10">
-        <v>9.8666355084589856</v>
+        <v>9.866635508458943</v>
       </c>
       <c r="AA61" s="11">
-        <v>8.0928215381501456</v>
+        <v>8.092821538150142</v>
       </c>
       <c r="AB61" s="14">
         <f t="shared" si="0"/>
-        <v>1482.6095442002145</v>
+        <v>1482.6095442002122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds 600lbs/MW limit to emissions constraints
Leads the model to develop more solar including a massive amount of solar in the first year.  600lb/MW GHG average over 25 years was mentioned in the  A10 prompt.
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jawessel\opl\ENV717A11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfi\Google Drive\School\College\Semester 6 (Spring 2020)\ENV 717\Assignments\Assignment 11 (group project)\ENV717A11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:AA44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -719,10 +719,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>519.20000000000005</v>
+        <v>0</v>
       </c>
       <c r="C3" s="4">
-        <v>519.20000000000005</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -734,49 +734,49 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>495.91917837745905</v>
+        <v>0</v>
       </c>
       <c r="H3" s="4">
-        <v>396.80584595542996</v>
+        <v>0</v>
       </c>
       <c r="I3" s="4">
-        <v>421.67530116494368</v>
+        <v>0</v>
       </c>
       <c r="J3" s="4">
-        <v>407.00758733669591</v>
+        <v>0</v>
       </c>
       <c r="K3" s="4">
-        <v>514.22584895567445</v>
+        <v>0</v>
       </c>
       <c r="L3" s="4">
-        <v>427.12120987952449</v>
+        <v>0</v>
       </c>
       <c r="M3" s="4">
-        <v>466.05298510390321</v>
+        <v>0</v>
       </c>
       <c r="N3" s="4">
-        <v>473.76113038564222</v>
+        <v>0</v>
       </c>
       <c r="O3" s="4">
-        <v>452.05418306797833</v>
+        <v>0</v>
       </c>
       <c r="P3" s="4">
-        <v>402.64424198762526</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="4">
-        <v>486.32270904100915</v>
+        <v>0</v>
       </c>
       <c r="R3" s="4">
-        <v>386.28310279959442</v>
+        <v>0</v>
       </c>
       <c r="S3" s="4">
-        <v>419.45037015797897</v>
+        <v>0</v>
       </c>
       <c r="T3" s="4">
-        <v>129.03291882238841</v>
+        <v>0</v>
       </c>
       <c r="U3" s="4">
-        <v>117.86808104206888</v>
+        <v>0</v>
       </c>
       <c r="V3" s="4">
         <v>0</v>
@@ -805,79 +805,79 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>130.26735234474739</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7">
-        <v>641.05189162049885</v>
+        <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="F4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="G4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="H4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="I4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="J4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="K4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="L4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="M4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="N4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="O4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="P4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="R4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="S4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="T4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="U4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="V4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="W4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="X4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="8">
-        <v>665.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
@@ -885,7 +885,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
@@ -894,73 +894,73 @@
         <v>0</v>
       </c>
       <c r="E5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="F5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="G5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="H5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="I5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="J5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="K5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="L5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="M5" s="7">
-        <v>46.5</v>
+        <v>1.3145040611561853E-13</v>
       </c>
       <c r="N5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="O5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="P5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="R5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="S5" s="7">
-        <v>42.477210131936829</v>
+        <v>0</v>
       </c>
       <c r="T5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="U5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="V5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="W5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="X5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="8">
-        <v>46.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
@@ -968,82 +968,82 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0</v>
+        <v>119.84999999999815</v>
       </c>
       <c r="C6" s="7">
-        <v>212</v>
+        <v>100.32499999999959</v>
       </c>
       <c r="D6" s="7">
-        <v>212</v>
+        <v>65.984274999999343</v>
       </c>
       <c r="E6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="F6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="G6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="H6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="I6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="J6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="K6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="L6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="M6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="N6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="O6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="P6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="R6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="S6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="T6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="U6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="V6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="W6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="X6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="8">
-        <v>212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
@@ -1051,82 +1051,82 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>192.67035526309442</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="D7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="E7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="F7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="G7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="H7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="I7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="J7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="K7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="L7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="M7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="N7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="O7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="P7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="R7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="S7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="T7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="U7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="V7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="W7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="X7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="8">
-        <v>464</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
@@ -1134,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
@@ -1149,55 +1149,55 @@
         <v>0</v>
       </c>
       <c r="G8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="H8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="I8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="J8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="K8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="L8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="M8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="N8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="O8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="P8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="R8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="S8" s="7">
         <v>0</v>
       </c>
       <c r="T8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="U8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="V8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="W8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="X8" s="7">
         <v>0</v>
@@ -1217,82 +1217,82 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>0</v>
+        <v>84.6</v>
       </c>
       <c r="C9" s="7">
-        <v>0</v>
+        <v>84.6</v>
       </c>
       <c r="D9" s="7">
         <v>84.6</v>
       </c>
       <c r="E9" s="7">
-        <v>84.6</v>
+        <v>84.429483474999074</v>
       </c>
       <c r="F9" s="7">
-        <v>84.6</v>
+        <v>82.462298826273468</v>
       </c>
       <c r="G9" s="7">
-        <v>84.6</v>
+        <v>83.684409515709945</v>
       </c>
       <c r="H9" s="7">
-        <v>84.6</v>
+        <v>77.807751388771521</v>
       </c>
       <c r="I9" s="7">
-        <v>84.6</v>
+        <v>81.703346874163003</v>
       </c>
       <c r="J9" s="7">
-        <v>84.6</v>
+        <v>81.365006141633444</v>
       </c>
       <c r="K9" s="7">
-        <v>84.6</v>
+        <v>80.500109638994331</v>
       </c>
       <c r="L9" s="7">
-        <v>84.6</v>
+        <v>77.694560625744884</v>
       </c>
       <c r="M9" s="7">
-        <v>84.6</v>
+        <v>80.088761671376218</v>
       </c>
       <c r="N9" s="7">
-        <v>84.6</v>
+        <v>77.684510526418194</v>
       </c>
       <c r="O9" s="7">
-        <v>84.6</v>
+        <v>80.483621121155807</v>
       </c>
       <c r="P9" s="7">
-        <v>84.6</v>
+        <v>78.487923711246253</v>
       </c>
       <c r="Q9" s="7">
-        <v>84.6</v>
+        <v>81.699265024647161</v>
       </c>
       <c r="R9" s="7">
-        <v>84.6</v>
+        <v>80.183102799596782</v>
       </c>
       <c r="S9" s="7">
-        <v>84.6</v>
+        <v>83.750533985557126</v>
       </c>
       <c r="T9" s="7">
-        <v>84.6</v>
+        <v>77.59423879142696</v>
       </c>
       <c r="U9" s="7">
-        <v>84.6</v>
+        <v>81.65253694054968</v>
       </c>
       <c r="V9" s="7">
-        <v>84.6</v>
+        <v>70.927359773014132</v>
       </c>
       <c r="W9" s="7">
-        <v>84.6</v>
+        <v>80.420656010971015</v>
       </c>
       <c r="X9" s="7">
-        <v>84.6</v>
+        <v>76.382744354061288</v>
       </c>
       <c r="Y9" s="7">
-        <v>84.6</v>
+        <v>83.109389053225982</v>
       </c>
       <c r="Z9" s="7">
-        <v>84.6</v>
+        <v>20.526573554725474</v>
       </c>
       <c r="AA9" s="8">
-        <v>84.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
@@ -1300,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -1312,64 +1312,64 @@
         <v>0</v>
       </c>
       <c r="F10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="G10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="H10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="I10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="J10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="K10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="L10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="M10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="N10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="O10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="P10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="R10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="S10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="T10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="U10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="V10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="W10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="X10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="7">
-        <v>85.51375562129715</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="7">
         <v>0</v>
@@ -1386,79 +1386,79 @@
         <v>0</v>
       </c>
       <c r="C11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="D11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="E11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="F11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="G11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="H11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="I11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="J11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="K11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="L11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="M11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="N11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="O11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="P11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="R11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="S11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="T11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="U11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="V11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="W11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="X11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="AA11" s="8">
-        <v>650</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
@@ -1466,82 +1466,82 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="C12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="D12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="E12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="F12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="G12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="H12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="I12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="J12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="K12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="L12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="M12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="N12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="O12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="P12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="R12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="S12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="T12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="U12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="V12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="W12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="X12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="AA12" s="8">
-        <v>186</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
@@ -1549,10 +1549,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="C13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="D13" s="7">
         <v>0</v>
@@ -1564,55 +1564,55 @@
         <v>0</v>
       </c>
       <c r="G13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="H13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="I13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="J13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="K13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="L13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="M13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="N13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="O13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="P13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="R13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="S13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="T13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="U13" s="7">
-        <v>153.99999999999935</v>
+        <v>0</v>
       </c>
       <c r="V13" s="7">
-        <v>90.066924690423036</v>
+        <v>0</v>
       </c>
       <c r="W13" s="7">
-        <v>44.932226380952073</v>
+        <v>0</v>
       </c>
       <c r="X13" s="7">
         <v>0</v>
@@ -1632,79 +1632,79 @@
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="C14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D14" s="7">
-        <v>85.515108379499111</v>
+        <v>0</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
       </c>
       <c r="F14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="G14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="I14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="J14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="K14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="L14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="M14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="N14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="O14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="P14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="R14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="S14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="T14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="U14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="V14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="W14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="X14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="7">
-        <v>132.96125884377807</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="8">
         <v>0</v>
@@ -1715,19 +1715,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>1848</v>
+        <v>0</v>
       </c>
       <c r="C15" s="7">
-        <v>1848</v>
+        <v>0</v>
       </c>
       <c r="D15" s="7">
-        <v>1848</v>
+        <v>0</v>
       </c>
       <c r="E15" s="7">
-        <v>1254.6797472637363</v>
+        <v>0</v>
       </c>
       <c r="F15" s="7">
-        <v>607.83770948546908</v>
+        <v>0</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -1798,7 +1798,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -1807,73 +1807,73 @@
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>604.92635573625989</v>
+        <v>0</v>
       </c>
       <c r="F16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="S16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="U16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="V16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="W16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="X16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="8">
-        <v>651.55241017337175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
@@ -1881,7 +1881,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="6">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
@@ -1893,58 +1893,58 @@
         <v>0</v>
       </c>
       <c r="F17" s="7">
-        <v>24.084748441526244</v>
+        <v>0</v>
       </c>
       <c r="G17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="H17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="I17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="J17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="K17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="L17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="M17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="N17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="O17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="P17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="R17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="S17" s="7">
-        <v>28.366370434874398</v>
+        <v>0</v>
       </c>
       <c r="T17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="U17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="V17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="W17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="X17" s="7">
         <v>0</v>
@@ -1964,82 +1964,82 @@
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>67</v>
+        <v>1.5916157281026244E-12</v>
       </c>
       <c r="C18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="D18" s="7">
         <v>0</v>
       </c>
       <c r="E18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="G18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="H18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="I18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="J18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="K18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="L18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="M18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="N18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="O18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="P18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="R18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="S18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="T18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="U18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="V18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="W18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="X18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="8">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
@@ -2047,22 +2047,22 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="C19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="D19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="E19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="F19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="G19" s="7">
-        <v>152.5020816708784</v>
+        <v>0</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
@@ -2098,28 +2098,28 @@
         <v>0</v>
       </c>
       <c r="S19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="T19" s="7">
-        <v>243.3262774589241</v>
+        <v>0</v>
       </c>
       <c r="U19" s="7">
-        <v>128.51664800577601</v>
+        <v>0</v>
       </c>
       <c r="V19" s="7">
-        <v>135.00956691885</v>
+        <v>0</v>
       </c>
       <c r="W19" s="7">
-        <v>55.50825365280312</v>
+        <v>0</v>
       </c>
       <c r="X19" s="7">
-        <v>79.06445869096126</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="7">
         <v>0</v>
       </c>
       <c r="Z19" s="7">
-        <v>42.671387508933805</v>
+        <v>0</v>
       </c>
       <c r="AA19" s="8">
         <v>0</v>
@@ -2130,55 +2130,55 @@
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>2269.6</v>
+        <v>0</v>
       </c>
       <c r="C20" s="7">
-        <v>2269.6</v>
+        <v>0</v>
       </c>
       <c r="D20" s="7">
-        <v>2269.6</v>
+        <v>0</v>
       </c>
       <c r="E20" s="7">
-        <v>2269.6</v>
+        <v>0</v>
       </c>
       <c r="F20" s="7">
-        <v>2269.6</v>
+        <v>0</v>
       </c>
       <c r="G20" s="7">
-        <v>2269.6</v>
+        <v>0</v>
       </c>
       <c r="H20" s="7">
-        <v>2237.1019054333419</v>
+        <v>0</v>
       </c>
       <c r="I20" s="7">
-        <v>1978.7119199863257</v>
+        <v>0</v>
       </c>
       <c r="J20" s="7">
-        <v>1760.4574188049342</v>
+        <v>0</v>
       </c>
       <c r="K20" s="7">
-        <v>1470.9206422412299</v>
+        <v>0</v>
       </c>
       <c r="L20" s="7">
-        <v>1326.3158997381511</v>
+        <v>0</v>
       </c>
       <c r="M20" s="7">
-        <v>1106.2893585003299</v>
+        <v>0</v>
       </c>
       <c r="N20" s="7">
-        <v>918.10659431102772</v>
+        <v>0</v>
       </c>
       <c r="O20" s="7">
-        <v>759.96465115096203</v>
+        <v>0</v>
       </c>
       <c r="P20" s="7">
-        <v>630.15706173928584</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="7">
-        <v>417.89810641941591</v>
+        <v>0</v>
       </c>
       <c r="R20" s="7">
-        <v>340</v>
+        <v>0</v>
       </c>
       <c r="S20" s="7">
         <v>0</v>
@@ -2187,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="7">
-        <v>-6.8212102632969618E-13</v>
+        <v>0</v>
       </c>
       <c r="V20" s="7">
         <v>0</v>
@@ -2213,7 +2213,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>15.829644736905736</v>
+        <v>0</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2258,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="7">
-        <v>2.6275825063407099E-11</v>
+        <v>0</v>
       </c>
       <c r="R21" s="7">
         <v>0</v>
@@ -2296,7 +2296,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -2308,70 +2308,70 @@
         <v>0</v>
       </c>
       <c r="F22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="G22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="H22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="I22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="J22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="K22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="L22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="M22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="N22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="O22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="P22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="R22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="S22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="T22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="U22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="V22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="W22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="X22" s="7">
-        <v>397.51828566309803</v>
+        <v>0</v>
       </c>
       <c r="Y22" s="7">
-        <v>355.79563343194741</v>
+        <v>0</v>
       </c>
       <c r="Z22" s="7">
-        <v>243.0939272020116</v>
+        <v>0</v>
       </c>
       <c r="AA22" s="8">
-        <v>301.38810254334294</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
@@ -2379,34 +2379,34 @@
         <v>21</v>
       </c>
       <c r="B23" s="6">
-        <v>0</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="C23" s="7">
-        <v>0</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="D23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.1</v>
       </c>
       <c r="E23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="F23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.1</v>
       </c>
       <c r="G23" s="7">
         <v>28.1</v>
       </c>
       <c r="H23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="I23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="J23" s="7">
         <v>28.099999999999994</v>
       </c>
       <c r="K23" s="7">
-        <v>28.1</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="L23" s="7">
         <v>28.100000000000009</v>
@@ -2433,28 +2433,28 @@
         <v>28.100000000000009</v>
       </c>
       <c r="T23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="U23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="V23" s="7">
         <v>28.100000000000009</v>
       </c>
-      <c r="U23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="V23" s="7">
-        <v>28.1</v>
-      </c>
       <c r="W23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="X23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="Y23" s="7">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="Z23" s="7">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="AA23" s="8">
         <v>28.099999999999994</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>28.099999999999994</v>
-      </c>
-      <c r="AA23" s="8">
-        <v>28.1</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
@@ -2462,10 +2462,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="6">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C24" s="7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D24" s="7">
         <v>25</v>
@@ -2545,10 +2545,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="6">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C25" s="7">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D25" s="7">
         <v>70</v>
@@ -2628,10 +2628,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="6">
-        <v>0</v>
+        <v>30.6</v>
       </c>
       <c r="C26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="D26" s="7">
         <v>30.6</v>
@@ -2643,10 +2643,10 @@
         <v>30.6</v>
       </c>
       <c r="G26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="H26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="I26" s="7">
         <v>30.6</v>
@@ -2655,7 +2655,7 @@
         <v>30.6</v>
       </c>
       <c r="K26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="L26" s="7">
         <v>30.6</v>
@@ -2685,7 +2685,7 @@
         <v>30.6</v>
       </c>
       <c r="U26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="V26" s="7">
         <v>30.6</v>
@@ -2700,7 +2700,7 @@
         <v>30.6</v>
       </c>
       <c r="Z26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="AA26" s="8">
         <v>30.599999999999998</v>
@@ -2711,7 +2711,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C27" s="7">
         <v>10</v>
@@ -2732,7 +2732,7 @@
         <v>10</v>
       </c>
       <c r="I27" s="7">
-        <v>9.9999999999999858</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="J27" s="7">
         <v>10</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="W27" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="X27" s="7">
         <v>10</v>
@@ -2786,7 +2786,7 @@
         <v>10</v>
       </c>
       <c r="AA27" s="8">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.35">
@@ -2794,7 +2794,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C28" s="7">
         <v>10</v>
@@ -2877,10 +2877,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C29" s="7">
-        <v>0.83264765525105133</v>
+        <v>10</v>
       </c>
       <c r="D29" s="7">
         <v>10</v>
@@ -2892,19 +2892,19 @@
         <v>10</v>
       </c>
       <c r="G29" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="H29" s="7">
         <v>10</v>
       </c>
       <c r="I29" s="7">
-        <v>10</v>
+        <v>10.000000000000014</v>
       </c>
       <c r="J29" s="7">
         <v>10</v>
       </c>
       <c r="K29" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="L29" s="7">
         <v>10</v>
@@ -2960,25 +2960,25 @@
         <v>28</v>
       </c>
       <c r="B30" s="6">
-        <v>0</v>
+        <v>52.2</v>
       </c>
       <c r="C30" s="7">
         <v>52.2</v>
       </c>
       <c r="D30" s="7">
-        <v>52.2</v>
+        <v>52.20000000000001</v>
       </c>
       <c r="E30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="F30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="G30" s="7">
         <v>52.200000000000017</v>
       </c>
       <c r="H30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.20000000000001</v>
       </c>
       <c r="I30" s="7">
         <v>52.2</v>
@@ -2987,7 +2987,7 @@
         <v>52.200000000000017</v>
       </c>
       <c r="K30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="L30" s="7">
         <v>52.2</v>
@@ -3017,16 +3017,16 @@
         <v>52.2</v>
       </c>
       <c r="U30" s="7">
-        <v>52.20000000000001</v>
+        <v>52.2</v>
       </c>
       <c r="V30" s="7">
         <v>52.2</v>
       </c>
       <c r="W30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="X30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="Y30" s="7">
         <v>52.2</v>
@@ -3043,7 +3043,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C31" s="7">
         <v>10</v>
@@ -3052,13 +3052,13 @@
         <v>10</v>
       </c>
       <c r="E31" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="F31" s="7">
         <v>10</v>
       </c>
       <c r="G31" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="H31" s="7">
         <v>10</v>
@@ -3070,7 +3070,7 @@
         <v>10</v>
       </c>
       <c r="K31" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="L31" s="7">
         <v>10</v>
@@ -3103,7 +3103,7 @@
         <v>10</v>
       </c>
       <c r="V31" s="7">
-        <v>10.000000000000014</v>
+        <v>10</v>
       </c>
       <c r="W31" s="7">
         <v>10</v>
@@ -3112,7 +3112,7 @@
         <v>10</v>
       </c>
       <c r="Y31" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="Z31" s="7">
         <v>10</v>
@@ -3126,37 +3126,37 @@
         <v>30</v>
       </c>
       <c r="B32" s="6">
-        <v>0</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="C32" s="7">
-        <v>20.2</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="D32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="E32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="F32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="G32" s="7">
-        <v>20.2</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="H32" s="7">
-        <v>20.2</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="I32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="J32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="K32" s="7">
         <v>20.2</v>
       </c>
       <c r="L32" s="7">
-        <v>20.2</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="M32" s="7">
         <v>20.199999999999996</v>
@@ -3180,25 +3180,25 @@
         <v>20.199999999999996</v>
       </c>
       <c r="T32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
       <c r="U32" s="7">
-        <v>20.2</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="V32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="W32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="X32" s="7">
-        <v>20.2</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="Y32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="Z32" s="7">
-        <v>20.2</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="AA32" s="8">
         <v>20.2</v>
@@ -3209,10 +3209,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="6">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C33" s="7">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D33" s="7">
         <v>70</v>
@@ -3292,10 +3292,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="6">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="C34" s="7">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="D34" s="7">
         <v>10.5</v>
@@ -3346,10 +3346,10 @@
         <v>10.5</v>
       </c>
       <c r="T34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="U34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="V34" s="7">
         <v>10.5</v>
@@ -3358,7 +3358,7 @@
         <v>10.5</v>
       </c>
       <c r="X34" s="7">
-        <v>10.499999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="Y34" s="7">
         <v>10.5</v>
@@ -3375,10 +3375,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C35" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D35" s="7">
         <v>10</v>
@@ -3435,7 +3435,7 @@
         <v>10</v>
       </c>
       <c r="V35" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="W35" s="7">
         <v>10</v>
@@ -3458,10 +3458,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C36" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D36" s="7">
         <v>10</v>
@@ -3527,7 +3527,7 @@
         <v>10</v>
       </c>
       <c r="Y36" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="Z36" s="7">
         <v>10</v>
@@ -3541,10 +3541,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C37" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D37" s="7">
         <v>10</v>
@@ -3610,7 +3610,7 @@
         <v>10</v>
       </c>
       <c r="Y37" s="7">
-        <v>10</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="Z37" s="7">
         <v>10</v>
@@ -3624,10 +3624,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C38" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D38" s="7">
         <v>10</v>
@@ -3707,28 +3707,28 @@
         <v>37</v>
       </c>
       <c r="B39" s="6">
-        <v>0</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="C39" s="7">
-        <v>0</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="D39" s="7">
-        <v>10.1</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="E39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="F39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="G39" s="7">
         <v>10.1</v>
-      </c>
-      <c r="G39" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="H39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="I39" s="7">
-        <v>10.1</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="J39" s="7">
         <v>10.099999999999994</v>
@@ -3758,13 +3758,13 @@
         <v>10.099999999999994</v>
       </c>
       <c r="S39" s="7">
-        <v>10.1</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="T39" s="7">
-        <v>10.1</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="U39" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="V39" s="7">
         <v>10.099999999999994</v>
@@ -3773,10 +3773,10 @@
         <v>10.099999999999994</v>
       </c>
       <c r="X39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="Y39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="Z39" s="7">
         <v>10.099999999999994</v>
@@ -3790,13 +3790,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="6">
-        <v>0</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="C40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="D40" s="7">
-        <v>10.1</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="E40" s="7">
         <v>10.100000000000001</v>
@@ -3811,16 +3811,16 @@
         <v>10.100000000000001</v>
       </c>
       <c r="I40" s="7">
-        <v>10.1</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="J40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="K40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="L40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.1</v>
       </c>
       <c r="M40" s="7">
         <v>10.100000000000001</v>
@@ -3841,22 +3841,22 @@
         <v>10.100000000000001</v>
       </c>
       <c r="S40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="T40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="U40" s="7">
         <v>10.1</v>
       </c>
-      <c r="T40" s="7">
+      <c r="V40" s="7">
         <v>10.1</v>
-      </c>
-      <c r="U40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="V40" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="W40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="X40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.1</v>
       </c>
       <c r="Y40" s="7">
         <v>10.1</v>
@@ -3873,10 +3873,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C41" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D41" s="7">
         <v>10</v>
@@ -3945,7 +3945,7 @@
         <v>10</v>
       </c>
       <c r="Z41" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="AA41" s="8">
         <v>10</v>
@@ -3956,7 +3956,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="6">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C42" s="7">
         <v>12</v>
@@ -3965,10 +3965,10 @@
         <v>12</v>
       </c>
       <c r="E42" s="7">
-        <v>12</v>
+        <v>11.999999999999993</v>
       </c>
       <c r="F42" s="7">
-        <v>12</v>
+        <v>11.999999999999993</v>
       </c>
       <c r="G42" s="7">
         <v>12</v>
@@ -4039,82 +4039,82 @@
         <v>41</v>
       </c>
       <c r="B43" s="6">
-        <v>0</v>
+        <v>5996.7499999999991</v>
       </c>
       <c r="C43" s="7">
-        <v>0</v>
+        <v>5999.2749999999978</v>
       </c>
       <c r="D43" s="7">
-        <v>0</v>
+        <v>5987.1827249999988</v>
       </c>
       <c r="E43" s="7">
-        <v>0</v>
+        <v>5950.4766195249977</v>
       </c>
       <c r="F43" s="7">
-        <v>0</v>
+        <v>5964.160159100722</v>
       </c>
       <c r="G43" s="7">
-        <v>0</v>
+        <v>5988.2368505326276</v>
       </c>
       <c r="H43" s="7">
-        <v>350</v>
+        <v>6000.0000000000018</v>
       </c>
       <c r="I43" s="7">
-        <v>650</v>
+        <v>6032.5838742771075</v>
       </c>
       <c r="J43" s="7">
-        <v>950</v>
+        <v>6049.9999999999973</v>
       </c>
       <c r="K43" s="7">
-        <v>1200</v>
+        <v>6078.5463815579114</v>
       </c>
       <c r="L43" s="7">
-        <v>1500</v>
+        <v>6099.642548991932</v>
       </c>
       <c r="M43" s="7">
-        <v>1750</v>
+        <v>6126.1535819328583</v>
       </c>
       <c r="N43" s="7">
-        <v>2000</v>
+        <v>6148.0832141702531</v>
       </c>
       <c r="O43" s="7">
-        <v>2250</v>
+        <v>6175.4352130977859</v>
       </c>
       <c r="P43" s="7">
-        <v>2500</v>
+        <v>6198.2133800156662</v>
       </c>
       <c r="Q43" s="7">
-        <v>2700</v>
+        <v>6226.4215504358053</v>
       </c>
       <c r="R43" s="7">
-        <v>2950</v>
+        <v>6249.9999999999991</v>
       </c>
       <c r="S43" s="7">
-        <v>3200</v>
+        <v>6279.1434167392345</v>
       </c>
       <c r="T43" s="7">
-        <v>3450</v>
+        <v>6298.6649574898875</v>
       </c>
       <c r="U43" s="7">
-        <v>3650</v>
+        <v>6328.6321921072949</v>
       </c>
       <c r="V43" s="7">
-        <v>3900</v>
+        <v>6344.049131836261</v>
       </c>
       <c r="W43" s="7">
-        <v>4100</v>
+        <v>6379.9198240227852</v>
       </c>
       <c r="X43" s="7">
-        <v>4350</v>
+        <v>6400</v>
       </c>
       <c r="Y43" s="7">
-        <v>4550</v>
+        <v>6400.0000000000309</v>
       </c>
       <c r="Z43" s="7">
-        <v>4800</v>
+        <v>6400</v>
       </c>
       <c r="AA43" s="8">
-        <v>5000</v>
+        <v>6399.9999999999827</v>
       </c>
       <c r="AB43" t="s">
         <v>17</v>
@@ -4125,82 +4125,82 @@
         <v>42</v>
       </c>
       <c r="B44" s="6">
-        <v>0</v>
+        <v>370</v>
       </c>
       <c r="C44" s="7">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="D44" s="7">
-        <v>0</v>
+        <v>560</v>
       </c>
       <c r="E44" s="7">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="F44" s="7">
-        <v>0</v>
+        <v>780</v>
       </c>
       <c r="G44" s="7">
-        <v>0</v>
+        <v>820</v>
       </c>
       <c r="H44" s="7">
-        <v>0</v>
+        <v>880</v>
       </c>
       <c r="I44" s="7">
-        <v>0</v>
+        <v>910</v>
       </c>
       <c r="J44" s="7">
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="K44" s="7">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="L44" s="7">
-        <v>0</v>
+        <v>1050</v>
       </c>
       <c r="M44" s="7">
-        <v>0</v>
+        <v>1090</v>
       </c>
       <c r="N44" s="7">
-        <v>0</v>
+        <v>1140</v>
       </c>
       <c r="O44" s="7">
-        <v>0</v>
+        <v>1180</v>
       </c>
       <c r="P44" s="7">
-        <v>0</v>
+        <v>1230</v>
       </c>
       <c r="Q44" s="7">
-        <v>0</v>
+        <v>1270</v>
       </c>
       <c r="R44" s="7">
-        <v>0</v>
+        <v>1320</v>
       </c>
       <c r="S44" s="7">
-        <v>0</v>
+        <v>1360</v>
       </c>
       <c r="T44" s="7">
-        <v>0</v>
+        <v>1420</v>
       </c>
       <c r="U44" s="7">
-        <v>0</v>
+        <v>1460</v>
       </c>
       <c r="V44" s="7">
-        <v>0</v>
+        <v>1530</v>
       </c>
       <c r="W44" s="7">
-        <v>0</v>
+        <v>1560</v>
       </c>
       <c r="X44" s="7">
-        <v>0</v>
+        <v>1620</v>
       </c>
       <c r="Y44" s="7">
-        <v>0</v>
+        <v>1689.9999999999902</v>
       </c>
       <c r="Z44" s="7">
-        <v>0</v>
+        <v>1830</v>
       </c>
       <c r="AA44" s="8">
-        <v>0</v>
+        <v>1928.6405127167338</v>
       </c>
       <c r="AB44" t="s">
         <v>18</v>
@@ -4307,82 +4307,82 @@
         <v>1</v>
       </c>
       <c r="B49" s="3">
-        <v>134.59011842103158</v>
+        <v>-1100.0000000000007</v>
       </c>
       <c r="C49" s="4">
-        <v>238.16156822983203</v>
+        <v>-1100</v>
       </c>
       <c r="D49" s="4">
-        <v>389.57841108033307</v>
+        <v>-1100</v>
       </c>
       <c r="E49" s="4">
-        <v>445.38034435000094</v>
+        <v>-1100</v>
       </c>
       <c r="F49" s="4">
-        <v>630.82005026299339</v>
+        <v>-1100</v>
       </c>
       <c r="G49" s="4">
-        <v>988.85720646479319</v>
+        <v>-1100</v>
       </c>
       <c r="H49" s="4">
-        <v>846.83951964716664</v>
+        <v>-1098.1931785417196</v>
       </c>
       <c r="I49" s="4">
-        <v>762.88527618929629</v>
+        <v>-1100</v>
       </c>
       <c r="J49" s="4">
-        <v>665.82177982875533</v>
+        <v>-1098.0924139029312</v>
       </c>
       <c r="K49" s="4">
-        <v>626.12404029153095</v>
+        <v>-1100</v>
       </c>
       <c r="L49" s="4">
-        <v>505.05639941523725</v>
+        <v>-1100</v>
       </c>
       <c r="M49" s="4">
-        <v>442.73926845512926</v>
+        <v>-1100</v>
       </c>
       <c r="N49" s="4">
-        <v>370.0866113431598</v>
+        <v>-1100</v>
       </c>
       <c r="O49" s="4">
-        <v>287.7019250148694</v>
+        <v>-1100</v>
       </c>
       <c r="P49" s="4">
-        <v>196.1565660973481</v>
+        <v>-1100</v>
       </c>
       <c r="Q49" s="4">
-        <v>165.71499815072264</v>
+        <v>-1100</v>
       </c>
       <c r="R49" s="4">
-        <v>57.442396259817713</v>
+        <v>-1099.9576037401812</v>
       </c>
       <c r="S49" s="4">
-        <v>-41.526512318802133</v>
+        <v>-1100</v>
       </c>
       <c r="T49" s="4">
-        <v>-177.93212082638382</v>
+        <v>-1100</v>
       </c>
       <c r="U49" s="4">
-        <v>-239.68408793039487</v>
+        <v>-1100</v>
       </c>
       <c r="V49" s="4">
-        <v>-332.28171754239202</v>
+        <v>-1100</v>
       </c>
       <c r="W49" s="4">
-        <v>-375.11101945637904</v>
+        <v>-1100</v>
       </c>
       <c r="X49" s="4">
-        <v>-468.42867982535927</v>
+        <v>-1099.1677650406721</v>
       </c>
       <c r="Y49" s="4">
-        <v>-526.97265273668881</v>
+        <v>-1087.9741082593891</v>
       </c>
       <c r="Z49" s="4">
-        <v>-624.09898603320789</v>
+        <v>-1099.8030419003735</v>
       </c>
       <c r="AA49" s="5">
-        <v>-635.81607690750707</v>
+        <v>-1097.5319401830441</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.35">
@@ -4390,82 +4390,82 @@
         <v>2</v>
       </c>
       <c r="B50" s="6">
-        <v>-371.30988157896866</v>
+        <v>1559.5499999999995</v>
       </c>
       <c r="C50" s="7">
-        <v>-210.30578411491643</v>
+        <v>1530.5749999999998</v>
       </c>
       <c r="D50" s="7">
-        <v>-241.38998054016702</v>
+        <v>1486.6992249999996</v>
       </c>
       <c r="E50" s="7">
-        <v>-291.56660415000147</v>
+        <v>1417.9235680249994</v>
       </c>
       <c r="F50" s="7">
-        <v>-584.15346921503601</v>
+        <v>1399.2489301372245</v>
       </c>
       <c r="G50" s="7">
-        <v>-712.60342355937644</v>
+        <v>1390.6762205084592</v>
       </c>
       <c r="H50" s="7">
-        <v>-537.56435604721923</v>
+        <v>1371.302945763895</v>
       </c>
       <c r="I50" s="7">
-        <v>-354.75833438633958</v>
+        <v>1368.8402637014724</v>
       </c>
       <c r="J50" s="7">
-        <v>-185.36072324205941</v>
+        <v>1354.6250830262511</v>
       </c>
       <c r="K50" s="7">
-        <v>-8.8992053069221129</v>
+        <v>1347.4231359594585</v>
       </c>
       <c r="L50" s="7">
-        <v>135.88784460639855</v>
+        <v>1334.3739941830934</v>
       </c>
       <c r="M50" s="7">
-        <v>289.11809665301132</v>
+        <v>1326.4324101307411</v>
       </c>
       <c r="N50" s="7">
-        <v>431.70274899482342</v>
+        <v>1313.5993518219175</v>
       </c>
       <c r="O50" s="7">
-        <v>564.24250790539827</v>
+        <v>1305.8757959883146</v>
       </c>
       <c r="P50" s="7">
-        <v>687.30591423389239</v>
+        <v>1293.2627281522095</v>
       </c>
       <c r="Q50" s="7">
-        <v>821.15459042049599</v>
+        <v>1285.7611427055792</v>
       </c>
       <c r="R50" s="7">
-        <v>926.85084486001972</v>
+        <v>1273.3508448600198</v>
       </c>
       <c r="S50" s="7">
-        <v>1041.5265123188021</v>
+        <v>1266.0964413768384</v>
       </c>
       <c r="T50" s="7">
-        <v>1118.4382810329591</v>
+        <v>1248.9353593492299</v>
       </c>
       <c r="U50" s="7">
-        <v>1219.6735475456819</v>
+        <v>1241.8898275833728</v>
       </c>
       <c r="V50" s="7">
-        <v>1275.7969613433938</v>
+        <v>1219.960886031623</v>
       </c>
       <c r="W50" s="7">
-        <v>1350.1509669076947</v>
+        <v>1218.1495840059074</v>
       </c>
       <c r="X50" s="7">
-        <v>1423.8799479976105</v>
+        <v>1201.0408627822962</v>
       </c>
       <c r="Y50" s="7">
-        <v>1526.9726527366884</v>
+        <v>1173.8711972140172</v>
       </c>
       <c r="Z50" s="7">
-        <v>1624.0989860332079</v>
+        <v>1123.3336713222634</v>
       </c>
       <c r="AA50" s="8">
-        <v>1635.8160769075071</v>
+        <v>1086.5478034585801</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.35">
@@ -4473,82 +4473,82 @@
         <v>3</v>
       </c>
       <c r="B51" s="9">
-        <v>236.71976315793711</v>
+        <v>-459.54999999999882</v>
       </c>
       <c r="C51" s="10">
-        <v>-27.855784114915593</v>
+        <v>-430.57499999999982</v>
       </c>
       <c r="D51" s="10">
-        <v>-148.18843054016605</v>
+        <v>-386.69922499999961</v>
       </c>
       <c r="E51" s="10">
-        <v>-153.81374019999947</v>
+        <v>-317.92356802499944</v>
       </c>
       <c r="F51" s="10">
-        <v>-46.666581047957266</v>
+        <v>-299.24893013722408</v>
       </c>
       <c r="G51" s="10">
-        <v>-276.25378290541647</v>
+        <v>-290.67622050845921</v>
       </c>
       <c r="H51" s="10">
-        <v>-309.27516359994735</v>
+        <v>-273.10976722217526</v>
       </c>
       <c r="I51" s="10">
-        <v>-408.12694180295694</v>
+        <v>-268.8402637014724</v>
       </c>
       <c r="J51" s="10">
-        <v>-480.46105658669592</v>
+        <v>-256.53266912331992</v>
       </c>
       <c r="K51" s="10">
-        <v>-617.22483498460883</v>
+        <v>-247.42313595945848</v>
       </c>
       <c r="L51" s="10">
-        <v>-640.94424402163565</v>
+        <v>-234.37399418309337</v>
       </c>
       <c r="M51" s="10">
-        <v>-731.85736510814058</v>
+        <v>-226.43241013074112</v>
       </c>
       <c r="N51" s="10">
-        <v>-801.78936033798323</v>
+        <v>-213.59935182191748</v>
       </c>
       <c r="O51" s="10">
-        <v>-851.94443292026767</v>
+        <v>-205.87579598831462</v>
       </c>
       <c r="P51" s="10">
-        <v>-883.4624803312405</v>
+        <v>-193.26272815220955</v>
       </c>
       <c r="Q51" s="10">
-        <v>-986.86958857121863</v>
+        <v>-185.76114270557923</v>
       </c>
       <c r="R51" s="10">
-        <v>-984.29324111983738</v>
+        <v>-173.39324111983865</v>
       </c>
       <c r="S51" s="10">
-        <v>-1000</v>
+        <v>-166.09644137683836</v>
       </c>
       <c r="T51" s="10">
-        <v>-940.50616020657537</v>
+        <v>-148.93535934922988</v>
       </c>
       <c r="U51" s="10">
-        <v>-979.98945961528705</v>
+        <v>-141.88982758337283</v>
       </c>
       <c r="V51" s="10">
-        <v>-943.51524380100182</v>
+        <v>-119.96088603162298</v>
       </c>
       <c r="W51" s="10">
-        <v>-975.03994745131558</v>
+        <v>-118.1495840059074</v>
       </c>
       <c r="X51" s="10">
-        <v>-955.45126817225139</v>
+        <v>-101.87309774162418</v>
       </c>
       <c r="Y51" s="10">
-        <v>-1000</v>
+        <v>-85.897088954628202</v>
       </c>
       <c r="Z51" s="10">
-        <v>-1000</v>
+        <v>-23.530629421889898</v>
       </c>
       <c r="AA51" s="11">
-        <v>-1000</v>
+        <v>10.984136724463951</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.35">
@@ -4639,86 +4639,86 @@
         <v>8</v>
       </c>
       <c r="B54" s="15">
-        <v>185343.2957730355</v>
+        <v>419066448.64103276</v>
       </c>
       <c r="C54" s="16">
-        <v>150354.42590554882</v>
+        <v>125273086.48681155</v>
       </c>
       <c r="D54" s="16">
-        <v>122850.98857876594</v>
+        <v>121082739.88063765</v>
       </c>
       <c r="E54" s="16">
-        <v>115767.04458876402</v>
+        <v>120287243.3532899</v>
       </c>
       <c r="F54" s="16">
-        <v>110839.76863109929</v>
+        <v>101061042.67947546</v>
       </c>
       <c r="G54" s="16">
-        <v>107601.0888445215</v>
+        <v>91054722.542002589</v>
       </c>
       <c r="H54" s="16">
-        <v>11641550.231811121</v>
+        <v>85756835.58219102</v>
       </c>
       <c r="I54" s="16">
-        <v>12324968.133583765</v>
+        <v>77835636.33026889</v>
       </c>
       <c r="J54" s="16">
-        <v>13729770.539331574</v>
+        <v>72095477.491315469</v>
       </c>
       <c r="K54" s="16">
-        <v>13539056.792083366</v>
+        <v>66837002.123430684</v>
       </c>
       <c r="L54" s="16">
-        <v>15173431.935465464</v>
+        <v>61305279.967726842</v>
       </c>
       <c r="M54" s="16">
-        <v>14667613.021367956</v>
+        <v>56802866.981785446</v>
       </c>
       <c r="N54" s="16">
-        <v>14771698.232724916</v>
+        <v>52088861.87211591</v>
       </c>
       <c r="O54" s="16">
-        <v>14735518.731834156</v>
+        <v>48238464.927511126</v>
       </c>
       <c r="P54" s="16">
-        <v>14583734.508809622</v>
+        <v>44224961.578445897</v>
       </c>
       <c r="Q54" s="16">
-        <v>13638852.260879792</v>
+        <v>40935877.731673487</v>
       </c>
       <c r="R54" s="16">
-        <v>13819966.051143175</v>
+        <v>37521716.813343227</v>
       </c>
       <c r="S54" s="16">
-        <v>13455936.071670964</v>
+        <v>34715087.464546926</v>
       </c>
       <c r="T54" s="16">
-        <v>13043632.510209475</v>
+        <v>32145404.736540187</v>
       </c>
       <c r="U54" s="16">
-        <v>12117802.26314237</v>
+        <v>29485302.677763384</v>
       </c>
       <c r="V54" s="16">
-        <v>11986589.48512092</v>
+        <v>27563924.879889011</v>
       </c>
       <c r="W54" s="16">
-        <v>11111677.895684551</v>
+        <v>24829028.306883618</v>
       </c>
       <c r="X54" s="16">
-        <v>10903515.051872116</v>
+        <v>23150557.073793795</v>
       </c>
       <c r="Y54" s="16">
-        <v>10089803.231113574</v>
+        <v>21517631.109444827</v>
       </c>
       <c r="Z54" s="16">
-        <v>9835358.2539883424</v>
+        <v>21155858.060010906</v>
       </c>
       <c r="AA54" s="17">
-        <v>9087917.6781258415</v>
+        <v>19062229.216091473</v>
       </c>
       <c r="AB54" s="18">
         <f>SUM(TotalCost)</f>
-        <v>255051149.4922848</v>
+        <v>1855093288.5080221</v>
       </c>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.35">
@@ -4812,86 +4812,86 @@
         <v>10</v>
       </c>
       <c r="B57" s="3">
-        <v>13395.809006237852</v>
+        <v>127.23839999999862</v>
       </c>
       <c r="C57" s="4">
-        <v>10788.134900264893</v>
+        <v>106.61999999999958</v>
       </c>
       <c r="D57" s="4">
-        <v>9558.804967341759</v>
+        <v>70.35619439999931</v>
       </c>
       <c r="E57" s="4">
-        <v>9312.0249598840437</v>
+        <v>174.35243586779998</v>
       </c>
       <c r="F57" s="4">
-        <v>8666.7645106792806</v>
+        <v>0.65969839061018776</v>
       </c>
       <c r="G57" s="4">
-        <v>7992.7910405343537</v>
+        <v>0.66947527612567959</v>
       </c>
       <c r="H57" s="4">
-        <v>7231.7522186328642</v>
+        <v>0.62246201111017219</v>
       </c>
       <c r="I57" s="4">
-        <v>6939.5927342366704</v>
+        <v>0.65362677499330402</v>
       </c>
       <c r="J57" s="4">
-        <v>6641.5502674662939</v>
+        <v>0.65092004913306756</v>
       </c>
       <c r="K57" s="4">
-        <v>6428.200739953425</v>
+        <v>0.64400087711195464</v>
       </c>
       <c r="L57" s="4">
-        <v>6119.5279553645905</v>
+        <v>0.62155648500595906</v>
       </c>
       <c r="M57" s="4">
-        <v>5896.2592355312281</v>
+        <v>0.64071009337427121</v>
       </c>
       <c r="N57" s="4">
-        <v>5668.5319125448623</v>
+        <v>0.62147608421134559</v>
       </c>
       <c r="O57" s="4">
-        <v>5436.6569033792557</v>
+        <v>0.6438689689692465</v>
       </c>
       <c r="P57" s="4">
-        <v>5200.9289870833718</v>
+        <v>0.62790338968997006</v>
       </c>
       <c r="Q57" s="4">
-        <v>5051.8183299385892</v>
+        <v>0.65359412019717733</v>
       </c>
       <c r="R57" s="4">
-        <v>4809.2087187230172</v>
+        <v>0.64146482239677427</v>
       </c>
       <c r="S57" s="4">
-        <v>5099.2167571217269</v>
+        <v>0.67000427188445699</v>
       </c>
       <c r="T57" s="4">
-        <v>4929.3134908072589</v>
+        <v>0.62075391033141569</v>
       </c>
       <c r="U57" s="4">
-        <v>4478.6003618073182</v>
+        <v>0.65322029552439742</v>
       </c>
       <c r="V57" s="4">
-        <v>4143.4773551581557</v>
+        <v>0.56741887818411307</v>
       </c>
       <c r="W57" s="4">
-        <v>3708.1193862656064</v>
+        <v>0.64336524808776818</v>
       </c>
       <c r="X57" s="4">
-        <v>3352.1940770678111</v>
+        <v>0.61106195483249026</v>
       </c>
       <c r="Y57" s="4">
-        <v>2961.9204175372606</v>
+        <v>0.66487511242580788</v>
       </c>
       <c r="Z57" s="4">
-        <v>2768.3019467310883</v>
+        <v>0.16421258843780379</v>
       </c>
       <c r="AA57" s="5">
-        <v>2672.733379103548</v>
+        <v>0</v>
       </c>
       <c r="AB57" s="12">
         <f>SUM(B57:AA57)</f>
-        <v>159252.23455939617</v>
+        <v>491.5126998704348</v>
       </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.35">
@@ -4899,86 +4899,86 @@
         <v>11</v>
       </c>
       <c r="B58" s="6">
-        <v>2413.9885322768887</v>
+        <v>0.47940000000000055</v>
       </c>
       <c r="C58" s="7">
-        <v>2265.7469347046895</v>
+        <v>0.40129999999999838</v>
       </c>
       <c r="D58" s="7">
-        <v>2260.5965095418974</v>
+        <v>0.26393709999999737</v>
       </c>
       <c r="E58" s="7">
-        <v>1949.7252897817255</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="F58" s="7">
-        <v>1610.7981043449747</v>
+        <v>0</v>
       </c>
       <c r="G58" s="7">
-        <v>1150.4026949077688</v>
+        <v>0</v>
       </c>
       <c r="H58" s="7">
-        <v>928.34771465728033</v>
+        <v>0</v>
       </c>
       <c r="I58" s="7">
-        <v>824.41550616380891</v>
+        <v>0</v>
       </c>
       <c r="J58" s="7">
-        <v>736.34160047708212</v>
+        <v>0</v>
       </c>
       <c r="K58" s="7">
-        <v>620.51602561486106</v>
+        <v>0</v>
       </c>
       <c r="L58" s="7">
-        <v>561.54347727351114</v>
+        <v>0</v>
       </c>
       <c r="M58" s="7">
-        <v>473.18423535646423</v>
+        <v>3.8120617773529373E-15</v>
       </c>
       <c r="N58" s="7">
-        <v>397.40824655042934</v>
+        <v>0</v>
       </c>
       <c r="O58" s="7">
-        <v>333.50338787838155</v>
+        <v>0</v>
       </c>
       <c r="P58" s="7">
-        <v>280.79564981683325</v>
+        <v>0</v>
       </c>
       <c r="Q58" s="7">
-        <v>195.92471855958934</v>
+        <v>0</v>
       </c>
       <c r="R58" s="7">
-        <v>163.73146482239679</v>
+        <v>0</v>
       </c>
       <c r="S58" s="7">
-        <v>376.80973050205012</v>
+        <v>0</v>
       </c>
       <c r="T58" s="7">
-        <v>356.79383208201045</v>
+        <v>0</v>
       </c>
       <c r="U58" s="7">
-        <v>199.98936917622052</v>
+        <v>0</v>
       </c>
       <c r="V58" s="7">
-        <v>207.39779424175362</v>
+        <v>0</v>
       </c>
       <c r="W58" s="7">
-        <v>98.517424047123882</v>
+        <v>0</v>
       </c>
       <c r="X58" s="7">
-        <v>128.3450141128038</v>
+        <v>0</v>
       </c>
       <c r="Y58" s="7">
-        <v>20.11007947899401</v>
+        <v>0</v>
       </c>
       <c r="Z58" s="7">
-        <v>76.764230252015167</v>
+        <v>0</v>
       </c>
       <c r="AA58" s="8">
-        <v>17.963283589017003</v>
+        <v>0</v>
       </c>
       <c r="AB58" s="13">
         <f t="shared" ref="AB58:AB61" si="0">SUM(B58:AA58)</f>
-        <v>18649.660850210566</v>
+        <v>1.3476371</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.35">
@@ -4986,86 +4986,86 @@
         <v>12</v>
       </c>
       <c r="B59" s="6">
-        <v>14017815.71121002</v>
+        <v>106950.48810000002</v>
       </c>
       <c r="C59" s="7">
-        <v>13261661.088989645</v>
+        <v>90435.657349999659</v>
       </c>
       <c r="D59" s="7">
-        <v>12546295.26186293</v>
+        <v>61389.24192324945</v>
       </c>
       <c r="E59" s="7">
-        <v>11869517.984329415</v>
+        <v>13084.016274990165</v>
       </c>
       <c r="F59" s="7">
-        <v>11229247.697411524</v>
+        <v>5436.8218239150356</v>
       </c>
       <c r="G59" s="7">
-        <v>10623515.126418673</v>
+        <v>5517.3968037802724</v>
       </c>
       <c r="H59" s="7">
-        <v>10050457.224063346</v>
+        <v>5129.9428568130952</v>
       </c>
       <c r="I59" s="7">
-        <v>9508311.4403000306</v>
+        <v>5386.7833627604405</v>
       </c>
       <c r="J59" s="7">
-        <v>8995410.3012627903</v>
+        <v>5364.476219924034</v>
       </c>
       <c r="K59" s="7">
-        <v>8510176.2806279529</v>
+        <v>5307.4527286085349</v>
       </c>
       <c r="L59" s="7">
-        <v>8051116.947627808</v>
+        <v>5122.480076615986</v>
       </c>
       <c r="M59" s="7">
-        <v>7616820.3767920891</v>
+        <v>5280.3321457556458</v>
       </c>
       <c r="N59" s="7">
-        <v>7205950.8052990194</v>
+        <v>5121.8174635172782</v>
       </c>
       <c r="O59" s="7">
-        <v>6817244.5245792577</v>
+        <v>5306.3656241389235</v>
       </c>
       <c r="P59" s="7">
-        <v>6449505.9935365934</v>
+        <v>5174.7872982061763</v>
       </c>
       <c r="Q59" s="7">
-        <v>6101604.161430845</v>
+        <v>5386.5142423400121</v>
       </c>
       <c r="R59" s="7">
-        <v>5772468.9891132778</v>
+        <v>5286.5521506802152</v>
       </c>
       <c r="S59" s="7">
-        <v>5461088.1579149337</v>
+        <v>5521.7564562017669</v>
       </c>
       <c r="T59" s="7">
-        <v>5166503.9560654238</v>
+        <v>5115.8657577575705</v>
       </c>
       <c r="U59" s="7">
-        <v>4887810.3330657603</v>
+        <v>5383.433413027381</v>
       </c>
       <c r="V59" s="7">
-        <v>4624150.1129553942</v>
+        <v>4676.311757194595</v>
       </c>
       <c r="W59" s="7">
-        <v>4374712.3579023099</v>
+        <v>5302.2142714593301</v>
       </c>
       <c r="X59" s="7">
-        <v>4138729.8740074006</v>
+        <v>5035.9907180076143</v>
       </c>
       <c r="Y59" s="7">
-        <v>3895260.8637902355</v>
+        <v>5479.4851296682418</v>
       </c>
       <c r="Z59" s="7">
-        <v>3685141.1441713171</v>
+        <v>1353.337521036605</v>
       </c>
       <c r="AA59" s="8">
-        <v>3479546.1153387381</v>
+        <v>0</v>
       </c>
       <c r="AB59" s="13">
         <f t="shared" si="0"/>
-        <v>198340062.83006674</v>
+        <v>378549.52146964805</v>
       </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.35">
@@ -5073,86 +5073,86 @@
         <v>13</v>
       </c>
       <c r="B60" s="6">
-        <v>1143.0110237631643</v>
+        <v>5.3156999999999783</v>
       </c>
       <c r="C60" s="7">
-        <v>1129.461877637516</v>
+        <v>4.8080499999999891</v>
       </c>
       <c r="D60" s="7">
-        <v>1120.2456230837952</v>
+        <v>3.9151911499999823</v>
       </c>
       <c r="E60" s="7">
-        <v>973.64233599940644</v>
+        <v>2.3351665703499758</v>
       </c>
       <c r="F60" s="7">
-        <v>815.41852060693975</v>
+        <v>2.1440197694831102</v>
       </c>
       <c r="G60" s="7">
-        <v>642.61487861710771</v>
+        <v>2.1757946474084586</v>
       </c>
       <c r="H60" s="7">
-        <v>595.01606521456551</v>
+        <v>2.0230015361080596</v>
       </c>
       <c r="I60" s="7">
-        <v>537.99196538490924</v>
+        <v>2.1242870187282379</v>
       </c>
       <c r="J60" s="7">
-        <v>488.96918648958103</v>
+        <v>2.1154901596824693</v>
       </c>
       <c r="K60" s="7">
-        <v>426.97572359473043</v>
+        <v>2.0930028506138525</v>
       </c>
       <c r="L60" s="7">
-        <v>392.63835467871627</v>
+        <v>2.020058576269367</v>
       </c>
       <c r="M60" s="7">
-        <v>344.50679858806723</v>
+        <v>2.0823078034557843</v>
       </c>
       <c r="N60" s="7">
-        <v>302.7270376606146</v>
+        <v>2.0197972736868728</v>
       </c>
       <c r="O60" s="7">
-        <v>266.94041760029597</v>
+        <v>2.0925741491500509</v>
       </c>
       <c r="P60" s="7">
-        <v>236.80748657556373</v>
+        <v>2.0406860164924026</v>
       </c>
       <c r="Q60" s="7">
-        <v>191.48202274851704</v>
+        <v>2.1241808906408259</v>
       </c>
       <c r="R60" s="7">
-        <v>171.70979446719025</v>
+        <v>2.0847606727895163</v>
       </c>
       <c r="S60" s="7">
-        <v>157.16414508817184</v>
+        <v>2.1775138836244854</v>
       </c>
       <c r="T60" s="7">
-        <v>150.30403313900942</v>
+        <v>2.0174502085771007</v>
       </c>
       <c r="U60" s="7">
-        <v>121.44847929844768</v>
+        <v>2.1229659604542914</v>
       </c>
       <c r="V60" s="7">
-        <v>118.44625605412547</v>
+        <v>1.8441113540983674</v>
       </c>
       <c r="W60" s="7">
-        <v>97.386657498214618</v>
+        <v>2.0909370562852465</v>
       </c>
       <c r="X60" s="7">
-        <v>97.772843926953001</v>
+        <v>1.9859513532055935</v>
       </c>
       <c r="Y60" s="7">
-        <v>76.892153504437616</v>
+        <v>2.1608441153838753</v>
       </c>
       <c r="Z60" s="7">
-        <v>81.722504254117055</v>
+        <v>0.53369091242286226</v>
       </c>
       <c r="AA60" s="8">
-        <v>69.096041433177916</v>
+        <v>0</v>
       </c>
       <c r="AB60" s="13">
         <f t="shared" si="0"/>
-        <v>10750.392226907335</v>
+        <v>58.447533928910758</v>
       </c>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.35">
@@ -5160,86 +5160,86 @@
         <v>14</v>
       </c>
       <c r="B61" s="9">
-        <v>163.18245218421194</v>
+        <v>0.61334999999999762</v>
       </c>
       <c r="C61" s="10">
-        <v>161.56613470468949</v>
+        <v>0.55477499999999869</v>
       </c>
       <c r="D61" s="10">
-        <v>161.01364910837947</v>
+        <v>0.45175282499999803</v>
       </c>
       <c r="E61" s="10">
-        <v>139.11516895775821</v>
+        <v>0.26728845042499721</v>
       </c>
       <c r="F61" s="10">
-        <v>115.37616262474334</v>
+        <v>0.24738689647882042</v>
       </c>
       <c r="G61" s="10">
-        <v>89.13771329690654</v>
+        <v>0.25105322854712986</v>
       </c>
       <c r="H61" s="10">
-        <v>82.409472665777812</v>
+        <v>0.23342325416631457</v>
       </c>
       <c r="I61" s="10">
-        <v>74.190732041892318</v>
+        <v>0.24511004062248901</v>
       </c>
       <c r="J61" s="10">
-        <v>67.177252576431286</v>
+        <v>0.24409501842490033</v>
       </c>
       <c r="K61" s="10">
-        <v>58.126512249630707</v>
+        <v>0.241500328916983</v>
       </c>
       <c r="L61" s="10">
-        <v>53.324951211379876</v>
+        <v>0.23308368187723466</v>
       </c>
       <c r="M61" s="10">
-        <v>46.361965442218363</v>
+        <v>0.24026628501412892</v>
       </c>
       <c r="N61" s="10">
-        <v>40.355533278724167</v>
+        <v>0.2330535315792546</v>
       </c>
       <c r="O61" s="10">
-        <v>35.251577202966736</v>
+        <v>0.24145086336346744</v>
       </c>
       <c r="P61" s="10">
-        <v>30.998914459632399</v>
+        <v>0.23546377113373876</v>
       </c>
       <c r="Q61" s="10">
-        <v>24.373984823503964</v>
+        <v>0.2450977950739415</v>
       </c>
       <c r="R61" s="10">
-        <v>21.681166205599194</v>
+        <v>0.24054930839879035</v>
       </c>
       <c r="S61" s="10">
-        <v>19.741154271884454</v>
+        <v>0.2512516019566714</v>
       </c>
       <c r="T61" s="10">
-        <v>19.046411826166047</v>
+        <v>0.23278271637428088</v>
       </c>
       <c r="U61" s="10">
-        <v>14.890935490292053</v>
+        <v>0.24495761082164905</v>
       </c>
       <c r="V61" s="10">
-        <v>14.697145183149871</v>
+        <v>0.21278207931904239</v>
       </c>
       <c r="W61" s="10">
-        <v>11.699693810643769</v>
+        <v>0.24126196803291305</v>
       </c>
       <c r="X61" s="10">
-        <v>11.955175369863898</v>
+        <v>0.22914823306218388</v>
       </c>
       <c r="Y61" s="10">
-        <v>8.9762281671597339</v>
+        <v>0.24932816715967795</v>
       </c>
       <c r="Z61" s="10">
-        <v>9.8666355084589856</v>
+        <v>6.157972066417642E-2</v>
       </c>
       <c r="AA61" s="11">
-        <v>8.0928215381501456</v>
+        <v>0</v>
       </c>
       <c r="AB61" s="14">
         <f t="shared" si="0"/>
-        <v>1482.6095442002145</v>
+        <v>6.7417923764127794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Drastically simplified to only check for adequate capacity during off-peak periods
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -727,10 +727,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>0</v>
+        <v>519.20000000000005</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>519.20000000000005</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -742,49 +742,49 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>0</v>
+        <v>495.91917837745336</v>
       </c>
       <c r="H3" s="4">
-        <v>0</v>
+        <v>396.80584595542905</v>
       </c>
       <c r="I3" s="4">
-        <v>0</v>
+        <v>421.67530116494049</v>
       </c>
       <c r="J3" s="4">
-        <v>0</v>
+        <v>407.00758733669346</v>
       </c>
       <c r="K3" s="4">
-        <v>0</v>
+        <v>514.22584895567297</v>
       </c>
       <c r="L3" s="4">
-        <v>0</v>
+        <v>427.12120987952324</v>
       </c>
       <c r="M3" s="4">
-        <v>0</v>
+        <v>466.0529851039019</v>
       </c>
       <c r="N3" s="4">
-        <v>0</v>
+        <v>473.76113038564114</v>
       </c>
       <c r="O3" s="4">
-        <v>0</v>
+        <v>452.05418306797816</v>
       </c>
       <c r="P3" s="4">
-        <v>0</v>
+        <v>402.64424198762578</v>
       </c>
       <c r="Q3" s="4">
-        <v>0</v>
+        <v>486.3227090409859</v>
       </c>
       <c r="R3" s="4">
-        <v>0</v>
+        <v>386.28310279959442</v>
       </c>
       <c r="S3" s="4">
-        <v>0</v>
+        <v>419.45037015797988</v>
       </c>
       <c r="T3" s="4">
-        <v>0</v>
+        <v>129.03291882238901</v>
       </c>
       <c r="U3" s="4">
-        <v>0</v>
+        <v>117.8680810420648</v>
       </c>
       <c r="V3" s="4">
         <v>0</v>
@@ -813,79 +813,79 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>0</v>
+        <v>130.26735234474813</v>
       </c>
       <c r="D4" s="7">
-        <v>0</v>
+        <v>641.05189162049328</v>
       </c>
       <c r="E4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="F4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="G4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="H4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="I4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="J4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="K4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="L4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="M4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="N4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="O4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="P4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="Q4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="R4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="S4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="T4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="U4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="V4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="W4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="X4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="Y4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="Z4" s="7">
-        <v>0</v>
+        <v>665.6</v>
       </c>
       <c r="AA4" s="8">
-        <v>0</v>
+        <v>665.6</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
@@ -893,7 +893,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
@@ -902,73 +902,73 @@
         <v>0</v>
       </c>
       <c r="E5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="F5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="G5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="H5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="I5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="J5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="K5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="L5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="M5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="N5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="O5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="P5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="R5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="S5" s="7">
+        <v>42.477210131935919</v>
+      </c>
+      <c r="T5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="U5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="V5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="W5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="X5" s="7">
+        <v>46.5</v>
+      </c>
+      <c r="Y5" s="7">
         <v>7</v>
       </c>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1.3145040611561853E-13</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0</v>
-      </c>
-      <c r="O5" s="7">
-        <v>0</v>
-      </c>
-      <c r="P5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>0</v>
-      </c>
-      <c r="R5" s="7">
-        <v>0</v>
-      </c>
-      <c r="S5" s="7">
-        <v>0</v>
-      </c>
-      <c r="T5" s="7">
-        <v>0</v>
-      </c>
-      <c r="U5" s="7">
-        <v>0</v>
-      </c>
-      <c r="V5" s="7">
-        <v>0</v>
-      </c>
-      <c r="W5" s="7">
-        <v>0</v>
-      </c>
-      <c r="X5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="7">
-        <v>0</v>
-      </c>
       <c r="Z5" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="AA5" s="8">
-        <v>0</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
@@ -976,82 +976,82 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>119.84999999999815</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7">
-        <v>100.32499999999959</v>
+        <v>212</v>
       </c>
       <c r="D6" s="7">
-        <v>65.984274999999343</v>
+        <v>212</v>
       </c>
       <c r="E6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="F6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="G6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="H6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="I6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="J6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="K6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="L6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="M6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="N6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="O6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="P6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="Q6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="R6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="S6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="T6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="U6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="V6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="W6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="X6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="Y6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="Z6" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="AA6" s="8">
-        <v>0</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
@@ -1059,82 +1059,82 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>0</v>
+        <v>192.67035526309559</v>
       </c>
       <c r="C7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="D7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="E7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="F7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="G7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="H7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="I7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="J7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="K7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="L7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="M7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="N7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="O7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="P7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="Q7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="R7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="S7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="T7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="U7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="V7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="W7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="X7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="Y7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="Z7" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="AA7" s="8">
-        <v>0</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
@@ -1142,7 +1142,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
@@ -1157,55 +1157,55 @@
         <v>0</v>
       </c>
       <c r="G8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="H8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="I8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="J8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="K8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="L8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="M8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="N8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="O8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="P8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="Q8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="R8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="S8" s="7">
         <v>0</v>
       </c>
       <c r="T8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="U8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="V8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="W8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="X8" s="7">
         <v>0</v>
@@ -1225,82 +1225,82 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>84.6</v>
+        <v>0</v>
       </c>
       <c r="C9" s="7">
-        <v>84.6</v>
+        <v>0</v>
       </c>
       <c r="D9" s="7">
         <v>84.6</v>
       </c>
       <c r="E9" s="7">
-        <v>84.429483474999074</v>
+        <v>84.6</v>
       </c>
       <c r="F9" s="7">
-        <v>82.462298826273468</v>
+        <v>84.6</v>
       </c>
       <c r="G9" s="7">
-        <v>83.684409515709945</v>
+        <v>84.6</v>
       </c>
       <c r="H9" s="7">
-        <v>77.807751388771521</v>
+        <v>84.6</v>
       </c>
       <c r="I9" s="7">
-        <v>81.703346874163003</v>
+        <v>84.6</v>
       </c>
       <c r="J9" s="7">
-        <v>81.365006141633444</v>
+        <v>84.6</v>
       </c>
       <c r="K9" s="7">
-        <v>80.500109638994331</v>
+        <v>84.6</v>
       </c>
       <c r="L9" s="7">
-        <v>77.694560625744884</v>
+        <v>84.6</v>
       </c>
       <c r="M9" s="7">
-        <v>80.088761671376218</v>
+        <v>84.6</v>
       </c>
       <c r="N9" s="7">
-        <v>77.684510526418194</v>
+        <v>84.6</v>
       </c>
       <c r="O9" s="7">
-        <v>80.483621121155807</v>
+        <v>84.6</v>
       </c>
       <c r="P9" s="7">
-        <v>78.487923711246253</v>
+        <v>84.6</v>
       </c>
       <c r="Q9" s="7">
-        <v>81.699265024647161</v>
+        <v>84.6</v>
       </c>
       <c r="R9" s="7">
-        <v>80.183102799596782</v>
+        <v>84.6</v>
       </c>
       <c r="S9" s="7">
-        <v>83.750533985557126</v>
+        <v>84.6</v>
       </c>
       <c r="T9" s="7">
-        <v>77.59423879142696</v>
+        <v>84.6</v>
       </c>
       <c r="U9" s="7">
-        <v>81.65253694054968</v>
+        <v>84.6</v>
       </c>
       <c r="V9" s="7">
-        <v>70.927359773014132</v>
+        <v>84.6</v>
       </c>
       <c r="W9" s="7">
-        <v>80.420656010971015</v>
+        <v>84.6</v>
       </c>
       <c r="X9" s="7">
-        <v>76.382744354061288</v>
+        <v>84.6</v>
       </c>
       <c r="Y9" s="7">
-        <v>83.109389053225982</v>
+        <v>80.286696024931487</v>
       </c>
       <c r="Z9" s="7">
-        <v>20.526573554725474</v>
+        <v>84.6</v>
       </c>
       <c r="AA9" s="8">
-        <v>0</v>
+        <v>84.6</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
@@ -1308,7 +1308,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -1320,64 +1320,64 @@
         <v>0</v>
       </c>
       <c r="F10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="G10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="H10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="I10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="K10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="L10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="M10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="N10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="O10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="P10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="Q10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="R10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="S10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="T10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="U10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="V10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="W10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="X10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="Y10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="Z10" s="7">
         <v>0</v>
@@ -1394,79 +1394,79 @@
         <v>0</v>
       </c>
       <c r="C11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="D11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="E11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="F11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="G11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="H11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="I11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="J11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="K11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="L11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="M11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="N11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="O11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="P11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="Q11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="R11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="S11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="T11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="U11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="V11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="W11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="X11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="Y11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="Z11" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="AA11" s="8">
-        <v>0</v>
+        <v>650</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
@@ -1474,82 +1474,82 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="C12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="D12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="F12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="G12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="H12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="I12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="J12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="K12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="L12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="M12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="N12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="O12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="P12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="Q12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="R12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="S12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="T12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="U12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="V12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="W12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="X12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="Y12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="Z12" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="AA12" s="8">
-        <v>0</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
@@ -1557,10 +1557,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="C13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="D13" s="7">
         <v>0</v>
@@ -1572,55 +1572,55 @@
         <v>0</v>
       </c>
       <c r="G13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="H13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="I13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="J13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="K13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="L13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="M13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="N13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="O13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="P13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="Q13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="R13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="S13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="T13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="U13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="V13" s="7">
-        <v>0</v>
+        <v>90.066924690421729</v>
       </c>
       <c r="W13" s="7">
-        <v>0</v>
+        <v>44.932226380951619</v>
       </c>
       <c r="X13" s="7">
         <v>0</v>
@@ -1640,79 +1640,79 @@
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D14" s="7">
-        <v>0</v>
+        <v>85.515108379504568</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
       </c>
       <c r="F14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="J14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="K14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="L14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="M14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="N14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="O14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="P14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Q14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="R14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="S14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="T14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="U14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="V14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="W14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="X14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Y14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Z14" s="7">
-        <v>0</v>
+        <v>132.96125884377807</v>
       </c>
       <c r="AA14" s="8">
         <v>0</v>
@@ -1723,19 +1723,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>0</v>
+        <v>1848</v>
       </c>
       <c r="C15" s="7">
-        <v>0</v>
+        <v>1848</v>
       </c>
       <c r="D15" s="7">
-        <v>0</v>
+        <v>1848</v>
       </c>
       <c r="E15" s="7">
-        <v>0</v>
+        <v>1254.6797472637372</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>607.8377094854726</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -1806,7 +1806,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -1815,73 +1815,73 @@
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>0</v>
+        <v>604.92635573625898</v>
       </c>
       <c r="F16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="G16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="H16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="I16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="J16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="K16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="L16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="M16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="N16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="O16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="P16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="Q16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="R16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="S16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="T16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="U16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="V16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="W16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="X16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="Y16" s="7">
-        <v>0</v>
+        <v>654.92269302831357</v>
       </c>
       <c r="Z16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="AA16" s="8">
-        <v>0</v>
+        <v>651.55241017337175</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
@@ -1889,7 +1889,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="6">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
@@ -1901,58 +1901,58 @@
         <v>0</v>
       </c>
       <c r="F17" s="7">
-        <v>0</v>
+        <v>24.084748441522727</v>
       </c>
       <c r="G17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="H17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="I17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="J17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="K17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="L17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="M17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="N17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="O17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="P17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="Q17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="R17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="S17" s="7">
-        <v>0</v>
+        <v>28.366370434874398</v>
       </c>
       <c r="T17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="U17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="V17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="W17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="X17" s="7">
         <v>0</v>
@@ -1972,82 +1972,82 @@
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>1.5916157281026244E-12</v>
+        <v>67</v>
       </c>
       <c r="C18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="D18" s="7">
         <v>0</v>
       </c>
       <c r="E18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="F18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="G18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="H18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="I18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="K18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="L18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="M18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="N18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="O18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="P18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Q18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="R18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="S18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="T18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="U18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="V18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="W18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="X18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Y18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Z18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="AA18" s="8">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
@@ -2055,22 +2055,22 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="C19" s="7">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="D19" s="7">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="E19" s="7">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="F19" s="7">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="G19" s="7">
-        <v>0</v>
+        <v>152.50208167088411</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
@@ -2106,28 +2106,28 @@
         <v>0</v>
       </c>
       <c r="S19" s="7">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="T19" s="7">
-        <v>0</v>
+        <v>243.3262774589235</v>
       </c>
       <c r="U19" s="7">
-        <v>0</v>
+        <v>128.51664800577814</v>
       </c>
       <c r="V19" s="7">
-        <v>0</v>
+        <v>135.00956691885131</v>
       </c>
       <c r="W19" s="7">
-        <v>0</v>
+        <v>55.508253652803575</v>
       </c>
       <c r="X19" s="7">
-        <v>0</v>
+        <v>79.064458690961544</v>
       </c>
       <c r="Y19" s="7">
         <v>0</v>
       </c>
       <c r="Z19" s="7">
-        <v>0</v>
+        <v>65.354925502311204</v>
       </c>
       <c r="AA19" s="8">
         <v>0</v>
@@ -2138,55 +2138,55 @@
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>0</v>
+        <v>2269.6</v>
       </c>
       <c r="C20" s="7">
-        <v>0</v>
+        <v>2269.6</v>
       </c>
       <c r="D20" s="7">
-        <v>0</v>
+        <v>2269.6</v>
       </c>
       <c r="E20" s="7">
-        <v>0</v>
+        <v>2269.6</v>
       </c>
       <c r="F20" s="7">
-        <v>0</v>
+        <v>2269.6</v>
       </c>
       <c r="G20" s="7">
-        <v>0</v>
+        <v>2269.6</v>
       </c>
       <c r="H20" s="7">
-        <v>0</v>
+        <v>2237.1019054333428</v>
       </c>
       <c r="I20" s="7">
-        <v>0</v>
+        <v>1978.7119199863289</v>
       </c>
       <c r="J20" s="7">
-        <v>0</v>
+        <v>1760.4574188049367</v>
       </c>
       <c r="K20" s="7">
-        <v>0</v>
+        <v>1470.9206422412312</v>
       </c>
       <c r="L20" s="7">
-        <v>0</v>
+        <v>1326.3158997381524</v>
       </c>
       <c r="M20" s="7">
-        <v>0</v>
+        <v>1106.2893585003312</v>
       </c>
       <c r="N20" s="7">
-        <v>0</v>
+        <v>918.10659431102886</v>
       </c>
       <c r="O20" s="7">
-        <v>0</v>
+        <v>759.96465115096225</v>
       </c>
       <c r="P20" s="7">
-        <v>0</v>
+        <v>630.15706173928538</v>
       </c>
       <c r="Q20" s="7">
-        <v>0</v>
+        <v>417.89810641946548</v>
       </c>
       <c r="R20" s="7">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="S20" s="7">
         <v>0</v>
@@ -2221,7 +2221,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>0</v>
+        <v>15.829644736904577</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2304,7 +2304,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -2316,70 +2316,70 @@
         <v>0</v>
       </c>
       <c r="F22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="G22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="H22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="I22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="J22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="K22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="L22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="M22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="N22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="O22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="P22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="Q22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="R22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="S22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="T22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="U22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="V22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="W22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="X22" s="7">
-        <v>0</v>
+        <v>397.51828566309774</v>
       </c>
       <c r="Y22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="Z22" s="7">
-        <v>0</v>
+        <v>220.4103892086342</v>
       </c>
       <c r="AA22" s="8">
-        <v>0</v>
+        <v>301.38810254334294</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
@@ -2387,82 +2387,82 @@
         <v>21</v>
       </c>
       <c r="B23" s="6">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="E23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="F23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="G23" s="7">
         <v>28.100000000000009</v>
       </c>
-      <c r="C23" s="7">
+      <c r="H23" s="7">
         <v>28.100000000000009</v>
       </c>
-      <c r="D23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="E23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="F23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="G23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="H23" s="7">
-        <v>28.1</v>
-      </c>
       <c r="I23" s="7">
-        <v>28.1</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="J23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="K23" s="7">
         <v>28.099999999999994</v>
       </c>
       <c r="L23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="M23" s="7">
         <v>28.100000000000009</v>
       </c>
       <c r="N23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.1</v>
       </c>
       <c r="O23" s="7">
         <v>28.099999999999994</v>
       </c>
       <c r="P23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="Q23" s="7">
         <v>28.100000000000009</v>
       </c>
       <c r="R23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="S23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="T23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="U23" s="7">
         <v>28.100000000000009</v>
-      </c>
-      <c r="S23" s="7">
-        <v>28.100000000000009</v>
-      </c>
-      <c r="T23" s="7">
-        <v>28.099999999999994</v>
-      </c>
-      <c r="U23" s="7">
-        <v>28.099999999999994</v>
       </c>
       <c r="V23" s="7">
         <v>28.100000000000009</v>
       </c>
       <c r="W23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="X23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="Y23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="Z23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="AA23" s="8">
         <v>28.100000000000009</v>
-      </c>
-      <c r="X23" s="7">
-        <v>28.100000000000009</v>
-      </c>
-      <c r="Y23" s="7">
-        <v>28.100000000000009</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>28.100000000000009</v>
-      </c>
-      <c r="AA23" s="8">
-        <v>28.099999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
@@ -2470,7 +2470,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="6">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C24" s="7">
         <v>25</v>
@@ -2553,7 +2553,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C25" s="7">
         <v>70</v>
@@ -2636,10 +2636,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="6">
-        <v>30.6</v>
+        <v>0</v>
       </c>
       <c r="C26" s="7">
-        <v>30.6</v>
+        <v>0</v>
       </c>
       <c r="D26" s="7">
         <v>30.6</v>
@@ -2660,10 +2660,10 @@
         <v>30.6</v>
       </c>
       <c r="J26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="K26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="L26" s="7">
         <v>30.6</v>
@@ -2678,10 +2678,10 @@
         <v>30.6</v>
       </c>
       <c r="P26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="Q26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="R26" s="7">
         <v>30.6</v>
@@ -2711,7 +2711,7 @@
         <v>30.6</v>
       </c>
       <c r="AA26" s="8">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
@@ -2719,10 +2719,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C27" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D27" s="7">
         <v>10</v>
@@ -2740,52 +2740,52 @@
         <v>10</v>
       </c>
       <c r="I27" s="7">
+        <v>10</v>
+      </c>
+      <c r="J27" s="7">
+        <v>10</v>
+      </c>
+      <c r="K27" s="7">
+        <v>10</v>
+      </c>
+      <c r="L27" s="7">
+        <v>10</v>
+      </c>
+      <c r="M27" s="7">
+        <v>10</v>
+      </c>
+      <c r="N27" s="7">
+        <v>10</v>
+      </c>
+      <c r="O27" s="7">
+        <v>10</v>
+      </c>
+      <c r="P27" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>10</v>
+      </c>
+      <c r="R27" s="7">
+        <v>10</v>
+      </c>
+      <c r="S27" s="7">
+        <v>10</v>
+      </c>
+      <c r="T27" s="7">
+        <v>10</v>
+      </c>
+      <c r="U27" s="7">
+        <v>10</v>
+      </c>
+      <c r="V27" s="7">
+        <v>10</v>
+      </c>
+      <c r="W27" s="7">
+        <v>10</v>
+      </c>
+      <c r="X27" s="7">
         <v>9.9999999999999929</v>
-      </c>
-      <c r="J27" s="7">
-        <v>10</v>
-      </c>
-      <c r="K27" s="7">
-        <v>10</v>
-      </c>
-      <c r="L27" s="7">
-        <v>10</v>
-      </c>
-      <c r="M27" s="7">
-        <v>10</v>
-      </c>
-      <c r="N27" s="7">
-        <v>10</v>
-      </c>
-      <c r="O27" s="7">
-        <v>10</v>
-      </c>
-      <c r="P27" s="7">
-        <v>10</v>
-      </c>
-      <c r="Q27" s="7">
-        <v>10</v>
-      </c>
-      <c r="R27" s="7">
-        <v>10</v>
-      </c>
-      <c r="S27" s="7">
-        <v>10</v>
-      </c>
-      <c r="T27" s="7">
-        <v>10</v>
-      </c>
-      <c r="U27" s="7">
-        <v>10</v>
-      </c>
-      <c r="V27" s="7">
-        <v>10</v>
-      </c>
-      <c r="W27" s="7">
-        <v>10</v>
-      </c>
-      <c r="X27" s="7">
-        <v>10</v>
       </c>
       <c r="Y27" s="7">
         <v>10</v>
@@ -2802,10 +2802,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C28" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D28" s="7">
         <v>10</v>
@@ -2829,10 +2829,10 @@
         <v>10</v>
       </c>
       <c r="K28" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="L28" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="M28" s="7">
         <v>10</v>
@@ -2885,10 +2885,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C29" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D29" s="7">
         <v>10</v>
@@ -2900,46 +2900,46 @@
         <v>10</v>
       </c>
       <c r="G29" s="7">
+        <v>10</v>
+      </c>
+      <c r="H29" s="7">
+        <v>10</v>
+      </c>
+      <c r="I29" s="7">
+        <v>10</v>
+      </c>
+      <c r="J29" s="7">
+        <v>10</v>
+      </c>
+      <c r="K29" s="7">
+        <v>10</v>
+      </c>
+      <c r="L29" s="7">
+        <v>10</v>
+      </c>
+      <c r="M29" s="7">
+        <v>10</v>
+      </c>
+      <c r="N29" s="7">
+        <v>10</v>
+      </c>
+      <c r="O29" s="7">
+        <v>10</v>
+      </c>
+      <c r="P29" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>10</v>
+      </c>
+      <c r="R29" s="7">
         <v>9.9999999999999929</v>
       </c>
-      <c r="H29" s="7">
-        <v>10</v>
-      </c>
-      <c r="I29" s="7">
-        <v>10.000000000000014</v>
-      </c>
-      <c r="J29" s="7">
-        <v>10</v>
-      </c>
-      <c r="K29" s="7">
-        <v>9.9999999999999858</v>
-      </c>
-      <c r="L29" s="7">
-        <v>10</v>
-      </c>
-      <c r="M29" s="7">
-        <v>10</v>
-      </c>
-      <c r="N29" s="7">
-        <v>10</v>
-      </c>
-      <c r="O29" s="7">
-        <v>10</v>
-      </c>
-      <c r="P29" s="7">
-        <v>10</v>
-      </c>
-      <c r="Q29" s="7">
-        <v>10</v>
-      </c>
-      <c r="R29" s="7">
-        <v>10</v>
-      </c>
       <c r="S29" s="7">
         <v>10</v>
       </c>
       <c r="T29" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="U29" s="7">
         <v>10</v>
@@ -2968,31 +2968,31 @@
         <v>28</v>
       </c>
       <c r="B30" s="6">
+        <v>0</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
         <v>52.2</v>
       </c>
-      <c r="C30" s="7">
+      <c r="E30" s="7">
         <v>52.2</v>
       </c>
-      <c r="D30" s="7">
-        <v>52.20000000000001</v>
-      </c>
-      <c r="E30" s="7">
-        <v>52.200000000000017</v>
-      </c>
       <c r="F30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="G30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="H30" s="7">
-        <v>52.20000000000001</v>
+        <v>52.2</v>
       </c>
       <c r="I30" s="7">
         <v>52.2</v>
       </c>
       <c r="J30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="K30" s="7">
         <v>52.2</v>
@@ -3004,22 +3004,22 @@
         <v>52.2</v>
       </c>
       <c r="N30" s="7">
-        <v>52.2</v>
+        <v>52.20000000000001</v>
       </c>
       <c r="O30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="P30" s="7">
-        <v>52.2</v>
+        <v>52.20000000000001</v>
       </c>
       <c r="Q30" s="7">
         <v>52.2</v>
       </c>
       <c r="R30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="S30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="T30" s="7">
         <v>52.2</v>
@@ -3031,19 +3031,19 @@
         <v>52.2</v>
       </c>
       <c r="W30" s="7">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="X30" s="7">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="Y30" s="7">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="Z30" s="7">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="AA30" s="8">
         <v>52.2</v>
-      </c>
-      <c r="X30" s="7">
-        <v>52.2</v>
-      </c>
-      <c r="Y30" s="7">
-        <v>52.2</v>
-      </c>
-      <c r="Z30" s="7">
-        <v>52.2</v>
-      </c>
-      <c r="AA30" s="8">
-        <v>52.200000000000017</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.35">
@@ -3051,10 +3051,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C31" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D31" s="7">
         <v>10</v>
@@ -3102,10 +3102,10 @@
         <v>10</v>
       </c>
       <c r="S31" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="T31" s="7">
-        <v>10</v>
+        <v>10.000000000000014</v>
       </c>
       <c r="U31" s="7">
         <v>10</v>
@@ -3134,73 +3134,73 @@
         <v>30</v>
       </c>
       <c r="B32" s="6">
-        <v>20.200000000000003</v>
+        <v>0</v>
       </c>
       <c r="C32" s="7">
-        <v>20.199999999999996</v>
+        <v>0</v>
       </c>
       <c r="D32" s="7">
         <v>20.200000000000003</v>
       </c>
       <c r="E32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
       <c r="F32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="G32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="H32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="I32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
       <c r="J32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
       <c r="K32" s="7">
         <v>20.2</v>
       </c>
       <c r="L32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="M32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="N32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="O32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="P32" s="7">
         <v>20.2</v>
       </c>
-      <c r="P32" s="7">
+      <c r="Q32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="R32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="S32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="T32" s="7">
         <v>20.200000000000003</v>
-      </c>
-      <c r="Q32" s="7">
-        <v>20.200000000000003</v>
-      </c>
-      <c r="R32" s="7">
-        <v>20.199999999999996</v>
-      </c>
-      <c r="S32" s="7">
-        <v>20.199999999999996</v>
-      </c>
-      <c r="T32" s="7">
-        <v>20.2</v>
       </c>
       <c r="U32" s="7">
         <v>20.200000000000003</v>
       </c>
       <c r="V32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="W32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
       <c r="X32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
       <c r="Y32" s="7">
         <v>20.199999999999996</v>
@@ -3209,7 +3209,7 @@
         <v>20.200000000000003</v>
       </c>
       <c r="AA32" s="8">
-        <v>20.2</v>
+        <v>20.200000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.35">
@@ -3217,10 +3217,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="6">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C33" s="7">
-        <v>70</v>
+        <v>30.932647655250321</v>
       </c>
       <c r="D33" s="7">
         <v>70</v>
@@ -3300,19 +3300,19 @@
         <v>32</v>
       </c>
       <c r="B34" s="6">
-        <v>10.5</v>
+        <v>0</v>
       </c>
       <c r="C34" s="7">
-        <v>10.5</v>
+        <v>0</v>
       </c>
       <c r="D34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="E34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="F34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="G34" s="7">
         <v>10.5</v>
@@ -3339,10 +3339,10 @@
         <v>10.5</v>
       </c>
       <c r="O34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="P34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="Q34" s="7">
         <v>10.5</v>
@@ -3354,10 +3354,10 @@
         <v>10.5</v>
       </c>
       <c r="T34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="U34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="V34" s="7">
         <v>10.5</v>
@@ -3383,10 +3383,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C35" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D35" s="7">
         <v>10</v>
@@ -3466,7 +3466,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C36" s="7">
         <v>10</v>
@@ -3535,7 +3535,7 @@
         <v>10</v>
       </c>
       <c r="Y36" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="Z36" s="7">
         <v>10</v>
@@ -3549,7 +3549,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C37" s="7">
         <v>10</v>
@@ -3618,7 +3618,7 @@
         <v>10</v>
       </c>
       <c r="Y37" s="7">
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="Z37" s="7">
         <v>10</v>
@@ -3632,7 +3632,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C38" s="7">
         <v>10</v>
@@ -3715,22 +3715,22 @@
         <v>37</v>
       </c>
       <c r="B39" s="6">
-        <v>10.099999999999994</v>
+        <v>0</v>
       </c>
       <c r="C39" s="7">
-        <v>10.099999999999994</v>
+        <v>0</v>
       </c>
       <c r="D39" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="E39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="F39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="G39" s="7">
-        <v>10.1</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="H39" s="7">
         <v>10.099999999999994</v>
@@ -3742,7 +3742,7 @@
         <v>10.099999999999994</v>
       </c>
       <c r="K39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="L39" s="7">
         <v>10.099999999999994</v>
@@ -3751,16 +3751,16 @@
         <v>10.099999999999994</v>
       </c>
       <c r="N39" s="7">
-        <v>10.1</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="O39" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="P39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="Q39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="R39" s="7">
         <v>10.099999999999994</v>
@@ -3769,22 +3769,22 @@
         <v>10.099999999999994</v>
       </c>
       <c r="T39" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="U39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="V39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="W39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="X39" s="7">
-        <v>10.1</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="Y39" s="7">
-        <v>10.1</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="Z39" s="7">
         <v>10.099999999999994</v>
@@ -3798,34 +3798,34 @@
         <v>38</v>
       </c>
       <c r="B40" s="6">
-        <v>10.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="C40" s="7">
-        <v>10.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="D40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="E40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="F40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="G40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="H40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="I40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="J40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="K40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="L40" s="7">
         <v>10.1</v>
@@ -3837,40 +3837,40 @@
         <v>10.1</v>
       </c>
       <c r="O40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="P40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="R40" s="7">
         <v>10.099999999999998</v>
       </c>
-      <c r="P40" s="7">
+      <c r="S40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="T40" s="7">
         <v>10.1</v>
       </c>
-      <c r="Q40" s="7">
+      <c r="U40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="V40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="W40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="X40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="Y40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="Z40" s="7">
         <v>10.1</v>
-      </c>
-      <c r="R40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="S40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="T40" s="7">
-        <v>10.099999999999998</v>
-      </c>
-      <c r="U40" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="V40" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="W40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="X40" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="Y40" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="Z40" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="AA40" s="8">
         <v>10.100000000000001</v>
@@ -3881,10 +3881,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C41" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D41" s="7">
         <v>10</v>
@@ -3964,19 +3964,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="6">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C42" s="7">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D42" s="7">
         <v>12</v>
       </c>
       <c r="E42" s="7">
-        <v>11.999999999999993</v>
+        <v>12</v>
       </c>
       <c r="F42" s="7">
-        <v>11.999999999999993</v>
+        <v>12</v>
       </c>
       <c r="G42" s="7">
         <v>12</v>
@@ -4047,82 +4047,82 @@
         <v>41</v>
       </c>
       <c r="B43" s="6">
-        <v>5996.7499999999991</v>
+        <v>0</v>
       </c>
       <c r="C43" s="7">
-        <v>5999.2749999999978</v>
+        <v>0</v>
       </c>
       <c r="D43" s="7">
-        <v>5987.1827249999988</v>
+        <v>0</v>
       </c>
       <c r="E43" s="7">
-        <v>5950.4766195249977</v>
+        <v>0</v>
       </c>
       <c r="F43" s="7">
-        <v>5964.160159100722</v>
+        <v>0</v>
       </c>
       <c r="G43" s="7">
-        <v>5988.2368505326276</v>
+        <v>0</v>
       </c>
       <c r="H43" s="7">
-        <v>6000.0000000000018</v>
+        <v>350</v>
       </c>
       <c r="I43" s="7">
-        <v>6032.5838742771075</v>
+        <v>650</v>
       </c>
       <c r="J43" s="7">
-        <v>6049.9999999999973</v>
+        <v>950</v>
       </c>
       <c r="K43" s="7">
-        <v>6078.5463815579114</v>
+        <v>1200</v>
       </c>
       <c r="L43" s="7">
-        <v>6099.642548991932</v>
+        <v>1500</v>
       </c>
       <c r="M43" s="7">
-        <v>6126.1535819328583</v>
+        <v>1750</v>
       </c>
       <c r="N43" s="7">
-        <v>6148.0832141702531</v>
+        <v>2000</v>
       </c>
       <c r="O43" s="7">
-        <v>6175.4352130977859</v>
+        <v>2250</v>
       </c>
       <c r="P43" s="7">
-        <v>6198.2133800156662</v>
+        <v>2500</v>
       </c>
       <c r="Q43" s="7">
-        <v>6226.4215504358053</v>
+        <v>2700</v>
       </c>
       <c r="R43" s="7">
-        <v>6249.9999999999991</v>
+        <v>2950</v>
       </c>
       <c r="S43" s="7">
-        <v>6279.1434167392345</v>
+        <v>3200</v>
       </c>
       <c r="T43" s="7">
-        <v>6298.6649574898875</v>
+        <v>3450</v>
       </c>
       <c r="U43" s="7">
-        <v>6328.6321921072949</v>
+        <v>3650</v>
       </c>
       <c r="V43" s="7">
-        <v>6344.049131836261</v>
+        <v>3900</v>
       </c>
       <c r="W43" s="7">
-        <v>6379.9198240227852</v>
+        <v>4100</v>
       </c>
       <c r="X43" s="7">
-        <v>6400</v>
+        <v>4350</v>
       </c>
       <c r="Y43" s="7">
-        <v>6400.0000000000309</v>
+        <v>4550</v>
       </c>
       <c r="Z43" s="7">
-        <v>6400</v>
+        <v>4800</v>
       </c>
       <c r="AA43" s="8">
-        <v>6399.9999999999827</v>
+        <v>5000</v>
       </c>
       <c r="AB43" t="s">
         <v>15</v>
@@ -4133,82 +4133,82 @@
         <v>42</v>
       </c>
       <c r="B44" s="6">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="C44" s="7">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="D44" s="7">
-        <v>560</v>
+        <v>0</v>
       </c>
       <c r="E44" s="7">
-        <v>720</v>
+        <v>0</v>
       </c>
       <c r="F44" s="7">
-        <v>780</v>
+        <v>0</v>
       </c>
       <c r="G44" s="7">
-        <v>820</v>
+        <v>0</v>
       </c>
       <c r="H44" s="7">
-        <v>880</v>
+        <v>0</v>
       </c>
       <c r="I44" s="7">
-        <v>910</v>
+        <v>0</v>
       </c>
       <c r="J44" s="7">
-        <v>960</v>
+        <v>0</v>
       </c>
       <c r="K44" s="7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L44" s="7">
-        <v>1050</v>
+        <v>0</v>
       </c>
       <c r="M44" s="7">
-        <v>1090</v>
+        <v>0</v>
       </c>
       <c r="N44" s="7">
-        <v>1140</v>
+        <v>0</v>
       </c>
       <c r="O44" s="7">
-        <v>1180</v>
+        <v>0</v>
       </c>
       <c r="P44" s="7">
-        <v>1230</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="7">
-        <v>1270</v>
+        <v>0</v>
       </c>
       <c r="R44" s="7">
-        <v>1320</v>
+        <v>0</v>
       </c>
       <c r="S44" s="7">
-        <v>1360</v>
+        <v>0</v>
       </c>
       <c r="T44" s="7">
-        <v>1420</v>
+        <v>0</v>
       </c>
       <c r="U44" s="7">
-        <v>1460</v>
+        <v>0</v>
       </c>
       <c r="V44" s="7">
-        <v>1530</v>
+        <v>0</v>
       </c>
       <c r="W44" s="7">
-        <v>1560</v>
+        <v>0</v>
       </c>
       <c r="X44" s="7">
-        <v>1620</v>
+        <v>0</v>
       </c>
       <c r="Y44" s="7">
-        <v>1689.9999999999902</v>
+        <v>0</v>
       </c>
       <c r="Z44" s="7">
-        <v>1830</v>
+        <v>0</v>
       </c>
       <c r="AA44" s="8">
-        <v>1928.6405127167338</v>
+        <v>0</v>
       </c>
       <c r="AB44" t="s">
         <v>16</v>
@@ -7984,82 +7984,82 @@
         <v>1</v>
       </c>
       <c r="B95" s="3">
-        <v>-1100.0000000000007</v>
+        <v>134.59011842103195</v>
       </c>
       <c r="C95" s="4">
-        <v>-1100</v>
+        <v>321.81666666666609</v>
       </c>
       <c r="D95" s="4">
-        <v>-1100</v>
+        <v>389.57841108032937</v>
       </c>
       <c r="E95" s="4">
-        <v>-1100</v>
+        <v>445.3803443500006</v>
       </c>
       <c r="F95" s="4">
-        <v>-1100</v>
+        <v>630.82005026299237</v>
       </c>
       <c r="G95" s="4">
-        <v>-1100</v>
+        <v>988.85720646479035</v>
       </c>
       <c r="H95" s="4">
-        <v>-1098.1931785417196</v>
+        <v>846.83951964716641</v>
       </c>
       <c r="I95" s="4">
-        <v>-1100</v>
+        <v>762.8852761892947</v>
       </c>
       <c r="J95" s="4">
-        <v>-1098.0924139029312</v>
+        <v>665.82177982875544</v>
       </c>
       <c r="K95" s="4">
-        <v>-1100</v>
+        <v>626.12404029153049</v>
       </c>
       <c r="L95" s="4">
-        <v>-1100</v>
+        <v>505.05639941523714</v>
       </c>
       <c r="M95" s="4">
-        <v>-1100</v>
+        <v>442.73926845512881</v>
       </c>
       <c r="N95" s="4">
-        <v>-1100</v>
+        <v>370.08661134315946</v>
       </c>
       <c r="O95" s="4">
-        <v>-1100</v>
+        <v>287.70192501486963</v>
       </c>
       <c r="P95" s="4">
-        <v>-1100</v>
+        <v>196.15656609734845</v>
       </c>
       <c r="Q95" s="4">
-        <v>-1100</v>
+        <v>165.71499815071491</v>
       </c>
       <c r="R95" s="4">
-        <v>-1099.9576037401812</v>
+        <v>57.442396259817713</v>
       </c>
       <c r="S95" s="4">
-        <v>-1100</v>
+        <v>-41.526512318802133</v>
       </c>
       <c r="T95" s="4">
-        <v>-1100</v>
+        <v>-177.93212082638343</v>
       </c>
       <c r="U95" s="4">
-        <v>-1100</v>
+        <v>-239.68408793039612</v>
       </c>
       <c r="V95" s="4">
-        <v>-1100</v>
+        <v>-332.28171754239173</v>
       </c>
       <c r="W95" s="4">
-        <v>-1100</v>
+        <v>-375.11101945637859</v>
       </c>
       <c r="X95" s="4">
-        <v>-1099.1677650406721</v>
+        <v>-468.4286798253595</v>
       </c>
       <c r="Y95" s="4">
-        <v>-1087.9741082593891</v>
+        <v>-540.35590361158188</v>
       </c>
       <c r="Z95" s="4">
-        <v>-1099.8030419003735</v>
+        <v>-624.09898603320789</v>
       </c>
       <c r="AA95" s="5">
-        <v>-1097.5319401830441</v>
+        <v>-635.81607690750707</v>
       </c>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.35">
@@ -8067,82 +8067,82 @@
         <v>2</v>
       </c>
       <c r="B96" s="6">
-        <v>1559.5499999999995</v>
+        <v>-371.30988157896832</v>
       </c>
       <c r="C96" s="7">
-        <v>1530.5749999999998</v>
+        <v>-221.68333333333345</v>
       </c>
       <c r="D96" s="7">
-        <v>1486.6992249999996</v>
+        <v>-241.3899805401652</v>
       </c>
       <c r="E96" s="7">
-        <v>1417.9235680249994</v>
+        <v>-291.56660415000079</v>
       </c>
       <c r="F96" s="7">
-        <v>1399.2489301372245</v>
+        <v>-584.15346921503317</v>
       </c>
       <c r="G96" s="7">
-        <v>1390.6762205084592</v>
+        <v>-712.60342355937803</v>
       </c>
       <c r="H96" s="7">
-        <v>1371.302945763895</v>
+        <v>-537.56435604721969</v>
       </c>
       <c r="I96" s="7">
-        <v>1368.8402637014724</v>
+        <v>-354.75833438633958</v>
       </c>
       <c r="J96" s="7">
-        <v>1354.6250830262511</v>
+        <v>-185.36072324206077</v>
       </c>
       <c r="K96" s="7">
-        <v>1347.4231359594585</v>
+        <v>-8.8992053069225676</v>
       </c>
       <c r="L96" s="7">
-        <v>1334.3739941830934</v>
+        <v>135.8878446063984</v>
       </c>
       <c r="M96" s="7">
-        <v>1326.4324101307411</v>
+        <v>289.11809665301087</v>
       </c>
       <c r="N96" s="7">
-        <v>1313.5993518219175</v>
+        <v>431.70274899482308</v>
       </c>
       <c r="O96" s="7">
-        <v>1305.8757959883146</v>
+        <v>564.2425079053985</v>
       </c>
       <c r="P96" s="7">
-        <v>1293.2627281522095</v>
+        <v>687.30591423389239</v>
       </c>
       <c r="Q96" s="7">
-        <v>1285.7611427055792</v>
+        <v>821.15459042048826</v>
       </c>
       <c r="R96" s="7">
-        <v>1273.3508448600198</v>
+        <v>926.85084486001972</v>
       </c>
       <c r="S96" s="7">
-        <v>1266.0964413768384</v>
+        <v>1041.5265123188021</v>
       </c>
       <c r="T96" s="7">
-        <v>1248.9353593492299</v>
+        <v>1118.4382810329596</v>
       </c>
       <c r="U96" s="7">
-        <v>1241.8898275833728</v>
+        <v>1219.6735475456815</v>
       </c>
       <c r="V96" s="7">
-        <v>1219.960886031623</v>
+        <v>1275.7969613433925</v>
       </c>
       <c r="W96" s="7">
-        <v>1218.1495840059074</v>
+        <v>1350.1509669076947</v>
       </c>
       <c r="X96" s="7">
-        <v>1201.0408627822962</v>
+        <v>1423.8799479976101</v>
       </c>
       <c r="Y96" s="7">
-        <v>1173.8711972140172</v>
+        <v>1512.4120948901086</v>
       </c>
       <c r="Z96" s="7">
-        <v>1123.3336713222634</v>
+        <v>1624.0989860332079</v>
       </c>
       <c r="AA96" s="8">
-        <v>1086.5478034585801</v>
+        <v>1635.8160769075071</v>
       </c>
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.35">
@@ -8150,82 +8150,82 @@
         <v>3</v>
       </c>
       <c r="B97" s="9">
-        <v>-459.54999999999882</v>
+        <v>236.71976315793634</v>
       </c>
       <c r="C97" s="10">
-        <v>-430.57499999999982</v>
+        <v>-100.13333333333259</v>
       </c>
       <c r="D97" s="10">
-        <v>-386.69922499999961</v>
+        <v>-148.18843054016418</v>
       </c>
       <c r="E97" s="10">
-        <v>-317.92356802499944</v>
+        <v>-153.81374019999981</v>
       </c>
       <c r="F97" s="10">
-        <v>-299.24893013722408</v>
+        <v>-46.666581047959198</v>
       </c>
       <c r="G97" s="10">
-        <v>-290.67622050845921</v>
+        <v>-276.25378290541232</v>
       </c>
       <c r="H97" s="10">
-        <v>-273.10976722217526</v>
+        <v>-309.27516359994678</v>
       </c>
       <c r="I97" s="10">
-        <v>-268.8402637014724</v>
+        <v>-408.12694180295512</v>
       </c>
       <c r="J97" s="10">
-        <v>-256.53266912331992</v>
+        <v>-480.46105658669467</v>
       </c>
       <c r="K97" s="10">
-        <v>-247.42313595945848</v>
+        <v>-617.22483498460792</v>
       </c>
       <c r="L97" s="10">
-        <v>-234.37399418309337</v>
+        <v>-640.94424402163554</v>
       </c>
       <c r="M97" s="10">
-        <v>-226.43241013074112</v>
+        <v>-731.85736510813967</v>
       </c>
       <c r="N97" s="10">
-        <v>-213.59935182191748</v>
+        <v>-801.78936033798254</v>
       </c>
       <c r="O97" s="10">
-        <v>-205.87579598831462</v>
+        <v>-851.94443292026813</v>
       </c>
       <c r="P97" s="10">
-        <v>-193.26272815220955</v>
+        <v>-883.46248033124084</v>
       </c>
       <c r="Q97" s="10">
-        <v>-185.76114270557923</v>
+        <v>-986.86958857120317</v>
       </c>
       <c r="R97" s="10">
-        <v>-173.39324111983865</v>
+        <v>-984.29324111983738</v>
       </c>
       <c r="S97" s="10">
-        <v>-166.09644137683836</v>
+        <v>-1000</v>
       </c>
       <c r="T97" s="10">
-        <v>-148.93535934922988</v>
+        <v>-940.50616020657617</v>
       </c>
       <c r="U97" s="10">
-        <v>-141.88982758337283</v>
+        <v>-979.98945961528545</v>
       </c>
       <c r="V97" s="10">
-        <v>-119.96088603162298</v>
+        <v>-943.51524380100068</v>
       </c>
       <c r="W97" s="10">
-        <v>-118.1495840059074</v>
+        <v>-975.03994745131627</v>
       </c>
       <c r="X97" s="10">
-        <v>-101.87309774162418</v>
+        <v>-955.45126817225048</v>
       </c>
       <c r="Y97" s="10">
-        <v>-85.897088954628202</v>
+        <v>-972.05619127852651</v>
       </c>
       <c r="Z97" s="10">
-        <v>-23.530629421889898</v>
+        <v>-1000</v>
       </c>
       <c r="AA97" s="11">
-        <v>10.984136724463951</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.35">
@@ -8575,86 +8575,86 @@
         <v>6</v>
       </c>
       <c r="B106" s="15">
-        <v>419066448.64103276</v>
+        <v>185343.29577303529</v>
       </c>
       <c r="C106" s="16">
-        <v>125273086.48681155</v>
+        <v>150354.42590554885</v>
       </c>
       <c r="D106" s="16">
-        <v>121082739.88063765</v>
+        <v>122850.988578766</v>
       </c>
       <c r="E106" s="16">
-        <v>120287243.3532899</v>
+        <v>115767.04458876402</v>
       </c>
       <c r="F106" s="16">
-        <v>101061042.67947546</v>
+        <v>110839.76863109926</v>
       </c>
       <c r="G106" s="16">
-        <v>91054722.542002589</v>
+        <v>107601.08884452145</v>
       </c>
       <c r="H106" s="16">
-        <v>85756835.58219102</v>
+        <v>11641550.231811121</v>
       </c>
       <c r="I106" s="16">
-        <v>77835636.33026889</v>
+        <v>12324968.133583765</v>
       </c>
       <c r="J106" s="16">
-        <v>72095477.491315469</v>
+        <v>13729770.539331574</v>
       </c>
       <c r="K106" s="16">
-        <v>66837002.123430684</v>
+        <v>13539056.792083366</v>
       </c>
       <c r="L106" s="16">
-        <v>61305279.967726842</v>
+        <v>15173431.935465464</v>
       </c>
       <c r="M106" s="16">
-        <v>56802866.981785446</v>
+        <v>14667613.021367956</v>
       </c>
       <c r="N106" s="16">
-        <v>52088861.87211591</v>
+        <v>14771698.232724916</v>
       </c>
       <c r="O106" s="16">
-        <v>48238464.927511126</v>
+        <v>14735518.731834156</v>
       </c>
       <c r="P106" s="16">
-        <v>44224961.578445897</v>
+        <v>14583734.508809622</v>
       </c>
       <c r="Q106" s="16">
-        <v>40935877.731673487</v>
+        <v>13638852.26087979</v>
       </c>
       <c r="R106" s="16">
-        <v>37521716.813343227</v>
+        <v>13819966.051143175</v>
       </c>
       <c r="S106" s="16">
-        <v>34715087.464546926</v>
+        <v>13455936.071670964</v>
       </c>
       <c r="T106" s="16">
-        <v>32145404.736540187</v>
+        <v>13043632.510209475</v>
       </c>
       <c r="U106" s="16">
-        <v>29485302.677763384</v>
+        <v>12117802.26314237</v>
       </c>
       <c r="V106" s="16">
-        <v>27563924.879889011</v>
+        <v>11986589.48512092</v>
       </c>
       <c r="W106" s="16">
-        <v>24829028.306883618</v>
+        <v>11111677.895684551</v>
       </c>
       <c r="X106" s="16">
-        <v>23150557.073793795</v>
+        <v>10903515.051872116</v>
       </c>
       <c r="Y106" s="16">
-        <v>21517631.109444827</v>
+        <v>10089854.202114003</v>
       </c>
       <c r="Z106" s="16">
-        <v>21155858.060010906</v>
+        <v>9835330.0367435943</v>
       </c>
       <c r="AA106" s="17">
-        <v>19062229.216091473</v>
+        <v>9087917.6781258415</v>
       </c>
       <c r="AB106" s="18">
         <f>SUM(TotalCost)</f>
-        <v>1855093288.5080221</v>
+        <v>255051172.24604046</v>
       </c>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.35">
@@ -8922,86 +8922,86 @@
         <v>10</v>
       </c>
       <c r="B111" s="6">
-        <v>106950.48810000002</v>
+        <v>81864043753.466522</v>
       </c>
       <c r="C111" s="7">
-        <v>90435.657349999659</v>
+        <v>77448100759.699539</v>
       </c>
       <c r="D111" s="7">
-        <v>61389.24192324945</v>
+        <v>73270364329.279526</v>
       </c>
       <c r="E111" s="7">
-        <v>13084.016274990165</v>
+        <v>69317985028.483795</v>
       </c>
       <c r="F111" s="7">
-        <v>5436.8218239150356</v>
+        <v>65578806552.883316</v>
       </c>
       <c r="G111" s="7">
-        <v>5517.3968037802724</v>
+        <v>62041328338.285065</v>
       </c>
       <c r="H111" s="7">
-        <v>5129.9428568130952</v>
+        <v>58694670188.529953</v>
       </c>
       <c r="I111" s="7">
-        <v>5386.7833627604405</v>
+        <v>55528538811.352196</v>
       </c>
       <c r="J111" s="7">
-        <v>5364.476219924034</v>
+        <v>52533196159.37471</v>
       </c>
       <c r="K111" s="7">
-        <v>5307.4527286085349</v>
+        <v>49699429478.867256</v>
       </c>
       <c r="L111" s="7">
-        <v>5122.480076615986</v>
+        <v>47018522974.146408</v>
       </c>
       <c r="M111" s="7">
-        <v>5280.3321457556458</v>
+        <v>44482231000.465813</v>
       </c>
       <c r="N111" s="7">
-        <v>5121.8174635172782</v>
+        <v>42082752702.946281</v>
       </c>
       <c r="O111" s="7">
-        <v>5306.3656241389235</v>
+        <v>39812708023.54287</v>
       </c>
       <c r="P111" s="7">
-        <v>5174.7872982061763</v>
+        <v>37665115002.253708</v>
       </c>
       <c r="Q111" s="7">
-        <v>5386.5142423400121</v>
+        <v>35633368302.756134</v>
       </c>
       <c r="R111" s="7">
-        <v>5286.5521506802152</v>
+        <v>33711218896.421543</v>
       </c>
       <c r="S111" s="7">
-        <v>5521.7564562017669</v>
+        <v>31892754842.223217</v>
       </c>
       <c r="T111" s="7">
-        <v>5115.8657577575705</v>
+        <v>30172383103.422077</v>
       </c>
       <c r="U111" s="7">
-        <v>5383.433413027381</v>
+        <v>28544812345.104042</v>
       </c>
       <c r="V111" s="7">
-        <v>4676.311757194595</v>
+        <v>27005036659.659504</v>
       </c>
       <c r="W111" s="7">
-        <v>5302.2142714593301</v>
+        <v>25548320170.14949</v>
       </c>
       <c r="X111" s="7">
-        <v>5035.9907180076143</v>
+        <v>24170182464.20322</v>
       </c>
       <c r="Y111" s="7">
-        <v>5479.4851296682418</v>
+        <v>22866384813.646187</v>
       </c>
       <c r="Z111" s="7">
-        <v>1353.337521036605</v>
+        <v>21632917137.47456</v>
       </c>
       <c r="AA111" s="8">
-        <v>0</v>
+        <v>20320549313.578232</v>
       </c>
       <c r="AB111" s="13">
         <f t="shared" si="0"/>
-        <v>378549.52146964805</v>
+        <v>1158535721152.2151</v>
       </c>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Readded non  GHG emissions dvars
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105:XFD105"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC61" sqref="AC61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added back 0 emissions in 2045 goal
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -742,55 +742,55 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>495.91917837745336</v>
+        <v>476.58096263725793</v>
       </c>
       <c r="H3" s="4">
-        <v>396.80584595542905</v>
+        <v>377.70348649885864</v>
       </c>
       <c r="I3" s="4">
-        <v>421.67530116494049</v>
+        <v>403.60336882312225</v>
       </c>
       <c r="J3" s="4">
-        <v>407.00758733669346</v>
+        <v>389.91049839803054</v>
       </c>
       <c r="K3" s="4">
-        <v>514.22584895567297</v>
+        <v>498.05101802737397</v>
       </c>
       <c r="L3" s="4">
-        <v>427.12120987952324</v>
+        <v>411.81888815109181</v>
       </c>
       <c r="M3" s="4">
-        <v>466.0529851039019</v>
+        <v>451.57610733507386</v>
       </c>
       <c r="N3" s="4">
-        <v>473.76113038564114</v>
+        <v>460.06517014817018</v>
       </c>
       <c r="O3" s="4">
-        <v>452.05418306797816</v>
+        <v>439.09701579602063</v>
       </c>
       <c r="P3" s="4">
-        <v>402.64424198762578</v>
+        <v>390.38601541551873</v>
       </c>
       <c r="Q3" s="4">
-        <v>486.3227090409859</v>
+        <v>474.72572062992197</v>
       </c>
       <c r="R3" s="4">
-        <v>386.28310279959442</v>
+        <v>375.31168377619593</v>
       </c>
       <c r="S3" s="4">
-        <v>419.45037015797988</v>
+        <v>435.1396077248308</v>
       </c>
       <c r="T3" s="4">
-        <v>129.03291882238901</v>
+        <v>243.2736785125249</v>
       </c>
       <c r="U3" s="4">
-        <v>117.8680810420648</v>
+        <v>78.059328724960324</v>
       </c>
       <c r="V3" s="4">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="W3" s="4">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="X3" s="4">
         <v>0</v>
@@ -813,10 +813,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>130.26735234474813</v>
+        <v>149.65758779767953</v>
       </c>
       <c r="D4" s="7">
-        <v>641.05189162049328</v>
+        <v>606.04188169903796</v>
       </c>
       <c r="E4" s="7">
         <v>665.6</v>
@@ -885,7 +885,7 @@
         <v>665.6</v>
       </c>
       <c r="AA4" s="8">
-        <v>665.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
@@ -944,7 +944,7 @@
         <v>46.5</v>
       </c>
       <c r="S5" s="7">
-        <v>42.477210131935919</v>
+        <v>26.787972565084999</v>
       </c>
       <c r="T5" s="7">
         <v>46.5</v>
@@ -959,16 +959,16 @@
         <v>46.5</v>
       </c>
       <c r="X5" s="7">
+        <v>34.372432155944182</v>
+      </c>
+      <c r="Y5" s="7">
         <v>46.5</v>
-      </c>
-      <c r="Y5" s="7">
-        <v>7</v>
       </c>
       <c r="Z5" s="7">
         <v>46.5</v>
       </c>
       <c r="AA5" s="8">
-        <v>46.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
@@ -1051,7 +1051,7 @@
         <v>212</v>
       </c>
       <c r="AA6" s="8">
-        <v>212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
@@ -1059,7 +1059,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>192.67035526309559</v>
+        <v>183.18806320476443</v>
       </c>
       <c r="C7" s="7">
         <v>464</v>
@@ -1134,7 +1134,7 @@
         <v>464</v>
       </c>
       <c r="AA7" s="8">
-        <v>464</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
@@ -1205,7 +1205,7 @@
         <v>101.5</v>
       </c>
       <c r="W8" s="7">
-        <v>101.5</v>
+        <v>38.087889959491179</v>
       </c>
       <c r="X8" s="7">
         <v>0</v>
@@ -1294,13 +1294,13 @@
         <v>84.6</v>
       </c>
       <c r="Y9" s="7">
-        <v>80.286696024931487</v>
+        <v>84.6</v>
       </c>
       <c r="Z9" s="7">
         <v>84.6</v>
       </c>
       <c r="AA9" s="8">
-        <v>84.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
@@ -1377,10 +1377,10 @@
         <v>88</v>
       </c>
       <c r="Y10" s="7">
-        <v>88</v>
+        <v>85.513755621297207</v>
       </c>
       <c r="Z10" s="7">
-        <v>0</v>
+        <v>16.480629421888807</v>
       </c>
       <c r="AA10" s="8">
         <v>0</v>
@@ -1466,7 +1466,7 @@
         <v>650</v>
       </c>
       <c r="AA11" s="8">
-        <v>650</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
@@ -1549,7 +1549,7 @@
         <v>186</v>
       </c>
       <c r="AA12" s="8">
-        <v>186</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
@@ -1617,13 +1617,13 @@
         <v>154</v>
       </c>
       <c r="V13" s="7">
-        <v>90.066924690421729</v>
+        <v>126.02157994994678</v>
       </c>
       <c r="W13" s="7">
-        <v>44.932226380951619</v>
+        <v>0</v>
       </c>
       <c r="X13" s="7">
-        <v>0</v>
+        <v>130.41031219811521</v>
       </c>
       <c r="Y13" s="7">
         <v>0</v>
@@ -1646,7 +1646,7 @@
         <v>150</v>
       </c>
       <c r="D14" s="7">
-        <v>85.515108379504568</v>
+        <v>120.52511830096</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -1712,7 +1712,7 @@
         <v>150</v>
       </c>
       <c r="Z14" s="7">
-        <v>132.96125884377807</v>
+        <v>150</v>
       </c>
       <c r="AA14" s="8">
         <v>0</v>
@@ -1732,10 +1732,10 @@
         <v>1848</v>
       </c>
       <c r="E15" s="7">
-        <v>1254.6797472637372</v>
+        <v>1267.9555255442688</v>
       </c>
       <c r="F15" s="7">
-        <v>607.8377094854726</v>
+        <v>621.3425041496821</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>604.92635573625898</v>
+        <v>591.65057745572744</v>
       </c>
       <c r="F16" s="7">
         <v>656.1</v>
@@ -1875,13 +1875,13 @@
         <v>656.1</v>
       </c>
       <c r="Y16" s="7">
-        <v>654.92269302831357</v>
+        <v>656.1</v>
       </c>
       <c r="Z16" s="7">
         <v>656.1</v>
       </c>
       <c r="AA16" s="8">
-        <v>651.55241017337175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
@@ -1901,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="7">
-        <v>24.084748441522727</v>
+        <v>10.579953777313113</v>
       </c>
       <c r="G17" s="7">
         <v>50.3</v>
@@ -2047,7 +2047,7 @@
         <v>67</v>
       </c>
       <c r="AA18" s="8">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
@@ -2070,7 +2070,7 @@
         <v>257</v>
       </c>
       <c r="G19" s="7">
-        <v>152.50208167088411</v>
+        <v>171.84029741107952</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
@@ -2109,25 +2109,25 @@
         <v>257</v>
       </c>
       <c r="T19" s="7">
-        <v>243.3262774589235</v>
+        <v>169.08551776878789</v>
       </c>
       <c r="U19" s="7">
-        <v>128.51664800577814</v>
+        <v>158.32540032288381</v>
       </c>
       <c r="V19" s="7">
-        <v>135.00956691885131</v>
+        <v>61.054911659326535</v>
       </c>
       <c r="W19" s="7">
-        <v>55.508253652803575</v>
+        <v>75.852590074264299</v>
       </c>
       <c r="X19" s="7">
-        <v>79.064458690961544</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="7">
-        <v>0</v>
+        <v>47.218760842125732</v>
       </c>
       <c r="Z19" s="7">
-        <v>65.354925502311204</v>
+        <v>0</v>
       </c>
       <c r="AA19" s="8">
         <v>0</v>
@@ -2156,37 +2156,37 @@
         <v>2269.6</v>
       </c>
       <c r="H20" s="7">
-        <v>2237.1019054333428</v>
+        <v>2256.2042648899132</v>
       </c>
       <c r="I20" s="7">
-        <v>1978.7119199863289</v>
+        <v>1996.7838523281471</v>
       </c>
       <c r="J20" s="7">
-        <v>1760.4574188049367</v>
+        <v>1777.5545077435995</v>
       </c>
       <c r="K20" s="7">
-        <v>1470.9206422412312</v>
+        <v>1487.0954731695301</v>
       </c>
       <c r="L20" s="7">
-        <v>1326.3158997381524</v>
+        <v>1341.6182214665837</v>
       </c>
       <c r="M20" s="7">
-        <v>1106.2893585003312</v>
+        <v>1120.7662362691592</v>
       </c>
       <c r="N20" s="7">
-        <v>918.10659431102886</v>
+        <v>931.80255454849976</v>
       </c>
       <c r="O20" s="7">
-        <v>759.96465115096225</v>
+        <v>772.92181842291973</v>
       </c>
       <c r="P20" s="7">
-        <v>630.15706173928538</v>
+        <v>642.41528831139237</v>
       </c>
       <c r="Q20" s="7">
-        <v>417.89810641946548</v>
+        <v>429.49509483052941</v>
       </c>
       <c r="R20" s="7">
-        <v>340</v>
+        <v>350.97141902339848</v>
       </c>
       <c r="S20" s="7">
         <v>0</v>
@@ -2221,7 +2221,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>15.829644736904577</v>
+        <v>25.311936795235738</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2370,16 +2370,16 @@
         <v>398.3</v>
       </c>
       <c r="X22" s="7">
-        <v>397.51828566309774</v>
+        <v>398.3</v>
       </c>
       <c r="Y22" s="7">
-        <v>398.3</v>
+        <v>298.5768725898219</v>
       </c>
       <c r="Z22" s="7">
-        <v>220.4103892086342</v>
+        <v>292.24594413283495</v>
       </c>
       <c r="AA22" s="8">
-        <v>301.38810254334294</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
@@ -2393,13 +2393,13 @@
         <v>0</v>
       </c>
       <c r="D23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="E23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="F23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="G23" s="7">
         <v>28.100000000000009</v>
@@ -2408,61 +2408,61 @@
         <v>28.100000000000009</v>
       </c>
       <c r="I23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="J23" s="7">
         <v>28.100000000000009</v>
       </c>
       <c r="K23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="L23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="M23" s="7">
         <v>28.100000000000009</v>
       </c>
       <c r="N23" s="7">
+        <v>28.100000000000009</v>
+      </c>
+      <c r="O23" s="7">
         <v>28.1</v>
-      </c>
-      <c r="O23" s="7">
-        <v>28.099999999999994</v>
       </c>
       <c r="P23" s="7">
         <v>28.1</v>
       </c>
       <c r="Q23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="R23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="S23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="T23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="U23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="V23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="W23" s="7">
         <v>28.100000000000009</v>
       </c>
-      <c r="R23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="S23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="T23" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="U23" s="7">
+      <c r="X23" s="7">
         <v>28.100000000000009</v>
-      </c>
-      <c r="V23" s="7">
-        <v>28.100000000000009</v>
-      </c>
-      <c r="W23" s="7">
-        <v>28.099999999999994</v>
-      </c>
-      <c r="X23" s="7">
-        <v>28.1</v>
       </c>
       <c r="Y23" s="7">
         <v>28.1</v>
       </c>
       <c r="Z23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="AA23" s="8">
-        <v>28.100000000000009</v>
+        <v>28.1</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="7">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D24" s="7">
         <v>25</v>
@@ -2556,7 +2556,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="7">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D25" s="7">
         <v>70</v>
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="7">
-        <v>0</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="D26" s="7">
         <v>30.6</v>
@@ -2654,19 +2654,19 @@
         <v>30.6</v>
       </c>
       <c r="H26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="I26" s="7">
         <v>30.6</v>
       </c>
       <c r="J26" s="7">
+        <v>30.6</v>
+      </c>
+      <c r="K26" s="7">
+        <v>30.6</v>
+      </c>
+      <c r="L26" s="7">
         <v>30.599999999999998</v>
-      </c>
-      <c r="K26" s="7">
-        <v>30.599999999999998</v>
-      </c>
-      <c r="L26" s="7">
-        <v>30.6</v>
       </c>
       <c r="M26" s="7">
         <v>30.6</v>
@@ -2678,10 +2678,10 @@
         <v>30.6</v>
       </c>
       <c r="P26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="Q26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="R26" s="7">
         <v>30.6</v>
@@ -2690,10 +2690,10 @@
         <v>30.6</v>
       </c>
       <c r="T26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="U26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="V26" s="7">
         <v>30.6</v>
@@ -2705,10 +2705,10 @@
         <v>30.6</v>
       </c>
       <c r="Y26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="Z26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="AA26" s="8">
         <v>30.6</v>
@@ -2722,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D27" s="7">
         <v>10</v>
@@ -2758,7 +2758,7 @@
         <v>10</v>
       </c>
       <c r="O27" s="7">
-        <v>10</v>
+        <v>10.000000000000014</v>
       </c>
       <c r="P27" s="7">
         <v>10</v>
@@ -2770,10 +2770,10 @@
         <v>10</v>
       </c>
       <c r="S27" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="T27" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="U27" s="7">
         <v>10</v>
@@ -2785,7 +2785,7 @@
         <v>10</v>
       </c>
       <c r="X27" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="Y27" s="7">
         <v>10</v>
@@ -2829,10 +2829,10 @@
         <v>10</v>
       </c>
       <c r="K28" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="L28" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="M28" s="7">
         <v>10</v>
@@ -2841,7 +2841,7 @@
         <v>10</v>
       </c>
       <c r="O28" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="P28" s="7">
         <v>10</v>
@@ -2862,7 +2862,7 @@
         <v>10</v>
       </c>
       <c r="V28" s="7">
-        <v>10</v>
+        <v>10.000000000000014</v>
       </c>
       <c r="W28" s="7">
         <v>10</v>
@@ -2933,28 +2933,28 @@
         <v>10</v>
       </c>
       <c r="R29" s="7">
+        <v>10</v>
+      </c>
+      <c r="S29" s="7">
+        <v>10</v>
+      </c>
+      <c r="T29" s="7">
+        <v>10</v>
+      </c>
+      <c r="U29" s="7">
+        <v>10</v>
+      </c>
+      <c r="V29" s="7">
+        <v>10</v>
+      </c>
+      <c r="W29" s="7">
+        <v>10</v>
+      </c>
+      <c r="X29" s="7">
+        <v>10</v>
+      </c>
+      <c r="Y29" s="7">
         <v>9.9999999999999929</v>
-      </c>
-      <c r="S29" s="7">
-        <v>10</v>
-      </c>
-      <c r="T29" s="7">
-        <v>9.9999999999999929</v>
-      </c>
-      <c r="U29" s="7">
-        <v>10</v>
-      </c>
-      <c r="V29" s="7">
-        <v>10</v>
-      </c>
-      <c r="W29" s="7">
-        <v>10</v>
-      </c>
-      <c r="X29" s="7">
-        <v>10</v>
-      </c>
-      <c r="Y29" s="7">
-        <v>10</v>
       </c>
       <c r="Z29" s="7">
         <v>10</v>
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="7">
-        <v>0</v>
+        <v>52.2</v>
       </c>
       <c r="D30" s="7">
         <v>52.2</v>
@@ -2989,7 +2989,7 @@
         <v>52.2</v>
       </c>
       <c r="I30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="J30" s="7">
         <v>52.2</v>
@@ -2998,16 +2998,16 @@
         <v>52.2</v>
       </c>
       <c r="L30" s="7">
-        <v>52.2</v>
+        <v>52.20000000000001</v>
       </c>
       <c r="M30" s="7">
         <v>52.2</v>
       </c>
       <c r="N30" s="7">
-        <v>52.20000000000001</v>
+        <v>52.2</v>
       </c>
       <c r="O30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="P30" s="7">
         <v>52.20000000000001</v>
@@ -3019,31 +3019,31 @@
         <v>52.200000000000017</v>
       </c>
       <c r="S30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="T30" s="7">
         <v>52.2</v>
       </c>
       <c r="U30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="V30" s="7">
         <v>52.2</v>
       </c>
       <c r="W30" s="7">
+        <v>52.2</v>
+      </c>
+      <c r="X30" s="7">
+        <v>52.2</v>
+      </c>
+      <c r="Y30" s="7">
         <v>52.200000000000017</v>
-      </c>
-      <c r="X30" s="7">
-        <v>52.200000000000017</v>
-      </c>
-      <c r="Y30" s="7">
-        <v>52.20000000000001</v>
       </c>
       <c r="Z30" s="7">
         <v>52.200000000000017</v>
       </c>
       <c r="AA30" s="8">
-        <v>52.2</v>
+        <v>52.20000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.35">
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="7">
-        <v>0</v>
+        <v>1.4424122023189199</v>
       </c>
       <c r="D31" s="7">
         <v>10</v>
@@ -3102,28 +3102,28 @@
         <v>10</v>
       </c>
       <c r="S31" s="7">
+        <v>10</v>
+      </c>
+      <c r="T31" s="7">
+        <v>10</v>
+      </c>
+      <c r="U31" s="7">
+        <v>10</v>
+      </c>
+      <c r="V31" s="7">
+        <v>10</v>
+      </c>
+      <c r="W31" s="7">
+        <v>10</v>
+      </c>
+      <c r="X31" s="7">
+        <v>10</v>
+      </c>
+      <c r="Y31" s="7">
+        <v>10</v>
+      </c>
+      <c r="Z31" s="7">
         <v>9.9999999999999929</v>
-      </c>
-      <c r="T31" s="7">
-        <v>10.000000000000014</v>
-      </c>
-      <c r="U31" s="7">
-        <v>10</v>
-      </c>
-      <c r="V31" s="7">
-        <v>10</v>
-      </c>
-      <c r="W31" s="7">
-        <v>10</v>
-      </c>
-      <c r="X31" s="7">
-        <v>10</v>
-      </c>
-      <c r="Y31" s="7">
-        <v>10</v>
-      </c>
-      <c r="Z31" s="7">
-        <v>10</v>
       </c>
       <c r="AA31" s="8">
         <v>10</v>
@@ -3137,37 +3137,37 @@
         <v>0</v>
       </c>
       <c r="C32" s="7">
-        <v>0</v>
+        <v>20.2</v>
       </c>
       <c r="D32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="E32" s="7">
         <v>20.200000000000003</v>
       </c>
-      <c r="E32" s="7">
+      <c r="F32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="G32" s="7">
         <v>20.2</v>
       </c>
-      <c r="F32" s="7">
+      <c r="H32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="I32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="J32" s="7">
         <v>20.200000000000003</v>
       </c>
-      <c r="G32" s="7">
+      <c r="K32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="L32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="M32" s="7">
         <v>20.200000000000003</v>
-      </c>
-      <c r="H32" s="7">
-        <v>20.199999999999996</v>
-      </c>
-      <c r="I32" s="7">
-        <v>20.2</v>
-      </c>
-      <c r="J32" s="7">
-        <v>20.2</v>
-      </c>
-      <c r="K32" s="7">
-        <v>20.2</v>
-      </c>
-      <c r="L32" s="7">
-        <v>20.199999999999996</v>
-      </c>
-      <c r="M32" s="7">
-        <v>20.199999999999996</v>
       </c>
       <c r="N32" s="7">
         <v>20.200000000000003</v>
@@ -3179,34 +3179,34 @@
         <v>20.2</v>
       </c>
       <c r="Q32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="R32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="S32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="T32" s="7">
         <v>20.2</v>
       </c>
-      <c r="R32" s="7">
+      <c r="U32" s="7">
         <v>20.2</v>
       </c>
-      <c r="S32" s="7">
+      <c r="V32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="W32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="X32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="Y32" s="7">
         <v>20.2</v>
       </c>
-      <c r="T32" s="7">
-        <v>20.200000000000003</v>
-      </c>
-      <c r="U32" s="7">
-        <v>20.200000000000003</v>
-      </c>
-      <c r="V32" s="7">
-        <v>20.199999999999996</v>
-      </c>
-      <c r="W32" s="7">
+      <c r="Z32" s="7">
         <v>20.2</v>
-      </c>
-      <c r="X32" s="7">
-        <v>20.2</v>
-      </c>
-      <c r="Y32" s="7">
-        <v>20.199999999999996</v>
-      </c>
-      <c r="Z32" s="7">
-        <v>20.200000000000003</v>
       </c>
       <c r="AA32" s="8">
         <v>20.200000000000003</v>
@@ -3220,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="7">
-        <v>30.932647655250321</v>
+        <v>0</v>
       </c>
       <c r="D33" s="7">
         <v>70</v>
@@ -3306,13 +3306,13 @@
         <v>0</v>
       </c>
       <c r="D34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="E34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="F34" s="7">
-        <v>10.499999999999986</v>
+        <v>10.5</v>
       </c>
       <c r="G34" s="7">
         <v>10.5</v>
@@ -3345,7 +3345,7 @@
         <v>10.5</v>
       </c>
       <c r="Q34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999986</v>
       </c>
       <c r="R34" s="7">
         <v>10.5</v>
@@ -3443,7 +3443,7 @@
         <v>10</v>
       </c>
       <c r="V35" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="W35" s="7">
         <v>10</v>
@@ -3469,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D36" s="7">
         <v>10</v>
@@ -3552,7 +3552,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D37" s="7">
         <v>10</v>
@@ -3606,7 +3606,7 @@
         <v>10</v>
       </c>
       <c r="U37" s="7">
-        <v>10</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="V37" s="7">
         <v>10</v>
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D38" s="7">
         <v>10</v>
@@ -3650,7 +3650,7 @@
         <v>10</v>
       </c>
       <c r="H38" s="7">
-        <v>10</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="I38" s="7">
         <v>10</v>
@@ -3721,10 +3721,10 @@
         <v>0</v>
       </c>
       <c r="D39" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="E39" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="F39" s="7">
         <v>10.099999999999994</v>
@@ -3733,22 +3733,22 @@
         <v>10.099999999999994</v>
       </c>
       <c r="H39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="I39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="J39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="K39" s="7">
-        <v>10.1</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="L39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="M39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="N39" s="7">
         <v>10.099999999999994</v>
@@ -3772,16 +3772,16 @@
         <v>10.099999999999994</v>
       </c>
       <c r="U39" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="V39" s="7">
         <v>10.099999999999994</v>
-      </c>
-      <c r="V39" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="W39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="X39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="Y39" s="7">
         <v>10.099999999999994</v>
@@ -3801,58 +3801,58 @@
         <v>0</v>
       </c>
       <c r="C40" s="7">
-        <v>0</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="D40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="E40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="F40" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="E40" s="7">
+      <c r="G40" s="7">
         <v>10.099999999999998</v>
-      </c>
-      <c r="F40" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="G40" s="7">
-        <v>10.1</v>
       </c>
       <c r="H40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="I40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="J40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="K40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="L40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="M40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="N40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="O40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="P40" s="7">
         <v>10.099999999999998</v>
-      </c>
-      <c r="J40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="K40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="L40" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="M40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="N40" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="O40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="P40" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="Q40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="R40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.1</v>
       </c>
       <c r="S40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.1</v>
       </c>
       <c r="T40" s="7">
-        <v>10.1</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="U40" s="7">
         <v>10.100000000000001</v>
@@ -3861,16 +3861,16 @@
         <v>10.100000000000001</v>
       </c>
       <c r="W40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.1</v>
       </c>
       <c r="X40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.1</v>
       </c>
       <c r="Y40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="Z40" s="7">
-        <v>10.1</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="AA40" s="8">
         <v>10.100000000000001</v>
@@ -3967,7 +3967,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="7">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D42" s="7">
         <v>12</v>
@@ -4101,28 +4101,28 @@
         <v>3200</v>
       </c>
       <c r="T43" s="7">
-        <v>3450</v>
+        <v>3400</v>
       </c>
       <c r="U43" s="7">
         <v>3650</v>
       </c>
       <c r="V43" s="7">
-        <v>3900</v>
+        <v>3850</v>
       </c>
       <c r="W43" s="7">
         <v>4100</v>
       </c>
       <c r="X43" s="7">
-        <v>4350</v>
+        <v>4300</v>
       </c>
       <c r="Y43" s="7">
         <v>4550</v>
       </c>
       <c r="Z43" s="7">
-        <v>4800</v>
+        <v>4750</v>
       </c>
       <c r="AA43" s="8">
-        <v>5000</v>
+        <v>6398.6405127167163</v>
       </c>
       <c r="AB43" t="s">
         <v>15</v>
@@ -4187,28 +4187,28 @@
         <v>0</v>
       </c>
       <c r="T44" s="7">
-        <v>0</v>
+        <v>9.9999999999997158</v>
       </c>
       <c r="U44" s="7">
-        <v>0</v>
+        <v>9.9999999999997158</v>
       </c>
       <c r="V44" s="7">
-        <v>0</v>
+        <v>9.9999999999997158</v>
       </c>
       <c r="W44" s="7">
-        <v>0</v>
+        <v>9.9999999999997158</v>
       </c>
       <c r="X44" s="7">
-        <v>0</v>
+        <v>9.9999999999997158</v>
       </c>
       <c r="Y44" s="7">
-        <v>0</v>
+        <v>9.9999999999997158</v>
       </c>
       <c r="Z44" s="7">
-        <v>0</v>
+        <v>9.9999999999997158</v>
       </c>
       <c r="AA44" s="8">
-        <v>0</v>
+        <v>1929.9999999999998</v>
       </c>
       <c r="AB44" t="s">
         <v>16</v>
@@ -7984,82 +7984,82 @@
         <v>1</v>
       </c>
       <c r="B95" s="3">
-        <v>134.59011842103195</v>
+        <v>131.42935440158806</v>
       </c>
       <c r="C95" s="4">
-        <v>321.81666666666609</v>
+        <v>251.08839186511989</v>
       </c>
       <c r="D95" s="4">
-        <v>389.57841108032937</v>
+        <v>366.23840446602577</v>
       </c>
       <c r="E95" s="4">
-        <v>445.3803443500006</v>
+        <v>445.38034435000094</v>
       </c>
       <c r="F95" s="4">
-        <v>630.82005026299237</v>
+        <v>626.31845204158913</v>
       </c>
       <c r="G95" s="4">
-        <v>988.85720646479035</v>
+        <v>982.41113455139237</v>
       </c>
       <c r="H95" s="4">
-        <v>846.83951964716641</v>
+        <v>840.47206649497662</v>
       </c>
       <c r="I95" s="4">
-        <v>762.8852761892947</v>
+        <v>756.861298742023</v>
       </c>
       <c r="J95" s="4">
-        <v>665.82177982875544</v>
+        <v>660.12275018253445</v>
       </c>
       <c r="K95" s="4">
-        <v>626.12404029153049</v>
+        <v>620.73242998209753</v>
       </c>
       <c r="L95" s="4">
-        <v>505.05639941523714</v>
+        <v>499.95562550576005</v>
       </c>
       <c r="M95" s="4">
-        <v>442.73926845512881</v>
+        <v>437.91364253218552</v>
       </c>
       <c r="N95" s="4">
-        <v>370.08661134315946</v>
+        <v>365.52129126400195</v>
       </c>
       <c r="O95" s="4">
-        <v>287.70192501486963</v>
+        <v>283.38286925755017</v>
       </c>
       <c r="P95" s="4">
-        <v>196.15656609734845</v>
+        <v>192.07049057331278</v>
       </c>
       <c r="Q95" s="4">
-        <v>165.71499815071491</v>
+        <v>161.84933534702691</v>
       </c>
       <c r="R95" s="4">
-        <v>57.442396259817713</v>
+        <v>53.785256585351476</v>
       </c>
       <c r="S95" s="4">
         <v>-41.526512318802133</v>
       </c>
       <c r="T95" s="4">
-        <v>-177.93212082638343</v>
+        <v>-123.18520092967128</v>
       </c>
       <c r="U95" s="4">
-        <v>-239.68408793039612</v>
+        <v>-252.95367203609771</v>
       </c>
       <c r="V95" s="4">
-        <v>-332.28171754239173</v>
+        <v>-301.59993596223347</v>
       </c>
       <c r="W95" s="4">
-        <v>-375.11101945637859</v>
+        <v>-355.27098067623137</v>
       </c>
       <c r="X95" s="4">
-        <v>-468.4286798253595</v>
+        <v>-499.27463983941703</v>
       </c>
       <c r="Y95" s="4">
-        <v>-540.35590361158188</v>
+        <v>-526.97265273668881</v>
       </c>
       <c r="Z95" s="4">
-        <v>-624.09898603320789</v>
+        <v>-607.61835661131897</v>
       </c>
       <c r="AA95" s="5">
-        <v>-635.81607690750707</v>
+        <v>-1097.0787777552882</v>
       </c>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.35">
@@ -8067,82 +8067,82 @@
         <v>2</v>
       </c>
       <c r="B96" s="6">
-        <v>-371.30988157896832</v>
+        <v>-374.47064559841192</v>
       </c>
       <c r="C96" s="7">
-        <v>-221.68333333333345</v>
+        <v>-216.76919593256002</v>
       </c>
       <c r="D96" s="7">
-        <v>-241.3899805401652</v>
+        <v>-229.71997723301337</v>
       </c>
       <c r="E96" s="7">
-        <v>-291.56660415000079</v>
+        <v>-291.56660415000147</v>
       </c>
       <c r="F96" s="7">
-        <v>-584.15346921503317</v>
+        <v>-575.1502727722268</v>
       </c>
       <c r="G96" s="7">
-        <v>-712.60342355937803</v>
+        <v>-719.04949547277727</v>
       </c>
       <c r="H96" s="7">
-        <v>-537.56435604721969</v>
+        <v>-543.93180919941005</v>
       </c>
       <c r="I96" s="7">
-        <v>-354.75833438633958</v>
+        <v>-360.78231183361288</v>
       </c>
       <c r="J96" s="7">
-        <v>-185.36072324206077</v>
+        <v>-191.05975288828176</v>
       </c>
       <c r="K96" s="7">
-        <v>-8.8992053069225676</v>
+        <v>-14.290815616355474</v>
       </c>
       <c r="L96" s="7">
-        <v>135.8878446063984</v>
+        <v>130.78707069692132</v>
       </c>
       <c r="M96" s="7">
-        <v>289.11809665301087</v>
+        <v>284.29247073006758</v>
       </c>
       <c r="N96" s="7">
-        <v>431.70274899482308</v>
+        <v>427.13742891566557</v>
       </c>
       <c r="O96" s="7">
-        <v>564.2425079053985</v>
+        <v>559.92345214807904</v>
       </c>
       <c r="P96" s="7">
-        <v>687.30591423389239</v>
+        <v>683.21983870985673</v>
       </c>
       <c r="Q96" s="7">
-        <v>821.15459042048826</v>
+        <v>817.28892761680027</v>
       </c>
       <c r="R96" s="7">
-        <v>926.85084486001972</v>
+        <v>923.19370518555354</v>
       </c>
       <c r="S96" s="7">
         <v>1041.5265123188021</v>
       </c>
       <c r="T96" s="7">
-        <v>1118.4382810329596</v>
+        <v>1123.1852009296717</v>
       </c>
       <c r="U96" s="7">
-        <v>1219.6735475456815</v>
+        <v>1206.4039634399799</v>
       </c>
       <c r="V96" s="7">
-        <v>1275.7969613433925</v>
+        <v>1292.433398183076</v>
       </c>
       <c r="W96" s="7">
-        <v>1350.1509669076947</v>
+        <v>1325.0587793068903</v>
       </c>
       <c r="X96" s="7">
-        <v>1423.8799479976101</v>
+        <v>1473.4443001816692</v>
       </c>
       <c r="Y96" s="7">
-        <v>1512.4120948901086</v>
+        <v>1526.9726527366884</v>
       </c>
       <c r="Z96" s="7">
-        <v>1624.0989860332079</v>
+        <v>1607.6183566113186</v>
       </c>
       <c r="AA96" s="8">
-        <v>1635.8160769075071</v>
+        <v>1085.6414786030691</v>
       </c>
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.35">
@@ -8150,82 +8150,82 @@
         <v>3</v>
       </c>
       <c r="B97" s="9">
-        <v>236.71976315793634</v>
+        <v>243.04129119682381</v>
       </c>
       <c r="C97" s="10">
-        <v>-100.13333333333259</v>
+        <v>-34.31919593255985</v>
       </c>
       <c r="D97" s="10">
-        <v>-148.18843054016418</v>
+        <v>-136.51842723301246</v>
       </c>
       <c r="E97" s="10">
-        <v>-153.81374019999981</v>
+        <v>-153.81374019999947</v>
       </c>
       <c r="F97" s="10">
-        <v>-46.666581047959198</v>
+        <v>-51.16817926936244</v>
       </c>
       <c r="G97" s="10">
-        <v>-276.25378290541232</v>
+        <v>-263.36163907861487</v>
       </c>
       <c r="H97" s="10">
-        <v>-309.27516359994678</v>
+        <v>-296.54025729556628</v>
       </c>
       <c r="I97" s="10">
-        <v>-408.12694180295512</v>
+        <v>-396.07898690841012</v>
       </c>
       <c r="J97" s="10">
-        <v>-480.46105658669467</v>
+        <v>-469.06299729425268</v>
       </c>
       <c r="K97" s="10">
-        <v>-617.22483498460792</v>
+        <v>-606.44161436574211</v>
       </c>
       <c r="L97" s="10">
-        <v>-640.94424402163554</v>
+        <v>-630.74269620268137</v>
       </c>
       <c r="M97" s="10">
-        <v>-731.85736510813967</v>
+        <v>-722.2061132622531</v>
       </c>
       <c r="N97" s="10">
-        <v>-801.78936033798254</v>
+        <v>-792.65872017966751</v>
       </c>
       <c r="O97" s="10">
-        <v>-851.94443292026813</v>
+        <v>-843.30632140562921</v>
       </c>
       <c r="P97" s="10">
-        <v>-883.46248033124084</v>
+        <v>-875.29032928316951</v>
       </c>
       <c r="Q97" s="10">
-        <v>-986.86958857120317</v>
+        <v>-979.13826296382717</v>
       </c>
       <c r="R97" s="10">
-        <v>-984.29324111983738</v>
+        <v>-976.97896177090502</v>
       </c>
       <c r="S97" s="10">
         <v>-1000</v>
       </c>
       <c r="T97" s="10">
-        <v>-940.50616020657617</v>
+        <v>-1000</v>
       </c>
       <c r="U97" s="10">
-        <v>-979.98945961528545</v>
+        <v>-953.45029140388203</v>
       </c>
       <c r="V97" s="10">
-        <v>-943.51524380100068</v>
+        <v>-990.83346222084242</v>
       </c>
       <c r="W97" s="10">
-        <v>-975.03994745131627</v>
+        <v>-969.78779863065893</v>
       </c>
       <c r="X97" s="10">
-        <v>-955.45126817225048</v>
+        <v>-974.1696603422522</v>
       </c>
       <c r="Y97" s="10">
-        <v>-972.05619127852651</v>
+        <v>-1000</v>
       </c>
       <c r="Z97" s="10">
         <v>-1000</v>
       </c>
       <c r="AA97" s="11">
-        <v>-1000</v>
+        <v>11.437299152219111</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.35">
@@ -8575,86 +8575,86 @@
         <v>6</v>
       </c>
       <c r="B106" s="15">
-        <v>185343.29577303529</v>
+        <v>187067.81092078128</v>
       </c>
       <c r="C106" s="16">
-        <v>150354.42590554885</v>
+        <v>150732.88932861557</v>
       </c>
       <c r="D106" s="16">
-        <v>122850.988578766</v>
+        <v>123175.51953414551</v>
       </c>
       <c r="E106" s="16">
-        <v>115767.04458876402</v>
+        <v>115689.69506787838</v>
       </c>
       <c r="F106" s="16">
-        <v>110839.76863109926</v>
+        <v>110744.52859723852</v>
       </c>
       <c r="G106" s="16">
-        <v>107601.08884452145</v>
+        <v>107424.10359766646</v>
       </c>
       <c r="H106" s="16">
-        <v>11641550.231811121</v>
+        <v>11641393.204089461</v>
       </c>
       <c r="I106" s="16">
-        <v>12324968.133583765</v>
+        <v>12324833.081520598</v>
       </c>
       <c r="J106" s="16">
-        <v>13729770.539331574</v>
+        <v>13729654.387485432</v>
       </c>
       <c r="K106" s="16">
-        <v>13539056.792083366</v>
+        <v>13538956.895413551</v>
       </c>
       <c r="L106" s="16">
-        <v>15173431.935465464</v>
+        <v>15173346.019098468</v>
       </c>
       <c r="M106" s="16">
-        <v>14667613.021367956</v>
+        <v>14667539.128793448</v>
       </c>
       <c r="N106" s="16">
-        <v>14771698.232724916</v>
+        <v>14771634.681241557</v>
       </c>
       <c r="O106" s="16">
-        <v>14735518.731834156</v>
+        <v>14735464.074230678</v>
       </c>
       <c r="P106" s="16">
-        <v>14583734.508809622</v>
+        <v>14583687.500408562</v>
       </c>
       <c r="Q106" s="16">
-        <v>13638852.26087979</v>
+        <v>13638811.831193347</v>
       </c>
       <c r="R106" s="16">
-        <v>13819966.051143175</v>
+        <v>13819931.279495789</v>
       </c>
       <c r="S106" s="16">
-        <v>13455936.071670964</v>
+        <v>13455968.66823986</v>
       </c>
       <c r="T106" s="16">
-        <v>13043632.510209475</v>
+        <v>12850723.047757942</v>
       </c>
       <c r="U106" s="16">
-        <v>12117802.26314237</v>
+        <v>12512626.558646161</v>
       </c>
       <c r="V106" s="16">
-        <v>11986589.48512092</v>
+        <v>11611405.027762979</v>
       </c>
       <c r="W106" s="16">
-        <v>11111677.895684551</v>
+        <v>11438012.743528252</v>
       </c>
       <c r="X106" s="16">
-        <v>10903515.051872116</v>
+        <v>10593462.841980059</v>
       </c>
       <c r="Y106" s="16">
-        <v>10089854.202114003</v>
+        <v>10359460.770883728</v>
       </c>
       <c r="Z106" s="16">
-        <v>9835330.0367435943</v>
+        <v>9579034.8366412465</v>
       </c>
       <c r="AA106" s="17">
-        <v>9087917.6781258415</v>
+        <v>49594736.655303575</v>
       </c>
       <c r="AB106" s="18">
         <f>SUM(TotalCost)</f>
-        <v>255051172.24604046</v>
+        <v>295415517.78076106</v>
       </c>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.35">
@@ -8748,86 +8748,86 @@
         <v>8</v>
       </c>
       <c r="B109" s="3">
-        <v>127.23839999999862</v>
+        <v>79109686.491201267</v>
       </c>
       <c r="C109" s="4">
-        <v>106.61999999999958</v>
+        <v>63008256.527324185</v>
       </c>
       <c r="D109" s="4">
-        <v>70.35619439999931</v>
+        <v>55897639.429508567</v>
       </c>
       <c r="E109" s="4">
-        <v>174.35243586779998</v>
+        <v>54564500.077389985</v>
       </c>
       <c r="F109" s="4">
-        <v>0.65969839061018776</v>
+        <v>50523285.409402966</v>
       </c>
       <c r="G109" s="4">
-        <v>0.66947527612567959</v>
+        <v>46943184.414359212</v>
       </c>
       <c r="H109" s="4">
-        <v>0.62246201111017219</v>
+        <v>42214691.249905884</v>
       </c>
       <c r="I109" s="4">
-        <v>0.65362677499330402</v>
+        <v>40509490.833682947</v>
       </c>
       <c r="J109" s="4">
-        <v>0.65092004913306756</v>
+        <v>38769879.26610364</v>
       </c>
       <c r="K109" s="4">
-        <v>0.64400087711195464</v>
+        <v>37524822.871207617</v>
       </c>
       <c r="L109" s="4">
-        <v>0.62155648500595906</v>
+        <v>35723029.845435001</v>
       </c>
       <c r="M109" s="4">
-        <v>0.64071009337427121</v>
+        <v>34419950.381185815</v>
       </c>
       <c r="N109" s="4">
-        <v>0.62147608421134559</v>
+        <v>33090788.988753803</v>
       </c>
       <c r="O109" s="4">
-        <v>0.6438689689692465</v>
+        <v>31737363.779780988</v>
       </c>
       <c r="P109" s="4">
-        <v>0.62790338968997006</v>
+        <v>30361398.493312463</v>
       </c>
       <c r="Q109" s="4">
-        <v>0.65359412019717733</v>
+        <v>29491241.009569217</v>
       </c>
       <c r="R109" s="4">
-        <v>0.64146482239677427</v>
+        <v>28075014.638710182</v>
       </c>
       <c r="S109" s="4">
-        <v>0.67000427188445699</v>
+        <v>27637779.666487332</v>
       </c>
       <c r="T109" s="4">
-        <v>0.62075391033141569</v>
+        <v>28104427.366363555</v>
       </c>
       <c r="U109" s="4">
-        <v>0.65322029552439742</v>
+        <v>26480026.546641205</v>
       </c>
       <c r="V109" s="4">
-        <v>0.56741887818411307</v>
+        <v>23842430.948070701</v>
       </c>
       <c r="W109" s="4">
-        <v>0.64336524808776818</v>
+        <v>21562393.070920095</v>
       </c>
       <c r="X109" s="4">
-        <v>0.61106195483249026</v>
+        <v>18348308.303627934</v>
       </c>
       <c r="Y109" s="4">
-        <v>0.66487511242580788</v>
+        <v>17639234.17504514</v>
       </c>
       <c r="Z109" s="4">
-        <v>0.16421258843780379</v>
+        <v>15992996.94091936</v>
       </c>
       <c r="AA109" s="5">
         <v>0</v>
       </c>
       <c r="AB109" s="12">
         <f>SUM(B109:AA109)</f>
-        <v>491.5126998704348</v>
+        <v>911571820.72490895</v>
       </c>
     </row>
     <row r="110" spans="1:28" x14ac:dyDescent="0.35">
@@ -8835,86 +8835,86 @@
         <v>9</v>
       </c>
       <c r="B110" s="6">
-        <v>0.47940000000000055</v>
+        <v>14596137.675668476</v>
       </c>
       <c r="C110" s="7">
-        <v>0.40129999999999838</v>
+        <v>13232188.576625478</v>
       </c>
       <c r="D110" s="7">
-        <v>0.26393709999999737</v>
+        <v>13202905.908014389</v>
       </c>
       <c r="E110" s="7">
-        <v>0.20300000000000001</v>
+        <v>11427176.759078547</v>
       </c>
       <c r="F110" s="7">
-        <v>0</v>
+        <v>9446021.7217891198</v>
       </c>
       <c r="G110" s="7">
-        <v>0</v>
+        <v>6871604.7774165729</v>
       </c>
       <c r="H110" s="7">
-        <v>0</v>
+        <v>5465615.9763929341</v>
       </c>
       <c r="I110" s="7">
-        <v>0</v>
+        <v>4856274.8895227564</v>
       </c>
       <c r="J110" s="7">
-        <v>0</v>
+        <v>4339674.5115498714</v>
       </c>
       <c r="K110" s="7">
-        <v>0</v>
+        <v>3661125.6895761918</v>
       </c>
       <c r="L110" s="7">
-        <v>0</v>
+        <v>3314713.3030404528</v>
       </c>
       <c r="M110" s="7">
-        <v>3.8120617773529373E-15</v>
+        <v>2796791.1961188861</v>
       </c>
       <c r="N110" s="7">
-        <v>0</v>
+        <v>2352458.0009303079</v>
       </c>
       <c r="O110" s="7">
-        <v>0</v>
+        <v>1977549.3786726999</v>
       </c>
       <c r="P110" s="7">
-        <v>0</v>
+        <v>1668123.8719868409</v>
       </c>
       <c r="Q110" s="7">
-        <v>0</v>
+        <v>1170952.2892533776</v>
       </c>
       <c r="R110" s="7">
-        <v>0</v>
+        <v>981500.62396597257</v>
       </c>
       <c r="S110" s="7">
-        <v>0</v>
+        <v>2198644.6980367741</v>
       </c>
       <c r="T110" s="7">
-        <v>0</v>
+        <v>1497195.667705775</v>
       </c>
       <c r="U110" s="7">
-        <v>0</v>
+        <v>1403701.5010519307</v>
       </c>
       <c r="V110" s="7">
-        <v>0</v>
+        <v>626990.14999874891</v>
       </c>
       <c r="W110" s="7">
-        <v>0</v>
+        <v>739063.59503600525</v>
       </c>
       <c r="X110" s="7">
-        <v>0</v>
+        <v>123335.44489582664</v>
       </c>
       <c r="Y110" s="7">
-        <v>0</v>
+        <v>491512.83514318842</v>
       </c>
       <c r="Z110" s="7">
-        <v>0</v>
+        <v>111619.72520274094</v>
       </c>
       <c r="AA110" s="8">
         <v>0</v>
       </c>
       <c r="AB110" s="13">
         <f t="shared" ref="AB110:AB113" si="0">SUM(B110:AA110)</f>
-        <v>1.3476371</v>
+        <v>108552878.76667392</v>
       </c>
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.35">
@@ -8922,86 +8922,86 @@
         <v>10</v>
       </c>
       <c r="B111" s="6">
-        <v>81864043753.466522</v>
+        <v>81973843561.409775</v>
       </c>
       <c r="C111" s="7">
-        <v>77448100759.699539</v>
+        <v>77551977702.482803</v>
       </c>
       <c r="D111" s="7">
-        <v>73270364329.279526</v>
+        <v>73368637900.464386</v>
       </c>
       <c r="E111" s="7">
-        <v>69317985028.483795</v>
+        <v>69410957487.38237</v>
       </c>
       <c r="F111" s="7">
-        <v>65578806552.883316</v>
+        <v>65666763854.214989</v>
       </c>
       <c r="G111" s="7">
-        <v>62041328338.285065</v>
+        <v>62124541011.685379</v>
       </c>
       <c r="H111" s="7">
-        <v>58694670188.529953</v>
+        <v>58773394170.616638</v>
       </c>
       <c r="I111" s="7">
-        <v>55528538811.352196</v>
+        <v>55603016232.907562</v>
       </c>
       <c r="J111" s="7">
-        <v>52533196159.37471</v>
+        <v>52603656090.065567</v>
       </c>
       <c r="K111" s="7">
-        <v>49699429478.867256</v>
+        <v>49766088631.792816</v>
       </c>
       <c r="L111" s="7">
-        <v>47018522974.146408</v>
+        <v>47081586372.381195</v>
       </c>
       <c r="M111" s="7">
-        <v>44482231000.465813</v>
+        <v>44541892607.647659</v>
       </c>
       <c r="N111" s="7">
-        <v>42082752702.946281</v>
+        <v>42139196019.848885</v>
       </c>
       <c r="O111" s="7">
-        <v>39812708023.54287</v>
+        <v>39866106652.467789</v>
       </c>
       <c r="P111" s="7">
-        <v>37665115002.253708</v>
+        <v>37715633180.977707</v>
       </c>
       <c r="Q111" s="7">
-        <v>35633368302.756134</v>
+        <v>35681161409.676132</v>
       </c>
       <c r="R111" s="7">
-        <v>33711218896.421543</v>
+        <v>33756433928.450821</v>
       </c>
       <c r="S111" s="7">
-        <v>31892754842.223217</v>
+        <v>31935530866.908756</v>
       </c>
       <c r="T111" s="7">
-        <v>30172383103.422077</v>
+        <v>30212851686.673618</v>
       </c>
       <c r="U111" s="7">
-        <v>28544812345.104042</v>
+        <v>28583097955.850395</v>
       </c>
       <c r="V111" s="7">
-        <v>27005036659.659504</v>
+        <v>27041257052.676731</v>
       </c>
       <c r="W111" s="7">
-        <v>25548320170.14949</v>
+        <v>25582586748.238422</v>
       </c>
       <c r="X111" s="7">
-        <v>24170182464.20322</v>
+        <v>24202600620.830246</v>
       </c>
       <c r="Y111" s="7">
-        <v>22866384813.646187</v>
+        <v>22897054257.101181</v>
       </c>
       <c r="Z111" s="7">
-        <v>21632917137.47456</v>
+        <v>21641622074.728207</v>
       </c>
       <c r="AA111" s="8">
-        <v>20320549313.578232</v>
+        <v>0</v>
       </c>
       <c r="AB111" s="13">
         <f t="shared" si="0"/>
-        <v>1158535721152.2151</v>
+        <v>1139721488077.48</v>
       </c>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.35">
@@ -9009,86 +9009,86 @@
         <v>11</v>
       </c>
       <c r="B112" s="6">
-        <v>5.3156999999999783</v>
+        <v>6680832.790510186</v>
       </c>
       <c r="C112" s="7">
-        <v>4.8080499999999891</v>
+        <v>6597869.1890038159</v>
       </c>
       <c r="D112" s="7">
-        <v>3.9151911499999823</v>
+        <v>6544279.0233887751</v>
       </c>
       <c r="E112" s="7">
-        <v>2.3351665703499758</v>
+        <v>5705298.8174357945</v>
       </c>
       <c r="F112" s="7">
-        <v>2.1440197694831102</v>
+        <v>4781524.5565517619</v>
       </c>
       <c r="G112" s="7">
-        <v>2.1757946474084586</v>
+        <v>3778281.306606533</v>
       </c>
       <c r="H112" s="7">
-        <v>2.0230015361080596</v>
+        <v>3497093.818919112</v>
       </c>
       <c r="I112" s="7">
-        <v>2.1242870187282379</v>
+        <v>3162875.5547382412</v>
       </c>
       <c r="J112" s="7">
-        <v>2.1154901596824693</v>
+        <v>2875449.6019801125</v>
       </c>
       <c r="K112" s="7">
-        <v>2.0930028506138525</v>
+        <v>2512335.9673048593</v>
       </c>
       <c r="L112" s="7">
-        <v>2.020058576269367</v>
+        <v>2310791.7375436183</v>
       </c>
       <c r="M112" s="7">
-        <v>2.0823078034557843</v>
+        <v>2028744.1520221352</v>
       </c>
       <c r="N112" s="7">
-        <v>2.0197972736868728</v>
+        <v>1783842.7970875695</v>
       </c>
       <c r="O112" s="7">
-        <v>2.0925741491500509</v>
+        <v>1573990.3403025069</v>
       </c>
       <c r="P112" s="7">
-        <v>2.0406860164924026</v>
+        <v>1397201.7421943315</v>
       </c>
       <c r="Q112" s="7">
-        <v>2.1241808906408259</v>
+        <v>1131732.5689031847</v>
       </c>
       <c r="R112" s="7">
-        <v>2.0847606727895163</v>
+        <v>1015535.744020624</v>
       </c>
       <c r="S112" s="7">
-        <v>2.1775138836244854</v>
+        <v>918205.10790448519</v>
       </c>
       <c r="T112" s="7">
-        <v>2.0174502085771007</v>
+        <v>785829.59529897617</v>
       </c>
       <c r="U112" s="7">
-        <v>2.1229659604542914</v>
+        <v>747026.21964761522</v>
       </c>
       <c r="V112" s="7">
-        <v>1.8441113540983674</v>
+        <v>600996.01909194165</v>
       </c>
       <c r="W112" s="7">
-        <v>2.0909370562852465</v>
+        <v>591538.01414856827</v>
       </c>
       <c r="X112" s="7">
-        <v>1.9859513532055935</v>
+        <v>476052.49032645009</v>
       </c>
       <c r="Y112" s="7">
-        <v>2.1608441153838753</v>
+        <v>508691.5555225148</v>
       </c>
       <c r="Z112" s="7">
-        <v>0.53369091242286226</v>
+        <v>428144.51811810886</v>
       </c>
       <c r="AA112" s="8">
         <v>0</v>
       </c>
       <c r="AB112" s="13">
         <f t="shared" si="0"/>
-        <v>58.447533928910758</v>
+        <v>62434163.228571825</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -9096,86 +9096,86 @@
         <v>12</v>
       </c>
       <c r="B113" s="9">
-        <v>0.61334999999999762</v>
+        <v>954203.80563945195</v>
       </c>
       <c r="C113" s="10">
-        <v>0.55477499999999869</v>
+        <v>943772.70462547685</v>
       </c>
       <c r="D113" s="10">
-        <v>0.45175282499999803</v>
+        <v>940524.16925087757</v>
       </c>
       <c r="E113" s="10">
-        <v>0.26728845042499721</v>
+        <v>815301.21688416554</v>
       </c>
       <c r="F113" s="10">
-        <v>0.24738689647882042</v>
+        <v>676714.90575954423</v>
       </c>
       <c r="G113" s="10">
-        <v>0.25105322854712986</v>
+        <v>524404.04177130852</v>
       </c>
       <c r="H113" s="10">
-        <v>0.23342325416631457</v>
+        <v>484618.05374493368</v>
       </c>
       <c r="I113" s="10">
-        <v>0.24511004062248901</v>
+        <v>436440.07767093822</v>
       </c>
       <c r="J113" s="10">
-        <v>0.24409501842490033</v>
+        <v>395310.56502841291</v>
       </c>
       <c r="K113" s="10">
-        <v>0.241500328916983</v>
+        <v>342292.66191648156</v>
       </c>
       <c r="L113" s="10">
-        <v>0.23308368187723466</v>
+        <v>314098.6818412799</v>
       </c>
       <c r="M113" s="10">
-        <v>0.24026628501412892</v>
+        <v>273290.22716765414</v>
       </c>
       <c r="N113" s="10">
-        <v>0.2330535315792546</v>
+        <v>238075.84658135427</v>
       </c>
       <c r="O113" s="10">
-        <v>0.24145086336346744</v>
+        <v>208139.30657137278</v>
       </c>
       <c r="P113" s="10">
-        <v>0.23546377113373876</v>
+        <v>183181.30173968629</v>
       </c>
       <c r="Q113" s="10">
-        <v>0.2450977950739415</v>
+        <v>144375.86373888684</v>
       </c>
       <c r="R113" s="10">
-        <v>0.24054930839879035</v>
+        <v>128540.20325359867</v>
       </c>
       <c r="S113" s="10">
-        <v>0.2512516019566714</v>
+        <v>115288.34094780521</v>
       </c>
       <c r="T113" s="10">
-        <v>0.23278271637428088</v>
+        <v>96956.999820736251</v>
       </c>
       <c r="U113" s="10">
-        <v>0.24495761082164905</v>
+        <v>92765.08912339063</v>
       </c>
       <c r="V113" s="10">
-        <v>0.21278207931904239</v>
+        <v>71824.066707979873</v>
       </c>
       <c r="W113" s="10">
-        <v>0.24126196803291305</v>
+        <v>71616.252369303606</v>
       </c>
       <c r="X113" s="10">
-        <v>0.22914823306218388</v>
+        <v>55352.546677292397</v>
       </c>
       <c r="Y113" s="10">
-        <v>0.24932816715967795</v>
+        <v>61345.972085707312</v>
       </c>
       <c r="Z113" s="10">
-        <v>6.157972066417642E-2</v>
+        <v>50098.321568678759</v>
       </c>
       <c r="AA113" s="11">
         <v>0</v>
       </c>
       <c r="AB113" s="14">
         <f t="shared" si="0"/>
-        <v>6.7417923764127794</v>
+        <v>8618531.222486319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial addition of storage
-currently does not choose to build any
-cap is constrained as 20% of solar cap
-round trip efficiency included in offpeak gen
-modeled after wind and solar
-peakgen in constraint is negative to reflect charging
-1MWh battery chosen for simplicity
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfi\Google Drive\School\College\Semester 6 (Spring 2020)\ENV 717\Assignments\Assignment 11 (group project)\ENV717A11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jawessel\opl\ENV717A11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -742,52 +742,52 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>476.58096263726014</v>
+        <v>490.11743424114729</v>
       </c>
       <c r="H3" s="4">
-        <v>379.42441201882252</v>
+        <v>392.79578763201243</v>
       </c>
       <c r="I3" s="4">
-        <v>405.3242943430842</v>
+        <v>417.97438586439841</v>
       </c>
       <c r="J3" s="4">
-        <v>391.63142391799244</v>
+        <v>403.59913914242748</v>
       </c>
       <c r="K3" s="4">
-        <v>499.77194354733638</v>
+        <v>511.0940914900491</v>
       </c>
       <c r="L3" s="4">
-        <v>413.53981367105558</v>
+        <v>424.25121778058224</v>
       </c>
       <c r="M3" s="4">
-        <v>453.29703285503615</v>
+        <v>463.43063811952624</v>
       </c>
       <c r="N3" s="4">
-        <v>461.78609566813196</v>
+        <v>471.37306994400296</v>
       </c>
       <c r="O3" s="4">
-        <v>440.81794131598269</v>
+        <v>449.88777119067481</v>
       </c>
       <c r="P3" s="4">
-        <v>392.10694093548045</v>
+        <v>400.68752241914024</v>
       </c>
       <c r="Q3" s="4">
-        <v>476.44664614988278</v>
+        <v>484.56437047491789</v>
       </c>
       <c r="R3" s="4">
-        <v>375.31168377619633</v>
+        <v>382.99151856860357</v>
       </c>
       <c r="S3" s="4">
-        <v>435.13960772482977</v>
+        <v>424.15736811887871</v>
       </c>
       <c r="T3" s="4">
-        <v>243.27367851252529</v>
+        <v>126.2113730651149</v>
       </c>
       <c r="U3" s="4">
-        <v>78.059328724959414</v>
+        <v>115.19873623464923</v>
       </c>
       <c r="V3" s="4">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="W3" s="4">
         <v>0</v>
@@ -813,10 +813,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>148.72323737661523</v>
+        <v>135.1503527254354</v>
       </c>
       <c r="D4" s="7">
-        <v>606.04188169904342</v>
+        <v>630.54838279100284</v>
       </c>
       <c r="E4" s="7">
         <v>665.6</v>
@@ -944,7 +944,7 @@
         <v>46.5</v>
       </c>
       <c r="S5" s="7">
-        <v>26.787972565086477</v>
+        <v>37.770212171037088</v>
       </c>
       <c r="T5" s="7">
         <v>46.5</v>
@@ -959,7 +959,7 @@
         <v>46.5</v>
       </c>
       <c r="X5" s="7">
-        <v>34.372432155943898</v>
+        <v>43.188165168920847</v>
       </c>
       <c r="Y5" s="7">
         <v>46.5</v>
@@ -1059,7 +1059,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>149.82931106635917</v>
+        <v>137.80142614627539</v>
       </c>
       <c r="C7" s="7">
         <v>464</v>
@@ -1205,7 +1205,7 @@
         <v>101.5</v>
       </c>
       <c r="W8" s="7">
-        <v>86.928738357001748</v>
+        <v>101.5</v>
       </c>
       <c r="X8" s="7">
         <v>0</v>
@@ -1225,10 +1225,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>0</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="C9" s="7">
-        <v>13</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="D9" s="7">
         <v>84.6</v>
@@ -1380,7 +1380,7 @@
         <v>85.51375562129715</v>
       </c>
       <c r="Z10" s="7">
-        <v>16.480629421889489</v>
+        <v>16.480629421889262</v>
       </c>
       <c r="AA10" s="8">
         <v>0</v>
@@ -1617,13 +1617,13 @@
         <v>154</v>
       </c>
       <c r="V13" s="7">
-        <v>126.02157994994501</v>
+        <v>87.627949026233381</v>
       </c>
       <c r="W13" s="7">
-        <v>23</v>
+        <v>42.624814917632364</v>
       </c>
       <c r="X13" s="7">
-        <v>130.41031219811521</v>
+        <v>121.59457918513826</v>
       </c>
       <c r="Y13" s="7">
         <v>0</v>
@@ -1646,7 +1646,7 @@
         <v>150</v>
       </c>
       <c r="D14" s="7">
-        <v>120.52511830095455</v>
+        <v>96.018617208995636</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -1732,10 +1732,10 @@
         <v>1848</v>
       </c>
       <c r="E15" s="7">
-        <v>1267.9555255442669</v>
+        <v>1258.6626725671222</v>
       </c>
       <c r="F15" s="7">
-        <v>621.34250414968039</v>
+        <v>611.88934301297775</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>591.65057745572904</v>
+        <v>600.94343043287427</v>
       </c>
       <c r="F16" s="7">
         <v>656.1</v>
@@ -1901,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="7">
-        <v>10.579953777314245</v>
+        <v>20.033114914017144</v>
       </c>
       <c r="G17" s="7">
         <v>50.3</v>
@@ -2070,37 +2070,37 @@
         <v>257</v>
       </c>
       <c r="G19" s="7">
-        <v>171.84029741107685</v>
+        <v>158.30382580719007</v>
       </c>
       <c r="H19" s="7">
         <v>39</v>
       </c>
       <c r="I19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="J19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="K19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="L19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="M19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="N19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="O19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="P19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="Q19" s="7">
-        <v>39</v>
+        <v>39.000000000000007</v>
       </c>
       <c r="R19" s="7">
         <v>0</v>
@@ -2109,22 +2109,22 @@
         <v>257</v>
       </c>
       <c r="T19" s="7">
-        <v>169.08551776878767</v>
+        <v>246.14782321619759</v>
       </c>
       <c r="U19" s="7">
-        <v>158.32540032288443</v>
+        <v>131.18599281319416</v>
       </c>
       <c r="V19" s="7">
-        <v>61.054911659328027</v>
+        <v>137.44854258303965</v>
       </c>
       <c r="W19" s="7">
-        <v>82.011741676753445</v>
+        <v>57.81566511612283</v>
       </c>
       <c r="X19" s="7">
         <v>0</v>
       </c>
       <c r="Y19" s="7">
-        <v>47.218760842124084</v>
+        <v>42.858822277242325</v>
       </c>
       <c r="Z19" s="7">
         <v>0</v>
@@ -2156,37 +2156,37 @@
         <v>2269.6</v>
       </c>
       <c r="H20" s="7">
-        <v>2215.4833393699491</v>
+        <v>2202.1119637567595</v>
       </c>
       <c r="I20" s="7">
-        <v>1956.0629268081852</v>
+        <v>1943.4128352868711</v>
       </c>
       <c r="J20" s="7">
-        <v>1736.8335822236377</v>
+        <v>1724.8658669992026</v>
       </c>
       <c r="K20" s="7">
-        <v>1446.3745476495678</v>
+        <v>1435.0523997068551</v>
       </c>
       <c r="L20" s="7">
-        <v>1300.8972959466209</v>
+        <v>1290.1858918370933</v>
       </c>
       <c r="M20" s="7">
-        <v>1080.0453107491969</v>
+        <v>1069.9117054847068</v>
       </c>
       <c r="N20" s="7">
-        <v>891.08162902853792</v>
+        <v>881.49465475266697</v>
       </c>
       <c r="O20" s="7">
-        <v>732.20089290295812</v>
+        <v>723.13106302826554</v>
       </c>
       <c r="P20" s="7">
-        <v>601.69436279143065</v>
+        <v>593.11378130777086</v>
       </c>
       <c r="Q20" s="7">
-        <v>388.77416931056905</v>
+        <v>380.65644498553348</v>
       </c>
       <c r="R20" s="7">
-        <v>350.97141902339808</v>
+        <v>343.29158423099085</v>
       </c>
       <c r="S20" s="7">
         <v>0</v>
@@ -2221,7 +2221,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>26.670688933641006</v>
+        <v>25.698573853724611</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2373,10 +2373,10 @@
         <v>398.3</v>
       </c>
       <c r="Y22" s="7">
-        <v>298.57687258982332</v>
+        <v>302.93681115470508</v>
       </c>
       <c r="Z22" s="7">
-        <v>292.24594413283467</v>
+        <v>292.24594413283421</v>
       </c>
       <c r="AA22" s="8">
         <v>0</v>
@@ -2390,22 +2390,22 @@
         <v>0</v>
       </c>
       <c r="C23" s="7">
-        <v>0</v>
+        <v>2.9496472745626505</v>
       </c>
       <c r="D23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="E23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.099999999999994</v>
       </c>
       <c r="F23" s="7">
         <v>28.1</v>
       </c>
       <c r="G23" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="H23" s="7">
         <v>28.100000000000009</v>
-      </c>
-      <c r="H23" s="7">
-        <v>28.099999999999994</v>
       </c>
       <c r="I23" s="7">
         <v>28.1</v>
@@ -2414,7 +2414,7 @@
         <v>28.099999999999994</v>
       </c>
       <c r="K23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.100000000000009</v>
       </c>
       <c r="L23" s="7">
         <v>28.100000000000009</v>
@@ -2423,10 +2423,10 @@
         <v>28.100000000000009</v>
       </c>
       <c r="N23" s="7">
+        <v>28.099999999999994</v>
+      </c>
+      <c r="O23" s="7">
         <v>28.100000000000009</v>
-      </c>
-      <c r="O23" s="7">
-        <v>28.1</v>
       </c>
       <c r="P23" s="7">
         <v>28.100000000000009</v>
@@ -2435,34 +2435,34 @@
         <v>28.1</v>
       </c>
       <c r="R23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="S23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="T23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.1</v>
       </c>
       <c r="U23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="V23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="W23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="X23" s="7">
-        <v>28.099999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="Y23" s="7">
         <v>28.099999999999994</v>
       </c>
       <c r="Z23" s="7">
-        <v>28.100000000000009</v>
+        <v>28.1</v>
       </c>
       <c r="AA23" s="8">
-        <v>28.1</v>
+        <v>28.099999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="7">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D24" s="7">
         <v>25</v>
@@ -2556,7 +2556,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="7">
-        <v>9.4767626233832232</v>
+        <v>0</v>
       </c>
       <c r="D25" s="7">
         <v>70</v>
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="7">
-        <v>0</v>
+        <v>30.6</v>
       </c>
       <c r="D26" s="7">
         <v>30.6</v>
@@ -2651,7 +2651,7 @@
         <v>30.6</v>
       </c>
       <c r="G26" s="7">
-        <v>30.599999999999998</v>
+        <v>30.6</v>
       </c>
       <c r="H26" s="7">
         <v>30.6</v>
@@ -2687,19 +2687,19 @@
         <v>30.6</v>
       </c>
       <c r="S26" s="7">
+        <v>30.6</v>
+      </c>
+      <c r="T26" s="7">
         <v>30.599999999999998</v>
       </c>
-      <c r="T26" s="7">
+      <c r="U26" s="7">
+        <v>30.599999999999998</v>
+      </c>
+      <c r="V26" s="7">
         <v>30.6</v>
       </c>
-      <c r="U26" s="7">
-        <v>30.6</v>
-      </c>
-      <c r="V26" s="7">
+      <c r="W26" s="7">
         <v>30.599999999999998</v>
-      </c>
-      <c r="W26" s="7">
-        <v>30.6</v>
       </c>
       <c r="X26" s="7">
         <v>30.6</v>
@@ -2708,7 +2708,7 @@
         <v>30.6</v>
       </c>
       <c r="Z26" s="7">
-        <v>30.6</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="AA26" s="8">
         <v>30.6</v>
@@ -2731,11 +2731,11 @@
         <v>10</v>
       </c>
       <c r="F27" s="7">
+        <v>10</v>
+      </c>
+      <c r="G27" s="7">
         <v>9.9999999999999929</v>
       </c>
-      <c r="G27" s="7">
-        <v>10</v>
-      </c>
       <c r="H27" s="7">
         <v>10</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>10</v>
       </c>
       <c r="Q27" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="R27" s="7">
         <v>10</v>
@@ -2776,25 +2776,25 @@
         <v>10</v>
       </c>
       <c r="U27" s="7">
+        <v>10</v>
+      </c>
+      <c r="V27" s="7">
+        <v>9.9999999999999929</v>
+      </c>
+      <c r="W27" s="7">
+        <v>10</v>
+      </c>
+      <c r="X27" s="7">
+        <v>10</v>
+      </c>
+      <c r="Y27" s="7">
+        <v>10</v>
+      </c>
+      <c r="Z27" s="7">
+        <v>10</v>
+      </c>
+      <c r="AA27" s="8">
         <v>9.9999999999999858</v>
-      </c>
-      <c r="V27" s="7">
-        <v>10</v>
-      </c>
-      <c r="W27" s="7">
-        <v>10</v>
-      </c>
-      <c r="X27" s="7">
-        <v>10</v>
-      </c>
-      <c r="Y27" s="7">
-        <v>10</v>
-      </c>
-      <c r="Z27" s="7">
-        <v>10</v>
-      </c>
-      <c r="AA27" s="8">
-        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.35">
@@ -2820,7 +2820,7 @@
         <v>10</v>
       </c>
       <c r="H28" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="I28" s="7">
         <v>10</v>
@@ -2877,7 +2877,7 @@
         <v>10</v>
       </c>
       <c r="AA28" s="8">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.35">
@@ -2957,7 +2957,7 @@
         <v>10</v>
       </c>
       <c r="Z29" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="AA29" s="8">
         <v>10</v>
@@ -2971,31 +2971,31 @@
         <v>0</v>
       </c>
       <c r="C30" s="7">
-        <v>0</v>
+        <v>52.2</v>
       </c>
       <c r="D30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="E30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="F30" s="7">
         <v>52.200000000000017</v>
       </c>
       <c r="G30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="H30" s="7">
         <v>52.2</v>
       </c>
       <c r="I30" s="7">
-        <v>52.20000000000001</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="J30" s="7">
         <v>52.200000000000017</v>
       </c>
       <c r="K30" s="7">
-        <v>52.200000000000017</v>
+        <v>52.2</v>
       </c>
       <c r="L30" s="7">
         <v>52.2</v>
@@ -3004,46 +3004,46 @@
         <v>52.2</v>
       </c>
       <c r="N30" s="7">
+        <v>52.200000000000017</v>
+      </c>
+      <c r="O30" s="7">
         <v>52.2</v>
-      </c>
-      <c r="O30" s="7">
-        <v>52.20000000000001</v>
       </c>
       <c r="P30" s="7">
         <v>52.2</v>
       </c>
       <c r="Q30" s="7">
-        <v>52.20000000000001</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="R30" s="7">
         <v>52.200000000000017</v>
       </c>
       <c r="S30" s="7">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="T30" s="7">
         <v>52.200000000000017</v>
       </c>
-      <c r="T30" s="7">
-        <v>52.2</v>
-      </c>
       <c r="U30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="V30" s="7">
-        <v>52.2</v>
+        <v>52.200000000000017</v>
       </c>
       <c r="W30" s="7">
         <v>52.200000000000017</v>
       </c>
       <c r="X30" s="7">
+        <v>52.20000000000001</v>
+      </c>
+      <c r="Y30" s="7">
+        <v>52.2</v>
+      </c>
+      <c r="Z30" s="7">
         <v>52.200000000000017</v>
       </c>
-      <c r="Y30" s="7">
-        <v>52.200000000000017</v>
-      </c>
-      <c r="Z30" s="7">
+      <c r="AA30" s="8">
         <v>52.2</v>
-      </c>
-      <c r="AA30" s="8">
-        <v>52.200000000000017</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.35">
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D31" s="7">
         <v>10</v>
@@ -3072,7 +3072,7 @@
         <v>10</v>
       </c>
       <c r="I31" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="J31" s="7">
         <v>10</v>
@@ -3105,13 +3105,13 @@
         <v>10</v>
       </c>
       <c r="T31" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="U31" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="V31" s="7">
-        <v>9.9999999999999858</v>
+        <v>10</v>
       </c>
       <c r="W31" s="7">
         <v>10</v>
@@ -3137,25 +3137,25 @@
         <v>0</v>
       </c>
       <c r="C32" s="7">
-        <v>0</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="D32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="E32" s="7">
         <v>20.200000000000003</v>
       </c>
       <c r="F32" s="7">
-        <v>20.2</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="G32" s="7">
-        <v>20.2</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="H32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="I32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="J32" s="7">
         <v>20.199999999999996</v>
@@ -3167,49 +3167,49 @@
         <v>20.199999999999996</v>
       </c>
       <c r="M32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.199999999999996</v>
       </c>
       <c r="N32" s="7">
-        <v>20.200000000000003</v>
+        <v>20.2</v>
       </c>
       <c r="O32" s="7">
         <v>20.200000000000003</v>
       </c>
       <c r="P32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="Q32" s="7">
         <v>20.200000000000003</v>
       </c>
       <c r="R32" s="7">
+        <v>20.199999999999996</v>
+      </c>
+      <c r="S32" s="7">
         <v>20.200000000000003</v>
       </c>
-      <c r="S32" s="7">
+      <c r="T32" s="7">
         <v>20.2</v>
-      </c>
-      <c r="T32" s="7">
-        <v>20.200000000000003</v>
       </c>
       <c r="U32" s="7">
         <v>20.2</v>
       </c>
       <c r="V32" s="7">
+        <v>20.200000000000003</v>
+      </c>
+      <c r="W32" s="7">
         <v>20.2</v>
       </c>
-      <c r="W32" s="7">
-        <v>20.199999999999996</v>
-      </c>
       <c r="X32" s="7">
-        <v>20.199999999999996</v>
+        <v>20.2</v>
       </c>
       <c r="Y32" s="7">
         <v>20.199999999999996</v>
       </c>
       <c r="Z32" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="AA32" s="8">
         <v>20.199999999999996</v>
-      </c>
-      <c r="AA32" s="8">
-        <v>20.200000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.35">
@@ -3220,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="7">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D33" s="7">
         <v>70</v>
@@ -3348,7 +3348,7 @@
         <v>10.5</v>
       </c>
       <c r="R34" s="7">
-        <v>10.5</v>
+        <v>10.499999999999993</v>
       </c>
       <c r="S34" s="7">
         <v>10.5</v>
@@ -3395,7 +3395,7 @@
         <v>10</v>
       </c>
       <c r="F35" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="G35" s="7">
         <v>10</v>
@@ -3469,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D36" s="7">
         <v>10</v>
@@ -3484,10 +3484,10 @@
         <v>10</v>
       </c>
       <c r="H36" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="I36" s="7">
-        <v>9.9999999999999929</v>
+        <v>10</v>
       </c>
       <c r="J36" s="7">
         <v>10</v>
@@ -3508,7 +3508,7 @@
         <v>10</v>
       </c>
       <c r="P36" s="7">
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="Q36" s="7">
         <v>10</v>
@@ -3552,10 +3552,10 @@
         <v>0</v>
       </c>
       <c r="C37" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D37" s="7">
-        <v>10</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="E37" s="7">
         <v>10</v>
@@ -3573,7 +3573,7 @@
         <v>10</v>
       </c>
       <c r="J37" s="7">
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="K37" s="7">
         <v>10</v>
@@ -3653,41 +3653,41 @@
         <v>10</v>
       </c>
       <c r="I38" s="7">
+        <v>10</v>
+      </c>
+      <c r="J38" s="7">
+        <v>10</v>
+      </c>
+      <c r="K38" s="7">
+        <v>10</v>
+      </c>
+      <c r="L38" s="7">
+        <v>10</v>
+      </c>
+      <c r="M38" s="7">
+        <v>10</v>
+      </c>
+      <c r="N38" s="7">
+        <v>10</v>
+      </c>
+      <c r="O38" s="7">
+        <v>10</v>
+      </c>
+      <c r="P38" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q38" s="7">
+        <v>10</v>
+      </c>
+      <c r="R38" s="7">
+        <v>10</v>
+      </c>
+      <c r="S38" s="7">
+        <v>10</v>
+      </c>
+      <c r="T38" s="7">
         <v>10.000000000000002</v>
       </c>
-      <c r="J38" s="7">
-        <v>10</v>
-      </c>
-      <c r="K38" s="7">
-        <v>10</v>
-      </c>
-      <c r="L38" s="7">
-        <v>10</v>
-      </c>
-      <c r="M38" s="7">
-        <v>10</v>
-      </c>
-      <c r="N38" s="7">
-        <v>10</v>
-      </c>
-      <c r="O38" s="7">
-        <v>10</v>
-      </c>
-      <c r="P38" s="7">
-        <v>10</v>
-      </c>
-      <c r="Q38" s="7">
-        <v>10</v>
-      </c>
-      <c r="R38" s="7">
-        <v>10</v>
-      </c>
-      <c r="S38" s="7">
-        <v>10</v>
-      </c>
-      <c r="T38" s="7">
-        <v>10</v>
-      </c>
       <c r="U38" s="7">
         <v>10</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>10</v>
       </c>
       <c r="Y38" s="7">
-        <v>10</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="Z38" s="7">
         <v>10</v>
@@ -3721,7 +3721,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="E39" s="7">
         <v>10.099999999999994</v>
@@ -3730,67 +3730,67 @@
         <v>10.099999999999994</v>
       </c>
       <c r="G39" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="H39" s="7">
         <v>10.1</v>
       </c>
-      <c r="H39" s="7">
+      <c r="I39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="J39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="K39" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="I39" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="J39" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="K39" s="7">
-        <v>10.099999999999994</v>
-      </c>
       <c r="L39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="M39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="N39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.1</v>
       </c>
       <c r="O39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="P39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="Q39" s="7">
         <v>10.1</v>
-      </c>
-      <c r="Q39" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="R39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="S39" s="7">
+        <v>10.099999999999994</v>
+      </c>
+      <c r="T39" s="7">
         <v>10.1</v>
       </c>
-      <c r="T39" s="7">
-        <v>10.099999999999994</v>
-      </c>
       <c r="U39" s="7">
-        <v>10.099999999999994</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="V39" s="7">
         <v>10.099999999999994</v>
       </c>
       <c r="W39" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="X39" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="Y39" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="Z39" s="7">
         <v>10.099999999999994</v>
       </c>
-      <c r="X39" s="7">
-        <v>10.099999999999994</v>
-      </c>
-      <c r="Y39" s="7">
-        <v>10.099999999999994</v>
-      </c>
-      <c r="Z39" s="7">
+      <c r="AA39" s="8">
         <v>10.100000000000001</v>
-      </c>
-      <c r="AA39" s="8">
-        <v>10.099999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.35">
@@ -3801,22 +3801,22 @@
         <v>0</v>
       </c>
       <c r="C40" s="7">
-        <v>0</v>
+        <v>10.1</v>
       </c>
       <c r="D40" s="7">
         <v>10.1</v>
       </c>
       <c r="E40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="F40" s="7">
         <v>10.1</v>
-      </c>
-      <c r="F40" s="7">
-        <v>10.099999999999998</v>
       </c>
       <c r="G40" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="H40" s="7">
-        <v>10.1</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="I40" s="7">
         <v>10.1</v>
@@ -3825,19 +3825,19 @@
         <v>10.1</v>
       </c>
       <c r="K40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="L40" s="7">
-        <v>10.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="M40" s="7">
         <v>10.1</v>
       </c>
       <c r="N40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="O40" s="7">
         <v>10.1</v>
-      </c>
-      <c r="O40" s="7">
-        <v>10.100000000000001</v>
       </c>
       <c r="P40" s="7">
         <v>10.1</v>
@@ -3846,16 +3846,16 @@
         <v>10.100000000000001</v>
       </c>
       <c r="R40" s="7">
+        <v>10.100000000000001</v>
+      </c>
+      <c r="S40" s="7">
         <v>10.1</v>
       </c>
-      <c r="S40" s="7">
+      <c r="T40" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="T40" s="7">
-        <v>10.1</v>
-      </c>
       <c r="U40" s="7">
-        <v>10.099999999999998</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="V40" s="7">
         <v>10.100000000000001</v>
@@ -3864,16 +3864,16 @@
         <v>10.100000000000001</v>
       </c>
       <c r="X40" s="7">
+        <v>10.099999999999998</v>
+      </c>
+      <c r="Y40" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="Z40" s="7">
         <v>10.100000000000001</v>
       </c>
-      <c r="Y40" s="7">
-        <v>10.100000000000001</v>
-      </c>
-      <c r="Z40" s="7">
+      <c r="AA40" s="8">
         <v>10.1</v>
-      </c>
-      <c r="AA40" s="8">
-        <v>10.100000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.35">
@@ -3950,7 +3950,7 @@
         <v>10</v>
       </c>
       <c r="Y41" s="7">
-        <v>10</v>
+        <v>9.9999999999999858</v>
       </c>
       <c r="Z41" s="7">
         <v>10</v>
@@ -3967,7 +3967,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="7">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D42" s="7">
         <v>12</v>
@@ -4027,7 +4027,7 @@
         <v>12</v>
       </c>
       <c r="W42" s="7">
-        <v>12</v>
+        <v>11.999999999999993</v>
       </c>
       <c r="X42" s="7">
         <v>12</v>
@@ -4101,13 +4101,13 @@
         <v>3200</v>
       </c>
       <c r="T43" s="7">
-        <v>3400</v>
+        <v>3450</v>
       </c>
       <c r="U43" s="7">
         <v>3650</v>
       </c>
       <c r="V43" s="7">
-        <v>3850</v>
+        <v>3900</v>
       </c>
       <c r="W43" s="7">
         <v>4100</v>
@@ -4187,16 +4187,16 @@
         <v>0</v>
       </c>
       <c r="T44" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U44" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V44" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W44" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="X44" s="7">
         <v>10</v>
@@ -4894,7 +4894,7 @@
         <v>7</v>
       </c>
       <c r="B55" s="6">
-        <v>0</v>
+        <v>84.6</v>
       </c>
       <c r="C55" s="7">
         <v>84.6</v>
@@ -5197,16 +5197,16 @@
         <v>0</v>
       </c>
       <c r="T58" s="7">
-        <v>10.817758884394085</v>
+        <v>20.817758884394152</v>
       </c>
       <c r="U58" s="7">
-        <v>33.025418714353322</v>
+        <v>43.025418714353684</v>
       </c>
       <c r="V58" s="7">
-        <v>55.432947482782197</v>
+        <v>65.432947482785224</v>
       </c>
       <c r="W58" s="7">
-        <v>78.042144010127004</v>
+        <v>88.042144010127117</v>
       </c>
       <c r="X58" s="7">
         <v>186</v>
@@ -5807,7 +5807,7 @@
         <v>18</v>
       </c>
       <c r="B66" s="6">
-        <v>1631</v>
+        <v>1546.3999999999999</v>
       </c>
       <c r="C66" s="7">
         <v>249.69999999999948</v>
@@ -5825,13 +5825,13 @@
         <v>327.01637801450141</v>
       </c>
       <c r="H66" s="7">
-        <v>346.78232541663152</v>
+        <v>346.78232541663169</v>
       </c>
       <c r="I66" s="7">
-        <v>366.72616634538105</v>
+        <v>366.72616634538127</v>
       </c>
       <c r="J66" s="7">
-        <v>386.84950184248936</v>
+        <v>386.84950184248942</v>
       </c>
       <c r="K66" s="7">
         <v>407.15394735907165</v>
@@ -5840,7 +5840,7 @@
         <v>427.64113288530291</v>
       </c>
       <c r="M66" s="7">
-        <v>448.31270308127046</v>
+        <v>448.3127030812704</v>
       </c>
       <c r="N66" s="7">
         <v>469.17031740900126</v>
@@ -5864,10 +5864,10 @@
         <v>0</v>
       </c>
       <c r="U66" s="7">
-        <v>2.2737367544323206E-13</v>
+        <v>-1.1368683772161603E-13</v>
       </c>
       <c r="V66" s="7">
-        <v>0</v>
+        <v>-3.1832314562052488E-12</v>
       </c>
       <c r="W66" s="7">
         <v>0</v>
@@ -7856,16 +7856,16 @@
         <v>0</v>
       </c>
       <c r="T90" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U90" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V90" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W90" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="X90" s="7">
         <v>10</v>
@@ -7984,82 +7984,82 @@
         <v>1</v>
       </c>
       <c r="B95" s="3">
-        <v>130.97643702211982</v>
+        <v>131.30047538209178</v>
       </c>
       <c r="C95" s="4">
-        <v>321.81666666666626</v>
+        <v>250.08356848362453</v>
       </c>
       <c r="D95" s="4">
-        <v>366.23840446602952</v>
+        <v>382.57607186066889</v>
       </c>
       <c r="E95" s="4">
-        <v>445.3803443500006</v>
+        <v>445.38034435000134</v>
       </c>
       <c r="F95" s="4">
-        <v>626.3184520415889</v>
+        <v>629.46950575382402</v>
       </c>
       <c r="G95" s="4">
-        <v>982.41113455139237</v>
+        <v>986.92329175268833</v>
       </c>
       <c r="H95" s="4">
-        <v>841.04570833496473</v>
+        <v>845.50283353936084</v>
       </c>
       <c r="I95" s="4">
-        <v>757.4349405820102</v>
+        <v>761.65163775578162</v>
       </c>
       <c r="J95" s="4">
-        <v>660.69639202252176</v>
+        <v>664.6856304306657</v>
       </c>
       <c r="K95" s="4">
-        <v>621.30607182208564</v>
+        <v>625.08012113632162</v>
       </c>
       <c r="L95" s="4">
-        <v>500.52926734574737</v>
+        <v>504.09973538225682</v>
       </c>
       <c r="M95" s="4">
-        <v>438.48728437217358</v>
+        <v>441.86515279367029</v>
       </c>
       <c r="N95" s="4">
-        <v>366.09493310398977</v>
+        <v>369.29059119594672</v>
       </c>
       <c r="O95" s="4">
-        <v>283.95651109753749</v>
+        <v>286.97978772243459</v>
       </c>
       <c r="P95" s="4">
-        <v>192.6441324132999</v>
+        <v>195.50432624118662</v>
       </c>
       <c r="Q95" s="4">
-        <v>162.42297718701388</v>
+        <v>165.12888529535888</v>
       </c>
       <c r="R95" s="4">
-        <v>53.78525658535159</v>
+        <v>56.34520151615402</v>
       </c>
       <c r="S95" s="4">
         <v>-41.526512318802133</v>
       </c>
       <c r="T95" s="4">
-        <v>-123.18520092967128</v>
+        <v>-178.87263607880823</v>
       </c>
       <c r="U95" s="4">
-        <v>-252.95367203609817</v>
+        <v>-240.573869532868</v>
       </c>
       <c r="V95" s="4">
-        <v>-301.59993596223262</v>
+        <v>-331.46872565432903</v>
       </c>
       <c r="W95" s="4">
-        <v>-372.65736454372745</v>
+        <v>-374.34188230193911</v>
       </c>
       <c r="X95" s="4">
-        <v>-499.27463983941669</v>
+        <v>-493.39748449743206</v>
       </c>
       <c r="Y95" s="4">
         <v>-526.97265273668881</v>
       </c>
       <c r="Z95" s="4">
-        <v>-607.61835661131897</v>
+        <v>-607.61835661131863</v>
       </c>
       <c r="AA95" s="5">
-        <v>-863.74544442195486</v>
+        <v>-863.7454444219552</v>
       </c>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.35">
@@ -8067,82 +8067,82 @@
         <v>2</v>
       </c>
       <c r="B96" s="6">
-        <v>-374.92356297788047</v>
+        <v>-374.59952461790817</v>
       </c>
       <c r="C96" s="7">
-        <v>-221.68333333333322</v>
+        <v>-216.26678424181236</v>
       </c>
       <c r="D96" s="7">
-        <v>-229.71997723301507</v>
+        <v>-237.88881093033467</v>
       </c>
       <c r="E96" s="7">
-        <v>-291.56660415000079</v>
+        <v>-291.56660415000113</v>
       </c>
       <c r="F96" s="7">
-        <v>-575.15027277222725</v>
+        <v>-581.45238019669614</v>
       </c>
       <c r="G96" s="7">
-        <v>-719.04949547277533</v>
+        <v>-714.53733827147994</v>
       </c>
       <c r="H96" s="7">
-        <v>-543.35816735942194</v>
+        <v>-538.90104215502515</v>
       </c>
       <c r="I96" s="7">
-        <v>-360.20866999362568</v>
+        <v>-355.99197281985425</v>
       </c>
       <c r="J96" s="7">
-        <v>-190.48611104829445</v>
+        <v>-186.49687264014892</v>
       </c>
       <c r="K96" s="7">
-        <v>-13.717173776367304</v>
+        <v>-9.9431244621301857</v>
       </c>
       <c r="L96" s="7">
-        <v>131.36071253690886</v>
+        <v>134.93118057341809</v>
       </c>
       <c r="M96" s="7">
-        <v>284.86611257005563</v>
+        <v>288.24398099155235</v>
       </c>
       <c r="N96" s="7">
-        <v>427.7110707556534</v>
+        <v>430.90672884761034</v>
       </c>
       <c r="O96" s="7">
-        <v>560.49709398806635</v>
+        <v>563.52037061296437</v>
       </c>
       <c r="P96" s="7">
-        <v>683.79348054984382</v>
+        <v>686.65367437773057</v>
       </c>
       <c r="Q96" s="7">
-        <v>817.86256945678724</v>
+        <v>820.5684775651323</v>
       </c>
       <c r="R96" s="7">
-        <v>923.19370518555365</v>
+        <v>925.75365011635608</v>
       </c>
       <c r="S96" s="7">
         <v>1041.5265123188021</v>
       </c>
       <c r="T96" s="7">
-        <v>1123.1852009296717</v>
+        <v>1117.4977657805348</v>
       </c>
       <c r="U96" s="7">
-        <v>1206.4039634399794</v>
+        <v>1218.7837659432096</v>
       </c>
       <c r="V96" s="7">
-        <v>1292.433398183075</v>
+        <v>1274.1709775672671</v>
       </c>
       <c r="W96" s="7">
-        <v>1330.6723954393942</v>
+        <v>1348.6126925988149</v>
       </c>
       <c r="X96" s="7">
-        <v>1473.4443001816683</v>
+        <v>1470.5057225106759</v>
       </c>
       <c r="Y96" s="7">
         <v>1526.9726527366884</v>
       </c>
       <c r="Z96" s="7">
-        <v>1607.6183566113186</v>
+        <v>1607.6183566113191</v>
       </c>
       <c r="AA96" s="8">
-        <v>618.97481193640238</v>
+        <v>618.9748119364026</v>
       </c>
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.35">
@@ -8150,73 +8150,73 @@
         <v>3</v>
       </c>
       <c r="B97" s="9">
-        <v>243.94712595576061</v>
+        <v>243.29904923581643</v>
       </c>
       <c r="C97" s="10">
-        <v>-100.13333333333304</v>
+        <v>-33.816784241812172</v>
       </c>
       <c r="D97" s="10">
-        <v>-136.51842723301448</v>
+        <v>-144.68726093033422</v>
       </c>
       <c r="E97" s="10">
-        <v>-153.81374019999978</v>
+        <v>-153.81374020000018</v>
       </c>
       <c r="F97" s="10">
-        <v>-51.168179269361758</v>
+        <v>-48.01712555712777</v>
       </c>
       <c r="G97" s="10">
-        <v>-263.36163907861692</v>
+        <v>-272.38595348120833</v>
       </c>
       <c r="H97" s="10">
-        <v>-297.68754097554302</v>
+        <v>-306.60179138433568</v>
       </c>
       <c r="I97" s="10">
-        <v>-397.22627058838452</v>
+        <v>-405.65966493592737</v>
       </c>
       <c r="J97" s="10">
-        <v>-470.21028097422732</v>
+        <v>-478.188757790517</v>
       </c>
       <c r="K97" s="10">
-        <v>-607.58889804571834</v>
+        <v>-615.13699667419166</v>
       </c>
       <c r="L97" s="10">
-        <v>-631.88997988265623</v>
+        <v>-639.03091595567491</v>
       </c>
       <c r="M97" s="10">
-        <v>-723.35339694222921</v>
+        <v>-730.10913378522264</v>
       </c>
       <c r="N97" s="10">
-        <v>-793.80600385964317</v>
+        <v>-800.19732004355706</v>
       </c>
       <c r="O97" s="10">
-        <v>-844.45360508560384</v>
+        <v>-850.50015833539896</v>
       </c>
       <c r="P97" s="10">
-        <v>-876.43761296314381</v>
+        <v>-882.15800061891719</v>
       </c>
       <c r="Q97" s="10">
-        <v>-980.28554664380113</v>
+        <v>-985.69736286049113</v>
       </c>
       <c r="R97" s="10">
-        <v>-976.97896177090547</v>
+        <v>-982.0988516325101</v>
       </c>
       <c r="S97" s="10">
         <v>-1000</v>
       </c>
       <c r="T97" s="10">
-        <v>-1000</v>
+        <v>-938.62512970172679</v>
       </c>
       <c r="U97" s="10">
-        <v>-953.45029140388135</v>
+        <v>-978.20989641034146</v>
       </c>
       <c r="V97" s="10">
-        <v>-990.83346222084231</v>
+        <v>-942.70225191293798</v>
       </c>
       <c r="W97" s="10">
-        <v>-958.01503089566677</v>
+        <v>-974.27081029687565</v>
       </c>
       <c r="X97" s="10">
-        <v>-974.16966034225152</v>
+        <v>-977.10823801324386</v>
       </c>
       <c r="Y97" s="10">
         <v>-1000</v>
@@ -8225,7 +8225,7 @@
         <v>-1000</v>
       </c>
       <c r="AA97" s="11">
-        <v>244.77063248555248</v>
+        <v>244.7706324855526</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.35">
@@ -8243,7 +8243,7 @@
         <v>1</v>
       </c>
       <c r="B101" s="3">
-        <v>315.66666666666663</v>
+        <v>343.86666666666667</v>
       </c>
       <c r="C101" s="4">
         <v>351.27166666666665</v>
@@ -8267,7 +8267,7 @@
         <v>364.92471940696117</v>
       </c>
       <c r="J101" s="4">
-        <v>367.27244188162382</v>
+        <v>367.27244188162376</v>
       </c>
       <c r="K101" s="4">
         <v>369.64129385855841</v>
@@ -8297,16 +8297,16 @@
         <v>559.1453500145135</v>
       </c>
       <c r="T101" s="4">
-        <v>558.50448557504785</v>
+        <v>555.17115224171448</v>
       </c>
       <c r="U101" s="4">
-        <v>553.69282594522338</v>
+        <v>550.35949261189</v>
       </c>
       <c r="V101" s="4">
-        <v>548.83786137873051</v>
+        <v>545.50452804539611</v>
       </c>
       <c r="W101" s="4">
-        <v>543.93920213113915</v>
+        <v>540.60586879780578</v>
       </c>
       <c r="X101" s="4">
         <v>453.32978828365276</v>
@@ -8326,7 +8326,7 @@
         <v>2</v>
       </c>
       <c r="B102" s="6">
-        <v>-734.33333333333326</v>
+        <v>-706.13333333333333</v>
       </c>
       <c r="C102" s="7">
         <v>-58.178333333333171</v>
@@ -8344,13 +8344,13 @@
         <v>-87.816278238892238</v>
       </c>
       <c r="H102" s="7">
-        <v>-95.393224743042111</v>
+        <v>-95.393224743042154</v>
       </c>
       <c r="I102" s="7">
-        <v>-103.03836376572943</v>
+        <v>-103.03836376572947</v>
       </c>
       <c r="J102" s="7">
-        <v>-110.75230903962093</v>
+        <v>-110.75230903962097</v>
       </c>
       <c r="K102" s="7">
         <v>-118.53567982097748</v>
@@ -8380,16 +8380,16 @@
         <v>-13.608742594205182</v>
       </c>
       <c r="T102" s="7">
-        <v>-14.436634982754981</v>
+        <v>-7.7699683160883524</v>
       </c>
       <c r="U102" s="7">
-        <v>-8.1444646975999895</v>
+        <v>-1.4777980309330965</v>
       </c>
       <c r="V102" s="7">
-        <v>-1.795664879878359</v>
+        <v>4.8710017867903534</v>
       </c>
       <c r="W102" s="7">
-        <v>4.6102741362026336</v>
+        <v>11.276940802869376</v>
       </c>
       <c r="X102" s="7">
         <v>182.4071999367618</v>
@@ -8409,7 +8409,7 @@
         <v>3</v>
       </c>
       <c r="B103" s="9">
-        <v>418.66666666666663</v>
+        <v>362.26666666666665</v>
       </c>
       <c r="C103" s="10">
         <v>-293.09333333333348</v>
@@ -8427,13 +8427,13 @@
         <v>-272.47563252946628</v>
       </c>
       <c r="H103" s="10">
-        <v>-267.20471322223165</v>
+        <v>-267.20471322223153</v>
       </c>
       <c r="I103" s="10">
-        <v>-261.88635564123177</v>
+        <v>-261.88635564123166</v>
       </c>
       <c r="J103" s="10">
-        <v>-256.52013284200285</v>
+        <v>-256.52013284200279</v>
       </c>
       <c r="K103" s="10">
         <v>-251.10561403758089</v>
@@ -8463,16 +8463,16 @@
         <v>-545.53660742030831</v>
       </c>
       <c r="T103" s="10">
-        <v>-544.06785059229287</v>
+        <v>-547.40118392562624</v>
       </c>
       <c r="U103" s="10">
-        <v>-545.54836124762346</v>
+        <v>-548.88169458095683</v>
       </c>
       <c r="V103" s="10">
-        <v>-547.04219649885204</v>
+        <v>-550.37552983218654</v>
       </c>
       <c r="W103" s="10">
-        <v>-548.54947626734179</v>
+        <v>-551.88280960067505</v>
       </c>
       <c r="X103" s="10">
         <v>-635.73698822041456</v>
@@ -8575,76 +8575,76 @@
         <v>6</v>
       </c>
       <c r="B106" s="15">
-        <v>231991.12588150462</v>
+        <v>229863.34998209408</v>
       </c>
       <c r="C106" s="16">
-        <v>190140.63153965492</v>
+        <v>189875.71261185518</v>
       </c>
       <c r="D106" s="16">
-        <v>159339.54690181487</v>
+        <v>159112.37992213608</v>
       </c>
       <c r="E106" s="16">
-        <v>148876.86993389658</v>
+        <v>148931.01348090786</v>
       </c>
       <c r="F106" s="16">
-        <v>141199.76340916846</v>
+        <v>141266.43005676562</v>
       </c>
       <c r="G106" s="16">
-        <v>135372.17299524634</v>
+        <v>135496.06011081822</v>
       </c>
       <c r="H106" s="16">
-        <v>11667050.655674972</v>
+        <v>11667160.572811268</v>
       </c>
       <c r="I106" s="16">
-        <v>12348378.054315709</v>
+        <v>12348472.588808587</v>
       </c>
       <c r="J106" s="16">
-        <v>13751260.723626044</v>
+        <v>13751342.028240088</v>
       </c>
       <c r="K106" s="16">
-        <v>13558784.138956418</v>
+        <v>13558854.0651819</v>
       </c>
       <c r="L106" s="16">
-        <v>15191540.591279879</v>
+        <v>15191600.731495388</v>
       </c>
       <c r="M106" s="16">
-        <v>14684235.406751253</v>
+        <v>14684287.130485751</v>
       </c>
       <c r="N106" s="16">
-        <v>14786955.988124127</v>
+        <v>14787000.473244235</v>
       </c>
       <c r="O106" s="16">
-        <v>14749523.58796652</v>
+        <v>14749561.847499218</v>
       </c>
       <c r="P106" s="16">
-        <v>14596589.087813787</v>
+        <v>14596621.993015315</v>
       </c>
       <c r="Q106" s="16">
-        <v>13650650.813546522</v>
+        <v>13650679.113742871</v>
       </c>
       <c r="R106" s="16">
-        <v>13830801.065545823</v>
+        <v>13830825.405196585</v>
       </c>
       <c r="S106" s="16">
-        <v>13466016.171551844</v>
+        <v>13465993.354424601</v>
       </c>
       <c r="T106" s="16">
-        <v>12859918.526223721</v>
+        <v>13052872.188199122</v>
       </c>
       <c r="U106" s="16">
-        <v>12521090.419230273</v>
+        <v>12126306.671921205</v>
       </c>
       <c r="V106" s="16">
-        <v>11619195.149856256</v>
+        <v>11994417.194799118</v>
       </c>
       <c r="W106" s="16">
-        <v>11445159.650363134</v>
+        <v>11118882.032706637</v>
       </c>
       <c r="X106" s="16">
-        <v>10600356.968824476</v>
+        <v>10778653.087909246</v>
       </c>
       <c r="Y106" s="16">
-        <v>10365533.221142804</v>
+        <v>10365539.187055131</v>
       </c>
       <c r="Z106" s="16">
         <v>9584881.0747875217</v>
@@ -8654,7 +8654,7 @@
       </c>
       <c r="AB106" s="18">
         <f>SUM(TotalCost)</f>
-        <v>304039169.01005739</v>
+        <v>304062823.29150337</v>
       </c>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.35">
@@ -8748,86 +8748,86 @@
         <v>8</v>
       </c>
       <c r="B109" s="3">
-        <v>79410814.945040509</v>
+        <v>79312435.467566609</v>
       </c>
       <c r="C109" s="4">
-        <v>63008596.513607681</v>
+        <v>63004712.496935904</v>
       </c>
       <c r="D109" s="4">
-        <v>55897639.429508552</v>
+        <v>55845687.607713684</v>
       </c>
       <c r="E109" s="4">
-        <v>54564500.07738997</v>
+        <v>54436910.692870244</v>
       </c>
       <c r="F109" s="4">
-        <v>50523285.409402966</v>
+        <v>50586717.633136034</v>
       </c>
       <c r="G109" s="4">
-        <v>46943184.414359182</v>
+        <v>46757488.931061611</v>
       </c>
       <c r="H109" s="4">
-        <v>42789651.604352027</v>
+        <v>42802770.528393649</v>
       </c>
       <c r="I109" s="4">
-        <v>41084451.18812909</v>
+        <v>41096862.445922486</v>
       </c>
       <c r="J109" s="4">
-        <v>39344839.620549791</v>
+        <v>39356581.385310784</v>
       </c>
       <c r="K109" s="4">
-        <v>38099783.225653768</v>
+        <v>38110891.611443318</v>
       </c>
       <c r="L109" s="4">
-        <v>36297990.199881151</v>
+        <v>36308499.372681089</v>
       </c>
       <c r="M109" s="4">
-        <v>34994910.735631958</v>
+        <v>35004853.018429048</v>
       </c>
       <c r="N109" s="4">
-        <v>33665749.343199946</v>
+        <v>33675155.315401487</v>
       </c>
       <c r="O109" s="4">
-        <v>32312324.134227134</v>
+        <v>32321222.725713793</v>
       </c>
       <c r="P109" s="4">
-        <v>30936358.847758602</v>
+        <v>30944777.427863855</v>
       </c>
       <c r="Q109" s="4">
-        <v>30066201.364015359</v>
+        <v>30074165.825705137</v>
       </c>
       <c r="R109" s="4">
-        <v>28075014.638710186</v>
+        <v>28082549.478221711</v>
       </c>
       <c r="S109" s="4">
-        <v>27637779.666487537</v>
+        <v>29136901.058816552</v>
       </c>
       <c r="T109" s="4">
-        <v>28104427.366363551</v>
+        <v>28825897.202459987</v>
       </c>
       <c r="U109" s="4">
-        <v>26480026.546641212</v>
+        <v>26191644.612118073</v>
       </c>
       <c r="V109" s="4">
-        <v>23842430.948070701</v>
+        <v>24209430.84098763</v>
       </c>
       <c r="W109" s="4">
-        <v>21764460.934464518</v>
+        <v>21666318.719694287</v>
       </c>
       <c r="X109" s="4">
-        <v>18348308.303627893</v>
+        <v>19472407.35692307</v>
       </c>
       <c r="Y109" s="4">
-        <v>17639234.175045125</v>
+        <v>17596356.097632479</v>
       </c>
       <c r="Z109" s="4">
-        <v>15992996.940919366</v>
+        <v>15992996.940919355</v>
       </c>
       <c r="AA109" s="5">
         <v>0</v>
       </c>
       <c r="AB109" s="12">
         <f>SUM(B109:AA109)</f>
-        <v>917824960.57303786</v>
+        <v>920814234.79392207</v>
       </c>
     </row>
     <row r="110" spans="1:28" x14ac:dyDescent="0.35">
@@ -8835,86 +8835,86 @@
         <v>9</v>
       </c>
       <c r="B110" s="6">
-        <v>14667374.743175548</v>
+        <v>14615895.097423073</v>
       </c>
       <c r="C110" s="7">
-        <v>13232177.66341256</v>
+        <v>13232019.132119834</v>
       </c>
       <c r="D110" s="7">
-        <v>13202905.908014389</v>
+        <v>13202190.318182502</v>
       </c>
       <c r="E110" s="7">
-        <v>11427176.759078542</v>
+        <v>11398630.601589229</v>
       </c>
       <c r="F110" s="7">
-        <v>9446021.7217891142</v>
+        <v>9418749.730036173</v>
       </c>
       <c r="G110" s="7">
-        <v>6871604.7774165524</v>
+        <v>6764329.8643323416</v>
       </c>
       <c r="H110" s="7">
-        <v>5680751.2654034821</v>
+        <v>5649906.1761389757</v>
       </c>
       <c r="I110" s="7">
-        <v>5071410.1785333082</v>
+        <v>5042228.9474119404</v>
       </c>
       <c r="J110" s="7">
-        <v>4554809.8005604241</v>
+        <v>4527202.6750806971</v>
       </c>
       <c r="K110" s="7">
-        <v>3876260.9785867427</v>
+        <v>3850143.0477124928</v>
       </c>
       <c r="L110" s="7">
-        <v>3529848.5920510031</v>
+        <v>3505139.5250511449</v>
       </c>
       <c r="M110" s="7">
-        <v>3011926.4851294374</v>
+        <v>2988550.2845053119</v>
       </c>
       <c r="N110" s="7">
-        <v>2567593.2899408601</v>
+        <v>2545478.0576812807</v>
       </c>
       <c r="O110" s="7">
-        <v>2192684.6676832531</v>
+        <v>2171762.3841283121</v>
       </c>
       <c r="P110" s="7">
-        <v>1883259.1609973933</v>
+        <v>1863465.4756308871</v>
       </c>
       <c r="Q110" s="7">
-        <v>1386087.5782639331</v>
+        <v>1367361.6117909409</v>
       </c>
       <c r="R110" s="7">
-        <v>981500.62396597164</v>
+        <v>963784.78106684668</v>
       </c>
       <c r="S110" s="7">
-        <v>2198644.6980367745</v>
+        <v>2199991.5599020482</v>
       </c>
       <c r="T110" s="7">
-        <v>1497195.6677057731</v>
+        <v>2106036.3908998435</v>
       </c>
       <c r="U110" s="7">
-        <v>1403701.5010519358</v>
+        <v>1189092.1532665414</v>
       </c>
       <c r="V110" s="7">
-        <v>626990.14999876067</v>
+        <v>1230531.7078334645</v>
       </c>
       <c r="W110" s="7">
-        <v>785592.28795040783</v>
+        <v>593627.71539263648</v>
       </c>
       <c r="X110" s="7">
-        <v>123335.4448958266</v>
+        <v>124416.60639253809</v>
       </c>
       <c r="Y110" s="7">
-        <v>491512.83514317533</v>
+        <v>456935.38316789625</v>
       </c>
       <c r="Z110" s="7">
-        <v>111619.72520274097</v>
+        <v>111619.72520274093</v>
       </c>
       <c r="AA110" s="8">
         <v>0</v>
       </c>
       <c r="AB110" s="13">
         <f t="shared" ref="AB110:AB113" si="0">SUM(B110:AA110)</f>
-        <v>110821986.50398794</v>
+        <v>111119088.95193969</v>
       </c>
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.35">
@@ -8922,86 +8922,86 @@
         <v>10</v>
       </c>
       <c r="B111" s="6">
-        <v>81973843561.409744</v>
+        <v>81896985282.326309</v>
       </c>
       <c r="C111" s="7">
-        <v>77551977702.482773</v>
+        <v>77479265343.432953</v>
       </c>
       <c r="D111" s="7">
-        <v>73368637900.464371</v>
+        <v>73299847820.57135</v>
       </c>
       <c r="E111" s="7">
-        <v>69410957487.382355</v>
+        <v>69345878109.494965</v>
       </c>
       <c r="F111" s="7">
-        <v>65666763854.214973</v>
+        <v>65605195014.161346</v>
       </c>
       <c r="G111" s="7">
-        <v>62124541011.685364</v>
+        <v>62066293342.629448</v>
       </c>
       <c r="H111" s="7">
-        <v>58773394170.616623</v>
+        <v>58718288520.623993</v>
       </c>
       <c r="I111" s="7">
-        <v>55603016232.907555</v>
+        <v>55550883113.929085</v>
       </c>
       <c r="J111" s="7">
-        <v>52603656090.065559</v>
+        <v>52554335156.644272</v>
       </c>
       <c r="K111" s="7">
-        <v>49766088631.792809</v>
+        <v>49719428187.890503</v>
       </c>
       <c r="L111" s="7">
-        <v>47081586372.381187</v>
+        <v>47037442904.808037</v>
       </c>
       <c r="M111" s="7">
-        <v>44541892607.647652</v>
+        <v>44500130344.659721</v>
       </c>
       <c r="N111" s="7">
-        <v>42139196019.848877</v>
+        <v>42099686513.555946</v>
       </c>
       <c r="O111" s="7">
-        <v>39866106652.467781</v>
+        <v>39828728383.767105</v>
       </c>
       <c r="P111" s="7">
-        <v>37715633180.977699</v>
+        <v>37680271185.798584</v>
       </c>
       <c r="Q111" s="7">
-        <v>35681161409.676132</v>
+        <v>35647706925.385765</v>
       </c>
       <c r="R111" s="7">
-        <v>33756433928.450821</v>
+        <v>33724784059.333832</v>
       </c>
       <c r="S111" s="7">
-        <v>31935530866.908756</v>
+        <v>31905588267.69162</v>
       </c>
       <c r="T111" s="7">
-        <v>30212851686.673618</v>
+        <v>30184524263.120491</v>
       </c>
       <c r="U111" s="7">
-        <v>28583097955.850395</v>
+        <v>28556298581.509541</v>
       </c>
       <c r="V111" s="7">
-        <v>27041257052.676731</v>
+        <v>27015903300.906319</v>
       </c>
       <c r="W111" s="7">
-        <v>25582586748.238422</v>
+        <v>25558600638.687508</v>
       </c>
       <c r="X111" s="7">
-        <v>24202600620.830246</v>
+        <v>24179908379.595169</v>
       </c>
       <c r="Y111" s="7">
-        <v>22897054257.101173</v>
+        <v>22875586089.819695</v>
       </c>
       <c r="Z111" s="7">
-        <v>21641622074.728207</v>
+        <v>21641622074.728203</v>
       </c>
       <c r="AA111" s="8">
         <v>0</v>
       </c>
       <c r="AB111" s="13">
         <f t="shared" si="0"/>
-        <v>1139721488077.48</v>
+        <v>1138673181805.0718</v>
       </c>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.35">
@@ -9009,86 +9009,86 @@
         <v>11</v>
       </c>
       <c r="B112" s="6">
-        <v>6683510.9719839916</v>
+        <v>6683691.1024731873</v>
       </c>
       <c r="C112" s="7">
-        <v>6599755.803300471</v>
+        <v>6598487.5529586654</v>
       </c>
       <c r="D112" s="7">
-        <v>6544279.0233887751</v>
+        <v>6542847.8437250052</v>
       </c>
       <c r="E112" s="7">
-        <v>5705298.8174357917</v>
+        <v>5691839.7926119342</v>
       </c>
       <c r="F112" s="7">
-        <v>4781524.5565517591</v>
+        <v>4767888.5606752886</v>
       </c>
       <c r="G112" s="7">
-        <v>3778281.3066065297</v>
+        <v>3760494.3829190223</v>
       </c>
       <c r="H112" s="7">
-        <v>3501015.5881168302</v>
+        <v>3485475.9102342054</v>
       </c>
       <c r="I112" s="7">
-        <v>3166797.3239359627</v>
+        <v>3152095.8935735524</v>
       </c>
       <c r="J112" s="7">
-        <v>2879371.3711778335</v>
+        <v>2865462.9712526039</v>
       </c>
       <c r="K112" s="7">
-        <v>2516257.7365025799</v>
+        <v>2503099.5890494771</v>
       </c>
       <c r="L112" s="7">
-        <v>2314713.5067413384</v>
+        <v>2302265.1413414096</v>
       </c>
       <c r="M112" s="7">
-        <v>2032665.9212198558</v>
+        <v>2020889.0505256758</v>
       </c>
       <c r="N112" s="7">
-        <v>1787764.5662852908</v>
+        <v>1776622.9682608445</v>
       </c>
       <c r="O112" s="7">
-        <v>1577912.1095002284</v>
+        <v>1567371.5160130558</v>
       </c>
       <c r="P112" s="7">
-        <v>1401123.5113920528</v>
+        <v>1391151.5028150028</v>
       </c>
       <c r="Q112" s="7">
-        <v>1135654.3381009076</v>
+        <v>1126220.2435993243</v>
       </c>
       <c r="R112" s="7">
-        <v>1015535.7440206235</v>
+        <v>1006610.5472182796</v>
       </c>
       <c r="S112" s="7">
-        <v>918205.10790448519</v>
+        <v>917948.56278729008</v>
       </c>
       <c r="T112" s="7">
-        <v>785829.59529897582</v>
+        <v>881483.06465687242</v>
       </c>
       <c r="U112" s="7">
-        <v>747026.21964761592</v>
+        <v>712766.6381798829</v>
       </c>
       <c r="V112" s="7">
-        <v>600996.01909194351</v>
+        <v>694873.97490732267</v>
       </c>
       <c r="W112" s="7">
-        <v>601309.34157280484</v>
+        <v>571716.1173205924</v>
       </c>
       <c r="X112" s="7">
-        <v>476052.49032645003</v>
+        <v>475640.61928008375</v>
       </c>
       <c r="Y112" s="7">
-        <v>508691.55552251264</v>
+        <v>503038.98237191478</v>
       </c>
       <c r="Z112" s="7">
-        <v>428144.51811810891</v>
+        <v>428144.5181181088</v>
       </c>
       <c r="AA112" s="8">
         <v>0</v>
       </c>
       <c r="AB112" s="13">
         <f t="shared" si="0"/>
-        <v>62487717.043743722</v>
+        <v>62428127.046868593</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -9096,86 +9096,86 @@
         <v>12</v>
       </c>
       <c r="B113" s="9">
-        <v>954565.25811419426</v>
+        <v>954516.28076872649</v>
       </c>
       <c r="C113" s="10">
-        <v>943989.55141255888</v>
+        <v>943831.02011983306</v>
       </c>
       <c r="D113" s="10">
-        <v>940524.16925087757</v>
+        <v>940381.05128450051</v>
       </c>
       <c r="E113" s="10">
-        <v>815301.21688416507</v>
+        <v>813293.21721286373</v>
       </c>
       <c r="F113" s="10">
-        <v>676714.90575954388</v>
+        <v>674672.26670112507</v>
       </c>
       <c r="G113" s="10">
-        <v>524404.04177130794</v>
+        <v>521716.23996964027</v>
       </c>
       <c r="H113" s="10">
-        <v>485227.58759383595</v>
+        <v>482884.92258640507</v>
       </c>
       <c r="I113" s="10">
-        <v>437049.6115198409</v>
+        <v>434833.31548530667</v>
       </c>
       <c r="J113" s="10">
-        <v>395920.09887731553</v>
+        <v>393823.35516999452</v>
       </c>
       <c r="K113" s="10">
-        <v>342902.19576538412</v>
+        <v>340918.55544582085</v>
       </c>
       <c r="L113" s="10">
-        <v>314708.21569018246</v>
+        <v>312831.5776901932</v>
       </c>
       <c r="M113" s="10">
-        <v>273899.76101655676</v>
+        <v>272124.3533742181</v>
       </c>
       <c r="N113" s="10">
-        <v>238685.38043025695</v>
+        <v>237005.74253712437</v>
       </c>
       <c r="O113" s="10">
-        <v>208748.84042027546</v>
+        <v>207159.80622622935</v>
       </c>
       <c r="P113" s="10">
-        <v>183790.83558858896</v>
+        <v>182287.51771265175</v>
       </c>
       <c r="Q113" s="10">
-        <v>144985.3975877898</v>
+        <v>143563.17228604353</v>
       </c>
       <c r="R113" s="10">
-        <v>128540.20325359861</v>
+        <v>127194.69619796886</v>
       </c>
       <c r="S113" s="10">
         <v>115288.34094780521</v>
       </c>
       <c r="T113" s="10">
-        <v>96956.999820736222</v>
+        <v>111791.29119037392</v>
       </c>
       <c r="U113" s="10">
-        <v>92765.089123390746</v>
+        <v>87493.088368266632</v>
       </c>
       <c r="V113" s="10">
-        <v>71824.066707980164</v>
+        <v>86301.367259597857</v>
       </c>
       <c r="W113" s="10">
-        <v>73258.764066135307</v>
+        <v>68770.896191370586</v>
       </c>
       <c r="X113" s="10">
-        <v>55352.546677292397</v>
+        <v>55301.062796496612</v>
       </c>
       <c r="Y113" s="10">
-        <v>61345.972085706991</v>
+        <v>60505.724725482978</v>
       </c>
       <c r="Z113" s="10">
-        <v>50098.321568678766</v>
+        <v>50098.321568678752</v>
       </c>
       <c r="AA113" s="11">
         <v>0</v>
       </c>
       <c r="AB113" s="14">
         <f t="shared" si="0"/>
-        <v>8626847.3719340004</v>
+        <v>8618587.1838167161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
playing with emissions constraints
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -320,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,6 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB113"/>
+  <dimension ref="A1:AB116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC61" sqref="AC61"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -730,67 +731,67 @@
         <v>519.20000000000005</v>
       </c>
       <c r="C3" s="4">
-        <v>519.20000000000005</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>444.39767768616434</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>489.05601470060719</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>342.89686747396632</v>
       </c>
       <c r="G3" s="4">
-        <v>476.58096263726509</v>
+        <v>177.42738062174587</v>
       </c>
       <c r="H3" s="4">
-        <v>379.42441201882548</v>
+        <v>78</v>
       </c>
       <c r="I3" s="4">
-        <v>405.32429434308688</v>
+        <v>0</v>
       </c>
       <c r="J3" s="4">
-        <v>391.63142391799283</v>
+        <v>0</v>
       </c>
       <c r="K3" s="4">
-        <v>499.77194354733729</v>
+        <v>0</v>
       </c>
       <c r="L3" s="4">
-        <v>413.5398136710528</v>
+        <v>0</v>
       </c>
       <c r="M3" s="4">
-        <v>453.29703285503911</v>
+        <v>0</v>
       </c>
       <c r="N3" s="4">
-        <v>461.78609566813248</v>
+        <v>0</v>
       </c>
       <c r="O3" s="4">
-        <v>440.81794131598326</v>
+        <v>0</v>
       </c>
       <c r="P3" s="4">
-        <v>392.10694093547863</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="4">
-        <v>476.44664614988051</v>
+        <v>0</v>
       </c>
       <c r="R3" s="4">
-        <v>375.31168377619451</v>
+        <v>0</v>
       </c>
       <c r="S3" s="4">
-        <v>435.13960772483006</v>
+        <v>0</v>
       </c>
       <c r="T3" s="4">
-        <v>243.27367851252507</v>
+        <v>0</v>
       </c>
       <c r="U3" s="4">
-        <v>78.059328724957595</v>
+        <v>0</v>
       </c>
       <c r="V3" s="4">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="W3" s="4">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="X3" s="4">
         <v>0</v>
@@ -813,10 +814,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>148.7232373766019</v>
+        <v>665.6</v>
       </c>
       <c r="D4" s="7">
-        <v>606.04188169906411</v>
+        <v>665.6</v>
       </c>
       <c r="E4" s="7">
         <v>665.6</v>
@@ -834,55 +835,55 @@
         <v>665.6</v>
       </c>
       <c r="J4" s="7">
-        <v>665.6</v>
+        <v>653.67922323560242</v>
       </c>
       <c r="K4" s="7">
         <v>665.6</v>
       </c>
       <c r="L4" s="7">
-        <v>665.6</v>
+        <v>661.09286013743906</v>
       </c>
       <c r="M4" s="7">
-        <v>665.6</v>
+        <v>322.93018137873707</v>
       </c>
       <c r="N4" s="7">
-        <v>665.6</v>
+        <v>269.08451052641817</v>
       </c>
       <c r="O4" s="7">
-        <v>665.6</v>
+        <v>281.88362112115578</v>
       </c>
       <c r="P4" s="7">
-        <v>665.6</v>
+        <v>100</v>
       </c>
       <c r="Q4" s="7">
-        <v>665.6</v>
+        <v>100</v>
       </c>
       <c r="R4" s="7">
-        <v>665.6</v>
+        <v>100</v>
       </c>
       <c r="S4" s="7">
-        <v>665.6</v>
+        <v>100</v>
       </c>
       <c r="T4" s="7">
-        <v>665.6</v>
+        <v>100</v>
       </c>
       <c r="U4" s="7">
-        <v>665.6</v>
+        <v>100</v>
       </c>
       <c r="V4" s="7">
-        <v>665.6</v>
+        <v>100</v>
       </c>
       <c r="W4" s="7">
-        <v>665.6</v>
+        <v>100</v>
       </c>
       <c r="X4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="8">
         <v>0</v>
@@ -896,10 +897,10 @@
         <v>46.5</v>
       </c>
       <c r="C5" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="D5" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="E5" s="7">
         <v>46.5</v>
@@ -911,61 +912,61 @@
         <v>46.5</v>
       </c>
       <c r="H5" s="7">
-        <v>46.5</v>
+        <v>8.6312241231941194</v>
       </c>
       <c r="I5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="J5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="K5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="L5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="M5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="N5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="O5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="P5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="Q5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="R5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="S5" s="7">
-        <v>26.787972565085738</v>
+        <v>7</v>
       </c>
       <c r="T5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="U5" s="7">
-        <v>46.5</v>
+        <v>7.0000000000000124</v>
       </c>
       <c r="V5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="W5" s="7">
-        <v>46.5</v>
+        <v>7</v>
       </c>
       <c r="X5" s="7">
-        <v>34.37243215594026</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="8">
         <v>0</v>
@@ -976,7 +977,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7">
         <v>212</v>
@@ -1018,37 +1019,37 @@
         <v>212</v>
       </c>
       <c r="P6" s="7">
-        <v>212</v>
+        <v>140.52171704068627</v>
       </c>
       <c r="Q6" s="7">
-        <v>212</v>
+        <v>168.15685600738999</v>
       </c>
       <c r="R6" s="7">
-        <v>212</v>
+        <v>184.58310279959551</v>
       </c>
       <c r="S6" s="7">
-        <v>212</v>
+        <v>117.15053398555699</v>
       </c>
       <c r="T6" s="7">
-        <v>212</v>
+        <v>59.659196281313598</v>
       </c>
       <c r="U6" s="7">
-        <v>212</v>
+        <v>32</v>
       </c>
       <c r="V6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="W6" s="7">
-        <v>212</v>
+        <v>33.952731507069984</v>
       </c>
       <c r="X6" s="7">
-        <v>212</v>
+        <v>32</v>
       </c>
       <c r="Y6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="8">
         <v>0</v>
@@ -1059,7 +1060,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>149.82931106636715</v>
+        <v>182.25324173761368</v>
       </c>
       <c r="C7" s="7">
         <v>464</v>
@@ -1086,52 +1087,52 @@
         <v>464</v>
       </c>
       <c r="K7" s="7">
-        <v>464</v>
+        <v>375.46618401444209</v>
       </c>
       <c r="L7" s="7">
-        <v>464</v>
+        <v>70</v>
       </c>
       <c r="M7" s="7">
-        <v>464</v>
+        <v>70</v>
       </c>
       <c r="N7" s="7">
-        <v>464</v>
+        <v>70</v>
       </c>
       <c r="O7" s="7">
-        <v>464</v>
+        <v>70</v>
       </c>
       <c r="P7" s="7">
-        <v>464</v>
+        <v>316.57958668622592</v>
       </c>
       <c r="Q7" s="7">
-        <v>464</v>
+        <v>177.36395945306248</v>
       </c>
       <c r="R7" s="7">
-        <v>464</v>
+        <v>70</v>
       </c>
       <c r="S7" s="7">
-        <v>464</v>
+        <v>70</v>
       </c>
       <c r="T7" s="7">
-        <v>464</v>
+        <v>70</v>
       </c>
       <c r="U7" s="7">
-        <v>464</v>
+        <v>74.736248586459894</v>
       </c>
       <c r="V7" s="7">
-        <v>464</v>
+        <v>73.591961217307173</v>
       </c>
       <c r="W7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="X7" s="7">
-        <v>464</v>
+        <v>70.180390886334806</v>
       </c>
       <c r="Y7" s="7">
-        <v>464</v>
+        <v>77.120563137821605</v>
       </c>
       <c r="Z7" s="7">
-        <v>464</v>
+        <v>70</v>
       </c>
       <c r="AA7" s="8">
         <v>0</v>
@@ -1148,64 +1149,64 @@
         <v>0</v>
       </c>
       <c r="D8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="E8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="F8" s="7">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="G8" s="7">
-        <v>101.5</v>
+        <v>42.093879426591023</v>
       </c>
       <c r="H8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="I8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="J8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="K8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="L8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="M8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="N8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="O8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="P8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="R8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="S8" s="7">
         <v>0</v>
       </c>
       <c r="T8" s="7">
-        <v>101.5</v>
+        <v>15</v>
       </c>
       <c r="U8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="V8" s="7">
-        <v>101.5</v>
+        <v>0</v>
       </c>
       <c r="W8" s="7">
-        <v>38.087889959489075</v>
+        <v>0</v>
       </c>
       <c r="X8" s="7">
         <v>0</v>
@@ -1228,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="7">
-        <v>13.000000000000002</v>
+        <v>84.6</v>
       </c>
       <c r="D9" s="7">
         <v>84.6</v>
@@ -1249,7 +1250,7 @@
         <v>84.6</v>
       </c>
       <c r="J9" s="7">
-        <v>84.6</v>
+        <v>80.386779221049665</v>
       </c>
       <c r="K9" s="7">
         <v>84.6</v>
@@ -1282,22 +1283,22 @@
         <v>84.6</v>
       </c>
       <c r="U9" s="7">
-        <v>84.6</v>
+        <v>82.916288354089829</v>
       </c>
       <c r="V9" s="7">
-        <v>84.6</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="W9" s="7">
-        <v>84.6</v>
+        <v>13</v>
       </c>
       <c r="X9" s="7">
-        <v>84.6</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="Y9" s="7">
-        <v>84.6</v>
+        <v>13</v>
       </c>
       <c r="Z9" s="7">
-        <v>84.6</v>
+        <v>13</v>
       </c>
       <c r="AA9" s="8">
         <v>0</v>
@@ -1311,13 +1312,13 @@
         <v>88</v>
       </c>
       <c r="C10" s="7">
-        <v>0</v>
+        <v>69.634618197440432</v>
       </c>
       <c r="D10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="E10" s="7">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="F10" s="7">
         <v>88</v>
@@ -1326,61 +1327,61 @@
         <v>88</v>
       </c>
       <c r="H10" s="7">
-        <v>88</v>
+        <v>84.261876432314565</v>
       </c>
       <c r="I10" s="7">
         <v>88</v>
       </c>
       <c r="J10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="K10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="L10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="M10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="N10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="O10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="P10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="R10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="S10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="T10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="U10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="V10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="W10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="X10" s="7">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="7">
-        <v>85.51375562129715</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="7">
-        <v>16.480629421889489</v>
+        <v>0</v>
       </c>
       <c r="AA10" s="8">
         <v>0</v>
@@ -1427,43 +1428,43 @@
         <v>650</v>
       </c>
       <c r="N11" s="7">
-        <v>650</v>
+        <v>376.73328663132179</v>
       </c>
       <c r="O11" s="7">
-        <v>650</v>
+        <v>196.9663196290264</v>
       </c>
       <c r="P11" s="7">
-        <v>650</v>
+        <v>98</v>
       </c>
       <c r="Q11" s="7">
-        <v>650</v>
+        <v>98</v>
       </c>
       <c r="R11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="S11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="T11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="U11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="V11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="W11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="X11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="AA11" s="8">
         <v>0</v>
@@ -1501,52 +1502,52 @@
         <v>186</v>
       </c>
       <c r="K12" s="7">
-        <v>186</v>
+        <v>104.38030718246284</v>
       </c>
       <c r="L12" s="7">
-        <v>186</v>
+        <v>32.64424948023759</v>
       </c>
       <c r="M12" s="7">
-        <v>186</v>
+        <v>39.712162225497082</v>
       </c>
       <c r="N12" s="7">
-        <v>186</v>
+        <v>86.34992753893107</v>
       </c>
       <c r="O12" s="7">
-        <v>186</v>
+        <v>53.468893468759262</v>
       </c>
       <c r="P12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="R12" s="7">
-        <v>186</v>
+        <v>28</v>
       </c>
       <c r="S12" s="7">
-        <v>186</v>
+        <v>29.396630603979872</v>
       </c>
       <c r="T12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="U12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="V12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="W12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="X12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="AA12" s="8">
         <v>0</v>
@@ -1560,70 +1561,70 @@
         <v>154</v>
       </c>
       <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
         <v>154</v>
       </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
       <c r="E13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="F13" s="7">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="G13" s="7">
         <v>154</v>
       </c>
       <c r="H13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="I13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="J13" s="7">
-        <v>154</v>
+        <v>23</v>
       </c>
       <c r="K13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="L13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="M13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="N13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="O13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="P13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="R13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="S13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="T13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="U13" s="7">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="V13" s="7">
-        <v>126.02157994994468</v>
+        <v>0</v>
       </c>
       <c r="W13" s="7">
         <v>0</v>
       </c>
       <c r="X13" s="7">
-        <v>130.41031219811885</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="7">
         <v>0</v>
@@ -1646,10 +1647,10 @@
         <v>150</v>
       </c>
       <c r="D14" s="7">
-        <v>120.52511830093437</v>
+        <v>150</v>
       </c>
       <c r="E14" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F14" s="7">
         <v>150</v>
@@ -1667,52 +1668,52 @@
         <v>150</v>
       </c>
       <c r="K14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="L14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="M14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="N14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="O14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="P14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="R14" s="7">
-        <v>150</v>
+        <v>23</v>
       </c>
       <c r="S14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="T14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="U14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="V14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="W14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="X14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="8">
         <v>0</v>
@@ -1726,16 +1727,16 @@
         <v>1848</v>
       </c>
       <c r="C15" s="7">
-        <v>1848</v>
+        <v>856.16538180255702</v>
       </c>
       <c r="D15" s="7">
-        <v>1848</v>
+        <v>0</v>
       </c>
       <c r="E15" s="7">
-        <v>1267.9555255442583</v>
+        <v>0</v>
       </c>
       <c r="F15" s="7">
-        <v>621.34250414967335</v>
+        <v>0</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -1809,13 +1810,13 @@
         <v>656.1</v>
       </c>
       <c r="C16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="D16" s="7">
-        <v>0</v>
+        <v>656.1</v>
       </c>
       <c r="E16" s="7">
-        <v>591.65057745573904</v>
+        <v>656.1</v>
       </c>
       <c r="F16" s="7">
         <v>656.1</v>
@@ -1827,58 +1828,58 @@
         <v>656.1</v>
       </c>
       <c r="I16" s="7">
-        <v>656.1</v>
+        <v>204.63990573415393</v>
       </c>
       <c r="J16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="S16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="U16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="V16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="W16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="X16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="7">
-        <v>656.1</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="8">
         <v>0</v>
@@ -1895,64 +1896,64 @@
         <v>0</v>
       </c>
       <c r="D17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="E17" s="7">
-        <v>0</v>
+        <v>50.3</v>
       </c>
       <c r="F17" s="7">
-        <v>10.579953777321862</v>
+        <v>50.3</v>
       </c>
       <c r="G17" s="7">
         <v>50.3</v>
       </c>
       <c r="H17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="I17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="J17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="K17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="L17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="M17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="N17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="O17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="P17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="R17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="S17" s="7">
-        <v>28.366370434874398</v>
+        <v>0</v>
       </c>
       <c r="T17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="U17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="V17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="W17" s="7">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="X17" s="7">
         <v>0</v>
@@ -1978,7 +1979,7 @@
         <v>67</v>
       </c>
       <c r="D18" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="E18" s="7">
         <v>67</v>
@@ -1996,55 +1997,55 @@
         <v>67</v>
       </c>
       <c r="J18" s="7">
-        <v>67</v>
+        <v>65.29900368497897</v>
       </c>
       <c r="K18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="L18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="M18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="N18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="O18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="P18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="Q18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="R18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="S18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="T18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="U18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="V18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="W18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="X18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="Y18" s="7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="Z18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="8">
         <v>0</v>
@@ -2061,70 +2062,70 @@
         <v>257</v>
       </c>
       <c r="D19" s="7">
-        <v>257</v>
+        <v>39</v>
       </c>
       <c r="E19" s="7">
-        <v>257</v>
+        <v>39</v>
       </c>
       <c r="F19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="G19" s="7">
-        <v>171.84029741107224</v>
+        <v>0</v>
       </c>
       <c r="H19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="I19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="J19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="K19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="L19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="M19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="N19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="P19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="7">
-        <v>39.000000000000007</v>
+        <v>0</v>
       </c>
       <c r="R19" s="7">
         <v>0</v>
       </c>
       <c r="S19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="T19" s="7">
-        <v>169.08551776878789</v>
+        <v>0</v>
       </c>
       <c r="U19" s="7">
-        <v>158.32540032288625</v>
+        <v>0</v>
       </c>
       <c r="V19" s="7">
-        <v>61.054911659328354</v>
+        <v>0</v>
       </c>
       <c r="W19" s="7">
-        <v>75.852590074266118</v>
+        <v>0</v>
       </c>
       <c r="X19" s="7">
         <v>0</v>
       </c>
       <c r="Y19" s="7">
-        <v>47.218760842125903</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="7">
         <v>0</v>
@@ -2144,49 +2145,49 @@
         <v>2269.6</v>
       </c>
       <c r="D20" s="7">
-        <v>2269.6</v>
+        <v>1690.4693223138331</v>
       </c>
       <c r="E20" s="7">
-        <v>2269.6</v>
+        <v>859.95008829938843</v>
       </c>
       <c r="F20" s="7">
-        <v>2269.6</v>
+        <v>359.82559045302827</v>
       </c>
       <c r="G20" s="7">
-        <v>2269.6</v>
+        <v>0</v>
       </c>
       <c r="H20" s="7">
-        <v>2215.4833393699464</v>
+        <v>0</v>
       </c>
       <c r="I20" s="7">
-        <v>1956.0629268081825</v>
+        <v>0</v>
       </c>
       <c r="J20" s="7">
-        <v>1736.8335822236368</v>
+        <v>0</v>
       </c>
       <c r="K20" s="7">
-        <v>1446.3745476495669</v>
+        <v>0</v>
       </c>
       <c r="L20" s="7">
-        <v>1300.8972959466228</v>
+        <v>0</v>
       </c>
       <c r="M20" s="7">
-        <v>1080.045310749194</v>
+        <v>0</v>
       </c>
       <c r="N20" s="7">
-        <v>891.08162902853746</v>
+        <v>0</v>
       </c>
       <c r="O20" s="7">
-        <v>732.20089290295709</v>
+        <v>0</v>
       </c>
       <c r="P20" s="7">
-        <v>601.69436279143247</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="7">
-        <v>388.77416931057087</v>
+        <v>0</v>
       </c>
       <c r="R20" s="7">
-        <v>350.9714190233999</v>
+        <v>0</v>
       </c>
       <c r="S20" s="7">
         <v>0</v>
@@ -2221,7 +2222,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>26.670688933635006</v>
+        <v>26.246758262386479</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2310,10 +2311,10 @@
         <v>0</v>
       </c>
       <c r="D22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="E22" s="7">
-        <v>0</v>
+        <v>398.3</v>
       </c>
       <c r="F22" s="7">
         <v>398.3</v>
@@ -2322,61 +2323,61 @@
         <v>398.3</v>
       </c>
       <c r="H22" s="7">
-        <v>398.3</v>
+        <v>151.61465083326357</v>
       </c>
       <c r="I22" s="7">
-        <v>398.3</v>
+        <v>145.44731541711573</v>
       </c>
       <c r="J22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="K22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="L22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="M22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="N22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="O22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="P22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="R22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="S22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="T22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="U22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="V22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="W22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="X22" s="7">
-        <v>398.3</v>
+        <v>0</v>
       </c>
       <c r="Y22" s="7">
-        <v>298.57687258982151</v>
+        <v>0</v>
       </c>
       <c r="Z22" s="7">
-        <v>292.24594413283467</v>
+        <v>0</v>
       </c>
       <c r="AA22" s="8">
         <v>0</v>
@@ -2473,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D24" s="7">
         <v>25</v>
@@ -2545,7 +2546,7 @@
         <v>25</v>
       </c>
       <c r="AA24" s="8">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.35">
@@ -2556,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="7">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D25" s="7">
         <v>70</v>
@@ -2628,7 +2629,7 @@
         <v>70</v>
       </c>
       <c r="AA25" s="8">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.35">
@@ -2639,7 +2640,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="7">
-        <v>0</v>
+        <v>30.6</v>
       </c>
       <c r="D26" s="7">
         <v>30.6</v>
@@ -2722,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D27" s="7">
         <v>10</v>
@@ -2805,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D28" s="7">
         <v>9.9999999999999858</v>
@@ -2888,7 +2889,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D29" s="7">
         <v>10</v>
@@ -2942,7 +2943,7 @@
         <v>10</v>
       </c>
       <c r="U29" s="7">
-        <v>10</v>
+        <v>3.6321921072951113</v>
       </c>
       <c r="V29" s="7">
         <v>10</v>
@@ -3137,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="7">
-        <v>0</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="D32" s="7">
         <v>20.199999999999996</v>
@@ -3220,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="7">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D33" s="7">
         <v>70</v>
@@ -3292,7 +3293,7 @@
         <v>70</v>
       </c>
       <c r="AA33" s="8">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.35">
@@ -3469,7 +3470,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D36" s="7">
         <v>10</v>
@@ -3541,7 +3542,7 @@
         <v>10</v>
       </c>
       <c r="AA36" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.35">
@@ -3552,7 +3553,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D37" s="7">
         <v>10</v>
@@ -3624,7 +3625,7 @@
         <v>10</v>
       </c>
       <c r="AA37" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.35">
@@ -3635,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D38" s="7">
         <v>10</v>
@@ -3707,7 +3708,7 @@
         <v>10</v>
       </c>
       <c r="AA38" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.35">
@@ -3718,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="7">
-        <v>0</v>
+        <v>10.099999999999994</v>
       </c>
       <c r="D39" s="7">
         <v>10.099999999999994</v>
@@ -3790,7 +3791,7 @@
         <v>10.099999999999994</v>
       </c>
       <c r="AA39" s="8">
-        <v>10.100000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.35">
@@ -3801,7 +3802,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="7">
-        <v>0</v>
+        <v>10.1</v>
       </c>
       <c r="D40" s="7">
         <v>10.1</v>
@@ -3884,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="7">
-        <v>1.6767626233960868</v>
+        <v>10</v>
       </c>
       <c r="D41" s="7">
         <v>10</v>
@@ -4053,76 +4054,76 @@
         <v>0</v>
       </c>
       <c r="D43" s="7">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="E43" s="7">
-        <v>0</v>
+        <v>1400</v>
       </c>
       <c r="F43" s="7">
-        <v>0</v>
+        <v>2150</v>
       </c>
       <c r="G43" s="7">
-        <v>0</v>
+        <v>2800</v>
       </c>
       <c r="H43" s="7">
-        <v>350</v>
+        <v>3500</v>
       </c>
       <c r="I43" s="7">
-        <v>650</v>
+        <v>4100</v>
       </c>
       <c r="J43" s="7">
-        <v>950</v>
+        <v>4600</v>
       </c>
       <c r="K43" s="7">
-        <v>1200</v>
+        <v>5050</v>
       </c>
       <c r="L43" s="7">
-        <v>1500</v>
+        <v>5500</v>
       </c>
       <c r="M43" s="7">
-        <v>1750</v>
+        <v>5900</v>
       </c>
       <c r="N43" s="7">
-        <v>2000</v>
+        <v>6250</v>
       </c>
       <c r="O43" s="7">
-        <v>2250</v>
+        <v>6500</v>
       </c>
       <c r="P43" s="7">
-        <v>2500</v>
+        <v>6550</v>
       </c>
       <c r="Q43" s="7">
-        <v>2700</v>
+        <v>6550</v>
       </c>
       <c r="R43" s="7">
-        <v>2950</v>
+        <v>6550</v>
       </c>
       <c r="S43" s="7">
-        <v>3200</v>
+        <v>6544.7467861352543</v>
       </c>
       <c r="T43" s="7">
-        <v>3400</v>
+        <v>6550</v>
       </c>
       <c r="U43" s="7">
-        <v>3650</v>
+        <v>6550</v>
       </c>
       <c r="V43" s="7">
-        <v>3850</v>
+        <v>6459.7137332805532</v>
       </c>
       <c r="W43" s="7">
-        <v>4100</v>
+        <v>6453.4518995188846</v>
       </c>
       <c r="X43" s="7">
-        <v>4300</v>
+        <v>6441.2943514102553</v>
       </c>
       <c r="Y43" s="7">
-        <v>4550</v>
+        <v>6102.9888259154241</v>
       </c>
       <c r="Z43" s="7">
-        <v>4750</v>
+        <v>6107.5265735547255</v>
       </c>
       <c r="AA43" s="8">
-        <v>5698.6405127167163</v>
+        <v>6202.3041794508499</v>
       </c>
       <c r="AB43" t="s">
         <v>15</v>
@@ -4172,43 +4173,43 @@
         <v>0</v>
       </c>
       <c r="O44" s="7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P44" s="7">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="Q44" s="7">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="R44" s="7">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="S44" s="7">
-        <v>0</v>
+        <v>760</v>
       </c>
       <c r="T44" s="7">
-        <v>10</v>
+        <v>900</v>
       </c>
       <c r="U44" s="7">
-        <v>10</v>
+        <v>1030</v>
       </c>
       <c r="V44" s="7">
-        <v>10</v>
+        <v>1298.6707971114138</v>
       </c>
       <c r="W44" s="7">
-        <v>10</v>
+        <v>1412.9358490078021</v>
       </c>
       <c r="X44" s="7">
-        <v>10</v>
+        <v>1529.9080020574711</v>
       </c>
       <c r="Y44" s="7">
-        <v>10</v>
+        <v>1970</v>
       </c>
       <c r="Z44" s="7">
-        <v>10</v>
+        <v>2060</v>
       </c>
       <c r="AA44" s="8">
-        <v>2630</v>
+        <v>2331.4363332658663</v>
       </c>
       <c r="AB44" t="s">
         <v>16</v>
@@ -4545,13 +4546,13 @@
         <v>665.6</v>
       </c>
       <c r="X50" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="Y50" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="Z50" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="AA50" s="8">
         <v>0</v>
@@ -4577,34 +4578,34 @@
         <v>0</v>
       </c>
       <c r="G51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="H51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="I51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="J51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="K51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="L51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="M51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="N51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="O51" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="P51" s="7">
-        <v>0</v>
+        <v>37.450391118073526</v>
       </c>
       <c r="Q51" s="7">
         <v>0</v>
@@ -4613,28 +4614,28 @@
         <v>0</v>
       </c>
       <c r="S51" s="7">
-        <v>45.308185217437426</v>
+        <v>46.5</v>
       </c>
       <c r="T51" s="7">
-        <v>46.500000000000021</v>
+        <v>46.5</v>
       </c>
       <c r="U51" s="7">
-        <v>46.500000000000078</v>
+        <v>33.52541871435335</v>
       </c>
       <c r="V51" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="W51" s="7">
-        <v>46.5</v>
+        <v>42.54214401012689</v>
       </c>
       <c r="X51" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="Y51" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="Z51" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="AA51" s="8">
         <v>0</v>
@@ -4645,7 +4646,7 @@
         <v>4</v>
       </c>
       <c r="B52" s="6">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="C52" s="7">
         <v>212</v>
@@ -4705,7 +4706,7 @@
         <v>212</v>
       </c>
       <c r="V52" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="W52" s="7">
         <v>212</v>
@@ -4714,10 +4715,10 @@
         <v>212</v>
       </c>
       <c r="Y52" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="Z52" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="AA52" s="8">
         <v>0</v>
@@ -4743,55 +4744,55 @@
         <v>0</v>
       </c>
       <c r="G53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="H53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="I53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="J53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="K53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="L53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="M53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="N53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="O53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="P53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="Q53" s="7">
-        <v>0</v>
+        <v>389.87624463813569</v>
       </c>
       <c r="R53" s="7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="S53" s="7">
         <v>464</v>
       </c>
       <c r="T53" s="7">
-        <v>463.99999999999977</v>
+        <v>464</v>
       </c>
       <c r="U53" s="7">
         <v>464</v>
       </c>
       <c r="V53" s="7">
-        <v>464</v>
+        <v>461.93294748278197</v>
       </c>
       <c r="W53" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="X53" s="7">
         <v>464</v>
@@ -4800,7 +4801,7 @@
         <v>464</v>
       </c>
       <c r="Z53" s="7">
-        <v>464</v>
+        <v>459.19797206641749</v>
       </c>
       <c r="AA53" s="8">
         <v>0</v>
@@ -4865,7 +4866,7 @@
         <v>0</v>
       </c>
       <c r="T54" s="7">
-        <v>0</v>
+        <v>27.817758884393811</v>
       </c>
       <c r="U54" s="7">
         <v>0</v>
@@ -5108,31 +5109,31 @@
         <v>650</v>
       </c>
       <c r="R57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="S57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="T57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="U57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="V57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="W57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="X57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="Y57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="Z57" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="AA57" s="8">
         <v>0</v>
@@ -5158,31 +5159,31 @@
         <v>0</v>
       </c>
       <c r="G58" s="7">
-        <v>0</v>
+        <v>6.5163780145016261</v>
       </c>
       <c r="H58" s="7">
-        <v>0</v>
+        <v>26.282325416631807</v>
       </c>
       <c r="I58" s="7">
-        <v>0</v>
+        <v>46.22616634538133</v>
       </c>
       <c r="J58" s="7">
-        <v>0</v>
+        <v>66.349501842489531</v>
       </c>
       <c r="K58" s="7">
-        <v>0</v>
+        <v>86.653947359071765</v>
       </c>
       <c r="L58" s="7">
-        <v>0</v>
+        <v>107.14113288530302</v>
       </c>
       <c r="M58" s="7">
-        <v>0</v>
+        <v>127.81270308127063</v>
       </c>
       <c r="N58" s="7">
-        <v>0</v>
+        <v>148.67031740900131</v>
       </c>
       <c r="O58" s="7">
-        <v>0</v>
+        <v>149.7156502656826</v>
       </c>
       <c r="P58" s="7">
         <v>0</v>
@@ -5191,31 +5192,31 @@
         <v>0</v>
       </c>
       <c r="R58" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="S58" s="7">
-        <v>0</v>
+        <v>145.80818521743771</v>
       </c>
       <c r="T58" s="7">
-        <v>10.817758884394168</v>
+        <v>0</v>
       </c>
       <c r="U58" s="7">
-        <v>33.025418714353229</v>
+        <v>0</v>
       </c>
       <c r="V58" s="7">
-        <v>55.432947482789984</v>
+        <v>0</v>
       </c>
       <c r="W58" s="7">
-        <v>78.042144010127004</v>
+        <v>0</v>
       </c>
       <c r="X58" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="Y58" s="7">
-        <v>123.87281671597373</v>
+        <v>0</v>
       </c>
       <c r="Z58" s="7">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="AA58" s="8">
         <v>0</v>
@@ -5357,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="R60" s="7">
-        <v>0</v>
+        <v>144.49493083987886</v>
       </c>
       <c r="S60" s="7">
         <v>0</v>
@@ -5449,7 +5450,7 @@
         <v>0</v>
       </c>
       <c r="U61" s="7">
-        <v>3.4816594052244909E-13</v>
+        <v>0</v>
       </c>
       <c r="V61" s="7">
         <v>0</v>
@@ -5541,13 +5542,13 @@
         <v>0</v>
       </c>
       <c r="X62" s="7">
-        <v>171.85482330621812</v>
+        <v>0</v>
       </c>
       <c r="Y62" s="7">
         <v>0</v>
       </c>
       <c r="Z62" s="7">
-        <v>218.09797206641741</v>
+        <v>0</v>
       </c>
       <c r="AA62" s="8">
         <v>0</v>
@@ -5656,64 +5657,64 @@
         <v>0</v>
       </c>
       <c r="G64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="H64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="I64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="K64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="L64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="M64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="N64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="O64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="P64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Q64" s="7">
         <v>0</v>
       </c>
       <c r="R64" s="7">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="S64" s="7">
         <v>67</v>
       </c>
       <c r="T64" s="7">
-        <v>66.999999999999929</v>
+        <v>67</v>
       </c>
       <c r="U64" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="V64" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="W64" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="X64" s="7">
-        <v>67</v>
+        <v>66.954823306218259</v>
       </c>
       <c r="Y64" s="7">
-        <v>67</v>
+        <v>61.972816715973295</v>
       </c>
       <c r="Z64" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="AA64" s="8">
         <v>0</v>
@@ -5736,64 +5737,64 @@
         <v>257</v>
       </c>
       <c r="F65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="G65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="H65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="I65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="J65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="K65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="L65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="M65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="N65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="O65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="P65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="Q65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="R65" s="7">
         <v>0</v>
       </c>
       <c r="S65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="T65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="U65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="V65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="W65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="X65" s="7">
         <v>0</v>
       </c>
       <c r="Y65" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="Z65" s="7">
         <v>0</v>
@@ -5807,67 +5808,67 @@
         <v>18</v>
       </c>
       <c r="B66" s="6">
-        <v>1631</v>
+        <v>1843</v>
       </c>
       <c r="C66" s="7">
         <v>249.69999999999948</v>
       </c>
       <c r="D66" s="7">
-        <v>268.77009999999956</v>
+        <v>268.7700999999995</v>
       </c>
       <c r="E66" s="7">
-        <v>288.01183089999921</v>
+        <v>288.01183089999927</v>
       </c>
       <c r="F66" s="7">
-        <v>307.42673737809878</v>
+        <v>564.42673737809878</v>
       </c>
       <c r="G66" s="7">
-        <v>327.01637801450141</v>
+        <v>0</v>
       </c>
       <c r="H66" s="7">
-        <v>346.78232541663152</v>
+        <v>0</v>
       </c>
       <c r="I66" s="7">
-        <v>366.72616634538105</v>
+        <v>0</v>
       </c>
       <c r="J66" s="7">
-        <v>386.84950184248936</v>
+        <v>0</v>
       </c>
       <c r="K66" s="7">
-        <v>407.15394735907165</v>
+        <v>0</v>
       </c>
       <c r="L66" s="7">
-        <v>427.64113288530291</v>
+        <v>0</v>
       </c>
       <c r="M66" s="7">
-        <v>448.3127030812704</v>
+        <v>0</v>
       </c>
       <c r="N66" s="7">
-        <v>469.17031740900126</v>
+        <v>0</v>
       </c>
       <c r="O66" s="7">
-        <v>490.21565026568237</v>
+        <v>0</v>
       </c>
       <c r="P66" s="7">
-        <v>511.45039111807336</v>
+        <v>0</v>
       </c>
       <c r="Q66" s="7">
-        <v>532.87624463813563</v>
+        <v>0</v>
       </c>
       <c r="R66" s="7">
-        <v>811.49493083987886</v>
+        <v>0</v>
       </c>
       <c r="S66" s="7">
         <v>0</v>
       </c>
       <c r="T66" s="7">
-        <v>1.1368683772161603E-13</v>
+        <v>0</v>
       </c>
       <c r="U66" s="7">
         <v>0</v>
       </c>
       <c r="V66" s="7">
-        <v>-7.9580786405131221E-12</v>
+        <v>0</v>
       </c>
       <c r="W66" s="7">
         <v>0</v>
@@ -7841,40 +7842,40 @@
         <v>0</v>
       </c>
       <c r="O90" s="7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P90" s="7">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="Q90" s="7">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="R90" s="7">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="S90" s="7">
-        <v>0</v>
+        <v>760</v>
       </c>
       <c r="T90" s="7">
-        <v>10</v>
+        <v>900</v>
       </c>
       <c r="U90" s="7">
-        <v>10</v>
+        <v>1030</v>
       </c>
       <c r="V90" s="7">
-        <v>10</v>
+        <v>1300</v>
       </c>
       <c r="W90" s="7">
-        <v>10</v>
+        <v>1530</v>
       </c>
       <c r="X90" s="7">
-        <v>10</v>
+        <v>1730</v>
       </c>
       <c r="Y90" s="7">
-        <v>10</v>
+        <v>1970</v>
       </c>
       <c r="Z90" s="7">
-        <v>10</v>
+        <v>2060</v>
       </c>
       <c r="AA90" s="8">
         <v>2627.2321538150145</v>
@@ -7984,82 +7985,82 @@
         <v>1</v>
       </c>
       <c r="B95" s="3">
-        <v>130.97643702212164</v>
+        <v>131.1177472458713</v>
       </c>
       <c r="C95" s="4">
-        <v>238.8321582510689</v>
+        <v>519.47307879829384</v>
       </c>
       <c r="D95" s="4">
-        <v>366.23840446604299</v>
+        <v>765.69870922872087</v>
       </c>
       <c r="E95" s="4">
-        <v>445.3803443500006</v>
+        <v>504.73438358353587</v>
       </c>
       <c r="F95" s="4">
-        <v>626.31845204159231</v>
+        <v>213.56490924947218</v>
       </c>
       <c r="G95" s="4">
-        <v>982.41113455139418</v>
+        <v>-70.442099644914833</v>
       </c>
       <c r="H95" s="4">
-        <v>841.04570833496518</v>
+        <v>-305.79806215280684</v>
       </c>
       <c r="I95" s="4">
-        <v>757.43494058201111</v>
+        <v>-372.85312611040291</v>
       </c>
       <c r="J95" s="4">
-        <v>660.69639202252074</v>
+        <v>-505.85874846459205</v>
       </c>
       <c r="K95" s="4">
-        <v>621.3060718220853</v>
+        <v>-587.22261708303461</v>
       </c>
       <c r="L95" s="4">
-        <v>500.52926734574658</v>
+        <v>-808.66780032553697</v>
       </c>
       <c r="M95" s="4">
-        <v>438.48728437217329</v>
+        <v>-1049.0390535284255</v>
       </c>
       <c r="N95" s="4">
-        <v>366.09493310398989</v>
+        <v>-1100</v>
       </c>
       <c r="O95" s="4">
-        <v>283.95651109753805</v>
+        <v>-1100</v>
       </c>
       <c r="P95" s="4">
-        <v>192.64413241329942</v>
+        <v>-1059.8577466562231</v>
       </c>
       <c r="Q95" s="4">
-        <v>162.42297718701309</v>
+        <v>-1091.0522997094629</v>
       </c>
       <c r="R95" s="4">
-        <v>53.785256585351021</v>
+        <v>-1097.2909370735151</v>
       </c>
       <c r="S95" s="4">
-        <v>-41.526512318802133</v>
+        <v>-1100</v>
       </c>
       <c r="T95" s="4">
-        <v>-123.18520092967151</v>
+        <v>-1097.5566950067421</v>
       </c>
       <c r="U95" s="4">
-        <v>-252.95367203609862</v>
+        <v>-1100</v>
       </c>
       <c r="V95" s="4">
-        <v>-301.59993596223279</v>
+        <v>-1100</v>
       </c>
       <c r="W95" s="4">
-        <v>-355.27098067623211</v>
+        <v>-1100</v>
       </c>
       <c r="X95" s="4">
-        <v>-499.27463983941919</v>
+        <v>-1100</v>
       </c>
       <c r="Y95" s="4">
-        <v>-526.97265273668881</v>
+        <v>-986.63332553632222</v>
       </c>
       <c r="Z95" s="4">
-        <v>-607.61835661131897</v>
+        <v>-981.48742427019033</v>
       </c>
       <c r="AA95" s="5">
-        <v>-863.7454444219552</v>
+        <v>-1100</v>
       </c>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.35">
@@ -8067,82 +8068,82 @@
         <v>2</v>
       </c>
       <c r="B96" s="6">
-        <v>-374.9235629778783</v>
+        <v>-374.78225275412893</v>
       </c>
       <c r="C96" s="7">
-        <v>-180.19107912553454</v>
+        <v>-350.96153939914706</v>
       </c>
       <c r="D96" s="7">
-        <v>-229.71997723302178</v>
+        <v>-288.68479077127756</v>
       </c>
       <c r="E96" s="7">
-        <v>-291.56660415000079</v>
+        <v>268.28133208353711</v>
       </c>
       <c r="F96" s="7">
-        <v>-575.15027277223271</v>
+        <v>694.75368028597393</v>
       </c>
       <c r="G96" s="7">
-        <v>-719.04949547277397</v>
+        <v>1028.0972703309155</v>
       </c>
       <c r="H96" s="7">
-        <v>-543.3581673594208</v>
+        <v>1305.7980621528068</v>
       </c>
       <c r="I96" s="7">
-        <v>-360.20866999362477</v>
+        <v>1354.0431690481153</v>
       </c>
       <c r="J96" s="7">
-        <v>-190.48611104829354</v>
+        <v>1505.8587484645921</v>
       </c>
       <c r="K96" s="7">
-        <v>-13.717173776367758</v>
+        <v>1586.0344445009755</v>
       </c>
       <c r="L96" s="7">
-        <v>131.36071253690807</v>
+        <v>1708.7078943458621</v>
       </c>
       <c r="M96" s="7">
-        <v>284.86611257005734</v>
+        <v>1840.9519368949539</v>
       </c>
       <c r="N96" s="7">
-        <v>427.71107075565351</v>
+        <v>1878.5993518219175</v>
       </c>
       <c r="O96" s="7">
-        <v>560.49709398806692</v>
+        <v>1880.8757959883146</v>
       </c>
       <c r="P96" s="7">
-        <v>683.79348054984337</v>
+        <v>1783.191601480321</v>
       </c>
       <c r="Q96" s="7">
-        <v>817.86256945678645</v>
+        <v>1716.2872925603106</v>
       </c>
       <c r="R96" s="7">
-        <v>923.19370518555309</v>
+        <v>1627.0175115266868</v>
       </c>
       <c r="S96" s="7">
-        <v>1041.5265123188021</v>
+        <v>1561.0964413768386</v>
       </c>
       <c r="T96" s="7">
-        <v>1123.1852009296715</v>
+        <v>1502.7137068526008</v>
       </c>
       <c r="U96" s="7">
-        <v>1206.403963439979</v>
+        <v>1456.8898275833728</v>
       </c>
       <c r="V96" s="7">
-        <v>1292.4333981830746</v>
+        <v>1335.6254874759161</v>
       </c>
       <c r="W96" s="7">
-        <v>1325.0587793068896</v>
+        <v>1291.6816595020064</v>
       </c>
       <c r="X96" s="7">
-        <v>1473.4443001816696</v>
+        <v>1241.502979233225</v>
       </c>
       <c r="Y96" s="7">
-        <v>1526.9726527366884</v>
+        <v>978.20080585247911</v>
       </c>
       <c r="Z96" s="7">
-        <v>1607.6183566113186</v>
+        <v>949.17586250717181</v>
       </c>
       <c r="AA96" s="8">
-        <v>618.9748119364026</v>
+        <v>886.38392309249184</v>
       </c>
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.35">
@@ -8150,82 +8151,82 @@
         <v>3</v>
       </c>
       <c r="B97" s="9">
-        <v>243.94712595575669</v>
+        <v>243.66450550825761</v>
       </c>
       <c r="C97" s="10">
-        <v>-58.641079125534361</v>
+        <v>-168.51153939914678</v>
       </c>
       <c r="D97" s="10">
-        <v>-136.51842723302121</v>
+        <v>-477.01391845744354</v>
       </c>
       <c r="E97" s="10">
-        <v>-153.81374019999981</v>
+        <v>-773.01571566707298</v>
       </c>
       <c r="F97" s="10">
-        <v>-51.168179269359598</v>
+        <v>-908.31858953544611</v>
       </c>
       <c r="G97" s="10">
-        <v>-263.36163907862021</v>
+        <v>-957.65517068600093</v>
       </c>
       <c r="H97" s="10">
-        <v>-297.68754097554438</v>
+        <v>-1000</v>
       </c>
       <c r="I97" s="10">
-        <v>-397.22627058838634</v>
+        <v>-981.19004293771241</v>
       </c>
       <c r="J97" s="10">
-        <v>-470.21028097422743</v>
+        <v>-1000</v>
       </c>
       <c r="K97" s="10">
-        <v>-607.58889804571754</v>
+        <v>-998.81182741794089</v>
       </c>
       <c r="L97" s="10">
-        <v>-631.88997988265464</v>
+        <v>-900.04009402032466</v>
       </c>
       <c r="M97" s="10">
-        <v>-723.35339694223057</v>
+        <v>-791.91288336652838</v>
       </c>
       <c r="N97" s="10">
-        <v>-793.8060038596434</v>
+        <v>-778.59935182191748</v>
       </c>
       <c r="O97" s="10">
-        <v>-844.45360508560498</v>
+        <v>-780.87579598831462</v>
       </c>
       <c r="P97" s="10">
-        <v>-876.43761296314278</v>
+        <v>-723.33385482409813</v>
       </c>
       <c r="Q97" s="10">
-        <v>-980.28554664379953</v>
+        <v>-625.2349928508479</v>
       </c>
       <c r="R97" s="10">
-        <v>-976.97896177090411</v>
+        <v>-529.72657445317168</v>
       </c>
       <c r="S97" s="10">
-        <v>-1000</v>
+        <v>-461.09644137683813</v>
       </c>
       <c r="T97" s="10">
-        <v>-1000</v>
+        <v>-405.15701184585896</v>
       </c>
       <c r="U97" s="10">
-        <v>-953.45029140388021</v>
+        <v>-356.88982758337283</v>
       </c>
       <c r="V97" s="10">
-        <v>-990.83346222084174</v>
+        <v>-235.62548747591609</v>
       </c>
       <c r="W97" s="10">
-        <v>-969.78779863065745</v>
+        <v>-191.68165950200637</v>
       </c>
       <c r="X97" s="10">
-        <v>-974.16966034225038</v>
+        <v>-141.50297923322501</v>
       </c>
       <c r="Y97" s="10">
-        <v>-1000</v>
+        <v>8.4325196838433385</v>
       </c>
       <c r="Z97" s="10">
-        <v>-1000</v>
+        <v>32.31156176301846</v>
       </c>
       <c r="AA97" s="11">
-        <v>244.7706324855526</v>
+        <v>213.61607690750816</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.35">
@@ -8243,7 +8244,7 @@
         <v>1</v>
       </c>
       <c r="B101" s="3">
-        <v>315.66666666666663</v>
+        <v>245</v>
       </c>
       <c r="C101" s="4">
         <v>351.27166666666665</v>
@@ -8258,64 +8259,64 @@
         <v>358.00645269411154</v>
       </c>
       <c r="G101" s="4">
-        <v>360.29191076835849</v>
+        <v>528.28645143019116</v>
       </c>
       <c r="H101" s="4">
-        <v>362.59793796527373</v>
+        <v>524.00382949306311</v>
       </c>
       <c r="I101" s="4">
-        <v>364.92471940696117</v>
+        <v>519.68266395850071</v>
       </c>
       <c r="J101" s="4">
-        <v>367.27244188162382</v>
+        <v>515.32260793412718</v>
       </c>
       <c r="K101" s="4">
-        <v>369.64129385855841</v>
+        <v>510.92331140553443</v>
       </c>
       <c r="L101" s="4">
-        <v>372.0314655032854</v>
+        <v>506.48442120818436</v>
       </c>
       <c r="M101" s="4">
-        <v>374.44314869281487</v>
+        <v>502.00558099905794</v>
       </c>
       <c r="N101" s="4">
-        <v>376.87653703105019</v>
+        <v>497.48643122804981</v>
       </c>
       <c r="O101" s="4">
-        <v>379.33182586432963</v>
+        <v>499.59327577576869</v>
       </c>
       <c r="P101" s="4">
-        <v>381.80921229710856</v>
+        <v>548.95934266979975</v>
       </c>
       <c r="Q101" s="4">
-        <v>384.30889520778254</v>
+        <v>514.26764342049444</v>
       </c>
       <c r="R101" s="4">
-        <v>386.83107526465255</v>
+        <v>647.9994316513596</v>
       </c>
       <c r="S101" s="4">
-        <v>559.1453500145135</v>
+        <v>727.6065598695551</v>
       </c>
       <c r="T101" s="4">
-        <v>558.50448557504785</v>
+        <v>788.04965816464392</v>
       </c>
       <c r="U101" s="4">
-        <v>553.69282594522338</v>
+        <v>777.04310508812569</v>
       </c>
       <c r="V101" s="4">
-        <v>548.83786137872789</v>
+        <v>697.12649303391856</v>
       </c>
       <c r="W101" s="4">
-        <v>543.93920213113915</v>
+        <v>630.63396480455708</v>
       </c>
       <c r="X101" s="4">
-        <v>453.32978828365276</v>
+        <v>551.91472938572554</v>
       </c>
       <c r="Y101" s="4">
-        <v>534.00922304487233</v>
+        <v>483.93349528353025</v>
       </c>
       <c r="Z101" s="4">
-        <v>443.31043938560953</v>
+        <v>485.04242076322117</v>
       </c>
       <c r="AA101" s="5">
         <v>306.51041794508501</v>
@@ -8326,7 +8327,7 @@
         <v>2</v>
       </c>
       <c r="B102" s="6">
-        <v>-734.33333333333326</v>
+        <v>-805</v>
       </c>
       <c r="C102" s="7">
         <v>-58.178333333333171</v>
@@ -8341,64 +8342,64 @@
         <v>-80.306915994937867</v>
       </c>
       <c r="G102" s="7">
-        <v>-87.816278238892238</v>
+        <v>86.694640437442104</v>
       </c>
       <c r="H102" s="7">
-        <v>-95.393224743042111</v>
+        <v>92.294992201379046</v>
       </c>
       <c r="I102" s="7">
-        <v>-103.03836376572943</v>
+        <v>97.945747131191411</v>
       </c>
       <c r="J102" s="7">
-        <v>-110.75230903962093</v>
+        <v>103.64735885537198</v>
       </c>
       <c r="K102" s="7">
-        <v>-118.53567982097748</v>
+        <v>109.40028508507032</v>
       </c>
       <c r="L102" s="7">
-        <v>-126.38910093936613</v>
+        <v>115.20498765083585</v>
       </c>
       <c r="M102" s="7">
-        <v>-134.31320284782035</v>
+        <v>121.06193253969332</v>
       </c>
       <c r="N102" s="7">
-        <v>-142.30862167345052</v>
+        <v>126.97158993255039</v>
       </c>
       <c r="O102" s="7">
-        <v>-150.37599926851158</v>
+        <v>119.60110090861008</v>
       </c>
       <c r="P102" s="7">
-        <v>-158.51598326192814</v>
+        <v>8.6341471107629673</v>
       </c>
       <c r="Q102" s="7">
-        <v>-166.72922711128538</v>
+        <v>-36.770478898573458</v>
       </c>
       <c r="R102" s="7">
-        <v>-175.0163901552869</v>
+        <v>-233.35310292870099</v>
       </c>
       <c r="S102" s="7">
-        <v>-13.608742594205182</v>
+        <v>-349.33934752172598</v>
       </c>
       <c r="T102" s="7">
-        <v>-14.436634982754981</v>
+        <v>-445.70922127755301</v>
       </c>
       <c r="U102" s="7">
-        <v>-8.1444646975998012</v>
+        <v>-467.81960426905101</v>
       </c>
       <c r="V102" s="7">
-        <v>-1.7956648798731294</v>
+        <v>-558.93998070747239</v>
       </c>
       <c r="W102" s="7">
-        <v>4.6102741362026336</v>
+        <v>-636.73710720050633</v>
       </c>
       <c r="X102" s="7">
-        <v>182.4071999367618</v>
+        <v>-726.86268226738366</v>
       </c>
       <c r="Y102" s="7">
-        <v>17.595631402859226</v>
+        <v>-806.35291307445652</v>
       </c>
       <c r="Z102" s="7">
-        <v>195.50942541881818</v>
+        <v>-816.85656526998753</v>
       </c>
       <c r="AA102" s="8">
         <v>-1007.1056589624222</v>
@@ -8409,7 +8410,7 @@
         <v>3</v>
       </c>
       <c r="B103" s="9">
-        <v>418.66666666666663</v>
+        <v>560</v>
       </c>
       <c r="C103" s="10">
         <v>-293.09333333333348</v>
@@ -8424,64 +8425,64 @@
         <v>-277.69953669917368</v>
       </c>
       <c r="G103" s="10">
-        <v>-272.47563252946628</v>
+        <v>-614.98109186763338</v>
       </c>
       <c r="H103" s="10">
-        <v>-267.20471322223165</v>
+        <v>-616.29882169444204</v>
       </c>
       <c r="I103" s="10">
-        <v>-261.88635564123177</v>
+        <v>-617.62841108969201</v>
       </c>
       <c r="J103" s="10">
-        <v>-256.52013284200285</v>
+        <v>-618.96996678949927</v>
       </c>
       <c r="K103" s="10">
-        <v>-251.10561403758089</v>
+        <v>-620.3235964906047</v>
       </c>
       <c r="L103" s="10">
-        <v>-245.64236456391927</v>
+        <v>-621.6894088590202</v>
       </c>
       <c r="M103" s="10">
-        <v>-240.12994584499455</v>
+        <v>-623.06751353875131</v>
       </c>
       <c r="N103" s="10">
-        <v>-234.5679153575997</v>
+        <v>-624.45802116060008</v>
       </c>
       <c r="O103" s="10">
-        <v>-228.95582659581805</v>
+        <v>-619.19437668437877</v>
       </c>
       <c r="P103" s="10">
-        <v>-223.29322903518045</v>
+        <v>-557.59348978056278</v>
       </c>
       <c r="Q103" s="10">
-        <v>-217.57966809649719</v>
+        <v>-477.49716452192098</v>
       </c>
       <c r="R103" s="10">
-        <v>-211.81468510936566</v>
+        <v>-414.64632872265861</v>
       </c>
       <c r="S103" s="10">
-        <v>-545.53660742030831</v>
+        <v>-378.26721234782912</v>
       </c>
       <c r="T103" s="10">
-        <v>-544.06785059229287</v>
+        <v>-342.3404368870909</v>
       </c>
       <c r="U103" s="10">
-        <v>-545.54836124762346</v>
+        <v>-309.22350081907467</v>
       </c>
       <c r="V103" s="10">
-        <v>-547.04219649885476</v>
+        <v>-138.18651232644606</v>
       </c>
       <c r="W103" s="10">
-        <v>-548.54947626734179</v>
+        <v>6.1031423959492486</v>
       </c>
       <c r="X103" s="10">
-        <v>-635.73698822041456</v>
+        <v>174.94795288165824</v>
       </c>
       <c r="Y103" s="10">
-        <v>-551.60485444773144</v>
+        <v>322.41941779092627</v>
       </c>
       <c r="Z103" s="10">
-        <v>-638.81986480442788</v>
+        <v>331.81414450676641</v>
       </c>
       <c r="AA103" s="11">
         <v>700.59524101733723</v>
@@ -8575,86 +8576,86 @@
         <v>6</v>
       </c>
       <c r="B106" s="15">
-        <v>231991.12588150357</v>
+        <v>232337.97601156379</v>
       </c>
       <c r="C106" s="16">
-        <v>190140.63153965469</v>
+        <v>178868.01833794318</v>
       </c>
       <c r="D106" s="16">
-        <v>159339.5469018147</v>
+        <v>26734319.930805065</v>
       </c>
       <c r="E106" s="16">
-        <v>148876.8699338967</v>
+        <v>44929887.883031353</v>
       </c>
       <c r="F106" s="16">
-        <v>141199.76340916852</v>
+        <v>47327429.201370098</v>
       </c>
       <c r="G106" s="16">
-        <v>135372.17299524636</v>
+        <v>47797219.81597846</v>
       </c>
       <c r="H106" s="16">
-        <v>11667050.655674972</v>
+        <v>51716614.661634952</v>
       </c>
       <c r="I106" s="16">
-        <v>12348378.054315709</v>
+        <v>50494819.782062761</v>
       </c>
       <c r="J106" s="16">
-        <v>13751260.723626044</v>
+        <v>48226806.176602289</v>
       </c>
       <c r="K106" s="16">
-        <v>13558784.138956418</v>
+        <v>46428511.624729328</v>
       </c>
       <c r="L106" s="16">
-        <v>15191540.591279879</v>
+        <v>45338069.111478627</v>
       </c>
       <c r="M106" s="16">
-        <v>14684235.406751253</v>
+        <v>43038456.236952685</v>
       </c>
       <c r="N106" s="16">
-        <v>14786955.988124127</v>
+        <v>40494968.262888253</v>
       </c>
       <c r="O106" s="16">
-        <v>14749523.58796652</v>
+        <v>38020554.265129432</v>
       </c>
       <c r="P106" s="16">
-        <v>14596589.087813787</v>
+        <v>40665089.963106111</v>
       </c>
       <c r="Q106" s="16">
-        <v>13650650.813546522</v>
+        <v>39074054.970545374</v>
       </c>
       <c r="R106" s="16">
-        <v>13830801.065545823</v>
+        <v>37244843.974598467</v>
       </c>
       <c r="S106" s="16">
-        <v>13466016.171551844</v>
+        <v>33962535.888263889</v>
       </c>
       <c r="T106" s="16">
-        <v>12859918.526223721</v>
+        <v>31349209.168412223</v>
       </c>
       <c r="U106" s="16">
-        <v>12521090.419230273</v>
+        <v>29103032.433956821</v>
       </c>
       <c r="V106" s="16">
-        <v>11619195.149856256</v>
+        <v>31066219.257415082</v>
       </c>
       <c r="W106" s="16">
-        <v>11445182.458804749</v>
+        <v>28687490.674660448</v>
       </c>
       <c r="X106" s="16">
-        <v>10600356.968824476</v>
+        <v>26517023.592867594</v>
       </c>
       <c r="Y106" s="16">
-        <v>10365533.221142804</v>
+        <v>25815627.381460711</v>
       </c>
       <c r="Z106" s="16">
-        <v>9584881.0747875217</v>
+        <v>21619979.022921167</v>
       </c>
       <c r="AA106" s="17">
-        <v>57754327.603814974</v>
+        <v>28167053.662725583</v>
       </c>
       <c r="AB106" s="18">
         <f>SUM(TotalCost)</f>
-        <v>304039191.81849897</v>
+        <v>904231022.93794632</v>
       </c>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.35">
@@ -8748,86 +8749,86 @@
         <v>8</v>
       </c>
       <c r="B109" s="3">
-        <v>79410814.945039973</v>
+        <v>79196260.980345547</v>
       </c>
       <c r="C109" s="4">
-        <v>63008596.513607681</v>
+        <v>49011597.220977031</v>
       </c>
       <c r="D109" s="4">
-        <v>55897639.429508507</v>
+        <v>39444054.567851424</v>
       </c>
       <c r="E109" s="4">
-        <v>54564500.077389851</v>
+        <v>33663886.082231902</v>
       </c>
       <c r="F109" s="4">
-        <v>50523285.409403026</v>
+        <v>27868604.817414697</v>
       </c>
       <c r="G109" s="4">
-        <v>46943184.414359115</v>
+        <v>23423367.307944994</v>
       </c>
       <c r="H109" s="4">
-        <v>42789651.604352042</v>
+        <v>9949182.2582214996</v>
       </c>
       <c r="I109" s="4">
-        <v>41084451.188129097</v>
+        <v>7985326.2211701991</v>
       </c>
       <c r="J109" s="4">
-        <v>39344839.620549783</v>
+        <v>5459075.0236490462</v>
       </c>
       <c r="K109" s="4">
-        <v>38099783.225653768</v>
+        <v>3903081.6028209636</v>
       </c>
       <c r="L109" s="4">
-        <v>36297990.199881144</v>
+        <v>3144155.2014126806</v>
       </c>
       <c r="M109" s="4">
-        <v>34994910.735631958</v>
+        <v>3101293.8224836946</v>
       </c>
       <c r="N109" s="4">
-        <v>33665749.343199946</v>
+        <v>3310731.4831707757</v>
       </c>
       <c r="O109" s="4">
-        <v>32312324.134227134</v>
+        <v>2977522.3094059438</v>
       </c>
       <c r="P109" s="4">
-        <v>30936358.847758602</v>
+        <v>2199385.6066358062</v>
       </c>
       <c r="Q109" s="4">
-        <v>30066201.364015356</v>
+        <v>1238753.8610101088</v>
       </c>
       <c r="R109" s="4">
-        <v>28075014.638710182</v>
+        <v>1508884.0502892176</v>
       </c>
       <c r="S109" s="4">
-        <v>27637779.666487433</v>
+        <v>2062610.6985920682</v>
       </c>
       <c r="T109" s="4">
-        <v>28104427.366363555</v>
+        <v>1582312.4418347122</v>
       </c>
       <c r="U109" s="4">
-        <v>26480026.546641231</v>
+        <v>1295611.052617806</v>
       </c>
       <c r="V109" s="4">
-        <v>23842430.948070701</v>
+        <v>79937.052314070723</v>
       </c>
       <c r="W109" s="4">
-        <v>21562393.070920121</v>
+        <v>1252884.8933133609</v>
       </c>
       <c r="X109" s="4">
-        <v>18348308.303627428</v>
+        <v>267164.15096759103</v>
       </c>
       <c r="Y109" s="4">
-        <v>17639234.17504514</v>
+        <v>74601.482469535636</v>
       </c>
       <c r="Z109" s="4">
-        <v>15992996.940919366</v>
+        <v>48845.760000000002</v>
       </c>
       <c r="AA109" s="5">
         <v>0</v>
       </c>
       <c r="AB109" s="12">
         <f>SUM(B109:AA109)</f>
-        <v>917622892.70949209</v>
+        <v>304049129.94914466</v>
       </c>
     </row>
     <row r="110" spans="1:28" x14ac:dyDescent="0.35">
@@ -8835,86 +8836,86 @@
         <v>9</v>
       </c>
       <c r="B110" s="6">
-        <v>14667374.743175231</v>
+        <v>14645277.351339288</v>
       </c>
       <c r="C110" s="7">
-        <v>13232177.66341256</v>
+        <v>10157409.364606641</v>
       </c>
       <c r="D110" s="7">
-        <v>13202905.908014387</v>
+        <v>4448155.8269535499</v>
       </c>
       <c r="E110" s="7">
-        <v>11427176.759078516</v>
+        <v>2495598.636821189</v>
       </c>
       <c r="F110" s="7">
-        <v>9446021.7217890956</v>
+        <v>1000824.6732913947</v>
       </c>
       <c r="G110" s="7">
-        <v>6871604.7774165161</v>
+        <v>146237.21522264797</v>
       </c>
       <c r="H110" s="7">
-        <v>5680751.2654034756</v>
+        <v>106268.16191048569</v>
       </c>
       <c r="I110" s="7">
-        <v>5071410.1785333026</v>
+        <v>83814.573600663905</v>
       </c>
       <c r="J110" s="7">
-        <v>4554809.8005604213</v>
+        <v>66277.304234993222</v>
       </c>
       <c r="K110" s="7">
-        <v>3876260.9785867403</v>
+        <v>50243.470512677537</v>
       </c>
       <c r="L110" s="7">
-        <v>3529848.5920510073</v>
+        <v>37081.828776051167</v>
       </c>
       <c r="M110" s="7">
-        <v>3011926.4851294304</v>
+        <v>33544.854792472674</v>
       </c>
       <c r="N110" s="7">
-        <v>2567593.2899408587</v>
+        <v>27660.194820856734</v>
       </c>
       <c r="O110" s="7">
-        <v>2192684.6676832503</v>
+        <v>20640.240606438208</v>
       </c>
       <c r="P110" s="7">
-        <v>1883259.1609973975</v>
+        <v>18033.831241308228</v>
       </c>
       <c r="Q110" s="7">
-        <v>1386087.5782639373</v>
+        <v>13136.771772362054</v>
       </c>
       <c r="R110" s="7">
-        <v>981500.62396597594</v>
+        <v>10391.301281398552</v>
       </c>
       <c r="S110" s="7">
-        <v>2198644.6980367745</v>
+        <v>9142.9197011750366</v>
       </c>
       <c r="T110" s="7">
-        <v>1497195.667705775</v>
+        <v>6083.1588251314861</v>
       </c>
       <c r="U110" s="7">
-        <v>1403701.5010519503</v>
+        <v>5283.338458724631</v>
       </c>
       <c r="V110" s="7">
-        <v>626990.14999876323</v>
+        <v>3316.8852675453695</v>
       </c>
       <c r="W110" s="7">
-        <v>739063.5950360198</v>
+        <v>3146.6558080051545</v>
       </c>
       <c r="X110" s="7">
-        <v>123335.44489582615</v>
+        <v>3088.7874138809761</v>
       </c>
       <c r="Y110" s="7">
-        <v>491512.83514318976</v>
+        <v>2543.9204436243908</v>
       </c>
       <c r="Z110" s="7">
-        <v>111619.72520274097</v>
+        <v>2044</v>
       </c>
       <c r="AA110" s="8">
         <v>0</v>
       </c>
       <c r="AB110" s="13">
         <f t="shared" ref="AB110:AB113" si="0">SUM(B110:AA110)</f>
-        <v>110775457.81107312</v>
+        <v>33395245.267702509</v>
       </c>
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.35">
@@ -8922,86 +8923,86 @@
         <v>10</v>
       </c>
       <c r="B111" s="6">
-        <v>81973843561.409683</v>
+        <v>81984668287.849655</v>
       </c>
       <c r="C111" s="7">
-        <v>77551977702.482712</v>
+        <v>65587734630.279724</v>
       </c>
       <c r="D111" s="7">
-        <v>73368637900.46431</v>
+        <v>52470187704.223778</v>
       </c>
       <c r="E111" s="7">
-        <v>69410957487.382309</v>
+        <v>41976150163.379021</v>
       </c>
       <c r="F111" s="7">
-        <v>65666763854.214943</v>
+        <v>33580920130.703217</v>
       </c>
       <c r="G111" s="7">
-        <v>62124541011.685341</v>
+        <v>26864736104.562572</v>
       </c>
       <c r="H111" s="7">
-        <v>58773394170.616608</v>
+        <v>21491788883.650059</v>
       </c>
       <c r="I111" s="7">
-        <v>55603016232.907539</v>
+        <v>17193431106.920048</v>
       </c>
       <c r="J111" s="7">
-        <v>52603656090.065552</v>
+        <v>13754744885.536039</v>
       </c>
       <c r="K111" s="7">
-        <v>49766088631.792801</v>
+        <v>11003795908.428831</v>
       </c>
       <c r="L111" s="7">
-        <v>47081586372.38118</v>
+        <v>8803036726.7430649</v>
       </c>
       <c r="M111" s="7">
-        <v>44541892607.647644</v>
+        <v>7042429381.3944521</v>
       </c>
       <c r="N111" s="7">
-        <v>42139196019.848877</v>
+        <v>5633943505.1155615</v>
       </c>
       <c r="O111" s="7">
-        <v>39866106652.467781</v>
+        <v>4507154804.0924492</v>
       </c>
       <c r="P111" s="7">
-        <v>37715633180.977707</v>
+        <v>3605723843.2739592</v>
       </c>
       <c r="Q111" s="7">
-        <v>35681161409.67614</v>
+        <v>2884579074.6191673</v>
       </c>
       <c r="R111" s="7">
-        <v>33756433928.450829</v>
+        <v>2307663259.695334</v>
       </c>
       <c r="S111" s="7">
-        <v>31935530866.908764</v>
+        <v>1840771698.1115513</v>
       </c>
       <c r="T111" s="7">
-        <v>30212851686.673626</v>
+        <v>1472617358.4892411</v>
       </c>
       <c r="U111" s="7">
-        <v>28583097955.850403</v>
+        <v>1175531208.2519529</v>
       </c>
       <c r="V111" s="7">
-        <v>27041257052.676739</v>
+        <v>940424966.60156238</v>
       </c>
       <c r="W111" s="7">
-        <v>25582586748.23843</v>
+        <v>752339973.28124988</v>
       </c>
       <c r="X111" s="7">
-        <v>24202600620.830254</v>
+        <v>601871978.62499988</v>
       </c>
       <c r="Y111" s="7">
-        <v>22897054257.101185</v>
+        <v>481497582.89999992</v>
       </c>
       <c r="Z111" s="7">
-        <v>21641622074.728207</v>
+        <v>385198066.31999993</v>
       </c>
       <c r="AA111" s="8">
         <v>0</v>
       </c>
       <c r="AB111" s="13">
         <f t="shared" si="0"/>
-        <v>1139721488077.4795</v>
+        <v>408342941233.04755</v>
       </c>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.35">
@@ -9009,86 +9010,86 @@
         <v>11</v>
       </c>
       <c r="B112" s="6">
-        <v>6683510.9719839878</v>
+        <v>6681389.644961739</v>
       </c>
       <c r="C112" s="7">
-        <v>6599755.8033004701</v>
+        <v>5089910.6879425514</v>
       </c>
       <c r="D112" s="7">
-        <v>6544279.0233887741</v>
+        <v>2826385.9863402438</v>
       </c>
       <c r="E112" s="7">
-        <v>5705298.8174357796</v>
+        <v>1751043.4900144965</v>
       </c>
       <c r="F112" s="7">
-        <v>4781524.5565517489</v>
+        <v>1022523.4479039389</v>
       </c>
       <c r="G112" s="7">
-        <v>3778281.3066065237</v>
+        <v>521009.09283178009</v>
       </c>
       <c r="H112" s="7">
-        <v>3501015.5881168274</v>
+        <v>423166.9297968254</v>
       </c>
       <c r="I112" s="7">
-        <v>3166797.3239359595</v>
+        <v>343111.18398164475</v>
       </c>
       <c r="J112" s="7">
-        <v>2879371.3711778326</v>
+        <v>277067.1602619036</v>
       </c>
       <c r="K112" s="7">
-        <v>2516257.7365025789</v>
+        <v>227081.31208900345</v>
       </c>
       <c r="L112" s="7">
-        <v>2314713.5067413407</v>
+        <v>188062.87885839242</v>
       </c>
       <c r="M112" s="7">
-        <v>2032665.9212198525</v>
+        <v>157455.59680555487</v>
       </c>
       <c r="N112" s="7">
-        <v>1787764.5662852901</v>
+        <v>130235.20959812964</v>
       </c>
       <c r="O112" s="7">
-        <v>1577912.1095002273</v>
+        <v>107925.44918554535</v>
       </c>
       <c r="P112" s="7">
-        <v>1401123.5113920548</v>
+        <v>85219.83809541876</v>
       </c>
       <c r="Q112" s="7">
-        <v>1135654.3381009097</v>
+        <v>74597.24938745625</v>
       </c>
       <c r="R112" s="7">
-        <v>1015535.7440206256</v>
+        <v>65167.162329090585</v>
       </c>
       <c r="S112" s="7">
-        <v>918205.10790448519</v>
+        <v>52449.232825820785</v>
       </c>
       <c r="T112" s="7">
-        <v>785829.59529897617</v>
+        <v>42052.316363354657</v>
       </c>
       <c r="U112" s="7">
-        <v>747026.21964761836</v>
+        <v>34593.844291603818</v>
       </c>
       <c r="V112" s="7">
-        <v>600996.01909194386</v>
+        <v>18194.352856145182</v>
       </c>
       <c r="W112" s="7">
-        <v>591538.01414857048</v>
+        <v>17290.902752033508</v>
       </c>
       <c r="X112" s="7">
-        <v>476052.49032645021</v>
+        <v>14383.255724419125</v>
       </c>
       <c r="Y112" s="7">
-        <v>508691.55552251503</v>
+        <v>10172.865419598049</v>
       </c>
       <c r="Z112" s="7">
-        <v>428144.51811810891</v>
+        <v>8514.7200000000012</v>
       </c>
       <c r="AA112" s="8">
         <v>0</v>
       </c>
       <c r="AB112" s="13">
         <f t="shared" si="0"/>
-        <v>62477945.716319442</v>
+        <v>20169003.810616687</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -9096,87 +9097,90 @@
         <v>12</v>
       </c>
       <c r="B113" s="9">
-        <v>954565.25811419345</v>
+        <v>954323.9115015514</v>
       </c>
       <c r="C113" s="10">
-        <v>943989.55141255865</v>
+        <v>724084.19169989647</v>
       </c>
       <c r="D113" s="10">
-        <v>940524.16925087734</v>
+        <v>387871.85582938354</v>
       </c>
       <c r="E113" s="10">
-        <v>815301.21688416321</v>
+        <v>233186.03075309278</v>
       </c>
       <c r="F113" s="10">
-        <v>676714.90575954237</v>
+        <v>129816.26575595785</v>
       </c>
       <c r="G113" s="10">
-        <v>524404.04177130712</v>
+        <v>59598.580573215862</v>
       </c>
       <c r="H113" s="10">
-        <v>485227.58759383543</v>
+        <v>49290.721455451836</v>
       </c>
       <c r="I113" s="10">
-        <v>437049.61151984037</v>
+        <v>40408.488114570246</v>
       </c>
       <c r="J113" s="10">
-        <v>395920.09887731541</v>
+        <v>32903.242062385179</v>
       </c>
       <c r="K113" s="10">
-        <v>342902.19576538401</v>
+        <v>26975.388011125433</v>
       </c>
       <c r="L113" s="10">
-        <v>314708.21569018275</v>
+        <v>22098.083857299047</v>
       </c>
       <c r="M113" s="10">
-        <v>273899.76101655624</v>
+        <v>18272.173600694357</v>
       </c>
       <c r="N113" s="10">
-        <v>238685.38043025689</v>
+        <v>15268.594601284474</v>
       </c>
       <c r="O113" s="10">
-        <v>208748.84042027534</v>
+        <v>12742.334321534789</v>
       </c>
       <c r="P113" s="10">
-        <v>183790.83558858931</v>
+        <v>10152.982055047942</v>
       </c>
       <c r="Q113" s="10">
-        <v>144985.3975877901</v>
+        <v>8812.5511636612409</v>
       </c>
       <c r="R113" s="10">
-        <v>128540.20325359893</v>
+        <v>7712.0079610489138</v>
       </c>
       <c r="S113" s="10">
-        <v>115288.34094780521</v>
+        <v>6233.8583236086861</v>
       </c>
       <c r="T113" s="10">
-        <v>96956.999820736251</v>
+        <v>4974.3811188486143</v>
       </c>
       <c r="U113" s="10">
-        <v>92765.08912339111</v>
+        <v>4136.0127554535047</v>
       </c>
       <c r="V113" s="10">
-        <v>71824.066707980222</v>
+        <v>2255.3141070181478</v>
       </c>
       <c r="W113" s="10">
-        <v>71616.252369303955</v>
+        <v>2072.371856003866</v>
       </c>
       <c r="X113" s="10">
-        <v>55352.546677292426</v>
+        <v>1724.9069655523904</v>
       </c>
       <c r="Y113" s="10">
-        <v>61345.972085707333</v>
+        <v>1245.3281774497561</v>
       </c>
       <c r="Z113" s="10">
-        <v>50098.321568678766</v>
+        <v>1045.3600000000001</v>
       </c>
       <c r="AA113" s="11">
         <v>0</v>
       </c>
       <c r="AB113" s="14">
         <f t="shared" si="0"/>
-        <v>8625204.8602371626</v>
-      </c>
+        <v>2757204.9366211356</v>
+      </c>
+    </row>
+    <row r="116" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B116" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
limiting wind to 3GW (not binding anyway)
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -1159,10 +1159,10 @@
         <v>0</v>
       </c>
       <c r="AS3" s="4">
-        <v>77.749101751249896</v>
+        <v>77.749101751249668</v>
       </c>
       <c r="AT3" s="4">
-        <v>56.365383667009894</v>
+        <v>56.365383667009723</v>
       </c>
       <c r="AU3" s="4">
         <v>0</v>
@@ -1267,13 +1267,13 @@
         <v>519.20000000000005</v>
       </c>
       <c r="CD3" s="4">
-        <v>507.05524145772756</v>
+        <v>507.05524145772733</v>
       </c>
       <c r="CE3" s="4">
-        <v>403.12527863084802</v>
+        <v>403.12527863084824</v>
       </c>
       <c r="CF3" s="5">
-        <v>289.78994613852274</v>
+        <v>289.78994613852319</v>
       </c>
       <c r="CH3">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>252.25419147572438</v>
       </c>
       <c r="I4" s="7">
-        <v>250.58540577074382</v>
+        <v>250.58540577073563</v>
       </c>
       <c r="J4" s="7">
         <v>665.6</v>
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="AJ4" s="7">
-        <v>90.049622825748486</v>
+        <v>90.049622825741835</v>
       </c>
       <c r="AK4" s="7">
         <v>665.6</v>
@@ -1623,10 +1623,10 @@
         <v>0</v>
       </c>
       <c r="CO4" s="7">
-        <v>336.38616975766672</v>
+        <v>336.38616975766649</v>
       </c>
       <c r="CP4" s="7">
-        <v>307.78388528548544</v>
+        <v>307.78388528548567</v>
       </c>
       <c r="CQ4" s="7">
         <v>665.6</v>
@@ -2439,13 +2439,13 @@
         <v>0</v>
       </c>
       <c r="AK7" s="7">
-        <v>31.167033126886452</v>
+        <v>31.167033126878323</v>
       </c>
       <c r="AL7" s="7">
-        <v>74.462944112259947</v>
+        <v>74.46294411225972</v>
       </c>
       <c r="AM7" s="7">
-        <v>310.55717598544015</v>
+        <v>310.55717598543907</v>
       </c>
       <c r="AN7" s="7">
         <v>464</v>
@@ -2798,7 +2798,7 @@
         <v>101.5</v>
       </c>
       <c r="AV8" s="7">
-        <v>40.414525029093568</v>
+        <v>40.414525029093753</v>
       </c>
       <c r="AW8" s="7">
         <v>0</v>
@@ -2951,7 +2951,7 @@
         <v>0</v>
       </c>
       <c r="CW8" s="7">
-        <v>0</v>
+        <v>-1.1368683772161603E-12</v>
       </c>
       <c r="CX8" s="7">
         <v>0</v>
@@ -3462,7 +3462,7 @@
         <v>88</v>
       </c>
       <c r="AZ10" s="7">
-        <v>49.490626765839238</v>
+        <v>49.490626765839011</v>
       </c>
       <c r="BA10" s="7">
         <v>0</v>
@@ -3737,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="AI11" s="7">
-        <v>197.91334951007471</v>
+        <v>197.91334951006976</v>
       </c>
       <c r="AJ11" s="7">
         <v>650</v>
@@ -4243,7 +4243,7 @@
         <v>0</v>
       </c>
       <c r="CS12" s="7">
-        <v>152.57170090893621</v>
+        <v>152.57170090893624</v>
       </c>
       <c r="CT12" s="7">
         <v>186</v>
@@ -4285,10 +4285,10 @@
         <v>186</v>
       </c>
       <c r="DG12" s="7">
-        <v>184.88064773215137</v>
+        <v>184.88064773215092</v>
       </c>
       <c r="DH12" s="8">
-        <v>53.523313561739087</v>
+        <v>53.523313561738632</v>
       </c>
     </row>
     <row r="13" spans="1:112" x14ac:dyDescent="0.35">
@@ -4425,7 +4425,7 @@
         <v>154</v>
       </c>
       <c r="AU13" s="7">
-        <v>79.419212120013867</v>
+        <v>79.419212120013924</v>
       </c>
       <c r="AV13" s="7">
         <v>0</v>
@@ -4769,7 +4769,7 @@
         <v>150</v>
       </c>
       <c r="BA14" s="7">
-        <v>81.253682406731173</v>
+        <v>81.253682406731286</v>
       </c>
       <c r="BB14" s="7">
         <v>0</v>
@@ -5041,13 +5041,13 @@
         <v>1703.4563686849979</v>
       </c>
       <c r="AI15" s="7">
-        <v>1267.5963664930885</v>
+        <v>1267.5963664930935</v>
       </c>
       <c r="AJ15" s="7">
-        <v>699.90992062144346</v>
+        <v>699.90992062144983</v>
       </c>
       <c r="AK15" s="7">
-        <v>68.042386211329884</v>
+        <v>68.042386211337998</v>
       </c>
       <c r="AL15" s="7">
         <v>0</v>
@@ -5128,10 +5128,10 @@
         <v>1848</v>
       </c>
       <c r="BM15" s="7">
-        <v>1374.982100970934</v>
+        <v>1374.9821009709335</v>
       </c>
       <c r="BN15" s="7">
-        <v>830.71757987967112</v>
+        <v>830.71757987967158</v>
       </c>
       <c r="BO15" s="7">
         <v>817.96367809858828</v>
@@ -5197,13 +5197,13 @@
         <v>1848</v>
       </c>
       <c r="CK15" s="7">
-        <v>1316.4550789999985</v>
+        <v>1316.4550789999987</v>
       </c>
       <c r="CL15" s="7">
         <v>1286.3954147109982</v>
       </c>
       <c r="CM15" s="7">
-        <v>1044.6952134433973</v>
+        <v>1044.6952134433975</v>
       </c>
       <c r="CN15" s="7">
         <v>365.35771036438712</v>
@@ -5388,7 +5388,7 @@
         <v>0</v>
       </c>
       <c r="AP16" s="7">
-        <v>587.53627426530511</v>
+        <v>587.53627426529852</v>
       </c>
       <c r="AQ16" s="7">
         <v>656.1</v>
@@ -5427,16 +5427,16 @@
         <v>619.58260554839126</v>
       </c>
       <c r="BC16" s="7">
-        <v>502.28158899832579</v>
+        <v>502.28158899832533</v>
       </c>
       <c r="BD16" s="8">
-        <v>375.45486329931009</v>
+        <v>375.45486329930964</v>
       </c>
       <c r="BF16">
         <v>14</v>
       </c>
       <c r="BG16" s="6">
-        <v>41.100000000000023</v>
+        <v>41.099999999999852</v>
       </c>
       <c r="BH16" s="7">
         <v>0</v>
@@ -5580,10 +5580,10 @@
         <v>488.61024670354891</v>
       </c>
       <c r="DD16" s="7">
-        <v>365.54047892388007</v>
+        <v>365.54047892387962</v>
       </c>
       <c r="DE16" s="7">
-        <v>242.89308323419459</v>
+        <v>242.89308323419482</v>
       </c>
       <c r="DF16" s="7">
         <v>120.67186098330217</v>
@@ -6196,7 +6196,7 @@
         <v>0</v>
       </c>
       <c r="CR18" s="7">
-        <v>34.339369419977629</v>
+        <v>34.339369419970353</v>
       </c>
       <c r="CS18" s="7">
         <v>67</v>
@@ -6447,7 +6447,7 @@
         <v>257</v>
       </c>
       <c r="BR19" s="7">
-        <v>151.21185152738587</v>
+        <v>151.21185152738599</v>
       </c>
       <c r="BS19" s="7">
         <v>0</v>
@@ -6581,7 +6581,7 @@
         <v>1996</v>
       </c>
       <c r="C20" s="7">
-        <v>1804.3642379757423</v>
+        <v>1804.3642379757473</v>
       </c>
       <c r="D20" s="7">
         <v>2269.6</v>
@@ -6599,7 +6599,7 @@
         <v>2269.6</v>
       </c>
       <c r="I20" s="7">
-        <v>2241.1374734282622</v>
+        <v>2241.1374734282699</v>
       </c>
       <c r="J20" s="7">
         <v>1796.3503851117962</v>
@@ -6617,7 +6617,7 @@
         <v>368.31361546809046</v>
       </c>
       <c r="O20" s="7">
-        <v>20.751948466969726</v>
+        <v>20.751948466977961</v>
       </c>
       <c r="P20" s="7">
         <v>0</v>
@@ -6683,16 +6683,16 @@
         <v>2269.6</v>
       </c>
       <c r="AM20" s="7">
-        <v>2009.1665746238293</v>
+        <v>2009.1665746238302</v>
       </c>
       <c r="AN20" s="7">
-        <v>1831.7955043647521</v>
+        <v>1831.7955043647517</v>
       </c>
       <c r="AO20" s="7">
         <v>1951.7819039040342</v>
       </c>
       <c r="AP20" s="7">
-        <v>1155.1504067738651</v>
+        <v>1155.1504067738722</v>
       </c>
       <c r="AQ20" s="7">
         <v>913.91360116852263</v>
@@ -6779,22 +6779,22 @@
         <v>2172.1467981911323</v>
       </c>
       <c r="BT20" s="7">
-        <v>1763.7157593748525</v>
+        <v>1763.715759374852</v>
       </c>
       <c r="BU20" s="7">
-        <v>929.123541209226</v>
+        <v>929.12354120922623</v>
       </c>
       <c r="BV20" s="7">
-        <v>920.07499308010574</v>
+        <v>920.07499308010551</v>
       </c>
       <c r="BW20" s="7">
-        <v>801.57500801782703</v>
+        <v>801.57500801782726</v>
       </c>
       <c r="BX20" s="7">
         <v>673.62852308998572</v>
       </c>
       <c r="BY20" s="7">
-        <v>546.24051979779642</v>
+        <v>546.24051979779597</v>
       </c>
       <c r="BZ20" s="7">
         <v>419.41602447597529</v>
@@ -6848,13 +6848,13 @@
         <v>1419.5541802530538</v>
       </c>
       <c r="CR20" s="7">
-        <v>1357.3610384553535</v>
+        <v>1357.3610384553608</v>
       </c>
       <c r="CS20" s="7">
-        <v>1355.1542506372725</v>
+        <v>1355.1542506372728</v>
       </c>
       <c r="CT20" s="7">
-        <v>638.53422511012457</v>
+        <v>638.53422511012468</v>
       </c>
       <c r="CU20" s="7">
         <v>373.82867313611484</v>
@@ -7269,13 +7269,13 @@
         <v>0</v>
       </c>
       <c r="O22" s="7">
-        <v>231.63228954033303</v>
+        <v>231.63228954032482</v>
       </c>
       <c r="P22" s="7">
-        <v>224.83349614936822</v>
+        <v>224.83349614936799</v>
       </c>
       <c r="Q22" s="7">
-        <v>197.66479761471226</v>
+        <v>197.66479761471248</v>
       </c>
       <c r="R22" s="7">
         <v>60.881580793244211</v>
@@ -7515,16 +7515,16 @@
         <v>347.51277119433951</v>
       </c>
       <c r="CW22" s="7">
-        <v>321.59002613508773</v>
+        <v>321.59002613508864</v>
       </c>
       <c r="CX22" s="7">
         <v>296.06397637030284</v>
       </c>
       <c r="CY22" s="7">
-        <v>160.93819215763529</v>
+        <v>160.93819215763506</v>
       </c>
       <c r="CZ22" s="7">
-        <v>16.216275887053712</v>
+        <v>16.216275887053825</v>
       </c>
       <c r="DA22" s="7">
         <v>0</v>
@@ -7571,25 +7571,25 @@
         <v>14.050000000000004</v>
       </c>
       <c r="G23" s="7">
+        <v>14.05</v>
+      </c>
+      <c r="H23" s="7">
+        <v>14.05</v>
+      </c>
+      <c r="I23" s="7">
         <v>14.049999999999997</v>
       </c>
-      <c r="H23" s="7">
-        <v>14.049999999999997</v>
-      </c>
-      <c r="I23" s="7">
+      <c r="J23" s="7">
         <v>14.05</v>
       </c>
-      <c r="J23" s="7">
-        <v>14.049999999999997</v>
-      </c>
       <c r="K23" s="7">
-        <v>14.049999999999997</v>
+        <v>14.050000000000004</v>
       </c>
       <c r="L23" s="7">
-        <v>14.050000000000004</v>
+        <v>14.05</v>
       </c>
       <c r="M23" s="7">
-        <v>14.049999999999997</v>
+        <v>14.05</v>
       </c>
       <c r="N23" s="7">
         <v>14.049999999999997</v>
@@ -7622,16 +7622,16 @@
         <v>14.049999999999997</v>
       </c>
       <c r="X23" s="7">
+        <v>14.049999999999997</v>
+      </c>
+      <c r="Y23" s="7">
         <v>14.050000000000004</v>
       </c>
-      <c r="Y23" s="7">
+      <c r="Z23" s="7">
+        <v>14.049999999999997</v>
+      </c>
+      <c r="AA23" s="8">
         <v>14.05</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>14.050000000000004</v>
-      </c>
-      <c r="AA23" s="8">
-        <v>14.049999999999997</v>
       </c>
       <c r="AD23">
         <v>21</v>
@@ -7652,7 +7652,7 @@
         <v>19.670000000000002</v>
       </c>
       <c r="AJ23" s="7">
-        <v>19.670000000000002</v>
+        <v>19.669999999999998</v>
       </c>
       <c r="AK23" s="7">
         <v>19.670000000000002</v>
@@ -7667,10 +7667,10 @@
         <v>19.669999999999998</v>
       </c>
       <c r="AO23" s="7">
-        <v>19.670000000000002</v>
+        <v>19.669999999999995</v>
       </c>
       <c r="AP23" s="7">
-        <v>19.670000000000002</v>
+        <v>19.669999999999995</v>
       </c>
       <c r="AQ23" s="7">
         <v>19.670000000000002</v>
@@ -7706,13 +7706,13 @@
         <v>19.670000000000002</v>
       </c>
       <c r="BB23" s="7">
-        <v>19.670000000000002</v>
+        <v>19.669999999999998</v>
       </c>
       <c r="BC23" s="7">
         <v>19.670000000000002</v>
       </c>
       <c r="BD23" s="8">
-        <v>19.670000000000002</v>
+        <v>19.669999999999998</v>
       </c>
       <c r="BF23">
         <v>21</v>
@@ -7733,25 +7733,25 @@
         <v>19.670000000000002</v>
       </c>
       <c r="BL23" s="7">
-        <v>19.669999999999998</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="BM23" s="7">
         <v>19.670000000000002</v>
       </c>
       <c r="BN23" s="7">
+        <v>19.669999999999995</v>
+      </c>
+      <c r="BO23" s="7">
         <v>19.670000000000002</v>
-      </c>
-      <c r="BO23" s="7">
-        <v>19.669999999999998</v>
       </c>
       <c r="BP23" s="7">
         <v>19.670000000000002</v>
       </c>
       <c r="BQ23" s="7">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="BR23" s="7">
         <v>19.669999999999998</v>
-      </c>
-      <c r="BR23" s="7">
-        <v>19.669999999999995</v>
       </c>
       <c r="BS23" s="7">
         <v>19.670000000000002</v>
@@ -7784,10 +7784,10 @@
         <v>19.670000000000002</v>
       </c>
       <c r="CC23" s="7">
-        <v>19.669999999999995</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="CD23" s="7">
-        <v>19.669999999999998</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="CE23" s="7">
         <v>19.670000000000002</v>
@@ -7814,19 +7814,19 @@
         <v>19.670000000000002</v>
       </c>
       <c r="CN23" s="7">
-        <v>19.669999999999998</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="CO23" s="7">
         <v>19.669999999999995</v>
       </c>
       <c r="CP23" s="7">
-        <v>19.670000000000002</v>
+        <v>19.669999999999998</v>
       </c>
       <c r="CQ23" s="7">
+        <v>19.669999999999995</v>
+      </c>
+      <c r="CR23" s="7">
         <v>19.669999999999998</v>
-      </c>
-      <c r="CR23" s="7">
-        <v>19.670000000000002</v>
       </c>
       <c r="CS23" s="7">
         <v>19.670000000000002</v>
@@ -7871,10 +7871,10 @@
         <v>19.670000000000002</v>
       </c>
       <c r="DG23" s="7">
-        <v>19.670000000000002</v>
+        <v>19.669999999999995</v>
       </c>
       <c r="DH23" s="8">
-        <v>19.670000000000002</v>
+        <v>19.669999999999995</v>
       </c>
     </row>
     <row r="24" spans="1:112" x14ac:dyDescent="0.35">
@@ -7981,7 +7981,7 @@
         <v>17.5</v>
       </c>
       <c r="AK24" s="7">
-        <v>17.499999999999993</v>
+        <v>17.5</v>
       </c>
       <c r="AL24" s="7">
         <v>17.5</v>
@@ -8080,7 +8080,7 @@
         <v>17.5</v>
       </c>
       <c r="BS24" s="7">
-        <v>17.499999999999993</v>
+        <v>17.5</v>
       </c>
       <c r="BT24" s="7">
         <v>17.5</v>
@@ -8110,7 +8110,7 @@
         <v>17.5</v>
       </c>
       <c r="CC24" s="7">
-        <v>17.5</v>
+        <v>17.499999999999993</v>
       </c>
       <c r="CD24" s="7">
         <v>17.5</v>
@@ -8200,7 +8200,7 @@
         <v>17.499999999999993</v>
       </c>
       <c r="DH24" s="8">
-        <v>17.5</v>
+        <v>17.499999999999993</v>
       </c>
     </row>
     <row r="25" spans="1:112" x14ac:dyDescent="0.35">
@@ -8211,7 +8211,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="7">
-        <v>22.067762024257036</v>
+        <v>22.067762024252033</v>
       </c>
       <c r="D25" s="7">
         <v>35</v>
@@ -8304,7 +8304,7 @@
         <v>49</v>
       </c>
       <c r="AJ25" s="7">
-        <v>48.999999999999993</v>
+        <v>49</v>
       </c>
       <c r="AK25" s="7">
         <v>49</v>
@@ -8316,13 +8316,13 @@
         <v>49</v>
       </c>
       <c r="AN25" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="AO25" s="7">
         <v>49</v>
       </c>
       <c r="AP25" s="7">
-        <v>48.999999999999993</v>
+        <v>49</v>
       </c>
       <c r="AQ25" s="7">
         <v>49</v>
@@ -8364,7 +8364,7 @@
         <v>49</v>
       </c>
       <c r="BD25" s="8">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="BF25">
         <v>23</v>
@@ -8388,7 +8388,7 @@
         <v>49</v>
       </c>
       <c r="BM25" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="BN25" s="7">
         <v>49</v>
@@ -8400,7 +8400,7 @@
         <v>49</v>
       </c>
       <c r="BQ25" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="BR25" s="7">
         <v>49</v>
@@ -8436,13 +8436,13 @@
         <v>49</v>
       </c>
       <c r="CC25" s="7">
+        <v>49</v>
+      </c>
+      <c r="CD25" s="7">
         <v>48.999999999999993</v>
       </c>
-      <c r="CD25" s="7">
+      <c r="CE25" s="7">
         <v>49</v>
-      </c>
-      <c r="CE25" s="7">
-        <v>48.999999999999993</v>
       </c>
       <c r="CF25" s="8">
         <v>49</v>
@@ -8469,10 +8469,10 @@
         <v>49</v>
       </c>
       <c r="CO25" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="CP25" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="CQ25" s="7">
         <v>49</v>
@@ -8481,10 +8481,10 @@
         <v>49</v>
       </c>
       <c r="CS25" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="CT25" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="CU25" s="7">
         <v>49</v>
@@ -8517,7 +8517,7 @@
         <v>49</v>
       </c>
       <c r="DE25" s="7">
-        <v>48.999999999999993</v>
+        <v>49</v>
       </c>
       <c r="DF25" s="7">
         <v>48.999999999999993</v>
@@ -8552,7 +8552,7 @@
         <v>15.3</v>
       </c>
       <c r="H26" s="7">
-        <v>15.299999999999999</v>
+        <v>15.3</v>
       </c>
       <c r="I26" s="7">
         <v>15.3</v>
@@ -8609,7 +8609,7 @@
         <v>15.3</v>
       </c>
       <c r="AA26" s="8">
-        <v>15.3</v>
+        <v>15.299999999999999</v>
       </c>
       <c r="AD26">
         <v>24</v>
@@ -8630,7 +8630,7 @@
         <v>21.419999999999998</v>
       </c>
       <c r="AJ26" s="7">
-        <v>21.419999999999995</v>
+        <v>21.419999999999998</v>
       </c>
       <c r="AK26" s="7">
         <v>21.419999999999998</v>
@@ -8642,10 +8642,10 @@
         <v>21.419999999999998</v>
       </c>
       <c r="AN26" s="7">
+        <v>21.419999999999998</v>
+      </c>
+      <c r="AO26" s="7">
         <v>21.419999999999995</v>
-      </c>
-      <c r="AO26" s="7">
-        <v>21.419999999999998</v>
       </c>
       <c r="AP26" s="7">
         <v>21.419999999999998</v>
@@ -8684,10 +8684,10 @@
         <v>21.419999999999998</v>
       </c>
       <c r="BB26" s="7">
-        <v>21.419999999999998</v>
+        <v>21.419999999999995</v>
       </c>
       <c r="BC26" s="7">
-        <v>21.419999999999998</v>
+        <v>21.419999999999995</v>
       </c>
       <c r="BD26" s="8">
         <v>21.419999999999998</v>
@@ -8714,7 +8714,7 @@
         <v>21.419999999999998</v>
       </c>
       <c r="BM26" s="7">
-        <v>21.419999999999998</v>
+        <v>21.419999999999995</v>
       </c>
       <c r="BN26" s="7">
         <v>21.419999999999998</v>
@@ -8765,13 +8765,13 @@
         <v>21.419999999999998</v>
       </c>
       <c r="CD26" s="7">
-        <v>21.419999999999998</v>
+        <v>21.419999999999995</v>
       </c>
       <c r="CE26" s="7">
         <v>21.419999999999995</v>
       </c>
       <c r="CF26" s="8">
-        <v>21.419999999999998</v>
+        <v>21.419999999999995</v>
       </c>
       <c r="CH26">
         <v>24</v>
@@ -8801,7 +8801,7 @@
         <v>21.419999999999998</v>
       </c>
       <c r="CQ26" s="7">
-        <v>21.419999999999995</v>
+        <v>21.419999999999998</v>
       </c>
       <c r="CR26" s="7">
         <v>21.419999999999998</v>
@@ -8846,7 +8846,7 @@
         <v>21.419999999999998</v>
       </c>
       <c r="DF26" s="7">
-        <v>21.419999999999998</v>
+        <v>21.419999999999995</v>
       </c>
       <c r="DG26" s="7">
         <v>21.419999999999998</v>
@@ -8875,7 +8875,7 @@
         <v>5</v>
       </c>
       <c r="G27" s="7">
-        <v>5</v>
+        <v>4.9999999999999964</v>
       </c>
       <c r="H27" s="7">
         <v>5</v>
@@ -8965,7 +8965,7 @@
         <v>7</v>
       </c>
       <c r="AM27" s="7">
-        <v>7.0000000000000018</v>
+        <v>7</v>
       </c>
       <c r="AN27" s="7">
         <v>7</v>
@@ -9007,13 +9007,13 @@
         <v>7</v>
       </c>
       <c r="BA27" s="7">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
       <c r="BB27" s="7">
-        <v>7.0000000000000018</v>
+        <v>7</v>
       </c>
       <c r="BC27" s="7">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
       <c r="BD27" s="8">
         <v>7</v>
@@ -9046,7 +9046,7 @@
         <v>7</v>
       </c>
       <c r="BO27" s="7">
-        <v>7.0000000000000036</v>
+        <v>7</v>
       </c>
       <c r="BP27" s="7">
         <v>7</v>
@@ -9127,7 +9127,7 @@
         <v>7</v>
       </c>
       <c r="CQ27" s="7">
-        <v>7.0000000000000036</v>
+        <v>7</v>
       </c>
       <c r="CR27" s="7">
         <v>7</v>
@@ -9291,7 +9291,7 @@
         <v>7</v>
       </c>
       <c r="AM28" s="7">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
       <c r="AN28" s="7">
         <v>7</v>
@@ -9333,10 +9333,10 @@
         <v>7</v>
       </c>
       <c r="BA28" s="7">
-        <v>7</v>
+        <v>7.0000000000000018</v>
       </c>
       <c r="BB28" s="7">
-        <v>7</v>
+        <v>7.0000000000000036</v>
       </c>
       <c r="BC28" s="7">
         <v>7</v>
@@ -9420,7 +9420,7 @@
         <v>7</v>
       </c>
       <c r="CE28" s="7">
-        <v>7.0000000000000018</v>
+        <v>7</v>
       </c>
       <c r="CF28" s="8">
         <v>7</v>
@@ -9492,7 +9492,7 @@
         <v>7</v>
       </c>
       <c r="DD28" s="7">
-        <v>7.0000000000000018</v>
+        <v>7</v>
       </c>
       <c r="DE28" s="7">
         <v>7</v>
@@ -9578,7 +9578,7 @@
         <v>5</v>
       </c>
       <c r="X29" s="7">
-        <v>5</v>
+        <v>4.9999999999999929</v>
       </c>
       <c r="Y29" s="7">
         <v>5</v>
@@ -9596,7 +9596,7 @@
         <v>0</v>
       </c>
       <c r="AF29" s="7">
-        <v>0.12499999999958789</v>
+        <v>7</v>
       </c>
       <c r="AG29" s="7">
         <v>7</v>
@@ -9611,7 +9611,7 @@
         <v>7</v>
       </c>
       <c r="AK29" s="7">
-        <v>7</v>
+        <v>6.9999999999999929</v>
       </c>
       <c r="AL29" s="7">
         <v>7</v>
@@ -9626,7 +9626,7 @@
         <v>7</v>
       </c>
       <c r="AP29" s="7">
-        <v>7.0000000000000018</v>
+        <v>7</v>
       </c>
       <c r="AQ29" s="7">
         <v>7</v>
@@ -9707,7 +9707,7 @@
         <v>7</v>
       </c>
       <c r="BR29" s="7">
-        <v>7</v>
+        <v>7.0000000000000036</v>
       </c>
       <c r="BS29" s="7">
         <v>7</v>
@@ -9856,19 +9856,19 @@
         <v>26.100000000000009</v>
       </c>
       <c r="H30" s="7">
-        <v>26.100000000000009</v>
+        <v>26.1</v>
       </c>
       <c r="I30" s="7">
+        <v>26.1</v>
+      </c>
+      <c r="J30" s="7">
         <v>26.100000000000005</v>
       </c>
-      <c r="J30" s="7">
-        <v>26.100000000000009</v>
-      </c>
       <c r="K30" s="7">
-        <v>26.100000000000009</v>
+        <v>26.1</v>
       </c>
       <c r="L30" s="7">
-        <v>26.1</v>
+        <v>26.100000000000005</v>
       </c>
       <c r="M30" s="7">
         <v>26.100000000000009</v>
@@ -9907,13 +9907,13 @@
         <v>26.1</v>
       </c>
       <c r="Y30" s="7">
-        <v>26.100000000000005</v>
+        <v>26.1</v>
       </c>
       <c r="Z30" s="7">
         <v>26.1</v>
       </c>
       <c r="AA30" s="8">
-        <v>26.1</v>
+        <v>26.100000000000009</v>
       </c>
       <c r="AD30">
         <v>28</v>
@@ -9934,25 +9934,25 @@
         <v>36.54</v>
       </c>
       <c r="AJ30" s="7">
+        <v>36.540000000000006</v>
+      </c>
+      <c r="AK30" s="7">
         <v>36.54</v>
-      </c>
-      <c r="AK30" s="7">
-        <v>36.539999999999992</v>
       </c>
       <c r="AL30" s="7">
         <v>36.54</v>
       </c>
       <c r="AM30" s="7">
+        <v>36.539999999999992</v>
+      </c>
+      <c r="AN30" s="7">
+        <v>36.540000000000006</v>
+      </c>
+      <c r="AO30" s="7">
         <v>36.54</v>
       </c>
-      <c r="AN30" s="7">
+      <c r="AP30" s="7">
         <v>36.54</v>
-      </c>
-      <c r="AO30" s="7">
-        <v>36.540000000000006</v>
-      </c>
-      <c r="AP30" s="7">
-        <v>36.539999999999992</v>
       </c>
       <c r="AQ30" s="7">
         <v>36.54</v>
@@ -9994,7 +9994,7 @@
         <v>36.54</v>
       </c>
       <c r="BD30" s="8">
-        <v>36.54</v>
+        <v>36.540000000000006</v>
       </c>
       <c r="BF30">
         <v>28</v>
@@ -10018,13 +10018,13 @@
         <v>36.539999999999992</v>
       </c>
       <c r="BM30" s="7">
+        <v>36.54</v>
+      </c>
+      <c r="BN30" s="7">
         <v>36.539999999999992</v>
       </c>
-      <c r="BN30" s="7">
-        <v>36.54</v>
-      </c>
       <c r="BO30" s="7">
-        <v>36.54</v>
+        <v>36.540000000000006</v>
       </c>
       <c r="BP30" s="7">
         <v>36.54</v>
@@ -10069,10 +10069,10 @@
         <v>36.54</v>
       </c>
       <c r="CD30" s="7">
+        <v>36.539999999999992</v>
+      </c>
+      <c r="CE30" s="7">
         <v>36.54</v>
-      </c>
-      <c r="CE30" s="7">
-        <v>36.539999999999992</v>
       </c>
       <c r="CF30" s="8">
         <v>36.54</v>
@@ -10096,25 +10096,25 @@
         <v>36.54</v>
       </c>
       <c r="CN30" s="7">
+        <v>36.54</v>
+      </c>
+      <c r="CO30" s="7">
+        <v>36.54</v>
+      </c>
+      <c r="CP30" s="7">
+        <v>36.540000000000006</v>
+      </c>
+      <c r="CQ30" s="7">
         <v>36.539999999999992</v>
       </c>
-      <c r="CO30" s="7">
-        <v>36.539999999999992</v>
-      </c>
-      <c r="CP30" s="7">
-        <v>36.539999999999992</v>
-      </c>
-      <c r="CQ30" s="7">
-        <v>36.54</v>
-      </c>
       <c r="CR30" s="7">
-        <v>36.54</v>
+        <v>36.540000000000006</v>
       </c>
       <c r="CS30" s="7">
         <v>36.539999999999992</v>
       </c>
       <c r="CT30" s="7">
-        <v>36.54</v>
+        <v>36.539999999999992</v>
       </c>
       <c r="CU30" s="7">
         <v>36.54</v>
@@ -10144,16 +10144,16 @@
         <v>36.539999999999992</v>
       </c>
       <c r="DD30" s="7">
-        <v>36.54</v>
+        <v>36.539999999999992</v>
       </c>
       <c r="DE30" s="7">
         <v>36.54</v>
       </c>
       <c r="DF30" s="7">
+        <v>36.54</v>
+      </c>
+      <c r="DG30" s="7">
         <v>36.539999999999992</v>
-      </c>
-      <c r="DG30" s="7">
-        <v>36.540000000000006</v>
       </c>
       <c r="DH30" s="8">
         <v>36.54</v>
@@ -10239,7 +10239,7 @@
         <v>5</v>
       </c>
       <c r="AA31" s="8">
-        <v>5</v>
+        <v>4.9999999999999964</v>
       </c>
       <c r="AD31">
         <v>29</v>
@@ -10272,7 +10272,7 @@
         <v>7</v>
       </c>
       <c r="AN31" s="7">
-        <v>7</v>
+        <v>7.0000000000000036</v>
       </c>
       <c r="AO31" s="7">
         <v>7</v>
@@ -10353,10 +10353,10 @@
         <v>7</v>
       </c>
       <c r="BP31" s="7">
+        <v>7</v>
+      </c>
+      <c r="BQ31" s="7">
         <v>6.9999999999999929</v>
-      </c>
-      <c r="BQ31" s="7">
-        <v>7</v>
       </c>
       <c r="BR31" s="7">
         <v>7</v>
@@ -10508,10 +10508,10 @@
         <v>10.099999999999998</v>
       </c>
       <c r="H32" s="7">
-        <v>10.1</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="I32" s="7">
-        <v>10.099999999999998</v>
+        <v>10.100000000000001</v>
       </c>
       <c r="J32" s="7">
         <v>10.100000000000001</v>
@@ -10520,10 +10520,10 @@
         <v>10.100000000000001</v>
       </c>
       <c r="L32" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="M32" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="N32" s="7">
         <v>10.100000000000001</v>
@@ -10559,13 +10559,13 @@
         <v>10.100000000000001</v>
       </c>
       <c r="Y32" s="7">
-        <v>10.100000000000001</v>
+        <v>10.099999999999998</v>
       </c>
       <c r="Z32" s="7">
         <v>10.100000000000001</v>
       </c>
       <c r="AA32" s="8">
-        <v>10.100000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="AD32">
         <v>30</v>
@@ -10598,10 +10598,10 @@
         <v>14.139999999999997</v>
       </c>
       <c r="AN32" s="7">
+        <v>14.139999999999997</v>
+      </c>
+      <c r="AO32" s="7">
         <v>14.139999999999999</v>
-      </c>
-      <c r="AO32" s="7">
-        <v>14.139999999999997</v>
       </c>
       <c r="AP32" s="7">
         <v>14.139999999999997</v>
@@ -10634,16 +10634,16 @@
         <v>14.139999999999999</v>
       </c>
       <c r="AZ32" s="7">
-        <v>14.139999999999997</v>
+        <v>14.139999999999999</v>
       </c>
       <c r="BA32" s="7">
         <v>14.139999999999999</v>
       </c>
       <c r="BB32" s="7">
-        <v>14.139999999999997</v>
+        <v>14.139999999999999</v>
       </c>
       <c r="BC32" s="7">
-        <v>14.139999999999997</v>
+        <v>14.139999999999999</v>
       </c>
       <c r="BD32" s="8">
         <v>14.139999999999997</v>
@@ -10679,7 +10679,7 @@
         <v>14.139999999999997</v>
       </c>
       <c r="BP32" s="7">
-        <v>14.139999999999997</v>
+        <v>14.139999999999999</v>
       </c>
       <c r="BQ32" s="7">
         <v>14.139999999999997</v>
@@ -10721,13 +10721,13 @@
         <v>14.139999999999997</v>
       </c>
       <c r="CD32" s="7">
-        <v>14.139999999999997</v>
+        <v>14.139999999999999</v>
       </c>
       <c r="CE32" s="7">
         <v>14.139999999999999</v>
       </c>
       <c r="CF32" s="8">
-        <v>14.139999999999997</v>
+        <v>14.139999999999999</v>
       </c>
       <c r="CH32">
         <v>30</v>
@@ -10763,7 +10763,7 @@
         <v>14.139999999999997</v>
       </c>
       <c r="CS32" s="7">
-        <v>14.139999999999997</v>
+        <v>14.139999999999999</v>
       </c>
       <c r="CT32" s="7">
         <v>14.139999999999997</v>
@@ -10802,7 +10802,7 @@
         <v>14.139999999999997</v>
       </c>
       <c r="DF32" s="7">
-        <v>14.139999999999997</v>
+        <v>14.139999999999999</v>
       </c>
       <c r="DG32" s="7">
         <v>14.139999999999997</v>
@@ -10918,7 +10918,7 @@
         <v>49</v>
       </c>
       <c r="AL33" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="AM33" s="7">
         <v>49</v>
@@ -10930,7 +10930,7 @@
         <v>48.999999999999993</v>
       </c>
       <c r="AP33" s="7">
-        <v>49</v>
+        <v>48.999999999999993</v>
       </c>
       <c r="AQ33" s="7">
         <v>49</v>
@@ -10963,7 +10963,7 @@
         <v>49</v>
       </c>
       <c r="BA33" s="7">
-        <v>48.999999999999993</v>
+        <v>49</v>
       </c>
       <c r="BB33" s="7">
         <v>49</v>
@@ -10993,19 +10993,19 @@
         <v>49</v>
       </c>
       <c r="BL33" s="7">
-        <v>48.999999999999993</v>
+        <v>49</v>
       </c>
       <c r="BM33" s="7">
         <v>49</v>
       </c>
       <c r="BN33" s="7">
+        <v>48.999999999999993</v>
+      </c>
+      <c r="BO33" s="7">
         <v>49</v>
       </c>
-      <c r="BO33" s="7">
+      <c r="BP33" s="7">
         <v>48.999999999999993</v>
-      </c>
-      <c r="BP33" s="7">
-        <v>49</v>
       </c>
       <c r="BQ33" s="7">
         <v>49</v>
@@ -11160,10 +11160,10 @@
         <v>5.25</v>
       </c>
       <c r="H34" s="7">
-        <v>5.25</v>
+        <v>5.2499999999999964</v>
       </c>
       <c r="I34" s="7">
-        <v>5.25</v>
+        <v>5.2499999999999929</v>
       </c>
       <c r="J34" s="7">
         <v>5.25</v>
@@ -11217,7 +11217,7 @@
         <v>5.25</v>
       </c>
       <c r="AA34" s="8">
-        <v>5.2499999999999929</v>
+        <v>5.25</v>
       </c>
       <c r="AD34">
         <v>32</v>
@@ -11238,7 +11238,7 @@
         <v>7.3499999999999943</v>
       </c>
       <c r="AJ34" s="7">
-        <v>7.3499999999999943</v>
+        <v>7.3499999999999979</v>
       </c>
       <c r="AK34" s="7">
         <v>7.3499999999999943</v>
@@ -11247,16 +11247,16 @@
         <v>7.3500000000000014</v>
       </c>
       <c r="AM34" s="7">
-        <v>7.35</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="AN34" s="7">
-        <v>7.3499999999999979</v>
+        <v>7.3500000000000014</v>
       </c>
       <c r="AO34" s="7">
-        <v>7.3500000000000014</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="AP34" s="7">
-        <v>7.35</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="AQ34" s="7">
         <v>7.3499999999999943</v>
@@ -11292,13 +11292,13 @@
         <v>7.35</v>
       </c>
       <c r="BB34" s="7">
-        <v>7.35</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="BC34" s="7">
-        <v>7.35</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="BD34" s="8">
-        <v>7.3499999999999943</v>
+        <v>7.3500000000000014</v>
       </c>
       <c r="BF34">
         <v>32</v>
@@ -11322,22 +11322,22 @@
         <v>7.3499999999999943</v>
       </c>
       <c r="BM34" s="7">
-        <v>7.3500000000000014</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="BN34" s="7">
-        <v>7.3500000000000014</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="BO34" s="7">
-        <v>7.3500000000000014</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="BP34" s="7">
         <v>7.3499999999999943</v>
       </c>
       <c r="BQ34" s="7">
+        <v>7.3499999999999943</v>
+      </c>
+      <c r="BR34" s="7">
         <v>7.3500000000000014</v>
-      </c>
-      <c r="BR34" s="7">
-        <v>7.35</v>
       </c>
       <c r="BS34" s="7">
         <v>7.3500000000000014</v>
@@ -11370,13 +11370,13 @@
         <v>7.3499999999999943</v>
       </c>
       <c r="CC34" s="7">
+        <v>7.3499999999999943</v>
+      </c>
+      <c r="CD34" s="7">
         <v>7.3500000000000014</v>
       </c>
-      <c r="CD34" s="7">
-        <v>7.3499999999999979</v>
-      </c>
       <c r="CE34" s="7">
-        <v>7.35</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="CF34" s="8">
         <v>7.3499999999999943</v>
@@ -11403,22 +11403,22 @@
         <v>7.3499999999999943</v>
       </c>
       <c r="CO34" s="7">
+        <v>7.3500000000000014</v>
+      </c>
+      <c r="CP34" s="7">
+        <v>7.3499999999999979</v>
+      </c>
+      <c r="CQ34" s="7">
         <v>7.3499999999999943</v>
       </c>
-      <c r="CP34" s="7">
-        <v>7.3500000000000014</v>
-      </c>
-      <c r="CQ34" s="7">
-        <v>7.3500000000000014</v>
-      </c>
       <c r="CR34" s="7">
-        <v>7.3499999999999943</v>
+        <v>7.3499999999999979</v>
       </c>
       <c r="CS34" s="7">
         <v>7.3499999999999943</v>
       </c>
       <c r="CT34" s="7">
-        <v>7.3500000000000014</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="CU34" s="7">
         <v>7.3499999999999943</v>
@@ -11448,19 +11448,19 @@
         <v>7.3499999999999943</v>
       </c>
       <c r="DD34" s="7">
-        <v>7.35</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="DE34" s="7">
-        <v>7.35</v>
+        <v>7.3500000000000014</v>
       </c>
       <c r="DF34" s="7">
-        <v>7.35</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="DG34" s="7">
-        <v>7.35</v>
+        <v>7.3499999999999943</v>
       </c>
       <c r="DH34" s="8">
-        <v>7.3500000000000014</v>
+        <v>7.3499999999999943</v>
       </c>
     </row>
     <row r="35" spans="1:112" x14ac:dyDescent="0.35">
@@ -11486,7 +11486,7 @@
         <v>5</v>
       </c>
       <c r="H35" s="7">
-        <v>5</v>
+        <v>5.0000000000000071</v>
       </c>
       <c r="I35" s="7">
         <v>5</v>
@@ -11624,7 +11624,7 @@
         <v>7</v>
       </c>
       <c r="BD35" s="8">
-        <v>7</v>
+        <v>7.0000000000000036</v>
       </c>
       <c r="BF35">
         <v>33</v>
@@ -11660,7 +11660,7 @@
         <v>7</v>
       </c>
       <c r="BQ35" s="7">
-        <v>7.0000000000000036</v>
+        <v>7</v>
       </c>
       <c r="BR35" s="7">
         <v>7</v>
@@ -11777,16 +11777,16 @@
         <v>7</v>
       </c>
       <c r="DE35" s="7">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
       <c r="DF35" s="7">
-        <v>7.0000000000000018</v>
+        <v>7</v>
       </c>
       <c r="DG35" s="7">
         <v>7</v>
       </c>
       <c r="DH35" s="8">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:112" x14ac:dyDescent="0.35">
@@ -11905,13 +11905,13 @@
         <v>7</v>
       </c>
       <c r="AO36" s="7">
-        <v>7</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="AP36" s="7">
         <v>7</v>
       </c>
       <c r="AQ36" s="7">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
       <c r="AR36" s="7">
         <v>7</v>
@@ -11983,7 +11983,7 @@
         <v>7</v>
       </c>
       <c r="BP36" s="7">
-        <v>7</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="BQ36" s="7">
         <v>7</v>
@@ -12147,7 +12147,7 @@
         <v>5</v>
       </c>
       <c r="K37" s="7">
-        <v>5.0000000000000009</v>
+        <v>5</v>
       </c>
       <c r="L37" s="7">
         <v>5</v>
@@ -12357,7 +12357,7 @@
         <v>7</v>
       </c>
       <c r="CF37" s="8">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
       <c r="CH37">
         <v>35</v>
@@ -12378,7 +12378,7 @@
         <v>6.9999999999999929</v>
       </c>
       <c r="CN37" s="7">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
       <c r="CO37" s="7">
         <v>7</v>
@@ -12393,7 +12393,7 @@
         <v>7</v>
       </c>
       <c r="CS37" s="7">
-        <v>6.9999999999999929</v>
+        <v>7</v>
       </c>
       <c r="CT37" s="7">
         <v>7</v>
@@ -12563,7 +12563,7 @@
         <v>7</v>
       </c>
       <c r="AQ38" s="7">
-        <v>7.0000000000000009</v>
+        <v>7</v>
       </c>
       <c r="AR38" s="7">
         <v>7</v>
@@ -12623,7 +12623,7 @@
         <v>7</v>
       </c>
       <c r="BL38" s="7">
-        <v>7.0000000000000009</v>
+        <v>7</v>
       </c>
       <c r="BM38" s="7">
         <v>7</v>
@@ -12674,7 +12674,7 @@
         <v>7</v>
       </c>
       <c r="CC38" s="7">
-        <v>7.0000000000000009</v>
+        <v>7</v>
       </c>
       <c r="CD38" s="7">
         <v>7</v>
@@ -12758,7 +12758,7 @@
         <v>7</v>
       </c>
       <c r="DF38" s="7">
-        <v>7</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="DG38" s="7">
         <v>7</v>
@@ -12790,7 +12790,7 @@
         <v>5.05</v>
       </c>
       <c r="H39" s="7">
-        <v>5.0499999999999972</v>
+        <v>5.0500000000000007</v>
       </c>
       <c r="I39" s="7">
         <v>5.0499999999999972</v>
@@ -12802,13 +12802,13 @@
         <v>5.05</v>
       </c>
       <c r="L39" s="7">
-        <v>5.0499999999999972</v>
+        <v>5.0500000000000007</v>
       </c>
       <c r="M39" s="7">
         <v>5.0499999999999972</v>
       </c>
       <c r="N39" s="7">
-        <v>5.0499999999999972</v>
+        <v>5.0500000000000007</v>
       </c>
       <c r="O39" s="7">
         <v>5.0500000000000007</v>
@@ -12847,7 +12847,7 @@
         <v>5.0499999999999972</v>
       </c>
       <c r="AA39" s="8">
-        <v>5.0500000000000007</v>
+        <v>5.0499999999999972</v>
       </c>
       <c r="AD39">
         <v>37</v>
@@ -12856,7 +12856,7 @@
         <v>0</v>
       </c>
       <c r="AF39" s="7">
-        <v>7.0699999999999932</v>
+        <v>0.19499999999925421</v>
       </c>
       <c r="AG39" s="7">
         <v>7.0699999999999932</v>
@@ -12868,28 +12868,28 @@
         <v>7.0699999999999932</v>
       </c>
       <c r="AJ39" s="7">
+        <v>7.0699999999999932</v>
+      </c>
+      <c r="AK39" s="7">
+        <v>7.0699999999999932</v>
+      </c>
+      <c r="AL39" s="7">
         <v>7.07</v>
-      </c>
-      <c r="AK39" s="7">
-        <v>7.07</v>
-      </c>
-      <c r="AL39" s="7">
-        <v>7.0699999999999932</v>
       </c>
       <c r="AM39" s="7">
         <v>7.0699999999999932</v>
       </c>
       <c r="AN39" s="7">
-        <v>7.0699999999999932</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="AO39" s="7">
         <v>7.0699999999999994</v>
       </c>
       <c r="AP39" s="7">
-        <v>7.0699999999999994</v>
+        <v>7.07</v>
       </c>
       <c r="AQ39" s="7">
-        <v>7.0699999999999994</v>
+        <v>7.0699999999999932</v>
       </c>
       <c r="AR39" s="7">
         <v>7.0699999999999994</v>
@@ -12919,7 +12919,7 @@
         <v>7.0699999999999994</v>
       </c>
       <c r="BA39" s="7">
-        <v>7.0699999999999994</v>
+        <v>7.0699999999999932</v>
       </c>
       <c r="BB39" s="7">
         <v>7.0699999999999932</v>
@@ -12928,7 +12928,7 @@
         <v>7.0699999999999932</v>
       </c>
       <c r="BD39" s="8">
-        <v>7.0699999999999932</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="BF39">
         <v>37</v>
@@ -12949,28 +12949,28 @@
         <v>7.0699999999999932</v>
       </c>
       <c r="BL39" s="7">
+        <v>7.0699999999999932</v>
+      </c>
+      <c r="BM39" s="7">
         <v>7.0699999999999994</v>
       </c>
-      <c r="BM39" s="7">
+      <c r="BN39" s="7">
+        <v>7.07</v>
+      </c>
+      <c r="BO39" s="7">
         <v>7.0699999999999932</v>
       </c>
-      <c r="BN39" s="7">
-        <v>7.0699999999999932</v>
-      </c>
-      <c r="BO39" s="7">
+      <c r="BP39" s="7">
         <v>7.0699999999999994</v>
       </c>
-      <c r="BP39" s="7">
-        <v>7.0699999999999932</v>
-      </c>
       <c r="BQ39" s="7">
-        <v>7.0699999999999932</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="BR39" s="7">
         <v>7.0699999999999932</v>
       </c>
       <c r="BS39" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999932</v>
       </c>
       <c r="BT39" s="7">
         <v>7.0699999999999932</v>
@@ -13003,13 +13003,13 @@
         <v>7.0699999999999994</v>
       </c>
       <c r="CD39" s="7">
+        <v>7.0699999999999994</v>
+      </c>
+      <c r="CE39" s="7">
         <v>7.0699999999999932</v>
       </c>
-      <c r="CE39" s="7">
-        <v>7.07</v>
-      </c>
       <c r="CF39" s="8">
-        <v>7.07</v>
+        <v>7.0699999999999932</v>
       </c>
       <c r="CH39">
         <v>37</v>
@@ -13030,25 +13030,25 @@
         <v>7.0699999999999994</v>
       </c>
       <c r="CN39" s="7">
+        <v>7.0699999999999932</v>
+      </c>
+      <c r="CO39" s="7">
         <v>7.07</v>
       </c>
-      <c r="CO39" s="7">
-        <v>7.0699999999999932</v>
-      </c>
       <c r="CP39" s="7">
-        <v>7.0699999999999932</v>
+        <v>7.07</v>
       </c>
       <c r="CQ39" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="CR39" s="7">
         <v>7.0699999999999932</v>
       </c>
       <c r="CS39" s="7">
+        <v>7.0699999999999994</v>
+      </c>
+      <c r="CT39" s="7">
         <v>7.07</v>
-      </c>
-      <c r="CT39" s="7">
-        <v>7.0699999999999932</v>
       </c>
       <c r="CU39" s="7">
         <v>7.0699999999999932</v>
@@ -13081,16 +13081,16 @@
         <v>7.0699999999999932</v>
       </c>
       <c r="DE39" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999932</v>
       </c>
       <c r="DF39" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="DG39" s="7">
         <v>7.07</v>
       </c>
       <c r="DH39" s="8">
-        <v>7.0699999999999932</v>
+        <v>7.0699999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:112" x14ac:dyDescent="0.35">
@@ -13116,7 +13116,7 @@
         <v>5.05</v>
       </c>
       <c r="H40" s="7">
-        <v>5.0500000000000007</v>
+        <v>5.05</v>
       </c>
       <c r="I40" s="7">
         <v>5.05</v>
@@ -13128,7 +13128,7 @@
         <v>5.05</v>
       </c>
       <c r="L40" s="7">
-        <v>5.0500000000000007</v>
+        <v>5.05</v>
       </c>
       <c r="M40" s="7">
         <v>5.0500000000000007</v>
@@ -13164,7 +13164,7 @@
         <v>5.0500000000000007</v>
       </c>
       <c r="X40" s="7">
-        <v>5.05</v>
+        <v>5.0500000000000007</v>
       </c>
       <c r="Y40" s="7">
         <v>5.0500000000000007</v>
@@ -13194,16 +13194,16 @@
         <v>7.07</v>
       </c>
       <c r="AJ40" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999985</v>
       </c>
       <c r="AK40" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="AL40" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="AM40" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="AN40" s="7">
         <v>7.07</v>
@@ -13242,16 +13242,16 @@
         <v>7.07</v>
       </c>
       <c r="AZ40" s="7">
-        <v>7.0699999999999994</v>
+        <v>7.0699999999999985</v>
       </c>
       <c r="BA40" s="7">
         <v>7.0699999999999985</v>
       </c>
       <c r="BB40" s="7">
-        <v>7.0699999999999994</v>
+        <v>7.07</v>
       </c>
       <c r="BC40" s="7">
-        <v>7.0699999999999994</v>
+        <v>7.07</v>
       </c>
       <c r="BD40" s="8">
         <v>7.0699999999999994</v>
@@ -13275,25 +13275,25 @@
         <v>7.07</v>
       </c>
       <c r="BL40" s="7">
+        <v>7.0699999999999994</v>
+      </c>
+      <c r="BM40" s="7">
         <v>7.07</v>
-      </c>
-      <c r="BM40" s="7">
-        <v>7.0699999999999985</v>
       </c>
       <c r="BN40" s="7">
         <v>7.07</v>
       </c>
       <c r="BO40" s="7">
+        <v>7.07</v>
+      </c>
+      <c r="BP40" s="7">
+        <v>7.0699999999999985</v>
+      </c>
+      <c r="BQ40" s="7">
+        <v>7.07</v>
+      </c>
+      <c r="BR40" s="7">
         <v>7.0699999999999994</v>
-      </c>
-      <c r="BP40" s="7">
-        <v>7.0699999999999994</v>
-      </c>
-      <c r="BQ40" s="7">
-        <v>7.0699999999999994</v>
-      </c>
-      <c r="BR40" s="7">
-        <v>7.07</v>
       </c>
       <c r="BS40" s="7">
         <v>7.0699999999999994</v>
@@ -13326,7 +13326,7 @@
         <v>7.07</v>
       </c>
       <c r="CC40" s="7">
-        <v>7.0699999999999994</v>
+        <v>7.07</v>
       </c>
       <c r="CD40" s="7">
         <v>7.07</v>
@@ -13335,7 +13335,7 @@
         <v>7.07</v>
       </c>
       <c r="CF40" s="8">
-        <v>7.0699999999999994</v>
+        <v>7.07</v>
       </c>
       <c r="CH40">
         <v>38</v>
@@ -13356,22 +13356,22 @@
         <v>7.07</v>
       </c>
       <c r="CN40" s="7">
+        <v>7.07</v>
+      </c>
+      <c r="CO40" s="7">
+        <v>7.07</v>
+      </c>
+      <c r="CP40" s="7">
         <v>7.0699999999999994</v>
       </c>
-      <c r="CO40" s="7">
-        <v>7.0699999999999994</v>
-      </c>
-      <c r="CP40" s="7">
-        <v>7.07</v>
-      </c>
       <c r="CQ40" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999985</v>
       </c>
       <c r="CR40" s="7">
         <v>7.0699999999999994</v>
       </c>
       <c r="CS40" s="7">
-        <v>7.0699999999999994</v>
+        <v>7.0699999999999985</v>
       </c>
       <c r="CT40" s="7">
         <v>7.0699999999999994</v>
@@ -13407,7 +13407,7 @@
         <v>7.0699999999999994</v>
       </c>
       <c r="DE40" s="7">
-        <v>7.07</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="DF40" s="7">
         <v>7.07</v>
@@ -13457,7 +13457,7 @@
         <v>5</v>
       </c>
       <c r="M41" s="7">
-        <v>5</v>
+        <v>4.9999999999999964</v>
       </c>
       <c r="N41" s="7">
         <v>5</v>
@@ -13496,7 +13496,7 @@
         <v>5</v>
       </c>
       <c r="Z41" s="7">
-        <v>5</v>
+        <v>4.9999999999999929</v>
       </c>
       <c r="AA41" s="8">
         <v>5</v>
@@ -13619,7 +13619,7 @@
         <v>7</v>
       </c>
       <c r="BR41" s="7">
-        <v>7.0000000000000018</v>
+        <v>7</v>
       </c>
       <c r="BS41" s="7">
         <v>7</v>
@@ -13846,25 +13846,25 @@
         <v>8.3999999999999986</v>
       </c>
       <c r="AJ42" s="7">
-        <v>8.3999999999999986</v>
+        <v>8.4000000000000057</v>
       </c>
       <c r="AK42" s="7">
+        <v>8.4000000000000057</v>
+      </c>
+      <c r="AL42" s="7">
         <v>8.3999999999999915</v>
       </c>
-      <c r="AL42" s="7">
+      <c r="AM42" s="7">
         <v>8.4000000000000057</v>
-      </c>
-      <c r="AM42" s="7">
-        <v>8.3999999999999986</v>
       </c>
       <c r="AN42" s="7">
         <v>8.3999999999999986</v>
       </c>
       <c r="AO42" s="7">
-        <v>8.3999999999999986</v>
+        <v>8.3999999999999915</v>
       </c>
       <c r="AP42" s="7">
-        <v>8.3999999999999986</v>
+        <v>8.3999999999999915</v>
       </c>
       <c r="AQ42" s="7">
         <v>8.3999999999999986</v>
@@ -13897,10 +13897,10 @@
         <v>8.3999999999999915</v>
       </c>
       <c r="BA42" s="7">
-        <v>8.3999999999999986</v>
+        <v>8.3999999999999915</v>
       </c>
       <c r="BB42" s="7">
-        <v>8.3999999999999986</v>
+        <v>8.4000000000000057</v>
       </c>
       <c r="BC42" s="7">
         <v>8.3999999999999986</v>
@@ -13927,25 +13927,25 @@
         <v>8.3999999999999986</v>
       </c>
       <c r="BL42" s="7">
-        <v>8.399999999999995</v>
+        <v>8.4000000000000057</v>
       </c>
       <c r="BM42" s="7">
         <v>8.3999999999999986</v>
       </c>
       <c r="BN42" s="7">
-        <v>8.4000000000000057</v>
+        <v>8.3999999999999986</v>
       </c>
       <c r="BO42" s="7">
         <v>8.4000000000000057</v>
       </c>
       <c r="BP42" s="7">
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="BQ42" s="7">
         <v>8.3999999999999915</v>
       </c>
-      <c r="BQ42" s="7">
-        <v>8.4000000000000057</v>
-      </c>
       <c r="BR42" s="7">
-        <v>8.4000000000000057</v>
+        <v>8.3999999999999986</v>
       </c>
       <c r="BS42" s="7">
         <v>8.4000000000000057</v>
@@ -14008,25 +14008,25 @@
         <v>8.3999999999999986</v>
       </c>
       <c r="CN42" s="7">
-        <v>8.399999999999995</v>
+        <v>8.3999999999999986</v>
       </c>
       <c r="CO42" s="7">
         <v>8.3999999999999986</v>
       </c>
       <c r="CP42" s="7">
+        <v>8.4000000000000057</v>
+      </c>
+      <c r="CQ42" s="7">
         <v>8.3999999999999986</v>
       </c>
-      <c r="CQ42" s="7">
+      <c r="CR42" s="7">
         <v>8.4000000000000057</v>
       </c>
-      <c r="CR42" s="7">
-        <v>8.3999999999999986</v>
-      </c>
       <c r="CS42" s="7">
-        <v>8.4000000000000057</v>
+        <v>8.3999999999999915</v>
       </c>
       <c r="CT42" s="7">
-        <v>8.4000000000000057</v>
+        <v>8.3999999999999915</v>
       </c>
       <c r="CU42" s="7">
         <v>8.3999999999999915</v>
@@ -14059,16 +14059,16 @@
         <v>8.4000000000000057</v>
       </c>
       <c r="DE42" s="7">
-        <v>8.4</v>
+        <v>8.3999999999999915</v>
       </c>
       <c r="DF42" s="7">
         <v>8.3999999999999986</v>
       </c>
       <c r="DG42" s="7">
-        <v>8.4</v>
+        <v>8.3999999999999986</v>
       </c>
       <c r="DH42" s="8">
-        <v>8.3999999999999986</v>
+        <v>8.3999999999999915</v>
       </c>
     </row>
     <row r="43" spans="1:112" x14ac:dyDescent="0.35">
@@ -15625,13 +15625,13 @@
         <v>0</v>
       </c>
       <c r="BW49" s="4">
-        <v>261.75259767564455</v>
+        <v>261.75259767559442</v>
       </c>
       <c r="BX49" s="4">
-        <v>316.55000546736562</v>
+        <v>316.55000546736574</v>
       </c>
       <c r="BY49" s="4">
-        <v>216.41519009961735</v>
+        <v>216.4151900995879</v>
       </c>
       <c r="BZ49" s="4">
         <v>0</v>
@@ -16890,7 +16890,7 @@
         <v>0</v>
       </c>
       <c r="BJ53" s="7">
-        <v>328.91357276170493</v>
+        <v>328.91357276168628</v>
       </c>
       <c r="BK53" s="7">
         <v>464</v>
@@ -17252,7 +17252,7 @@
         <v>0</v>
       </c>
       <c r="BV54" s="7">
-        <v>20.087809024798688</v>
+        <v>20.08780902479154</v>
       </c>
       <c r="BW54" s="7">
         <v>101.5</v>
@@ -17267,10 +17267,10 @@
         <v>101.5</v>
       </c>
       <c r="CA54" s="7">
-        <v>92.891244952234956</v>
+        <v>92.891244952208581</v>
       </c>
       <c r="CB54" s="7">
-        <v>79.297362093758935</v>
+        <v>79.297362093745733</v>
       </c>
       <c r="CC54" s="7">
         <v>0</v>
@@ -17934,7 +17934,7 @@
         <v>88</v>
       </c>
       <c r="CF56" s="8">
-        <v>25.199059684504221</v>
+        <v>25.199059684487132</v>
       </c>
       <c r="CH56">
         <v>8</v>
@@ -18110,7 +18110,7 @@
         <v>0</v>
       </c>
       <c r="AG57" s="7">
-        <v>121.20991685459065</v>
+        <v>121.20991685457776</v>
       </c>
       <c r="AH57" s="7">
         <v>650</v>
@@ -18466,7 +18466,7 @@
         <v>0</v>
       </c>
       <c r="AQ58" s="7">
-        <v>46.486457174325842</v>
+        <v>46.486457174316001</v>
       </c>
       <c r="AR58" s="7">
         <v>186</v>
@@ -18894,7 +18894,7 @@
         <v>154</v>
       </c>
       <c r="BZ59" s="7">
-        <v>124.38505899871092</v>
+        <v>124.38505899870385</v>
       </c>
       <c r="CA59" s="7">
         <v>0</v>
@@ -19414,7 +19414,7 @@
         <v>1335.2499999999995</v>
       </c>
       <c r="AG61" s="7">
-        <v>968.8181331454083</v>
+        <v>968.81813314542126</v>
       </c>
       <c r="AH61" s="7">
         <v>0</v>
@@ -19498,7 +19498,7 @@
         <v>1848</v>
       </c>
       <c r="BJ61" s="7">
-        <v>397.75026579929255</v>
+        <v>397.75026579931136</v>
       </c>
       <c r="BK61" s="7">
         <v>238.97301310804596</v>
@@ -19794,7 +19794,7 @@
         <v>555.91330752054</v>
       </c>
       <c r="AY62" s="7">
-        <v>419.12782728822458</v>
+        <v>419.12782728822447</v>
       </c>
       <c r="AZ62" s="7">
         <v>292.73127773381839</v>
@@ -19938,7 +19938,7 @@
         <v>0</v>
       </c>
       <c r="CW62" s="7">
-        <v>390.13665316574316</v>
+        <v>390.13665316572661</v>
       </c>
       <c r="CX62" s="7">
         <v>656.1</v>
@@ -20207,7 +20207,7 @@
         <v>50.3</v>
       </c>
       <c r="CC63" s="7">
-        <v>9.4985030692667092</v>
+        <v>9.4985030692343955</v>
       </c>
       <c r="CD63" s="7">
         <v>0</v>
@@ -20826,7 +20826,7 @@
         <v>257</v>
       </c>
       <c r="BR65" s="7">
-        <v>228.51958558765898</v>
+        <v>228.51958558765909</v>
       </c>
       <c r="BS65" s="7">
         <v>22.269961857947123</v>
@@ -20957,7 +20957,7 @@
         <v>18</v>
       </c>
       <c r="B66" s="6">
-        <v>1525.0646635152286</v>
+        <v>1525.0646635150945</v>
       </c>
       <c r="C66" s="7">
         <v>2269.6</v>
@@ -20990,7 +20990,7 @@
         <v>858.55241006221001</v>
       </c>
       <c r="M66" s="7">
-        <v>825.22968175276935</v>
+        <v>825.22968175276947</v>
       </c>
       <c r="N66" s="7">
         <v>1049.2370488885435</v>
@@ -20999,7 +20999,7 @@
         <v>830.57748232853999</v>
       </c>
       <c r="P66" s="7">
-        <v>798.2539796694964</v>
+        <v>798.25397966949629</v>
       </c>
       <c r="Q66" s="7">
         <v>0</v>
@@ -21074,7 +21074,7 @@
         <v>1439.7887845138803</v>
       </c>
       <c r="AQ66" s="7">
-        <v>1363.5277264001786</v>
+        <v>1363.5277264001886</v>
       </c>
       <c r="AR66" s="7">
         <v>1194.6016112266743</v>
@@ -21164,37 +21164,37 @@
         <v>1596.6180043382992</v>
       </c>
       <c r="BV66" s="7">
-        <v>871.03595735254419</v>
+        <v>871.03595735255112</v>
       </c>
       <c r="BW66" s="7">
-        <v>245.4368825990947</v>
+        <v>245.43688259914461</v>
       </c>
       <c r="BX66" s="7">
-        <v>52.669280129846015</v>
+        <v>52.669280129845909</v>
       </c>
       <c r="BY66" s="7">
-        <v>15.302169067968171</v>
+        <v>15.302169067997625</v>
       </c>
       <c r="BZ66" s="7">
-        <v>124.3028564013826</v>
+        <v>124.30285640138966</v>
       </c>
       <c r="CA66" s="7">
-        <v>130.74396168645853</v>
+        <v>130.74396168648491</v>
       </c>
       <c r="CB66" s="7">
-        <v>28.266161404681256</v>
+        <v>28.266161404694458</v>
       </c>
       <c r="CC66" s="7">
-        <v>32.778692140659565</v>
+        <v>32.778692140691767</v>
       </c>
       <c r="CD66" s="7">
-        <v>74.923703955973764</v>
+        <v>74.923703955986497</v>
       </c>
       <c r="CE66" s="7">
         <v>0</v>
       </c>
       <c r="CF66" s="8">
-        <v>149.57515862949884</v>
+        <v>149.57515862951547</v>
       </c>
       <c r="CH66">
         <v>18</v>
@@ -21242,7 +21242,7 @@
         <v>891.24817047822842</v>
       </c>
       <c r="CW66" s="7">
-        <v>469.33405084678907</v>
+        <v>469.3340508468055</v>
       </c>
       <c r="CX66" s="7">
         <v>0</v>
@@ -21283,7 +21283,7 @@
         <v>19</v>
       </c>
       <c r="B67" s="6">
-        <v>25.935336484771369</v>
+        <v>25.935336484905516</v>
       </c>
       <c r="C67" s="7">
         <v>0</v>
@@ -21840,7 +21840,7 @@
         <v>398.3</v>
       </c>
       <c r="CD68" s="7">
-        <v>250.55688601084117</v>
+        <v>250.55688601082844</v>
       </c>
       <c r="CE68" s="7">
         <v>210.87811527651456</v>
@@ -29470,10 +29470,10 @@
         <v>1</v>
       </c>
       <c r="B95" s="3">
-        <v>-134.39999999999992</v>
+        <v>-134.4</v>
       </c>
       <c r="C95" s="4">
-        <v>-140.43617932524776</v>
+        <v>-140.43617932524944</v>
       </c>
       <c r="D95" s="4">
         <v>96.604125100000331</v>
@@ -29485,13 +29485,13 @@
         <v>251.52755900259996</v>
       </c>
       <c r="G95" s="4">
-        <v>446.7035046224737</v>
+        <v>446.70350462247382</v>
       </c>
       <c r="H95" s="4">
-        <v>432.98438616407589</v>
+        <v>432.98438616407594</v>
       </c>
       <c r="I95" s="4">
-        <v>428.91280449679857</v>
+        <v>428.91280449679584</v>
       </c>
       <c r="J95" s="4">
         <v>563.77754492970962</v>
@@ -29503,10 +29503,10 @@
         <v>727.12439310291666</v>
       </c>
       <c r="M95" s="4">
-        <v>661.77879597417621</v>
+        <v>661.77879597417655</v>
       </c>
       <c r="N95" s="4">
-        <v>389.77658847127714</v>
+        <v>389.77658847127725</v>
       </c>
       <c r="O95" s="4">
         <v>415.8514944341855</v>
@@ -29515,10 +29515,10 @@
         <v>412.63724121742626</v>
       </c>
       <c r="Q95" s="4">
-        <v>409.46755972171633</v>
+        <v>409.46755972171616</v>
       </c>
       <c r="R95" s="4">
-        <v>406.34285109254506</v>
+        <v>406.34285109254512</v>
       </c>
       <c r="S95" s="4">
         <v>374.75929175917236</v>
@@ -29533,13 +29533,13 @@
         <v>506.41076606408444</v>
       </c>
       <c r="W95" s="4">
-        <v>545.11811295866141</v>
+        <v>545.1181129586613</v>
       </c>
       <c r="X95" s="4">
         <v>583.73732597528942</v>
       </c>
       <c r="Y95" s="4">
-        <v>622.26761190906677</v>
+        <v>622.267611909067</v>
       </c>
       <c r="Z95" s="4">
         <v>660.70817041624878</v>
@@ -29554,37 +29554,37 @@
         <v>29.550000000000029</v>
       </c>
       <c r="AF95" s="4">
-        <v>-59.251749999999745</v>
+        <v>-63.835083333333685</v>
       </c>
       <c r="AG95" s="4">
-        <v>2.9395409166669424</v>
+        <v>2.9395409166669042</v>
       </c>
       <c r="AH95" s="4">
-        <v>8.6464534515837759</v>
+        <v>8.6464534515839659</v>
       </c>
       <c r="AI95" s="4">
         <v>155.60156153264791</v>
       </c>
       <c r="AJ95" s="4">
-        <v>221.17051413694071</v>
+        <v>221.1705141369363</v>
       </c>
       <c r="AK95" s="4">
-        <v>631.09798122797747</v>
+        <v>631.09798122797201</v>
       </c>
       <c r="AL95" s="4">
-        <v>665.3236581838504</v>
+        <v>665.32365818385017</v>
       </c>
       <c r="AM95" s="4">
-        <v>741.18216289956149</v>
+        <v>741.18216289956115</v>
       </c>
       <c r="AN95" s="4">
-        <v>789.53814217588774</v>
+        <v>789.53814217588763</v>
       </c>
       <c r="AO95" s="4">
-        <v>802.29488878880409</v>
+        <v>802.2948887888042</v>
       </c>
       <c r="AP95" s="4">
-        <v>541.75502136613477</v>
+        <v>541.75502136613704</v>
       </c>
       <c r="AQ95" s="4">
         <v>466.25525346966089</v>
@@ -29593,19 +29593,19 @@
         <v>492.99308741755459</v>
       </c>
       <c r="AS95" s="4">
-        <v>498.86409578806274</v>
+        <v>498.86409578806217</v>
       </c>
       <c r="AT95" s="4">
-        <v>489.24142265015496</v>
+        <v>489.24142265015462</v>
       </c>
       <c r="AU95" s="4">
-        <v>492.86950404066374</v>
+        <v>492.86950404066363</v>
       </c>
       <c r="AV95" s="4">
-        <v>496.5885362630919</v>
+        <v>496.58853626309229</v>
       </c>
       <c r="AW95" s="4">
-        <v>480.77678450467448</v>
+        <v>480.77678450467471</v>
       </c>
       <c r="AX95" s="4">
         <v>478.48897889854999</v>
@@ -29614,13 +29614,13 @@
         <v>476.25408304197009</v>
       </c>
       <c r="AZ95" s="4">
-        <v>461.23611537796074</v>
+        <v>461.23611537796097</v>
       </c>
       <c r="BA95" s="4">
-        <v>465.52703547854156</v>
+        <v>465.52703547854151</v>
       </c>
       <c r="BB95" s="4">
-        <v>502.71076879784835</v>
+        <v>502.71076879784869</v>
       </c>
       <c r="BC95" s="4">
         <v>539.79265571702956</v>
@@ -29632,31 +29632,31 @@
         <v>1</v>
       </c>
       <c r="BG95" s="3">
-        <v>194.00000000000003</v>
+        <v>193.99999999999994</v>
       </c>
       <c r="BH95" s="4">
-        <v>51.778033333333042</v>
+        <v>51.778033333333191</v>
       </c>
       <c r="BI95" s="4">
         <v>44.690485633332926</v>
       </c>
       <c r="BJ95" s="4">
-        <v>37.822650004032006</v>
+        <v>37.822650004032461</v>
       </c>
       <c r="BK95" s="4">
-        <v>31.176503854068564</v>
+        <v>31.176503854068109</v>
       </c>
       <c r="BL95" s="4">
         <v>24.754042388754897</v>
       </c>
       <c r="BM95" s="4">
-        <v>333.90254478963089</v>
+        <v>333.90254478963118</v>
       </c>
       <c r="BN95" s="4">
-        <v>668.44319102607142</v>
+        <v>668.44319102607108</v>
       </c>
       <c r="BO95" s="4">
-        <v>671.20653641197237</v>
+        <v>671.20653641197259</v>
       </c>
       <c r="BP95" s="4">
         <v>704.85825190634705</v>
@@ -29665,16 +29665,16 @@
         <v>707.39733284017132</v>
       </c>
       <c r="BR95" s="4">
-        <v>674.56004934486145</v>
+        <v>674.56004934486214</v>
       </c>
       <c r="BS95" s="4">
-        <v>652.64912645563209</v>
+        <v>652.6491264556322</v>
       </c>
       <c r="BT95" s="4">
-        <v>651.46717192706615</v>
+        <v>651.46717192706603</v>
       </c>
       <c r="BU95" s="4">
-        <v>805.91474647440975</v>
+        <v>805.91474647440941</v>
       </c>
       <c r="BV95" s="4">
         <v>804.85908252601314</v>
@@ -29689,52 +29689,52 @@
         <v>802.07839397640976</v>
       </c>
       <c r="BZ95" s="4">
-        <v>801.28220285553073</v>
+        <v>801.28220285553061</v>
       </c>
       <c r="CA95" s="4">
-        <v>800.55234601456414</v>
+        <v>800.55234601456357</v>
       </c>
       <c r="CB95" s="4">
         <v>799.88942046202828</v>
       </c>
       <c r="CC95" s="4">
-        <v>799.29402857951959</v>
+        <v>799.29402857951948</v>
       </c>
       <c r="CD95" s="4">
-        <v>794.71852532264438</v>
+        <v>794.71852532264415</v>
       </c>
       <c r="CE95" s="4">
         <v>759.61670871721492</v>
       </c>
       <c r="CF95" s="5">
-        <v>721.44914242900211</v>
+        <v>721.44914242900234</v>
       </c>
       <c r="CH95" s="1" t="s">
         <v>1</v>
       </c>
       <c r="CI95" s="3">
-        <v>-115.61666666666663</v>
+        <v>-115.6166666666667</v>
       </c>
       <c r="CJ95" s="4">
         <v>-119.20638333333341</v>
       </c>
       <c r="CK95" s="4">
-        <v>92.496732883333564</v>
+        <v>92.496732883333749</v>
       </c>
       <c r="CL95" s="4">
         <v>99.009660145950562</v>
       </c>
       <c r="CM95" s="4">
-        <v>246.77803708726393</v>
+        <v>246.77803708726395</v>
       </c>
       <c r="CN95" s="4">
         <v>253.13449608771612</v>
       </c>
       <c r="CO95" s="4">
-        <v>483.66910972428343</v>
+        <v>483.66910972428332</v>
       </c>
       <c r="CP95" s="4">
-        <v>470.79808171180173</v>
+        <v>470.79808171180196</v>
       </c>
       <c r="CQ95" s="4">
         <v>741.44332102952296</v>
@@ -29743,19 +29743,19 @@
         <v>738.19371425212194</v>
       </c>
       <c r="CS95" s="4">
-        <v>699.63112737741244</v>
+        <v>699.6311273774121</v>
       </c>
       <c r="CT95" s="4">
-        <v>466.62765959618133</v>
+        <v>466.62765959618127</v>
       </c>
       <c r="CU95" s="4">
         <v>442.84534519921351</v>
       </c>
       <c r="CV95" s="4">
-        <v>439.77515663933957</v>
+        <v>439.77515663933968</v>
       </c>
       <c r="CW95" s="4">
-        <v>436.75083638242694</v>
+        <v>436.7508363824266</v>
       </c>
       <c r="CX95" s="4">
         <v>433.77279724320198</v>
@@ -29764,7 +29764,7 @@
         <v>430.84145575172403</v>
       </c>
       <c r="CZ95" s="4">
-        <v>427.95723218682292</v>
+        <v>427.95723218682281</v>
       </c>
       <c r="DA95" s="4">
         <v>409.15326315315872</v>
@@ -29773,22 +29773,22 @@
         <v>454.33229918820393</v>
       </c>
       <c r="DC95" s="4">
-        <v>496.08811321423127</v>
+        <v>496.08811321423104</v>
       </c>
       <c r="DD95" s="4">
         <v>534.41989623315942</v>
       </c>
       <c r="DE95" s="4">
-        <v>572.66016529925787</v>
+        <v>572.66016529925776</v>
       </c>
       <c r="DF95" s="4">
-        <v>610.80809678695107</v>
+        <v>610.80809678695118</v>
       </c>
       <c r="DG95" s="4">
-        <v>648.86285965803381</v>
+        <v>648.86285965803393</v>
       </c>
       <c r="DH95" s="5">
-        <v>690.15694872828999</v>
+        <v>690.15694872828976</v>
       </c>
     </row>
     <row r="96" spans="1:112" x14ac:dyDescent="0.35">
@@ -29796,10 +29796,10 @@
         <v>2</v>
       </c>
       <c r="B96" s="6">
-        <v>-350.40000000000009</v>
+        <v>-350.40000000000003</v>
       </c>
       <c r="C96" s="7">
-        <v>-258.92717932524727</v>
+        <v>-258.92717932524897</v>
       </c>
       <c r="D96" s="7">
         <v>-615.6438559000004</v>
@@ -29817,7 +29817,7 @@
         <v>-805.54270957378617</v>
       </c>
       <c r="I96" s="7">
-        <v>-794.54863510270411</v>
+        <v>-794.54863510270684</v>
       </c>
       <c r="J96" s="7">
         <v>-644.79764762618868</v>
@@ -29829,22 +29829,22 @@
         <v>-452.223005909584</v>
       </c>
       <c r="M96" s="7">
-        <v>-317.23032962943677</v>
+        <v>-317.23032962943694</v>
       </c>
       <c r="N96" s="7">
-        <v>231.01978073723205</v>
+        <v>231.019780737232</v>
       </c>
       <c r="O96" s="7">
         <v>271.05937543053375</v>
       </c>
       <c r="P96" s="7">
-        <v>281.62049314274213</v>
+        <v>281.62049314274225</v>
       </c>
       <c r="Q96" s="7">
-        <v>292.0351609143604</v>
+        <v>292.03516091436029</v>
       </c>
       <c r="R96" s="7">
-        <v>302.30206069592305</v>
+        <v>302.30206069592316</v>
       </c>
       <c r="S96" s="7">
         <v>283.91563424898101</v>
@@ -29859,16 +29859,16 @@
         <v>29.647459762351218</v>
       </c>
       <c r="W96" s="7">
-        <v>-44.046763099787995</v>
+        <v>-44.046763099787611</v>
       </c>
       <c r="X96" s="7">
         <v>-117.62573396768619</v>
       </c>
       <c r="Y96" s="7">
-        <v>-191.08841557339531</v>
+        <v>-191.0884155733952</v>
       </c>
       <c r="Z96" s="7">
-        <v>-264.43376131355615</v>
+        <v>-264.43376131355581</v>
       </c>
       <c r="AA96" s="8">
         <v>-318.40216967821391</v>
@@ -29880,37 +29880,37 @@
         <v>-469.95</v>
       </c>
       <c r="AF96" s="7">
-        <v>-438.10925000000026</v>
+        <v>-435.81758333333329</v>
       </c>
       <c r="AG96" s="7">
         <v>-473.88247658333364</v>
       </c>
       <c r="AH96" s="7">
-        <v>-481.34536220591713</v>
+        <v>-481.34536220591735</v>
       </c>
       <c r="AI96" s="7">
         <v>-559.36358046577038</v>
       </c>
       <c r="AJ96" s="7">
-        <v>-596.61933696521169</v>
+        <v>-596.61933696520941</v>
       </c>
       <c r="AK96" s="7">
-        <v>-805.98434222980086</v>
+        <v>-805.98434222979813</v>
       </c>
       <c r="AL96" s="7">
-        <v>-827.42781387227978</v>
+        <v>-827.42781387227956</v>
       </c>
       <c r="AM96" s="7">
-        <v>-739.39971240507316</v>
+        <v>-739.39971240507361</v>
       </c>
       <c r="AN96" s="7">
-        <v>-679.07961000648845</v>
+        <v>-679.07961000648811</v>
       </c>
       <c r="AO96" s="7">
-        <v>-654.56606316321324</v>
+        <v>-654.56606316321313</v>
       </c>
       <c r="AP96" s="7">
-        <v>-130.02204488814505</v>
+        <v>-130.02204488814971</v>
       </c>
       <c r="AQ96" s="7">
         <v>24.378452885399724</v>
@@ -29919,19 +29919,19 @@
         <v>62.239855628034846</v>
       </c>
       <c r="AS96" s="7">
-        <v>233.01954491243748</v>
+        <v>233.01954491243782</v>
       </c>
       <c r="AT96" s="7">
-        <v>234.08873081664939</v>
+        <v>234.08873081664893</v>
       </c>
       <c r="AU96" s="7">
-        <v>173.60911010067036</v>
+        <v>173.60911010067073</v>
       </c>
       <c r="AV96" s="7">
-        <v>108.16127374854528</v>
+        <v>108.16127374854511</v>
       </c>
       <c r="AW96" s="7">
-        <v>102.37913662749716</v>
+        <v>102.37913662749739</v>
       </c>
       <c r="AX96" s="7">
         <v>109.89621219047834</v>
@@ -29940,16 +29940,16 @@
         <v>117.2394414335262</v>
       </c>
       <c r="AZ96" s="7">
-        <v>111.57080199504136</v>
+        <v>111.57080199504153</v>
       </c>
       <c r="BA96" s="7">
-        <v>56.233876681907226</v>
+        <v>56.233876681907262</v>
       </c>
       <c r="BB96" s="7">
-        <v>-15.467928427955741</v>
+        <v>-15.46792842795594</v>
       </c>
       <c r="BC96" s="7">
-        <v>-87.036549783808027</v>
+        <v>-87.036549783807828</v>
       </c>
       <c r="BD96" s="8">
         <v>-165.13745539852891</v>
@@ -29958,31 +29958,31 @@
         <v>2</v>
       </c>
       <c r="BG96" s="6">
-        <v>-564.9</v>
+        <v>-564.89999999999975</v>
       </c>
       <c r="BH96" s="7">
-        <v>-280.14496666666673</v>
+        <v>-280.14496666666685</v>
       </c>
       <c r="BI96" s="7">
         <v>-279.3574613666666</v>
       </c>
       <c r="BJ96" s="7">
-        <v>-278.59436851896646</v>
+        <v>-278.59436851896663</v>
       </c>
       <c r="BK96" s="7">
-        <v>-277.85590783563731</v>
+        <v>-277.85590783563714</v>
       </c>
       <c r="BL96" s="7">
         <v>-277.14230100615805</v>
       </c>
       <c r="BM96" s="7">
-        <v>-434.12640472490205</v>
+        <v>-434.12640472490222</v>
       </c>
       <c r="BN96" s="7">
-        <v>-637.21801903409323</v>
+        <v>-637.218019034093</v>
       </c>
       <c r="BO96" s="7">
-        <v>-640.83162453873331</v>
+        <v>-640.83162453873342</v>
       </c>
       <c r="BP96" s="7">
         <v>-659.79925249291546</v>
@@ -29991,61 +29991,61 @@
         <v>-663.11958909868531</v>
       </c>
       <c r="BR96" s="7">
-        <v>-595.765876418831</v>
+        <v>-595.76587641883145</v>
       </c>
       <c r="BS96" s="7">
-        <v>-462.34427263993416</v>
+        <v>-462.34427263993422</v>
       </c>
       <c r="BT96" s="7">
-        <v>-458.46070776036026</v>
+        <v>-458.46070776035998</v>
       </c>
       <c r="BU96" s="7">
         <v>-145.2170241302033</v>
       </c>
       <c r="BV96" s="7">
-        <v>-141.74841401404075</v>
+        <v>-141.74841401404063</v>
       </c>
       <c r="BW96" s="7">
-        <v>-138.49008640683377</v>
+        <v>-138.49008640683388</v>
       </c>
       <c r="BX96" s="7">
-        <v>-135.44393385116138</v>
+        <v>-135.44393385116126</v>
       </c>
       <c r="BY96" s="7">
-        <v>-132.61186592248879</v>
+        <v>-132.61186592248873</v>
       </c>
       <c r="BZ96" s="7">
-        <v>-129.99580938245725</v>
+        <v>-129.99580938245754</v>
       </c>
       <c r="CA96" s="7">
-        <v>-127.59770833356572</v>
+        <v>-127.59770833356606</v>
       </c>
       <c r="CB96" s="7">
         <v>-125.41952437523423</v>
       </c>
       <c r="CC96" s="7">
-        <v>-123.46323676127781</v>
+        <v>-123.46323676127776</v>
       </c>
       <c r="CD96" s="7">
-        <v>-125.77909540621965</v>
+        <v>-125.77909540621991</v>
       </c>
       <c r="CE96" s="7">
-        <v>-158.91593059820872</v>
+        <v>-158.91593059820866</v>
       </c>
       <c r="CF96" s="8">
-        <v>-195.41583064026008</v>
+        <v>-195.41583064025991</v>
       </c>
       <c r="CH96" t="s">
         <v>2</v>
       </c>
       <c r="CI96" s="6">
-        <v>-412.11666666666679</v>
+        <v>-412.11666666666673</v>
       </c>
       <c r="CJ96" s="7">
         <v>-400.32188333333329</v>
       </c>
       <c r="CK96" s="7">
-        <v>-590.99572761666695</v>
+        <v>-590.99572761666707</v>
       </c>
       <c r="CL96" s="7">
         <v>-599.51263249855049</v>
@@ -30060,37 +30060,37 @@
         <v>-807.24397515455007</v>
       </c>
       <c r="CP96" s="7">
-        <v>-805.81386093094079</v>
+        <v>-805.81386093094102</v>
       </c>
       <c r="CQ96" s="7">
         <v>-521.05376909700385</v>
       </c>
       <c r="CR96" s="7">
-        <v>-510.37648968554367</v>
+        <v>-510.37648968554356</v>
       </c>
       <c r="CS96" s="7">
-        <v>-382.63014748675619</v>
+        <v>-382.63014748675602</v>
       </c>
       <c r="CT96" s="7">
-        <v>87.440547041118947</v>
+        <v>87.440547041118862</v>
       </c>
       <c r="CU96" s="7">
         <v>227.01100863115602</v>
       </c>
       <c r="CV96" s="7">
-        <v>237.09877104216986</v>
+        <v>237.09877104216969</v>
       </c>
       <c r="CW96" s="7">
-        <v>247.03582331488298</v>
+        <v>247.03582331488266</v>
       </c>
       <c r="CX96" s="7">
         <v>256.8208090580506</v>
       </c>
       <c r="CY96" s="7">
-        <v>266.45235967290648</v>
+        <v>266.4523596729066</v>
       </c>
       <c r="CZ96" s="7">
-        <v>275.92909424329616</v>
+        <v>275.92909424329611</v>
       </c>
       <c r="DA96" s="7">
         <v>229.18419433817712</v>
@@ -30099,22 +30099,22 @@
         <v>142.41160875388732</v>
       </c>
       <c r="DC96" s="7">
-        <v>62.423236566005244</v>
+        <v>62.423236566005698</v>
       </c>
       <c r="DD96" s="7">
-        <v>-10.779864304900684</v>
+        <v>-10.779864304900759</v>
       </c>
       <c r="DE96" s="7">
-        <v>-83.863293083644749</v>
+        <v>-83.863293083644592</v>
       </c>
       <c r="DF96" s="7">
-        <v>-156.8259727213977</v>
+        <v>-156.82597272139765</v>
       </c>
       <c r="DG96" s="7">
-        <v>-229.6668164758903</v>
+        <v>-229.66681647589058</v>
       </c>
       <c r="DH96" s="8">
-        <v>-309.05139449084072</v>
+        <v>-309.05139449084061</v>
       </c>
     </row>
     <row r="97" spans="1:112" x14ac:dyDescent="0.35">
@@ -30122,10 +30122,10 @@
         <v>3</v>
       </c>
       <c r="B97" s="9">
-        <v>484.79999999999995</v>
+        <v>484.8</v>
       </c>
       <c r="C97" s="10">
-        <v>399.363358650495</v>
+        <v>399.36335865049841</v>
       </c>
       <c r="D97" s="10">
         <v>519.03973080000003</v>
@@ -30137,13 +30137,13 @@
         <v>452.55463353926177</v>
       </c>
       <c r="G97" s="10">
-        <v>360.36355144669005</v>
+        <v>360.36355144669</v>
       </c>
       <c r="H97" s="10">
         <v>372.55832340971028</v>
       </c>
       <c r="I97" s="10">
-        <v>365.63583060590554</v>
+        <v>365.635830605911</v>
       </c>
       <c r="J97" s="10">
         <v>81.020102696479057</v>
@@ -30155,7 +30155,7 @@
         <v>-274.90138719333265</v>
       </c>
       <c r="M97" s="10">
-        <v>-344.54846634473944</v>
+        <v>-344.54846634473961</v>
       </c>
       <c r="N97" s="10">
         <v>-620.79636920850908</v>
@@ -30164,13 +30164,13 @@
         <v>-686.91086986471919</v>
       </c>
       <c r="P97" s="10">
-        <v>-694.25773436016846</v>
+        <v>-694.25773436016857</v>
       </c>
       <c r="Q97" s="10">
-        <v>-701.50272063607656</v>
+        <v>-701.50272063607645</v>
       </c>
       <c r="R97" s="10">
-        <v>-708.64491178846811</v>
+        <v>-708.64491178846833</v>
       </c>
       <c r="S97" s="10">
         <v>-658.67492600815331</v>
@@ -30185,16 +30185,16 @@
         <v>-536.05822582643555</v>
       </c>
       <c r="W97" s="10">
-        <v>-501.07134985887342</v>
+        <v>-501.07134985887353</v>
       </c>
       <c r="X97" s="10">
         <v>-466.11159200760324</v>
       </c>
       <c r="Y97" s="10">
-        <v>-431.17919633567146</v>
+        <v>-431.1791963356718</v>
       </c>
       <c r="Z97" s="10">
-        <v>-396.27440910269263</v>
+        <v>-396.27440910269274</v>
       </c>
       <c r="AA97" s="11">
         <v>-347.77675152819904</v>
@@ -30206,37 +30206,37 @@
         <v>440.39999999999992</v>
       </c>
       <c r="AF97" s="10">
-        <v>497.36100000000005</v>
+        <v>499.65266666666702</v>
       </c>
       <c r="AG97" s="10">
-        <v>470.94293566666659</v>
+        <v>470.9429356666667</v>
       </c>
       <c r="AH97" s="10">
-        <v>472.6989087543335</v>
+        <v>472.69890875433327</v>
       </c>
       <c r="AI97" s="10">
         <v>403.76201893312259</v>
       </c>
       <c r="AJ97" s="10">
-        <v>375.44882282827098</v>
+        <v>375.44882282827325</v>
       </c>
       <c r="AK97" s="10">
-        <v>174.88636100182345</v>
+        <v>174.88636100182612</v>
       </c>
       <c r="AL97" s="10">
-        <v>162.10415568842944</v>
+        <v>162.1041556884295</v>
       </c>
       <c r="AM97" s="10">
-        <v>-1.7824504944882733</v>
+        <v>-1.7824504944875343</v>
       </c>
       <c r="AN97" s="10">
-        <v>-110.45853216939929</v>
+        <v>-110.45853216939946</v>
       </c>
       <c r="AO97" s="10">
-        <v>-147.72882562559073</v>
+        <v>-147.72882562559107</v>
       </c>
       <c r="AP97" s="10">
-        <v>-411.73297647798972</v>
+        <v>-411.73297647798745</v>
       </c>
       <c r="AQ97" s="10">
         <v>-490.63370635506067</v>
@@ -30245,19 +30245,19 @@
         <v>-555.23294304558954</v>
       </c>
       <c r="AS97" s="10">
-        <v>-731.88364070050022</v>
+        <v>-731.88364070049988</v>
       </c>
       <c r="AT97" s="10">
-        <v>-723.3301534668044</v>
+        <v>-723.33015346680349</v>
       </c>
       <c r="AU97" s="10">
-        <v>-666.47861414133422</v>
+        <v>-666.47861414133433</v>
       </c>
       <c r="AV97" s="10">
-        <v>-604.74981001163724</v>
+        <v>-604.74981001163746</v>
       </c>
       <c r="AW97" s="10">
-        <v>-583.15592113217167</v>
+        <v>-583.15592113217212</v>
       </c>
       <c r="AX97" s="10">
         <v>-588.38519108902835</v>
@@ -30266,13 +30266,13 @@
         <v>-593.49352447549632</v>
       </c>
       <c r="AZ97" s="10">
-        <v>-572.80691737300208</v>
+        <v>-572.80691737300253</v>
       </c>
       <c r="BA97" s="10">
-        <v>-521.7609121604487</v>
+        <v>-521.76091216044881</v>
       </c>
       <c r="BB97" s="10">
-        <v>-487.24284036989252</v>
+        <v>-487.24284036989275</v>
       </c>
       <c r="BC97" s="10">
         <v>-452.75610593322165</v>
@@ -30284,31 +30284,31 @@
         <v>3</v>
       </c>
       <c r="BG97" s="9">
-        <v>370.89999999999975</v>
+        <v>370.9</v>
       </c>
       <c r="BH97" s="10">
-        <v>228.36693333333369</v>
+        <v>228.36693333333361</v>
       </c>
       <c r="BI97" s="10">
         <v>234.66697573333371</v>
       </c>
       <c r="BJ97" s="10">
-        <v>240.77171851493441</v>
+        <v>240.77171851493421</v>
       </c>
       <c r="BK97" s="10">
-        <v>246.67940398156878</v>
+        <v>246.67940398156898</v>
       </c>
       <c r="BL97" s="10">
         <v>252.38825861740315</v>
       </c>
       <c r="BM97" s="10">
-        <v>100.22385993527121</v>
+        <v>100.22385993527107</v>
       </c>
       <c r="BN97" s="10">
-        <v>-31.225171991978186</v>
+        <v>-31.225171991977959</v>
       </c>
       <c r="BO97" s="10">
-        <v>-30.374911873239057</v>
+        <v>-30.374911873239171</v>
       </c>
       <c r="BP97" s="10">
         <v>-45.05899941343165</v>
@@ -30317,34 +30317,34 @@
         <v>-44.277743741486006</v>
       </c>
       <c r="BR97" s="10">
-        <v>-78.794172926030456</v>
+        <v>-78.794172926030797</v>
       </c>
       <c r="BS97" s="10">
-        <v>-190.30485381569792</v>
+        <v>-190.30485381569798</v>
       </c>
       <c r="BT97" s="10">
-        <v>-193.00646416670588</v>
+        <v>-193.00646416670605</v>
       </c>
       <c r="BU97" s="10">
-        <v>-660.69772234420634</v>
+        <v>-660.69772234420611</v>
       </c>
       <c r="BV97" s="10">
-        <v>-663.11066851197234</v>
+        <v>-663.11066851197256</v>
       </c>
       <c r="BW97" s="10">
-        <v>-665.37733119524637</v>
+        <v>-665.37733119524614</v>
       </c>
       <c r="BX97" s="10">
-        <v>-667.49639384267107</v>
+        <v>-667.4963938426713</v>
       </c>
       <c r="BY97" s="10">
-        <v>-669.46652805392091</v>
+        <v>-669.4665280539208</v>
       </c>
       <c r="BZ97" s="10">
-        <v>-671.28639347307353</v>
+        <v>-671.28639347307308</v>
       </c>
       <c r="CA97" s="10">
-        <v>-672.95463768099842</v>
+        <v>-672.95463768099751</v>
       </c>
       <c r="CB97" s="10">
         <v>-674.46989608679405</v>
@@ -30353,13 +30353,13 @@
         <v>-675.83079181824178</v>
       </c>
       <c r="CD97" s="10">
-        <v>-668.93942991642473</v>
+        <v>-668.93942991642393</v>
       </c>
       <c r="CE97" s="10">
-        <v>-600.70077811900603</v>
+        <v>-600.70077811900626</v>
       </c>
       <c r="CF97" s="11">
-        <v>-526.03331178874203</v>
+        <v>-526.03331178874248</v>
       </c>
       <c r="CH97" t="s">
         <v>3</v>
@@ -30371,7 +30371,7 @@
         <v>519.5282666666667</v>
       </c>
       <c r="CK97" s="10">
-        <v>498.49899473333335</v>
+        <v>498.49899473333323</v>
       </c>
       <c r="CL97" s="10">
         <v>500.50297235259984</v>
@@ -30383,19 +30383,19 @@
         <v>433.77215264237418</v>
       </c>
       <c r="CO97" s="10">
-        <v>323.5748654302667</v>
+        <v>323.57486543026675</v>
       </c>
       <c r="CP97" s="10">
-        <v>335.01577921913901</v>
+        <v>335.01577921913912</v>
       </c>
       <c r="CQ97" s="10">
-        <v>-220.38955193251905</v>
+        <v>-220.38955193251911</v>
       </c>
       <c r="CR97" s="10">
-        <v>-227.81722456657826</v>
+        <v>-227.81722456657849</v>
       </c>
       <c r="CS97" s="10">
-        <v>-317.00097989065631</v>
+        <v>-317.00097989065608</v>
       </c>
       <c r="CT97" s="10">
         <v>-554.06820663730014</v>
@@ -30404,16 +30404,16 @@
         <v>-669.85635383036947</v>
       </c>
       <c r="CV97" s="10">
-        <v>-676.87392768150926</v>
+        <v>-676.87392768150949</v>
       </c>
       <c r="CW97" s="10">
-        <v>-683.78665969730991</v>
+        <v>-683.78665969730923</v>
       </c>
       <c r="CX97" s="10">
         <v>-690.59360630125241</v>
       </c>
       <c r="CY97" s="10">
-        <v>-697.29381542463045</v>
+        <v>-697.29381542463057</v>
       </c>
       <c r="CZ97" s="10">
         <v>-703.88632643011897</v>
@@ -30425,22 +30425,22 @@
         <v>-596.74390794209125</v>
       </c>
       <c r="DC97" s="10">
-        <v>-558.51134978023651</v>
+        <v>-558.51134978023674</v>
       </c>
       <c r="DD97" s="10">
-        <v>-523.64003192825862</v>
+        <v>-523.64003192825874</v>
       </c>
       <c r="DE97" s="10">
-        <v>-488.79687221561312</v>
+        <v>-488.79687221561323</v>
       </c>
       <c r="DF97" s="10">
-        <v>-453.98212406555336</v>
+        <v>-453.98212406555353</v>
       </c>
       <c r="DG97" s="10">
-        <v>-419.19604318214351</v>
+        <v>-419.1960431821434</v>
       </c>
       <c r="DH97" s="11">
-        <v>-381.10555423744904</v>
+        <v>-381.10555423744916</v>
       </c>
     </row>
     <row r="99" spans="1:112" x14ac:dyDescent="0.35">
@@ -30476,13 +30476,13 @@
         <v>1</v>
       </c>
       <c r="B101" s="3">
-        <v>-189.4666666666667</v>
+        <v>-189.46666666666664</v>
       </c>
       <c r="C101" s="4">
-        <v>114.36763333333329</v>
+        <v>114.36763333333343</v>
       </c>
       <c r="D101" s="4">
-        <v>263.53654203333349</v>
+        <v>263.53654203333338</v>
       </c>
       <c r="E101" s="4">
         <v>320.8462270809664</v>
@@ -30491,13 +30491,13 @@
         <v>304.84764312469463</v>
       </c>
       <c r="G101" s="4">
-        <v>288.98857191281684</v>
+        <v>288.98857191281701</v>
       </c>
       <c r="H101" s="4">
         <v>294.21308032912043</v>
       </c>
       <c r="I101" s="4">
-        <v>501.57004976682725</v>
+        <v>501.57004976682748</v>
       </c>
       <c r="J101" s="4">
         <v>497.56891354806214</v>
@@ -30506,13 +30506,13 @@
         <v>648.27193376999469</v>
       </c>
       <c r="L101" s="4">
-        <v>659.84611450725765</v>
+        <v>659.84611450725788</v>
       </c>
       <c r="M101" s="4">
-        <v>655.95846287115637</v>
+        <v>655.95846287115626</v>
       </c>
       <c r="N101" s="4">
-        <v>652.10932237032989</v>
+        <v>652.10932237033012</v>
       </c>
       <c r="O101" s="4">
         <v>586.29903960499632</v>
@@ -30530,7 +30530,7 @@
         <v>413.67678193998233</v>
       </c>
       <c r="T101" s="4">
-        <v>460.38233964410887</v>
+        <v>460.38233964410892</v>
       </c>
       <c r="U101" s="4">
         <v>507.01174736757264</v>
@@ -30539,10 +30539,10 @@
         <v>550.23098642721413</v>
       </c>
       <c r="W101" s="4">
-        <v>590.03936530505905</v>
+        <v>590.03936530505928</v>
       </c>
       <c r="X101" s="4">
-        <v>601.85817725596974</v>
+        <v>601.85817725596985</v>
       </c>
       <c r="Y101" s="4">
         <v>577.7364008512734</v>
@@ -30551,7 +30551,7 @@
         <v>531.44669512560142</v>
       </c>
       <c r="AA101" s="5">
-        <v>481.99054871506479</v>
+        <v>481.99054871506462</v>
       </c>
       <c r="AD101" s="1" t="s">
         <v>1</v>
@@ -30578,10 +30578,10 @@
         <v>427.12275622467229</v>
       </c>
       <c r="AL101" s="4">
-        <v>541.81672076104405</v>
+        <v>541.81672076104428</v>
       </c>
       <c r="AM101" s="4">
-        <v>538.17780458122672</v>
+        <v>538.17780458122684</v>
       </c>
       <c r="AN101" s="4">
         <v>689.24630482245789</v>
@@ -30593,7 +30593,7 @@
         <v>697.67369152661922</v>
       </c>
       <c r="AQ101" s="4">
-        <v>678.70450235891701</v>
+        <v>678.70450235892019</v>
       </c>
       <c r="AR101" s="4">
         <v>628.76852130977852</v>
@@ -30605,7 +30605,7 @@
         <v>382.66715504358069</v>
       </c>
       <c r="AU101" s="4">
-        <v>379.364692772306</v>
+        <v>379.36469277230617</v>
       </c>
       <c r="AV101" s="4">
         <v>361.61841312322923</v>
@@ -30614,10 +30614,10 @@
         <v>377.89674598997317</v>
       </c>
       <c r="AX101" s="4">
-        <v>423.78378337054983</v>
+        <v>423.78378337054971</v>
       </c>
       <c r="AY101" s="4">
-        <v>466.25397075421802</v>
+        <v>466.25397075421813</v>
       </c>
       <c r="AZ101" s="4">
         <v>505.30655649100618</v>
@@ -30644,10 +30644,10 @@
         <v>-24.784216666666467</v>
       </c>
       <c r="BI101" s="4">
-        <v>-19.473007949999655</v>
+        <v>-19.473007949999726</v>
       </c>
       <c r="BJ101" s="4">
-        <v>648.75855015292041</v>
+        <v>648.75855015290813</v>
       </c>
       <c r="BK101" s="4">
         <v>743.94918049325679</v>
@@ -30671,49 +30671,49 @@
         <v>823.55984636791572</v>
       </c>
       <c r="BR101" s="4">
-        <v>821.14561831856031</v>
+        <v>821.1456183185602</v>
       </c>
       <c r="BS101" s="4">
         <v>756.78316221676062</v>
       </c>
       <c r="BT101" s="4">
-        <v>754.47294401004467</v>
+        <v>754.47294401004456</v>
       </c>
       <c r="BU101" s="4">
-        <v>533.51543383946819</v>
+        <v>533.5154338394683</v>
       </c>
       <c r="BV101" s="4">
-        <v>517.34037575228967</v>
+        <v>517.3403757522874</v>
       </c>
       <c r="BW101" s="4">
-        <v>578.24463859060108</v>
+        <v>578.24463859058437</v>
       </c>
       <c r="BX101" s="4">
         <v>594.41391847546333</v>
       </c>
       <c r="BY101" s="4">
-        <v>558.99375526942401</v>
+        <v>558.99375526941424</v>
       </c>
       <c r="BZ101" s="4">
-        <v>494.74023713044056</v>
+        <v>494.74023713044272</v>
       </c>
       <c r="CA101" s="4">
-        <v>531.40118909192586</v>
+        <v>531.4011890919171</v>
       </c>
       <c r="CB101" s="4">
-        <v>524.99486510607096</v>
+        <v>524.99486510606664</v>
       </c>
       <c r="CC101" s="4">
-        <v>496.7440061078247</v>
+        <v>496.74400610782459</v>
       </c>
       <c r="CD101" s="4">
-        <v>494.9827354961285</v>
+        <v>494.98273549612827</v>
       </c>
       <c r="CE101" s="4">
-        <v>493.27911344892686</v>
+        <v>493.27911344892669</v>
       </c>
       <c r="CF101" s="5">
-        <v>470.70001203146865</v>
+        <v>470.70001203146262</v>
       </c>
       <c r="CH101" s="1" t="s">
         <v>1</v>
@@ -30725,19 +30725,19 @@
         <v>102.5623333333333</v>
       </c>
       <c r="CK101" s="4">
-        <v>251.62499433333338</v>
+        <v>251.62499433333352</v>
       </c>
       <c r="CL101" s="4">
-        <v>345.80824969566612</v>
+        <v>345.80824969566595</v>
       </c>
       <c r="CM101" s="4">
         <v>330.03432394292673</v>
       </c>
       <c r="CN101" s="4">
-        <v>314.40193285841292</v>
+        <v>314.40193285841303</v>
       </c>
       <c r="CO101" s="4">
-        <v>298.91235025413857</v>
+        <v>298.91235025413846</v>
       </c>
       <c r="CP101" s="4">
         <v>508.27782826586332</v>
@@ -30752,31 +30752,31 @@
         <v>666.73663790591365</v>
       </c>
       <c r="CT101" s="4">
-        <v>662.91100098039999</v>
+        <v>662.91100098040033</v>
       </c>
       <c r="CU101" s="4">
         <v>597.12443332255702</v>
       </c>
       <c r="CV101" s="4">
-        <v>593.37728655579349</v>
+        <v>593.37728655579338</v>
       </c>
       <c r="CW101" s="4">
-        <v>459.62436441288116</v>
+        <v>459.62436441288673</v>
       </c>
       <c r="CX101" s="4">
-        <v>324.61509149022334</v>
+        <v>324.61509149022345</v>
       </c>
       <c r="CY101" s="4">
         <v>353.3923103057806</v>
       </c>
       <c r="CZ101" s="4">
-        <v>400.05180776519938</v>
+        <v>400.05180776519933</v>
       </c>
       <c r="DA101" s="4">
-        <v>446.63474070175289</v>
+        <v>446.634740701753</v>
       </c>
       <c r="DB101" s="4">
-        <v>493.14042003473537</v>
+        <v>493.14042003473543</v>
       </c>
       <c r="DC101" s="4">
         <v>536.23481714838158</v>
@@ -30794,7 +30794,7 @@
         <v>561.57635737379826</v>
       </c>
       <c r="DH101" s="5">
-        <v>512.3913779234955</v>
+        <v>512.39137792349538</v>
       </c>
     </row>
     <row r="102" spans="1:112" x14ac:dyDescent="0.35">
@@ -30802,13 +30802,13 @@
         <v>2</v>
       </c>
       <c r="B102" s="6">
-        <v>-169.4666666666667</v>
+        <v>-169.46666666666664</v>
       </c>
       <c r="C102" s="7">
-        <v>-687.0653666666667</v>
+        <v>-687.06536666666682</v>
       </c>
       <c r="D102" s="7">
-        <v>-767.97855496666682</v>
+        <v>-767.97855496666671</v>
       </c>
       <c r="E102" s="7">
         <v>-802.90884004603333</v>
@@ -30817,13 +30817,13 @@
         <v>-801.13121960644753</v>
       </c>
       <c r="G102" s="7">
-        <v>-799.3691005829055</v>
+        <v>-799.36910058290562</v>
       </c>
       <c r="H102" s="7">
         <v>-808.09402812269593</v>
       </c>
       <c r="I102" s="7">
-        <v>-552.01587780528996</v>
+        <v>-552.01587780529007</v>
       </c>
       <c r="J102" s="7">
         <v>-538.8692873722041</v>
@@ -30838,13 +30838,13 @@
         <v>-330.00637800522833</v>
       </c>
       <c r="N102" s="7">
-        <v>-317.35920207394167</v>
+        <v>-317.35920207394179</v>
       </c>
       <c r="O102" s="7">
         <v>-180.83970155927369</v>
       </c>
       <c r="P102" s="7">
-        <v>-168.44902553997372</v>
+        <v>-168.44902553997366</v>
       </c>
       <c r="Q102" s="7">
         <v>354.65804355451417</v>
@@ -30856,7 +30856,7 @@
         <v>183.49190054002315</v>
       </c>
       <c r="T102" s="7">
-        <v>94.723094311550042</v>
+        <v>94.723094311549858</v>
       </c>
       <c r="U102" s="7">
         <v>6.0538688270203238</v>
@@ -30865,10 +30865,10 @@
         <v>-75.848213020203161</v>
       </c>
       <c r="W102" s="7">
-        <v>-150.9822469373849</v>
+        <v>-150.98224693738513</v>
       </c>
       <c r="X102" s="7">
-        <v>-212.0583159914039</v>
+        <v>-212.05831599140424</v>
       </c>
       <c r="Y102" s="7">
         <v>-221.60034083532673</v>
@@ -30877,7 +30877,7 @@
         <v>-253.49407723617804</v>
       </c>
       <c r="AA102" s="8">
-        <v>-288.73969059797003</v>
+        <v>-288.7396905979702</v>
       </c>
       <c r="AD102" t="s">
         <v>2</v>
@@ -30907,7 +30907,7 @@
         <v>-684.25493964343104</v>
       </c>
       <c r="AM102" s="7">
-        <v>-672.29850076688842</v>
+        <v>-672.2985007668882</v>
       </c>
       <c r="AN102" s="7">
         <v>-505.80928727379001</v>
@@ -30919,31 +30919,31 @@
         <v>-467.07070073032082</v>
       </c>
       <c r="AQ102" s="7">
-        <v>-424.6661322540096</v>
+        <v>-424.66613225401585</v>
       </c>
       <c r="AR102" s="7">
         <v>-320.38228430355849</v>
       </c>
       <c r="AS102" s="7">
-        <v>-309.24749152895697</v>
+        <v>-309.24749152895708</v>
       </c>
       <c r="AT102" s="7">
         <v>268.4793477139491</v>
       </c>
       <c r="AU102" s="7">
-        <v>279.3302951767082</v>
+        <v>279.33029517670826</v>
       </c>
       <c r="AV102" s="7">
         <v>275.54980594927065</v>
       </c>
       <c r="AW102" s="7">
-        <v>202.58887062849658</v>
+        <v>202.58887062849681</v>
       </c>
       <c r="AX102" s="7">
-        <v>114.89043713081946</v>
+        <v>114.89043713081981</v>
       </c>
       <c r="AY102" s="7">
-        <v>33.967884398330398</v>
+        <v>33.967884398330114</v>
       </c>
       <c r="AZ102" s="7">
         <v>-40.177804642084993</v>
@@ -30970,10 +30970,10 @@
         <v>-390.94371666666689</v>
       </c>
       <c r="BI102" s="7">
-        <v>-397.8891434500004</v>
+        <v>-397.88914345000035</v>
       </c>
       <c r="BJ102" s="7">
-        <v>-736.22310332828556</v>
+        <v>-736.22310332827942</v>
       </c>
       <c r="BK102" s="7">
         <v>-787.96431295272032</v>
@@ -31003,43 +31003,43 @@
         <v>-741.00181871221321</v>
       </c>
       <c r="BT102" s="7">
-        <v>-733.41110174728942</v>
+        <v>-733.41110174728931</v>
       </c>
       <c r="BU102" s="7">
-        <v>-288.59356832968137</v>
+        <v>-288.59356832968143</v>
       </c>
       <c r="BV102" s="7">
-        <v>-145.32150743638192</v>
+        <v>-145.32150743638425</v>
       </c>
       <c r="BW102" s="7">
-        <v>78.799898453231663</v>
+        <v>78.799898453214837</v>
       </c>
       <c r="BX102" s="7">
-        <v>103.95427567685738</v>
+        <v>103.95427567685772</v>
       </c>
       <c r="BY102" s="7">
-        <v>77.285075685631455</v>
+        <v>77.285075685621678</v>
       </c>
       <c r="BZ102" s="7">
-        <v>-8.068661570895074</v>
+        <v>-8.0686615708999057</v>
       </c>
       <c r="CA102" s="7">
-        <v>-87.516414227420682</v>
+        <v>-87.516414227429436</v>
       </c>
       <c r="CB102" s="7">
-        <v>-85.886896643149043</v>
+        <v>-85.886896643153591</v>
       </c>
       <c r="CC102" s="7">
-        <v>-106.34459149713825</v>
+        <v>-106.3445914971384</v>
       </c>
       <c r="CD102" s="7">
-        <v>-100.55755948727915</v>
+        <v>-100.55755948727906</v>
       </c>
       <c r="CE102" s="7">
-        <v>-94.959944189330713</v>
+        <v>-94.959944189330599</v>
       </c>
       <c r="CF102" s="8">
-        <v>-110.48709712553341</v>
+        <v>-110.48709712553875</v>
       </c>
       <c r="CH102" t="s">
         <v>2</v>
@@ -31051,10 +31051,10 @@
         <v>-671.62766666666676</v>
       </c>
       <c r="CK102" s="7">
-        <v>-752.40191566666692</v>
+        <v>-752.40191566666681</v>
       </c>
       <c r="CL102" s="7">
-        <v>-805.6823981143333</v>
+        <v>-805.68239811433318</v>
       </c>
       <c r="CM102" s="7">
         <v>-803.92973969736215</v>
@@ -31078,31 +31078,31 @@
         <v>-365.42038169085924</v>
       </c>
       <c r="CT102" s="7">
-        <v>-352.85043179274345</v>
+        <v>-352.85043179274362</v>
       </c>
       <c r="CU102" s="7">
-        <v>-216.40885234554463</v>
+        <v>-216.40885234554452</v>
       </c>
       <c r="CV102" s="7">
-        <v>-204.09679868332108</v>
+        <v>-204.09679868332083</v>
       </c>
       <c r="CW102" s="7">
-        <v>68.1756655723579</v>
+        <v>68.175665572346929</v>
       </c>
       <c r="CX102" s="7">
-        <v>364.84647131590123</v>
+        <v>364.846471315901</v>
       </c>
       <c r="CY102" s="7">
-        <v>290.01774806167145</v>
+        <v>290.01774806167174</v>
       </c>
       <c r="CZ102" s="7">
-        <v>201.30917446089313</v>
+        <v>201.30917446089342</v>
       </c>
       <c r="DA102" s="7">
-        <v>112.70072369770787</v>
+        <v>112.70072369770764</v>
       </c>
       <c r="DB102" s="7">
-        <v>24.193296877653893</v>
+        <v>24.193296877653665</v>
       </c>
       <c r="DC102" s="7">
         <v>-57.545530117114367</v>
@@ -31117,10 +31117,10 @@
         <v>-227.86191020068873</v>
       </c>
       <c r="DG102" s="7">
-        <v>-256.84181748597746</v>
+        <v>-256.84181748597763</v>
       </c>
       <c r="DH102" s="8">
-        <v>-292.11756051001811</v>
+        <v>-292.11756051001788</v>
       </c>
     </row>
     <row r="103" spans="1:112" x14ac:dyDescent="0.35">
@@ -31128,13 +31128,13 @@
         <v>3</v>
       </c>
       <c r="B103" s="9">
-        <v>358.93333333333339</v>
+        <v>358.93333333333328</v>
       </c>
       <c r="C103" s="10">
-        <v>572.69773333333342</v>
+        <v>572.6977333333333</v>
       </c>
       <c r="D103" s="10">
-        <v>504.44201293333333</v>
+        <v>504.44201293333344</v>
       </c>
       <c r="E103" s="10">
         <v>482.06261296506716</v>
@@ -31143,13 +31143,13 @@
         <v>496.28357648175279</v>
       </c>
       <c r="G103" s="10">
-        <v>510.38052867008878</v>
+        <v>510.38052867008867</v>
       </c>
       <c r="H103" s="10">
         <v>513.8809477935755</v>
       </c>
       <c r="I103" s="10">
-        <v>50.445828038462764</v>
+        <v>50.445828038462622</v>
       </c>
       <c r="J103" s="10">
         <v>41.300373824142014</v>
@@ -31158,19 +31158,19 @@
         <v>-277.09272281144092</v>
       </c>
       <c r="L103" s="10">
-        <v>-317.0660239834105</v>
+        <v>-317.06602398341067</v>
       </c>
       <c r="M103" s="10">
-        <v>-325.95208486592804</v>
+        <v>-325.95208486592793</v>
       </c>
       <c r="N103" s="10">
-        <v>-334.75012029638822</v>
+        <v>-334.75012029638833</v>
       </c>
       <c r="O103" s="10">
         <v>-405.45933804572263</v>
       </c>
       <c r="P103" s="10">
-        <v>-414.0789387548009</v>
+        <v>-414.07893875480096</v>
       </c>
       <c r="Q103" s="10">
         <v>-678.03130436576805</v>
@@ -31182,7 +31182,7 @@
         <v>-597.16868248000537</v>
       </c>
       <c r="T103" s="10">
-        <v>-555.10543395565901</v>
+        <v>-555.10543395565878</v>
       </c>
       <c r="U103" s="10">
         <v>-513.06561619459308</v>
@@ -31191,10 +31191,10 @@
         <v>-474.38277340701109</v>
       </c>
       <c r="W103" s="10">
-        <v>-439.05711836767421</v>
+        <v>-439.05711836767415</v>
       </c>
       <c r="X103" s="10">
-        <v>-389.79986126456572</v>
+        <v>-389.79986126456561</v>
       </c>
       <c r="Y103" s="10">
         <v>-356.13606001594667</v>
@@ -31203,7 +31203,7 @@
         <v>-277.95261788942338</v>
       </c>
       <c r="AA103" s="11">
-        <v>-193.25085811709477</v>
+        <v>-193.25085811709442</v>
       </c>
       <c r="AD103" t="s">
         <v>3</v>
@@ -31227,13 +31227,13 @@
         <v>374.84260362690827</v>
       </c>
       <c r="AK103" s="10">
-        <v>387.59458705955058</v>
+        <v>387.59458705955052</v>
       </c>
       <c r="AL103" s="10">
-        <v>142.43821888238676</v>
+        <v>142.43821888238682</v>
       </c>
       <c r="AM103" s="10">
-        <v>134.12069618566159</v>
+        <v>134.12069618566136</v>
       </c>
       <c r="AN103" s="10">
         <v>-183.43701754866777</v>
@@ -31245,31 +31245,31 @@
         <v>-230.6029907962984</v>
       </c>
       <c r="AQ103" s="10">
-        <v>-254.0383701049075</v>
+        <v>-254.03837010490429</v>
       </c>
       <c r="AR103" s="10">
         <v>-308.38623700622003</v>
       </c>
       <c r="AS103" s="10">
-        <v>-316.132179805943</v>
+        <v>-316.13217980594288</v>
       </c>
       <c r="AT103" s="10">
         <v>-651.14650275752979</v>
       </c>
       <c r="AU103" s="10">
-        <v>-658.69498794901426</v>
+        <v>-658.69498794901438</v>
       </c>
       <c r="AV103" s="10">
         <v>-637.16821907250005</v>
       </c>
       <c r="AW103" s="10">
-        <v>-580.48561661846975</v>
+        <v>-580.48561661846986</v>
       </c>
       <c r="AX103" s="10">
-        <v>-538.67422050136929</v>
+        <v>-538.6742205013694</v>
       </c>
       <c r="AY103" s="10">
-        <v>-500.22185515254841</v>
+        <v>-500.22185515254824</v>
       </c>
       <c r="AZ103" s="10">
         <v>-465.12875184892118</v>
@@ -31296,10 +31296,10 @@
         <v>415.72793333333334</v>
       </c>
       <c r="BI103" s="10">
-        <v>417.36215140000007</v>
+        <v>417.36215140000013</v>
       </c>
       <c r="BJ103" s="10">
-        <v>87.464553175365154</v>
+        <v>87.464553175371293</v>
       </c>
       <c r="BK103" s="10">
         <v>44.01513245946353</v>
@@ -31323,49 +31323,49 @@
         <v>57.13679169809302</v>
       </c>
       <c r="BR103" s="10">
-        <v>51.618556156708905</v>
+        <v>51.618556156709076</v>
       </c>
       <c r="BS103" s="10">
         <v>-15.781343504547294</v>
       </c>
       <c r="BT103" s="10">
-        <v>-21.061842262755249</v>
+        <v>-21.061842262755135</v>
       </c>
       <c r="BU103" s="10">
         <v>-244.92186550978681</v>
       </c>
       <c r="BV103" s="10">
-        <v>-372.01886831590787</v>
+        <v>-372.01886831590321</v>
       </c>
       <c r="BW103" s="10">
-        <v>-657.04453704383275</v>
+        <v>-657.04453704379921</v>
       </c>
       <c r="BX103" s="10">
-        <v>-698.36819415232071</v>
+        <v>-698.36819415232094</v>
       </c>
       <c r="BY103" s="10">
-        <v>-636.27883095505547</v>
+        <v>-636.27883095503591</v>
       </c>
       <c r="BZ103" s="10">
-        <v>-486.67157555954549</v>
+        <v>-486.67157555954282</v>
       </c>
       <c r="CA103" s="10">
-        <v>-443.88477486450518</v>
+        <v>-443.88477486448755</v>
       </c>
       <c r="CB103" s="10">
-        <v>-439.10796846292192</v>
+        <v>-439.10796846291305</v>
       </c>
       <c r="CC103" s="10">
-        <v>-390.39941461068645</v>
+        <v>-390.39941461068616</v>
       </c>
       <c r="CD103" s="10">
-        <v>-394.42517600884935</v>
+        <v>-394.42517600884918</v>
       </c>
       <c r="CE103" s="10">
-        <v>-398.31916925959615</v>
+        <v>-398.31916925959604</v>
       </c>
       <c r="CF103" s="11">
-        <v>-360.21291490593524</v>
+        <v>-360.21291490592387</v>
       </c>
       <c r="CH103" t="s">
         <v>3</v>
@@ -31377,19 +31377,19 @@
         <v>569.06533333333346</v>
       </c>
       <c r="CK103" s="10">
-        <v>500.77692133333346</v>
+        <v>500.77692133333329</v>
       </c>
       <c r="CL103" s="10">
-        <v>459.87414841866723</v>
+        <v>459.87414841866735</v>
       </c>
       <c r="CM103" s="10">
         <v>473.89541575443548</v>
       </c>
       <c r="CN103" s="10">
-        <v>487.79087449622557</v>
+        <v>487.79087449622551</v>
       </c>
       <c r="CO103" s="10">
-        <v>501.55939236669155</v>
+        <v>501.55939236669178</v>
       </c>
       <c r="CP103" s="10">
         <v>65.777893179116631</v>
@@ -31404,31 +31404,31 @@
         <v>-301.31625621505441</v>
       </c>
       <c r="CT103" s="10">
-        <v>-310.06056918765654</v>
+        <v>-310.06056918765671</v>
       </c>
       <c r="CU103" s="10">
-        <v>-380.71558097701239</v>
+        <v>-380.71558097701256</v>
       </c>
       <c r="CV103" s="10">
-        <v>-389.28048787247241</v>
+        <v>-389.28048787247246</v>
       </c>
       <c r="CW103" s="10">
-        <v>-527.80002998523912</v>
+        <v>-527.80002998523355</v>
       </c>
       <c r="CX103" s="10">
-        <v>-689.46156280612456</v>
+        <v>-689.46156280612445</v>
       </c>
       <c r="CY103" s="10">
         <v>-643.41005836745217</v>
       </c>
       <c r="CZ103" s="10">
-        <v>-601.36098222609246</v>
+        <v>-601.36098222609257</v>
       </c>
       <c r="DA103" s="10">
-        <v>-559.33546439946076</v>
+        <v>-559.33546439946053</v>
       </c>
       <c r="DB103" s="10">
-        <v>-517.33371691238915</v>
+        <v>-517.33371691238904</v>
       </c>
       <c r="DC103" s="10">
         <v>-478.68928703126721</v>
@@ -31443,10 +31443,10 @@
         <v>-376.79171464299907</v>
       </c>
       <c r="DG103" s="10">
-        <v>-304.73453988782069</v>
+        <v>-304.73453988782063</v>
       </c>
       <c r="DH103" s="11">
-        <v>-220.27381741347739</v>
+        <v>-220.27381741347756</v>
       </c>
     </row>
     <row r="105" spans="1:112" x14ac:dyDescent="0.35">
@@ -31537,7 +31537,7 @@
         <v>6</v>
       </c>
       <c r="B106" s="15">
-        <v>10864915.645055851</v>
+        <v>10864915.645055875</v>
       </c>
       <c r="C106" s="16">
         <v>10688858.721648078</v>
@@ -31576,7 +31576,7 @@
         <v>10225567.125074334</v>
       </c>
       <c r="O106" s="16">
-        <v>10209911.156445287</v>
+        <v>10209911.156445289</v>
       </c>
       <c r="P106" s="16">
         <v>10196871.668380335</v>
@@ -31884,86 +31884,86 @@
         <v>10</v>
       </c>
       <c r="B111" s="6">
-        <v>92018449605.561722</v>
+        <v>92018449605.561783</v>
       </c>
       <c r="C111" s="7">
-        <v>87054753589.558701</v>
+        <v>87054753589.558716</v>
       </c>
       <c r="D111" s="7">
-        <v>82358811249.529282</v>
+        <v>82358811249.529297</v>
       </c>
       <c r="E111" s="7">
-        <v>77916179309.582672</v>
+        <v>77916179309.582687</v>
       </c>
       <c r="F111" s="7">
-        <v>73713193598.793442</v>
+        <v>73713193598.793457</v>
       </c>
       <c r="G111" s="7">
-        <v>69736927024.409882</v>
+        <v>69736927024.409897</v>
       </c>
       <c r="H111" s="7">
-        <v>65975149812.088356</v>
+        <v>65975149812.088364</v>
       </c>
       <c r="I111" s="7">
-        <v>62416291890.864761</v>
+        <v>62416291890.864769</v>
       </c>
       <c r="J111" s="7">
-        <v>59049407307.170975</v>
+        <v>59049407307.170982</v>
       </c>
       <c r="K111" s="7">
-        <v>55864140558.444633</v>
+        <v>55864140558.444641</v>
       </c>
       <c r="L111" s="7">
-        <v>52850694742.78479</v>
+        <v>52850694742.784798</v>
       </c>
       <c r="M111" s="7">
-        <v>49999801426.691597</v>
+        <v>49999801426.691605</v>
       </c>
       <c r="N111" s="7">
-        <v>47302692138.212425</v>
+        <v>47302692138.212433</v>
       </c>
       <c r="O111" s="7">
-        <v>44751071397.816116</v>
+        <v>44751071397.816124</v>
       </c>
       <c r="P111" s="7">
-        <v>42337091204.046562</v>
+        <v>42337091204.04657</v>
       </c>
       <c r="Q111" s="7">
-        <v>40053326895.4814</v>
+        <v>40053326895.481407</v>
       </c>
       <c r="R111" s="7">
-        <v>37892754314.754585</v>
+        <v>37892754314.754593</v>
       </c>
       <c r="S111" s="7">
-        <v>35848728204.406364</v>
+        <v>35848728204.406372</v>
       </c>
       <c r="T111" s="7">
-        <v>33914961768.112995</v>
+        <v>33914961768.113003</v>
       </c>
       <c r="U111" s="7">
-        <v>32085507334.432735</v>
+        <v>32085507334.432743</v>
       </c>
       <c r="V111" s="7">
-        <v>30354738063.595829</v>
+        <v>30354738063.595837</v>
       </c>
       <c r="W111" s="7">
-        <v>28717330641.074116</v>
+        <v>28717330641.074123</v>
       </c>
       <c r="X111" s="7">
-        <v>27168248904.701038</v>
+        <v>27168248904.701046</v>
       </c>
       <c r="Y111" s="7">
-        <v>25702728354.984093</v>
+        <v>25702728354.9841</v>
       </c>
       <c r="Z111" s="7">
-        <v>24316261500.968197</v>
+        <v>24316261500.968204</v>
       </c>
       <c r="AA111" s="8">
-        <v>23004583996.578365</v>
+        <v>23004583996.578377</v>
       </c>
       <c r="AB111" s="13">
         <f t="shared" si="0"/>
-        <v>1302403824834.646</v>
+        <v>1302403824834.6462</v>
       </c>
     </row>
     <row r="112" spans="1:112" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Solar capex time series
-Updated shading of cells in data_in to better represent changable inputs
-Added time series for solar capex to data_in
-Adjusted objective function to use solar capex time series
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DH119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM46" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="DR94" sqref="DR94"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="BY60" sqref="BY60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1374,7 +1374,7 @@
         <v>665.6</v>
       </c>
       <c r="C4" s="7">
-        <v>457.273792493884</v>
+        <v>471.4669395962901</v>
       </c>
       <c r="D4" s="7">
         <v>665.6</v>
@@ -2242,22 +2242,22 @@
         <v>0</v>
       </c>
       <c r="BZ6" s="7">
-        <v>7.9160244759759735</v>
+        <v>0</v>
       </c>
       <c r="CA6" s="7">
-        <v>11.660108696259158</v>
+        <v>0</v>
       </c>
       <c r="CB6" s="7">
-        <v>15.977889674524704</v>
+        <v>0</v>
       </c>
       <c r="CC6" s="7">
-        <v>20.874530681594479</v>
+        <v>10.874530681594479</v>
       </c>
       <c r="CD6" s="7">
-        <v>16.355241457727971</v>
+        <v>6.3552414577279706</v>
       </c>
       <c r="CE6" s="7">
-        <v>12.42527863084797</v>
+        <v>2.4252786308479699</v>
       </c>
       <c r="CF6" s="8">
         <v>0</v>
@@ -3181,52 +3181,52 @@
         <v>77.552686789826112</v>
       </c>
       <c r="BM9" s="7">
-        <v>83.782100970934152</v>
+        <v>53.782100970934152</v>
       </c>
       <c r="BN9" s="7">
-        <v>80.517579879671757</v>
+        <v>30.517579879671757</v>
       </c>
       <c r="BO9" s="7">
-        <v>57.763678098588571</v>
+        <v>7.7636780985885707</v>
       </c>
       <c r="BP9" s="7">
-        <v>25.524991201475132</v>
+        <v>0</v>
       </c>
       <c r="BQ9" s="7">
-        <v>3.8061561222875753</v>
+        <v>0</v>
       </c>
       <c r="BR9" s="7">
-        <v>2.6118515273865341</v>
+        <v>0</v>
       </c>
       <c r="BS9" s="7">
-        <v>1.9467981911329844</v>
+        <v>0</v>
       </c>
       <c r="BT9" s="7">
-        <v>1.8157593748528598</v>
+        <v>0</v>
       </c>
       <c r="BU9" s="7">
-        <v>2.2235412092268234</v>
+        <v>0</v>
       </c>
       <c r="BV9" s="7">
-        <v>3.174993080107015</v>
+        <v>0</v>
       </c>
       <c r="BW9" s="7">
-        <v>4.6750080178280768</v>
+        <v>0</v>
       </c>
       <c r="BX9" s="7">
-        <v>6.728523089986993</v>
+        <v>0</v>
       </c>
       <c r="BY9" s="7">
-        <v>49.340519797797242</v>
+        <v>0</v>
       </c>
       <c r="BZ9" s="7">
-        <v>84.6</v>
+        <v>22.516024475976337</v>
       </c>
       <c r="CA9" s="7">
-        <v>84.6</v>
+        <v>66.260108696259522</v>
       </c>
       <c r="CB9" s="7">
-        <v>84.6</v>
+        <v>80.577889674525068</v>
       </c>
       <c r="CC9" s="7">
         <v>84.6</v>
@@ -3238,7 +3238,7 @@
         <v>84.6</v>
       </c>
       <c r="CF9" s="8">
-        <v>83.689946138523737</v>
+        <v>13.689946138523737</v>
       </c>
       <c r="CH9">
         <v>7</v>
@@ -6590,10 +6590,10 @@
         <v>2114.4</v>
       </c>
       <c r="C20" s="7">
-        <v>1085.5082075061152</v>
+        <v>1046.3150604037091</v>
       </c>
       <c r="D20" s="7">
-        <v>915.30403799999885</v>
+        <v>890.30403799999885</v>
       </c>
       <c r="E20" s="7">
         <v>0</v>
@@ -6671,10 +6671,10 @@
         <v>2269.6</v>
       </c>
       <c r="AF20" s="7">
-        <v>1519.1249999999986</v>
+        <v>1484.1249999999986</v>
       </c>
       <c r="AG20" s="7">
-        <v>896.79596499999843</v>
+        <v>861.79596499999843</v>
       </c>
       <c r="AH20" s="7">
         <v>0</v>
@@ -6752,10 +6752,10 @@
         <v>2269.6</v>
       </c>
       <c r="BH20" s="7">
-        <v>1974.0059999999994</v>
+        <v>1924.0059999999994</v>
       </c>
       <c r="BI20" s="7">
-        <v>1362.6558939999982</v>
+        <v>1312.6558939999982</v>
       </c>
       <c r="BJ20" s="7">
         <v>0</v>
@@ -6833,10 +6833,10 @@
         <v>2189.64</v>
       </c>
       <c r="CJ20" s="7">
-        <v>443.87099999999964</v>
+        <v>408.87099999999964</v>
       </c>
       <c r="CK20" s="7">
-        <v>483.45507899999893</v>
+        <v>448.45507899999893</v>
       </c>
       <c r="CL20" s="7">
         <v>0</v>
@@ -8591,7 +8591,7 @@
         <v>15.3</v>
       </c>
       <c r="R26" s="7">
-        <v>15.3</v>
+        <v>6.5163161586489879</v>
       </c>
       <c r="S26" s="7">
         <v>15.3</v>
@@ -8690,7 +8690,7 @@
         <v>21.419999999999998</v>
       </c>
       <c r="BA26" s="7">
-        <v>0</v>
+        <v>17.142736481346155</v>
       </c>
       <c r="BB26" s="7">
         <v>0</v>
@@ -8750,7 +8750,7 @@
         <v>21.419999999999995</v>
       </c>
       <c r="BV26" s="7">
-        <v>21.419999999999998</v>
+        <v>0</v>
       </c>
       <c r="BW26" s="7">
         <v>21.419999999999998</v>
@@ -8843,7 +8843,7 @@
         <v>21.419999999999998</v>
       </c>
       <c r="DB26" s="7">
-        <v>21.419999999999998</v>
+        <v>10.091723826273146</v>
       </c>
       <c r="DC26" s="7">
         <v>21.419999999999998</v>
@@ -10045,7 +10045,7 @@
         <v>36.539999999999992</v>
       </c>
       <c r="BS30" s="7">
-        <v>36.540000000000006</v>
+        <v>13.886798191133025</v>
       </c>
       <c r="BT30" s="7">
         <v>36.540000000000006</v>
@@ -10371,7 +10371,7 @@
         <v>7</v>
       </c>
       <c r="BS31" s="7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BT31" s="7">
         <v>7</v>
@@ -10547,7 +10547,7 @@
         <v>10.100000000000001</v>
       </c>
       <c r="R32" s="7">
-        <v>10.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="S32" s="7">
         <v>10.100000000000001</v>
@@ -10643,7 +10643,7 @@
         <v>14.139999999999997</v>
       </c>
       <c r="AZ32" s="7">
-        <v>5.3701253531687705</v>
+        <v>14.139999999999997</v>
       </c>
       <c r="BA32" s="7">
         <v>0</v>
@@ -10706,7 +10706,7 @@
         <v>14.139999999999999</v>
       </c>
       <c r="BV32" s="7">
-        <v>14.139999999999999</v>
+        <v>0</v>
       </c>
       <c r="BW32" s="7">
         <v>14.139999999999999</v>
@@ -10796,10 +10796,10 @@
         <v>14.139999999999997</v>
       </c>
       <c r="DA32" s="7">
-        <v>14.139999999999997</v>
+        <v>6.5223724740072448</v>
       </c>
       <c r="DB32" s="7">
-        <v>8.6717238262742846</v>
+        <v>0</v>
       </c>
       <c r="DC32" s="7">
         <v>14.139999999999997</v>
@@ -13254,7 +13254,7 @@
         <v>7.0699999999999994</v>
       </c>
       <c r="BA40" s="7">
-        <v>0</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="BB40" s="7">
         <v>0</v>
@@ -13314,7 +13314,7 @@
         <v>7.07</v>
       </c>
       <c r="BV40" s="7">
-        <v>7.0699999999999985</v>
+        <v>0</v>
       </c>
       <c r="BW40" s="7">
         <v>7.0699999999999985</v>
@@ -13404,7 +13404,7 @@
         <v>7.07</v>
       </c>
       <c r="DA40" s="7">
-        <v>7.07</v>
+        <v>0</v>
       </c>
       <c r="DB40" s="7">
         <v>7.0699999999999994</v>
@@ -13957,7 +13957,7 @@
         <v>8.3999999999999986</v>
       </c>
       <c r="BS42" s="7">
-        <v>8.4000000000000057</v>
+        <v>0</v>
       </c>
       <c r="BT42" s="7">
         <v>8.4000000000000057</v>
@@ -14088,22 +14088,22 @@
         <v>0</v>
       </c>
       <c r="C43" s="7">
-        <v>1275</v>
+        <v>1300</v>
       </c>
       <c r="D43" s="7">
-        <v>1275</v>
+        <v>1300</v>
       </c>
       <c r="E43" s="7">
-        <v>897.96917434199895</v>
+        <v>947.96917434199895</v>
       </c>
       <c r="F43" s="7">
-        <v>876.78049691107663</v>
+        <v>926.78049691107663</v>
       </c>
       <c r="G43" s="7">
-        <v>855.94112138327546</v>
+        <v>905.94112138327546</v>
       </c>
       <c r="H43" s="7">
-        <v>845.45419147572466</v>
+        <v>865.45419147572466</v>
       </c>
       <c r="I43" s="7">
         <v>825.32287919900591</v>
@@ -14112,16 +14112,16 @@
         <v>785.55038511179646</v>
       </c>
       <c r="K43" s="7">
-        <v>736.13993857780224</v>
+        <v>756.13993857780224</v>
       </c>
       <c r="L43" s="7">
-        <v>697.09479802500209</v>
+        <v>727.09479802500209</v>
       </c>
       <c r="M43" s="7">
-        <v>678.4182512072266</v>
+        <v>698.4182512072266</v>
       </c>
       <c r="N43" s="7">
-        <v>660.11361546809076</v>
+        <v>670.11361546809076</v>
       </c>
       <c r="O43" s="7">
         <v>642.18423800730307</v>
@@ -14130,10 +14130,10 @@
         <v>624.63349614936851</v>
       </c>
       <c r="Q43" s="7">
-        <v>607.46479761471255</v>
+        <v>597.46479761471255</v>
       </c>
       <c r="R43" s="7">
-        <v>590.68158079324439</v>
+        <v>589.56526463459522</v>
       </c>
       <c r="S43" s="7">
         <v>624.44985201630652</v>
@@ -14172,22 +14172,22 @@
         <v>0</v>
       </c>
       <c r="AF43" s="7">
-        <v>1785</v>
+        <v>1820</v>
       </c>
       <c r="AG43" s="7">
-        <v>1785</v>
+        <v>1820</v>
       </c>
       <c r="AH43" s="7">
-        <v>1394.6563686849986</v>
+        <v>1444.6563686849986</v>
       </c>
       <c r="AI43" s="7">
-        <v>1378.7097160031635</v>
+        <v>1428.7097160031635</v>
       </c>
       <c r="AJ43" s="7">
-        <v>1363.1595434471919</v>
+        <v>1413.1595434471919</v>
       </c>
       <c r="AK43" s="7">
-        <v>1358.0094193382165</v>
+        <v>1378.0094193382165</v>
       </c>
       <c r="AL43" s="7">
         <v>1343.2629441122599</v>
@@ -14196,16 +14196,16 @@
         <v>1308.9237506092695</v>
       </c>
       <c r="AN43" s="7">
-        <v>1264.9955043647524</v>
+        <v>1284.9955043647524</v>
       </c>
       <c r="AO43" s="7">
-        <v>1231.4819039040349</v>
+        <v>1261.4819039040349</v>
       </c>
       <c r="AP43" s="7">
-        <v>1218.386681039171</v>
+        <v>1238.386681039171</v>
       </c>
       <c r="AQ43" s="7">
-        <v>1205.7136011685234</v>
+        <v>1215.7136011685234</v>
       </c>
       <c r="AR43" s="7">
         <v>1193.4664635790396</v>
@@ -14214,31 +14214,31 @@
         <v>1181.6491017512508</v>
       </c>
       <c r="AT43" s="7">
-        <v>1313.8353836670103</v>
+        <v>1303.8353836670103</v>
       </c>
       <c r="AU43" s="7">
-        <v>1159.3192121200136</v>
+        <v>1139.3192121200136</v>
       </c>
       <c r="AV43" s="7">
-        <v>1148.8145250290936</v>
+        <v>1128.8145250290936</v>
       </c>
       <c r="AW43" s="7">
-        <v>1178.7552957543548</v>
+        <v>1158.7552957543548</v>
       </c>
       <c r="AX43" s="7">
-        <v>1209.1455334161437</v>
+        <v>1189.1455334161437</v>
       </c>
       <c r="AY43" s="7">
-        <v>1199.989283216888</v>
+        <v>1219.989283216888</v>
       </c>
       <c r="AZ43" s="7">
-        <v>1200.0605014126709</v>
+        <v>1221.2906267658391</v>
       </c>
       <c r="BA43" s="7">
-        <v>1241.4709459253854</v>
+        <v>1241.4709459253852</v>
       </c>
       <c r="BB43" s="7">
-        <v>1785</v>
+        <v>1819.9999999999998</v>
       </c>
       <c r="BC43" s="7">
         <v>1325.4132711986604</v>
@@ -14253,79 +14253,79 @@
         <v>0</v>
       </c>
       <c r="BH43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BI43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BJ43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BK43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BL43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BM43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BN43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BO43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BP43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BQ43" s="7">
-        <v>2550</v>
+        <v>2583.8061561222876</v>
       </c>
       <c r="BR43" s="7">
-        <v>2550</v>
+        <v>2572.6118515273865</v>
       </c>
       <c r="BS43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BT43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="BU43" s="7">
-        <v>2550</v>
+        <v>2552.2235412092268</v>
       </c>
       <c r="BV43" s="7">
-        <v>2550</v>
+        <v>2585.8049930801071</v>
       </c>
       <c r="BW43" s="7">
-        <v>2550</v>
+        <v>2534.6750080178281</v>
       </c>
       <c r="BX43" s="7">
-        <v>2550</v>
+        <v>2536.728523089987</v>
       </c>
       <c r="BY43" s="7">
-        <v>2550</v>
+        <v>2579.3405197977972</v>
       </c>
       <c r="BZ43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="CA43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="CB43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="CC43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="CD43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="CE43" s="7">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="CF43" s="8">
-        <v>2550</v>
+        <v>2600</v>
       </c>
       <c r="CH43">
         <v>41</v>
@@ -14334,22 +14334,22 @@
         <v>0</v>
       </c>
       <c r="CJ43" s="7">
-        <v>1785</v>
+        <v>1820</v>
       </c>
       <c r="CK43" s="7">
-        <v>1785</v>
+        <v>1820</v>
       </c>
       <c r="CL43" s="7">
-        <v>977.59541471099874</v>
+        <v>1027.5954147109987</v>
       </c>
       <c r="CM43" s="7">
-        <v>957.89521344339755</v>
+        <v>1007.8952134433976</v>
       </c>
       <c r="CN43" s="7">
-        <v>938.55771036438728</v>
+        <v>988.55771036438728</v>
       </c>
       <c r="CO43" s="7">
-        <v>929.58616975766654</v>
+        <v>949.58616975766654</v>
       </c>
       <c r="CP43" s="7">
         <v>910.98388528548548</v>
@@ -14358,16 +14358,16 @@
         <v>872.75418025305407</v>
       </c>
       <c r="CR43" s="7">
-        <v>824.90040787533144</v>
+        <v>844.90040787533144</v>
       </c>
       <c r="CS43" s="7">
-        <v>787.42595154620903</v>
+        <v>817.42595154620903</v>
       </c>
       <c r="CT43" s="7">
-        <v>770.33422511012486</v>
+        <v>790.33422511012486</v>
       </c>
       <c r="CU43" s="7">
-        <v>753.62867313611514</v>
+        <v>763.62867313611514</v>
       </c>
       <c r="CV43" s="7">
         <v>737.3127711943398</v>
@@ -14376,19 +14376,19 @@
         <v>721.39002613508819</v>
       </c>
       <c r="CX43" s="7">
-        <v>705.86397637030313</v>
+        <v>695.86397637030313</v>
       </c>
       <c r="CY43" s="7">
-        <v>690.73819215763524</v>
+        <v>670.73819215763524</v>
       </c>
       <c r="CZ43" s="7">
-        <v>676.01627588705378</v>
+        <v>659.84102070964309</v>
       </c>
       <c r="DA43" s="7">
-        <v>701.70186237003691</v>
+        <v>696.38948989602954</v>
       </c>
       <c r="DB43" s="7">
-        <v>733.2668953050927</v>
+        <v>733.26689530509361</v>
       </c>
       <c r="DC43" s="7">
         <v>770.47619736283923</v>
@@ -14423,16 +14423,16 @@
         <v>0</v>
       </c>
       <c r="E44" s="7">
-        <v>3200</v>
+        <v>3150</v>
       </c>
       <c r="F44" s="7">
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="G44" s="7">
-        <v>3320</v>
+        <v>3270</v>
       </c>
       <c r="H44" s="7">
-        <v>3370</v>
+        <v>3350</v>
       </c>
       <c r="I44" s="7">
         <v>3430</v>
@@ -14441,16 +14441,16 @@
         <v>3510</v>
       </c>
       <c r="K44" s="7">
-        <v>3600</v>
+        <v>3580</v>
       </c>
       <c r="L44" s="7">
-        <v>3680</v>
+        <v>3650</v>
       </c>
       <c r="M44" s="7">
-        <v>3740</v>
+        <v>3720</v>
       </c>
       <c r="N44" s="7">
-        <v>3800</v>
+        <v>3790</v>
       </c>
       <c r="O44" s="7">
         <v>3860</v>
@@ -14459,10 +14459,10 @@
         <v>3920</v>
       </c>
       <c r="Q44" s="7">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="R44" s="7">
-        <v>4040</v>
+        <v>4060</v>
       </c>
       <c r="S44" s="7">
         <v>4049.8374630040767</v>
@@ -14507,16 +14507,16 @@
         <v>0</v>
       </c>
       <c r="AH44" s="7">
-        <v>3200</v>
+        <v>3150</v>
       </c>
       <c r="AI44" s="7">
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="AJ44" s="7">
-        <v>3320</v>
+        <v>3270</v>
       </c>
       <c r="AK44" s="7">
-        <v>3370</v>
+        <v>3350</v>
       </c>
       <c r="AL44" s="7">
         <v>3430</v>
@@ -14525,16 +14525,16 @@
         <v>3510</v>
       </c>
       <c r="AN44" s="7">
-        <v>3600</v>
+        <v>3580</v>
       </c>
       <c r="AO44" s="7">
-        <v>3680</v>
+        <v>3650</v>
       </c>
       <c r="AP44" s="7">
-        <v>3740</v>
+        <v>3720</v>
       </c>
       <c r="AQ44" s="7">
-        <v>3800</v>
+        <v>3790</v>
       </c>
       <c r="AR44" s="7">
         <v>3860</v>
@@ -14543,31 +14543,31 @@
         <v>3920</v>
       </c>
       <c r="AT44" s="7">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="AU44" s="7">
-        <v>4040</v>
+        <v>4060</v>
       </c>
       <c r="AV44" s="7">
-        <v>4100</v>
+        <v>4120</v>
       </c>
       <c r="AW44" s="7">
-        <v>4120</v>
+        <v>4140</v>
       </c>
       <c r="AX44" s="7">
-        <v>4140</v>
+        <v>4160</v>
       </c>
       <c r="AY44" s="7">
-        <v>4200</v>
+        <v>4180</v>
       </c>
       <c r="AZ44" s="7">
-        <v>4260</v>
+        <v>4230</v>
       </c>
       <c r="BA44" s="7">
-        <v>4304.2127364813459</v>
+        <v>4280</v>
       </c>
       <c r="BB44" s="7">
-        <v>3812.9126055483912</v>
+        <v>3777.9126055483912</v>
       </c>
       <c r="BC44" s="7">
         <v>4325.1983177996653</v>
@@ -14588,16 +14588,16 @@
         <v>0</v>
       </c>
       <c r="BJ44" s="7">
-        <v>3200</v>
+        <v>3150</v>
       </c>
       <c r="BK44" s="7">
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="BL44" s="7">
-        <v>3320</v>
+        <v>3270</v>
       </c>
       <c r="BM44" s="7">
-        <v>3370</v>
+        <v>3350</v>
       </c>
       <c r="BN44" s="7">
         <v>3430</v>
@@ -14606,55 +14606,55 @@
         <v>3510</v>
       </c>
       <c r="BP44" s="7">
-        <v>3600</v>
+        <v>3575.5249912014751</v>
       </c>
       <c r="BQ44" s="7">
-        <v>3680</v>
+        <v>3650</v>
       </c>
       <c r="BR44" s="7">
-        <v>3740</v>
+        <v>3720</v>
       </c>
       <c r="BS44" s="7">
-        <v>3800</v>
+        <v>3790</v>
       </c>
       <c r="BT44" s="7">
-        <v>3860</v>
+        <v>3811.8157593748529</v>
       </c>
       <c r="BU44" s="7">
         <v>3920</v>
       </c>
       <c r="BV44" s="7">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="BW44" s="7">
-        <v>4040</v>
+        <v>4060</v>
       </c>
       <c r="BX44" s="7">
-        <v>4100</v>
+        <v>4120</v>
       </c>
       <c r="BY44" s="7">
-        <v>4120</v>
+        <v>4140</v>
       </c>
       <c r="BZ44" s="7">
-        <v>4140</v>
+        <v>4160</v>
       </c>
       <c r="CA44" s="7">
-        <v>4200</v>
+        <v>4180</v>
       </c>
       <c r="CB44" s="7">
-        <v>4260</v>
+        <v>4230</v>
       </c>
       <c r="CC44" s="7">
-        <v>4320</v>
+        <v>4280</v>
       </c>
       <c r="CD44" s="7">
-        <v>4390</v>
+        <v>4350</v>
       </c>
       <c r="CE44" s="7">
-        <v>4460</v>
+        <v>4420</v>
       </c>
       <c r="CF44" s="8">
-        <v>4540</v>
+        <v>4560</v>
       </c>
       <c r="CH44">
         <v>42</v>
@@ -14669,16 +14669,16 @@
         <v>0</v>
       </c>
       <c r="CL44" s="7">
-        <v>3200</v>
+        <v>3150</v>
       </c>
       <c r="CM44" s="7">
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="CN44" s="7">
-        <v>3320</v>
+        <v>3270</v>
       </c>
       <c r="CO44" s="7">
-        <v>3370</v>
+        <v>3350</v>
       </c>
       <c r="CP44" s="7">
         <v>3430</v>
@@ -14687,16 +14687,16 @@
         <v>3510</v>
       </c>
       <c r="CR44" s="7">
-        <v>3600</v>
+        <v>3580</v>
       </c>
       <c r="CS44" s="7">
-        <v>3680</v>
+        <v>3650</v>
       </c>
       <c r="CT44" s="7">
-        <v>3740</v>
+        <v>3720</v>
       </c>
       <c r="CU44" s="7">
-        <v>3800</v>
+        <v>3790</v>
       </c>
       <c r="CV44" s="7">
         <v>3860</v>
@@ -14705,19 +14705,19 @@
         <v>3920</v>
       </c>
       <c r="CX44" s="7">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="CY44" s="7">
-        <v>4040</v>
+        <v>4060</v>
       </c>
       <c r="CZ44" s="7">
-        <v>4100</v>
+        <v>4116.1752551774107</v>
       </c>
       <c r="DA44" s="7">
-        <v>4120</v>
+        <v>4140</v>
       </c>
       <c r="DB44" s="7">
-        <v>4140</v>
+        <v>4160</v>
       </c>
       <c r="DC44" s="7">
         <v>4143.8340493407095</v>
@@ -16208,7 +16208,7 @@
         <v>73.107518076478414</v>
       </c>
       <c r="AV51" s="7">
-        <v>89.934885739166475</v>
+        <v>89.934885739166702</v>
       </c>
       <c r="AW51" s="7">
         <v>106.91369971081872</v>
@@ -16223,16 +16223,16 @@
         <v>0</v>
       </c>
       <c r="BA51" s="7">
-        <v>36.91456815331594</v>
+        <v>0</v>
       </c>
       <c r="BB51" s="7">
-        <v>98.036199266695803</v>
+        <v>58.036199266695803</v>
       </c>
       <c r="BC51" s="7">
-        <v>159.07792506009628</v>
+        <v>119.07792506009628</v>
       </c>
       <c r="BD51" s="8">
-        <v>230.03902638563704</v>
+        <v>230.12194722872619</v>
       </c>
       <c r="BF51">
         <v>2</v>
@@ -16247,7 +16247,7 @@
         <v>665.6</v>
       </c>
       <c r="BJ51" s="7">
-        <v>165.82611370416544</v>
+        <v>261.58553542439881</v>
       </c>
       <c r="BK51" s="7">
         <v>280.10920524321841</v>
@@ -16256,16 +16256,16 @@
         <v>298.79958809040727</v>
       </c>
       <c r="BM51" s="7">
-        <v>317.65818438322071</v>
+        <v>317.65818438322026</v>
       </c>
       <c r="BN51" s="7">
         <v>336.6865080426694</v>
       </c>
       <c r="BO51" s="7">
-        <v>355.88608661505282</v>
+        <v>355.88608661505327</v>
       </c>
       <c r="BP51" s="7">
-        <v>375.25846139458815</v>
+        <v>375.25846139458849</v>
       </c>
       <c r="BQ51" s="7">
         <v>394.80518754713955</v>
@@ -16286,28 +16286,28 @@
         <v>495.20950655093725</v>
       </c>
       <c r="BW51" s="7">
-        <v>500.64777300769947</v>
+        <v>515.83579210989569</v>
       </c>
       <c r="BX51" s="7">
-        <v>490.57227917738282</v>
+        <v>536.64771423888419</v>
       </c>
       <c r="BY51" s="7">
-        <v>256.34366264175742</v>
+        <v>335.96508679719312</v>
       </c>
       <c r="BZ51" s="7">
-        <v>363.60952756336383</v>
+        <v>268.15254289301748</v>
       </c>
       <c r="CA51" s="7">
-        <v>374.99432985262422</v>
+        <v>488.01190916595169</v>
       </c>
       <c r="CB51" s="7">
-        <v>447.55614125698077</v>
+        <v>559.72204143410488</v>
       </c>
       <c r="CC51" s="7">
-        <v>563.54828524621166</v>
+        <v>665.6</v>
       </c>
       <c r="CD51" s="7">
-        <v>651.0703703088609</v>
+        <v>665.6</v>
       </c>
       <c r="CE51" s="7">
         <v>665.6</v>
@@ -16382,7 +16382,7 @@
         <v>0</v>
       </c>
       <c r="DD51" s="7">
-        <v>28.414343687291648</v>
+        <v>20.892828156354426</v>
       </c>
       <c r="DE51" s="7">
         <v>44.839472780477195</v>
@@ -16740,52 +16740,52 @@
         <v>0</v>
       </c>
       <c r="F53" s="7">
-        <v>0</v>
+        <v>59.941662939991829</v>
       </c>
       <c r="G53" s="7">
-        <v>0</v>
+        <v>203.27894998393339</v>
       </c>
       <c r="H53" s="7">
-        <v>14.910437245356661</v>
+        <v>212</v>
       </c>
       <c r="I53" s="7">
         <v>195.57185514423463</v>
       </c>
       <c r="J53" s="7">
-        <v>151.27640184053234</v>
+        <v>156.15514273469071</v>
       </c>
       <c r="K53" s="7">
-        <v>97.302289457096322</v>
+        <v>180.73800643552298</v>
       </c>
       <c r="L53" s="7">
-        <v>53.652410062210038</v>
+        <v>212</v>
       </c>
       <c r="M53" s="7">
-        <v>153.95457502017643</v>
+        <v>212</v>
       </c>
       <c r="N53" s="7">
-        <v>199.84088052659854</v>
+        <v>212</v>
       </c>
       <c r="O53" s="7">
-        <v>122.51144681878031</v>
+        <v>212</v>
       </c>
       <c r="P53" s="7">
-        <v>152.49862794785849</v>
+        <v>212</v>
       </c>
       <c r="Q53" s="7">
-        <v>174.89348967831893</v>
+        <v>187.36956548652051</v>
       </c>
       <c r="R53" s="7">
-        <v>175.72729157589856</v>
+        <v>146.88587473854693</v>
       </c>
       <c r="S53" s="7">
-        <v>154.43023720008114</v>
+        <v>151.01209488003258</v>
       </c>
       <c r="T53" s="7">
-        <v>173.48150933488159</v>
+        <v>166.63260373395269</v>
       </c>
       <c r="U53" s="7">
-        <v>192.88424291889532</v>
+        <v>182.39369716755823</v>
       </c>
       <c r="V53" s="7">
         <v>198.29664044206618</v>
@@ -16818,13 +16818,13 @@
         <v>212</v>
       </c>
       <c r="AH53" s="7">
-        <v>79.534840979999331</v>
+        <v>212</v>
       </c>
       <c r="AI53" s="7">
-        <v>99.412096424523043</v>
+        <v>212</v>
       </c>
       <c r="AJ53" s="7">
-        <v>109.62406303975831</v>
+        <v>212</v>
       </c>
       <c r="AK53" s="7">
         <v>212</v>
@@ -16980,49 +16980,49 @@
         <v>212</v>
       </c>
       <c r="CL53" s="7">
-        <v>0</v>
+        <v>122.02341423766984</v>
       </c>
       <c r="CM53" s="7">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="CN53" s="7">
-        <v>133.56396162497799</v>
+        <v>212</v>
       </c>
       <c r="CO53" s="7">
+        <v>200.77401689151725</v>
+      </c>
+      <c r="CP53" s="7">
+        <v>201.25772080142997</v>
+      </c>
+      <c r="CQ53" s="7">
         <v>212</v>
       </c>
-      <c r="CP53" s="7">
-        <v>151.90893521210319</v>
-      </c>
-      <c r="CQ53" s="7">
-        <v>170.50618155598067</v>
-      </c>
       <c r="CR53" s="7">
-        <v>122.5618982891333</v>
+        <v>212</v>
       </c>
       <c r="CS53" s="7">
-        <v>118.28499079786911</v>
+        <v>195.84215296768775</v>
       </c>
       <c r="CT53" s="7">
-        <v>89.922865546287085</v>
+        <v>200.61744941421762</v>
       </c>
       <c r="CU53" s="7">
-        <v>99.026628534481233</v>
+        <v>189.70727471940432</v>
       </c>
       <c r="CV53" s="7">
-        <v>212</v>
+        <v>162.20365213587718</v>
       </c>
       <c r="CW53" s="7">
-        <v>212</v>
+        <v>189.45620894095509</v>
       </c>
       <c r="CX53" s="7">
-        <v>212</v>
+        <v>170.7578206180182</v>
       </c>
       <c r="CY53" s="7">
-        <v>212</v>
+        <v>160.46035020471277</v>
       </c>
       <c r="CZ53" s="7">
-        <v>212</v>
+        <v>188.18530023208612</v>
       </c>
       <c r="DA53" s="7">
         <v>212</v>
@@ -17282,16 +17282,16 @@
         <v>0</v>
       </c>
       <c r="CC54" s="7">
-        <v>0</v>
+        <v>3.4694567661127991</v>
       </c>
       <c r="CD54" s="7">
-        <v>0</v>
+        <v>90.180663822496726</v>
       </c>
       <c r="CE54" s="7">
-        <v>69.265989025278472</v>
+        <v>172.8651409528257</v>
       </c>
       <c r="CF54" s="8">
-        <v>114.37421831400206</v>
+        <v>94.374218314002064</v>
       </c>
       <c r="CH54">
         <v>5</v>
@@ -18505,16 +18505,16 @@
         <v>317.5450221870542</v>
       </c>
       <c r="BA58" s="7">
-        <v>278.91259108010536</v>
+        <v>355.8271592334213</v>
       </c>
       <c r="BB58" s="7">
-        <v>192.18280439982573</v>
+        <v>272.18280439982573</v>
       </c>
       <c r="BC58" s="7">
-        <v>105.93244963942379</v>
+        <v>185.93244963942379</v>
       </c>
       <c r="BD58" s="8">
-        <v>0.16584168617828254</v>
+        <v>0</v>
       </c>
       <c r="BF58">
         <v>9</v>
@@ -18568,13 +18568,13 @@
         <v>0</v>
       </c>
       <c r="BW58" s="7">
-        <v>30.376038204391989</v>
+        <v>0</v>
       </c>
       <c r="BX58" s="7">
-        <v>92.150870123003187</v>
+        <v>0</v>
       </c>
       <c r="BY58" s="7">
-        <v>602.60656205055329</v>
+        <v>443.36371373968188</v>
       </c>
       <c r="BZ58" s="7">
         <v>650</v>
@@ -18664,7 +18664,7 @@
         <v>24.271444375207011</v>
       </c>
       <c r="DD58" s="7">
-        <v>0</v>
+        <v>15.043031061874444</v>
       </c>
       <c r="DE58" s="7">
         <v>0</v>
@@ -19833,7 +19833,7 @@
         <v>429.76772899999833</v>
       </c>
       <c r="BJ62" s="7">
-        <v>191.51884344046721</v>
+        <v>0</v>
       </c>
       <c r="BK62" s="7">
         <v>0</v>
@@ -20990,31 +20990,31 @@
         <v>257</v>
       </c>
       <c r="J66" s="7">
-        <v>257</v>
+        <v>252.12125910584163</v>
       </c>
       <c r="K66" s="7">
-        <v>257</v>
+        <v>193.56428302157335</v>
       </c>
       <c r="L66" s="7">
-        <v>257</v>
+        <v>128.65241006221004</v>
       </c>
       <c r="M66" s="7">
-        <v>133.37510673259294</v>
+        <v>95.329681752769375</v>
       </c>
       <c r="N66" s="7">
-        <v>64.49616836194491</v>
+        <v>62.33704888854345</v>
       </c>
       <c r="O66" s="7">
-        <v>119.16603550975924</v>
+        <v>29.677482328540009</v>
       </c>
       <c r="P66" s="7">
-        <v>66.855351721637362</v>
+        <v>7.3539796694963115</v>
       </c>
       <c r="Q66" s="7">
-        <v>22.476075808201585</v>
+        <v>0</v>
       </c>
       <c r="R66" s="7">
-        <v>0</v>
+        <v>8.8414168373516304</v>
       </c>
       <c r="S66" s="7">
         <v>0</v>
@@ -21095,22 +21095,22 @@
         <v>257</v>
       </c>
       <c r="AU66" s="7">
-        <v>257</v>
+        <v>244.56127711471697</v>
       </c>
       <c r="AV66" s="7">
-        <v>229.80232860874958</v>
+        <v>209.80232860874935</v>
       </c>
       <c r="AW66" s="7">
-        <v>235.27054956622783</v>
+        <v>215.27054956622783</v>
       </c>
       <c r="AX66" s="7">
-        <v>116.92266150410796</v>
+        <v>96.922661504107964</v>
       </c>
       <c r="AY66" s="7">
-        <v>65.565565457644652</v>
+        <v>85.565565457644652</v>
       </c>
       <c r="AZ66" s="7">
-        <v>14.286255546763641</v>
+        <v>44.286255546763641</v>
       </c>
       <c r="BA66" s="7">
         <v>0</v>
@@ -21194,13 +21194,13 @@
         <v>257</v>
       </c>
       <c r="CC66" s="7">
-        <v>257</v>
+        <v>204.70773844381245</v>
       </c>
       <c r="CD66" s="7">
-        <v>167.61021965795345</v>
+        <v>102.89992614431721</v>
       </c>
       <c r="CE66" s="7">
-        <v>69.212126251235091</v>
+        <v>5.6129743236878795</v>
       </c>
       <c r="CF66" s="8">
         <v>0</v>
@@ -21233,43 +21233,43 @@
         <v>257</v>
       </c>
       <c r="CQ66" s="7">
-        <v>257</v>
+        <v>254.28910331648103</v>
       </c>
       <c r="CR66" s="7">
-        <v>257</v>
+        <v>220.83710524632943</v>
       </c>
       <c r="CS66" s="7">
-        <v>251.42904839567677</v>
+        <v>203.87188622585813</v>
       </c>
       <c r="CT66" s="7">
-        <v>257</v>
+        <v>166.30541613206947</v>
       </c>
       <c r="CU66" s="7">
-        <v>225.4399428017216</v>
+        <v>144.75929661679851</v>
       </c>
       <c r="CV66" s="7">
-        <v>90.34817047822844</v>
+        <v>140.14451834235081</v>
       </c>
       <c r="CW66" s="7">
-        <v>68.570704012532133</v>
+        <v>91.114495071576584</v>
       </c>
       <c r="CX66" s="7">
-        <v>47.137240348644355</v>
+        <v>78.379419730625699</v>
       </c>
       <c r="CY66" s="7">
-        <v>26.050875511782124</v>
+        <v>57.590525307068901</v>
       </c>
       <c r="CZ66" s="7">
-        <v>5.3147333913875627</v>
+        <v>9.1294331593014419</v>
       </c>
       <c r="DA66" s="7">
-        <v>24.931965991909237</v>
+        <v>4.9319659919092373</v>
       </c>
       <c r="DB66" s="7">
-        <v>44.905753685836316</v>
+        <v>24.905753685836316</v>
       </c>
       <c r="DC66" s="7">
-        <v>0.96786109380127527</v>
+        <v>20.967861093801275</v>
       </c>
       <c r="DD66" s="7">
         <v>0</v>
@@ -21301,16 +21301,16 @@
         <v>1924.1698059999994</v>
       </c>
       <c r="E67" s="7">
-        <v>285.91013425399888</v>
+        <v>335.91013425399888</v>
       </c>
       <c r="F67" s="7">
-        <v>260.35772546228463</v>
+        <v>250.4160625222928</v>
       </c>
       <c r="G67" s="7">
-        <v>235.115344991445</v>
+        <v>81.836395007511626</v>
       </c>
       <c r="H67" s="7">
-        <v>205.27534585101057</v>
+        <v>28.185783096367231</v>
       </c>
       <c r="I67" s="7">
         <v>0</v>
@@ -21382,16 +21382,16 @@
         <v>2254.028049999999</v>
       </c>
       <c r="AH67" s="7">
-        <v>539.20226146999914</v>
+        <v>456.73710244999847</v>
       </c>
       <c r="AI67" s="7">
-        <v>496.76803994752481</v>
+        <v>434.18013637204831</v>
       </c>
       <c r="AJ67" s="7">
-        <v>464.33609455963733</v>
+        <v>411.9601575993961</v>
       </c>
       <c r="AK67" s="7">
-        <v>350.08019901779016</v>
+        <v>370.08019901779016</v>
       </c>
       <c r="AL67" s="7">
         <v>328.54332080895028</v>
@@ -21400,16 +21400,16 @@
         <v>287.35261069623039</v>
       </c>
       <c r="AN67" s="7">
-        <v>236.51118419249588</v>
+        <v>256.51118419249588</v>
       </c>
       <c r="AO67" s="7">
-        <v>196.02218485022786</v>
+        <v>226.02218485022786</v>
       </c>
       <c r="AP67" s="7">
-        <v>175.88878451387973</v>
+        <v>195.88878451387973</v>
       </c>
       <c r="AQ67" s="7">
-        <v>148.82851014470225</v>
+        <v>158.82851014470225</v>
       </c>
       <c r="AR67" s="7">
         <v>113.18096673600417</v>
@@ -21418,10 +21418,10 @@
         <v>77.752595436627985</v>
       </c>
       <c r="AT67" s="7">
-        <v>42.545368795557465</v>
+        <v>32.545368795557465</v>
       </c>
       <c r="AU67" s="7">
-        <v>7.5612771147169724</v>
+        <v>0</v>
       </c>
       <c r="AV67" s="7">
         <v>0</v>
@@ -21463,34 +21463,34 @@
         <v>2269.6</v>
       </c>
       <c r="BJ67" s="7">
-        <v>1034.5188814163648</v>
+        <v>1180.2783031365987</v>
       </c>
       <c r="BK67" s="7">
-        <v>1098.0638078648274</v>
+        <v>1148.0638078648274</v>
       </c>
       <c r="BL67" s="7">
-        <v>1066.0993821356105</v>
+        <v>1116.0993821356105</v>
       </c>
       <c r="BM67" s="7">
-        <v>1044.3872765748304</v>
+        <v>1064.3872765748308</v>
       </c>
       <c r="BN67" s="7">
         <v>1012.9297620640039</v>
       </c>
       <c r="BO67" s="7">
-        <v>961.72912992257966</v>
+        <v>961.7291299225792</v>
       </c>
       <c r="BP67" s="7">
-        <v>900.7876920918826</v>
+        <v>920.78769209188226</v>
       </c>
       <c r="BQ67" s="7">
-        <v>850.10778132070902</v>
+        <v>880.10778132070902</v>
       </c>
       <c r="BR67" s="7">
-        <v>819.69175135259525</v>
+        <v>839.69175135259525</v>
       </c>
       <c r="BS67" s="7">
-        <v>789.54197711476809</v>
+        <v>799.54197711476809</v>
       </c>
       <c r="BT67" s="7">
         <v>759.66085490880073</v>
@@ -21499,28 +21499,28 @@
         <v>730.05080260297927</v>
       </c>
       <c r="BV67" s="7">
-        <v>700.71425982640562</v>
+        <v>690.71425982640562</v>
       </c>
       <c r="BW67" s="7">
-        <v>656.46566906264707</v>
+        <v>651.65368816484283</v>
       </c>
       <c r="BX67" s="7">
-        <v>596.7961362968249</v>
+        <v>622.87157135832672</v>
       </c>
       <c r="BY67" s="7">
-        <v>353.06713447527409</v>
+        <v>412.68855863070974</v>
       </c>
       <c r="BZ67" s="7">
-        <v>231.37838783672896</v>
+        <v>306.83537250707531</v>
       </c>
       <c r="CA67" s="7">
-        <v>213.44087678606851</v>
+        <v>120.4232974727411</v>
       </c>
       <c r="CB67" s="7">
-        <v>134.8073822414587</v>
+        <v>52.641482064334582</v>
       </c>
       <c r="CC67" s="7">
-        <v>13.228909963713932</v>
+        <v>0</v>
       </c>
       <c r="CD67" s="7">
         <v>0</v>
@@ -21544,25 +21544,25 @@
         <v>1979.1461799999993</v>
       </c>
       <c r="CL67" s="7">
-        <v>341.38129561999858</v>
+        <v>269.35788138232874</v>
       </c>
       <c r="CM67" s="7">
-        <v>316.32812728057752</v>
+        <v>154.32812728057752</v>
       </c>
       <c r="CN67" s="7">
-        <v>158.02551880112492</v>
+        <v>129.58948042610291</v>
       </c>
       <c r="CO67" s="7">
-        <v>65.168185749937493</v>
+        <v>96.394168858420244</v>
       </c>
       <c r="CP67" s="7">
-        <v>101.15816420958345</v>
+        <v>51.809378620256666</v>
       </c>
       <c r="CQ67" s="7">
-        <v>38.782921760500358</v>
+        <v>0</v>
       </c>
       <c r="CR67" s="7">
-        <v>33.275206957196133</v>
+        <v>0</v>
       </c>
       <c r="CS67" s="7">
         <v>0</v>
@@ -29128,16 +29128,16 @@
         <v>0</v>
       </c>
       <c r="E91" s="7">
-        <v>3200</v>
+        <v>3150</v>
       </c>
       <c r="F91" s="7">
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="G91" s="7">
-        <v>3320</v>
+        <v>3270</v>
       </c>
       <c r="H91" s="7">
-        <v>3370</v>
+        <v>3350</v>
       </c>
       <c r="I91" s="7">
         <v>3430</v>
@@ -29146,16 +29146,16 @@
         <v>3510</v>
       </c>
       <c r="K91" s="7">
-        <v>3600</v>
+        <v>3580</v>
       </c>
       <c r="L91" s="7">
-        <v>3680</v>
+        <v>3650</v>
       </c>
       <c r="M91" s="7">
-        <v>3740</v>
+        <v>3720</v>
       </c>
       <c r="N91" s="7">
-        <v>3800</v>
+        <v>3790</v>
       </c>
       <c r="O91" s="7">
         <v>3860</v>
@@ -29164,19 +29164,19 @@
         <v>3920</v>
       </c>
       <c r="Q91" s="7">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="R91" s="7">
-        <v>4040</v>
+        <v>4060</v>
       </c>
       <c r="S91" s="7">
-        <v>4100</v>
+        <v>4103.4181423200489</v>
       </c>
       <c r="T91" s="7">
-        <v>4120</v>
+        <v>4126.8489056009294</v>
       </c>
       <c r="U91" s="7">
-        <v>4140</v>
+        <v>4150.4905457513369</v>
       </c>
       <c r="V91" s="7">
         <v>4174.3449606630993</v>
@@ -29212,16 +29212,16 @@
         <v>0</v>
       </c>
       <c r="AH91" s="7">
-        <v>3200</v>
+        <v>3150</v>
       </c>
       <c r="AI91" s="7">
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="AJ91" s="7">
-        <v>3320</v>
+        <v>3270</v>
       </c>
       <c r="AK91" s="7">
-        <v>3370</v>
+        <v>3350</v>
       </c>
       <c r="AL91" s="7">
         <v>3430</v>
@@ -29230,16 +29230,16 @@
         <v>3510</v>
       </c>
       <c r="AN91" s="7">
-        <v>3600</v>
+        <v>3580</v>
       </c>
       <c r="AO91" s="7">
-        <v>3680</v>
+        <v>3650</v>
       </c>
       <c r="AP91" s="7">
-        <v>3740</v>
+        <v>3720</v>
       </c>
       <c r="AQ91" s="7">
-        <v>3800</v>
+        <v>3790</v>
       </c>
       <c r="AR91" s="7">
         <v>3860</v>
@@ -29248,37 +29248,37 @@
         <v>3920</v>
       </c>
       <c r="AT91" s="7">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="AU91" s="7">
-        <v>4040</v>
+        <v>4060</v>
       </c>
       <c r="AV91" s="7">
-        <v>4100</v>
+        <v>4120</v>
       </c>
       <c r="AW91" s="7">
-        <v>4120</v>
+        <v>4140</v>
       </c>
       <c r="AX91" s="7">
-        <v>4140</v>
+        <v>4160</v>
       </c>
       <c r="AY91" s="7">
-        <v>4200</v>
+        <v>4180</v>
       </c>
       <c r="AZ91" s="7">
-        <v>4260</v>
+        <v>4230</v>
       </c>
       <c r="BA91" s="7">
-        <v>4320</v>
+        <v>4280</v>
       </c>
       <c r="BB91" s="7">
-        <v>4390</v>
+        <v>4350</v>
       </c>
       <c r="BC91" s="7">
-        <v>4460</v>
+        <v>4420</v>
       </c>
       <c r="BD91" s="8">
-        <v>4540</v>
+        <v>4540.0829208430896</v>
       </c>
       <c r="BF91">
         <v>42</v>
@@ -29293,16 +29293,16 @@
         <v>0</v>
       </c>
       <c r="BJ91" s="7">
-        <v>3200</v>
+        <v>3150</v>
       </c>
       <c r="BK91" s="7">
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="BL91" s="7">
-        <v>3320</v>
+        <v>3270</v>
       </c>
       <c r="BM91" s="7">
-        <v>3370</v>
+        <v>3350</v>
       </c>
       <c r="BN91" s="7">
         <v>3430</v>
@@ -29311,16 +29311,16 @@
         <v>3510</v>
       </c>
       <c r="BP91" s="7">
-        <v>3600</v>
+        <v>3580</v>
       </c>
       <c r="BQ91" s="7">
-        <v>3680</v>
+        <v>3650</v>
       </c>
       <c r="BR91" s="7">
-        <v>3740</v>
+        <v>3720</v>
       </c>
       <c r="BS91" s="7">
-        <v>3800</v>
+        <v>3790</v>
       </c>
       <c r="BT91" s="7">
         <v>3860</v>
@@ -29329,37 +29329,37 @@
         <v>3920</v>
       </c>
       <c r="BV91" s="7">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="BW91" s="7">
-        <v>4040</v>
+        <v>4060</v>
       </c>
       <c r="BX91" s="7">
-        <v>4100</v>
+        <v>4120</v>
       </c>
       <c r="BY91" s="7">
-        <v>4120</v>
+        <v>4140</v>
       </c>
       <c r="BZ91" s="7">
-        <v>4140</v>
+        <v>4160</v>
       </c>
       <c r="CA91" s="7">
-        <v>4200</v>
+        <v>4180</v>
       </c>
       <c r="CB91" s="7">
-        <v>4260</v>
+        <v>4230</v>
       </c>
       <c r="CC91" s="7">
-        <v>4320</v>
+        <v>4280</v>
       </c>
       <c r="CD91" s="7">
-        <v>4390</v>
+        <v>4350</v>
       </c>
       <c r="CE91" s="7">
-        <v>4460</v>
+        <v>4420</v>
       </c>
       <c r="CF91" s="8">
-        <v>4540</v>
+        <v>4560</v>
       </c>
       <c r="CH91">
         <v>42</v>
@@ -29374,16 +29374,16 @@
         <v>0</v>
       </c>
       <c r="CL91" s="7">
-        <v>3200</v>
+        <v>3150</v>
       </c>
       <c r="CM91" s="7">
-        <v>3260</v>
+        <v>3210</v>
       </c>
       <c r="CN91" s="7">
-        <v>3320</v>
+        <v>3270</v>
       </c>
       <c r="CO91" s="7">
-        <v>3370</v>
+        <v>3350</v>
       </c>
       <c r="CP91" s="7">
         <v>3430</v>
@@ -29392,16 +29392,16 @@
         <v>3510</v>
       </c>
       <c r="CR91" s="7">
-        <v>3600</v>
+        <v>3580</v>
       </c>
       <c r="CS91" s="7">
-        <v>3680</v>
+        <v>3650</v>
       </c>
       <c r="CT91" s="7">
-        <v>3740</v>
+        <v>3720</v>
       </c>
       <c r="CU91" s="7">
-        <v>3800</v>
+        <v>3790</v>
       </c>
       <c r="CV91" s="7">
         <v>3860</v>
@@ -29410,25 +29410,25 @@
         <v>3920</v>
       </c>
       <c r="CX91" s="7">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="CY91" s="7">
-        <v>4040</v>
+        <v>4060</v>
       </c>
       <c r="CZ91" s="7">
-        <v>4100</v>
+        <v>4120</v>
       </c>
       <c r="DA91" s="7">
-        <v>4120</v>
+        <v>4140</v>
       </c>
       <c r="DB91" s="7">
-        <v>4140</v>
+        <v>4160</v>
       </c>
       <c r="DC91" s="7">
-        <v>4200</v>
+        <v>4180</v>
       </c>
       <c r="DD91" s="7">
-        <v>4237.521515530937</v>
+        <v>4230</v>
       </c>
       <c r="DE91" s="7">
         <v>4262.1592091707153</v>
@@ -30134,22 +30134,22 @@
         <v>600.88333333333344</v>
       </c>
       <c r="C97" s="4">
-        <v>110.84916416462795</v>
+        <v>107.24687986542995</v>
       </c>
       <c r="D97" s="4">
-        <v>184.73880443333331</v>
+        <v>176.4054711</v>
       </c>
       <c r="E97" s="4">
-        <v>210.83667889256699</v>
+        <v>194.17001222590034</v>
       </c>
       <c r="F97" s="4">
-        <v>222.42755900260028</v>
+        <v>205.76089233593362</v>
       </c>
       <c r="G97" s="4">
-        <v>233.94275703362374</v>
+        <v>217.27609036695708</v>
       </c>
       <c r="H97" s="4">
-        <v>242.04825851359311</v>
+        <v>235.38159184692645</v>
       </c>
       <c r="I97" s="4">
         <v>253.41004284021557</v>
@@ -30158,16 +30158,16 @@
         <v>271.36074989244418</v>
       </c>
       <c r="K97" s="4">
-        <v>292.56634664147634</v>
+        <v>285.89967997480971</v>
       </c>
       <c r="L97" s="4">
-        <v>310.35946042791625</v>
+        <v>300.35946042791625</v>
       </c>
       <c r="M97" s="4">
-        <v>321.40604557176738</v>
+        <v>314.73937890510075</v>
       </c>
       <c r="N97" s="4">
-        <v>332.37204998191373</v>
+        <v>329.03871664858036</v>
       </c>
       <c r="O97" s="4">
         <v>343.25674843175108</v>
@@ -30176,10 +30176,10 @@
         <v>354.05940916763677</v>
       </c>
       <c r="Q97" s="4">
-        <v>364.77929385014568</v>
+        <v>368.11262718347899</v>
       </c>
       <c r="R97" s="4">
-        <v>375.41565749479679</v>
+        <v>375.78776288101335</v>
       </c>
       <c r="S97" s="4">
         <v>369.24690274694251</v>
@@ -30215,22 +30215,22 @@
         <v>778.53333333333308</v>
       </c>
       <c r="AF97" s="4">
-        <v>-142.01008333333351</v>
+        <v>-153.6767500000002</v>
       </c>
       <c r="AG97" s="4">
-        <v>84.904862583332999</v>
+        <v>73.238195916666342</v>
       </c>
       <c r="AH97" s="4">
-        <v>116.04645345158374</v>
+        <v>99.379786784917087</v>
       </c>
       <c r="AI97" s="4">
-        <v>126.50156153264811</v>
+        <v>109.83489486598137</v>
       </c>
       <c r="AJ97" s="4">
-        <v>136.87076558644176</v>
+        <v>120.20409891977511</v>
       </c>
       <c r="AK97" s="4">
-        <v>143.81995914338646</v>
+        <v>137.1532924767198</v>
       </c>
       <c r="AL97" s="4">
         <v>154.01502877567705</v>
@@ -30239,16 +30239,16 @@
         <v>170.78852070132513</v>
       </c>
       <c r="AN97" s="4">
-        <v>190.80630738763716</v>
+        <v>184.13964072097048</v>
       </c>
       <c r="AO97" s="4">
-        <v>207.40092082079246</v>
+        <v>197.40092082079246</v>
       </c>
       <c r="AP97" s="4">
-        <v>217.23821910817975</v>
+        <v>210.57155244151309</v>
       </c>
       <c r="AQ97" s="4">
-        <v>226.98405308015327</v>
+        <v>223.65071974681996</v>
       </c>
       <c r="AR97" s="4">
         <v>236.63759955787478</v>
@@ -30257,31 +30257,31 @@
         <v>246.19802795389569</v>
       </c>
       <c r="AT97" s="4">
-        <v>159.95116687214809</v>
+        <v>163.28450020548144</v>
       </c>
       <c r="AU97" s="4">
-        <v>265.03617070733031</v>
+        <v>271.70283737399694</v>
       </c>
       <c r="AV97" s="4">
-        <v>274.31218624369649</v>
+        <v>280.97885291036312</v>
       </c>
       <c r="AW97" s="4">
-        <v>270.15835258655653</v>
+        <v>276.82501925322322</v>
       </c>
       <c r="AX97" s="4">
-        <v>265.90713442650224</v>
+        <v>272.57380109316892</v>
       </c>
       <c r="AY97" s="4">
-        <v>274.89098863634092</v>
+        <v>268.22432196967429</v>
       </c>
       <c r="AZ97" s="4">
-        <v>280.85240598512428</v>
+        <v>273.77569753406806</v>
       </c>
       <c r="BA97" s="4">
         <v>273.08794763899027</v>
       </c>
       <c r="BB97" s="4">
-        <v>98.004970647312419</v>
+        <v>86.338303980645748</v>
       </c>
       <c r="BC97" s="4">
         <v>257.34876165025116</v>
@@ -30296,79 +30296,79 @@
         <v>630.89</v>
       </c>
       <c r="BH97" s="4">
-        <v>-254.69063333333327</v>
+        <v>-271.3572999999999</v>
       </c>
       <c r="BI97" s="4">
-        <v>-26.494812366666999</v>
+        <v>-43.161479033333663</v>
       </c>
       <c r="BJ97" s="4">
-        <v>-95.975362344633737</v>
+        <v>-112.64202901130041</v>
       </c>
       <c r="BK97" s="4">
-        <v>-90.456829479264798</v>
+        <v>-107.12349614593145</v>
       </c>
       <c r="BL97" s="4">
-        <v>-85.379290944578003</v>
+        <v>-102.04595761124467</v>
       </c>
       <c r="BM97" s="4">
-        <v>-76.742721229746167</v>
+        <v>-103.40938789641282</v>
       </c>
       <c r="BN97" s="4">
-        <v>-71.211755720814224</v>
+        <v>-104.54508905414755</v>
       </c>
       <c r="BO97" s="4">
-        <v>-72.117678188968284</v>
+        <v>-105.45101152230161</v>
       </c>
       <c r="BP97" s="4">
-        <v>-76.125087292669377</v>
+        <v>-101.30008435982768</v>
       </c>
       <c r="BQ97" s="4">
-        <v>-76.565229744970566</v>
+        <v>-89.10266715982894</v>
       </c>
       <c r="BR97" s="4">
-        <v>-70.102666812676034</v>
+        <v>-78.510567830933724</v>
       </c>
       <c r="BS97" s="4">
-        <v>-63.401940813989917</v>
+        <v>-68.033139608078571</v>
       </c>
       <c r="BT97" s="4">
-        <v>-56.460908281315895</v>
+        <v>-73.732828072933586</v>
       </c>
       <c r="BU97" s="4">
-        <v>-49.277406455847611</v>
+        <v>-50.759767261998832</v>
       </c>
       <c r="BV97" s="4">
-        <v>-41.849253113951818</v>
+        <v>-54.842581834023193</v>
       </c>
       <c r="BW97" s="4">
-        <v>-34.174246391977249</v>
+        <v>-30.624251737195966</v>
       </c>
       <c r="BX97" s="4">
-        <v>-26.250164609505948</v>
+        <v>-24.06918000283061</v>
       </c>
       <c r="BY97" s="4">
-        <v>-4.7414327576576998</v>
+        <v>-30.968445956189193</v>
       </c>
       <c r="BZ97" s="4">
-        <v>17.020877680856074</v>
+        <v>-22.979122319143773</v>
       </c>
       <c r="CA97" s="4">
-        <v>25.705715579983309</v>
+        <v>-0.96095108668320484</v>
       </c>
       <c r="CB97" s="4">
-        <v>34.648717020202938</v>
+        <v>11.31538368686976</v>
       </c>
       <c r="CC97" s="4">
-        <v>43.852205473384473</v>
+        <v>23.852205473384476</v>
       </c>
       <c r="CD97" s="4">
-        <v>49.985191989311033</v>
+        <v>29.985191989311033</v>
       </c>
       <c r="CE97" s="4">
-        <v>56.383375383881685</v>
+        <v>36.383375383881685</v>
       </c>
       <c r="CF97" s="5">
-        <v>59.715809095668945</v>
+        <v>19.715809095668948</v>
       </c>
       <c r="CH97" s="1" t="s">
         <v>1</v>
@@ -30377,22 +30377,22 @@
         <v>622.48666666666668</v>
       </c>
       <c r="CJ97" s="4">
-        <v>32.063616666666611</v>
+        <v>20.396949999999947</v>
       </c>
       <c r="CK97" s="4">
-        <v>36.681759216666592</v>
+        <v>25.015092549999924</v>
       </c>
       <c r="CL97" s="4">
-        <v>206.40966014595034</v>
+        <v>189.74299347928368</v>
       </c>
       <c r="CM97" s="4">
-        <v>217.6780370872641</v>
+        <v>201.01137042059742</v>
       </c>
       <c r="CN97" s="4">
-        <v>228.86782942104946</v>
+        <v>212.20116275438278</v>
       </c>
       <c r="CO97" s="4">
-        <v>236.64499655250575</v>
+        <v>229.97832988583906</v>
       </c>
       <c r="CP97" s="4">
         <v>247.67549152147831</v>
@@ -30401,16 +30401,16 @@
         <v>265.29192761183833</v>
       </c>
       <c r="CR97" s="4">
-        <v>286.16024496034504</v>
+        <v>279.49357829367841</v>
       </c>
       <c r="CS97" s="4">
-        <v>303.61304383165481</v>
+        <v>293.61304383165486</v>
       </c>
       <c r="CT97" s="4">
-        <v>314.31625122613968</v>
+        <v>307.649584559473</v>
       </c>
       <c r="CU97" s="4">
-        <v>324.93578748717511</v>
+        <v>321.60245415384179</v>
       </c>
       <c r="CV97" s="4">
         <v>335.47089957455984</v>
@@ -30419,16 +30419,16 @@
         <v>345.920827670731</v>
       </c>
       <c r="CX97" s="4">
-        <v>356.2848051197675</v>
+        <v>359.61813845310081</v>
       </c>
       <c r="CY97" s="4">
-        <v>366.5620583658457</v>
+        <v>373.22872503251239</v>
       </c>
       <c r="CZ97" s="4">
-        <v>376.75180689113841</v>
+        <v>382.14355861694207</v>
       </c>
       <c r="DA97" s="4">
-        <v>373.51992981982522</v>
+        <v>375.29072064449451</v>
       </c>
       <c r="DB97" s="4">
         <v>368.37620713029514</v>
@@ -30460,22 +30460,22 @@
         <v>-766.71666666666681</v>
       </c>
       <c r="C98" s="7">
-        <v>-0.6418358353718645</v>
+        <v>20.755879865430188</v>
       </c>
       <c r="D98" s="7">
-        <v>54.186785433333654</v>
+        <v>70.853452100000311</v>
       </c>
       <c r="E98" s="7">
-        <v>-965.97873393643385</v>
+        <v>-932.64540060310048</v>
       </c>
       <c r="F98" s="7">
-        <v>-994.98219254186176</v>
+        <v>-961.64885920852851</v>
       </c>
       <c r="G98" s="7">
-        <v>-1023.8866822747389</v>
+        <v>-990.55334894140549</v>
       </c>
       <c r="H98" s="7">
-        <v>-1046.0246457485446</v>
+        <v>-1032.6913124152115</v>
       </c>
       <c r="I98" s="7">
         <v>-1074.7285175602817</v>
@@ -30484,16 +30484,16 @@
         <v>-1116.6640575516578</v>
       </c>
       <c r="K98" s="7">
-        <v>-1165.1636840696228</v>
+        <v>-1151.8303507362893</v>
       </c>
       <c r="L98" s="7">
-        <v>-1206.8931405595827</v>
+        <v>-1186.8931405595827</v>
       </c>
       <c r="M98" s="7">
-        <v>-1235.1848288246188</v>
+        <v>-1221.8514954912855</v>
       </c>
       <c r="N98" s="7">
-        <v>-1263.3711422840411</v>
+        <v>-1256.7044756173743</v>
       </c>
       <c r="O98" s="7">
         <v>-1291.4511325645976</v>
@@ -30502,10 +30502,10 @@
         <v>-1319.4238427576788</v>
       </c>
       <c r="Q98" s="7">
-        <v>-1347.2883073424982</v>
+        <v>-1353.9549740091647</v>
       </c>
       <c r="R98" s="7">
-        <v>-1375.0435521085808</v>
+        <v>-1375.7877628810134</v>
       </c>
       <c r="S98" s="7">
         <v>-1369.2469027469424</v>
@@ -30541,22 +30541,22 @@
         <v>-840.00666666666643</v>
       </c>
       <c r="AF98" s="7">
-        <v>3.0074166666672397</v>
+        <v>26.340750000000583</v>
       </c>
       <c r="AG98" s="7">
-        <v>208.2868800833341</v>
+        <v>231.62021341666747</v>
       </c>
       <c r="AH98" s="7">
-        <v>-822.74536220591733</v>
+        <v>-789.41202887258396</v>
       </c>
       <c r="AI98" s="7">
-        <v>-850.26358046577047</v>
+        <v>-816.93024713243722</v>
       </c>
       <c r="AJ98" s="7">
-        <v>-877.66946268996219</v>
+        <v>-844.33612935662882</v>
       </c>
       <c r="AK98" s="7">
-        <v>-898.29533118750544</v>
+        <v>-884.96199785417207</v>
       </c>
       <c r="AL98" s="7">
         <v>-925.47349916819314</v>
@@ -30565,16 +30565,16 @@
         <v>-965.8696039940404</v>
       </c>
       <c r="AN98" s="7">
-        <v>-1012.815940429987</v>
+        <v>-999.48260709665362</v>
       </c>
       <c r="AO98" s="7">
-        <v>-1052.9781272271903</v>
+        <v>-1032.9781272271903</v>
       </c>
       <c r="AP98" s="7">
-        <v>-1079.6884403722347</v>
+        <v>-1066.3551070389017</v>
       </c>
       <c r="AQ98" s="7">
-        <v>-1106.2791463355852</v>
+        <v>-1099.6124796689185</v>
       </c>
       <c r="AR98" s="7">
         <v>-1132.7491686526055</v>
@@ -30583,31 +30583,31 @@
         <v>-1159.097421170479</v>
       </c>
       <c r="AT98" s="7">
-        <v>-1137.4661412943472</v>
+        <v>-1144.1328079610139</v>
       </c>
       <c r="AU98" s="7">
-        <v>-1211.4242232326628</v>
+        <v>-1224.7575565659961</v>
       </c>
       <c r="AV98" s="7">
-        <v>-1237.4005512417571</v>
+        <v>-1250.7338845750903</v>
       </c>
       <c r="AW98" s="7">
-        <v>-1236.5839995362662</v>
+        <v>-1249.9173328695997</v>
       </c>
       <c r="AX98" s="7">
-        <v>-1235.6400988654259</v>
+        <v>-1248.9734321987594</v>
       </c>
       <c r="AY98" s="7">
-        <v>-1261.2343697552151</v>
+        <v>-1247.9010364218818</v>
       </c>
       <c r="AZ98" s="7">
-        <v>-1280.8524059851243</v>
+        <v>-1266.6989890830123</v>
       </c>
       <c r="BA98" s="7">
         <v>-1273.0879476389903</v>
       </c>
       <c r="BB98" s="7">
-        <v>-930.75633212688319</v>
+        <v>-907.42299879354994</v>
       </c>
       <c r="BC98" s="7">
         <v>-1257.3487616502512</v>
@@ -30622,79 +30622,79 @@
         <v>-588.1099999999999</v>
       </c>
       <c r="BH98" s="7">
-        <v>45.386366666666675</v>
+        <v>78.719699999999989</v>
       </c>
       <c r="BI98" s="7">
-        <v>246.45724063333421</v>
+        <v>279.79057396666752</v>
       </c>
       <c r="BJ98" s="7">
-        <v>-500.39238086763214</v>
+        <v>-467.05904753429888</v>
       </c>
       <c r="BK98" s="7">
-        <v>-522.48924116897069</v>
+        <v>-489.15590783563738</v>
       </c>
       <c r="BL98" s="7">
-        <v>-545.2756343394916</v>
+        <v>-511.94230100615835</v>
       </c>
       <c r="BM98" s="7">
-        <v>-564.75377171521359</v>
+        <v>-541.42043838188022</v>
       </c>
       <c r="BN98" s="7">
-        <v>-587.59054566065049</v>
+        <v>-570.92387899398375</v>
       </c>
       <c r="BO98" s="7">
-        <v>-617.11951723826292</v>
+        <v>-600.45285057159629</v>
       </c>
       <c r="BP98" s="7">
-        <v>-650.00758289340729</v>
+        <v>-625.18257996056559</v>
       </c>
       <c r="BQ98" s="7">
-        <v>-679.58830780611447</v>
+        <v>-658.31958909868524</v>
       </c>
       <c r="BR98" s="7">
-        <v>-702.52859257636942</v>
+        <v>-688.32464206724057</v>
       </c>
       <c r="BS98" s="7">
-        <v>-725.49533990955695</v>
+        <v>-718.17974051251269</v>
       </c>
       <c r="BT98" s="7">
-        <v>-748.48878796874294</v>
+        <v>-715.76070776036056</v>
       </c>
       <c r="BU98" s="7">
-        <v>-771.50917706046164</v>
+        <v>-770.76799665738599</v>
       </c>
       <c r="BV98" s="7">
-        <v>-794.55674965400544</v>
+        <v>-771.74508529396974</v>
       </c>
       <c r="BW98" s="7">
-        <v>-817.63175040089163</v>
+        <v>-829.40674772828231</v>
       </c>
       <c r="BX98" s="7">
-        <v>-840.73442615449937</v>
+        <v>-851.82491845783704</v>
       </c>
       <c r="BY98" s="7">
-        <v>-850.53169265655686</v>
+        <v>-847.41818605729111</v>
       </c>
       <c r="BZ98" s="7">
-        <v>-860.35713455713221</v>
+        <v>-850.35713455713233</v>
       </c>
       <c r="CA98" s="7">
-        <v>-883.5443387681463</v>
+        <v>-860.21100543481305</v>
       </c>
       <c r="CB98" s="7">
-        <v>-906.76022781705967</v>
+        <v>-880.09356115039316</v>
       </c>
       <c r="CC98" s="7">
-        <v>-930.00505986741325</v>
+        <v>-900.00505986741325</v>
       </c>
       <c r="CD98" s="7">
-        <v>-956.61242873955302</v>
+        <v>-926.61242873955302</v>
       </c>
       <c r="CE98" s="7">
-        <v>-983.2492639315426</v>
+        <v>-953.2492639315426</v>
       </c>
       <c r="CF98" s="8">
-        <v>-1013.2491639735928</v>
+        <v>-1003.2491639735928</v>
       </c>
       <c r="CH98" t="s">
         <v>2</v>
@@ -30703,22 +30703,22 @@
         <v>-793.05333333333328</v>
       </c>
       <c r="CJ98" s="7">
-        <v>381.90811666666684</v>
+        <v>405.24145000000016</v>
       </c>
       <c r="CK98" s="7">
-        <v>366.73421971666704</v>
+        <v>390.06755305000036</v>
       </c>
       <c r="CL98" s="7">
-        <v>-940.91263249855035</v>
+        <v>-907.57929916521709</v>
       </c>
       <c r="CM98" s="7">
-        <v>-969.49435619103747</v>
+        <v>-936.1610228577041</v>
       </c>
       <c r="CN98" s="7">
-        <v>-997.97331539675702</v>
+        <v>-964.63998206342364</v>
       </c>
       <c r="CO98" s="7">
-        <v>-1019.6819185686613</v>
+        <v>-1006.348585235328</v>
       </c>
       <c r="CP98" s="7">
         <v>-1047.9525658357793</v>
@@ -30727,16 +30727,16 @@
         <v>-1089.4509822616346</v>
       </c>
       <c r="CR98" s="7">
-        <v>-1137.5095511019895</v>
+        <v>-1124.1762177686562</v>
       </c>
       <c r="CS98" s="7">
-        <v>-1178.7939803952409</v>
+        <v>-1158.7939803952409</v>
       </c>
       <c r="CT98" s="7">
-        <v>-1206.636636218798</v>
+        <v>-1193.3033028854647</v>
       </c>
       <c r="CU98" s="7">
-        <v>-1234.3698759447675</v>
+        <v>-1227.7032092781008</v>
       </c>
       <c r="CV98" s="7">
         <v>-1261.9927148282704</v>
@@ -30745,16 +30745,16 @@
         <v>-1289.5041592617251</v>
       </c>
       <c r="CX98" s="7">
-        <v>-1316.9032066950808</v>
+        <v>-1323.5698733617476</v>
       </c>
       <c r="CY98" s="7">
-        <v>-1344.1888455553367</v>
+        <v>-1357.5221788886702</v>
       </c>
       <c r="CZ98" s="7">
-        <v>-1371.3600551653349</v>
+        <v>-1382.1435586169421</v>
       </c>
       <c r="DA98" s="7">
-        <v>-1371.7491389951563</v>
+        <v>-1375.2907206444945</v>
       </c>
       <c r="DB98" s="7">
         <v>-1368.3762071302951</v>
@@ -30786,22 +30786,22 @@
         <v>165.83333333333337</v>
       </c>
       <c r="C99" s="10">
-        <v>-110.20732832925631</v>
+        <v>-128.00275973086036</v>
       </c>
       <c r="D99" s="10">
-        <v>-238.92558986666697</v>
+        <v>-247.25892320000031</v>
       </c>
       <c r="E99" s="10">
-        <v>755.14205504386678</v>
+        <v>738.47538837720015</v>
       </c>
       <c r="F99" s="10">
-        <v>772.55463353926177</v>
+        <v>755.88796687259503</v>
       </c>
       <c r="G99" s="10">
-        <v>789.94392524111504</v>
+        <v>773.27725857444841</v>
       </c>
       <c r="H99" s="10">
-        <v>803.97638723495186</v>
+        <v>797.30972056828512</v>
       </c>
       <c r="I99" s="10">
         <v>821.31847472006643</v>
@@ -30810,16 +30810,16 @@
         <v>845.30330765921371</v>
       </c>
       <c r="K99" s="10">
-        <v>872.5973374281466</v>
+        <v>865.93067076147997</v>
       </c>
       <c r="L99" s="10">
-        <v>896.53368013166653</v>
+        <v>886.53368013166653</v>
       </c>
       <c r="M99" s="10">
-        <v>913.77878325285133</v>
+        <v>907.11211658618481</v>
       </c>
       <c r="N99" s="10">
-        <v>930.99909230212734</v>
+        <v>927.66575896879408</v>
       </c>
       <c r="O99" s="10">
         <v>948.19438413284661</v>
@@ -30828,10 +30828,10 @@
         <v>965.36443359004215</v>
       </c>
       <c r="Q99" s="10">
-        <v>982.50901349235255</v>
+        <v>985.84234682568592</v>
       </c>
       <c r="R99" s="10">
-        <v>999.62789461378384</v>
+        <v>1000</v>
       </c>
       <c r="S99" s="10">
         <v>1000</v>
@@ -30867,22 +30867,22 @@
         <v>61.473333333333471</v>
       </c>
       <c r="AF99" s="10">
-        <v>139.00266666666627</v>
+        <v>127.33599999999961</v>
       </c>
       <c r="AG99" s="10">
-        <v>-293.19174266666715</v>
+        <v>-304.85840933333378</v>
       </c>
       <c r="AH99" s="10">
-        <v>706.6989087543335</v>
+        <v>690.03224208766687</v>
       </c>
       <c r="AI99" s="10">
-        <v>723.76201893312259</v>
+        <v>707.09535226645585</v>
       </c>
       <c r="AJ99" s="10">
-        <v>740.79869710352057</v>
+        <v>724.13203043685394</v>
       </c>
       <c r="AK99" s="10">
-        <v>754.4753720441189</v>
+        <v>747.80870537745227</v>
       </c>
       <c r="AL99" s="10">
         <v>771.45847039251601</v>
@@ -30891,16 +30891,16 @@
         <v>795.08108329271556</v>
       </c>
       <c r="AN99" s="10">
-        <v>822.00963304235006</v>
+        <v>815.34296637568343</v>
       </c>
       <c r="AO99" s="10">
-        <v>845.57720640639775</v>
+        <v>835.57720640639775</v>
       </c>
       <c r="AP99" s="10">
-        <v>862.45022126405536</v>
+        <v>855.78355459738862</v>
       </c>
       <c r="AQ99" s="10">
-        <v>879.29509325543188</v>
+        <v>875.96175992209851</v>
       </c>
       <c r="AR99" s="10">
         <v>896.11156909473073</v>
@@ -30909,31 +30909,31 @@
         <v>912.89939321658335</v>
       </c>
       <c r="AT99" s="10">
-        <v>977.5149744221992</v>
+        <v>980.84830775553246</v>
       </c>
       <c r="AU99" s="10">
-        <v>946.38805252533234</v>
+        <v>953.05471919199908</v>
       </c>
       <c r="AV99" s="10">
-        <v>963.08836499806057</v>
+        <v>969.75503166472731</v>
       </c>
       <c r="AW99" s="10">
-        <v>966.42564694970986</v>
+        <v>973.09231361637649</v>
       </c>
       <c r="AX99" s="10">
-        <v>969.73296443892377</v>
+        <v>976.3996311055904</v>
       </c>
       <c r="AY99" s="10">
-        <v>986.34338111887428</v>
+        <v>979.67671445220753</v>
       </c>
       <c r="AZ99" s="10">
-        <v>1000</v>
+        <v>992.92329154894423</v>
       </c>
       <c r="BA99" s="10">
         <v>1000</v>
       </c>
       <c r="BB99" s="10">
-        <v>832.75136147957107</v>
+        <v>821.08469481290433</v>
       </c>
       <c r="BC99" s="10">
         <v>1000</v>
@@ -30948,79 +30948,79 @@
         <v>-42.78000000000003</v>
       </c>
       <c r="BH99" s="10">
-        <v>209.30426666666659</v>
+        <v>192.63759999999991</v>
       </c>
       <c r="BI99" s="10">
-        <v>-219.96242826666719</v>
+        <v>-236.62909493333387</v>
       </c>
       <c r="BJ99" s="10">
-        <v>596.36774321226596</v>
+        <v>579.70107654559922</v>
       </c>
       <c r="BK99" s="10">
-        <v>612.94607064823549</v>
+        <v>596.27940398156875</v>
       </c>
       <c r="BL99" s="10">
-        <v>630.65492528406969</v>
+        <v>613.98825861740295</v>
       </c>
       <c r="BM99" s="10">
-        <v>641.49649294495975</v>
+        <v>644.82982627829313</v>
       </c>
       <c r="BN99" s="10">
-        <v>658.80230138146464</v>
+        <v>675.46896804813139</v>
       </c>
       <c r="BO99" s="10">
-        <v>689.23719542723143</v>
+        <v>705.90386209389806</v>
       </c>
       <c r="BP99" s="10">
-        <v>726.13267018607667</v>
+        <v>726.4826643203935</v>
       </c>
       <c r="BQ99" s="10">
-        <v>756.15353755108504</v>
+        <v>747.42225625851427</v>
       </c>
       <c r="BR99" s="10">
-        <v>772.63125938904545</v>
+        <v>766.8352098981743</v>
       </c>
       <c r="BS99" s="10">
-        <v>788.89728072354694</v>
+        <v>786.21288012059119</v>
       </c>
       <c r="BT99" s="10">
-        <v>804.94969625005899</v>
+        <v>789.49353583329423</v>
       </c>
       <c r="BU99" s="10">
-        <v>820.78658351630941</v>
+        <v>821.52776391938505</v>
       </c>
       <c r="BV99" s="10">
-        <v>836.40600276795726</v>
+        <v>826.58766712799286</v>
       </c>
       <c r="BW99" s="10">
-        <v>851.80599679286888</v>
+        <v>860.0309994654782</v>
       </c>
       <c r="BX99" s="10">
-        <v>866.98459076400525</v>
+        <v>875.89409846066758</v>
       </c>
       <c r="BY99" s="10">
-        <v>855.27312541421463</v>
+        <v>878.38663201348038</v>
       </c>
       <c r="BZ99" s="10">
-        <v>843.33625687627637</v>
+        <v>873.33625687627625</v>
       </c>
       <c r="CA99" s="10">
-        <v>857.83862318816307</v>
+        <v>861.17195652149633</v>
       </c>
       <c r="CB99" s="10">
-        <v>872.11151079685681</v>
+        <v>868.77817746352332</v>
       </c>
       <c r="CC99" s="10">
-        <v>886.15285439402908</v>
+        <v>876.15285439402908</v>
       </c>
       <c r="CD99" s="10">
-        <v>906.62723675024222</v>
+        <v>896.62723675024222</v>
       </c>
       <c r="CE99" s="10">
-        <v>926.86588854766092</v>
+        <v>916.86588854766092</v>
       </c>
       <c r="CF99" s="11">
-        <v>953.5333548779239</v>
+        <v>983.5333548779239</v>
       </c>
       <c r="CH99" t="s">
         <v>3</v>
@@ -31029,22 +31029,22 @@
         <v>170.56666666666661</v>
       </c>
       <c r="CJ99" s="10">
-        <v>-413.97173333333342</v>
+        <v>-425.6384000000001</v>
       </c>
       <c r="CK99" s="10">
-        <v>-403.41597893333363</v>
+        <v>-415.08264560000032</v>
       </c>
       <c r="CL99" s="10">
-        <v>734.50297235260007</v>
+        <v>717.83630568593333</v>
       </c>
       <c r="CM99" s="10">
-        <v>751.81631910377359</v>
+        <v>735.14965243710697</v>
       </c>
       <c r="CN99" s="10">
-        <v>769.10548597570755</v>
+        <v>752.43881930904092</v>
       </c>
       <c r="CO99" s="10">
-        <v>783.03692201615559</v>
+        <v>776.37025534948896</v>
       </c>
       <c r="CP99" s="10">
         <v>800.27707431430099</v>
@@ -31053,16 +31053,16 @@
         <v>824.15905464979642</v>
       </c>
       <c r="CR99" s="10">
-        <v>851.34930614164477</v>
+        <v>844.68263947497803</v>
       </c>
       <c r="CS99" s="10">
-        <v>875.18093656358622</v>
+        <v>865.18093656358633</v>
       </c>
       <c r="CT99" s="10">
-        <v>892.32038499265832</v>
+        <v>885.65371832599169</v>
       </c>
       <c r="CU99" s="10">
-        <v>909.43408845759234</v>
+        <v>906.10075512425897</v>
       </c>
       <c r="CV99" s="10">
         <v>926.52181525371077</v>
@@ -31071,16 +31071,16 @@
         <v>943.58333159099425</v>
       </c>
       <c r="CX99" s="10">
-        <v>960.61840157531333</v>
+        <v>963.95173490864659</v>
       </c>
       <c r="CY99" s="10">
-        <v>977.6267871894911</v>
+        <v>984.29345385615773</v>
       </c>
       <c r="CZ99" s="10">
-        <v>994.6082482741964</v>
+        <v>1000</v>
       </c>
       <c r="DA99" s="10">
-        <v>998.22920917533088</v>
+        <v>1000</v>
       </c>
       <c r="DB99" s="10">
         <v>1000</v>
@@ -31149,52 +31149,52 @@
         <v>474.74284899630015</v>
       </c>
       <c r="F103" s="4">
-        <v>478.76173463726678</v>
+        <v>498.74228895059724</v>
       </c>
       <c r="G103" s="4">
-        <v>482.81679024900205</v>
+        <v>550.57644024364652</v>
       </c>
       <c r="H103" s="4">
-        <v>491.87848710969507</v>
+        <v>557.57500802790958</v>
       </c>
       <c r="I103" s="4">
         <v>556.22733481490559</v>
       </c>
       <c r="J103" s="4">
-        <v>545.62771416157284</v>
+        <v>547.25396112629232</v>
       </c>
       <c r="K103" s="4">
-        <v>531.83936358902656</v>
+        <v>559.65126924850222</v>
       </c>
       <c r="L103" s="4">
-        <v>521.53025119466088</v>
+        <v>574.31278117392435</v>
       </c>
       <c r="M103" s="4">
-        <v>559.24332121121552</v>
+        <v>578.59179620448981</v>
       </c>
       <c r="N103" s="4">
-        <v>578.856282545863</v>
+        <v>582.90932237033007</v>
       </c>
       <c r="O103" s="4">
-        <v>557.43618854458987</v>
+        <v>587.26570627166291</v>
       </c>
       <c r="P103" s="4">
-        <v>571.8275069440607</v>
+        <v>591.66129762810806</v>
       </c>
       <c r="Q103" s="4">
-        <v>583.72761253286717</v>
+        <v>587.88630446893433</v>
       </c>
       <c r="R103" s="4">
-        <v>588.48061454248761</v>
+        <v>578.86680893003711</v>
       </c>
       <c r="S103" s="4">
-        <v>585.89694007336993</v>
+        <v>584.75755930002038</v>
       </c>
       <c r="T103" s="4">
-        <v>596.8033458673633</v>
+        <v>594.52037733372049</v>
       </c>
       <c r="U103" s="4">
-        <v>607.86790931350299</v>
+        <v>604.37106072972392</v>
       </c>
       <c r="V103" s="4">
         <v>614.31040027629138</v>
@@ -31227,13 +31227,13 @@
         <v>585.10993916666666</v>
       </c>
       <c r="AH103" s="4">
-        <v>540.0842756124996</v>
+        <v>584.23932861916637</v>
       </c>
       <c r="AI103" s="4">
-        <v>551.07838138491343</v>
+        <v>588.60768257673885</v>
       </c>
       <c r="AJ103" s="4">
-        <v>558.890039399849</v>
+        <v>593.01535171992941</v>
       </c>
       <c r="AK103" s="4">
         <v>597.46268988540885</v>
@@ -31248,7 +31248,7 @@
         <v>611.04630482245784</v>
       </c>
       <c r="AO103" s="4">
-        <v>615.65592156586001</v>
+        <v>615.6559215658599</v>
       </c>
       <c r="AP103" s="4">
         <v>620.30702485995278</v>
@@ -31269,7 +31269,7 @@
         <v>668.56719879779905</v>
       </c>
       <c r="AV103" s="4">
-        <v>679.0843035869791</v>
+        <v>679.08430358697933</v>
       </c>
       <c r="AW103" s="4">
         <v>689.69606231926173</v>
@@ -31284,16 +31284,16 @@
         <v>563.33530833992734</v>
       </c>
       <c r="BA103" s="4">
-        <v>593.65049426830274</v>
+        <v>555.7074488327587</v>
       </c>
       <c r="BB103" s="4">
-        <v>648.11334871671761</v>
+        <v>608.11334871671761</v>
       </c>
       <c r="BC103" s="4">
-        <v>702.43636885516821</v>
+        <v>662.43636885516821</v>
       </c>
       <c r="BD103" s="5">
-        <v>766.61829617486478</v>
+        <v>766.70121701795392</v>
       </c>
       <c r="BF103" s="1" t="s">
         <v>1</v>
@@ -31308,7 +31308,7 @@
         <v>710.42699205000031</v>
       </c>
       <c r="BJ103" s="4">
-        <v>690.60653792001585</v>
+        <v>786.36595964024923</v>
       </c>
       <c r="BK103" s="4">
         <v>797.94325327701154</v>
@@ -31317,16 +31317,16 @@
         <v>809.62474255650454</v>
       </c>
       <c r="BM103" s="4">
-        <v>821.41136523951309</v>
+        <v>821.41136523951263</v>
       </c>
       <c r="BN103" s="4">
         <v>833.3040675266684</v>
       </c>
       <c r="BO103" s="4">
-        <v>845.30380413440798</v>
+        <v>845.30380413440844</v>
       </c>
       <c r="BP103" s="4">
-        <v>857.41153837161755</v>
+        <v>857.41153837161789</v>
       </c>
       <c r="BQ103" s="4">
         <v>869.62824221696224</v>
@@ -31347,34 +31347,34 @@
         <v>932.38094159433581</v>
       </c>
       <c r="BW103" s="4">
-        <v>930.08435096648873</v>
+        <v>945.27237006868495</v>
       </c>
       <c r="BX103" s="4">
-        <v>912.20438633780122</v>
+        <v>958.27982139930259</v>
       </c>
       <c r="BY103" s="4">
-        <v>670.10105876661964</v>
+        <v>749.72248292205541</v>
       </c>
       <c r="BZ103" s="4">
-        <v>696.23843265113237</v>
+        <v>664.41943776101675</v>
       </c>
       <c r="CA103" s="4">
-        <v>706.26888405872228</v>
+        <v>743.94141049649829</v>
       </c>
       <c r="CB103" s="4">
-        <v>736.74779149381197</v>
+        <v>774.13642488618666</v>
       </c>
       <c r="CC103" s="4">
-        <v>781.76010118989529</v>
+        <v>816.93382502986231</v>
       </c>
       <c r="CD103" s="4">
-        <v>817.33952559908198</v>
+        <v>852.24295677029409</v>
       </c>
       <c r="CE103" s="4">
-        <v>851.73444312401909</v>
+        <v>886.26749376653481</v>
       </c>
       <c r="CF103" s="5">
-        <v>873.29173157463435</v>
+        <v>866.62506490796761</v>
       </c>
       <c r="CH103" s="1" t="s">
         <v>1</v>
@@ -31389,49 +31389,49 @@
         <v>553.04038766666667</v>
       </c>
       <c r="CL103" s="4">
-        <v>481.21448448899991</v>
+        <v>521.88895590155653</v>
       </c>
       <c r="CM103" s="4">
-        <v>485.29161484940084</v>
+        <v>555.95828151606736</v>
       </c>
       <c r="CN103" s="4">
-        <v>533.92675992470481</v>
+        <v>560.07210604971215</v>
       </c>
       <c r="CO103" s="4">
-        <v>564.22295500415942</v>
+        <v>560.48096063466517</v>
       </c>
       <c r="CP103" s="4">
-        <v>548.38080666989777</v>
+        <v>564.83040186634003</v>
       </c>
       <c r="CQ103" s="4">
-        <v>558.80578923891653</v>
+        <v>572.6370620535896</v>
       </c>
       <c r="CR103" s="4">
-        <v>547.08829504178289</v>
+        <v>576.90099561207182</v>
       </c>
       <c r="CS103" s="4">
-        <v>549.96496817187017</v>
+        <v>575.81735556180956</v>
       </c>
       <c r="CT103" s="4">
-        <v>544.85195616249575</v>
+        <v>581.75015078513934</v>
       </c>
       <c r="CU103" s="4">
-        <v>552.2666428340508</v>
+        <v>582.49352489569173</v>
       </c>
       <c r="CV103" s="4">
-        <v>594.34395322245985</v>
+        <v>577.74517060108565</v>
       </c>
       <c r="CW103" s="4">
-        <v>598.80324880146225</v>
+        <v>591.28865178178035</v>
       </c>
       <c r="CX103" s="4">
-        <v>603.30267804067512</v>
+        <v>589.5552849133478</v>
       </c>
       <c r="CY103" s="4">
-        <v>607.84260214304118</v>
+        <v>590.66271887794551</v>
       </c>
       <c r="CZ103" s="4">
-        <v>612.42338556232858</v>
+        <v>604.48515230635712</v>
       </c>
       <c r="DA103" s="4">
         <v>617.04539603238936</v>
@@ -31443,7 +31443,7 @@
         <v>618.32410417964877</v>
       </c>
       <c r="DD103" s="4">
-        <v>640.63396480455731</v>
+        <v>633.11244927362009</v>
       </c>
       <c r="DE103" s="4">
         <v>650.89967048779829</v>
@@ -31475,52 +31475,52 @@
         <v>-1439.0122181306997</v>
       </c>
       <c r="F104" s="7">
-        <v>-1452.2171280938758</v>
+        <v>-1432.2365737805453</v>
       </c>
       <c r="G104" s="7">
-        <v>-1465.5408822467207</v>
+        <v>-1397.7812322520765</v>
       </c>
       <c r="H104" s="7">
-        <v>-1474.0144044384886</v>
+        <v>-1408.3178835202741</v>
       </c>
       <c r="I104" s="7">
         <v>-1427.3585927572117</v>
       </c>
       <c r="J104" s="7">
-        <v>-1455.8104867586933</v>
+        <v>-1454.1842397939738</v>
       </c>
       <c r="K104" s="7">
-        <v>-1487.6117811395213</v>
+        <v>-1459.7998754800458</v>
       </c>
       <c r="L104" s="7">
-        <v>-1516.0959538364441</v>
+        <v>-1463.3134238571806</v>
       </c>
       <c r="M104" s="7">
-        <v>-1496.7215196651691</v>
+        <v>-1477.3730446718951</v>
       </c>
       <c r="N104" s="7">
-        <v>-1495.6122418984089</v>
+        <v>-1491.5592020739418</v>
       </c>
       <c r="O104" s="7">
-        <v>-1535.7025526196801</v>
+        <v>-1505.8730348926067</v>
       </c>
       <c r="P104" s="7">
-        <v>-1540.1494828906873</v>
+        <v>-1520.3156922066405</v>
       </c>
       <c r="Q104" s="7">
-        <v>-1547.2571702103933</v>
+        <v>-1543.0984782743262</v>
       </c>
       <c r="R104" s="7">
-        <v>-1561.6830312454615</v>
+        <v>-1571.2968368579122</v>
       </c>
       <c r="S104" s="7">
-        <v>-1583.6181785266708</v>
+        <v>-1584.7575593000204</v>
       </c>
       <c r="T104" s="7">
-        <v>-1592.2374088000774</v>
+        <v>-1594.5203773337205</v>
       </c>
       <c r="U104" s="7">
-        <v>-1600.8742121459447</v>
+        <v>-1604.3710607297239</v>
       </c>
       <c r="V104" s="7">
         <v>-1614.3104002762914</v>
@@ -31553,13 +31553,13 @@
         <v>-826.50408583333308</v>
       </c>
       <c r="AH104" s="7">
-        <v>-1540.0842756124996</v>
+        <v>-1495.9292226058328</v>
       </c>
       <c r="AI104" s="7">
-        <v>-1547.8116868011107</v>
+        <v>-1510.282385609285</v>
       </c>
       <c r="AJ104" s="7">
-        <v>-1558.8900393998488</v>
+        <v>-1524.7647270797684</v>
       </c>
       <c r="AK104" s="7">
         <v>-1539.3774096234863</v>
@@ -31574,7 +31574,7 @@
         <v>-1584.0092872737901</v>
       </c>
       <c r="AO104" s="7">
-        <v>-1599.1551708592542</v>
+        <v>-1599.155170859254</v>
       </c>
       <c r="AP104" s="7">
         <v>-1614.4373673969872</v>
@@ -31595,7 +31595,7 @@
         <v>-1668.5671987977989</v>
       </c>
       <c r="AV104" s="7">
-        <v>-1679.0843035869791</v>
+        <v>-1679.0843035869789</v>
       </c>
       <c r="AW104" s="7">
         <v>-1689.6960623192617</v>
@@ -31610,16 +31610,16 @@
         <v>-1563.3353083399275</v>
       </c>
       <c r="BA104" s="7">
-        <v>-1593.6504942683027</v>
+        <v>-1554.6789715505306</v>
       </c>
       <c r="BB104" s="7">
-        <v>-1648.1133487167176</v>
+        <v>-1608.1133487167176</v>
       </c>
       <c r="BC104" s="7">
-        <v>-1702.4363688551682</v>
+        <v>-1662.4363688551682</v>
       </c>
       <c r="BD104" s="8">
-        <v>-1766.6182961748648</v>
+        <v>-1766.7012170179539</v>
       </c>
       <c r="BF104" t="s">
         <v>2</v>
@@ -31634,7 +31634,7 @@
         <v>-759.58914345000039</v>
       </c>
       <c r="BJ104" s="7">
-        <v>-1690.6065379200159</v>
+        <v>-1786.3659596402497</v>
       </c>
       <c r="BK104" s="7">
         <v>-1797.9432532770115</v>
@@ -31643,16 +31643,16 @@
         <v>-1809.6247425565045</v>
       </c>
       <c r="BM104" s="7">
-        <v>-1821.4113652395126</v>
+        <v>-1821.4113652395131</v>
       </c>
       <c r="BN104" s="7">
         <v>-1833.3040675266684</v>
       </c>
       <c r="BO104" s="7">
-        <v>-1845.3038041344084</v>
+        <v>-1845.303804134408</v>
       </c>
       <c r="BP104" s="7">
-        <v>-1857.411538371618</v>
+        <v>-1857.4115383716176</v>
       </c>
       <c r="BQ104" s="7">
         <v>-1869.6282422169622</v>
@@ -31673,34 +31673,34 @@
         <v>-1932.3809415943358</v>
       </c>
       <c r="BW104" s="7">
-        <v>-1930.0843509664887</v>
+        <v>-1945.2723700686845</v>
       </c>
       <c r="BX104" s="7">
-        <v>-1912.2043863378012</v>
+        <v>-1958.279821399303</v>
       </c>
       <c r="BY104" s="7">
-        <v>-1670.1010587666196</v>
+        <v>-1749.7224829220554</v>
       </c>
       <c r="BZ104" s="7">
-        <v>-1623.0555250489142</v>
+        <v>-1654.8745199390296</v>
       </c>
       <c r="CA104" s="7">
-        <v>-1639.7487192606243</v>
+        <v>-1602.0761928228483</v>
       </c>
       <c r="CB104" s="7">
-        <v>-1636.2339702554084</v>
+        <v>-1598.8453368630337</v>
       </c>
       <c r="CC104" s="7">
-        <v>-1618.4284964150677</v>
+        <v>-1583.2547725751006</v>
       </c>
       <c r="CD104" s="7">
-        <v>-1610.3007693843253</v>
+        <v>-1575.3973382131132</v>
       </c>
       <c r="CE104" s="7">
-        <v>-1603.604614514237</v>
+        <v>-1569.0715638717213</v>
       </c>
       <c r="CF104" s="8">
-        <v>-1609.9953775823669</v>
+        <v>-1616.6620442490334</v>
       </c>
       <c r="CH104" t="s">
         <v>2</v>
@@ -31715,49 +31715,49 @@
         <v>-721.1327023333331</v>
       </c>
       <c r="CL104" s="7">
-        <v>-1460.2761633209996</v>
+        <v>-1419.6016919084429</v>
       </c>
       <c r="CM104" s="7">
-        <v>-1473.672448790888</v>
+        <v>-1403.0057821242215</v>
       </c>
       <c r="CN104" s="7">
-        <v>-1442.6679802883473</v>
+        <v>-1416.5226341633397</v>
       </c>
       <c r="CO104" s="7">
-        <v>-1430.1611378708094</v>
+        <v>-1433.9031322403039</v>
       </c>
       <c r="CP104" s="7">
-        <v>-1463.9527430409455</v>
+        <v>-1447.503147844503</v>
       </c>
       <c r="CQ104" s="7">
-        <v>-1471.6387624193242</v>
+        <v>-1457.807489604651</v>
       </c>
       <c r="CR104" s="7">
-        <v>-1501.630257581382</v>
+        <v>-1471.817557011093</v>
       </c>
       <c r="CS104" s="7">
-        <v>-1517.1920514249027</v>
+        <v>-1491.3396640349633</v>
       </c>
       <c r="CT104" s="7">
-        <v>-1540.9094766106477</v>
+        <v>-1504.0112819880042</v>
       </c>
       <c r="CU104" s="7">
-        <v>-1552.2666428340508</v>
+        <v>-1522.0397607724096</v>
       </c>
       <c r="CV104" s="7">
-        <v>-1529.1301320166542</v>
+        <v>-1545.7289146380283</v>
       </c>
       <c r="CW104" s="7">
-        <v>-1543.7821032048043</v>
+        <v>-1551.2967002244857</v>
       </c>
       <c r="CX104" s="7">
-        <v>-1558.5659421336468</v>
+        <v>-1572.3133352609739</v>
       </c>
       <c r="CY104" s="7">
-        <v>-1573.4828356128496</v>
+        <v>-1590.6627188779455</v>
       </c>
       <c r="CZ104" s="7">
-        <v>-1588.5339811333654</v>
+        <v>-1596.4722143893368</v>
       </c>
       <c r="DA104" s="7">
         <v>-1603.7205869635652</v>
@@ -31769,7 +31769,7 @@
         <v>-1618.3241041796487</v>
       </c>
       <c r="DD104" s="7">
-        <v>-1640.6339648045573</v>
+        <v>-1633.1124492736201</v>
       </c>
       <c r="DE104" s="7">
         <v>-1650.8996704877982</v>
@@ -31801,52 +31801,52 @@
         <v>964.26936913439988</v>
       </c>
       <c r="F105" s="10">
-        <v>973.4553934566095</v>
+        <v>933.49428482994824</v>
       </c>
       <c r="G105" s="10">
-        <v>982.7240919977188</v>
+        <v>847.20479200842988</v>
       </c>
       <c r="H105" s="10">
-        <v>982.13591732879354</v>
+        <v>850.74287549236465</v>
       </c>
       <c r="I105" s="10">
         <v>871.13125794230609</v>
       </c>
       <c r="J105" s="10">
-        <v>910.18277259712045</v>
+        <v>906.93027866768148</v>
       </c>
       <c r="K105" s="10">
-        <v>955.77241755049477</v>
+        <v>900.14860623154368</v>
       </c>
       <c r="L105" s="10">
-        <v>994.56570264178254</v>
+        <v>889.00064268325605</v>
       </c>
       <c r="M105" s="10">
-        <v>937.47819845395418</v>
+        <v>898.78124846740513</v>
       </c>
       <c r="N105" s="10">
-        <v>916.75595935254591</v>
+        <v>908.64987970361165</v>
       </c>
       <c r="O105" s="10">
-        <v>978.26636407509011</v>
+        <v>918.6073286209438</v>
       </c>
       <c r="P105" s="10">
-        <v>968.32197594662671</v>
+        <v>928.65439457853245</v>
       </c>
       <c r="Q105" s="10">
-        <v>963.52955767752621</v>
+        <v>955.2121738053919</v>
       </c>
       <c r="R105" s="10">
-        <v>973.20241670297389</v>
+        <v>992.43002792787513</v>
       </c>
       <c r="S105" s="10">
-        <v>997.72123845330043</v>
+        <v>1000</v>
       </c>
       <c r="T105" s="10">
-        <v>995.43406293271391</v>
+        <v>1000</v>
       </c>
       <c r="U105" s="10">
-        <v>993.00630283244186</v>
+        <v>1000</v>
       </c>
       <c r="V105" s="10">
         <v>1000</v>
@@ -31879,13 +31879,13 @@
         <v>241.39414666666642</v>
       </c>
       <c r="AH105" s="10">
-        <v>1000</v>
+        <v>911.68989398666645</v>
       </c>
       <c r="AI105" s="10">
-        <v>996.73330541619725</v>
+        <v>921.6747030325464</v>
       </c>
       <c r="AJ105" s="10">
-        <v>1000</v>
+        <v>931.74937535983918</v>
       </c>
       <c r="AK105" s="10">
         <v>941.91471973807734</v>
@@ -31900,7 +31900,7 @@
         <v>972.96298245133221</v>
       </c>
       <c r="AO105" s="10">
-        <v>983.4992492933942</v>
+        <v>983.49924929339409</v>
       </c>
       <c r="AP105" s="10">
         <v>994.13034253703472</v>
@@ -31936,7 +31936,7 @@
         <v>1000</v>
       </c>
       <c r="BA105" s="10">
-        <v>1000</v>
+        <v>998.9715227177719</v>
       </c>
       <c r="BB105" s="10">
         <v>1000</v>
@@ -32008,25 +32008,25 @@
         <v>1000</v>
       </c>
       <c r="BZ105" s="10">
-        <v>926.81709239778206</v>
+        <v>990.45508217801319</v>
       </c>
       <c r="CA105" s="10">
-        <v>933.47983520190212</v>
+        <v>858.13478232635055</v>
       </c>
       <c r="CB105" s="10">
-        <v>899.48617876159631</v>
+        <v>824.70891197684682</v>
       </c>
       <c r="CC105" s="10">
-        <v>836.66839522517239</v>
+        <v>766.32094754523814</v>
       </c>
       <c r="CD105" s="10">
-        <v>792.96124378524325</v>
+        <v>723.15438144281961</v>
       </c>
       <c r="CE105" s="10">
-        <v>751.87017139021805</v>
+        <v>682.80407010518661</v>
       </c>
       <c r="CF105" s="11">
-        <v>736.70364600773257</v>
+        <v>750.03697934106583</v>
       </c>
       <c r="CH105" t="s">
         <v>3</v>
@@ -32041,49 +32041,49 @@
         <v>168.0923146666666</v>
       </c>
       <c r="CL105" s="10">
-        <v>979.06167883199964</v>
+        <v>897.71273600688642</v>
       </c>
       <c r="CM105" s="10">
-        <v>988.38083394148748</v>
+        <v>847.047500608154</v>
       </c>
       <c r="CN105" s="10">
-        <v>908.74122036364236</v>
+        <v>856.45052811362757</v>
       </c>
       <c r="CO105" s="10">
-        <v>865.93818286664998</v>
+        <v>873.4221716056386</v>
       </c>
       <c r="CP105" s="10">
-        <v>915.57193637104763</v>
+        <v>882.67274597816311</v>
       </c>
       <c r="CQ105" s="10">
-        <v>912.83297318040752</v>
+        <v>885.17042755106149</v>
       </c>
       <c r="CR105" s="10">
-        <v>954.54196253959901</v>
+        <v>894.91656139902125</v>
       </c>
       <c r="CS105" s="10">
-        <v>967.22708325303267</v>
+        <v>915.52230847315377</v>
       </c>
       <c r="CT105" s="10">
-        <v>996.05752044815199</v>
+        <v>922.26113120286493</v>
       </c>
       <c r="CU105" s="10">
+        <v>939.5462358767179</v>
+      </c>
+      <c r="CV105" s="10">
+        <v>967.98374403694265</v>
+      </c>
+      <c r="CW105" s="10">
+        <v>960.00804844270499</v>
+      </c>
+      <c r="CX105" s="10">
+        <v>982.75805034762607</v>
+      </c>
+      <c r="CY105" s="10">
         <v>1000</v>
       </c>
-      <c r="CV105" s="10">
-        <v>934.78617879419448</v>
-      </c>
-      <c r="CW105" s="10">
-        <v>944.97885440334198</v>
-      </c>
-      <c r="CX105" s="10">
-        <v>955.26326409297178</v>
-      </c>
-      <c r="CY105" s="10">
-        <v>965.64023346980866</v>
-      </c>
       <c r="CZ105" s="10">
-        <v>976.1105955710367</v>
+        <v>991.98706208297915</v>
       </c>
       <c r="DA105" s="10">
         <v>986.67519093117585</v>
@@ -32198,86 +32198,86 @@
         <v>6</v>
       </c>
       <c r="B108" s="15">
-        <v>1384132345.062906</v>
+        <v>1324676752.4978151</v>
       </c>
       <c r="C108" s="16">
-        <v>584399638.97178626</v>
+        <v>581075287.4170475</v>
       </c>
       <c r="D108" s="16">
-        <v>537781668.45782018</v>
+        <v>534760000.55819589</v>
       </c>
       <c r="E108" s="16">
-        <v>181463585.07183787</v>
+        <v>185790103.97364777</v>
       </c>
       <c r="F108" s="16">
-        <v>166354453.14765292</v>
+        <v>169418467.14182264</v>
       </c>
       <c r="G108" s="16">
-        <v>153559096.76404506</v>
+        <v>154544750.13017818</v>
       </c>
       <c r="H108" s="16">
-        <v>141016827.27245948</v>
+        <v>139982652.85848188</v>
       </c>
       <c r="I108" s="16">
-        <v>127927462.40969157</v>
+        <v>127555998.12083706</v>
       </c>
       <c r="J108" s="16">
-        <v>115231567.90387717</v>
+        <v>116250368.71814576</v>
       </c>
       <c r="K108" s="16">
-        <v>104960376.18775457</v>
+        <v>106045397.28938025</v>
       </c>
       <c r="L108" s="16">
-        <v>95685939.918858379</v>
+        <v>96754790.688043579</v>
       </c>
       <c r="M108" s="16">
-        <v>87370859.121303529</v>
+        <v>87780018.664477572</v>
       </c>
       <c r="N108" s="16">
-        <v>79790110.41318661</v>
+        <v>80575240.689377084</v>
       </c>
       <c r="O108" s="16">
-        <v>72878036.309049785</v>
+        <v>73546583.697467491</v>
       </c>
       <c r="P108" s="16">
-        <v>66572119.061260641</v>
+        <v>66798044.723667927</v>
       </c>
       <c r="Q108" s="16">
-        <v>59428492.901967056</v>
+        <v>59595895.238672584</v>
       </c>
       <c r="R108" s="16">
-        <v>54307045.132211983</v>
+        <v>54421965.973738737</v>
       </c>
       <c r="S108" s="16">
-        <v>50784212.706368402</v>
+        <v>49779098.287889443</v>
       </c>
       <c r="T108" s="16">
-        <v>46578481.671553552</v>
+        <v>46418007.806459099</v>
       </c>
       <c r="U108" s="16">
-        <v>42762156.991299599</v>
+        <v>42563254.91878321</v>
       </c>
       <c r="V108" s="16">
-        <v>39371493.60807725</v>
+        <v>39470792.180570625</v>
       </c>
       <c r="W108" s="16">
-        <v>36121242.643304043</v>
+        <v>36161239.98085171</v>
       </c>
       <c r="X108" s="16">
-        <v>33346535.654131219</v>
+        <v>34451379.893826783</v>
       </c>
       <c r="Y108" s="16">
-        <v>29301076.527761646</v>
+        <v>29335153.617023565</v>
       </c>
       <c r="Z108" s="16">
-        <v>26899742.542724803</v>
+        <v>26931005.010520928</v>
       </c>
       <c r="AA108" s="17">
-        <v>24678464.103820167</v>
+        <v>24790539.828422952</v>
       </c>
       <c r="AB108" s="18">
         <f>SUM(TotalCost)</f>
-        <v>4342703030.5567102</v>
+        <v>4289472789.9053454</v>
       </c>
     </row>
     <row r="110" spans="1:112" x14ac:dyDescent="0.35">
@@ -32374,83 +32374,83 @@
         <v>40209082.125439994</v>
       </c>
       <c r="C111" s="4">
-        <v>29322632.053442735</v>
+        <v>29028568.012613229</v>
       </c>
       <c r="D111" s="4">
-        <v>26754467.291793648</v>
+        <v>26485337.771793649</v>
       </c>
       <c r="E111" s="4">
-        <v>5517801.0701686461</v>
+        <v>5370071.801232243</v>
       </c>
       <c r="F111" s="4">
-        <v>5113235.449678123</v>
+        <v>5238623.6495696185</v>
       </c>
       <c r="G111" s="4">
-        <v>4994786.3792752959</v>
+        <v>5120714.4363529822</v>
       </c>
       <c r="H111" s="4">
-        <v>4906718.1597691104</v>
+        <v>4952008.6993450094</v>
       </c>
       <c r="I111" s="4">
-        <v>4794803.5200220728</v>
+        <v>4786478.409602805</v>
       </c>
       <c r="J111" s="4">
-        <v>4631871.9962764718</v>
+        <v>4610166.6716081016</v>
       </c>
       <c r="K111" s="4">
-        <v>4444858.9555292064</v>
+        <v>4309898.2991251014</v>
       </c>
       <c r="L111" s="4">
-        <v>4277454.9661466088</v>
+        <v>4031435.0272658197</v>
       </c>
       <c r="M111" s="4">
-        <v>3963894.3245400419</v>
+        <v>3774757.7065619589</v>
       </c>
       <c r="N111" s="4">
-        <v>3677968.9295408828</v>
+        <v>3545545.5500420234</v>
       </c>
       <c r="O111" s="4">
-        <v>3420032.4249733407</v>
+        <v>3344167.1482943618</v>
       </c>
       <c r="P111" s="4">
-        <v>3180489.3414878245</v>
+        <v>3108804.0486599728</v>
       </c>
       <c r="Q111" s="4">
-        <v>2958230.6028099065</v>
+        <v>2942835.0056714206</v>
       </c>
       <c r="R111" s="4">
-        <v>2767834.5601770198</v>
+        <v>2770730.5793694658</v>
       </c>
       <c r="S111" s="4">
-        <v>2560171.9486991633</v>
+        <v>2514944.365909026</v>
       </c>
       <c r="T111" s="4">
-        <v>2440220.1866302872</v>
+        <v>2372524.0116405245</v>
       </c>
       <c r="U111" s="4">
-        <v>2101227.6703677592</v>
+        <v>2036394.4516432886</v>
       </c>
       <c r="V111" s="4">
-        <v>1834364.9984163074</v>
+        <v>1844077.1969583482</v>
       </c>
       <c r="W111" s="4">
-        <v>1638361.6085555698</v>
+        <v>1624104.0771693215</v>
       </c>
       <c r="X111" s="4">
-        <v>1497402.1760431731</v>
+        <v>1331046.4721497726</v>
       </c>
       <c r="Y111" s="4">
-        <v>1230270.7267541748</v>
+        <v>1046116.239576439</v>
       </c>
       <c r="Z111" s="4">
-        <v>954728.85594020726</v>
+        <v>774311.93263730826</v>
       </c>
       <c r="AA111" s="5">
-        <v>743874.8717112923</v>
+        <v>741306.64957830892</v>
       </c>
       <c r="AB111" s="12">
         <f>SUM(B111:AA111)</f>
-        <v>169936785.19418883</v>
+        <v>167914050.3398101</v>
       </c>
     </row>
     <row r="112" spans="1:112" x14ac:dyDescent="0.35">
@@ -32461,83 +32461,83 @@
         <v>11672227.954879999</v>
       </c>
       <c r="C112" s="7">
-        <v>8784628.5229423307</v>
+        <v>8690964.5920795165</v>
       </c>
       <c r="D112" s="7">
-        <v>7923506.3592439955</v>
+        <v>7838038.1192439953</v>
       </c>
       <c r="E112" s="7">
-        <v>1753843.5528523177</v>
+        <v>1691783.6736335622</v>
       </c>
       <c r="F112" s="7">
-        <v>1666485.6921266154</v>
+        <v>1613143.2496698389</v>
       </c>
       <c r="G112" s="7">
-        <v>1593662.0864543105</v>
+        <v>1541330.9257688485</v>
       </c>
       <c r="H112" s="7">
-        <v>1518100.384936668</v>
+        <v>1488312.3624520837</v>
       </c>
       <c r="I112" s="7">
-        <v>1453934.8866562878</v>
+        <v>1439442.9248849838</v>
       </c>
       <c r="J112" s="7">
-        <v>1408118.1195174167</v>
+        <v>1389232.7014402431</v>
       </c>
       <c r="K112" s="7">
-        <v>1373224.6309016529</v>
+        <v>1276983.0657211021</v>
       </c>
       <c r="L112" s="7">
-        <v>1330737.7158522622</v>
+        <v>1175204.0064035645</v>
       </c>
       <c r="M112" s="7">
-        <v>1200141.9201020235</v>
+        <v>1083928.365373624</v>
       </c>
       <c r="N112" s="7">
-        <v>1084058.3428351693</v>
+        <v>1007083.2579199411</v>
       </c>
       <c r="O112" s="7">
-        <v>982910.97096340451</v>
+        <v>945100.15040016407</v>
       </c>
       <c r="P112" s="7">
-        <v>890584.85795796767</v>
+        <v>854860.2987853142</v>
       </c>
       <c r="Q112" s="7">
-        <v>806523.95418736304</v>
+        <v>809836.20409960335</v>
       </c>
       <c r="R112" s="7">
-        <v>740008.47495703201</v>
+        <v>764053.35266843205</v>
       </c>
       <c r="S112" s="7">
-        <v>672408.09400791302</v>
+        <v>663749.02973783121</v>
       </c>
       <c r="T112" s="7">
-        <v>626871.54056492378</v>
+        <v>604099.99614726135</v>
       </c>
       <c r="U112" s="7">
-        <v>494421.66378007131</v>
+        <v>476618.27408386028</v>
       </c>
       <c r="V112" s="7">
-        <v>394194.46750399325</v>
+        <v>406669.61649577145</v>
       </c>
       <c r="W112" s="7">
-        <v>319196.06964550371</v>
+        <v>324751.92339987057</v>
       </c>
       <c r="X112" s="7">
-        <v>269098.57378596958</v>
+        <v>212970.20475150773</v>
       </c>
       <c r="Y112" s="7">
-        <v>175293.663458603</v>
+        <v>110810.44664083561</v>
       </c>
       <c r="Z112" s="7">
-        <v>76515.425985282913</v>
+        <v>13176.498871885267</v>
       </c>
       <c r="AA112" s="8">
-        <v>6842.1085711386258</v>
+        <v>6768.0256401484748</v>
       </c>
       <c r="AB112" s="13">
         <f t="shared" ref="AB112:AB115" si="0">SUM(B112:AA112)</f>
-        <v>49217540.034670204</v>
+        <v>48101139.22119379</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -32548,83 +32548,83 @@
         <v>65731902143.913589</v>
       </c>
       <c r="C113" s="7">
-        <v>46813503044.38726</v>
+        <v>46309907376.131966</v>
       </c>
       <c r="D113" s="7">
-        <v>44288270337.765701</v>
+        <v>43811839828.485703</v>
       </c>
       <c r="E113" s="7">
-        <v>6012150137.5639048</v>
+        <v>5942587390.532445</v>
       </c>
       <c r="F113" s="7">
-        <v>5687840329.9833775</v>
+        <v>5622029964.4773874</v>
       </c>
       <c r="G113" s="7">
-        <v>5381024571.7672825</v>
+        <v>5318764175.3215618</v>
       </c>
       <c r="H113" s="7">
-        <v>5090759191.9071836</v>
+        <v>5031857270.6706963</v>
       </c>
       <c r="I113" s="7">
-        <v>4816151423.2736502</v>
+        <v>4760426813.0332689</v>
       </c>
       <c r="J113" s="7">
-        <v>4556356656.7388535</v>
+        <v>4503637965.7139034</v>
       </c>
       <c r="K113" s="7">
-        <v>4310575843.4183836</v>
+        <v>4260700925.1121774</v>
       </c>
       <c r="L113" s="7">
-        <v>4078053037.0423722</v>
+        <v>4030868491.5294061</v>
       </c>
       <c r="M113" s="7">
-        <v>3858073068.897018</v>
+        <v>3813433771.01193</v>
       </c>
       <c r="N113" s="7">
-        <v>3649959348.1853476</v>
+        <v>3607728001.1624961</v>
       </c>
       <c r="O113" s="7">
-        <v>3453071781.0417943</v>
+        <v>3413118494.2325883</v>
       </c>
       <c r="P113" s="7">
-        <v>3266804801.8001256</v>
+        <v>3229006691.1692963</v>
       </c>
       <c r="Q113" s="7">
-        <v>3090585510.4595027</v>
+        <v>3054826320.6315656</v>
       </c>
       <c r="R113" s="7">
-        <v>2923871910.6200924</v>
+        <v>2890041657.3135295</v>
       </c>
       <c r="S113" s="7">
-        <v>2766151242.4686594</v>
+        <v>2734145874.21806</v>
       </c>
       <c r="T113" s="7">
-        <v>2616938405.6869183</v>
+        <v>2586659483.8126397</v>
       </c>
       <c r="U113" s="7">
-        <v>2475774467.4319925</v>
+        <v>2447128863.2730246</v>
       </c>
       <c r="V113" s="7">
-        <v>2342225250.7999892</v>
+        <v>2315124859.2788057</v>
       </c>
       <c r="W113" s="7">
-        <v>2215879999.4312358</v>
+        <v>2190241468.0696445</v>
       </c>
       <c r="X113" s="7">
-        <v>2096350114.1499164</v>
+        <v>2072094586.7024446</v>
       </c>
       <c r="Y113" s="7">
-        <v>1983267957.7523961</v>
+        <v>1960320831.6687067</v>
       </c>
       <c r="Z113" s="7">
-        <v>1876285724.2681334</v>
+        <v>1854576421.2385006</v>
       </c>
       <c r="AA113" s="8">
-        <v>1775074369.2153721</v>
+        <v>1754536118.0934854</v>
       </c>
       <c r="AB113" s="13">
         <f t="shared" si="0"/>
-        <v>237156900669.97003</v>
+        <v>235247505786.7988</v>
       </c>
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.35">
@@ -32635,83 +32635,83 @@
         <v>5541727.7904000003</v>
       </c>
       <c r="C114" s="7">
-        <v>3919777.0300294226</v>
+        <v>3868252.4967411375</v>
       </c>
       <c r="D114" s="7">
-        <v>3480195.0106522222</v>
+        <v>3432901.1706522219</v>
       </c>
       <c r="E114" s="7">
-        <v>602654.29278755514</v>
+        <v>576744.25993909221</v>
       </c>
       <c r="F114" s="7">
-        <v>560242.72841145471</v>
+        <v>537413.39216086571</v>
       </c>
       <c r="G114" s="7">
-        <v>522502.29908100568</v>
+        <v>500172.26736412343</v>
       </c>
       <c r="H114" s="7">
-        <v>484536.71501251141</v>
+        <v>470084.24917425797</v>
       </c>
       <c r="I114" s="7">
-        <v>451156.4436852237</v>
+        <v>442087.6645650561</v>
       </c>
       <c r="J114" s="7">
-        <v>424710.3208263875</v>
+        <v>415945.24274565023</v>
       </c>
       <c r="K114" s="7">
-        <v>402616.78663061699</v>
+        <v>387981.23305202962</v>
       </c>
       <c r="L114" s="7">
-        <v>379743.29043105594</v>
+        <v>362114.51027092419</v>
       </c>
       <c r="M114" s="7">
-        <v>351861.57989121904</v>
+        <v>338054.08501372673</v>
       </c>
       <c r="N114" s="7">
-        <v>325714.60219227918</v>
+        <v>315694.75301221979</v>
       </c>
       <c r="O114" s="7">
-        <v>301201.65833151317</v>
+        <v>294936.85847218492</v>
       </c>
       <c r="P114" s="7">
-        <v>278227.30604640272</v>
+        <v>272288.73371949024</v>
       </c>
       <c r="Q114" s="7">
-        <v>256701.27558958688</v>
+        <v>254455.43994026602</v>
       </c>
       <c r="R114" s="7">
-        <v>236599.24005840142</v>
+        <v>237763.64709179732</v>
       </c>
       <c r="S114" s="7">
-        <v>217423.5667820875</v>
+        <v>217321.48276733322</v>
       </c>
       <c r="T114" s="7">
-        <v>188196.67723166524</v>
+        <v>187502.90308532992</v>
       </c>
       <c r="U114" s="7">
-        <v>156343.77671669217</v>
+        <v>157438.13622872377</v>
       </c>
       <c r="V114" s="7">
-        <v>137191.14709383028</v>
+        <v>129397.81285028625</v>
       </c>
       <c r="W114" s="7">
-        <v>116585.72756463903</v>
+        <v>109204.30504946921</v>
       </c>
       <c r="X114" s="7">
-        <v>95898.603896424029</v>
+        <v>85581.885267116013</v>
       </c>
       <c r="Y114" s="7">
-        <v>78161.932259066045</v>
+        <v>67735.613444999588</v>
       </c>
       <c r="Z114" s="7">
-        <v>60933.069446807982</v>
+        <v>50697.298081056768</v>
       </c>
       <c r="AA114" s="8">
-        <v>48100.679874978217</v>
+        <v>45184.912547502841</v>
       </c>
       <c r="AB114" s="13">
         <f t="shared" si="0"/>
-        <v>19619003.550923049</v>
+        <v>19298682.14363686</v>
       </c>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.35">
@@ -32722,83 +32722,83 @@
         <v>789555.89344000001</v>
       </c>
       <c r="C115" s="10">
-        <v>556958.41757226398</v>
+        <v>549558.71361744008</v>
       </c>
       <c r="D115" s="10">
-        <v>493154.59270067158</v>
+        <v>486368.03270067158</v>
       </c>
       <c r="E115" s="10">
-        <v>86314.234840079356</v>
+        <v>82343.131667600042</v>
       </c>
       <c r="F115" s="10">
-        <v>80098.916298565804</v>
+        <v>76617.450556093318</v>
       </c>
       <c r="G115" s="10">
-        <v>74606.486713805934</v>
+        <v>71198.522653960317</v>
       </c>
       <c r="H115" s="10">
-        <v>69043.179683148381</v>
+        <v>66903.876996298874</v>
       </c>
       <c r="I115" s="10">
-        <v>64189.802349808146</v>
+        <v>62915.701870189543</v>
       </c>
       <c r="J115" s="10">
-        <v>60428.449658851168</v>
+        <v>59198.105834500522</v>
       </c>
       <c r="K115" s="10">
-        <v>57342.742378320567</v>
+        <v>55158.560976695881</v>
       </c>
       <c r="L115" s="10">
-        <v>54103.727037149583</v>
+        <v>51418.791960011105</v>
       </c>
       <c r="M115" s="10">
-        <v>50039.378495909215</v>
+        <v>47945.415209059371</v>
       </c>
       <c r="N115" s="10">
-        <v>46233.517118363408</v>
+        <v>44726.207844323944</v>
       </c>
       <c r="O115" s="10">
-        <v>42671.992850488292</v>
+        <v>41747.180130426976</v>
       </c>
       <c r="P115" s="10">
-        <v>39336.615490943477</v>
+        <v>38460.587330246737</v>
       </c>
       <c r="Q115" s="10">
-        <v>36214.012902886534</v>
+        <v>35912.610625071473</v>
       </c>
       <c r="R115" s="10">
-        <v>33301.022328622304</v>
+        <v>33531.294472233516</v>
       </c>
       <c r="S115" s="10">
-        <v>30520.985345903086</v>
+        <v>30554.526034647446</v>
       </c>
       <c r="T115" s="10">
-        <v>26104.421958231433</v>
+        <v>26104.661632058371</v>
       </c>
       <c r="U115" s="10">
-        <v>21331.757686654142</v>
+        <v>21582.548329352503</v>
       </c>
       <c r="V115" s="10">
-        <v>18530.195173367028</v>
+        <v>17427.407022128762</v>
       </c>
       <c r="W115" s="10">
-        <v>15524.385221562141</v>
+        <v>14463.313816512782</v>
       </c>
       <c r="X115" s="10">
-        <v>12523.909738835433</v>
+        <v>10996.213853654594</v>
       </c>
       <c r="Y115" s="10">
-        <v>9963.3802012587803</v>
+        <v>8417.0298163735461</v>
       </c>
       <c r="Z115" s="10">
-        <v>7473.8637814699023</v>
+        <v>5955.3186036349607</v>
       </c>
       <c r="AA115" s="11">
-        <v>5645.6389010064158</v>
+        <v>5306.9581682588787</v>
       </c>
       <c r="AB115" s="14">
         <f t="shared" si="0"/>
-        <v>2781211.5198681667</v>
+        <v>2734368.0551614449</v>
       </c>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Wind capex time series
-Added wind capex time series to data_in
-Adjusted mod to replace float value with range for wind capex
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -679,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DH119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="BY60" sqref="BY60"/>
     </sheetView>
   </sheetViews>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="BL6" s="7">
-        <v>0</v>
+        <v>2.9526867898263638</v>
       </c>
       <c r="BM6" s="7">
         <v>0</v>
@@ -2251,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="CC6" s="7">
-        <v>10.874530681594479</v>
+        <v>0.87453068159378233</v>
       </c>
       <c r="CD6" s="7">
         <v>6.3552414577279706</v>
@@ -3172,25 +3172,25 @@
         <v>84.6</v>
       </c>
       <c r="BJ9" s="7">
-        <v>84.6</v>
+        <v>76.594037045997538</v>
       </c>
       <c r="BK9" s="7">
         <v>81.8248233794111</v>
       </c>
       <c r="BL9" s="7">
-        <v>77.552686789826112</v>
+        <v>84.599999999999753</v>
       </c>
       <c r="BM9" s="7">
-        <v>53.782100970934152</v>
+        <v>63.782100970934152</v>
       </c>
       <c r="BN9" s="7">
-        <v>30.517579879671757</v>
+        <v>40.517579879671757</v>
       </c>
       <c r="BO9" s="7">
-        <v>7.7636780985885707</v>
+        <v>27.763678098588571</v>
       </c>
       <c r="BP9" s="7">
-        <v>0</v>
+        <v>5.5249912014751317</v>
       </c>
       <c r="BQ9" s="7">
         <v>0</v>
@@ -3220,16 +3220,16 @@
         <v>0</v>
       </c>
       <c r="BZ9" s="7">
-        <v>22.516024475976337</v>
+        <v>32.516024475976337</v>
       </c>
       <c r="CA9" s="7">
-        <v>66.260108696259522</v>
+        <v>76.260108696259522</v>
       </c>
       <c r="CB9" s="7">
         <v>80.577889674525068</v>
       </c>
       <c r="CC9" s="7">
-        <v>84.6</v>
+        <v>84.60000000000106</v>
       </c>
       <c r="CD9" s="7">
         <v>84.6</v>
@@ -3238,7 +3238,7 @@
         <v>84.6</v>
       </c>
       <c r="CF9" s="8">
-        <v>13.689946138523737</v>
+        <v>33.689946138523737</v>
       </c>
       <c r="CH9">
         <v>7</v>
@@ -6432,7 +6432,7 @@
         <v>257</v>
       </c>
       <c r="BJ19" s="7">
-        <v>1.9940370459971746</v>
+        <v>0</v>
       </c>
       <c r="BK19" s="7">
         <v>0</v>
@@ -7640,7 +7640,7 @@
         <v>14.05</v>
       </c>
       <c r="AA23" s="8">
-        <v>0</v>
+        <v>14.050000000000004</v>
       </c>
       <c r="AD23">
         <v>21</v>
@@ -8591,7 +8591,7 @@
         <v>15.3</v>
       </c>
       <c r="R26" s="7">
-        <v>6.5163161586489879</v>
+        <v>15.3</v>
       </c>
       <c r="S26" s="7">
         <v>15.3</v>
@@ -8690,7 +8690,7 @@
         <v>21.419999999999998</v>
       </c>
       <c r="BA26" s="7">
-        <v>17.142736481346155</v>
+        <v>7.142736481346156</v>
       </c>
       <c r="BB26" s="7">
         <v>0</v>
@@ -8843,7 +8843,7 @@
         <v>21.419999999999998</v>
       </c>
       <c r="DB26" s="7">
-        <v>10.091723826273146</v>
+        <v>20.091723826273146</v>
       </c>
       <c r="DC26" s="7">
         <v>21.419999999999998</v>
@@ -8944,7 +8944,7 @@
         <v>5</v>
       </c>
       <c r="AA27" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD27">
         <v>25</v>
@@ -9270,7 +9270,7 @@
         <v>5</v>
       </c>
       <c r="AA28" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD28">
         <v>26</v>
@@ -9402,7 +9402,7 @@
         <v>7</v>
       </c>
       <c r="BV28" s="7">
-        <v>7</v>
+        <v>4.1549930801071753</v>
       </c>
       <c r="BW28" s="7">
         <v>7</v>
@@ -9596,7 +9596,7 @@
         <v>5</v>
       </c>
       <c r="AA29" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD29">
         <v>27</v>
@@ -9728,7 +9728,7 @@
         <v>7</v>
       </c>
       <c r="BV29" s="7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BW29" s="7">
         <v>7</v>
@@ -9922,7 +9922,7 @@
         <v>26.100000000000005</v>
       </c>
       <c r="AA30" s="8">
-        <v>0</v>
+        <v>26.1</v>
       </c>
       <c r="AD30">
         <v>28</v>
@@ -10045,7 +10045,7 @@
         <v>36.539999999999992</v>
       </c>
       <c r="BS30" s="7">
-        <v>13.886798191133025</v>
+        <v>23.886798191133025</v>
       </c>
       <c r="BT30" s="7">
         <v>36.540000000000006</v>
@@ -10248,7 +10248,7 @@
         <v>5</v>
       </c>
       <c r="AA31" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD31">
         <v>29</v>
@@ -10380,7 +10380,7 @@
         <v>7</v>
       </c>
       <c r="BV31" s="7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BW31" s="7">
         <v>7</v>
@@ -10547,7 +10547,7 @@
         <v>10.100000000000001</v>
       </c>
       <c r="R32" s="7">
-        <v>0</v>
+        <v>1.2163161586489863</v>
       </c>
       <c r="S32" s="7">
         <v>10.100000000000001</v>
@@ -10796,7 +10796,7 @@
         <v>14.139999999999997</v>
       </c>
       <c r="DA32" s="7">
-        <v>6.5223724740072448</v>
+        <v>14.139999999999997</v>
       </c>
       <c r="DB32" s="7">
         <v>0</v>
@@ -11226,7 +11226,7 @@
         <v>5.25</v>
       </c>
       <c r="AA34" s="8">
-        <v>0</v>
+        <v>5.25</v>
       </c>
       <c r="AD34">
         <v>32</v>
@@ -11358,7 +11358,7 @@
         <v>7.3499999999999979</v>
       </c>
       <c r="BV34" s="7">
-        <v>7.3499999999999943</v>
+        <v>0</v>
       </c>
       <c r="BW34" s="7">
         <v>7.3499999999999979</v>
@@ -11552,7 +11552,7 @@
         <v>5</v>
       </c>
       <c r="AA35" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD35">
         <v>33</v>
@@ -13404,7 +13404,7 @@
         <v>7.07</v>
       </c>
       <c r="DA40" s="7">
-        <v>0</v>
+        <v>7.07</v>
       </c>
       <c r="DB40" s="7">
         <v>7.0699999999999994</v>
@@ -13508,7 +13508,7 @@
         <v>5</v>
       </c>
       <c r="AA41" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD41">
         <v>39</v>
@@ -13834,7 +13834,7 @@
         <v>6</v>
       </c>
       <c r="AA42" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AD42">
         <v>40</v>
@@ -14094,43 +14094,43 @@
         <v>1300</v>
       </c>
       <c r="E43" s="7">
-        <v>947.96917434199895</v>
+        <v>937.96917434199895</v>
       </c>
       <c r="F43" s="7">
         <v>926.78049691107663</v>
       </c>
       <c r="G43" s="7">
-        <v>905.94112138327546</v>
+        <v>915.94112138327546</v>
       </c>
       <c r="H43" s="7">
-        <v>865.45419147572466</v>
+        <v>875.45419147572466</v>
       </c>
       <c r="I43" s="7">
-        <v>825.32287919900591</v>
+        <v>835.32287919900591</v>
       </c>
       <c r="J43" s="7">
-        <v>785.55038511179646</v>
+        <v>805.55038511179646</v>
       </c>
       <c r="K43" s="7">
-        <v>756.13993857780224</v>
+        <v>766.13993857780224</v>
       </c>
       <c r="L43" s="7">
-        <v>727.09479802500209</v>
+        <v>737.09479802500209</v>
       </c>
       <c r="M43" s="7">
-        <v>698.4182512072266</v>
+        <v>708.4182512072266</v>
       </c>
       <c r="N43" s="7">
-        <v>670.11361546809076</v>
+        <v>680.11361546809076</v>
       </c>
       <c r="O43" s="7">
-        <v>642.18423800730307</v>
+        <v>622.18423800730307</v>
       </c>
       <c r="P43" s="7">
-        <v>624.63349614936851</v>
+        <v>604.63349614936851</v>
       </c>
       <c r="Q43" s="7">
-        <v>597.46479761471255</v>
+        <v>587.46479761471255</v>
       </c>
       <c r="R43" s="7">
         <v>589.56526463459522</v>
@@ -14160,7 +14160,7 @@
         <v>877.59290923231219</v>
       </c>
       <c r="AA43" s="8">
-        <v>996.46974541540294</v>
+        <v>915.06974541540285</v>
       </c>
       <c r="AB43" t="s">
         <v>15</v>
@@ -14178,58 +14178,58 @@
         <v>1820</v>
       </c>
       <c r="AH43" s="7">
-        <v>1444.6563686849986</v>
+        <v>1434.6563686849986</v>
       </c>
       <c r="AI43" s="7">
         <v>1428.7097160031635</v>
       </c>
       <c r="AJ43" s="7">
-        <v>1413.1595434471919</v>
+        <v>1423.1595434471919</v>
       </c>
       <c r="AK43" s="7">
-        <v>1378.0094193382165</v>
+        <v>1388.0094193382165</v>
       </c>
       <c r="AL43" s="7">
-        <v>1343.2629441122599</v>
+        <v>1353.2629441122599</v>
       </c>
       <c r="AM43" s="7">
-        <v>1308.9237506092695</v>
+        <v>1328.9237506092695</v>
       </c>
       <c r="AN43" s="7">
-        <v>1284.9955043647524</v>
+        <v>1294.9955043647524</v>
       </c>
       <c r="AO43" s="7">
-        <v>1261.4819039040349</v>
+        <v>1271.4819039040349</v>
       </c>
       <c r="AP43" s="7">
-        <v>1238.386681039171</v>
+        <v>1248.386681039171</v>
       </c>
       <c r="AQ43" s="7">
-        <v>1215.7136011685234</v>
+        <v>1225.7136011685234</v>
       </c>
       <c r="AR43" s="7">
-        <v>1193.4664635790396</v>
+        <v>1173.4664635790396</v>
       </c>
       <c r="AS43" s="7">
-        <v>1181.6491017512508</v>
+        <v>1161.6491017512508</v>
       </c>
       <c r="AT43" s="7">
-        <v>1303.8353836670103</v>
+        <v>1293.8353836670103</v>
       </c>
       <c r="AU43" s="7">
-        <v>1139.3192121200136</v>
+        <v>1149.3192121200136</v>
       </c>
       <c r="AV43" s="7">
-        <v>1128.8145250290936</v>
+        <v>1148.8145250290936</v>
       </c>
       <c r="AW43" s="7">
-        <v>1158.7552957543548</v>
+        <v>1178.7552957543548</v>
       </c>
       <c r="AX43" s="7">
-        <v>1189.1455334161437</v>
+        <v>1199.1455334161437</v>
       </c>
       <c r="AY43" s="7">
-        <v>1219.989283216888</v>
+        <v>1229.989283216888</v>
       </c>
       <c r="AZ43" s="7">
         <v>1221.2906267658391</v>
@@ -14238,7 +14238,7 @@
         <v>1241.4709459253852</v>
       </c>
       <c r="BB43" s="7">
-        <v>1819.9999999999998</v>
+        <v>1283.2540844387131</v>
       </c>
       <c r="BC43" s="7">
         <v>1325.4132711986604</v>
@@ -14280,10 +14280,10 @@
         <v>2600</v>
       </c>
       <c r="BQ43" s="7">
-        <v>2583.8061561222876</v>
+        <v>2600</v>
       </c>
       <c r="BR43" s="7">
-        <v>2572.6118515273865</v>
+        <v>2600</v>
       </c>
       <c r="BS43" s="7">
         <v>2600</v>
@@ -14292,19 +14292,19 @@
         <v>2600</v>
       </c>
       <c r="BU43" s="7">
-        <v>2552.2235412092268</v>
+        <v>2532.2235412092268</v>
       </c>
       <c r="BV43" s="7">
-        <v>2585.8049930801071</v>
+        <v>2600</v>
       </c>
       <c r="BW43" s="7">
-        <v>2534.6750080178281</v>
+        <v>2544.6750080178281</v>
       </c>
       <c r="BX43" s="7">
-        <v>2536.728523089987</v>
+        <v>2556.728523089987</v>
       </c>
       <c r="BY43" s="7">
-        <v>2579.3405197977972</v>
+        <v>2600</v>
       </c>
       <c r="BZ43" s="7">
         <v>2600</v>
@@ -14340,58 +14340,58 @@
         <v>1820</v>
       </c>
       <c r="CL43" s="7">
-        <v>1027.5954147109987</v>
+        <v>1017.5954147109987</v>
       </c>
       <c r="CM43" s="7">
         <v>1007.8952134433976</v>
       </c>
       <c r="CN43" s="7">
-        <v>988.55771036438728</v>
+        <v>998.55771036438728</v>
       </c>
       <c r="CO43" s="7">
-        <v>949.58616975766654</v>
+        <v>959.58616975766654</v>
       </c>
       <c r="CP43" s="7">
-        <v>910.98388528548548</v>
+        <v>920.98388528548548</v>
       </c>
       <c r="CQ43" s="7">
-        <v>872.75418025305407</v>
+        <v>892.75418025305407</v>
       </c>
       <c r="CR43" s="7">
-        <v>844.90040787533144</v>
+        <v>854.90040787533144</v>
       </c>
       <c r="CS43" s="7">
-        <v>817.42595154620903</v>
+        <v>827.42595154620903</v>
       </c>
       <c r="CT43" s="7">
-        <v>790.33422511012486</v>
+        <v>800.33422511012486</v>
       </c>
       <c r="CU43" s="7">
-        <v>763.62867313611514</v>
+        <v>773.62867313611514</v>
       </c>
       <c r="CV43" s="7">
-        <v>737.3127711943398</v>
+        <v>717.3127711943398</v>
       </c>
       <c r="CW43" s="7">
-        <v>721.39002613508819</v>
+        <v>701.39002613508819</v>
       </c>
       <c r="CX43" s="7">
-        <v>695.86397637030313</v>
+        <v>685.86397637030313</v>
       </c>
       <c r="CY43" s="7">
-        <v>670.73819215763524</v>
+        <v>680.73819215763524</v>
       </c>
       <c r="CZ43" s="7">
-        <v>659.84102070964309</v>
+        <v>676.01627588705378</v>
       </c>
       <c r="DA43" s="7">
-        <v>696.38948989602954</v>
+        <v>701.70186237003691</v>
       </c>
       <c r="DB43" s="7">
         <v>733.26689530509361</v>
       </c>
       <c r="DC43" s="7">
-        <v>770.47619736283923</v>
+        <v>770.47619736283878</v>
       </c>
       <c r="DD43" s="7">
         <v>808.02038313910339</v>
@@ -14423,46 +14423,46 @@
         <v>0</v>
       </c>
       <c r="E44" s="7">
-        <v>3150</v>
+        <v>3160</v>
       </c>
       <c r="F44" s="7">
         <v>3210</v>
       </c>
       <c r="G44" s="7">
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="H44" s="7">
-        <v>3350</v>
+        <v>3340</v>
       </c>
       <c r="I44" s="7">
-        <v>3430</v>
+        <v>3420</v>
       </c>
       <c r="J44" s="7">
-        <v>3510</v>
+        <v>3490</v>
       </c>
       <c r="K44" s="7">
-        <v>3580</v>
+        <v>3570</v>
       </c>
       <c r="L44" s="7">
-        <v>3650</v>
+        <v>3640</v>
       </c>
       <c r="M44" s="7">
-        <v>3720</v>
+        <v>3710</v>
       </c>
       <c r="N44" s="7">
-        <v>3790</v>
+        <v>3780</v>
       </c>
       <c r="O44" s="7">
-        <v>3860</v>
+        <v>3880</v>
       </c>
       <c r="P44" s="7">
-        <v>3920</v>
+        <v>3940</v>
       </c>
       <c r="Q44" s="7">
-        <v>3990</v>
+        <v>4000</v>
       </c>
       <c r="R44" s="7">
-        <v>4060</v>
+        <v>4050</v>
       </c>
       <c r="S44" s="7">
         <v>4049.8374630040767</v>
@@ -14489,7 +14489,7 @@
         <v>4143.5732273080785</v>
       </c>
       <c r="AA44" s="8">
-        <v>4152.9424363538501</v>
+        <v>4152.942436353851</v>
       </c>
       <c r="AB44" t="s">
         <v>16</v>
@@ -14507,67 +14507,67 @@
         <v>0</v>
       </c>
       <c r="AH44" s="7">
-        <v>3150</v>
+        <v>3160</v>
       </c>
       <c r="AI44" s="7">
         <v>3210</v>
       </c>
       <c r="AJ44" s="7">
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="AK44" s="7">
-        <v>3350</v>
+        <v>3340</v>
       </c>
       <c r="AL44" s="7">
-        <v>3430</v>
+        <v>3420</v>
       </c>
       <c r="AM44" s="7">
-        <v>3510</v>
+        <v>3490</v>
       </c>
       <c r="AN44" s="7">
-        <v>3580</v>
+        <v>3570</v>
       </c>
       <c r="AO44" s="7">
-        <v>3650</v>
+        <v>3640</v>
       </c>
       <c r="AP44" s="7">
-        <v>3720</v>
+        <v>3710</v>
       </c>
       <c r="AQ44" s="7">
-        <v>3790</v>
+        <v>3780</v>
       </c>
       <c r="AR44" s="7">
-        <v>3860</v>
+        <v>3880</v>
       </c>
       <c r="AS44" s="7">
-        <v>3920</v>
+        <v>3940</v>
       </c>
       <c r="AT44" s="7">
-        <v>3990</v>
+        <v>4000</v>
       </c>
       <c r="AU44" s="7">
-        <v>4060</v>
+        <v>4050</v>
       </c>
       <c r="AV44" s="7">
+        <v>4100</v>
+      </c>
+      <c r="AW44" s="7">
         <v>4120</v>
       </c>
-      <c r="AW44" s="7">
-        <v>4140</v>
-      </c>
       <c r="AX44" s="7">
-        <v>4160</v>
+        <v>4150</v>
       </c>
       <c r="AY44" s="7">
-        <v>4180</v>
+        <v>4170</v>
       </c>
       <c r="AZ44" s="7">
         <v>4230</v>
       </c>
       <c r="BA44" s="7">
-        <v>4280</v>
+        <v>4290</v>
       </c>
       <c r="BB44" s="7">
-        <v>3777.9126055483912</v>
+        <v>4314.6585211096781</v>
       </c>
       <c r="BC44" s="7">
         <v>4325.1983177996653</v>
@@ -14588,64 +14588,64 @@
         <v>0</v>
       </c>
       <c r="BJ44" s="7">
-        <v>3150</v>
+        <v>3160</v>
       </c>
       <c r="BK44" s="7">
         <v>3210</v>
       </c>
       <c r="BL44" s="7">
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="BM44" s="7">
-        <v>3350</v>
+        <v>3340</v>
       </c>
       <c r="BN44" s="7">
-        <v>3430</v>
+        <v>3420</v>
       </c>
       <c r="BO44" s="7">
-        <v>3510</v>
+        <v>3490</v>
       </c>
       <c r="BP44" s="7">
-        <v>3575.5249912014751</v>
+        <v>3570</v>
       </c>
       <c r="BQ44" s="7">
-        <v>3650</v>
+        <v>3633.8061561222876</v>
       </c>
       <c r="BR44" s="7">
-        <v>3720</v>
+        <v>3692.6118515273865</v>
       </c>
       <c r="BS44" s="7">
-        <v>3790</v>
+        <v>3780</v>
       </c>
       <c r="BT44" s="7">
         <v>3811.8157593748529</v>
       </c>
       <c r="BU44" s="7">
-        <v>3920</v>
+        <v>3940</v>
       </c>
       <c r="BV44" s="7">
-        <v>3990</v>
+        <v>4000</v>
       </c>
       <c r="BW44" s="7">
-        <v>4060</v>
+        <v>4050</v>
       </c>
       <c r="BX44" s="7">
-        <v>4120</v>
+        <v>4100</v>
       </c>
       <c r="BY44" s="7">
-        <v>4140</v>
+        <v>4119.3405197977972</v>
       </c>
       <c r="BZ44" s="7">
-        <v>4160</v>
+        <v>4150</v>
       </c>
       <c r="CA44" s="7">
-        <v>4180</v>
+        <v>4170</v>
       </c>
       <c r="CB44" s="7">
         <v>4230</v>
       </c>
       <c r="CC44" s="7">
-        <v>4280</v>
+        <v>4290</v>
       </c>
       <c r="CD44" s="7">
         <v>4350</v>
@@ -14654,7 +14654,7 @@
         <v>4420</v>
       </c>
       <c r="CF44" s="8">
-        <v>4560</v>
+        <v>4540</v>
       </c>
       <c r="CH44">
         <v>42</v>
@@ -14669,58 +14669,58 @@
         <v>0</v>
       </c>
       <c r="CL44" s="7">
-        <v>3150</v>
+        <v>3160</v>
       </c>
       <c r="CM44" s="7">
         <v>3210</v>
       </c>
       <c r="CN44" s="7">
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="CO44" s="7">
-        <v>3350</v>
+        <v>3340</v>
       </c>
       <c r="CP44" s="7">
-        <v>3430</v>
+        <v>3420</v>
       </c>
       <c r="CQ44" s="7">
-        <v>3510</v>
+        <v>3490</v>
       </c>
       <c r="CR44" s="7">
-        <v>3580</v>
+        <v>3570</v>
       </c>
       <c r="CS44" s="7">
-        <v>3650</v>
+        <v>3640</v>
       </c>
       <c r="CT44" s="7">
-        <v>3720</v>
+        <v>3710</v>
       </c>
       <c r="CU44" s="7">
-        <v>3790</v>
+        <v>3780</v>
       </c>
       <c r="CV44" s="7">
-        <v>3860</v>
+        <v>3880</v>
       </c>
       <c r="CW44" s="7">
-        <v>3920</v>
+        <v>3940</v>
       </c>
       <c r="CX44" s="7">
-        <v>3990</v>
+        <v>4000</v>
       </c>
       <c r="CY44" s="7">
-        <v>4060</v>
+        <v>4050</v>
       </c>
       <c r="CZ44" s="7">
-        <v>4116.1752551774107</v>
+        <v>4100</v>
       </c>
       <c r="DA44" s="7">
-        <v>4140</v>
+        <v>4120</v>
       </c>
       <c r="DB44" s="7">
-        <v>4160</v>
+        <v>4150</v>
       </c>
       <c r="DC44" s="7">
-        <v>4143.8340493407095</v>
+        <v>4143.8340493407104</v>
       </c>
       <c r="DD44" s="7">
         <v>4195.8500957847764</v>
@@ -16205,10 +16205,10 @@
         <v>56.430245863705181</v>
       </c>
       <c r="AU51" s="7">
-        <v>73.107518076478414</v>
+        <v>73.107518076478073</v>
       </c>
       <c r="AV51" s="7">
-        <v>89.934885739166702</v>
+        <v>89.934885739166475</v>
       </c>
       <c r="AW51" s="7">
         <v>106.91369971081872</v>
@@ -16223,7 +16223,7 @@
         <v>0</v>
       </c>
       <c r="BA51" s="7">
-        <v>0</v>
+        <v>6.9145681533159404</v>
       </c>
       <c r="BB51" s="7">
         <v>58.036199266695803</v>
@@ -16232,7 +16232,7 @@
         <v>119.07792506009628</v>
       </c>
       <c r="BD51" s="8">
-        <v>230.12194722872619</v>
+        <v>230.03902638563659</v>
       </c>
       <c r="BF51">
         <v>2</v>
@@ -16253,28 +16253,28 @@
         <v>280.10920524321841</v>
       </c>
       <c r="BL51" s="7">
-        <v>298.79958809040727</v>
+        <v>284.98208115821672</v>
       </c>
       <c r="BM51" s="7">
-        <v>317.65818438322026</v>
+        <v>307.49752105780635</v>
       </c>
       <c r="BN51" s="7">
         <v>336.6865080426694</v>
       </c>
       <c r="BO51" s="7">
-        <v>355.88608661505327</v>
+        <v>319.53227291711937</v>
       </c>
       <c r="BP51" s="7">
-        <v>375.25846139458849</v>
+        <v>375.25846139458815</v>
       </c>
       <c r="BQ51" s="7">
-        <v>394.80518754713955</v>
+        <v>381.62214902168034</v>
       </c>
       <c r="BR51" s="7">
-        <v>414.52783423506366</v>
+        <v>394.26340819798224</v>
       </c>
       <c r="BS51" s="7">
-        <v>434.42798474317897</v>
+        <v>423.9673832757012</v>
       </c>
       <c r="BT51" s="7">
         <v>454.50723660586732</v>
@@ -16286,25 +16286,25 @@
         <v>495.20950655093725</v>
       </c>
       <c r="BW51" s="7">
-        <v>515.83579210989569</v>
+        <v>515.83579210989524</v>
       </c>
       <c r="BX51" s="7">
-        <v>536.64771423888419</v>
+        <v>483.55911460638026</v>
       </c>
       <c r="BY51" s="7">
-        <v>335.96508679719312</v>
+        <v>253.94253172138633</v>
       </c>
       <c r="BZ51" s="7">
-        <v>268.15254289301748</v>
+        <v>298.07317731451894</v>
       </c>
       <c r="CA51" s="7">
-        <v>488.01190916595169</v>
+        <v>521.53843833266228</v>
       </c>
       <c r="CB51" s="7">
-        <v>559.72204143410488</v>
+        <v>539.70566144043153</v>
       </c>
       <c r="CC51" s="7">
-        <v>665.6</v>
+        <v>614.74124319010525</v>
       </c>
       <c r="CD51" s="7">
         <v>665.6</v>
@@ -16740,22 +16740,22 @@
         <v>0</v>
       </c>
       <c r="F53" s="7">
-        <v>59.941662939991829</v>
+        <v>212</v>
       </c>
       <c r="G53" s="7">
-        <v>203.27894998393339</v>
+        <v>212</v>
       </c>
       <c r="H53" s="7">
         <v>212</v>
       </c>
       <c r="I53" s="7">
-        <v>195.57185514423463</v>
+        <v>208.33664834322053</v>
       </c>
       <c r="J53" s="7">
-        <v>156.15514273469071</v>
+        <v>212</v>
       </c>
       <c r="K53" s="7">
-        <v>180.73800643552298</v>
+        <v>212</v>
       </c>
       <c r="L53" s="7">
         <v>212</v>
@@ -16767,28 +16767,28 @@
         <v>212</v>
       </c>
       <c r="O53" s="7">
-        <v>212</v>
+        <v>89.910992931415421</v>
       </c>
       <c r="P53" s="7">
-        <v>212</v>
+        <v>104.98159186779844</v>
       </c>
       <c r="Q53" s="7">
-        <v>187.36956548652051</v>
+        <v>120.18782619460808</v>
       </c>
       <c r="R53" s="7">
-        <v>146.88587473854693</v>
+        <v>135.53091663035912</v>
       </c>
       <c r="S53" s="7">
-        <v>151.01209488003258</v>
+        <v>154.43023720008114</v>
       </c>
       <c r="T53" s="7">
-        <v>166.63260373395269</v>
+        <v>173.48150933488159</v>
       </c>
       <c r="U53" s="7">
-        <v>182.39369716755823</v>
+        <v>182.88424291889532</v>
       </c>
       <c r="V53" s="7">
-        <v>198.29664044206618</v>
+        <v>202.64160110516514</v>
       </c>
       <c r="W53" s="7">
         <v>212</v>
@@ -16818,7 +16818,7 @@
         <v>212</v>
       </c>
       <c r="AH53" s="7">
-        <v>212</v>
+        <v>79.534840979999331</v>
       </c>
       <c r="AI53" s="7">
         <v>212</v>
@@ -16980,49 +16980,49 @@
         <v>212</v>
       </c>
       <c r="CL53" s="7">
-        <v>122.02341423766984</v>
+        <v>130.64083692929626</v>
       </c>
       <c r="CM53" s="7">
-        <v>212</v>
+        <v>14.490785249118517</v>
       </c>
       <c r="CN53" s="7">
         <v>212</v>
       </c>
       <c r="CO53" s="7">
-        <v>200.77401689151725</v>
+        <v>212</v>
       </c>
       <c r="CP53" s="7">
-        <v>201.25772080142997</v>
+        <v>212</v>
       </c>
       <c r="CQ53" s="7">
         <v>212</v>
       </c>
       <c r="CR53" s="7">
+        <v>208.45848269935072</v>
+      </c>
+      <c r="CS53" s="7">
         <v>212</v>
       </c>
-      <c r="CS53" s="7">
-        <v>195.84215296768775</v>
-      </c>
       <c r="CT53" s="7">
-        <v>200.61744941421762</v>
+        <v>212</v>
       </c>
       <c r="CU53" s="7">
-        <v>189.70727471940432</v>
+        <v>212</v>
       </c>
       <c r="CV53" s="7">
-        <v>162.20365213587718</v>
+        <v>127.32454040853531</v>
       </c>
       <c r="CW53" s="7">
-        <v>189.45620894095509</v>
+        <v>141.3960855429965</v>
       </c>
       <c r="CX53" s="7">
-        <v>170.7578206180182</v>
+        <v>147.88367000003342</v>
       </c>
       <c r="CY53" s="7">
-        <v>160.46035020471277</v>
+        <v>209.94399899041744</v>
       </c>
       <c r="CZ53" s="7">
-        <v>188.18530023208612</v>
+        <v>212</v>
       </c>
       <c r="DA53" s="7">
         <v>212</v>
@@ -17282,16 +17282,16 @@
         <v>0</v>
       </c>
       <c r="CC54" s="7">
-        <v>3.4694567661127991</v>
+        <v>0</v>
       </c>
       <c r="CD54" s="7">
-        <v>90.180663822496726</v>
+        <v>72.510690090155904</v>
       </c>
       <c r="CE54" s="7">
-        <v>172.8651409528257</v>
+        <v>156.14832801154375</v>
       </c>
       <c r="CF54" s="8">
-        <v>94.374218314002064</v>
+        <v>114.37421831400206</v>
       </c>
       <c r="CH54">
         <v>5</v>
@@ -18505,7 +18505,7 @@
         <v>317.5450221870542</v>
       </c>
       <c r="BA58" s="7">
-        <v>355.8271592334213</v>
+        <v>338.91259108010536</v>
       </c>
       <c r="BB58" s="7">
         <v>272.18280439982573</v>
@@ -18514,7 +18514,7 @@
         <v>185.93244963942379</v>
       </c>
       <c r="BD58" s="8">
-        <v>0</v>
+        <v>0.16584168617919204</v>
       </c>
       <c r="BF58">
         <v>9</v>
@@ -18535,28 +18535,28 @@
         <v>0</v>
       </c>
       <c r="BL58" s="7">
-        <v>0</v>
+        <v>27.635013864381108</v>
       </c>
       <c r="BM58" s="7">
-        <v>0</v>
+        <v>20.321326650828269</v>
       </c>
       <c r="BN58" s="7">
         <v>0</v>
       </c>
       <c r="BO58" s="7">
-        <v>0</v>
+        <v>72.707627395867348</v>
       </c>
       <c r="BP58" s="7">
         <v>0</v>
       </c>
       <c r="BQ58" s="7">
-        <v>0</v>
+        <v>26.36607705091842</v>
       </c>
       <c r="BR58" s="7">
-        <v>0</v>
+        <v>40.528852074162842</v>
       </c>
       <c r="BS58" s="7">
-        <v>0</v>
+        <v>20.921202934955545</v>
       </c>
       <c r="BT58" s="7">
         <v>0</v>
@@ -18571,10 +18571,10 @@
         <v>0</v>
       </c>
       <c r="BX58" s="7">
-        <v>0</v>
+        <v>106.17719926500831</v>
       </c>
       <c r="BY58" s="7">
-        <v>443.36371373968188</v>
+        <v>607.40882389129547</v>
       </c>
       <c r="BZ58" s="7">
         <v>650</v>
@@ -20987,34 +20987,34 @@
         <v>257</v>
       </c>
       <c r="I66" s="7">
-        <v>257</v>
+        <v>254.2352068010141</v>
       </c>
       <c r="J66" s="7">
-        <v>252.12125910584163</v>
+        <v>216.27640184053234</v>
       </c>
       <c r="K66" s="7">
-        <v>193.56428302157335</v>
+        <v>172.30228945709632</v>
       </c>
       <c r="L66" s="7">
-        <v>128.65241006221004</v>
+        <v>138.65241006221004</v>
       </c>
       <c r="M66" s="7">
-        <v>95.329681752769375</v>
+        <v>105.32968175276937</v>
       </c>
       <c r="N66" s="7">
-        <v>62.33704888854345</v>
+        <v>72.33704888854345</v>
       </c>
       <c r="O66" s="7">
-        <v>29.677482328540009</v>
+        <v>131.76648939712413</v>
       </c>
       <c r="P66" s="7">
-        <v>7.3539796694963115</v>
+        <v>94.372387801697414</v>
       </c>
       <c r="Q66" s="7">
-        <v>0</v>
+        <v>57.181739291912436</v>
       </c>
       <c r="R66" s="7">
-        <v>8.8414168373516304</v>
+        <v>30.196374945539446</v>
       </c>
       <c r="S66" s="7">
         <v>0</v>
@@ -21095,19 +21095,19 @@
         <v>257</v>
       </c>
       <c r="AU66" s="7">
-        <v>244.56127711471697</v>
+        <v>254.56127711471731</v>
       </c>
       <c r="AV66" s="7">
-        <v>209.80232860874935</v>
+        <v>229.80232860874958</v>
       </c>
       <c r="AW66" s="7">
-        <v>215.27054956622783</v>
+        <v>235.27054956622783</v>
       </c>
       <c r="AX66" s="7">
-        <v>96.922661504107964</v>
+        <v>106.92266150410796</v>
       </c>
       <c r="AY66" s="7">
-        <v>85.565565457644652</v>
+        <v>95.565565457644652</v>
       </c>
       <c r="AZ66" s="7">
         <v>44.286255546763641</v>
@@ -21194,13 +21194,13 @@
         <v>257</v>
       </c>
       <c r="CC66" s="7">
-        <v>204.70773844381245</v>
+        <v>249.03595201982034</v>
       </c>
       <c r="CD66" s="7">
-        <v>102.89992614431721</v>
+        <v>120.56989987665803</v>
       </c>
       <c r="CE66" s="7">
-        <v>5.6129743236878795</v>
+        <v>22.329787264969823</v>
       </c>
       <c r="CF66" s="8">
         <v>0</v>
@@ -21233,43 +21233,43 @@
         <v>257</v>
       </c>
       <c r="CQ66" s="7">
-        <v>254.28910331648103</v>
+        <v>257</v>
       </c>
       <c r="CR66" s="7">
-        <v>220.83710524632943</v>
+        <v>234.3786225469787</v>
       </c>
       <c r="CS66" s="7">
-        <v>203.87188622585813</v>
+        <v>197.71403919354589</v>
       </c>
       <c r="CT66" s="7">
-        <v>166.30541613206947</v>
+        <v>164.92286554628708</v>
       </c>
       <c r="CU66" s="7">
-        <v>144.75929661679851</v>
+        <v>132.46657133620329</v>
       </c>
       <c r="CV66" s="7">
-        <v>140.14451834235081</v>
+        <v>155.02363006969267</v>
       </c>
       <c r="CW66" s="7">
-        <v>91.114495071576584</v>
+        <v>119.17461846953518</v>
       </c>
       <c r="CX66" s="7">
-        <v>78.379419730625699</v>
+        <v>91.253570348610481</v>
       </c>
       <c r="CY66" s="7">
-        <v>57.590525307068901</v>
+        <v>18.106876521364228</v>
       </c>
       <c r="CZ66" s="7">
-        <v>9.1294331593014419</v>
+        <v>5.3147333913875627</v>
       </c>
       <c r="DA66" s="7">
-        <v>4.9319659919092373</v>
+        <v>24.931965991909237</v>
       </c>
       <c r="DB66" s="7">
-        <v>24.905753685836316</v>
+        <v>34.905753685836316</v>
       </c>
       <c r="DC66" s="7">
-        <v>20.967861093801275</v>
+        <v>30.967861093801275</v>
       </c>
       <c r="DD66" s="7">
         <v>0</v>
@@ -21301,16 +21301,16 @@
         <v>1924.1698059999994</v>
       </c>
       <c r="E67" s="7">
-        <v>335.91013425399888</v>
+        <v>325.91013425399888</v>
       </c>
       <c r="F67" s="7">
-        <v>250.4160625222928</v>
+        <v>98.357725462284634</v>
       </c>
       <c r="G67" s="7">
-        <v>81.836395007511626</v>
+        <v>83.115344991444999</v>
       </c>
       <c r="H67" s="7">
-        <v>28.185783096367231</v>
+        <v>38.185783096367231</v>
       </c>
       <c r="I67" s="7">
         <v>0</v>
@@ -21382,43 +21382,43 @@
         <v>2254.028049999999</v>
       </c>
       <c r="AH67" s="7">
-        <v>456.73710244999847</v>
+        <v>579.20226146999914</v>
       </c>
       <c r="AI67" s="7">
         <v>434.18013637204831</v>
       </c>
       <c r="AJ67" s="7">
-        <v>411.9601575993961</v>
+        <v>421.9601575993961</v>
       </c>
       <c r="AK67" s="7">
-        <v>370.08019901779016</v>
+        <v>380.08019901779016</v>
       </c>
       <c r="AL67" s="7">
-        <v>328.54332080895028</v>
+        <v>338.54332080895028</v>
       </c>
       <c r="AM67" s="7">
-        <v>287.35261069623039</v>
+        <v>307.35261069623039</v>
       </c>
       <c r="AN67" s="7">
-        <v>256.51118419249588</v>
+        <v>266.51118419249588</v>
       </c>
       <c r="AO67" s="7">
-        <v>226.02218485022786</v>
+        <v>236.02218485022786</v>
       </c>
       <c r="AP67" s="7">
-        <v>195.88878451387973</v>
+        <v>205.88878451387973</v>
       </c>
       <c r="AQ67" s="7">
-        <v>158.82851014470225</v>
+        <v>168.82851014470225</v>
       </c>
       <c r="AR67" s="7">
-        <v>113.18096673600417</v>
+        <v>93.180966736004166</v>
       </c>
       <c r="AS67" s="7">
-        <v>77.752595436627985</v>
+        <v>57.752595436627985</v>
       </c>
       <c r="AT67" s="7">
-        <v>32.545368795557465</v>
+        <v>22.545368795557465</v>
       </c>
       <c r="AU67" s="7">
         <v>0</v>
@@ -21463,61 +21463,61 @@
         <v>2269.6</v>
       </c>
       <c r="BJ67" s="7">
-        <v>1180.2783031365987</v>
+        <v>1170.2783031365987</v>
       </c>
       <c r="BK67" s="7">
         <v>1148.0638078648274</v>
       </c>
       <c r="BL67" s="7">
-        <v>1116.0993821356105</v>
+        <v>1112.28187520342</v>
       </c>
       <c r="BM67" s="7">
-        <v>1064.3872765748308</v>
+        <v>1064.2266132494165</v>
       </c>
       <c r="BN67" s="7">
-        <v>1012.9297620640039</v>
+        <v>1022.9297620640039</v>
       </c>
       <c r="BO67" s="7">
-        <v>961.7291299225792</v>
+        <v>945.37531622464576</v>
       </c>
       <c r="BP67" s="7">
-        <v>920.78769209188226</v>
+        <v>930.7876920918826</v>
       </c>
       <c r="BQ67" s="7">
-        <v>880.10778132070902</v>
+        <v>876.92474279524981</v>
       </c>
       <c r="BR67" s="7">
-        <v>839.69175135259525</v>
+        <v>829.42732531551383</v>
       </c>
       <c r="BS67" s="7">
-        <v>799.54197711476809</v>
+        <v>799.08137564729032</v>
       </c>
       <c r="BT67" s="7">
-        <v>759.66085490880073</v>
+        <v>739.66085490880073</v>
       </c>
       <c r="BU67" s="7">
-        <v>730.05080260297927</v>
+        <v>710.05080260297927</v>
       </c>
       <c r="BV67" s="7">
-        <v>690.71425982640562</v>
+        <v>680.71425982640562</v>
       </c>
       <c r="BW67" s="7">
-        <v>651.65368816484283</v>
+        <v>661.65368816484329</v>
       </c>
       <c r="BX67" s="7">
-        <v>622.87157135832672</v>
+        <v>589.78297172582234</v>
       </c>
       <c r="BY67" s="7">
-        <v>412.68855863070974</v>
+        <v>350.666003554903</v>
       </c>
       <c r="BZ67" s="7">
-        <v>306.83537250707531</v>
+        <v>286.91473808557384</v>
       </c>
       <c r="CA67" s="7">
-        <v>120.4232974727411</v>
+        <v>96.896768306030481</v>
       </c>
       <c r="CB67" s="7">
-        <v>52.641482064334582</v>
+        <v>72.657862058007936</v>
       </c>
       <c r="CC67" s="7">
         <v>0</v>
@@ -21544,22 +21544,22 @@
         <v>1979.1461799999993</v>
       </c>
       <c r="CL67" s="7">
-        <v>269.35788138232874</v>
+        <v>250.74045869070233</v>
       </c>
       <c r="CM67" s="7">
-        <v>154.32812728057752</v>
+        <v>351.837342031459</v>
       </c>
       <c r="CN67" s="7">
-        <v>129.58948042610291</v>
+        <v>139.58948042610291</v>
       </c>
       <c r="CO67" s="7">
-        <v>96.394168858420244</v>
+        <v>95.168185749937493</v>
       </c>
       <c r="CP67" s="7">
-        <v>51.809378620256666</v>
+        <v>51.067099421686635</v>
       </c>
       <c r="CQ67" s="7">
-        <v>0</v>
+        <v>17.289103316481032</v>
       </c>
       <c r="CR67" s="7">
         <v>0</v>
@@ -29128,58 +29128,58 @@
         <v>0</v>
       </c>
       <c r="E91" s="7">
-        <v>3150</v>
+        <v>3160</v>
       </c>
       <c r="F91" s="7">
         <v>3210</v>
       </c>
       <c r="G91" s="7">
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="H91" s="7">
-        <v>3350</v>
+        <v>3340</v>
       </c>
       <c r="I91" s="7">
-        <v>3430</v>
+        <v>3420</v>
       </c>
       <c r="J91" s="7">
-        <v>3510</v>
+        <v>3490</v>
       </c>
       <c r="K91" s="7">
-        <v>3580</v>
+        <v>3570</v>
       </c>
       <c r="L91" s="7">
-        <v>3650</v>
+        <v>3640</v>
       </c>
       <c r="M91" s="7">
-        <v>3720</v>
+        <v>3710</v>
       </c>
       <c r="N91" s="7">
-        <v>3790</v>
+        <v>3780</v>
       </c>
       <c r="O91" s="7">
-        <v>3860</v>
+        <v>3880</v>
       </c>
       <c r="P91" s="7">
-        <v>3920</v>
+        <v>3940</v>
       </c>
       <c r="Q91" s="7">
-        <v>3990</v>
+        <v>4000</v>
       </c>
       <c r="R91" s="7">
-        <v>4060</v>
+        <v>4050</v>
       </c>
       <c r="S91" s="7">
-        <v>4103.4181423200489</v>
+        <v>4100</v>
       </c>
       <c r="T91" s="7">
-        <v>4126.8489056009294</v>
+        <v>4120</v>
       </c>
       <c r="U91" s="7">
-        <v>4150.4905457513369</v>
+        <v>4150</v>
       </c>
       <c r="V91" s="7">
-        <v>4174.3449606630993</v>
+        <v>4170</v>
       </c>
       <c r="W91" s="7">
         <v>4198.4140653090662</v>
@@ -29212,64 +29212,64 @@
         <v>0</v>
       </c>
       <c r="AH91" s="7">
-        <v>3150</v>
+        <v>3160</v>
       </c>
       <c r="AI91" s="7">
         <v>3210</v>
       </c>
       <c r="AJ91" s="7">
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="AK91" s="7">
-        <v>3350</v>
+        <v>3340</v>
       </c>
       <c r="AL91" s="7">
-        <v>3430</v>
+        <v>3420</v>
       </c>
       <c r="AM91" s="7">
-        <v>3510</v>
+        <v>3490</v>
       </c>
       <c r="AN91" s="7">
-        <v>3580</v>
+        <v>3570</v>
       </c>
       <c r="AO91" s="7">
-        <v>3650</v>
+        <v>3640</v>
       </c>
       <c r="AP91" s="7">
-        <v>3720</v>
+        <v>3710</v>
       </c>
       <c r="AQ91" s="7">
-        <v>3790</v>
+        <v>3780</v>
       </c>
       <c r="AR91" s="7">
-        <v>3860</v>
+        <v>3880</v>
       </c>
       <c r="AS91" s="7">
-        <v>3920</v>
+        <v>3940</v>
       </c>
       <c r="AT91" s="7">
-        <v>3990</v>
+        <v>4000</v>
       </c>
       <c r="AU91" s="7">
-        <v>4060</v>
+        <v>4050</v>
       </c>
       <c r="AV91" s="7">
+        <v>4100</v>
+      </c>
+      <c r="AW91" s="7">
         <v>4120</v>
       </c>
-      <c r="AW91" s="7">
-        <v>4140</v>
-      </c>
       <c r="AX91" s="7">
-        <v>4160</v>
+        <v>4150</v>
       </c>
       <c r="AY91" s="7">
-        <v>4180</v>
+        <v>4170</v>
       </c>
       <c r="AZ91" s="7">
         <v>4230</v>
       </c>
       <c r="BA91" s="7">
-        <v>4280</v>
+        <v>4290</v>
       </c>
       <c r="BB91" s="7">
         <v>4350</v>
@@ -29278,7 +29278,7 @@
         <v>4420</v>
       </c>
       <c r="BD91" s="8">
-        <v>4540.0829208430896</v>
+        <v>4540</v>
       </c>
       <c r="BF91">
         <v>42</v>
@@ -29293,64 +29293,64 @@
         <v>0</v>
       </c>
       <c r="BJ91" s="7">
-        <v>3150</v>
+        <v>3160</v>
       </c>
       <c r="BK91" s="7">
         <v>3210</v>
       </c>
       <c r="BL91" s="7">
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="BM91" s="7">
-        <v>3350</v>
+        <v>3340</v>
       </c>
       <c r="BN91" s="7">
-        <v>3430</v>
+        <v>3420</v>
       </c>
       <c r="BO91" s="7">
-        <v>3510</v>
+        <v>3490</v>
       </c>
       <c r="BP91" s="7">
-        <v>3580</v>
+        <v>3570</v>
       </c>
       <c r="BQ91" s="7">
-        <v>3650</v>
+        <v>3640</v>
       </c>
       <c r="BR91" s="7">
-        <v>3720</v>
+        <v>3710</v>
       </c>
       <c r="BS91" s="7">
-        <v>3790</v>
+        <v>3780</v>
       </c>
       <c r="BT91" s="7">
-        <v>3860</v>
+        <v>3880</v>
       </c>
       <c r="BU91" s="7">
-        <v>3920</v>
+        <v>3940</v>
       </c>
       <c r="BV91" s="7">
-        <v>3990</v>
+        <v>4000</v>
       </c>
       <c r="BW91" s="7">
-        <v>4060</v>
+        <v>4050</v>
       </c>
       <c r="BX91" s="7">
+        <v>4100</v>
+      </c>
+      <c r="BY91" s="7">
         <v>4120</v>
       </c>
-      <c r="BY91" s="7">
-        <v>4140</v>
-      </c>
       <c r="BZ91" s="7">
-        <v>4160</v>
+        <v>4150</v>
       </c>
       <c r="CA91" s="7">
-        <v>4180</v>
+        <v>4170</v>
       </c>
       <c r="CB91" s="7">
         <v>4230</v>
       </c>
       <c r="CC91" s="7">
-        <v>4280</v>
+        <v>4290</v>
       </c>
       <c r="CD91" s="7">
         <v>4350</v>
@@ -29359,7 +29359,7 @@
         <v>4420</v>
       </c>
       <c r="CF91" s="8">
-        <v>4560</v>
+        <v>4540</v>
       </c>
       <c r="CH91">
         <v>42</v>
@@ -29374,58 +29374,58 @@
         <v>0</v>
       </c>
       <c r="CL91" s="7">
-        <v>3150</v>
+        <v>3160</v>
       </c>
       <c r="CM91" s="7">
         <v>3210</v>
       </c>
       <c r="CN91" s="7">
-        <v>3270</v>
+        <v>3260</v>
       </c>
       <c r="CO91" s="7">
-        <v>3350</v>
+        <v>3340</v>
       </c>
       <c r="CP91" s="7">
-        <v>3430</v>
+        <v>3420</v>
       </c>
       <c r="CQ91" s="7">
-        <v>3510</v>
+        <v>3490</v>
       </c>
       <c r="CR91" s="7">
-        <v>3580</v>
+        <v>3570</v>
       </c>
       <c r="CS91" s="7">
-        <v>3650</v>
+        <v>3640</v>
       </c>
       <c r="CT91" s="7">
-        <v>3720</v>
+        <v>3710</v>
       </c>
       <c r="CU91" s="7">
-        <v>3790</v>
+        <v>3780</v>
       </c>
       <c r="CV91" s="7">
-        <v>3860</v>
+        <v>3880</v>
       </c>
       <c r="CW91" s="7">
-        <v>3920</v>
+        <v>3940</v>
       </c>
       <c r="CX91" s="7">
-        <v>3990</v>
+        <v>4000</v>
       </c>
       <c r="CY91" s="7">
-        <v>4060</v>
+        <v>4050</v>
       </c>
       <c r="CZ91" s="7">
+        <v>4100</v>
+      </c>
+      <c r="DA91" s="7">
         <v>4120</v>
       </c>
-      <c r="DA91" s="7">
-        <v>4140</v>
-      </c>
       <c r="DB91" s="7">
-        <v>4160</v>
+        <v>4150</v>
       </c>
       <c r="DC91" s="7">
-        <v>4180</v>
+        <v>4170</v>
       </c>
       <c r="DD91" s="7">
         <v>4230</v>
@@ -30140,43 +30140,43 @@
         <v>176.4054711</v>
       </c>
       <c r="E97" s="4">
-        <v>194.17001222590034</v>
+        <v>197.50334555923365</v>
       </c>
       <c r="F97" s="4">
         <v>205.76089233593362</v>
       </c>
       <c r="G97" s="4">
-        <v>217.27609036695708</v>
+        <v>213.94275703362374</v>
       </c>
       <c r="H97" s="4">
-        <v>235.38159184692645</v>
+        <v>232.04825851359311</v>
       </c>
       <c r="I97" s="4">
-        <v>253.41004284021557</v>
+        <v>250.07670950688225</v>
       </c>
       <c r="J97" s="4">
-        <v>271.36074989244418</v>
+        <v>264.69408322577749</v>
       </c>
       <c r="K97" s="4">
-        <v>285.89967997480971</v>
+        <v>282.56634664147634</v>
       </c>
       <c r="L97" s="4">
-        <v>300.35946042791625</v>
+        <v>297.02612709458288</v>
       </c>
       <c r="M97" s="4">
-        <v>314.73937890510075</v>
+        <v>311.40604557176772</v>
       </c>
       <c r="N97" s="4">
-        <v>329.03871664858036</v>
+        <v>325.70538331524705</v>
       </c>
       <c r="O97" s="4">
-        <v>343.25674843175108</v>
+        <v>349.92341509841776</v>
       </c>
       <c r="P97" s="4">
-        <v>354.05940916763677</v>
+        <v>360.72607583430346</v>
       </c>
       <c r="Q97" s="4">
-        <v>368.11262718347899</v>
+        <v>371.44596051681231</v>
       </c>
       <c r="R97" s="4">
         <v>375.78776288101335</v>
@@ -30221,67 +30221,67 @@
         <v>73.238195916666342</v>
       </c>
       <c r="AH97" s="4">
-        <v>99.379786784917087</v>
+        <v>102.71312011825042</v>
       </c>
       <c r="AI97" s="4">
         <v>109.83489486598137</v>
       </c>
       <c r="AJ97" s="4">
-        <v>120.20409891977511</v>
+        <v>116.87076558644176</v>
       </c>
       <c r="AK97" s="4">
-        <v>137.1532924767198</v>
+        <v>133.81995914338646</v>
       </c>
       <c r="AL97" s="4">
-        <v>154.01502877567705</v>
+        <v>150.68169544234371</v>
       </c>
       <c r="AM97" s="4">
-        <v>170.78852070132513</v>
+        <v>164.12185403465847</v>
       </c>
       <c r="AN97" s="4">
-        <v>184.13964072097048</v>
+        <v>180.80630738763716</v>
       </c>
       <c r="AO97" s="4">
-        <v>197.40092082079246</v>
+        <v>194.06758748745915</v>
       </c>
       <c r="AP97" s="4">
-        <v>210.57155244151309</v>
+        <v>207.23821910817975</v>
       </c>
       <c r="AQ97" s="4">
-        <v>223.65071974681996</v>
+        <v>220.31738641348662</v>
       </c>
       <c r="AR97" s="4">
-        <v>236.63759955787478</v>
+        <v>243.30426622454144</v>
       </c>
       <c r="AS97" s="4">
-        <v>246.19802795389569</v>
+        <v>252.86469462056235</v>
       </c>
       <c r="AT97" s="4">
-        <v>163.28450020548144</v>
+        <v>166.61783353881475</v>
       </c>
       <c r="AU97" s="4">
-        <v>271.70283737399694</v>
+        <v>268.36950404066357</v>
       </c>
       <c r="AV97" s="4">
-        <v>280.97885291036312</v>
+        <v>274.31218624369649</v>
       </c>
       <c r="AW97" s="4">
-        <v>276.82501925322322</v>
+        <v>270.15835258655653</v>
       </c>
       <c r="AX97" s="4">
-        <v>272.57380109316892</v>
+        <v>269.24046775983561</v>
       </c>
       <c r="AY97" s="4">
-        <v>268.22432196967429</v>
+        <v>264.89098863634092</v>
       </c>
       <c r="AZ97" s="4">
-        <v>273.77569753406806</v>
+        <v>273.77569753406834</v>
       </c>
       <c r="BA97" s="4">
         <v>273.08794763899027</v>
       </c>
       <c r="BB97" s="4">
-        <v>86.338303980645748</v>
+        <v>265.25360916774139</v>
       </c>
       <c r="BC97" s="4">
         <v>257.34876165025116</v>
@@ -30302,64 +30302,64 @@
         <v>-43.161479033333663</v>
       </c>
       <c r="BJ97" s="4">
-        <v>-112.64202901130041</v>
+        <v>-115.3106833293012</v>
       </c>
       <c r="BK97" s="4">
         <v>-107.12349614593145</v>
       </c>
       <c r="BL97" s="4">
-        <v>-102.04595761124467</v>
+        <v>-98.712624277911345</v>
       </c>
       <c r="BM97" s="4">
-        <v>-103.40938789641282</v>
+        <v>-100.0760545630795</v>
       </c>
       <c r="BN97" s="4">
-        <v>-104.54508905414755</v>
+        <v>-101.21175572081422</v>
       </c>
       <c r="BO97" s="4">
-        <v>-105.45101152230161</v>
+        <v>-98.784344855634941</v>
       </c>
       <c r="BP97" s="4">
-        <v>-101.30008435982768</v>
+        <v>-99.458420626002706</v>
       </c>
       <c r="BQ97" s="4">
-        <v>-89.10266715982894</v>
+        <v>-94.500615119066424</v>
       </c>
       <c r="BR97" s="4">
-        <v>-78.510567830933724</v>
+        <v>-87.639950655138207</v>
       </c>
       <c r="BS97" s="4">
-        <v>-68.033139608078571</v>
+        <v>-71.366472941411899</v>
       </c>
       <c r="BT97" s="4">
         <v>-73.732828072933586</v>
       </c>
       <c r="BU97" s="4">
-        <v>-50.759767261998832</v>
+        <v>-44.09310059533216</v>
       </c>
       <c r="BV97" s="4">
-        <v>-54.842581834023193</v>
+        <v>-51.509248500689864</v>
       </c>
       <c r="BW97" s="4">
-        <v>-30.624251737195966</v>
+        <v>-33.957585070529298</v>
       </c>
       <c r="BX97" s="4">
-        <v>-24.06918000283061</v>
+        <v>-30.735846669497278</v>
       </c>
       <c r="BY97" s="4">
-        <v>-30.968445956189193</v>
+        <v>-37.854939356923445</v>
       </c>
       <c r="BZ97" s="4">
-        <v>-22.979122319143773</v>
+        <v>-19.645788985810441</v>
       </c>
       <c r="CA97" s="4">
-        <v>-0.96095108668320484</v>
+        <v>2.3723822466501283</v>
       </c>
       <c r="CB97" s="4">
         <v>11.31538368686976</v>
       </c>
       <c r="CC97" s="4">
-        <v>23.852205473384476</v>
+        <v>20.51887214005129</v>
       </c>
       <c r="CD97" s="4">
         <v>29.985191989311033</v>
@@ -30368,7 +30368,7 @@
         <v>36.383375383881685</v>
       </c>
       <c r="CF97" s="5">
-        <v>19.715809095668948</v>
+        <v>26.382475762335616</v>
       </c>
       <c r="CH97" s="1" t="s">
         <v>1</v>
@@ -30383,52 +30383,52 @@
         <v>25.015092549999924</v>
       </c>
       <c r="CL97" s="4">
-        <v>189.74299347928368</v>
+        <v>193.07632681261703</v>
       </c>
       <c r="CM97" s="4">
         <v>201.01137042059742</v>
       </c>
       <c r="CN97" s="4">
-        <v>212.20116275438278</v>
+        <v>208.86782942104946</v>
       </c>
       <c r="CO97" s="4">
-        <v>229.97832988583906</v>
+        <v>226.64499655250575</v>
       </c>
       <c r="CP97" s="4">
-        <v>247.67549152147831</v>
+        <v>244.34215818814496</v>
       </c>
       <c r="CQ97" s="4">
-        <v>265.29192761183833</v>
+        <v>258.6252609451717</v>
       </c>
       <c r="CR97" s="4">
-        <v>279.49357829367841</v>
+        <v>276.16024496034504</v>
       </c>
       <c r="CS97" s="4">
-        <v>293.61304383165486</v>
+        <v>290.27971049832155</v>
       </c>
       <c r="CT97" s="4">
-        <v>307.649584559473</v>
+        <v>304.31625122613968</v>
       </c>
       <c r="CU97" s="4">
-        <v>321.60245415384179</v>
+        <v>318.26912082050842</v>
       </c>
       <c r="CV97" s="4">
-        <v>335.47089957455984</v>
+        <v>342.13756624122652</v>
       </c>
       <c r="CW97" s="4">
-        <v>345.920827670731</v>
+        <v>352.58749433739769</v>
       </c>
       <c r="CX97" s="4">
-        <v>359.61813845310081</v>
+        <v>362.95147178643413</v>
       </c>
       <c r="CY97" s="4">
-        <v>373.22872503251239</v>
+        <v>369.89539169917907</v>
       </c>
       <c r="CZ97" s="4">
-        <v>382.14355861694207</v>
+        <v>376.75180689113841</v>
       </c>
       <c r="DA97" s="4">
-        <v>375.29072064449451</v>
+        <v>373.51992981982522</v>
       </c>
       <c r="DB97" s="4">
         <v>368.37620713029514</v>
@@ -30466,43 +30466,43 @@
         <v>70.853452100000311</v>
       </c>
       <c r="E98" s="7">
-        <v>-932.64540060310048</v>
+        <v>-939.31206726976711</v>
       </c>
       <c r="F98" s="7">
         <v>-961.64885920852851</v>
       </c>
       <c r="G98" s="7">
-        <v>-990.55334894140549</v>
+        <v>-983.88668227473886</v>
       </c>
       <c r="H98" s="7">
-        <v>-1032.6913124152115</v>
+        <v>-1026.0246457485446</v>
       </c>
       <c r="I98" s="7">
-        <v>-1074.7285175602817</v>
+        <v>-1068.061850893615</v>
       </c>
       <c r="J98" s="7">
-        <v>-1116.6640575516578</v>
+        <v>-1103.3307242183246</v>
       </c>
       <c r="K98" s="7">
-        <v>-1151.8303507362893</v>
+        <v>-1145.1636840696228</v>
       </c>
       <c r="L98" s="7">
-        <v>-1186.8931405595827</v>
+        <v>-1180.2264738929161</v>
       </c>
       <c r="M98" s="7">
-        <v>-1221.8514954912855</v>
+        <v>-1215.1848288246194</v>
       </c>
       <c r="N98" s="7">
-        <v>-1256.7044756173743</v>
+        <v>-1250.0378089507076</v>
       </c>
       <c r="O98" s="7">
-        <v>-1291.4511325645976</v>
+        <v>-1304.7844658979311</v>
       </c>
       <c r="P98" s="7">
-        <v>-1319.4238427576788</v>
+        <v>-1332.7571760910123</v>
       </c>
       <c r="Q98" s="7">
-        <v>-1353.9549740091647</v>
+        <v>-1360.6216406758315</v>
       </c>
       <c r="R98" s="7">
         <v>-1375.7877628810134</v>
@@ -30547,58 +30547,58 @@
         <v>231.62021341666747</v>
       </c>
       <c r="AH98" s="7">
-        <v>-789.41202887258396</v>
+        <v>-796.07869553925059</v>
       </c>
       <c r="AI98" s="7">
         <v>-816.93024713243722</v>
       </c>
       <c r="AJ98" s="7">
-        <v>-844.33612935662882</v>
+        <v>-837.66946268996219</v>
       </c>
       <c r="AK98" s="7">
-        <v>-884.96199785417207</v>
+        <v>-878.29533118750544</v>
       </c>
       <c r="AL98" s="7">
-        <v>-925.47349916819314</v>
+        <v>-918.8068325015264</v>
       </c>
       <c r="AM98" s="7">
-        <v>-965.8696039940404</v>
+        <v>-952.53627066070715</v>
       </c>
       <c r="AN98" s="7">
-        <v>-999.48260709665362</v>
+        <v>-992.81594042998699</v>
       </c>
       <c r="AO98" s="7">
-        <v>-1032.9781272271903</v>
+        <v>-1026.3114605605235</v>
       </c>
       <c r="AP98" s="7">
-        <v>-1066.3551070389017</v>
+        <v>-1059.6884403722347</v>
       </c>
       <c r="AQ98" s="7">
-        <v>-1099.6124796689185</v>
+        <v>-1092.9458130022517</v>
       </c>
       <c r="AR98" s="7">
-        <v>-1132.7491686526055</v>
+        <v>-1146.082501985939</v>
       </c>
       <c r="AS98" s="7">
-        <v>-1159.097421170479</v>
+        <v>-1172.4307545038123</v>
       </c>
       <c r="AT98" s="7">
-        <v>-1144.1328079610139</v>
+        <v>-1150.7994746276806</v>
       </c>
       <c r="AU98" s="7">
-        <v>-1224.7575565659961</v>
+        <v>-1218.0908898993293</v>
       </c>
       <c r="AV98" s="7">
-        <v>-1250.7338845750903</v>
+        <v>-1237.4005512417571</v>
       </c>
       <c r="AW98" s="7">
-        <v>-1249.9173328695997</v>
+        <v>-1236.5839995362662</v>
       </c>
       <c r="AX98" s="7">
-        <v>-1248.9734321987594</v>
+        <v>-1242.3067655320926</v>
       </c>
       <c r="AY98" s="7">
-        <v>-1247.9010364218818</v>
+        <v>-1241.2343697552151</v>
       </c>
       <c r="AZ98" s="7">
         <v>-1266.6989890830123</v>
@@ -30607,7 +30607,7 @@
         <v>-1273.0879476389903</v>
       </c>
       <c r="BB98" s="7">
-        <v>-907.42299879354994</v>
+        <v>-1265.2536091677414</v>
       </c>
       <c r="BC98" s="7">
         <v>-1257.3487616502512</v>
@@ -30628,64 +30628,64 @@
         <v>279.79057396666752</v>
       </c>
       <c r="BJ98" s="7">
-        <v>-467.05904753429888</v>
+        <v>-469.7277018522999</v>
       </c>
       <c r="BK98" s="7">
         <v>-489.15590783563738</v>
       </c>
       <c r="BL98" s="7">
-        <v>-511.94230100615835</v>
+        <v>-508.60896767282497</v>
       </c>
       <c r="BM98" s="7">
-        <v>-541.42043838188022</v>
+        <v>-538.08710504854696</v>
       </c>
       <c r="BN98" s="7">
-        <v>-570.92387899398375</v>
+        <v>-567.59054566065049</v>
       </c>
       <c r="BO98" s="7">
-        <v>-600.45285057159629</v>
+        <v>-593.78618390492954</v>
       </c>
       <c r="BP98" s="7">
-        <v>-625.18257996056559</v>
+        <v>-623.34091622674066</v>
       </c>
       <c r="BQ98" s="7">
-        <v>-658.31958909868524</v>
+        <v>-647.52369318021033</v>
       </c>
       <c r="BR98" s="7">
-        <v>-688.32464206724057</v>
+        <v>-670.06587641883164</v>
       </c>
       <c r="BS98" s="7">
-        <v>-718.17974051251269</v>
+        <v>-711.51307384584595</v>
       </c>
       <c r="BT98" s="7">
         <v>-715.76070776036056</v>
       </c>
       <c r="BU98" s="7">
-        <v>-770.76799665738599</v>
+        <v>-784.10132999071936</v>
       </c>
       <c r="BV98" s="7">
-        <v>-771.74508529396974</v>
+        <v>-778.41175196063637</v>
       </c>
       <c r="BW98" s="7">
-        <v>-829.40674772828231</v>
+        <v>-822.74008106161557</v>
       </c>
       <c r="BX98" s="7">
-        <v>-851.82491845783704</v>
+        <v>-838.49158512450367</v>
       </c>
       <c r="BY98" s="7">
-        <v>-847.41818605729111</v>
+        <v>-833.6451992558226</v>
       </c>
       <c r="BZ98" s="7">
-        <v>-850.35713455713233</v>
+        <v>-847.02380122379896</v>
       </c>
       <c r="CA98" s="7">
-        <v>-860.21100543481305</v>
+        <v>-856.87767210147979</v>
       </c>
       <c r="CB98" s="7">
         <v>-880.09356115039316</v>
       </c>
       <c r="CC98" s="7">
-        <v>-900.00505986741325</v>
+        <v>-903.33839320074674</v>
       </c>
       <c r="CD98" s="7">
         <v>-926.61242873955302</v>
@@ -30694,7 +30694,7 @@
         <v>-953.2492639315426</v>
       </c>
       <c r="CF98" s="8">
-        <v>-1003.2491639735928</v>
+        <v>-996.58249730692614</v>
       </c>
       <c r="CH98" t="s">
         <v>2</v>
@@ -30709,52 +30709,52 @@
         <v>390.06755305000036</v>
       </c>
       <c r="CL98" s="7">
-        <v>-907.57929916521709</v>
+        <v>-914.24596583188372</v>
       </c>
       <c r="CM98" s="7">
         <v>-936.1610228577041</v>
       </c>
       <c r="CN98" s="7">
-        <v>-964.63998206342364</v>
+        <v>-957.97331539675702</v>
       </c>
       <c r="CO98" s="7">
-        <v>-1006.348585235328</v>
+        <v>-999.68191856866133</v>
       </c>
       <c r="CP98" s="7">
-        <v>-1047.9525658357793</v>
+        <v>-1041.2858991691128</v>
       </c>
       <c r="CQ98" s="7">
-        <v>-1089.4509822616346</v>
+        <v>-1076.1176489283014</v>
       </c>
       <c r="CR98" s="7">
-        <v>-1124.1762177686562</v>
+        <v>-1117.5095511019895</v>
       </c>
       <c r="CS98" s="7">
-        <v>-1158.7939803952409</v>
+        <v>-1152.1273137285743</v>
       </c>
       <c r="CT98" s="7">
-        <v>-1193.3033028854647</v>
+        <v>-1186.636636218798</v>
       </c>
       <c r="CU98" s="7">
-        <v>-1227.7032092781008</v>
+        <v>-1221.036542611434</v>
       </c>
       <c r="CV98" s="7">
-        <v>-1261.9927148282704</v>
+        <v>-1275.3260481616039</v>
       </c>
       <c r="CW98" s="7">
-        <v>-1289.5041592617251</v>
+        <v>-1302.8374925950584</v>
       </c>
       <c r="CX98" s="7">
-        <v>-1323.5698733617476</v>
+        <v>-1330.2365400284141</v>
       </c>
       <c r="CY98" s="7">
-        <v>-1357.5221788886702</v>
+        <v>-1350.8555122220034</v>
       </c>
       <c r="CZ98" s="7">
-        <v>-1382.1435586169421</v>
+        <v>-1371.3600551653349</v>
       </c>
       <c r="DA98" s="7">
-        <v>-1375.2907206444945</v>
+        <v>-1371.7491389951563</v>
       </c>
       <c r="DB98" s="7">
         <v>-1368.3762071302951</v>
@@ -30792,43 +30792,43 @@
         <v>-247.25892320000031</v>
       </c>
       <c r="E99" s="10">
-        <v>738.47538837720015</v>
+        <v>741.80872171053352</v>
       </c>
       <c r="F99" s="10">
         <v>755.88796687259503</v>
       </c>
       <c r="G99" s="10">
-        <v>773.27725857444841</v>
+        <v>769.94392524111504</v>
       </c>
       <c r="H99" s="10">
-        <v>797.30972056828512</v>
+        <v>793.97638723495186</v>
       </c>
       <c r="I99" s="10">
-        <v>821.31847472006643</v>
+        <v>817.98514138673306</v>
       </c>
       <c r="J99" s="10">
-        <v>845.30330765921371</v>
+        <v>838.63664099254697</v>
       </c>
       <c r="K99" s="10">
-        <v>865.93067076147997</v>
+        <v>862.5973374281466</v>
       </c>
       <c r="L99" s="10">
-        <v>886.53368013166653</v>
+        <v>883.20034679833316</v>
       </c>
       <c r="M99" s="10">
-        <v>907.11211658618481</v>
+        <v>903.77878325285178</v>
       </c>
       <c r="N99" s="10">
-        <v>927.66575896879408</v>
+        <v>924.33242563546071</v>
       </c>
       <c r="O99" s="10">
-        <v>948.19438413284661</v>
+        <v>954.86105079951324</v>
       </c>
       <c r="P99" s="10">
-        <v>965.36443359004215</v>
+        <v>972.03110025670878</v>
       </c>
       <c r="Q99" s="10">
-        <v>985.84234682568592</v>
+        <v>989.17568015901929</v>
       </c>
       <c r="R99" s="10">
         <v>1000</v>
@@ -30873,67 +30873,67 @@
         <v>-304.85840933333378</v>
       </c>
       <c r="AH99" s="10">
-        <v>690.03224208766687</v>
+        <v>693.36557542100024</v>
       </c>
       <c r="AI99" s="10">
         <v>707.09535226645585</v>
       </c>
       <c r="AJ99" s="10">
-        <v>724.13203043685394</v>
+        <v>720.79869710352057</v>
       </c>
       <c r="AK99" s="10">
-        <v>747.80870537745227</v>
+        <v>744.4753720441189</v>
       </c>
       <c r="AL99" s="10">
-        <v>771.45847039251601</v>
+        <v>768.12513705918275</v>
       </c>
       <c r="AM99" s="10">
-        <v>795.08108329271556</v>
+        <v>788.41441662604882</v>
       </c>
       <c r="AN99" s="10">
-        <v>815.34296637568343</v>
+        <v>812.00963304235006</v>
       </c>
       <c r="AO99" s="10">
-        <v>835.57720640639775</v>
+        <v>832.24387307306438</v>
       </c>
       <c r="AP99" s="10">
-        <v>855.78355459738862</v>
+        <v>852.45022126405536</v>
       </c>
       <c r="AQ99" s="10">
-        <v>875.96175992209851</v>
+        <v>872.62842658876514</v>
       </c>
       <c r="AR99" s="10">
-        <v>896.11156909473073</v>
+        <v>902.77823576139747</v>
       </c>
       <c r="AS99" s="10">
-        <v>912.89939321658335</v>
+        <v>919.56605988324998</v>
       </c>
       <c r="AT99" s="10">
-        <v>980.84830775553246</v>
+        <v>984.18164108886572</v>
       </c>
       <c r="AU99" s="10">
-        <v>953.05471919199908</v>
+        <v>949.7213858586656</v>
       </c>
       <c r="AV99" s="10">
-        <v>969.75503166472731</v>
+        <v>963.08836499806057</v>
       </c>
       <c r="AW99" s="10">
-        <v>973.09231361637649</v>
+        <v>966.42564694970986</v>
       </c>
       <c r="AX99" s="10">
-        <v>976.3996311055904</v>
+        <v>973.06629777225703</v>
       </c>
       <c r="AY99" s="10">
-        <v>979.67671445220753</v>
+        <v>976.34338111887428</v>
       </c>
       <c r="AZ99" s="10">
-        <v>992.92329154894423</v>
+        <v>992.92329154894412</v>
       </c>
       <c r="BA99" s="10">
         <v>1000</v>
       </c>
       <c r="BB99" s="10">
-        <v>821.08469481290433</v>
+        <v>1000</v>
       </c>
       <c r="BC99" s="10">
         <v>1000</v>
@@ -30954,64 +30954,64 @@
         <v>-236.62909493333387</v>
       </c>
       <c r="BJ99" s="10">
-        <v>579.70107654559922</v>
+        <v>585.03838518160103</v>
       </c>
       <c r="BK99" s="10">
         <v>596.27940398156875</v>
       </c>
       <c r="BL99" s="10">
-        <v>613.98825861740295</v>
+        <v>607.32159195073632</v>
       </c>
       <c r="BM99" s="10">
-        <v>644.82982627829313</v>
+        <v>638.16315961162638</v>
       </c>
       <c r="BN99" s="10">
-        <v>675.46896804813139</v>
+        <v>668.80230138146464</v>
       </c>
       <c r="BO99" s="10">
-        <v>705.90386209389806</v>
+        <v>692.5705287605648</v>
       </c>
       <c r="BP99" s="10">
-        <v>726.4826643203935</v>
+        <v>722.79933685274329</v>
       </c>
       <c r="BQ99" s="10">
-        <v>747.42225625851427</v>
+        <v>742.02430829927675</v>
       </c>
       <c r="BR99" s="10">
-        <v>766.8352098981743</v>
+        <v>757.70582707396977</v>
       </c>
       <c r="BS99" s="10">
-        <v>786.21288012059119</v>
+        <v>782.87954678725794</v>
       </c>
       <c r="BT99" s="10">
         <v>789.49353583329423</v>
       </c>
       <c r="BU99" s="10">
-        <v>821.52776391938505</v>
+        <v>828.19443058605168</v>
       </c>
       <c r="BV99" s="10">
-        <v>826.58766712799286</v>
+        <v>829.92100046132623</v>
       </c>
       <c r="BW99" s="10">
-        <v>860.0309994654782</v>
+        <v>856.69766613214495</v>
       </c>
       <c r="BX99" s="10">
-        <v>875.89409846066758</v>
+        <v>869.22743179400095</v>
       </c>
       <c r="BY99" s="10">
-        <v>878.38663201348038</v>
+        <v>871.50013861274613</v>
       </c>
       <c r="BZ99" s="10">
-        <v>873.33625687627625</v>
+        <v>866.66959020960962</v>
       </c>
       <c r="CA99" s="10">
-        <v>861.17195652149633</v>
+        <v>854.50528985482958</v>
       </c>
       <c r="CB99" s="10">
         <v>868.77817746352332</v>
       </c>
       <c r="CC99" s="10">
-        <v>876.15285439402908</v>
+        <v>882.81952106069559</v>
       </c>
       <c r="CD99" s="10">
         <v>896.62723675024222</v>
@@ -31020,7 +31020,7 @@
         <v>916.86588854766092</v>
       </c>
       <c r="CF99" s="11">
-        <v>983.5333548779239</v>
+        <v>970.20002154459053</v>
       </c>
       <c r="CH99" t="s">
         <v>3</v>
@@ -31035,52 +31035,52 @@
         <v>-415.08264560000032</v>
       </c>
       <c r="CL99" s="10">
-        <v>717.83630568593333</v>
+        <v>721.1696390192667</v>
       </c>
       <c r="CM99" s="10">
         <v>735.14965243710697</v>
       </c>
       <c r="CN99" s="10">
-        <v>752.43881930904092</v>
+        <v>749.10548597570755</v>
       </c>
       <c r="CO99" s="10">
-        <v>776.37025534948896</v>
+        <v>773.03692201615559</v>
       </c>
       <c r="CP99" s="10">
-        <v>800.27707431430099</v>
+        <v>796.94374098096762</v>
       </c>
       <c r="CQ99" s="10">
-        <v>824.15905464979642</v>
+        <v>817.49238798312967</v>
       </c>
       <c r="CR99" s="10">
-        <v>844.68263947497803</v>
+        <v>841.34930614164477</v>
       </c>
       <c r="CS99" s="10">
-        <v>865.18093656358633</v>
+        <v>861.84760323025296</v>
       </c>
       <c r="CT99" s="10">
-        <v>885.65371832599169</v>
+        <v>882.32038499265832</v>
       </c>
       <c r="CU99" s="10">
-        <v>906.10075512425897</v>
+        <v>902.76742179092571</v>
       </c>
       <c r="CV99" s="10">
-        <v>926.52181525371077</v>
+        <v>933.1884819203774</v>
       </c>
       <c r="CW99" s="10">
-        <v>943.58333159099425</v>
+        <v>950.24999825766088</v>
       </c>
       <c r="CX99" s="10">
-        <v>963.95173490864659</v>
+        <v>967.28506824198007</v>
       </c>
       <c r="CY99" s="10">
-        <v>984.29345385615773</v>
+        <v>980.96012052282435</v>
       </c>
       <c r="CZ99" s="10">
-        <v>1000</v>
+        <v>994.6082482741964</v>
       </c>
       <c r="DA99" s="10">
-        <v>1000</v>
+        <v>998.22920917533088</v>
       </c>
       <c r="DB99" s="10">
         <v>1000</v>
@@ -31149,25 +31149,25 @@
         <v>474.74284899630015</v>
       </c>
       <c r="F103" s="4">
-        <v>498.74228895059724</v>
+        <v>549.42840130393324</v>
       </c>
       <c r="G103" s="4">
-        <v>550.57644024364652</v>
+        <v>553.48345691566885</v>
       </c>
       <c r="H103" s="4">
         <v>557.57500802790958</v>
       </c>
       <c r="I103" s="4">
-        <v>556.22733481490559</v>
+        <v>560.4822658812343</v>
       </c>
       <c r="J103" s="4">
-        <v>547.25396112629232</v>
+        <v>565.86891354806198</v>
       </c>
       <c r="K103" s="4">
-        <v>559.65126924850222</v>
+        <v>570.07193376999464</v>
       </c>
       <c r="L103" s="4">
-        <v>574.31278117392435</v>
+        <v>574.31278117392458</v>
       </c>
       <c r="M103" s="4">
         <v>578.59179620448981</v>
@@ -31176,28 +31176,28 @@
         <v>582.90932237033007</v>
       </c>
       <c r="O103" s="4">
-        <v>587.26570627166291</v>
+        <v>546.56937058213498</v>
       </c>
       <c r="P103" s="4">
-        <v>591.66129762810806</v>
+        <v>555.98849491737406</v>
       </c>
       <c r="Q103" s="4">
-        <v>587.88630446893433</v>
+        <v>565.49239137163022</v>
       </c>
       <c r="R103" s="4">
-        <v>578.86680893003711</v>
+        <v>575.08182289397485</v>
       </c>
       <c r="S103" s="4">
-        <v>584.75755930002038</v>
+        <v>585.89694007336993</v>
       </c>
       <c r="T103" s="4">
-        <v>594.52037733372049</v>
+        <v>596.8033458673633</v>
       </c>
       <c r="U103" s="4">
-        <v>604.37106072972392</v>
+        <v>604.53457598016962</v>
       </c>
       <c r="V103" s="4">
-        <v>614.31040027629138</v>
+        <v>615.75872049732436</v>
       </c>
       <c r="W103" s="4">
         <v>624.33919387877813</v>
@@ -31227,13 +31227,13 @@
         <v>585.10993916666666</v>
       </c>
       <c r="AH103" s="4">
-        <v>584.23932861916637</v>
+        <v>540.0842756124996</v>
       </c>
       <c r="AI103" s="4">
-        <v>588.60768257673885</v>
+        <v>588.60768257673897</v>
       </c>
       <c r="AJ103" s="4">
-        <v>593.01535171992941</v>
+        <v>593.01535171992964</v>
       </c>
       <c r="AK103" s="4">
         <v>597.46268988540885</v>
@@ -31266,10 +31266,10 @@
         <v>658.14390366481575</v>
       </c>
       <c r="AU103" s="4">
-        <v>668.56719879779905</v>
+        <v>668.56719879779871</v>
       </c>
       <c r="AV103" s="4">
-        <v>679.08430358697933</v>
+        <v>679.0843035869791</v>
       </c>
       <c r="AW103" s="4">
         <v>689.69606231926173</v>
@@ -31284,7 +31284,7 @@
         <v>563.33530833992734</v>
       </c>
       <c r="BA103" s="4">
-        <v>555.7074488327587</v>
+        <v>563.65049426830274</v>
       </c>
       <c r="BB103" s="4">
         <v>608.11334871671761</v>
@@ -31293,7 +31293,7 @@
         <v>662.43636885516821</v>
       </c>
       <c r="BD103" s="5">
-        <v>766.70121701795392</v>
+        <v>766.61829617486433</v>
       </c>
       <c r="BF103" s="1" t="s">
         <v>1</v>
@@ -31314,28 +31314,28 @@
         <v>797.94325327701154</v>
       </c>
       <c r="BL103" s="4">
-        <v>809.62474255650454</v>
+        <v>795.80723562431399</v>
       </c>
       <c r="BM103" s="4">
-        <v>821.41136523951263</v>
+        <v>811.25070191409873</v>
       </c>
       <c r="BN103" s="4">
         <v>833.3040675266684</v>
       </c>
       <c r="BO103" s="4">
-        <v>845.30380413440844</v>
+        <v>808.94999043647454</v>
       </c>
       <c r="BP103" s="4">
-        <v>857.41153837161789</v>
+        <v>857.41153837161755</v>
       </c>
       <c r="BQ103" s="4">
-        <v>869.62824221696224</v>
+        <v>856.44520369150302</v>
       </c>
       <c r="BR103" s="4">
-        <v>881.95489639691482</v>
+        <v>861.6904703598334</v>
       </c>
       <c r="BS103" s="4">
-        <v>894.39249046448685</v>
+        <v>883.93188899700908</v>
       </c>
       <c r="BT103" s="4">
         <v>906.9420228786671</v>
@@ -31347,34 +31347,34 @@
         <v>932.38094159433581</v>
       </c>
       <c r="BW103" s="4">
-        <v>945.27237006868495</v>
+        <v>945.27237006868449</v>
       </c>
       <c r="BX103" s="4">
-        <v>958.27982139930259</v>
+        <v>905.19122176679866</v>
       </c>
       <c r="BY103" s="4">
-        <v>749.72248292205541</v>
+        <v>667.69992784624856</v>
       </c>
       <c r="BZ103" s="4">
-        <v>664.41943776101675</v>
+        <v>674.39298256818381</v>
       </c>
       <c r="CA103" s="4">
-        <v>743.94141049649829</v>
+        <v>755.11692021873489</v>
       </c>
       <c r="CB103" s="4">
-        <v>774.13642488618666</v>
+        <v>767.46429822162895</v>
       </c>
       <c r="CC103" s="4">
-        <v>816.93382502986231</v>
+        <v>798.82442050452664</v>
       </c>
       <c r="CD103" s="4">
-        <v>852.24295677029409</v>
+        <v>846.35296552618047</v>
       </c>
       <c r="CE103" s="4">
-        <v>886.26749376653481</v>
+        <v>880.69522278610748</v>
       </c>
       <c r="CF103" s="5">
-        <v>866.62506490796761</v>
+        <v>873.29173157463435</v>
       </c>
       <c r="CH103" s="1" t="s">
         <v>1</v>
@@ -31389,55 +31389,55 @@
         <v>553.04038766666667</v>
       </c>
       <c r="CL103" s="4">
-        <v>521.88895590155653</v>
+        <v>524.76143013209867</v>
       </c>
       <c r="CM103" s="4">
-        <v>555.95828151606736</v>
+        <v>490.12187659910688</v>
       </c>
       <c r="CN103" s="4">
         <v>560.07210604971215</v>
       </c>
       <c r="CO103" s="4">
-        <v>560.48096063466517</v>
+        <v>564.22295500415942</v>
       </c>
       <c r="CP103" s="4">
-        <v>564.83040186634003</v>
+        <v>568.4111615991967</v>
       </c>
       <c r="CQ103" s="4">
-        <v>572.6370620535896</v>
+        <v>572.63706205358937</v>
       </c>
       <c r="CR103" s="4">
-        <v>576.90099561207182</v>
+        <v>575.72048984518869</v>
       </c>
       <c r="CS103" s="4">
-        <v>575.81735556180956</v>
+        <v>581.20330457258024</v>
       </c>
       <c r="CT103" s="4">
-        <v>581.75015078513934</v>
+        <v>585.54433431373354</v>
       </c>
       <c r="CU103" s="4">
-        <v>582.49352489569173</v>
+        <v>589.92443332255698</v>
       </c>
       <c r="CV103" s="4">
-        <v>577.74517060108565</v>
+        <v>566.11880002530506</v>
       </c>
       <c r="CW103" s="4">
-        <v>591.28865178178035</v>
+        <v>575.2686106491276</v>
       </c>
       <c r="CX103" s="4">
-        <v>589.5552849133478</v>
+        <v>581.93056804068647</v>
       </c>
       <c r="CY103" s="4">
-        <v>590.66271887794551</v>
+        <v>607.15726847318058</v>
       </c>
       <c r="CZ103" s="4">
-        <v>604.48515230635712</v>
+        <v>612.42338556232858</v>
       </c>
       <c r="DA103" s="4">
-        <v>617.04539603238936</v>
+        <v>617.04539603238948</v>
       </c>
       <c r="DB103" s="4">
-        <v>621.7090045966811</v>
+        <v>621.70900459668087</v>
       </c>
       <c r="DC103" s="4">
         <v>618.32410417964877</v>
@@ -31475,22 +31475,22 @@
         <v>-1439.0122181306997</v>
       </c>
       <c r="F104" s="7">
-        <v>-1432.2365737805453</v>
+        <v>-1381.5504614272093</v>
       </c>
       <c r="G104" s="7">
-        <v>-1397.7812322520765</v>
+        <v>-1394.8742155800539</v>
       </c>
       <c r="H104" s="7">
         <v>-1408.3178835202741</v>
       </c>
       <c r="I104" s="7">
-        <v>-1427.3585927572117</v>
+        <v>-1423.103661690883</v>
       </c>
       <c r="J104" s="7">
-        <v>-1454.1842397939738</v>
+        <v>-1435.5692873722039</v>
       </c>
       <c r="K104" s="7">
-        <v>-1459.7998754800458</v>
+        <v>-1449.3792109585534</v>
       </c>
       <c r="L104" s="7">
         <v>-1463.3134238571806</v>
@@ -31499,31 +31499,31 @@
         <v>-1477.3730446718951</v>
       </c>
       <c r="N104" s="7">
-        <v>-1491.5592020739418</v>
+        <v>-1491.5592020739416</v>
       </c>
       <c r="O104" s="7">
-        <v>-1505.8730348926067</v>
+        <v>-1546.569370582135</v>
       </c>
       <c r="P104" s="7">
-        <v>-1520.3156922066405</v>
+        <v>-1555.9884949173741</v>
       </c>
       <c r="Q104" s="7">
-        <v>-1543.0984782743262</v>
+        <v>-1565.4923913716302</v>
       </c>
       <c r="R104" s="7">
-        <v>-1571.2968368579122</v>
+        <v>-1575.0818228939747</v>
       </c>
       <c r="S104" s="7">
-        <v>-1584.7575593000204</v>
+        <v>-1583.6181785266708</v>
       </c>
       <c r="T104" s="7">
-        <v>-1594.5203773337205</v>
+        <v>-1592.2374088000774</v>
       </c>
       <c r="U104" s="7">
-        <v>-1604.3710607297239</v>
+        <v>-1604.207545479278</v>
       </c>
       <c r="V104" s="7">
-        <v>-1614.3104002762914</v>
+        <v>-1612.8620800552583</v>
       </c>
       <c r="W104" s="7">
         <v>-1624.3391938787777</v>
@@ -31553,13 +31553,13 @@
         <v>-826.50408583333308</v>
       </c>
       <c r="AH104" s="7">
-        <v>-1495.9292226058328</v>
+        <v>-1540.0842756124996</v>
       </c>
       <c r="AI104" s="7">
-        <v>-1510.282385609285</v>
+        <v>-1510.2823856092853</v>
       </c>
       <c r="AJ104" s="7">
-        <v>-1524.7647270797684</v>
+        <v>-1524.7647270797686</v>
       </c>
       <c r="AK104" s="7">
         <v>-1539.3774096234863</v>
@@ -31592,10 +31592,10 @@
         <v>-1658.1439036648158</v>
       </c>
       <c r="AU104" s="7">
-        <v>-1668.5671987977989</v>
+        <v>-1668.5671987977992</v>
       </c>
       <c r="AV104" s="7">
-        <v>-1679.0843035869789</v>
+        <v>-1679.0843035869791</v>
       </c>
       <c r="AW104" s="7">
         <v>-1689.6960623192617</v>
@@ -31610,7 +31610,7 @@
         <v>-1563.3353083399275</v>
       </c>
       <c r="BA104" s="7">
-        <v>-1554.6789715505306</v>
+        <v>-1563.6504942683027</v>
       </c>
       <c r="BB104" s="7">
         <v>-1608.1133487167176</v>
@@ -31619,7 +31619,7 @@
         <v>-1662.4363688551682</v>
       </c>
       <c r="BD104" s="8">
-        <v>-1766.7012170179539</v>
+        <v>-1766.6182961748643</v>
       </c>
       <c r="BF104" t="s">
         <v>2</v>
@@ -31640,28 +31640,28 @@
         <v>-1797.9432532770115</v>
       </c>
       <c r="BL104" s="7">
-        <v>-1809.6247425565045</v>
+        <v>-1795.807235624314</v>
       </c>
       <c r="BM104" s="7">
-        <v>-1821.4113652395131</v>
+        <v>-1811.2507019140987</v>
       </c>
       <c r="BN104" s="7">
         <v>-1833.3040675266684</v>
       </c>
       <c r="BO104" s="7">
-        <v>-1845.303804134408</v>
+        <v>-1808.9499904364745</v>
       </c>
       <c r="BP104" s="7">
-        <v>-1857.4115383716176</v>
+        <v>-1857.411538371618</v>
       </c>
       <c r="BQ104" s="7">
-        <v>-1869.6282422169622</v>
+        <v>-1856.4452036915031</v>
       </c>
       <c r="BR104" s="7">
-        <v>-1881.9548963969148</v>
+        <v>-1861.6904703598334</v>
       </c>
       <c r="BS104" s="7">
-        <v>-1894.3924904644869</v>
+        <v>-1883.9318889970091</v>
       </c>
       <c r="BT104" s="7">
         <v>-1906.9420228786671</v>
@@ -31673,34 +31673,34 @@
         <v>-1932.3809415943358</v>
       </c>
       <c r="BW104" s="7">
-        <v>-1945.2723700686845</v>
+        <v>-1945.2723700686849</v>
       </c>
       <c r="BX104" s="7">
-        <v>-1958.279821399303</v>
+        <v>-1905.1912217667987</v>
       </c>
       <c r="BY104" s="7">
-        <v>-1749.7224829220554</v>
+        <v>-1667.6999278462486</v>
       </c>
       <c r="BZ104" s="7">
-        <v>-1654.8745199390296</v>
+        <v>-1644.9009751318624</v>
       </c>
       <c r="CA104" s="7">
-        <v>-1602.0761928228483</v>
+        <v>-1590.9006831006118</v>
       </c>
       <c r="CB104" s="7">
-        <v>-1598.8453368630337</v>
+        <v>-1605.5174635275914</v>
       </c>
       <c r="CC104" s="7">
-        <v>-1583.2547725751006</v>
+        <v>-1601.3641771004363</v>
       </c>
       <c r="CD104" s="7">
-        <v>-1575.3973382131132</v>
+        <v>-1581.2873294572269</v>
       </c>
       <c r="CE104" s="7">
-        <v>-1569.0715638717213</v>
+        <v>-1574.6438348521488</v>
       </c>
       <c r="CF104" s="8">
-        <v>-1616.6620442490334</v>
+        <v>-1609.9953775823669</v>
       </c>
       <c r="CH104" t="s">
         <v>2</v>
@@ -31715,52 +31715,52 @@
         <v>-721.1327023333331</v>
       </c>
       <c r="CL104" s="7">
-        <v>-1419.6016919084429</v>
+        <v>-1416.7292176779008</v>
       </c>
       <c r="CM104" s="7">
-        <v>-1403.0057821242215</v>
+        <v>-1468.8421870411821</v>
       </c>
       <c r="CN104" s="7">
         <v>-1416.5226341633397</v>
       </c>
       <c r="CO104" s="7">
-        <v>-1433.9031322403039</v>
+        <v>-1430.1611378708094</v>
       </c>
       <c r="CP104" s="7">
-        <v>-1447.503147844503</v>
+        <v>-1443.9223881116463</v>
       </c>
       <c r="CQ104" s="7">
         <v>-1457.807489604651</v>
       </c>
       <c r="CR104" s="7">
-        <v>-1471.817557011093</v>
+        <v>-1472.998062777976</v>
       </c>
       <c r="CS104" s="7">
-        <v>-1491.3396640349633</v>
+        <v>-1485.9537150241924</v>
       </c>
       <c r="CT104" s="7">
-        <v>-1504.0112819880042</v>
+        <v>-1500.2170984594102</v>
       </c>
       <c r="CU104" s="7">
-        <v>-1522.0397607724096</v>
+        <v>-1514.6088523455446</v>
       </c>
       <c r="CV104" s="7">
-        <v>-1545.7289146380283</v>
+        <v>-1557.3552852138091</v>
       </c>
       <c r="CW104" s="7">
-        <v>-1551.2967002244857</v>
+        <v>-1567.3167413571384</v>
       </c>
       <c r="CX104" s="7">
-        <v>-1572.3133352609739</v>
+        <v>-1579.9380521336357</v>
       </c>
       <c r="CY104" s="7">
-        <v>-1590.6627188779455</v>
+        <v>-1574.1681692827106</v>
       </c>
       <c r="CZ104" s="7">
-        <v>-1596.4722143893368</v>
+        <v>-1588.5339811333652</v>
       </c>
       <c r="DA104" s="7">
-        <v>-1603.7205869635652</v>
+        <v>-1603.7205869635654</v>
       </c>
       <c r="DB104" s="7">
         <v>-1619.0438722462372</v>
@@ -31801,22 +31801,22 @@
         <v>964.26936913439988</v>
       </c>
       <c r="F105" s="10">
-        <v>933.49428482994824</v>
+        <v>832.12206012327601</v>
       </c>
       <c r="G105" s="10">
-        <v>847.20479200842988</v>
+        <v>841.39075866438566</v>
       </c>
       <c r="H105" s="10">
         <v>850.74287549236465</v>
       </c>
       <c r="I105" s="10">
-        <v>871.13125794230609</v>
+        <v>862.62139580964879</v>
       </c>
       <c r="J105" s="10">
-        <v>906.93027866768148</v>
+        <v>869.70037382414182</v>
       </c>
       <c r="K105" s="10">
-        <v>900.14860623154368</v>
+        <v>879.30727718855906</v>
       </c>
       <c r="L105" s="10">
         <v>889.00064268325605</v>
@@ -31825,31 +31825,31 @@
         <v>898.78124846740513</v>
       </c>
       <c r="N105" s="10">
-        <v>908.64987970361165</v>
+        <v>908.64987970361153</v>
       </c>
       <c r="O105" s="10">
-        <v>918.6073286209438</v>
+        <v>1000</v>
       </c>
       <c r="P105" s="10">
-        <v>928.65439457853245</v>
+        <v>1000</v>
       </c>
       <c r="Q105" s="10">
-        <v>955.2121738053919</v>
+        <v>1000</v>
       </c>
       <c r="R105" s="10">
-        <v>992.43002792787513</v>
+        <v>1000</v>
       </c>
       <c r="S105" s="10">
-        <v>1000</v>
+        <v>997.72123845330043</v>
       </c>
       <c r="T105" s="10">
-        <v>1000</v>
+        <v>995.43406293271391</v>
       </c>
       <c r="U105" s="10">
-        <v>1000</v>
+        <v>999.6729694991086</v>
       </c>
       <c r="V105" s="10">
-        <v>1000</v>
+        <v>997.10335955793357</v>
       </c>
       <c r="W105" s="10">
         <v>1000</v>
@@ -31879,13 +31879,13 @@
         <v>241.39414666666642</v>
       </c>
       <c r="AH105" s="10">
-        <v>911.68989398666645</v>
+        <v>1000</v>
       </c>
       <c r="AI105" s="10">
-        <v>921.6747030325464</v>
+        <v>921.67470303254618</v>
       </c>
       <c r="AJ105" s="10">
-        <v>931.74937535983918</v>
+        <v>931.74937535983895</v>
       </c>
       <c r="AK105" s="10">
         <v>941.91471973807734</v>
@@ -31936,7 +31936,7 @@
         <v>1000</v>
       </c>
       <c r="BA105" s="10">
-        <v>998.9715227177719</v>
+        <v>1000</v>
       </c>
       <c r="BB105" s="10">
         <v>1000</v>
@@ -32008,25 +32008,25 @@
         <v>1000</v>
       </c>
       <c r="BZ105" s="10">
-        <v>990.45508217801319</v>
+        <v>970.50799256367895</v>
       </c>
       <c r="CA105" s="10">
-        <v>858.13478232635055</v>
+        <v>835.78376288187678</v>
       </c>
       <c r="CB105" s="10">
-        <v>824.70891197684682</v>
+        <v>838.05316530596247</v>
       </c>
       <c r="CC105" s="10">
-        <v>766.32094754523814</v>
+        <v>802.53975659590992</v>
       </c>
       <c r="CD105" s="10">
-        <v>723.15438144281961</v>
+        <v>734.93436393104651</v>
       </c>
       <c r="CE105" s="10">
-        <v>682.80407010518661</v>
+        <v>693.94861206604128</v>
       </c>
       <c r="CF105" s="11">
-        <v>750.03697934106583</v>
+        <v>736.70364600773257</v>
       </c>
       <c r="CH105" t="s">
         <v>3</v>
@@ -32041,55 +32041,55 @@
         <v>168.0923146666666</v>
       </c>
       <c r="CL105" s="10">
-        <v>897.71273600688642</v>
+        <v>891.96778754580214</v>
       </c>
       <c r="CM105" s="10">
-        <v>847.047500608154</v>
+        <v>978.72031044207517</v>
       </c>
       <c r="CN105" s="10">
         <v>856.45052811362757</v>
       </c>
       <c r="CO105" s="10">
-        <v>873.4221716056386</v>
+        <v>865.9381828666501</v>
       </c>
       <c r="CP105" s="10">
-        <v>882.67274597816311</v>
+        <v>875.51122651244975</v>
       </c>
       <c r="CQ105" s="10">
         <v>885.17042755106149</v>
       </c>
       <c r="CR105" s="10">
-        <v>894.91656139902125</v>
+        <v>897.27757293278717</v>
       </c>
       <c r="CS105" s="10">
-        <v>915.52230847315377</v>
+        <v>904.7504104516122</v>
       </c>
       <c r="CT105" s="10">
-        <v>922.26113120286493</v>
+        <v>914.67276414567664</v>
       </c>
       <c r="CU105" s="10">
-        <v>939.5462358767179</v>
+        <v>924.68441902298764</v>
       </c>
       <c r="CV105" s="10">
-        <v>967.98374403694265</v>
+        <v>991.23648518850393</v>
       </c>
       <c r="CW105" s="10">
-        <v>960.00804844270499</v>
+        <v>992.04813070801106</v>
       </c>
       <c r="CX105" s="10">
-        <v>982.75805034762607</v>
+        <v>998.0074840929492</v>
       </c>
       <c r="CY105" s="10">
-        <v>1000</v>
+        <v>967.01090080952963</v>
       </c>
       <c r="CZ105" s="10">
-        <v>991.98706208297915</v>
+        <v>976.1105955710367</v>
       </c>
       <c r="DA105" s="10">
         <v>986.67519093117585</v>
       </c>
       <c r="DB105" s="10">
-        <v>997.3348676495566</v>
+        <v>997.33486764955637</v>
       </c>
       <c r="DC105" s="10">
         <v>1000</v>
@@ -32198,86 +32198,86 @@
         <v>6</v>
       </c>
       <c r="B108" s="15">
-        <v>1324676752.4978151</v>
+        <v>1306285036.0487242</v>
       </c>
       <c r="C108" s="16">
-        <v>581075287.4170475</v>
+        <v>579356608.67531204</v>
       </c>
       <c r="D108" s="16">
-        <v>534760000.55819589</v>
+        <v>533094172.31101334</v>
       </c>
       <c r="E108" s="16">
-        <v>185790103.97364777</v>
+        <v>184841943.46673578</v>
       </c>
       <c r="F108" s="16">
-        <v>169418467.14182264</v>
+        <v>168570204.17271858</v>
       </c>
       <c r="G108" s="16">
-        <v>154544750.13017818</v>
+        <v>153025843.89547342</v>
       </c>
       <c r="H108" s="16">
-        <v>139982652.85848188</v>
+        <v>139975100.34213752</v>
       </c>
       <c r="I108" s="16">
-        <v>127555998.12083706</v>
+        <v>126817107.25391293</v>
       </c>
       <c r="J108" s="16">
-        <v>116250368.71814576</v>
+        <v>115595970.39645541</v>
       </c>
       <c r="K108" s="16">
-        <v>106045397.28938025</v>
+        <v>105280096.9205493</v>
       </c>
       <c r="L108" s="16">
-        <v>96754790.688043579</v>
+        <v>97307247.78722097</v>
       </c>
       <c r="M108" s="16">
-        <v>87780018.664477572</v>
+        <v>87177280.496049002</v>
       </c>
       <c r="N108" s="16">
-        <v>80575240.689377084</v>
+        <v>79544025.325954393</v>
       </c>
       <c r="O108" s="16">
-        <v>73546583.697467491</v>
+        <v>72130121.691569299</v>
       </c>
       <c r="P108" s="16">
-        <v>66798044.723667927</v>
+        <v>65879858.716053113</v>
       </c>
       <c r="Q108" s="16">
-        <v>59595895.238672584</v>
+        <v>59392922.238912396</v>
       </c>
       <c r="R108" s="16">
-        <v>54421965.973738737</v>
+        <v>54537429.42708905</v>
       </c>
       <c r="S108" s="16">
-        <v>49779098.287889443</v>
+        <v>49661317.616155699</v>
       </c>
       <c r="T108" s="16">
-        <v>46418007.806459099</v>
+        <v>46302202.15054895</v>
       </c>
       <c r="U108" s="16">
-        <v>42563254.91878321</v>
+        <v>42427547.146672413</v>
       </c>
       <c r="V108" s="16">
-        <v>39470792.180570625</v>
+        <v>38915326.101924524</v>
       </c>
       <c r="W108" s="16">
-        <v>36161239.98085171</v>
+        <v>35766672.419499099</v>
       </c>
       <c r="X108" s="16">
-        <v>34451379.893826783</v>
+        <v>33438778.620788019</v>
       </c>
       <c r="Y108" s="16">
-        <v>29335153.617023565</v>
+        <v>29334509.074663833</v>
       </c>
       <c r="Z108" s="16">
-        <v>26931005.010520928</v>
+        <v>26930450.670340978</v>
       </c>
       <c r="AA108" s="17">
-        <v>24790539.828422952</v>
+        <v>24751324.672486119</v>
       </c>
       <c r="AB108" s="18">
         <f>SUM(TotalCost)</f>
-        <v>4289472789.9053454</v>
+        <v>4256339097.6389599</v>
       </c>
     </row>
     <row r="110" spans="1:112" x14ac:dyDescent="0.35">
@@ -32380,77 +32380,77 @@
         <v>26485337.771793649</v>
       </c>
       <c r="E111" s="4">
-        <v>5370071.801232243</v>
+        <v>5340999.611805208</v>
       </c>
       <c r="F111" s="4">
-        <v>5238623.6495696185</v>
+        <v>5246267.1075761616</v>
       </c>
       <c r="G111" s="4">
-        <v>5120714.4363529822</v>
+        <v>5149368.6995071499</v>
       </c>
       <c r="H111" s="4">
-        <v>4952008.6993450094</v>
+        <v>4978791.4859935977</v>
       </c>
       <c r="I111" s="4">
-        <v>4786478.409602805</v>
+        <v>4814998.8464654768</v>
       </c>
       <c r="J111" s="4">
-        <v>4610166.6716081016</v>
+        <v>4585133.0152629307</v>
       </c>
       <c r="K111" s="4">
-        <v>4309898.2991251014</v>
+        <v>4329333.0067530023</v>
       </c>
       <c r="L111" s="4">
-        <v>4031435.0272658197</v>
+        <v>4061474.7737073675</v>
       </c>
       <c r="M111" s="4">
-        <v>3774757.7065619589</v>
+        <v>3808377.8266529194</v>
       </c>
       <c r="N111" s="4">
-        <v>3545545.5500420234</v>
+        <v>3565570.8938974361</v>
       </c>
       <c r="O111" s="4">
-        <v>3344167.1482943618</v>
+        <v>3506822.5621998836</v>
       </c>
       <c r="P111" s="4">
-        <v>3108804.0486599728</v>
+        <v>3268321.0364256771</v>
       </c>
       <c r="Q111" s="4">
-        <v>2942835.0056714206</v>
+        <v>3047145.6857773084</v>
       </c>
       <c r="R111" s="4">
-        <v>2770730.5793694658</v>
+        <v>2785649.4591947803</v>
       </c>
       <c r="S111" s="4">
-        <v>2514944.365909026</v>
+        <v>2554136.1243618624</v>
       </c>
       <c r="T111" s="4">
-        <v>2372524.0116405245</v>
+        <v>2437599.7665287163</v>
       </c>
       <c r="U111" s="4">
-        <v>2036394.4516432886</v>
+        <v>2074785.7273291906</v>
       </c>
       <c r="V111" s="4">
-        <v>1844077.1969583482</v>
+        <v>1882161.2563803426</v>
       </c>
       <c r="W111" s="4">
-        <v>1624104.0771693215</v>
+        <v>1642077.1850932406</v>
       </c>
       <c r="X111" s="4">
-        <v>1331046.4721497726</v>
+        <v>1436123.9807943325</v>
       </c>
       <c r="Y111" s="4">
-        <v>1046116.239576439</v>
+        <v>1093818.9488230054</v>
       </c>
       <c r="Z111" s="4">
-        <v>774311.93263730826</v>
+        <v>819441.44326061418</v>
       </c>
       <c r="AA111" s="5">
-        <v>741306.64957830892</v>
+        <v>743286.07171129237</v>
       </c>
       <c r="AB111" s="12">
         <f>SUM(B111:AA111)</f>
-        <v>167914050.3398101</v>
+        <v>168894672.42534843</v>
       </c>
     </row>
     <row r="112" spans="1:112" x14ac:dyDescent="0.35">
@@ -32467,77 +32467,77 @@
         <v>7838038.1192439953</v>
       </c>
       <c r="E112" s="7">
-        <v>1691783.6736335622</v>
+        <v>1711956.2877313248</v>
       </c>
       <c r="F112" s="7">
-        <v>1613143.2496698389</v>
+        <v>1627461.2766398424</v>
       </c>
       <c r="G112" s="7">
-        <v>1541330.9257688485</v>
+        <v>1546593.5023247248</v>
       </c>
       <c r="H112" s="7">
-        <v>1488312.3624520837</v>
+        <v>1493829.3873065496</v>
       </c>
       <c r="I112" s="7">
-        <v>1439442.9248849838</v>
+        <v>1442473.8280548649</v>
       </c>
       <c r="J112" s="7">
-        <v>1389232.7014402431</v>
+        <v>1363247.8297911836</v>
       </c>
       <c r="K112" s="7">
-        <v>1276983.0657211021</v>
+        <v>1275670.6567013911</v>
       </c>
       <c r="L112" s="7">
-        <v>1175204.0064035645</v>
+        <v>1180960.502702564</v>
       </c>
       <c r="M112" s="7">
-        <v>1083928.365373624</v>
+        <v>1092409.5560445481</v>
       </c>
       <c r="N112" s="7">
-        <v>1007083.2579199411</v>
+        <v>1007485.9381186449</v>
       </c>
       <c r="O112" s="7">
-        <v>945100.15040016407</v>
+        <v>1048127.2369076426</v>
       </c>
       <c r="P112" s="7">
-        <v>854860.2987853142</v>
+        <v>956322.77064946224</v>
       </c>
       <c r="Q112" s="7">
-        <v>809836.20409960335</v>
+        <v>872807.55924396706</v>
       </c>
       <c r="R112" s="7">
-        <v>764053.35266843205</v>
+        <v>758390.41016376263</v>
       </c>
       <c r="S112" s="7">
-        <v>663749.02973783121</v>
+        <v>670369.22680383117</v>
       </c>
       <c r="T112" s="7">
-        <v>604099.99614726135</v>
+        <v>626173.48378375359</v>
       </c>
       <c r="U112" s="7">
-        <v>476618.27408386028</v>
+        <v>490738.71049499983</v>
       </c>
       <c r="V112" s="7">
-        <v>406669.61649577145</v>
+        <v>419736.92427033489</v>
       </c>
       <c r="W112" s="7">
-        <v>324751.92339987057</v>
+        <v>330659.47772568336</v>
       </c>
       <c r="X112" s="7">
-        <v>212970.20475150773</v>
+        <v>257306.088130738</v>
       </c>
       <c r="Y112" s="7">
-        <v>110810.44664083561</v>
+        <v>128497.38354795949</v>
       </c>
       <c r="Z112" s="7">
-        <v>13176.498871885267</v>
+        <v>29909.35995359084</v>
       </c>
       <c r="AA112" s="8">
-        <v>6768.0256401484748</v>
+        <v>6842.1085711386277</v>
       </c>
       <c r="AB112" s="13">
         <f t="shared" ref="AB112:AB115" si="0">SUM(B112:AA112)</f>
-        <v>48101139.22119379</v>
+        <v>48539200.171866022</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -32554,77 +32554,77 @@
         <v>43811839828.485703</v>
       </c>
       <c r="E113" s="7">
-        <v>5942587390.532445</v>
+        <v>5995714720.0338411</v>
       </c>
       <c r="F113" s="7">
-        <v>5622029964.4773874</v>
+        <v>5672291478.3198881</v>
       </c>
       <c r="G113" s="7">
-        <v>5318764175.3215618</v>
+        <v>5366314462.4797659</v>
       </c>
       <c r="H113" s="7">
-        <v>5031857270.6706963</v>
+        <v>5076842581.2188969</v>
       </c>
       <c r="I113" s="7">
-        <v>4760426813.0332689</v>
+        <v>4802985507.9657545</v>
       </c>
       <c r="J113" s="7">
-        <v>4503637965.7139034</v>
+        <v>4543900942.5008631</v>
       </c>
       <c r="K113" s="7">
-        <v>4260700925.1121774</v>
+        <v>4298792020.3001051</v>
       </c>
       <c r="L113" s="7">
-        <v>4030868491.5294061</v>
+        <v>4066904861.6242685</v>
       </c>
       <c r="M113" s="7">
-        <v>3813433771.01193</v>
+        <v>3847526252.8165879</v>
       </c>
       <c r="N113" s="7">
-        <v>3607728001.1624961</v>
+        <v>3639981452.6766548</v>
       </c>
       <c r="O113" s="7">
-        <v>3413118494.2325883</v>
+        <v>3443632117.1637897</v>
       </c>
       <c r="P113" s="7">
-        <v>3229006691.1692963</v>
+        <v>3257874336.0468941</v>
       </c>
       <c r="Q113" s="7">
-        <v>3054826320.6315656</v>
+        <v>3082136775.4621181</v>
       </c>
       <c r="R113" s="7">
-        <v>2890041657.3135295</v>
+        <v>2915878920.6654305</v>
       </c>
       <c r="S113" s="7">
-        <v>2734145874.21806</v>
+        <v>2758589413.5753279</v>
       </c>
       <c r="T113" s="7">
-        <v>2586659483.8126397</v>
+        <v>2609784479.9924822</v>
       </c>
       <c r="U113" s="7">
-        <v>2447128863.2730246</v>
+        <v>2469006441.658936</v>
       </c>
       <c r="V113" s="7">
-        <v>2315124859.2788057</v>
+        <v>2335822308.5803933</v>
       </c>
       <c r="W113" s="7">
-        <v>2190241468.0696445</v>
+        <v>2209822447.2820263</v>
       </c>
       <c r="X113" s="7">
-        <v>2072094586.7024446</v>
+        <v>2090619320.9017603</v>
       </c>
       <c r="Y113" s="7">
-        <v>1960320831.6687067</v>
+        <v>1977846297.2459493</v>
       </c>
       <c r="Z113" s="7">
-        <v>1854576421.2385006</v>
+        <v>1871156521.1413894</v>
       </c>
       <c r="AA113" s="8">
-        <v>1754536118.0934854</v>
+        <v>1770221847.6153724</v>
       </c>
       <c r="AB113" s="13">
         <f t="shared" si="0"/>
-        <v>235247505786.7988</v>
+        <v>235957294855.79977</v>
       </c>
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.35">
@@ -32641,77 +32641,77 @@
         <v>3432901.1706522219</v>
       </c>
       <c r="E114" s="7">
-        <v>576744.25993909221</v>
+        <v>586943.55120962951</v>
       </c>
       <c r="F114" s="7">
-        <v>537413.39216086571</v>
+        <v>544482.69369743415</v>
       </c>
       <c r="G114" s="7">
-        <v>500172.26736412343</v>
+        <v>503765.14755411987</v>
       </c>
       <c r="H114" s="7">
-        <v>470084.24917425797</v>
+        <v>473832.80704526929</v>
       </c>
       <c r="I114" s="7">
-        <v>442087.6645650561</v>
+        <v>445562.12482346781</v>
       </c>
       <c r="J114" s="7">
-        <v>415945.24274565023</v>
+        <v>415762.15758508717</v>
       </c>
       <c r="K114" s="7">
-        <v>387981.23305202962</v>
+        <v>390644.68198010116</v>
       </c>
       <c r="L114" s="7">
-        <v>362114.51027092419</v>
+        <v>364383.06373319303</v>
       </c>
       <c r="M114" s="7">
-        <v>338054.08501372673</v>
+        <v>340048.38238583517</v>
       </c>
       <c r="N114" s="7">
-        <v>315694.75301221979</v>
+        <v>317363.15505331336</v>
       </c>
       <c r="O114" s="7">
-        <v>294936.85847218492</v>
+        <v>306483.78829670197</v>
       </c>
       <c r="P114" s="7">
-        <v>272288.73371949024</v>
+        <v>283579.30126225657</v>
       </c>
       <c r="Q114" s="7">
-        <v>254455.43994026602</v>
+        <v>262106.26859360407</v>
       </c>
       <c r="R114" s="7">
-        <v>237763.64709179732</v>
+        <v>238544.58685774793</v>
       </c>
       <c r="S114" s="7">
-        <v>217321.48276733322</v>
+        <v>216118.22985416319</v>
       </c>
       <c r="T114" s="7">
-        <v>187502.90308532992</v>
+        <v>185949.56868941316</v>
       </c>
       <c r="U114" s="7">
-        <v>157438.13622872377</v>
+        <v>158558.21074980422</v>
       </c>
       <c r="V114" s="7">
-        <v>129397.81285028625</v>
+        <v>130040.67674229275</v>
       </c>
       <c r="W114" s="7">
-        <v>109204.30504946921</v>
+        <v>112253.84057426534</v>
       </c>
       <c r="X114" s="7">
-        <v>85581.885267116013</v>
+        <v>92542.054345607234</v>
       </c>
       <c r="Y114" s="7">
-        <v>67735.613444999588</v>
+        <v>70765.801900411243</v>
       </c>
       <c r="Z114" s="7">
-        <v>50697.298081056768</v>
+        <v>53564.030898731326</v>
       </c>
       <c r="AA114" s="8">
-        <v>45184.912547502841</v>
+        <v>46187.079874978226</v>
       </c>
       <c r="AB114" s="13">
         <f t="shared" si="0"/>
-        <v>19298682.14363686</v>
+        <v>19382362.661500789</v>
       </c>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.35">
@@ -32728,77 +32728,77 @@
         <v>486368.03270067158</v>
       </c>
       <c r="E115" s="10">
-        <v>82343.131667600042</v>
+        <v>83880.383491353874</v>
       </c>
       <c r="F115" s="10">
-        <v>76617.450556093318</v>
+        <v>77658.109157923158</v>
       </c>
       <c r="G115" s="10">
-        <v>71198.522653960317</v>
+        <v>71689.896576562096</v>
       </c>
       <c r="H115" s="10">
-        <v>66903.876996298874</v>
+        <v>67418.482166606293</v>
       </c>
       <c r="I115" s="10">
-        <v>62915.701870189543</v>
+        <v>63390.48717656736</v>
       </c>
       <c r="J115" s="10">
-        <v>59198.105834500522</v>
+        <v>59091.240699262686</v>
       </c>
       <c r="K115" s="10">
-        <v>55158.560976695881</v>
+        <v>55518.830742947801</v>
       </c>
       <c r="L115" s="10">
-        <v>51418.791960011105</v>
+        <v>51727.908680648172</v>
       </c>
       <c r="M115" s="10">
-        <v>47945.415209059371</v>
+        <v>48214.157293533128</v>
       </c>
       <c r="N115" s="10">
-        <v>44726.207844323944</v>
+        <v>44946.432052306933</v>
       </c>
       <c r="O115" s="10">
-        <v>41747.180130426976</v>
+        <v>43509.878804010223</v>
       </c>
       <c r="P115" s="10">
-        <v>38460.587330246737</v>
+        <v>40185.348984557451</v>
       </c>
       <c r="Q115" s="10">
-        <v>35912.610625071473</v>
+        <v>37071.776120856928</v>
       </c>
       <c r="R115" s="10">
-        <v>33531.294472233516</v>
+        <v>33620.989415176882</v>
       </c>
       <c r="S115" s="10">
-        <v>30554.526034647446</v>
+        <v>30336.421514209964</v>
       </c>
       <c r="T115" s="10">
-        <v>26104.661632058371</v>
+        <v>25833.517252082565</v>
       </c>
       <c r="U115" s="10">
-        <v>21582.548329352503</v>
+        <v>21729.680300148637</v>
       </c>
       <c r="V115" s="10">
-        <v>17427.407022128762</v>
+        <v>17503.246373160084</v>
       </c>
       <c r="W115" s="10">
-        <v>14463.313816512782</v>
+        <v>14905.275486773091</v>
       </c>
       <c r="X115" s="10">
-        <v>10996.213853654594</v>
+        <v>12032.043070180616</v>
       </c>
       <c r="Y115" s="10">
-        <v>8417.0298163735461</v>
+        <v>8859.2032390516433</v>
       </c>
       <c r="Z115" s="10">
-        <v>5955.3186036349607</v>
+        <v>6373.6401306776006</v>
       </c>
       <c r="AA115" s="11">
-        <v>5306.9581682588787</v>
+        <v>5424.8389010064175</v>
       </c>
       <c r="AB115" s="14">
         <f t="shared" si="0"/>
-        <v>2734368.0551614449</v>
+        <v>2746404.4273877153</v>
       </c>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fixed reserves to include storage
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfi\Google Drive\School\College\Semester 6 (Spring 2020)\ENV 717\Assignments\Assignment 11 (group project)\ENV717A11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jawessel\opl\ENV717A11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="AE3" s="3">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AF3" s="4">
         <v>0</v>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="BG3" s="3">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BH3" s="4">
         <v>0</v>
@@ -1395,19 +1395,19 @@
         <v>0</v>
       </c>
       <c r="I4" s="7">
-        <v>48.147894881528721</v>
+        <v>0</v>
       </c>
       <c r="J4" s="7">
-        <v>410.09394605356465</v>
+        <v>410.09700160914394</v>
       </c>
       <c r="K4" s="7">
-        <v>280.8164360819776</v>
+        <v>665.6</v>
       </c>
       <c r="L4" s="7">
-        <v>173.0273917286288</v>
+        <v>665.6</v>
       </c>
       <c r="M4" s="7">
-        <v>544.2280930486229</v>
+        <v>544.2260597153072</v>
       </c>
       <c r="N4" s="7">
         <v>665.6</v>
@@ -1422,7 +1422,7 @@
         <v>663.23839761471152</v>
       </c>
       <c r="R4" s="7">
-        <v>624.81603079324384</v>
+        <v>624.81603079324429</v>
       </c>
       <c r="S4" s="7">
         <v>586.78261502038242</v>
@@ -1437,7 +1437,7 @@
         <v>475.05123739653379</v>
       </c>
       <c r="W4" s="7">
-        <v>438.60894788310145</v>
+        <v>438.60894788310162</v>
       </c>
       <c r="X4" s="7">
         <v>402.57343011404885</v>
@@ -1476,34 +1476,34 @@
         <v>0</v>
       </c>
       <c r="AL4" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AM4" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AN4" s="7">
-        <v>1E-3</v>
+        <v>73.906010576332051</v>
       </c>
       <c r="AO4" s="7">
-        <v>466.89025390403492</v>
+        <v>0</v>
       </c>
       <c r="AP4" s="7">
-        <v>432.15588103917105</v>
+        <v>432.15688103917074</v>
       </c>
       <c r="AQ4" s="7">
-        <v>397.84465116852346</v>
+        <v>397.844651168523</v>
       </c>
       <c r="AR4" s="7">
-        <v>363.95836357903966</v>
+        <v>363.9583635790392</v>
       </c>
       <c r="AS4" s="7">
-        <v>330.50185175125091</v>
+        <v>330.50185175125023</v>
       </c>
       <c r="AT4" s="7">
-        <v>297.47898366701088</v>
+        <v>297.47898366701077</v>
       </c>
       <c r="AU4" s="7">
-        <v>264.89366212001278</v>
+        <v>264.89366212001295</v>
       </c>
       <c r="AV4" s="7">
         <v>232.74982502909268</v>
@@ -1518,7 +1518,7 @@
         <v>139.00713321688727</v>
       </c>
       <c r="AZ4" s="7">
-        <v>108.66932676583849</v>
+        <v>108.66932676583866</v>
       </c>
       <c r="BA4" s="7">
         <v>78.793232406730453</v>
@@ -1539,7 +1539,7 @@
         <v>665.6</v>
       </c>
       <c r="BH4" s="7">
-        <v>577.59406771433612</v>
+        <v>665.6</v>
       </c>
       <c r="BI4" s="7">
         <v>665.6</v>
@@ -1557,31 +1557,31 @@
         <v>0</v>
       </c>
       <c r="BN4" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BO4" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BP4" s="7">
-        <v>387.57249120147515</v>
+        <v>0</v>
       </c>
       <c r="BQ4" s="7">
-        <v>364.21450612228762</v>
+        <v>364.21550612228748</v>
       </c>
       <c r="BR4" s="7">
-        <v>341.3810515273866</v>
+        <v>341.38205152738703</v>
       </c>
       <c r="BS4" s="7">
-        <v>319.07784819113306</v>
+        <v>319.07784819113249</v>
       </c>
       <c r="BT4" s="7">
-        <v>297.30765937485307</v>
+        <v>297.30765937485239</v>
       </c>
       <c r="BU4" s="7">
-        <v>276.07629120922707</v>
+        <v>276.07629120922559</v>
       </c>
       <c r="BV4" s="7">
-        <v>255.38859308010728</v>
+        <v>255.38859308010706</v>
       </c>
       <c r="BW4" s="7">
         <v>235.24945801782724</v>
@@ -1596,10 +1596,10 @@
         <v>178.17302447597558</v>
       </c>
       <c r="CA4" s="7">
-        <v>160.27795869625879</v>
+        <v>160.27795869625868</v>
       </c>
       <c r="CB4" s="7">
-        <v>142.95658967452414</v>
+        <v>142.95658967452448</v>
       </c>
       <c r="CC4" s="7">
         <v>126.21408068159371</v>
@@ -1620,10 +1620,10 @@
         <v>665.6</v>
       </c>
       <c r="CJ4" s="7">
-        <v>665.6</v>
+        <v>577.5940677143883</v>
       </c>
       <c r="CK4" s="7">
-        <v>488.11619368583524</v>
+        <v>488.11619368587753</v>
       </c>
       <c r="CL4" s="7">
         <v>0</v>
@@ -1638,16 +1638,16 @@
         <v>0</v>
       </c>
       <c r="CP4" s="7">
-        <v>1E-3</v>
+        <v>47.104190644998198</v>
       </c>
       <c r="CQ4" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="CR4" s="7">
-        <v>61.947907875331573</v>
+        <v>0</v>
       </c>
       <c r="CS4" s="7">
-        <v>22.83430154620919</v>
+        <v>2.7841532945328709</v>
       </c>
       <c r="CT4" s="7">
         <v>0</v>
@@ -2182,7 +2182,7 @@
         <v>212</v>
       </c>
       <c r="BD6" s="8">
-        <v>203.97696329930955</v>
+        <v>203.97696329930943</v>
       </c>
       <c r="BF6">
         <v>4</v>
@@ -2302,19 +2302,19 @@
         <v>212</v>
       </c>
       <c r="CT6" s="7">
-        <v>196.10442511012445</v>
+        <v>196.10442511012468</v>
       </c>
       <c r="CU6" s="7">
-        <v>157.75972313611535</v>
+        <v>157.75972313611487</v>
       </c>
       <c r="CV6" s="7">
-        <v>119.80467119434003</v>
+        <v>119.80467119433956</v>
       </c>
       <c r="CW6" s="7">
-        <v>82.242776135088462</v>
+        <v>82.242776135087979</v>
       </c>
       <c r="CX6" s="7">
-        <v>45.077576370303419</v>
+        <v>45.077576370303063</v>
       </c>
       <c r="CY6" s="7">
         <v>8.3126421576345138</v>
@@ -3298,7 +3298,7 @@
         <v>84.6</v>
       </c>
       <c r="CZ9" s="7">
-        <v>56.551575887052991</v>
+        <v>56.551575887053218</v>
       </c>
       <c r="DA9" s="7">
         <v>20.598012370036372</v>
@@ -3692,13 +3692,13 @@
         <v>0</v>
       </c>
       <c r="N11" s="7">
-        <v>30.373943645047163</v>
+        <v>0</v>
       </c>
       <c r="O11" s="7">
-        <v>75.636138007303089</v>
+        <v>75.636138007302861</v>
       </c>
       <c r="P11" s="7">
-        <v>36.446246149368548</v>
+        <v>36.446246149368335</v>
       </c>
       <c r="Q11" s="7">
         <v>0</v>
@@ -3731,7 +3731,7 @@
         <v>0</v>
       </c>
       <c r="AA11" s="8">
-        <v>296.94428176925294</v>
+        <v>296.94428176925288</v>
       </c>
       <c r="AD11">
         <v>9</v>
@@ -3893,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="CF11" s="8">
-        <v>79.512046138523402</v>
+        <v>79.512046138523601</v>
       </c>
       <c r="CH11">
         <v>9</v>
@@ -4144,7 +4144,7 @@
         <v>10</v>
       </c>
       <c r="BG12" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BH12" s="7">
         <v>0</v>
@@ -4225,7 +4225,7 @@
         <v>10</v>
       </c>
       <c r="CI12" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="CJ12" s="7">
         <v>0</v>
@@ -4796,7 +4796,7 @@
         <v>12</v>
       </c>
       <c r="BG14" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BH14" s="7">
         <v>0</v>
@@ -4972,7 +4972,7 @@
         <v>1328.4125743419984</v>
       </c>
       <c r="F15" s="7">
-        <v>1235.5847469110761</v>
+        <v>1235.5847469110763</v>
       </c>
       <c r="G15" s="7">
         <v>1143.1062213832749</v>
@@ -4981,22 +4981,22 @@
         <v>1050.9801414757246</v>
       </c>
       <c r="I15" s="7">
-        <v>936.06178431747719</v>
+        <v>984.20967919900556</v>
       </c>
       <c r="J15" s="7">
-        <v>532.70408905823183</v>
+        <v>532.70103350265208</v>
       </c>
       <c r="K15" s="7">
-        <v>620.93200249582446</v>
+        <v>236.14843857780193</v>
       </c>
       <c r="L15" s="7">
-        <v>688.03675629637291</v>
+        <v>195.4641480250018</v>
       </c>
       <c r="M15" s="7">
-        <v>276.52035815860347</v>
+        <v>276.52239149191905</v>
       </c>
       <c r="N15" s="7">
-        <v>84.830721823043532</v>
+        <v>115.20466546809064</v>
       </c>
       <c r="O15" s="7">
         <v>0</v>
@@ -5044,7 +5044,7 @@
         <v>1848</v>
       </c>
       <c r="AF15" s="7">
-        <v>972.2866999999992</v>
+        <v>972.28669999999909</v>
       </c>
       <c r="AG15" s="7">
         <v>828.91851499999871</v>
@@ -5062,19 +5062,19 @@
         <v>644.97536933821607</v>
       </c>
       <c r="AL15" s="7">
-        <v>573.58874411225986</v>
+        <v>573.5897441122595</v>
       </c>
       <c r="AM15" s="7">
-        <v>537.6104006092695</v>
+        <v>537.61140060926903</v>
       </c>
       <c r="AN15" s="7">
-        <v>502.04300436475233</v>
+        <v>428.13799378842009</v>
       </c>
       <c r="AO15" s="7">
-        <v>1E-3</v>
+        <v>466.89125390403444</v>
       </c>
       <c r="AP15" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AQ15" s="7">
         <v>0</v>
@@ -5125,7 +5125,7 @@
         <v>1848</v>
       </c>
       <c r="BH15" s="7">
-        <v>1215.1736322856632</v>
+        <v>1127.1676999999988</v>
       </c>
       <c r="BI15" s="7">
         <v>949.7784439999989</v>
@@ -5143,19 +5143,19 @@
         <v>510.74805097093395</v>
       </c>
       <c r="BN15" s="7">
-        <v>435.84337987967172</v>
+        <v>435.84437987967135</v>
       </c>
       <c r="BO15" s="7">
-        <v>411.45032809858856</v>
+        <v>411.45132809858819</v>
       </c>
       <c r="BP15" s="7">
-        <v>1E-3</v>
+        <v>387.57349120147478</v>
       </c>
       <c r="BQ15" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BR15" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BS15" s="7">
         <v>0</v>
@@ -5206,34 +5206,34 @@
         <v>1848</v>
       </c>
       <c r="CJ15" s="7">
-        <v>562.63269999999955</v>
+        <v>650.63863228561127</v>
       </c>
       <c r="CK15" s="7">
-        <v>593.06143531416342</v>
+        <v>593.06143531412113</v>
       </c>
       <c r="CL15" s="7">
-        <v>549.47881471099834</v>
+        <v>549.47881471099845</v>
       </c>
       <c r="CM15" s="7">
-        <v>438.13946344339718</v>
+        <v>438.13946344339729</v>
       </c>
       <c r="CN15" s="7">
-        <v>327.16181036438684</v>
+        <v>327.16181036438661</v>
       </c>
       <c r="CO15" s="7">
         <v>216.55211975766622</v>
       </c>
       <c r="CP15" s="7">
-        <v>141.30968528548553</v>
+        <v>94.206494640486994</v>
       </c>
       <c r="CQ15" s="7">
-        <v>101.44083025305419</v>
+        <v>101.44183025305358</v>
       </c>
       <c r="CR15" s="7">
-        <v>1E-3</v>
+        <v>61.948907875331201</v>
       </c>
       <c r="CS15" s="7">
-        <v>1E-3</v>
+        <v>20.051148251675841</v>
       </c>
       <c r="CT15" s="7">
         <v>0</v>
@@ -5286,7 +5286,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -5367,7 +5367,7 @@
         <v>14</v>
       </c>
       <c r="AE16" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AF16" s="7">
         <v>0</v>
@@ -5448,7 +5448,7 @@
         <v>14</v>
       </c>
       <c r="BG16" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BH16" s="7">
         <v>0</v>
@@ -5529,7 +5529,7 @@
         <v>14</v>
       </c>
       <c r="CI16" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="CJ16" s="7">
         <v>0</v>
@@ -6019,7 +6019,7 @@
         <v>16</v>
       </c>
       <c r="AE18" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AF18" s="7">
         <v>0</v>
@@ -6181,7 +6181,7 @@
         <v>16</v>
       </c>
       <c r="CI18" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="CJ18" s="7">
         <v>0</v>
@@ -6264,7 +6264,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>31.358850000000206</v>
+        <v>31.360850000000028</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
@@ -6507,7 +6507,7 @@
         <v>17</v>
       </c>
       <c r="CI19" s="6">
-        <v>128.03685000000021</v>
+        <v>128.03984999999963</v>
       </c>
       <c r="CJ19" s="7">
         <v>0</v>
@@ -6590,7 +6590,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
@@ -6671,7 +6671,7 @@
         <v>18</v>
       </c>
       <c r="AE20" s="6">
-        <v>277.03785000000028</v>
+        <v>277.04084999999975</v>
       </c>
       <c r="AF20" s="7">
         <v>0</v>
@@ -6752,7 +6752,7 @@
         <v>18</v>
       </c>
       <c r="BG20" s="6">
-        <v>1486.0358499999993</v>
+        <v>1486.0408500000001</v>
       </c>
       <c r="BH20" s="7">
         <v>0</v>
@@ -7404,7 +7404,7 @@
         <v>20</v>
       </c>
       <c r="BG22" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BH22" s="7">
         <v>0</v>
@@ -7616,7 +7616,7 @@
         <v>10.537500000000001</v>
       </c>
       <c r="R23" s="7">
-        <v>10.537500000000001</v>
+        <v>10.537500000000003</v>
       </c>
       <c r="S23" s="7">
         <v>10.537500000000001</v>
@@ -7874,16 +7874,16 @@
         <v>14.752500000000001</v>
       </c>
       <c r="DD23" s="7">
-        <v>14.752500000000001</v>
+        <v>0</v>
       </c>
       <c r="DE23" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF23" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG23" s="7">
-        <v>1E-3</v>
+        <v>4.4793977321508303</v>
       </c>
       <c r="DH23" s="8">
         <v>5.7654135617385691</v>
@@ -7966,7 +7966,7 @@
         <v>9.375</v>
       </c>
       <c r="Z24" s="7">
-        <v>9.375</v>
+        <v>9.3750000000000018</v>
       </c>
       <c r="AA24" s="8">
         <v>9.375</v>
@@ -8200,16 +8200,16 @@
         <v>13.125</v>
       </c>
       <c r="DD24" s="7">
-        <v>1E-3</v>
+        <v>13.125</v>
       </c>
       <c r="DE24" s="7">
-        <v>1E-3</v>
+        <v>13.125</v>
       </c>
       <c r="DF24" s="7">
-        <v>13.11576098330206</v>
+        <v>0</v>
       </c>
       <c r="DG24" s="7">
-        <v>1E-3</v>
+        <v>13.125</v>
       </c>
       <c r="DH24" s="8">
         <v>0</v>
@@ -8268,7 +8268,7 @@
         <v>26.25</v>
       </c>
       <c r="R25" s="7">
-        <v>26.25</v>
+        <v>26.250000000000007</v>
       </c>
       <c r="S25" s="7">
         <v>26.25</v>
@@ -8529,13 +8529,13 @@
         <v>36.75</v>
       </c>
       <c r="DE25" s="7">
-        <v>20.676633234194483</v>
+        <v>23.312633234194323</v>
       </c>
       <c r="DF25" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG25" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH25" s="8">
         <v>0</v>
@@ -8756,7 +8756,7 @@
         <v>16.065000000000001</v>
       </c>
       <c r="BW26" s="7">
-        <v>16.065000000000001</v>
+        <v>16.065000000000005</v>
       </c>
       <c r="BX26" s="7">
         <v>16.065000000000001</v>
@@ -8858,10 +8858,10 @@
         <v>16.065000000000001</v>
       </c>
       <c r="DF26" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG26" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH26" s="8">
         <v>0</v>
@@ -8947,7 +8947,7 @@
         <v>3.75</v>
       </c>
       <c r="AA27" s="8">
-        <v>3.75</v>
+        <v>3.7500000000000009</v>
       </c>
       <c r="AD27">
         <v>25</v>
@@ -9178,16 +9178,16 @@
         <v>5.25</v>
       </c>
       <c r="DD27" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DE27" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DF27" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG27" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH27" s="8">
         <v>0</v>
@@ -9501,19 +9501,19 @@
         <v>5.25</v>
       </c>
       <c r="DC28" s="7">
-        <v>5.25</v>
+        <v>4.6330967035479489</v>
       </c>
       <c r="DD28" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DE28" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF28" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG28" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH28" s="8">
         <v>0</v>
@@ -9824,22 +9824,22 @@
         <v>5.25</v>
       </c>
       <c r="DB29" s="7">
-        <v>5.25</v>
+        <v>1.8556191313658701</v>
       </c>
       <c r="DC29" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DD29" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DE29" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DF29" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG29" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH29" s="8">
         <v>0</v>
@@ -10153,19 +10153,19 @@
         <v>27.405000000000001</v>
       </c>
       <c r="DC30" s="7">
-        <v>10.299096703548093</v>
+        <v>0</v>
       </c>
       <c r="DD30" s="7">
-        <v>27.405000000000001</v>
+        <v>0</v>
       </c>
       <c r="DE30" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF30" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG30" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH30" s="8">
         <v>0</v>
@@ -10476,22 +10476,22 @@
         <v>5.25</v>
       </c>
       <c r="DB31" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DC31" s="7">
         <v>5.25</v>
       </c>
       <c r="DD31" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DE31" s="7">
-        <v>1E-3</v>
+        <v>5.25</v>
       </c>
       <c r="DF31" s="7">
-        <v>1E-3</v>
+        <v>5.25</v>
       </c>
       <c r="DG31" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH31" s="8">
         <v>0</v>
@@ -10802,22 +10802,22 @@
         <v>10.604999999999999</v>
       </c>
       <c r="DB32" s="7">
-        <v>6.2111191313661935</v>
+        <v>10.604999999999999</v>
       </c>
       <c r="DC32" s="7">
-        <v>1E-3</v>
+        <v>10.604999999999999</v>
       </c>
       <c r="DD32" s="7">
-        <v>1E-3</v>
+        <v>10.604999999999999</v>
       </c>
       <c r="DE32" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF32" s="7">
-        <v>1E-3</v>
+        <v>10.604999999999999</v>
       </c>
       <c r="DG32" s="7">
-        <v>1E-3</v>
+        <v>10.604999999999999</v>
       </c>
       <c r="DH32" s="8">
         <v>0</v>
@@ -11134,7 +11134,7 @@
         <v>36.75</v>
       </c>
       <c r="DD33" s="7">
-        <v>1E-3</v>
+        <v>36.75</v>
       </c>
       <c r="DE33" s="7">
         <v>36.75</v>
@@ -11143,7 +11143,7 @@
         <v>36.75</v>
       </c>
       <c r="DG33" s="7">
-        <v>27.194897732151151</v>
+        <v>0</v>
       </c>
       <c r="DH33" s="8">
         <v>0</v>
@@ -11457,19 +11457,19 @@
         <v>5.5124999999999993</v>
       </c>
       <c r="DC34" s="7">
-        <v>1E-3</v>
+        <v>5.5124999999999993</v>
       </c>
       <c r="DD34" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DE34" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF34" s="7">
-        <v>5.5124999999999993</v>
+        <v>2.6822609833018989</v>
       </c>
       <c r="DG34" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH34" s="8">
         <v>0</v>
@@ -11783,19 +11783,19 @@
         <v>5.25</v>
       </c>
       <c r="DC35" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DD35" s="7">
         <v>5.25</v>
       </c>
       <c r="DE35" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DF35" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG35" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH35" s="8">
         <v>0</v>
@@ -12112,16 +12112,16 @@
         <v>5.25</v>
       </c>
       <c r="DD36" s="7">
-        <v>1E-3</v>
+        <v>5.25</v>
       </c>
       <c r="DE36" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF36" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG36" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH36" s="8">
         <v>0</v>
@@ -12198,7 +12198,7 @@
         <v>3.75</v>
       </c>
       <c r="X37" s="7">
-        <v>3.75</v>
+        <v>3.7500000000000009</v>
       </c>
       <c r="Y37" s="7">
         <v>3.75</v>
@@ -12435,19 +12435,19 @@
         <v>5.25</v>
       </c>
       <c r="DC37" s="7">
-        <v>1E-3</v>
+        <v>5.25</v>
       </c>
       <c r="DD37" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DE37" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF37" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DG37" s="7">
-        <v>1E-3</v>
+        <v>5.25</v>
       </c>
       <c r="DH37" s="8">
         <v>0</v>
@@ -12503,7 +12503,7 @@
         <v>3.75</v>
       </c>
       <c r="Q38" s="7">
-        <v>3.75</v>
+        <v>3.7500000000000009</v>
       </c>
       <c r="R38" s="7">
         <v>3.75</v>
@@ -12758,22 +12758,22 @@
         <v>5.25</v>
       </c>
       <c r="DB38" s="7">
-        <v>1E-3</v>
+        <v>5.25</v>
       </c>
       <c r="DC38" s="7">
         <v>5.25</v>
       </c>
       <c r="DD38" s="7">
-        <v>1E-3</v>
+        <v>5.25</v>
       </c>
       <c r="DE38" s="7">
         <v>5.25</v>
       </c>
       <c r="DF38" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DG38" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DH38" s="8">
         <v>0</v>
@@ -12829,7 +12829,7 @@
         <v>3.7874999999999996</v>
       </c>
       <c r="Q39" s="7">
-        <v>3.7874999999999996</v>
+        <v>3.7875000000000005</v>
       </c>
       <c r="R39" s="7">
         <v>3.7874999999999996</v>
@@ -13090,16 +13090,16 @@
         <v>5.3024999999999993</v>
       </c>
       <c r="DD39" s="7">
-        <v>3.307178923879766</v>
+        <v>5.3024999999999993</v>
       </c>
       <c r="DE39" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF39" s="7">
-        <v>1E-3</v>
+        <v>5.3024999999999993</v>
       </c>
       <c r="DG39" s="7">
-        <v>1E-3</v>
+        <v>5.3024999999999993</v>
       </c>
       <c r="DH39" s="8">
         <v>0</v>
@@ -13182,7 +13182,7 @@
         <v>3.7874999999999996</v>
       </c>
       <c r="Z40" s="7">
-        <v>3.7874999999999996</v>
+        <v>3.7875000000000005</v>
       </c>
       <c r="AA40" s="8">
         <v>3.7874999999999996</v>
@@ -13410,22 +13410,22 @@
         <v>5.3024999999999993</v>
       </c>
       <c r="DB40" s="7">
-        <v>1E-3</v>
+        <v>5.3024999999999993</v>
       </c>
       <c r="DC40" s="7">
-        <v>1E-3</v>
+        <v>5.3024999999999993</v>
       </c>
       <c r="DD40" s="7">
         <v>5.3024999999999993</v>
       </c>
       <c r="DE40" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DF40" s="7">
-        <v>1E-3</v>
+        <v>5.3024999999999993</v>
       </c>
       <c r="DG40" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH40" s="8">
         <v>0</v>
@@ -13739,19 +13739,19 @@
         <v>5.25</v>
       </c>
       <c r="DC41" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DD41" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DE41" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DF41" s="7">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="DG41" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DH41" s="8">
         <v>0</v>
@@ -14062,13 +14062,13 @@
         <v>6.3</v>
       </c>
       <c r="DB42" s="7">
-        <v>6.3</v>
+        <v>0</v>
       </c>
       <c r="DC42" s="7">
         <v>0</v>
       </c>
       <c r="DD42" s="7">
-        <v>1E-3</v>
+        <v>0.68917892387946722</v>
       </c>
       <c r="DE42" s="7">
         <v>6.3</v>
@@ -14077,7 +14077,7 @@
         <v>6.3</v>
       </c>
       <c r="DG42" s="7">
-        <v>6.3</v>
+        <v>0</v>
       </c>
       <c r="DH42" s="8">
         <v>0</v>
@@ -15993,7 +15993,7 @@
         <v>0</v>
       </c>
       <c r="CF50" s="5">
-        <v>170.05631831400279</v>
+        <v>170.0563183140024</v>
       </c>
       <c r="CH50">
         <v>1</v>
@@ -17063,13 +17063,13 @@
         <v>464</v>
       </c>
       <c r="C54" s="7">
-        <v>136.05569999999989</v>
+        <v>136.05569999999955</v>
       </c>
       <c r="D54" s="7">
-        <v>88.252355999999509</v>
+        <v>88.25235599999894</v>
       </c>
       <c r="E54" s="7">
-        <v>38.566336503728053</v>
+        <v>38.566336503828893</v>
       </c>
       <c r="F54" s="7">
         <v>0</v>
@@ -17102,7 +17102,7 @@
         <v>0</v>
       </c>
       <c r="P54" s="7">
-        <v>168.52885022722467</v>
+        <v>464</v>
       </c>
       <c r="Q54" s="7">
         <v>464</v>
@@ -17144,49 +17144,49 @@
         <v>464</v>
       </c>
       <c r="AF54" s="7">
-        <v>462.9716999999996</v>
+        <v>462.97169999999937</v>
       </c>
       <c r="AG54" s="7">
-        <v>418.11059999999907</v>
+        <v>418.1105999999985</v>
       </c>
       <c r="AH54" s="7">
-        <v>116.58050244999868</v>
+        <v>116.58050244999833</v>
       </c>
       <c r="AI54" s="7">
-        <v>142.53341851513505</v>
+        <v>142.53341851521805</v>
       </c>
       <c r="AJ54" s="7">
-        <v>74.659166947035374</v>
+        <v>74.659166947106769</v>
       </c>
       <c r="AK54" s="7">
         <v>1E-3</v>
       </c>
       <c r="AL54" s="7">
-        <v>198.8301208089506</v>
+        <v>198.83012080895026</v>
       </c>
       <c r="AM54" s="7">
-        <v>156.00026069623073</v>
+        <v>156.00026069623004</v>
       </c>
       <c r="AN54" s="7">
         <v>113.51968419249624</v>
       </c>
       <c r="AO54" s="7">
-        <v>71.391534850228709</v>
+        <v>71.391534850228254</v>
       </c>
       <c r="AP54" s="7">
-        <v>29.618984513880605</v>
+        <v>29.618984513879923</v>
       </c>
       <c r="AQ54" s="7">
         <v>0</v>
       </c>
       <c r="AR54" s="7">
-        <v>95.199081208019379</v>
+        <v>95.199081208057237</v>
       </c>
       <c r="AS54" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="AT54" s="7">
-        <v>464</v>
+        <v>192.45258368267423</v>
       </c>
       <c r="AU54" s="7">
         <v>464</v>
@@ -17306,10 +17306,10 @@
         <v>464</v>
       </c>
       <c r="CJ54" s="7">
-        <v>190.54169999999976</v>
+        <v>190.54169999999937</v>
       </c>
       <c r="CK54" s="7">
-        <v>143.22872999999936</v>
+        <v>143.22872999999885</v>
       </c>
       <c r="CL54" s="7">
         <v>1E-3</v>
@@ -17345,10 +17345,10 @@
         <v>0</v>
       </c>
       <c r="CW54" s="7">
-        <v>0</v>
+        <v>169.90865783100173</v>
       </c>
       <c r="CX54" s="7">
-        <v>195.40418603392516</v>
+        <v>464</v>
       </c>
       <c r="CY54" s="7">
         <v>464</v>
@@ -18376,31 +18376,31 @@
         <v>650</v>
       </c>
       <c r="F58" s="7">
-        <v>643.56197546228486</v>
+        <v>643.56197546228452</v>
       </c>
       <c r="G58" s="7">
-        <v>596.68044499144526</v>
+        <v>596.6804449914448</v>
       </c>
       <c r="H58" s="7">
         <v>550.11173309636752</v>
       </c>
       <c r="I58" s="7">
-        <v>503.85865514423494</v>
+        <v>503.85865514423438</v>
       </c>
       <c r="J58" s="7">
-        <v>457.92405184053223</v>
+        <v>457.924051840532</v>
       </c>
       <c r="K58" s="7">
-        <v>412.31078945709623</v>
+        <v>412.31078945709646</v>
       </c>
       <c r="L58" s="7">
-        <v>367.02176006220998</v>
+        <v>367.02176006220975</v>
       </c>
       <c r="M58" s="7">
-        <v>322.05988175276934</v>
+        <v>322.05988175276877</v>
       </c>
       <c r="N58" s="7">
-        <v>650</v>
+        <v>391.36234465603411</v>
       </c>
       <c r="O58" s="7">
         <v>650</v>
@@ -18625,25 +18625,25 @@
         <v>650</v>
       </c>
       <c r="CO58" s="7">
-        <v>567.96952832778084</v>
+        <v>567.96952832785132</v>
       </c>
       <c r="CP58" s="7">
-        <v>561.35389942168695</v>
+        <v>561.35389942168638</v>
       </c>
       <c r="CQ58" s="7">
         <v>515.93675331648092</v>
       </c>
       <c r="CR58" s="7">
-        <v>470.84560524632934</v>
+        <v>470.84560524632917</v>
       </c>
       <c r="CS58" s="7">
-        <v>426.08338919354583</v>
+        <v>426.08338919354566</v>
       </c>
       <c r="CT58" s="7">
-        <v>381.65306554628705</v>
+        <v>381.6530655462866</v>
       </c>
       <c r="CU58" s="7">
-        <v>337.55762133620306</v>
+        <v>650</v>
       </c>
       <c r="CV58" s="7">
         <v>650</v>
@@ -18828,7 +18828,7 @@
         <v>0</v>
       </c>
       <c r="AX59" s="7">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="AY59" s="7">
         <v>186</v>
@@ -18909,7 +18909,7 @@
         <v>0</v>
       </c>
       <c r="BZ59" s="7">
-        <v>156.0155105216304</v>
+        <v>0</v>
       </c>
       <c r="CA59" s="7">
         <v>186</v>
@@ -18990,7 +18990,7 @@
         <v>0</v>
       </c>
       <c r="DB59" s="7">
-        <v>186</v>
+        <v>158.03724965208562</v>
       </c>
       <c r="DC59" s="7">
         <v>186</v>
@@ -19668,7 +19668,7 @@
         <v>13</v>
       </c>
       <c r="B62" s="6">
-        <v>1568.1608500000002</v>
+        <v>1568.1608499999998</v>
       </c>
       <c r="C62" s="7">
         <v>1848</v>
@@ -19704,22 +19704,22 @@
         <v>1848</v>
       </c>
       <c r="N62" s="7">
-        <v>1475.4280988885434</v>
+        <v>1734.0657542325093</v>
       </c>
       <c r="O62" s="7">
-        <v>1431.12938232854</v>
+        <v>1431.1293823285398</v>
       </c>
       <c r="P62" s="7">
-        <v>1218.6378794422717</v>
+        <v>923.16672966949591</v>
       </c>
       <c r="Q62" s="7">
-        <v>879.54316548652105</v>
+        <v>879.54316548652082</v>
       </c>
       <c r="R62" s="7">
         <v>789.76174157589867</v>
       </c>
       <c r="S62" s="7">
-        <v>43.39739736394904</v>
+        <v>422.82553720008127</v>
       </c>
       <c r="T62" s="7">
         <v>0</v>
@@ -19785,25 +19785,25 @@
         <v>1848</v>
       </c>
       <c r="AQ62" s="7">
-        <v>1836.2052335745047</v>
+        <v>1836.2052335745043</v>
       </c>
       <c r="AR62" s="7">
-        <v>1699.9544300186553</v>
+        <v>1699.9544300186169</v>
       </c>
       <c r="AS62" s="7">
-        <v>1290.4670757277145</v>
+        <v>1754.467075727714</v>
       </c>
       <c r="AT62" s="7">
-        <v>1250.1492146592636</v>
+        <v>1521.6966309765892</v>
       </c>
       <c r="AU62" s="7">
         <v>1163.7032451911955</v>
       </c>
       <c r="AV62" s="7">
-        <v>800.13251434791619</v>
+        <v>800.13251434791596</v>
       </c>
       <c r="AW62" s="7">
-        <v>0</v>
+        <v>760.94039927704659</v>
       </c>
       <c r="AX62" s="7">
         <v>0</v>
@@ -19881,10 +19881,10 @@
         <v>1848</v>
       </c>
       <c r="BX62" s="7">
-        <v>1848</v>
+        <v>1476.8202979862906</v>
       </c>
       <c r="BY62" s="7">
-        <v>481.50834888635967</v>
+        <v>172.52715689762886</v>
       </c>
       <c r="BZ62" s="7">
         <v>0</v>
@@ -19911,7 +19911,7 @@
         <v>13</v>
       </c>
       <c r="CI62" s="6">
-        <v>1622.1608500000002</v>
+        <v>1622.16085</v>
       </c>
       <c r="CJ62" s="7">
         <v>1848</v>
@@ -19947,25 +19947,25 @@
         <v>1848</v>
       </c>
       <c r="CU62" s="7">
-        <v>1848</v>
+        <v>1535.5576213362031</v>
       </c>
       <c r="CV62" s="7">
         <v>1491.800070478228</v>
       </c>
       <c r="CW62" s="7">
-        <v>1448.3834540125317</v>
+        <v>1278.4747961815301</v>
       </c>
       <c r="CX62" s="7">
-        <v>1209.9066543147192</v>
+        <v>941.31084034864421</v>
       </c>
       <c r="CY62" s="7">
-        <v>852.08532551178268</v>
+        <v>852.08532551178155</v>
       </c>
       <c r="CZ62" s="7">
         <v>485.71003339138747</v>
       </c>
       <c r="DA62" s="7">
-        <v>443.68811599190917</v>
+        <v>0</v>
       </c>
       <c r="DB62" s="7">
         <v>0</v>
@@ -20063,13 +20063,13 @@
         <v>0</v>
       </c>
       <c r="Y63" s="7">
-        <v>167.39809833421143</v>
+        <v>243.63388337319964</v>
       </c>
       <c r="Z63" s="7">
-        <v>203.20279472355833</v>
+        <v>203.2027947235581</v>
       </c>
       <c r="AA63" s="8">
-        <v>163.14257862606974</v>
+        <v>163.14257862606928</v>
       </c>
       <c r="AD63">
         <v>14</v>
@@ -20138,19 +20138,19 @@
         <v>0</v>
       </c>
       <c r="AZ63" s="7">
-        <v>0</v>
+        <v>361.58447731637409</v>
       </c>
       <c r="BA63" s="7">
-        <v>278.51300167350496</v>
+        <v>278.51300167352201</v>
       </c>
       <c r="BB63" s="7">
-        <v>641.77940366652183</v>
+        <v>641.77940366652172</v>
       </c>
       <c r="BC63" s="7">
-        <v>604.9316246995204</v>
+        <v>604.93162469952006</v>
       </c>
       <c r="BD63" s="8">
-        <v>568.48696807181568</v>
+        <v>568.48696807181545</v>
       </c>
       <c r="BF63">
         <v>14</v>
@@ -20216,16 +20216,16 @@
         <v>0</v>
       </c>
       <c r="CA63" s="7">
-        <v>0</v>
+        <v>161.24800123170291</v>
       </c>
       <c r="CB63" s="7">
-        <v>357.6542112585696</v>
+        <v>0</v>
       </c>
       <c r="CC63" s="7">
         <v>656.1</v>
       </c>
       <c r="CD63" s="7">
-        <v>656.1</v>
+        <v>581.52151463578014</v>
       </c>
       <c r="CE63" s="7">
         <v>656.1</v>
@@ -20297,13 +20297,13 @@
         <v>0</v>
       </c>
       <c r="DC63" s="7">
-        <v>161.24800123168723</v>
+        <v>0</v>
       </c>
       <c r="DD63" s="7">
-        <v>390.77455921822911</v>
+        <v>390.77455921822923</v>
       </c>
       <c r="DE63" s="7">
-        <v>350.19823195119238</v>
+        <v>350.1982319511925</v>
       </c>
       <c r="DF63" s="7">
         <v>309.99147008875298</v>
@@ -20312,7 +20312,7 @@
         <v>270.1575997195514</v>
       </c>
       <c r="DH63" s="8">
-        <v>230.69997686702663</v>
+        <v>230.69997686702629</v>
       </c>
     </row>
     <row r="64" spans="1:112" x14ac:dyDescent="0.35">
@@ -20856,7 +20856,7 @@
         <v>0</v>
       </c>
       <c r="BW65" s="7">
-        <v>17.765923041190263</v>
+        <v>17.765923041217775</v>
       </c>
       <c r="BX65" s="7">
         <v>67</v>
@@ -20981,7 +20981,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="7">
-        <v>2.1871977502710251</v>
+        <v>2.1871977501696165</v>
       </c>
       <c r="F66" s="7">
         <v>0</v>
@@ -21053,7 +21053,7 @@
         <v>17</v>
       </c>
       <c r="AE66" s="6">
-        <v>44.16085000000021</v>
+        <v>44.160849999999868</v>
       </c>
       <c r="AF66" s="7">
         <v>0</v>
@@ -21065,13 +21065,13 @@
         <v>257</v>
       </c>
       <c r="AI66" s="7">
-        <v>186.85096785691348</v>
+        <v>186.85096785683027</v>
       </c>
       <c r="AJ66" s="7">
-        <v>210.86609065236098</v>
+        <v>210.86609065228913</v>
       </c>
       <c r="AK66" s="7">
-        <v>242.00514901779044</v>
+        <v>242.00514901779036</v>
       </c>
       <c r="AL66" s="7">
         <v>0</v>
@@ -21224,16 +21224,16 @@
         <v>0</v>
       </c>
       <c r="CL66" s="7">
-        <v>96.223695619998779</v>
+        <v>96.223695619998466</v>
       </c>
       <c r="CM66" s="7">
-        <v>49.53137728057775</v>
+        <v>49.531377280578113</v>
       </c>
       <c r="CN66" s="7">
-        <v>3.1535804261031664</v>
+        <v>3.1535804261028488</v>
       </c>
       <c r="CO66" s="7">
-        <v>39.124607422156942</v>
+        <v>39.124607422086115</v>
       </c>
       <c r="CP66" s="7">
         <v>0</v>
@@ -21349,25 +21349,25 @@
         <v>0</v>
       </c>
       <c r="S67" s="7">
-        <v>379.42813983613223</v>
+        <v>0</v>
       </c>
       <c r="T67" s="7">
         <v>380.23765933488176</v>
       </c>
       <c r="U67" s="7">
-        <v>338.00124291889551</v>
+        <v>338.00124291889534</v>
       </c>
       <c r="V67" s="7">
-        <v>367.11945110516535</v>
+        <v>367.11945110516547</v>
       </c>
       <c r="W67" s="7">
-        <v>325.5954755151115</v>
+        <v>325.59547551511162</v>
       </c>
       <c r="X67" s="7">
-        <v>284.43253649474718</v>
+        <v>284.43253649474696</v>
       </c>
       <c r="Y67" s="7">
-        <v>76.235785038988325</v>
+        <v>0</v>
       </c>
       <c r="Z67" s="7">
         <v>0</v>
@@ -21433,19 +21433,19 @@
         <v>0</v>
       </c>
       <c r="AW67" s="7">
-        <v>760.94039927704671</v>
+        <v>0</v>
       </c>
       <c r="AX67" s="7">
-        <v>722.13030752053965</v>
+        <v>536.13030752053942</v>
       </c>
       <c r="AY67" s="7">
-        <v>754.70567728822425</v>
+        <v>754.70567728822414</v>
       </c>
       <c r="AZ67" s="7">
-        <v>716.66997773381809</v>
+        <v>355.08550041744382</v>
       </c>
       <c r="BA67" s="7">
-        <v>400.51370755991661</v>
+        <v>400.51370755989933</v>
       </c>
       <c r="BB67" s="7">
         <v>0</v>
@@ -21463,76 +21463,76 @@
         <v>746.16084999999975</v>
       </c>
       <c r="BH67" s="7">
-        <v>709.602699999999</v>
+        <v>709.60269999999923</v>
       </c>
       <c r="BI67" s="7">
-        <v>673.45027899999832</v>
+        <v>673.45027899999843</v>
       </c>
       <c r="BJ67" s="7">
         <v>637.70723856099767</v>
       </c>
       <c r="BK67" s="7">
-        <v>602.37726310804601</v>
+        <v>602.37726310804612</v>
       </c>
       <c r="BL67" s="7">
-        <v>567.46407022601852</v>
+        <v>567.46407022601807</v>
       </c>
       <c r="BM67" s="7">
-        <v>532.97141095805182</v>
+        <v>532.97141095805159</v>
       </c>
       <c r="BN67" s="7">
-        <v>498.90307010667402</v>
+        <v>498.90307010667362</v>
       </c>
       <c r="BO67" s="7">
-        <v>465.26286653763327</v>
+        <v>465.2628665376327</v>
       </c>
       <c r="BP67" s="7">
-        <v>432.05465348647158</v>
+        <v>432.05465348647124</v>
       </c>
       <c r="BQ67" s="7">
-        <v>399.28231886784943</v>
+        <v>399.28231886784886</v>
       </c>
       <c r="BR67" s="7">
-        <v>366.94978558765979</v>
+        <v>366.94978558765922</v>
       </c>
       <c r="BS67" s="7">
-        <v>335.06101185794796</v>
+        <v>335.06101185794751</v>
       </c>
       <c r="BT67" s="7">
-        <v>303.61999151466898</v>
+        <v>303.61999151466841</v>
       </c>
       <c r="BU67" s="7">
-        <v>272.63075433829999</v>
+        <v>272.63075433829937</v>
       </c>
       <c r="BV67" s="7">
-        <v>242.09736637734295</v>
+        <v>242.09736637734306</v>
       </c>
       <c r="BW67" s="7">
-        <v>147.75800723354837</v>
+        <v>147.75800723352086</v>
       </c>
       <c r="BX67" s="7">
-        <v>68.914585597211044</v>
+        <v>440.09428761092022</v>
       </c>
       <c r="BY67" s="7">
-        <v>1406.2651602812252</v>
+        <v>1715.2463522699563</v>
       </c>
       <c r="BZ67" s="7">
-        <v>1703.0894048784626</v>
+        <v>1859.1049154000925</v>
       </c>
       <c r="CA67" s="7">
-        <v>1901.913056638693</v>
+        <v>1740.6650554069897</v>
       </c>
       <c r="CB67" s="7">
-        <v>1516.5480122398701</v>
+        <v>1874.2022234984402</v>
       </c>
       <c r="CC67" s="7">
-        <v>1190.876745209926</v>
+        <v>1190.8767452099255</v>
       </c>
       <c r="CD67" s="7">
-        <v>1164.1409899668147</v>
+        <v>1238.7194753310341</v>
       </c>
       <c r="CE67" s="7">
-        <v>602.30422489354271</v>
+        <v>602.30422489353202</v>
       </c>
       <c r="CF67" s="8">
         <v>0</v>
@@ -21595,13 +21595,13 @@
         <v>0</v>
       </c>
       <c r="DA67" s="7">
-        <v>0</v>
+        <v>443.68811599190917</v>
       </c>
       <c r="DB67" s="7">
-        <v>216.02275368583634</v>
+        <v>243.98550403375066</v>
       </c>
       <c r="DC67" s="7">
-        <v>270.46915423732111</v>
+        <v>431.71715546900828</v>
       </c>
       <c r="DD67" s="7">
         <v>0</v>
@@ -22184,7 +22184,7 @@
         <v>0</v>
       </c>
       <c r="CE69" s="7">
-        <v>42.095140382971977</v>
+        <v>42.095140382982663</v>
       </c>
       <c r="CF69" s="8">
         <v>398.3</v>
@@ -30140,7 +30140,7 @@
         <v>1</v>
       </c>
       <c r="B97" s="3">
-        <v>128.26259916666658</v>
+        <v>128.26293250000009</v>
       </c>
       <c r="C97" s="4">
         <v>-182.02163499999983</v>
@@ -30152,7 +30152,7 @@
         <v>-606.97189110743295</v>
       </c>
       <c r="F97" s="4">
-        <v>-597.69252849739973</v>
+        <v>-597.69252849739985</v>
       </c>
       <c r="G97" s="4">
         <v>-588.48884796637628</v>
@@ -30161,40 +30161,40 @@
         <v>-579.36153065307371</v>
       </c>
       <c r="I97" s="4">
-        <v>-538.21266723876545</v>
+        <v>-570.31126382645118</v>
       </c>
       <c r="J97" s="4">
-        <v>-287.94277690517924</v>
+        <v>-287.94073986812646</v>
       </c>
       <c r="K97" s="4">
-        <v>-365.233704303872</v>
+        <v>-108.7113283585237</v>
       </c>
       <c r="L97" s="4">
-        <v>-428.27813758633118</v>
+        <v>-99.896398738750349</v>
       </c>
       <c r="M97" s="4">
-        <v>-172.07593572915036</v>
+        <v>-172.07729128469418</v>
       </c>
       <c r="N97" s="4">
-        <v>-82.506844184752907</v>
+        <v>-82.506844184752936</v>
       </c>
       <c r="O97" s="4">
-        <v>-73.933663234915599</v>
+        <v>-73.933663234915571</v>
       </c>
       <c r="P97" s="4">
-        <v>-65.44251999902977</v>
+        <v>-65.442519999029741</v>
       </c>
       <c r="Q97" s="4">
-        <v>-58.608554406713154</v>
+        <v>-58.60855440671336</v>
       </c>
       <c r="R97" s="4">
-        <v>-75.89861947637371</v>
+        <v>-75.898619476373398</v>
       </c>
       <c r="S97" s="4">
-        <v>-93.013656574161246</v>
+        <v>-93.013656574161274</v>
       </c>
       <c r="T97" s="4">
-        <v>-109.95209044832893</v>
+        <v>-109.95209044832889</v>
       </c>
       <c r="U97" s="4">
         <v>-126.71233166986428</v>
@@ -30203,7 +30203,7 @@
         <v>-143.29277650489314</v>
       </c>
       <c r="W97" s="4">
-        <v>-159.69180678593773</v>
+        <v>-159.69180678593762</v>
       </c>
       <c r="X97" s="4">
         <v>-175.90778978201138</v>
@@ -30215,13 +30215,13 @@
         <v>-207.78400939015773</v>
       </c>
       <c r="AA97" s="5">
-        <v>-421.40376105000485</v>
+        <v>-421.40376105000479</v>
       </c>
       <c r="AD97" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AE97" s="3">
-        <v>196.52793250000025</v>
+        <v>196.52793250000008</v>
       </c>
       <c r="AF97" s="4">
         <v>-282.42228499999976</v>
@@ -30242,31 +30242,31 @@
         <v>-685.44149668994669</v>
       </c>
       <c r="AL97" s="4">
-        <v>-677.55727789098944</v>
+        <v>-677.55794455765613</v>
       </c>
       <c r="AM97" s="4">
-        <v>-669.76197013200817</v>
+        <v>-669.76263679867486</v>
       </c>
       <c r="AN97" s="4">
-        <v>-662.05570094569634</v>
+        <v>-612.78569389480822</v>
       </c>
       <c r="AO97" s="4">
-        <v>-343.17976907651752</v>
+        <v>-654.43993834587411</v>
       </c>
       <c r="AP97" s="4">
-        <v>-358.81023686570626</v>
+        <v>-358.80957019903968</v>
       </c>
       <c r="AQ97" s="4">
-        <v>-374.25007364083103</v>
+        <v>-374.25007364083115</v>
       </c>
       <c r="AR97" s="4">
-        <v>-389.49890305609858</v>
+        <v>-389.49890305609892</v>
       </c>
       <c r="AS97" s="4">
-        <v>-404.55433337860359</v>
+        <v>-404.55433337860393</v>
       </c>
       <c r="AT97" s="4">
-        <v>-419.41462401651177</v>
+        <v>-419.41462401651188</v>
       </c>
       <c r="AU97" s="4">
         <v>-434.07801871266088</v>
@@ -30284,7 +30284,7 @@
         <v>-490.7269567190674</v>
       </c>
       <c r="AZ97" s="4">
-        <v>-504.37896962203934</v>
+        <v>-504.37896962203928</v>
       </c>
       <c r="BA97" s="4">
         <v>-517.82321208363794</v>
@@ -30296,16 +30296,16 @@
         <v>-544.08088911742038</v>
       </c>
       <c r="BD97" s="5">
-        <v>-556.89053318197728</v>
+        <v>-556.89053318197739</v>
       </c>
       <c r="BF97" s="1" t="s">
         <v>1</v>
       </c>
       <c r="BG97" s="3">
-        <v>337.57726583333363</v>
+        <v>337.57793250000003</v>
       </c>
       <c r="BH97" s="4">
-        <v>-605.40045652377569</v>
+        <v>-546.72983499999964</v>
       </c>
       <c r="BI97" s="4">
         <v>-540.79549619999966</v>
@@ -30323,31 +30323,31 @@
         <v>-961.85891104370239</v>
       </c>
       <c r="BN97" s="4">
-        <v>-956.46244897392887</v>
+        <v>-956.46311564059533</v>
       </c>
       <c r="BO97" s="4">
-        <v>-951.17728775469391</v>
+        <v>-951.1779544213606</v>
       </c>
       <c r="BP97" s="4">
-        <v>-687.62276229266945</v>
+        <v>-946.0044230936528</v>
       </c>
       <c r="BQ97" s="4">
-        <v>-698.13385557830372</v>
+        <v>-698.13318891163726</v>
       </c>
       <c r="BR97" s="4">
-        <v>-708.40891014600925</v>
+        <v>-708.40824347934233</v>
       </c>
       <c r="BS97" s="4">
-        <v>-718.44513498065669</v>
+        <v>-718.4451349806568</v>
       </c>
       <c r="BT97" s="4">
-        <v>-728.24171994798257</v>
+        <v>-728.24171994798303</v>
       </c>
       <c r="BU97" s="4">
-        <v>-737.79583562251412</v>
+        <v>-737.79583562251503</v>
       </c>
       <c r="BV97" s="4">
-        <v>-747.10529978061834</v>
+        <v>-747.10529978061845</v>
       </c>
       <c r="BW97" s="4">
         <v>-756.16791055864451</v>
@@ -30362,73 +30362,73 @@
         <v>-781.85230565247775</v>
       </c>
       <c r="CA97" s="4">
-        <v>-789.90508525335019</v>
+        <v>-789.90508525335008</v>
       </c>
       <c r="CB97" s="4">
-        <v>-797.69970131313084</v>
+        <v>-797.69970131313062</v>
       </c>
       <c r="CC97" s="4">
         <v>-805.23383035994948</v>
       </c>
       <c r="CD97" s="4">
-        <v>-812.50512801068908</v>
+        <v>-812.5051280106893</v>
       </c>
       <c r="CE97" s="4">
         <v>-819.51122878278557</v>
       </c>
       <c r="CF97" s="5">
-        <v>-879.25777666334648</v>
+        <v>-879.2577766633467</v>
       </c>
       <c r="CH97" s="1" t="s">
         <v>1</v>
       </c>
       <c r="CI97" s="3">
-        <v>149.16059916666649</v>
+        <v>149.16126583333335</v>
       </c>
       <c r="CJ97" s="4">
-        <v>-193.66391833333319</v>
+        <v>-252.33453985707433</v>
       </c>
       <c r="CK97" s="4">
-        <v>-302.87452382610945</v>
+        <v>-302.87452382608126</v>
       </c>
       <c r="CL97" s="4">
-        <v>-619.25057652071621</v>
+        <v>-619.25057652071632</v>
       </c>
       <c r="CM97" s="4">
         <v>-610.29371707940265</v>
       </c>
       <c r="CN97" s="4">
-        <v>-601.41477557895041</v>
+        <v>-601.4147755789503</v>
       </c>
       <c r="CO97" s="4">
         <v>-592.6164592808276</v>
       </c>
       <c r="CP97" s="4">
-        <v>-583.89681514518838</v>
+        <v>-552.4946880485229</v>
       </c>
       <c r="CQ97" s="4">
-        <v>-575.25856322149502</v>
+        <v>-575.25922988816149</v>
       </c>
       <c r="CR97" s="4">
-        <v>-525.403824789434</v>
+        <v>-566.70243003965504</v>
       </c>
       <c r="CS97" s="4">
-        <v>-543.00494763753909</v>
+        <v>-556.37171313865656</v>
       </c>
       <c r="CT97" s="4">
         <v>-560.43317536711049</v>
       </c>
       <c r="CU97" s="4">
-        <v>-577.6882912554147</v>
+        <v>-577.68829125541492</v>
       </c>
       <c r="CV97" s="4">
-        <v>-594.76806462921343</v>
+        <v>-594.76806462921377</v>
       </c>
       <c r="CW97" s="4">
-        <v>-611.67091740587659</v>
+        <v>-611.67091740587693</v>
       </c>
       <c r="CX97" s="4">
-        <v>-628.39525730002993</v>
+        <v>-628.39525730003027</v>
       </c>
       <c r="CY97" s="4">
         <v>-644.93947769573106</v>
@@ -30440,25 +30440,25 @@
         <v>-677.48106110015033</v>
       </c>
       <c r="DB97" s="4">
-        <v>-690.24334443467387</v>
+        <v>-683.51221747846262</v>
       </c>
       <c r="DC97" s="4">
-        <v>-684.70242095243543</v>
+        <v>-675.90125428576869</v>
       </c>
       <c r="DD97" s="4">
-        <v>-713.49320281758742</v>
+        <v>-671.88098876684057</v>
       </c>
       <c r="DE97" s="4">
-        <v>-696.25198171127909</v>
+        <v>-685.74798171127918</v>
       </c>
       <c r="DF97" s="4">
-        <v>-699.31081589084738</v>
+        <v>-702.72082321304879</v>
       </c>
       <c r="DG97" s="4">
-        <v>-707.18081268719857</v>
+        <v>-709.49507784196589</v>
       </c>
       <c r="DH97" s="5">
-        <v>-721.66583960504329</v>
+        <v>-721.66583960504352</v>
       </c>
     </row>
     <row r="98" spans="1:112" x14ac:dyDescent="0.35">
@@ -30466,7 +30466,7 @@
         <v>2</v>
       </c>
       <c r="B98" s="6">
-        <v>629.13317416666655</v>
+        <v>629.13250749999997</v>
       </c>
       <c r="C98" s="7">
         <v>792.28021499999988</v>
@@ -30478,7 +30478,7 @@
         <v>989.58439606356615</v>
       </c>
       <c r="F98" s="7">
-        <v>977.44984495813821</v>
+        <v>977.44984495813833</v>
       </c>
       <c r="G98" s="7">
         <v>965.4142627252611</v>
@@ -30487,34 +30487,34 @@
         <v>953.47854008478862</v>
       </c>
       <c r="I98" s="7">
-        <v>925.59427747920881</v>
+        <v>941.64357577305145</v>
       </c>
       <c r="J98" s="7">
-        <v>793.21229459715391</v>
+        <v>793.21127607862752</v>
       </c>
       <c r="K98" s="7">
-        <v>824.6740789030514</v>
+        <v>696.41289093037722</v>
       </c>
       <c r="L98" s="7">
-        <v>849.07654469754095</v>
+        <v>684.88567527375051</v>
       </c>
       <c r="M98" s="7">
-        <v>713.92019682583964</v>
+        <v>713.92087460361165</v>
       </c>
       <c r="N98" s="7">
         <v>662.14548854929239</v>
       </c>
       <c r="O98" s="7">
-        <v>650.93440576873593</v>
+        <v>650.93440576873581</v>
       </c>
       <c r="P98" s="7">
-        <v>639.83060307565449</v>
+        <v>639.83060307565438</v>
       </c>
       <c r="Q98" s="7">
-        <v>629.622246785931</v>
+        <v>629.62224678593145</v>
       </c>
       <c r="R98" s="7">
-        <v>631.54336512700456</v>
+        <v>631.54336512700445</v>
       </c>
       <c r="S98" s="7">
         <v>633.44503591564762</v>
@@ -30529,7 +30529,7 @@
         <v>639.03160479684016</v>
       </c>
       <c r="W98" s="7">
-        <v>640.85371927251163</v>
+        <v>640.85371927251174</v>
       </c>
       <c r="X98" s="7">
         <v>642.65549516096428</v>
@@ -30547,10 +30547,10 @@
         <v>2</v>
       </c>
       <c r="AE98" s="6">
-        <v>438.31850749999967</v>
+        <v>438.31750750000003</v>
       </c>
       <c r="AF98" s="7">
-        <v>938.03106499999978</v>
+        <v>938.03106499999967</v>
       </c>
       <c r="AG98" s="7">
         <v>927.16007924999951</v>
@@ -30568,28 +30568,28 @@
         <v>1106.6561879791611</v>
       </c>
       <c r="AL98" s="7">
-        <v>1096.34659416514</v>
+        <v>1096.3469274984734</v>
       </c>
       <c r="AM98" s="7">
-        <v>1086.152730172626</v>
+        <v>1086.1530635059594</v>
       </c>
       <c r="AN98" s="7">
-        <v>1076.0753012366795</v>
+        <v>1051.4402977112356</v>
       </c>
       <c r="AO98" s="7">
-        <v>910.48560397146457</v>
+        <v>1066.1156886061428</v>
       </c>
       <c r="AP98" s="7">
-        <v>912.22232261470776</v>
+        <v>912.2219892813747</v>
       </c>
       <c r="AQ98" s="7">
-        <v>913.93760077490685</v>
+        <v>913.93760077490708</v>
       </c>
       <c r="AR98" s="7">
-        <v>915.63191515438098</v>
+        <v>915.6319151543812</v>
       </c>
       <c r="AS98" s="7">
-        <v>917.30474074577035</v>
+        <v>917.30474074577057</v>
       </c>
       <c r="AT98" s="7">
         <v>918.95588414998269</v>
@@ -30628,10 +30628,10 @@
         <v>2</v>
       </c>
       <c r="BG98" s="6">
-        <v>-25.130159166666374</v>
+        <v>-25.132492499999973</v>
       </c>
       <c r="BH98" s="7">
-        <v>1312.9993257618876</v>
+        <v>1283.6640149999994</v>
       </c>
       <c r="BI98" s="7">
         <v>1275.9037257999996</v>
@@ -30649,31 +30649,31 @@
         <v>1468.1251144417645</v>
       </c>
       <c r="BN98" s="7">
-        <v>1461.068740965907</v>
+        <v>1461.0690742992401</v>
       </c>
       <c r="BO98" s="7">
-        <v>1454.1573762945998</v>
+        <v>1454.1577096279332</v>
       </c>
       <c r="BP98" s="7">
-        <v>1318.2014921065929</v>
+        <v>1447.3923225070844</v>
       </c>
       <c r="BQ98" s="7">
-        <v>1319.3693913605521</v>
+        <v>1319.3690580272187</v>
       </c>
       <c r="BR98" s="7">
-        <v>1320.5110640902972</v>
+        <v>1320.5107307569638</v>
       </c>
       <c r="BS98" s="7">
         <v>1321.6259409237766</v>
       </c>
       <c r="BT98" s="7">
-        <v>1322.7144503645904</v>
+        <v>1322.7144503645907</v>
       </c>
       <c r="BU98" s="7">
-        <v>1323.7760187728713</v>
+        <v>1323.776018772872</v>
       </c>
       <c r="BV98" s="7">
-        <v>1324.8104036793277</v>
+        <v>1324.8104036793279</v>
       </c>
       <c r="BW98" s="7">
         <v>1325.817360432442</v>
@@ -30688,7 +30688,7 @@
         <v>1328.6711821095346</v>
       </c>
       <c r="CA98" s="7">
-        <v>1329.5659353985204</v>
+        <v>1329.5659353985207</v>
       </c>
       <c r="CB98" s="7">
         <v>1330.4320038496071</v>
@@ -30697,7 +30697,7 @@
         <v>1331.2691292992536</v>
       </c>
       <c r="CD98" s="7">
-        <v>1332.0770512604472</v>
+        <v>1332.077051260447</v>
       </c>
       <c r="CE98" s="7">
         <v>1332.8555069017912</v>
@@ -30709,82 +30709,82 @@
         <v>2</v>
       </c>
       <c r="CI98" s="6">
-        <v>593.95217416666651</v>
+        <v>593.95084083333336</v>
       </c>
       <c r="CJ98" s="7">
-        <v>821.96243166666648</v>
+        <v>851.29774242853705</v>
       </c>
       <c r="CK98" s="7">
-        <v>869.20809698805442</v>
+        <v>869.20809698804032</v>
       </c>
       <c r="CL98" s="7">
         <v>1020.0988308347828</v>
       </c>
       <c r="CM98" s="7">
-        <v>1008.3860146422958</v>
+        <v>1008.3860146422959</v>
       </c>
       <c r="CN98" s="7">
-        <v>996.77562960324281</v>
+        <v>996.77562960324269</v>
       </c>
       <c r="CO98" s="7">
         <v>985.26960059800535</v>
       </c>
       <c r="CP98" s="7">
-        <v>973.86752749755408</v>
+        <v>958.16646394922134</v>
       </c>
       <c r="CQ98" s="7">
-        <v>962.57135190503209</v>
+        <v>962.57168523836503</v>
       </c>
       <c r="CR98" s="7">
-        <v>930.73272127289988</v>
+        <v>951.3820238980104</v>
       </c>
       <c r="CS98" s="7">
-        <v>932.6884015893562</v>
+        <v>939.37178433991471</v>
       </c>
       <c r="CT98" s="7">
-        <v>934.62461207782701</v>
+        <v>934.6246120778269</v>
       </c>
       <c r="CU98" s="7">
-        <v>936.54184717652754</v>
+        <v>936.54184717652743</v>
       </c>
       <c r="CV98" s="7">
-        <v>938.43959977361601</v>
+        <v>938.43959977361624</v>
       </c>
       <c r="CW98" s="7">
-        <v>940.31769452657863</v>
+        <v>940.31769452657875</v>
       </c>
       <c r="CX98" s="7">
-        <v>942.17595451481793</v>
+        <v>942.17595451481805</v>
       </c>
       <c r="CY98" s="7">
         <v>944.01420122545164</v>
       </c>
       <c r="CZ98" s="7">
-        <v>945.83225453898069</v>
+        <v>945.83225453898058</v>
       </c>
       <c r="DA98" s="7">
         <v>947.62993271483151</v>
       </c>
       <c r="DB98" s="7">
-        <v>952.63884599964297</v>
+        <v>944.42559208722025</v>
       </c>
       <c r="DC98" s="7">
-        <v>946.82612739933859</v>
+        <v>934.47279406600524</v>
       </c>
       <c r="DD98" s="7">
-        <v>952.49670772047261</v>
+        <v>926.38860069509917</v>
       </c>
       <c r="DE98" s="7">
-        <v>940.52670167162353</v>
+        <v>935.27570167162355</v>
       </c>
       <c r="DF98" s="7">
-        <v>944.16255361750154</v>
+        <v>937.9153072786022</v>
       </c>
       <c r="DG98" s="7">
-        <v>942.24723844672565</v>
+        <v>938.10337102410926</v>
       </c>
       <c r="DH98" s="8">
-        <v>943.71686717582554</v>
+        <v>943.71686717582588</v>
       </c>
     </row>
     <row r="99" spans="1:112" x14ac:dyDescent="0.35">
@@ -30792,7 +30792,7 @@
         <v>3</v>
       </c>
       <c r="B99" s="9">
-        <v>-757.39577333333318</v>
+        <v>-757.39544000000001</v>
       </c>
       <c r="C99" s="10">
         <v>-610.25858000000005</v>
@@ -30813,40 +30813,40 @@
         <v>-374.11700943171513</v>
       </c>
       <c r="I99" s="10">
-        <v>-387.38161024044337</v>
+        <v>-371.33231194660056</v>
       </c>
       <c r="J99" s="10">
-        <v>-505.26951769197467</v>
+        <v>-505.27053621050106</v>
       </c>
       <c r="K99" s="10">
-        <v>-459.44037459917945</v>
+        <v>-587.70156257185351</v>
       </c>
       <c r="L99" s="10">
-        <v>-420.79840711120971</v>
+        <v>-584.98927653500016</v>
       </c>
       <c r="M99" s="10">
-        <v>-541.84426109668925</v>
+        <v>-541.84358331891747</v>
       </c>
       <c r="N99" s="10">
         <v>-579.63864436453946</v>
       </c>
       <c r="O99" s="10">
-        <v>-577.00074253382024</v>
+        <v>-577.00074253382013</v>
       </c>
       <c r="P99" s="10">
-        <v>-574.38808307662464</v>
+        <v>-574.38808307662453</v>
       </c>
       <c r="Q99" s="10">
-        <v>-571.0136923792179</v>
+        <v>-571.01369237921801</v>
       </c>
       <c r="R99" s="10">
-        <v>-555.64474565063085</v>
+        <v>-555.64474565063108</v>
       </c>
       <c r="S99" s="10">
         <v>-540.43137934148626</v>
       </c>
       <c r="T99" s="10">
-        <v>-525.37499367555949</v>
+        <v>-525.37499367555961</v>
       </c>
       <c r="U99" s="10">
         <v>-510.47700147863918</v>
@@ -30867,13 +30867,13 @@
         <v>-438.41328794948942</v>
       </c>
       <c r="AA99" s="11">
-        <v>-325.51461878461691</v>
+        <v>-325.5146187846168</v>
       </c>
       <c r="AD99" t="s">
         <v>3</v>
       </c>
       <c r="AE99" s="9">
-        <v>-634.8464399999998</v>
+        <v>-634.84544000000005</v>
       </c>
       <c r="AF99" s="10">
         <v>-655.60878000000002</v>
@@ -30894,34 +30894,34 @@
         <v>-421.21469128921433</v>
       </c>
       <c r="AL99" s="10">
-        <v>-418.78931627415062</v>
+        <v>-418.78898294081728</v>
       </c>
       <c r="AM99" s="10">
-        <v>-416.39076004061792</v>
+        <v>-416.39042670728452</v>
       </c>
       <c r="AN99" s="10">
-        <v>-414.01960029098348</v>
+        <v>-438.65460381642743</v>
       </c>
       <c r="AO99" s="10">
-        <v>-567.30583489494734</v>
+        <v>-411.67575026026901</v>
       </c>
       <c r="AP99" s="10">
-        <v>-553.41208574900179</v>
+        <v>-553.41241908233485</v>
       </c>
       <c r="AQ99" s="10">
-        <v>-539.68752713407605</v>
+        <v>-539.68752713407571</v>
       </c>
       <c r="AR99" s="10">
-        <v>-526.13301209828251</v>
+        <v>-526.13301209828228</v>
       </c>
       <c r="AS99" s="10">
-        <v>-512.75040736716699</v>
+        <v>-512.75040736716664</v>
       </c>
       <c r="AT99" s="10">
         <v>-499.54126013347093</v>
       </c>
       <c r="AU99" s="10">
-        <v>-486.50713151467164</v>
+        <v>-486.50713151467181</v>
       </c>
       <c r="AV99" s="10">
         <v>-473.64959667830368</v>
@@ -30936,7 +30936,7 @@
         <v>-436.15251995342157</v>
       </c>
       <c r="AZ99" s="10">
-        <v>-424.0173973730021</v>
+        <v>-424.01739737300215</v>
       </c>
       <c r="BA99" s="10">
         <v>-412.06695962935879</v>
@@ -30948,16 +30948,16 @@
         <v>-388.72680226599653</v>
       </c>
       <c r="BD99" s="11">
-        <v>-377.34045198639052</v>
+        <v>-377.34045198639046</v>
       </c>
       <c r="BF99" t="s">
         <v>3</v>
       </c>
       <c r="BG99" s="9">
-        <v>-312.44710666666725</v>
+        <v>-312.44544000000002</v>
       </c>
       <c r="BH99" s="10">
-        <v>-707.59886923811189</v>
+        <v>-736.93417999999997</v>
       </c>
       <c r="BI99" s="10">
         <v>-735.10822959999996</v>
@@ -30975,31 +30975,31 @@
         <v>-506.26620339806232</v>
       </c>
       <c r="BN99" s="10">
-        <v>-504.6062919919782</v>
+        <v>-504.60595865864468</v>
       </c>
       <c r="BO99" s="10">
-        <v>-502.98008853990586</v>
+        <v>-502.97975520657252</v>
       </c>
       <c r="BP99" s="10">
-        <v>-630.57872981392336</v>
+        <v>-501.38789941343157</v>
       </c>
       <c r="BQ99" s="10">
-        <v>-621.23553578224823</v>
+        <v>-621.23586911558164</v>
       </c>
       <c r="BR99" s="10">
-        <v>-612.10215394428792</v>
+        <v>-612.10248727762132</v>
       </c>
       <c r="BS99" s="10">
-        <v>-603.18080594311994</v>
+        <v>-603.18080594311959</v>
       </c>
       <c r="BT99" s="10">
-        <v>-594.47273041660799</v>
+        <v>-594.47273041660765</v>
       </c>
       <c r="BU99" s="10">
-        <v>-585.98018315035756</v>
+        <v>-585.98018315035688</v>
       </c>
       <c r="BV99" s="10">
-        <v>-577.70510389870969</v>
+        <v>-577.70510389870947</v>
       </c>
       <c r="BW99" s="10">
         <v>-569.64944987379761</v>
@@ -31014,103 +31014,103 @@
         <v>-546.81887645705694</v>
       </c>
       <c r="CA99" s="10">
-        <v>-539.66085014517012</v>
+        <v>-539.66085014516989</v>
       </c>
       <c r="CB99" s="10">
-        <v>-532.73230253647637</v>
+        <v>-532.73230253647648</v>
       </c>
       <c r="CC99" s="10">
         <v>-526.0352989393042</v>
       </c>
       <c r="CD99" s="10">
-        <v>-519.57192324975745</v>
+        <v>-519.57192324975767</v>
       </c>
       <c r="CE99" s="10">
         <v>-513.34427811900537</v>
       </c>
       <c r="CF99" s="11">
-        <v>-480.85046974256852</v>
+        <v>-480.85046974256824</v>
       </c>
       <c r="CH99" t="s">
         <v>3</v>
       </c>
       <c r="CI99" s="9">
-        <v>-743.11277333333305</v>
+        <v>-743.1121066666667</v>
       </c>
       <c r="CJ99" s="10">
-        <v>-628.29851333333329</v>
+        <v>-598.96320257146272</v>
       </c>
       <c r="CK99" s="10">
-        <v>-566.33357316194497</v>
+        <v>-566.33357316195907</v>
       </c>
       <c r="CL99" s="10">
         <v>-400.84825431406654</v>
       </c>
       <c r="CM99" s="10">
-        <v>-398.09229756289318</v>
+        <v>-398.09229756289312</v>
       </c>
       <c r="CN99" s="10">
-        <v>-395.36085402429239</v>
+        <v>-395.36085402429234</v>
       </c>
       <c r="CO99" s="10">
-        <v>-392.65314131717781</v>
+        <v>-392.65314131717776</v>
       </c>
       <c r="CP99" s="10">
-        <v>-389.97071235236569</v>
+        <v>-405.67177590069844</v>
       </c>
       <c r="CQ99" s="10">
-        <v>-387.31278868353706</v>
+        <v>-387.31245535020355</v>
       </c>
       <c r="CR99" s="10">
-        <v>-405.32889648346594</v>
+        <v>-384.67959385835536</v>
       </c>
       <c r="CS99" s="10">
-        <v>-389.683453951817</v>
+        <v>-383.00007120125809</v>
       </c>
       <c r="CT99" s="10">
-        <v>-374.19143671071635</v>
+        <v>-374.19143671071652</v>
       </c>
       <c r="CU99" s="10">
-        <v>-358.85355592111284</v>
+        <v>-358.85355592111262</v>
       </c>
       <c r="CV99" s="10">
-        <v>-343.67153514440264</v>
+        <v>-343.67153514440247</v>
       </c>
       <c r="CW99" s="10">
-        <v>-328.64677712070198</v>
+        <v>-328.64677712070181</v>
       </c>
       <c r="CX99" s="10">
-        <v>-313.78069721478801</v>
+        <v>-313.78069721478784</v>
       </c>
       <c r="CY99" s="10">
         <v>-299.07472352972036</v>
       </c>
       <c r="CZ99" s="10">
-        <v>-284.5302970214878</v>
+        <v>-284.53029702148797</v>
       </c>
       <c r="DA99" s="10">
         <v>-270.14887161468118</v>
       </c>
       <c r="DB99" s="10">
-        <v>-262.39550156496898</v>
+        <v>-260.91337460875786</v>
       </c>
       <c r="DC99" s="10">
-        <v>-262.12370644690316</v>
+        <v>-258.57153978023649</v>
       </c>
       <c r="DD99" s="10">
-        <v>-239.0035049028852</v>
+        <v>-254.5076119282586</v>
       </c>
       <c r="DE99" s="10">
-        <v>-244.27471996034444</v>
+        <v>-249.52771996034437</v>
       </c>
       <c r="DF99" s="10">
-        <v>-244.85173772665416</v>
+        <v>-235.19448406555341</v>
       </c>
       <c r="DG99" s="10">
-        <v>-235.06642575952708</v>
+        <v>-228.60829318214337</v>
       </c>
       <c r="DH99" s="11">
-        <v>-222.05102757078237</v>
+        <v>-222.05102757078265</v>
       </c>
     </row>
     <row r="101" spans="1:112" x14ac:dyDescent="0.35">
@@ -31146,58 +31146,58 @@
         <v>1</v>
       </c>
       <c r="B103" s="3">
-        <v>161.18848249999988</v>
+        <v>161.18848250000002</v>
       </c>
       <c r="C103" s="4">
-        <v>-47.018268333333253</v>
+        <v>-47.018268333333481</v>
       </c>
       <c r="D103" s="4">
-        <v>-68.529773133333634</v>
+        <v>-68.52977313333372</v>
       </c>
       <c r="E103" s="4">
-        <v>-90.633308835791013</v>
+        <v>-90.633308835757134</v>
       </c>
       <c r="F103" s="4">
-        <v>-106.84842801682831</v>
+        <v>-106.84842801682828</v>
       </c>
       <c r="G103" s="4">
-        <v>-96.690763081479943</v>
+        <v>-96.690763081479645</v>
       </c>
       <c r="H103" s="4">
-        <v>-86.60087550421288</v>
+        <v>-86.600875504212922</v>
       </c>
       <c r="I103" s="4">
-        <v>-76.579375281251032</v>
+        <v>-76.579375281250691</v>
       </c>
       <c r="J103" s="4">
-        <v>-66.626877898782055</v>
+        <v>-66.626877898781913</v>
       </c>
       <c r="K103" s="4">
-        <v>-56.744004382370726</v>
+        <v>-56.744004382370917</v>
       </c>
       <c r="L103" s="4">
-        <v>-46.931381346812259</v>
+        <v>-46.931381346812145</v>
       </c>
       <c r="M103" s="4">
-        <v>-37.18964104643328</v>
+        <v>-37.189641046433167</v>
       </c>
       <c r="N103" s="4">
-        <v>-27.519421425851153</v>
+        <v>-27.519421425851</v>
       </c>
       <c r="O103" s="4">
-        <v>-17.921366171183763</v>
+        <v>-17.921366171183536</v>
       </c>
       <c r="P103" s="4">
-        <v>103.95644205642563</v>
+        <v>300.93720857160929</v>
       </c>
       <c r="Q103" s="4">
-        <v>310.38898081125382</v>
+        <v>310.38898081125376</v>
       </c>
       <c r="R103" s="4">
         <v>350.76662265855521</v>
       </c>
       <c r="S103" s="4">
-        <v>594.54551355202636</v>
+        <v>468.06946693998236</v>
       </c>
       <c r="T103" s="4">
         <v>604.04272692240284</v>
@@ -31212,103 +31212,103 @@
         <v>527.38447214342955</v>
       </c>
       <c r="X103" s="4">
-        <v>522.58212925772057</v>
+        <v>522.58212925772045</v>
       </c>
       <c r="Y103" s="4">
-        <v>462.02292028213617</v>
+        <v>436.61099193580674</v>
       </c>
       <c r="Z103" s="4">
-        <v>445.37106114322899</v>
+        <v>445.3710611432291</v>
       </c>
       <c r="AA103" s="5">
-        <v>454.05077463101804</v>
+        <v>454.05077463101838</v>
       </c>
       <c r="AD103" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AE103" s="3">
-        <v>105.70876583333332</v>
+        <v>105.70876583333342</v>
       </c>
       <c r="AF103" s="4">
-        <v>100.09393166666662</v>
+        <v>100.09393166666644</v>
       </c>
       <c r="AG103" s="4">
-        <v>79.90643666666611</v>
+        <v>79.906436666666082</v>
       </c>
       <c r="AH103" s="4">
         <v>-25.798773897500723</v>
       </c>
       <c r="AI103" s="4">
-        <v>-22.304015418215904</v>
+        <v>-22.304015418188335</v>
       </c>
       <c r="AJ103" s="4">
-        <v>-50.045664297725466</v>
+        <v>-50.045664297701478</v>
       </c>
       <c r="AK103" s="4">
-        <v>-80.00894928125777</v>
+        <v>-80.008949281257799</v>
       </c>
       <c r="AL103" s="4">
-        <v>-18.769778969305584</v>
+        <v>-18.769778969305662</v>
       </c>
       <c r="AM103" s="4">
-        <v>-38.043216020029675</v>
+        <v>-38.043216020029718</v>
       </c>
       <c r="AN103" s="4">
-        <v>-57.159475446709919</v>
+        <v>-57.159475446710019</v>
       </c>
       <c r="AO103" s="4">
-        <v>-76.117142650730244</v>
+        <v>-76.117142650730557</v>
       </c>
       <c r="AP103" s="4">
         <v>-94.914790302087255</v>
       </c>
       <c r="AQ103" s="4">
-        <v>-105.68780060780929</v>
+        <v>-105.68780060780917</v>
       </c>
       <c r="AR103" s="4">
-        <v>-33.32720662709994</v>
+        <v>-33.327206627074474</v>
       </c>
       <c r="AS103" s="4">
-        <v>221.35546692566209</v>
+        <v>-87.977866407671286</v>
       </c>
       <c r="AT103" s="4">
-        <v>230.09100349049277</v>
+        <v>49.059392612275815</v>
       </c>
       <c r="AU103" s="4">
-        <v>269.74596354190754</v>
+        <v>269.7459635419076</v>
       </c>
       <c r="AV103" s="4">
         <v>386.3196218912849</v>
       </c>
       <c r="AW103" s="4">
-        <v>648.45804658232214</v>
+        <v>394.81124682330653</v>
       </c>
       <c r="AX103" s="4">
-        <v>643.93020254406292</v>
+        <v>581.93020254406292</v>
       </c>
       <c r="AY103" s="4">
-        <v>577.44732901695954</v>
+        <v>577.44732901695943</v>
       </c>
       <c r="AZ103" s="4">
-        <v>573.00983073561213</v>
+        <v>452.48167163015404</v>
       </c>
       <c r="BA103" s="4">
-        <v>475.78044885273084</v>
+        <v>475.78044885272516</v>
       </c>
       <c r="BB103" s="4">
         <v>350.34612920558698</v>
       </c>
       <c r="BC103" s="4">
-        <v>358.32981464843726</v>
+        <v>358.32981464843738</v>
       </c>
       <c r="BD103" s="5">
-        <v>366.22615691777315</v>
+        <v>366.22615691777332</v>
       </c>
       <c r="BF103" s="1" t="s">
         <v>1</v>
       </c>
       <c r="BG103" s="3">
-        <v>217.59209916666669</v>
+        <v>217.59209916666674</v>
       </c>
       <c r="BH103" s="4">
         <v>213.32698166666665</v>
@@ -31317,67 +31317,67 @@
         <v>209.10919921666655</v>
       </c>
       <c r="BJ103" s="4">
-        <v>204.93917783211648</v>
+        <v>204.93917783211651</v>
       </c>
       <c r="BK103" s="4">
-        <v>200.81734736260546</v>
+        <v>200.81734736260543</v>
       </c>
       <c r="BL103" s="4">
-        <v>196.74414152636896</v>
+        <v>196.74414152636882</v>
       </c>
       <c r="BM103" s="4">
-        <v>192.71999794510614</v>
+        <v>192.71999794510606</v>
       </c>
       <c r="BN103" s="4">
-        <v>188.74535817911183</v>
+        <v>188.74535817911197</v>
       </c>
       <c r="BO103" s="4">
-        <v>184.82066776272376</v>
+        <v>184.82066776272399</v>
       </c>
       <c r="BP103" s="4">
-        <v>180.9463762400882</v>
+        <v>180.94637624008837</v>
       </c>
       <c r="BQ103" s="4">
-        <v>177.12293720124893</v>
+        <v>177.1229372012491</v>
       </c>
       <c r="BR103" s="4">
-        <v>173.35080831856015</v>
+        <v>173.35080831856038</v>
       </c>
       <c r="BS103" s="4">
-        <v>169.6304513834271</v>
+        <v>169.63045138342727</v>
       </c>
       <c r="BT103" s="4">
-        <v>165.96233234337788</v>
+        <v>165.96233234337814</v>
       </c>
       <c r="BU103" s="4">
-        <v>162.34692133946811</v>
+        <v>162.34692133946834</v>
       </c>
       <c r="BV103" s="4">
-        <v>158.78469274402337</v>
+        <v>158.78469274402332</v>
       </c>
       <c r="BW103" s="4">
-        <v>170.77612519871946</v>
+        <v>170.77612519871954</v>
       </c>
       <c r="BX103" s="4">
-        <v>167.32170165300795</v>
+        <v>291.04826899091108</v>
       </c>
       <c r="BY103" s="4">
-        <v>619.4191264407649</v>
+        <v>722.41285710367526</v>
       </c>
       <c r="BZ103" s="4">
-        <v>724.57206995613399</v>
+        <v>776.57724013001086</v>
       </c>
       <c r="CA103" s="4">
-        <v>711.2881899411808</v>
+        <v>657.53885619727987</v>
       </c>
       <c r="CB103" s="4">
-        <v>588.83718898862821</v>
+        <v>708.05525940815141</v>
       </c>
       <c r="CC103" s="4">
         <v>486.17895360782467</v>
       </c>
       <c r="CD103" s="4">
-        <v>483.05978216279505</v>
+        <v>507.91927728420166</v>
       </c>
       <c r="CE103" s="4">
         <v>441.83159261559342</v>
@@ -31389,7 +31389,7 @@
         <v>1</v>
       </c>
       <c r="CI103" s="3">
-        <v>149.48848249999992</v>
+        <v>149.48848249999998</v>
       </c>
       <c r="CJ103" s="4">
         <v>-22.499568333333549</v>
@@ -31398,31 +31398,31 @@
         <v>-43.790404833333767</v>
       </c>
       <c r="CL103" s="4">
-        <v>-97.016785511000307</v>
+        <v>-97.016785511000137</v>
       </c>
       <c r="CM103" s="4">
-        <v>-102.46422265059905</v>
+        <v>-102.46422265059925</v>
       </c>
       <c r="CN103" s="4">
-        <v>-107.87496561695448</v>
+        <v>-107.87496561695468</v>
       </c>
       <c r="CO103" s="4">
-        <v>-85.905526938434264</v>
+        <v>-85.905526938457683</v>
       </c>
       <c r="CP103" s="4">
-        <v>-89.036678208032299</v>
+        <v>-89.036678208031958</v>
       </c>
       <c r="CQ103" s="4">
-        <v>-79.196296551904041</v>
+        <v>-79.196296551904197</v>
       </c>
       <c r="CR103" s="4">
-        <v>-69.426547803371392</v>
+        <v>-69.426547803371321</v>
       </c>
       <c r="CS103" s="4">
-        <v>-59.728067658601653</v>
+        <v>-59.728067658601574</v>
       </c>
       <c r="CT103" s="4">
-        <v>-50.101497535029011</v>
+        <v>-50.101497535028706</v>
       </c>
       <c r="CU103" s="4">
         <v>-40.547484622843967</v>
@@ -31431,25 +31431,25 @@
         <v>-31.066681936949294</v>
       </c>
       <c r="CW103" s="4">
-        <v>-21.659748369381759</v>
+        <v>91.612690184619396</v>
       </c>
       <c r="CX103" s="4">
-        <v>117.94210861374393</v>
+        <v>297.00598459112712</v>
       </c>
       <c r="CY103" s="4">
-        <v>337.26317947244718</v>
+        <v>337.26317947244729</v>
       </c>
       <c r="CZ103" s="4">
-        <v>454.44449276519924</v>
+        <v>454.44449276519936</v>
       </c>
       <c r="DA103" s="4">
-        <v>463.54924153508637</v>
+        <v>611.44528019905613</v>
       </c>
       <c r="DB103" s="4">
-        <v>544.58432126334753</v>
+        <v>553.9052380459857</v>
       </c>
       <c r="DC103" s="4">
-        <v>486.01600106082191</v>
+        <v>539.76533480471767</v>
       </c>
       <c r="DD103" s="4">
         <v>404.73051216938359</v>
@@ -31464,7 +31464,7 @@
         <v>430.86418672743048</v>
       </c>
       <c r="DH103" s="5">
-        <v>439.4133383454776</v>
+        <v>439.41333834547765</v>
       </c>
     </row>
     <row r="104" spans="1:112" x14ac:dyDescent="0.35">
@@ -31472,37 +31472,37 @@
         <v>2</v>
       </c>
       <c r="B104" s="6">
-        <v>557.16890750000005</v>
+        <v>557.16890749999982</v>
       </c>
       <c r="C104" s="7">
-        <v>652.85388166666655</v>
+        <v>652.85388166666667</v>
       </c>
       <c r="D104" s="7">
-        <v>655.24404886666673</v>
+        <v>655.24404886666662</v>
       </c>
       <c r="E104" s="7">
-        <v>656.88992403720954</v>
+        <v>656.88992403724342</v>
       </c>
       <c r="F104" s="7">
-        <v>657.83255971431402</v>
+        <v>657.8325597143139</v>
       </c>
       <c r="G104" s="7">
-        <v>644.54945941424273</v>
+        <v>644.54945941424262</v>
       </c>
       <c r="H104" s="7">
         <v>631.3549910439707</v>
       </c>
       <c r="I104" s="7">
-        <v>618.24995229086653</v>
+        <v>618.2499522908663</v>
       </c>
       <c r="J104" s="7">
-        <v>605.23514802148418</v>
+        <v>605.23514802148406</v>
       </c>
       <c r="K104" s="7">
         <v>592.31139034617729</v>
       </c>
       <c r="L104" s="7">
-        <v>579.47949868429282</v>
+        <v>579.47949868429271</v>
       </c>
       <c r="M104" s="7">
         <v>566.74029982995103</v>
@@ -31511,43 +31511,43 @@
         <v>554.09462801842062</v>
       </c>
       <c r="O104" s="7">
-        <v>541.54332499308634</v>
+        <v>541.54332499308623</v>
       </c>
       <c r="P104" s="7">
-        <v>472.91095666394909</v>
+        <v>374.42057340635711</v>
       </c>
       <c r="Q104" s="7">
-        <v>362.06056355451437</v>
+        <v>362.0605635545142</v>
       </c>
       <c r="R104" s="7">
         <v>334.29749344650463</v>
       </c>
       <c r="S104" s="7">
-        <v>-146.81985768406508</v>
+        <v>106.13223554002305</v>
       </c>
       <c r="T104" s="7">
         <v>-159.42610274503795</v>
       </c>
       <c r="U104" s="7">
-        <v>-143.23547645224318</v>
+        <v>-143.23547645224323</v>
       </c>
       <c r="V104" s="7">
-        <v>-3.1807895903132248</v>
+        <v>-3.1807895903133385</v>
       </c>
       <c r="W104" s="7">
-        <v>12.736734385874001</v>
+        <v>12.736734385873888</v>
       </c>
       <c r="X104" s="7">
-        <v>28.515861010347027</v>
+        <v>28.515861010346953</v>
       </c>
       <c r="Y104" s="7">
-        <v>155.75407692974778</v>
+        <v>206.57793362240665</v>
       </c>
       <c r="Z104" s="7">
-        <v>195.12245850500824</v>
+        <v>195.12245850500813</v>
       </c>
       <c r="AA104" s="8">
-        <v>183.77206394405306</v>
+        <v>183.77206394405289</v>
       </c>
       <c r="AD104" t="s">
         <v>2</v>
@@ -31556,7 +31556,7 @@
         <v>619.52834083333335</v>
       </c>
       <c r="AF104" s="7">
-        <v>636.50808166666661</v>
+        <v>636.50808166666673</v>
       </c>
       <c r="AG104" s="7">
         <v>638.75113666666664</v>
@@ -31565,145 +31565,145 @@
         <v>555.31097487750003</v>
       </c>
       <c r="AI104" s="7">
-        <v>580.90379139575975</v>
+        <v>580.90379139578749</v>
       </c>
       <c r="AJ104" s="7">
-        <v>575.09170690257645</v>
+        <v>575.09170690260044</v>
       </c>
       <c r="AK104" s="7">
-        <v>566.88797620984678</v>
+        <v>566.88797620984701</v>
       </c>
       <c r="AL104" s="7">
-        <v>649.71516062621924</v>
+        <v>649.71516062621913</v>
       </c>
       <c r="AM104" s="7">
         <v>651.85665363185501</v>
       </c>
       <c r="AN104" s="7">
-        <v>653.98068245704167</v>
+        <v>653.98068245704189</v>
       </c>
       <c r="AO104" s="7">
-        <v>656.08708992415507</v>
+        <v>656.08708992415518</v>
       </c>
       <c r="AP104" s="7">
         <v>658.17571744097256</v>
       </c>
       <c r="AQ104" s="7">
-        <v>656.31481617944314</v>
+        <v>656.3148161794428</v>
       </c>
       <c r="AR104" s="7">
-        <v>612.95046777821824</v>
+        <v>612.95046777820517</v>
       </c>
       <c r="AS104" s="7">
-        <v>478.48900478951884</v>
+        <v>633.15567145618547</v>
       </c>
       <c r="AT104" s="7">
-        <v>467.06561082012468</v>
+        <v>557.58141625923315</v>
       </c>
       <c r="AU104" s="7">
-        <v>440.24758613750544</v>
+        <v>440.24758613750538</v>
       </c>
       <c r="AV104" s="7">
-        <v>213.03587906524302</v>
+        <v>213.0358790652428</v>
       </c>
       <c r="AW104" s="7">
-        <v>-305.36215305620112</v>
+        <v>201.93144646182989</v>
       </c>
       <c r="AX104" s="7">
-        <v>-290.48495121620675</v>
+        <v>-166.48495121620681</v>
       </c>
       <c r="AY104" s="7">
-        <v>-151.75550962715249</v>
+        <v>-151.75550962715261</v>
       </c>
       <c r="AZ104" s="7">
-        <v>-137.175158131297</v>
+        <v>103.88116007961918</v>
       </c>
       <c r="BA104" s="7">
-        <v>62.930095909525093</v>
+        <v>62.930095909536476</v>
       </c>
       <c r="BB104" s="7">
-        <v>319.38583103884793</v>
+        <v>319.38583103884787</v>
       </c>
       <c r="BC104" s="7">
         <v>308.94562699819733</v>
       </c>
       <c r="BD104" s="8">
-        <v>298.61964095368114</v>
+        <v>298.61964095368103</v>
       </c>
       <c r="BF104" t="s">
         <v>2</v>
       </c>
       <c r="BG104" s="6">
-        <v>251.91167416666667</v>
+        <v>251.9116741666667</v>
       </c>
       <c r="BH104" s="7">
-        <v>265.92563166666707</v>
+        <v>265.92563166666696</v>
       </c>
       <c r="BI104" s="7">
-        <v>279.78405971666729</v>
+        <v>279.78405971666723</v>
       </c>
       <c r="BJ104" s="7">
-        <v>293.48555855161754</v>
+        <v>293.48555855161749</v>
       </c>
       <c r="BK104" s="7">
-        <v>307.02871580858232</v>
+        <v>307.02871580858226</v>
       </c>
       <c r="BL104" s="7">
-        <v>320.41210641335931</v>
+        <v>320.41210641335965</v>
       </c>
       <c r="BM104" s="7">
-        <v>333.63429246607996</v>
+        <v>333.63429246608024</v>
       </c>
       <c r="BN104" s="7">
-        <v>346.69382312577494</v>
+        <v>346.69382312577505</v>
       </c>
       <c r="BO104" s="7">
-        <v>359.58923449390727</v>
+        <v>359.58923449390738</v>
       </c>
       <c r="BP104" s="7">
-        <v>372.31904949685253</v>
+        <v>372.31904949685264</v>
       </c>
       <c r="BQ104" s="7">
-        <v>384.88177776732437</v>
+        <v>384.88177776732448</v>
       </c>
       <c r="BR104" s="7">
-        <v>397.27591552473041</v>
+        <v>397.27591552473052</v>
       </c>
       <c r="BS104" s="7">
-        <v>409.49994545445327</v>
+        <v>409.49994545445338</v>
       </c>
       <c r="BT104" s="7">
-        <v>421.55233658604351</v>
+        <v>421.55233658604368</v>
       </c>
       <c r="BU104" s="7">
-        <v>433.43154417031826</v>
+        <v>433.43154417031843</v>
       </c>
       <c r="BV104" s="7">
-        <v>445.13600955535202</v>
+        <v>445.1360095553519</v>
       </c>
       <c r="BW104" s="7">
-        <v>472.16416006135023</v>
+        <v>472.16416006135029</v>
       </c>
       <c r="BX104" s="7">
-        <v>483.51440885440252</v>
+        <v>236.06127417859625</v>
       </c>
       <c r="BY104" s="7">
-        <v>-416.30927925666765</v>
+        <v>-622.29674058248827</v>
       </c>
       <c r="BZ104" s="7">
-        <v>-622.31487722228189</v>
+        <v>-726.32521757003553</v>
       </c>
       <c r="CA104" s="7">
-        <v>-591.51833837816548</v>
+        <v>-484.01967089036361</v>
       </c>
       <c r="CB104" s="7">
-        <v>-342.4597115020224</v>
+        <v>-580.8958523410688</v>
       </c>
       <c r="CC104" s="7">
         <v>-133.05941899713812</v>
       </c>
       <c r="CD104" s="7">
-        <v>-122.81071282061214</v>
+        <v>-172.52970306342547</v>
       </c>
       <c r="CE104" s="7">
         <v>153.08190997733595</v>
@@ -31715,7 +31715,7 @@
         <v>2</v>
       </c>
       <c r="CI104" s="6">
-        <v>572.46890750000011</v>
+        <v>572.46890749999989</v>
       </c>
       <c r="CJ104" s="7">
         <v>650.1295816666667</v>
@@ -31724,31 +31724,31 @@
         <v>652.4952301666666</v>
       </c>
       <c r="CL104" s="7">
-        <v>622.77086667900039</v>
+        <v>622.77086667900051</v>
       </c>
       <c r="CM104" s="7">
-        <v>640.66958870911196</v>
+        <v>640.66958870911174</v>
       </c>
       <c r="CN104" s="7">
-        <v>658.4477441699936</v>
+        <v>658.44774416999383</v>
       </c>
       <c r="CO104" s="7">
-        <v>621.41693351437766</v>
+        <v>621.41693351442484</v>
       </c>
       <c r="CP104" s="7">
-        <v>634.54027150281127</v>
+        <v>634.54027150281104</v>
       </c>
       <c r="CQ104" s="7">
-        <v>621.67208010633624</v>
+        <v>621.67208010633613</v>
       </c>
       <c r="CR104" s="7">
-        <v>608.8962548197934</v>
+        <v>608.89625481979328</v>
       </c>
       <c r="CS104" s="7">
-        <v>596.21362693817139</v>
+        <v>596.21362693817127</v>
       </c>
       <c r="CT104" s="7">
-        <v>583.62503523811461</v>
+        <v>583.62503523811449</v>
       </c>
       <c r="CU104" s="7">
         <v>571.13132604525754</v>
@@ -31757,40 +31757,40 @@
         <v>558.73335330216446</v>
       </c>
       <c r="CW104" s="7">
-        <v>546.43197863688385</v>
+        <v>489.79575935988328</v>
       </c>
       <c r="CX104" s="7">
-        <v>469.09334275414074</v>
+        <v>379.56140476544908</v>
       </c>
       <c r="CY104" s="7">
-        <v>351.95584222833827</v>
+        <v>351.95584222833816</v>
       </c>
       <c r="CZ104" s="7">
-        <v>123.94950946089298</v>
+        <v>123.94950946089307</v>
       </c>
       <c r="DA104" s="7">
-        <v>112.04329953104093</v>
+        <v>-183.74877779689851</v>
       </c>
       <c r="DB104" s="7">
-        <v>-43.777055579570629</v>
+        <v>-62.418889144846844</v>
       </c>
       <c r="DC104" s="7">
-        <v>79.555424558004972</v>
+        <v>-27.943242929786493</v>
       </c>
       <c r="DD104" s="7">
-        <v>248.26779177849826</v>
+        <v>248.26779177849835</v>
       </c>
       <c r="DE104" s="7">
-        <v>236.77116571950447</v>
+        <v>236.77116571950455</v>
       </c>
       <c r="DF104" s="7">
         <v>225.37924985848008</v>
       </c>
       <c r="DG104" s="7">
-        <v>214.09298658720633</v>
+        <v>214.09298658720627</v>
       </c>
       <c r="DH104" s="8">
-        <v>202.91332677899072</v>
+        <v>202.91332677899078</v>
       </c>
     </row>
     <row r="105" spans="1:112" x14ac:dyDescent="0.35">
@@ -31798,49 +31798,49 @@
         <v>3</v>
       </c>
       <c r="B105" s="9">
-        <v>-718.35738999999978</v>
+        <v>-718.35739000000001</v>
       </c>
       <c r="C105" s="10">
-        <v>-605.8356133333333</v>
+        <v>-605.83561333333319</v>
       </c>
       <c r="D105" s="10">
-        <v>-586.71427573333301</v>
+        <v>-586.7142757333329</v>
       </c>
       <c r="E105" s="10">
-        <v>-566.25661520141864</v>
+        <v>-566.25661520148628</v>
       </c>
       <c r="F105" s="10">
         <v>-550.98413169748562</v>
       </c>
       <c r="G105" s="10">
-        <v>-547.85869633276286</v>
+        <v>-547.85869633276297</v>
       </c>
       <c r="H105" s="10">
         <v>-544.75411553975789</v>
       </c>
       <c r="I105" s="10">
-        <v>-541.6705770096155</v>
+        <v>-541.67057700961561</v>
       </c>
       <c r="J105" s="10">
-        <v>-538.60827012270204</v>
+        <v>-538.60827012270215</v>
       </c>
       <c r="K105" s="10">
         <v>-535.56738596380649</v>
       </c>
       <c r="L105" s="10">
-        <v>-532.54811733748056</v>
+        <v>-532.54811733748068</v>
       </c>
       <c r="M105" s="10">
-        <v>-529.55065878351797</v>
+        <v>-529.55065878351786</v>
       </c>
       <c r="N105" s="10">
         <v>-526.57520659256954</v>
       </c>
       <c r="O105" s="10">
-        <v>-523.62195882190258</v>
+        <v>-523.62195882190269</v>
       </c>
       <c r="P105" s="10">
-        <v>-576.86739872037469</v>
+        <v>-675.3577819779664</v>
       </c>
       <c r="Q105" s="10">
         <v>-672.44954436576813</v>
@@ -31849,13 +31849,13 @@
         <v>-685.06411610505984</v>
       </c>
       <c r="S105" s="10">
-        <v>-447.72565586796134</v>
+        <v>-574.20170248000534</v>
       </c>
       <c r="T105" s="10">
         <v>-444.61662417736488</v>
       </c>
       <c r="U105" s="10">
-        <v>-455.87966855496131</v>
+        <v>-455.87966855496126</v>
       </c>
       <c r="V105" s="10">
         <v>-529.04814637195591</v>
@@ -31864,106 +31864,106 @@
         <v>-540.12120652930355</v>
       </c>
       <c r="X105" s="10">
-        <v>-551.09799026806729</v>
+        <v>-551.09799026806741</v>
       </c>
       <c r="Y105" s="10">
-        <v>-617.7769972118839</v>
+        <v>-643.18892555821333</v>
       </c>
       <c r="Z105" s="10">
-        <v>-640.49351964823711</v>
+        <v>-640.49351964823722</v>
       </c>
       <c r="AA105" s="11">
-        <v>-637.82283857507105</v>
+        <v>-637.82283857507127</v>
       </c>
       <c r="AD105" t="s">
         <v>3</v>
       </c>
       <c r="AE105" s="9">
-        <v>-725.23710666666636</v>
+        <v>-725.2371066666667</v>
       </c>
       <c r="AF105" s="10">
         <v>-736.60201333333316</v>
       </c>
       <c r="AG105" s="10">
-        <v>-718.65757333333283</v>
+        <v>-718.65757333333272</v>
       </c>
       <c r="AH105" s="10">
         <v>-529.51220097999931</v>
       </c>
       <c r="AI105" s="10">
-        <v>-558.5997759775438</v>
+        <v>-558.59977597759917</v>
       </c>
       <c r="AJ105" s="10">
-        <v>-525.04604260485098</v>
+        <v>-525.04604260489896</v>
       </c>
       <c r="AK105" s="10">
-        <v>-486.87902692858933</v>
+        <v>-486.87902692858927</v>
       </c>
       <c r="AL105" s="10">
-        <v>-630.94538165691336</v>
+        <v>-630.94538165691347</v>
       </c>
       <c r="AM105" s="10">
-        <v>-613.81343761182541</v>
+        <v>-613.81343761182529</v>
       </c>
       <c r="AN105" s="10">
         <v>-596.82120701033182</v>
       </c>
       <c r="AO105" s="10">
-        <v>-579.96994727342474</v>
+        <v>-579.96994727342462</v>
       </c>
       <c r="AP105" s="10">
         <v>-563.26092713888522</v>
       </c>
       <c r="AQ105" s="10">
-        <v>-550.62701557163382</v>
+        <v>-550.62701557163371</v>
       </c>
       <c r="AR105" s="10">
-        <v>-579.6232611511183</v>
+        <v>-579.62326115113069</v>
       </c>
       <c r="AS105" s="10">
-        <v>-699.84447171518093</v>
+        <v>-545.1778050485143</v>
       </c>
       <c r="AT105" s="10">
-        <v>-697.15661431061744</v>
+        <v>-606.64080887150897</v>
       </c>
       <c r="AU105" s="10">
-        <v>-709.99354967941292</v>
+        <v>-709.99354967941304</v>
       </c>
       <c r="AV105" s="10">
         <v>-599.35550095652775</v>
       </c>
       <c r="AW105" s="10">
-        <v>-343.0958935261209</v>
+        <v>-596.74269328513651</v>
       </c>
       <c r="AX105" s="10">
-        <v>-353.44525132785623</v>
+        <v>-415.44525132785617</v>
       </c>
       <c r="AY105" s="10">
         <v>-425.69181938980694</v>
       </c>
       <c r="AZ105" s="10">
-        <v>-435.83467260431513</v>
+        <v>-556.36283170977322</v>
       </c>
       <c r="BA105" s="10">
-        <v>-538.71054476225595</v>
+        <v>-538.71054476226163</v>
       </c>
       <c r="BB105" s="10">
         <v>-669.73196024443484</v>
       </c>
       <c r="BC105" s="10">
-        <v>-667.2754416466347</v>
+        <v>-667.27544164663459</v>
       </c>
       <c r="BD105" s="11">
-        <v>-664.84579787145424</v>
+        <v>-664.84579787145435</v>
       </c>
       <c r="BF105" t="s">
         <v>3</v>
       </c>
       <c r="BG105" s="9">
-        <v>-469.50377333333336</v>
+        <v>-469.5037733333333</v>
       </c>
       <c r="BH105" s="10">
-        <v>-479.25261333333367</v>
+        <v>-479.25261333333361</v>
       </c>
       <c r="BI105" s="10">
         <v>-488.89325893333381</v>
@@ -31972,64 +31972,64 @@
         <v>-498.42473638373389</v>
       </c>
       <c r="BK105" s="10">
-        <v>-507.84606317118778</v>
+        <v>-507.84606317118767</v>
       </c>
       <c r="BL105" s="10">
-        <v>-517.15624793972836</v>
+        <v>-517.15624793972847</v>
       </c>
       <c r="BM105" s="10">
         <v>-526.3542904111863</v>
       </c>
       <c r="BN105" s="10">
-        <v>-535.43918130488669</v>
+        <v>-535.43918130488703</v>
       </c>
       <c r="BO105" s="10">
-        <v>-544.40990225663086</v>
+        <v>-544.40990225663131</v>
       </c>
       <c r="BP105" s="10">
-        <v>-553.26542573694064</v>
+        <v>-553.26542573694098</v>
       </c>
       <c r="BQ105" s="10">
-        <v>-562.00471496857313</v>
+        <v>-562.00471496857358</v>
       </c>
       <c r="BR105" s="10">
-        <v>-570.62672384329039</v>
+        <v>-570.62672384329085</v>
       </c>
       <c r="BS105" s="10">
-        <v>-579.13039683788031</v>
+        <v>-579.13039683788065</v>
       </c>
       <c r="BT105" s="10">
-        <v>-587.5146689294213</v>
+        <v>-587.51466892942176</v>
       </c>
       <c r="BU105" s="10">
-        <v>-595.77846550978632</v>
+        <v>-595.77846550978677</v>
       </c>
       <c r="BV105" s="10">
-        <v>-603.92070229937508</v>
+        <v>-603.92070229937519</v>
       </c>
       <c r="BW105" s="10">
         <v>-642.94028526006969</v>
       </c>
       <c r="BX105" s="10">
-        <v>-650.83611050741047</v>
+        <v>-527.10954316950733</v>
       </c>
       <c r="BY105" s="10">
-        <v>-203.10984718409736</v>
+        <v>-100.116116521187</v>
       </c>
       <c r="BZ105" s="10">
-        <v>-102.25719273385209</v>
+        <v>-50.252022559975252</v>
       </c>
       <c r="CA105" s="10">
-        <v>-119.76985156301532</v>
+        <v>-173.51918530691626</v>
       </c>
       <c r="CB105" s="10">
-        <v>-246.3774774866057</v>
+        <v>-127.1594070670825</v>
       </c>
       <c r="CC105" s="10">
         <v>-353.11953461068646</v>
       </c>
       <c r="CD105" s="10">
-        <v>-360.24906934218279</v>
+        <v>-335.38957422077618</v>
       </c>
       <c r="CE105" s="10">
         <v>-594.91350259292938</v>
@@ -32041,7 +32041,7 @@
         <v>3</v>
       </c>
       <c r="CI105" s="9">
-        <v>-721.9573899999998</v>
+        <v>-721.95739000000003</v>
       </c>
       <c r="CJ105" s="10">
         <v>-627.63001333333307</v>
@@ -32050,31 +32050,31 @@
         <v>-608.70482533333291</v>
       </c>
       <c r="CL105" s="10">
-        <v>-525.75408116800008</v>
+        <v>-525.75408116800031</v>
       </c>
       <c r="CM105" s="10">
-        <v>-538.2053660585126</v>
+        <v>-538.20536605851248</v>
       </c>
       <c r="CN105" s="10">
-        <v>-550.57277855303903</v>
+        <v>-550.57277855303914</v>
       </c>
       <c r="CO105" s="10">
-        <v>-535.5114065759434</v>
+        <v>-535.51140657596716</v>
       </c>
       <c r="CP105" s="10">
-        <v>-545.50359329477897</v>
+        <v>-545.50359329477908</v>
       </c>
       <c r="CQ105" s="10">
-        <v>-542.47578355443204</v>
+        <v>-542.47578355443216</v>
       </c>
       <c r="CR105" s="10">
-        <v>-539.46970701642192</v>
+        <v>-539.46970701642203</v>
       </c>
       <c r="CS105" s="10">
-        <v>-536.48555927956966</v>
+        <v>-536.48555927956977</v>
       </c>
       <c r="CT105" s="10">
-        <v>-533.52353770308559</v>
+        <v>-533.52353770308571</v>
       </c>
       <c r="CU105" s="10">
         <v>-530.58384142241357</v>
@@ -32083,31 +32083,31 @@
         <v>-527.66667136521517</v>
       </c>
       <c r="CW105" s="10">
-        <v>-524.7722302675021</v>
+        <v>-581.40844954450267</v>
       </c>
       <c r="CX105" s="10">
-        <v>-587.03545136788466</v>
+        <v>-676.56738935657631</v>
       </c>
       <c r="CY105" s="10">
         <v>-689.21902170078533</v>
       </c>
       <c r="CZ105" s="10">
-        <v>-578.39400222609254</v>
+        <v>-578.39400222609243</v>
       </c>
       <c r="DA105" s="10">
-        <v>-575.5925410661273</v>
+        <v>-427.69650240215753</v>
       </c>
       <c r="DB105" s="10">
-        <v>-500.80726568377696</v>
+        <v>-491.48634890113885</v>
       </c>
       <c r="DC105" s="10">
-        <v>-565.57142561882688</v>
+        <v>-511.82209187493117</v>
       </c>
       <c r="DD105" s="10">
-        <v>-652.99830394788194</v>
+        <v>-652.99830394788182</v>
       </c>
       <c r="DE105" s="10">
-        <v>-650.29321546341282</v>
+        <v>-650.29321546341271</v>
       </c>
       <c r="DF105" s="10">
         <v>-647.61276467258358</v>
@@ -32116,7 +32116,7 @@
         <v>-644.95717331463675</v>
       </c>
       <c r="DH105" s="11">
-        <v>-642.32666512446849</v>
+        <v>-642.32666512446838</v>
       </c>
     </row>
     <row r="107" spans="1:112" x14ac:dyDescent="0.35">
@@ -32207,86 +32207,86 @@
         <v>6</v>
       </c>
       <c r="B108" s="15">
-        <v>4661545674.1639547</v>
+        <v>4661545545.3187819</v>
       </c>
       <c r="C108" s="16">
-        <v>812364292.23078156</v>
+        <v>812364292.23078132</v>
       </c>
       <c r="D108" s="16">
-        <v>1197815781.5387373</v>
+        <v>1197815781.5387371</v>
       </c>
       <c r="E108" s="16">
-        <v>584638424.27443945</v>
+        <v>584638424.27443933</v>
       </c>
       <c r="F108" s="16">
-        <v>528946338.26324528</v>
+        <v>528946338.26324517</v>
       </c>
       <c r="G108" s="16">
-        <v>478272349.81042486</v>
+        <v>478272349.81042469</v>
       </c>
       <c r="H108" s="16">
-        <v>402681595.9171024</v>
+        <v>402681595.91710228</v>
       </c>
       <c r="I108" s="16">
-        <v>338941628.48139793</v>
+        <v>338941628.48139787</v>
       </c>
       <c r="J108" s="16">
-        <v>310407609.96892494</v>
+        <v>310407609.96892488</v>
       </c>
       <c r="K108" s="16">
         <v>284280575.25051749</v>
       </c>
       <c r="L108" s="16">
-        <v>260356225.10975936</v>
+        <v>260356225.10975927</v>
       </c>
       <c r="M108" s="16">
-        <v>238465655.1729618</v>
+        <v>238465655.17296174</v>
       </c>
       <c r="N108" s="16">
-        <v>218464143.30382639</v>
+        <v>218464143.30382633</v>
       </c>
       <c r="O108" s="16">
-        <v>200157060.49841955</v>
+        <v>200157060.49841946</v>
       </c>
       <c r="P108" s="16">
-        <v>183400985.56374288</v>
+        <v>183400985.56374282</v>
       </c>
       <c r="Q108" s="16">
-        <v>168047552.91453198</v>
+        <v>168047552.91453195</v>
       </c>
       <c r="R108" s="16">
         <v>154150953.88463506</v>
       </c>
       <c r="S108" s="16">
-        <v>142069431.7878544</v>
+        <v>142069431.78785443</v>
       </c>
       <c r="T108" s="16">
-        <v>131102066.72049348</v>
+        <v>131102066.7204935</v>
       </c>
       <c r="U108" s="16">
-        <v>121065473.16000971</v>
+        <v>121065473.16000973</v>
       </c>
       <c r="V108" s="16">
-        <v>112021452.84694031</v>
+        <v>112021452.84694034</v>
       </c>
       <c r="W108" s="16">
-        <v>103961311.8906517</v>
+        <v>103961311.89065173</v>
       </c>
       <c r="X108" s="16">
-        <v>96425202.782605052</v>
+        <v>96425202.782605082</v>
       </c>
       <c r="Y108" s="16">
-        <v>89386823.434690207</v>
+        <v>89386823.434690222</v>
       </c>
       <c r="Z108" s="16">
-        <v>83019295.641113877</v>
+        <v>83019295.641113892</v>
       </c>
       <c r="AA108" s="17">
-        <v>77297346.698409989</v>
+        <v>77297346.698409975</v>
       </c>
       <c r="AB108" s="18">
         <f>SUM(TotalCost)</f>
-        <v>11979285251.310175</v>
+        <v>11979285122.464998</v>
       </c>
     </row>
     <row r="110" spans="1:112" x14ac:dyDescent="0.35">
@@ -32380,86 +32380,86 @@
         <v>8</v>
       </c>
       <c r="B111" s="3">
-        <v>55104186.340473607</v>
+        <v>55104211.948537596</v>
       </c>
       <c r="C111" s="4">
-        <v>34357971.406072415</v>
+        <v>34357971.406072207</v>
       </c>
       <c r="D111" s="4">
-        <v>32318462.221825525</v>
+        <v>32318462.221825358</v>
       </c>
       <c r="E111" s="4">
-        <v>34248174.436014675</v>
+        <v>34248174.436014406</v>
       </c>
       <c r="F111" s="4">
-        <v>32129962.474392615</v>
+        <v>32129962.474392395</v>
       </c>
       <c r="G111" s="4">
-        <v>30277766.691973425</v>
+        <v>30277766.691973232</v>
       </c>
       <c r="H111" s="4">
-        <v>28676041.735994853</v>
+        <v>28676041.735994659</v>
       </c>
       <c r="I111" s="4">
-        <v>26541733.214512516</v>
+        <v>26541733.214512412</v>
       </c>
       <c r="J111" s="4">
-        <v>24532512.636476815</v>
+        <v>24532512.636476714</v>
       </c>
       <c r="K111" s="4">
-        <v>22653326.616769154</v>
+        <v>22653326.61676906</v>
       </c>
       <c r="L111" s="4">
-        <v>20896823.714211311</v>
+        <v>20896823.714211218</v>
       </c>
       <c r="M111" s="4">
-        <v>19229729.392528825</v>
+        <v>19229729.392528754</v>
       </c>
       <c r="N111" s="4">
-        <v>17647715.719736893</v>
+        <v>17647715.719736807</v>
       </c>
       <c r="O111" s="4">
-        <v>16175533.170437135</v>
+        <v>16175533.170437058</v>
       </c>
       <c r="P111" s="4">
-        <v>14802084.614716556</v>
+        <v>14802084.614716511</v>
       </c>
       <c r="Q111" s="4">
-        <v>13519240.732661979</v>
+        <v>13519240.732661929</v>
       </c>
       <c r="R111" s="4">
-        <v>15693171.764753081</v>
+        <v>15693171.76475306</v>
       </c>
       <c r="S111" s="4">
-        <v>15200283.218220178</v>
+        <v>15200283.21822007</v>
       </c>
       <c r="T111" s="4">
-        <v>12624235.257461332</v>
+        <v>12624235.257461242</v>
       </c>
       <c r="U111" s="4">
         <v>11485312.420467805</v>
       </c>
       <c r="V111" s="4">
-        <v>9358037.9211615287</v>
+        <v>9358037.9211615194</v>
       </c>
       <c r="W111" s="4">
-        <v>8834548.1094163246</v>
+        <v>8834548.1094163135</v>
       </c>
       <c r="X111" s="4">
-        <v>8347511.2856087135</v>
+        <v>8347511.2856087014</v>
       </c>
       <c r="Y111" s="4">
-        <v>7894778.1470450358</v>
+        <v>7894778.1470450303</v>
       </c>
       <c r="Z111" s="4">
-        <v>7899157.4760805946</v>
+        <v>7899157.476080602</v>
       </c>
       <c r="AA111" s="5">
         <v>8179326.5577635802</v>
       </c>
       <c r="AB111" s="12">
         <f>SUM(B111:AA111)</f>
-        <v>528627627.27677631</v>
+        <v>528627652.88483822</v>
       </c>
     </row>
     <row r="112" spans="1:112" x14ac:dyDescent="0.35">
@@ -32467,86 +32467,86 @@
         <v>9</v>
       </c>
       <c r="B112" s="6">
-        <v>11413907.416598001</v>
+        <v>11413921.39271</v>
       </c>
       <c r="C112" s="7">
-        <v>6428544.4408859052</v>
+        <v>6428544.4408858651</v>
       </c>
       <c r="D112" s="7">
-        <v>6030474.5357231088</v>
+        <v>6030474.5357230753</v>
       </c>
       <c r="E112" s="7">
-        <v>6598627.357297997</v>
+        <v>6598627.3572978973</v>
       </c>
       <c r="F112" s="7">
-        <v>6128043.4996852474</v>
+        <v>6128043.4996851645</v>
       </c>
       <c r="G112" s="7">
-        <v>5754522.898488461</v>
+        <v>5754522.8984883893</v>
       </c>
       <c r="H112" s="7">
-        <v>5471874.8666465878</v>
+        <v>5471874.8666465171</v>
       </c>
       <c r="I112" s="7">
-        <v>4921246.5773487939</v>
+        <v>4921246.5773487734</v>
       </c>
       <c r="J112" s="7">
-        <v>4523898.2585312882</v>
+        <v>4523898.2585312687</v>
       </c>
       <c r="K112" s="7">
-        <v>4152228.8844427792</v>
+        <v>4152228.8844427611</v>
       </c>
       <c r="L112" s="7">
-        <v>3804788.0158199817</v>
+        <v>3804788.0158199635</v>
       </c>
       <c r="M112" s="7">
-        <v>3479612.5313849379</v>
+        <v>3479612.5313849244</v>
       </c>
       <c r="N112" s="7">
-        <v>3176559.4255006299</v>
+        <v>3176559.4255006132</v>
       </c>
       <c r="O112" s="7">
-        <v>2893958.829264089</v>
+        <v>2893958.8292640741</v>
       </c>
       <c r="P112" s="7">
-        <v>2628584.5726899761</v>
+        <v>2628584.5726899672</v>
       </c>
       <c r="Q112" s="7">
-        <v>2381338.9268881865</v>
+        <v>2381338.9268881767</v>
       </c>
       <c r="R112" s="7">
-        <v>2149500.5994941285</v>
+        <v>2149500.5994941196</v>
       </c>
       <c r="S112" s="7">
-        <v>2431747.4957153555</v>
+        <v>2431747.4957153457</v>
       </c>
       <c r="T112" s="7">
-        <v>2171974.5009293519</v>
+        <v>2171974.5009293435</v>
       </c>
       <c r="U112" s="7">
-        <v>1939768.588843843</v>
+        <v>1939768.5888438364</v>
       </c>
       <c r="V112" s="7">
-        <v>1012042.1855100931</v>
+        <v>1012042.1855100883</v>
       </c>
       <c r="W112" s="7">
-        <v>797089.71681231039</v>
+        <v>797089.71681230539</v>
       </c>
       <c r="X112" s="7">
-        <v>598301.75838386442</v>
+        <v>598301.75838385918</v>
       </c>
       <c r="Y112" s="7">
-        <v>414708.97000388568</v>
+        <v>414708.97000388324</v>
       </c>
       <c r="Z112" s="7">
-        <v>227913.62405979628</v>
+        <v>227913.62405979316</v>
       </c>
       <c r="AA112" s="8">
-        <v>54338.11139119447</v>
+        <v>54338.111391194463</v>
       </c>
       <c r="AB112" s="13">
         <f t="shared" ref="AB112:AB115" si="0">SUM(B112:AA112)</f>
-        <v>91585596.588339821</v>
+        <v>91585610.564451218</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -32554,86 +32554,86 @@
         <v>10</v>
       </c>
       <c r="B113" s="6">
-        <v>66117305188.450974</v>
+        <v>66117321812.58522</v>
       </c>
       <c r="C113" s="7">
-        <v>39412136279.096947</v>
+        <v>39412136279.096832</v>
       </c>
       <c r="D113" s="7">
-        <v>37286151059.075386</v>
+        <v>37286151059.075279</v>
       </c>
       <c r="E113" s="7">
-        <v>35274846584.186317</v>
+        <v>35274846584.186218</v>
       </c>
       <c r="F113" s="7">
-        <v>33372036699.803501</v>
+        <v>33372036699.803413</v>
       </c>
       <c r="G113" s="7">
-        <v>31571868947.328018</v>
+        <v>31571868947.327938</v>
       </c>
       <c r="H113" s="7">
-        <v>29868806563.823669</v>
+        <v>29868806563.823597</v>
       </c>
       <c r="I113" s="7">
-        <v>28257611452.635265</v>
+        <v>28257611452.635201</v>
       </c>
       <c r="J113" s="7">
-        <v>26733328072.612633</v>
+        <v>26733328072.612572</v>
       </c>
       <c r="K113" s="7">
-        <v>25291268196.388531</v>
+        <v>25291268196.388477</v>
       </c>
       <c r="L113" s="7">
-        <v>23926996490.831661</v>
+        <v>23926996490.831612</v>
       </c>
       <c r="M113" s="7">
-        <v>22636316875.324623</v>
+        <v>22636316875.324577</v>
       </c>
       <c r="N113" s="7">
-        <v>21415259615.909111</v>
+        <v>21415259615.909069</v>
       </c>
       <c r="O113" s="7">
-        <v>20260069115.603893</v>
+        <v>20260069115.603855</v>
       </c>
       <c r="P113" s="7">
-        <v>19167192363.342342</v>
+        <v>19167192363.342308</v>
       </c>
       <c r="Q113" s="7">
-        <v>18133268006.001984</v>
+        <v>18133268006.001953</v>
       </c>
       <c r="R113" s="7">
-        <v>17155116009.91502</v>
+        <v>17155116009.914995</v>
       </c>
       <c r="S113" s="7">
-        <v>16229727880.061779</v>
+        <v>16229727880.061758</v>
       </c>
       <c r="T113" s="7">
-        <v>15354257406.864334</v>
+        <v>15354257406.864315</v>
       </c>
       <c r="U113" s="7">
-        <v>14526011912.120295</v>
+        <v>14526011912.120277</v>
       </c>
       <c r="V113" s="7">
-        <v>13742443967.151936</v>
+        <v>13742443967.151922</v>
       </c>
       <c r="W113" s="7">
-        <v>13001143557.698238</v>
+        <v>13001143557.698227</v>
       </c>
       <c r="X113" s="7">
-        <v>12299830671.451456</v>
+        <v>12299830671.451447</v>
       </c>
       <c r="Y113" s="7">
-        <v>11636348285.439753</v>
+        <v>11636348285.439745</v>
       </c>
       <c r="Z113" s="7">
-        <v>11008655731.687246</v>
+        <v>11008655731.687241</v>
       </c>
       <c r="AA113" s="8">
-        <v>10414822420.746283</v>
+        <v>10414822420.746281</v>
       </c>
       <c r="AB113" s="13">
         <f t="shared" si="0"/>
-        <v>614092819353.55115</v>
+        <v>614092835977.68433</v>
       </c>
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.35">
@@ -32641,86 +32641,86 @@
         <v>11</v>
       </c>
       <c r="B114" s="6">
-        <v>5664130.1828996008</v>
+        <v>5664133.8732675994</v>
       </c>
       <c r="C114" s="7">
-        <v>3418054.8928181189</v>
+        <v>3418054.8928180989</v>
       </c>
       <c r="D114" s="7">
-        <v>3209656.9527732618</v>
+        <v>3209656.952773246</v>
       </c>
       <c r="E114" s="7">
-        <v>3324708.1294016647</v>
+        <v>3324708.129401648</v>
       </c>
       <c r="F114" s="7">
-        <v>3121581.7041416289</v>
+        <v>3121581.7041416154</v>
       </c>
       <c r="G114" s="7">
-        <v>2935512.3936430844</v>
+        <v>2935512.3936430714</v>
       </c>
       <c r="H114" s="7">
-        <v>2765382.6428108579</v>
+        <v>2765382.6428108457</v>
       </c>
       <c r="I114" s="7">
-        <v>2577110.4758842872</v>
+        <v>2577110.4758842774</v>
       </c>
       <c r="J114" s="7">
-        <v>2378811.7496876745</v>
+        <v>2378811.7496876651</v>
       </c>
       <c r="K114" s="7">
-        <v>2193045.7741749994</v>
+        <v>2193045.7741749906</v>
       </c>
       <c r="L114" s="7">
-        <v>2019108.3199224018</v>
+        <v>2019108.319922393</v>
       </c>
       <c r="M114" s="7">
-        <v>1855834.8167593975</v>
+        <v>1855834.8167593908</v>
       </c>
       <c r="N114" s="7">
-        <v>1703225.8996418533</v>
+        <v>1703225.8996418454</v>
       </c>
       <c r="O114" s="7">
-        <v>1560511.1139932408</v>
+        <v>1560511.1139932331</v>
       </c>
       <c r="P114" s="7">
-        <v>1425572.1892359583</v>
+        <v>1425572.1892359538</v>
       </c>
       <c r="Q114" s="7">
-        <v>1299556.6158445498</v>
+        <v>1299556.6158445452</v>
       </c>
       <c r="R114" s="7">
-        <v>1179532.703405316</v>
+        <v>1179532.7034053116</v>
       </c>
       <c r="S114" s="7">
-        <v>1073249.9273125087</v>
+        <v>1073249.927312505</v>
       </c>
       <c r="T114" s="7">
-        <v>960768.89977539913</v>
+        <v>960768.89977539598</v>
       </c>
       <c r="U114" s="7">
-        <v>848512.6475219581</v>
+        <v>848512.64752195484</v>
       </c>
       <c r="V114" s="7">
-        <v>721276.79676960385</v>
+        <v>721276.79676960164</v>
       </c>
       <c r="W114" s="7">
-        <v>610076.04271425272</v>
+        <v>610076.04271425016</v>
       </c>
       <c r="X114" s="7">
-        <v>506974.78670000029</v>
+        <v>506974.78669999773</v>
       </c>
       <c r="Y114" s="7">
-        <v>411491.32900664391</v>
+        <v>411491.32900664269</v>
       </c>
       <c r="Z114" s="7">
-        <v>315117.17527629796</v>
+        <v>315117.17527629633</v>
       </c>
       <c r="AA114" s="8">
-        <v>224304.3284481733</v>
+        <v>224304.32844817327</v>
       </c>
       <c r="AB114" s="13">
         <f t="shared" si="0"/>
-        <v>48303108.490562737</v>
+        <v>48303112.180930562</v>
       </c>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.35">
@@ -32728,86 +32728,86 @@
         <v>12</v>
       </c>
       <c r="B115" s="9">
-        <v>815751.33560480003</v>
+        <v>815751.8805808</v>
       </c>
       <c r="C115" s="10">
-        <v>493149.42508433067</v>
+        <v>493149.42508432776</v>
       </c>
       <c r="D115" s="10">
-        <v>462819.56763843674</v>
+        <v>462819.56763843441</v>
       </c>
       <c r="E115" s="10">
-        <v>480877.58680932107</v>
+        <v>480877.58680931851</v>
       </c>
       <c r="F115" s="10">
-        <v>451274.89326299378</v>
+        <v>451274.8932629918</v>
       </c>
       <c r="G115" s="10">
-        <v>424169.35862309398</v>
+        <v>424169.35862309218</v>
       </c>
       <c r="H115" s="10">
-        <v>399406.96042371646</v>
+        <v>399406.96042371466</v>
       </c>
       <c r="I115" s="10">
-        <v>371959.77761437465</v>
+        <v>371959.77761437313</v>
       </c>
       <c r="J115" s="10">
-        <v>342902.00497741729</v>
+        <v>342902.00497741584</v>
       </c>
       <c r="K115" s="10">
-        <v>315688.60810759931</v>
+        <v>315688.60810759803</v>
       </c>
       <c r="L115" s="10">
-        <v>290215.84949209413</v>
+        <v>290215.84949209285</v>
       </c>
       <c r="M115" s="10">
-        <v>266323.25367430551</v>
+        <v>266323.25367430452</v>
       </c>
       <c r="N115" s="10">
-        <v>243923.55770091648</v>
+        <v>243923.55770091526</v>
       </c>
       <c r="O115" s="10">
-        <v>222965.35919987355</v>
+        <v>222965.35919987247</v>
       </c>
       <c r="P115" s="10">
-        <v>203254.2734117026</v>
+        <v>203254.27341170193</v>
       </c>
       <c r="Q115" s="10">
-        <v>184854.56831552379</v>
+        <v>184854.56831552312</v>
       </c>
       <c r="R115" s="10">
-        <v>167261.31221045216</v>
+        <v>167261.31221045152</v>
       </c>
       <c r="S115" s="10">
-        <v>151427.98178278308</v>
+        <v>151427.98178278244</v>
       </c>
       <c r="T115" s="10">
-        <v>134238.93953660491</v>
+        <v>134238.93953660442</v>
       </c>
       <c r="U115" s="10">
-        <v>117614.07125859924</v>
+        <v>117614.07125859879</v>
       </c>
       <c r="V115" s="10">
-        <v>98974.758074872283</v>
+        <v>98974.758074871948</v>
       </c>
       <c r="W115" s="10">
-        <v>82737.962516088635</v>
+        <v>82737.962516088272</v>
       </c>
       <c r="X115" s="10">
-        <v>67691.758992165618</v>
+        <v>67691.75899216524</v>
       </c>
       <c r="Y115" s="10">
-        <v>53765.221913271744</v>
+        <v>53765.221913271569</v>
       </c>
       <c r="Z115" s="10">
-        <v>39636.356620474391</v>
+        <v>39636.356620474158</v>
       </c>
       <c r="AA115" s="11">
-        <v>26106.662328600411</v>
+        <v>26106.662328600407</v>
       </c>
       <c r="AB115" s="14">
         <f t="shared" si="0"/>
-        <v>6908991.4051744109</v>
+        <v>6908991.9501503836</v>
       </c>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
adding transportation CO2 to total
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -1380,10 +1380,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="7">
-        <v>393.74873215363738</v>
+        <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>665.6</v>
+        <v>621.16220471892393</v>
       </c>
       <c r="F4" s="7">
         <v>665.6</v>
@@ -1461,10 +1461,10 @@
         <v>52.151300499999081</v>
       </c>
       <c r="AG4" s="7">
-        <v>665.6</v>
+        <v>129.48653569999806</v>
       </c>
       <c r="AH4" s="7">
-        <v>665.6</v>
+        <v>208.22226634399806</v>
       </c>
       <c r="AI4" s="7">
         <v>665.6</v>
@@ -1527,10 +1527,10 @@
         <v>665.6</v>
       </c>
       <c r="BC4" s="7">
-        <v>665.6</v>
+        <v>662.55957706066624</v>
       </c>
       <c r="BD4" s="8">
-        <v>665.6</v>
+        <v>187.13164929451375</v>
       </c>
       <c r="BF4">
         <v>2</v>
@@ -1602,16 +1602,16 @@
         <v>665.6</v>
       </c>
       <c r="CC4" s="7">
-        <v>665.6</v>
+        <v>556.73396521109134</v>
       </c>
       <c r="CD4" s="7">
-        <v>665.6</v>
+        <v>401.07723657567954</v>
       </c>
       <c r="CE4" s="7">
-        <v>665.6</v>
+        <v>373.58402939749953</v>
       </c>
       <c r="CF4" s="8">
-        <v>665.6</v>
+        <v>195.65712581945664</v>
       </c>
       <c r="CH4">
         <v>2</v>
@@ -1623,10 +1623,10 @@
         <v>0</v>
       </c>
       <c r="CK4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="CL4" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="CM4" s="7">
         <v>665.6</v>
@@ -1689,10 +1689,10 @@
         <v>665.6</v>
       </c>
       <c r="DG4" s="7">
-        <v>665.6</v>
+        <v>462.32399903437374</v>
       </c>
       <c r="DH4" s="8">
-        <v>665.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:112" x14ac:dyDescent="0.35">
@@ -1715,10 +1715,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="H5" s="7">
-        <v>46.5</v>
+        <v>4.8841722620550172</v>
       </c>
       <c r="I5" s="7">
         <v>46.5</v>
@@ -1760,13 +1760,13 @@
         <v>46.5</v>
       </c>
       <c r="V5" s="7">
-        <v>10.973989944887649</v>
+        <v>42.199630749181779</v>
       </c>
       <c r="W5" s="7">
-        <v>4.5065835597594059</v>
+        <v>0</v>
       </c>
       <c r="X5" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="7">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>0</v>
       </c>
       <c r="AA5" s="8">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="AD5">
         <v>3</v>
@@ -1796,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="7">
         <v>46.5</v>
@@ -1835,10 +1835,10 @@
         <v>46.5</v>
       </c>
       <c r="AW5" s="7">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="AX5" s="7">
-        <v>4.2666595144801818</v>
+        <v>0</v>
       </c>
       <c r="AY5" s="7">
         <v>0</v>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="BL5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="BM5" s="7">
         <v>46.5</v>
@@ -1913,13 +1913,13 @@
         <v>46.5</v>
       </c>
       <c r="BX5" s="7">
-        <v>46.5</v>
+        <v>31.891244432901772</v>
       </c>
       <c r="BY5" s="7">
-        <v>26.490515986408354</v>
+        <v>34.437053556210003</v>
       </c>
       <c r="BZ5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="CA5" s="7">
         <v>0</v>
@@ -1958,10 +1958,10 @@
         <v>0</v>
       </c>
       <c r="CN5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="CO5" s="7">
-        <v>46.5</v>
+        <v>0.23198132801985594</v>
       </c>
       <c r="CP5" s="7">
         <v>46.5</v>
@@ -1991,13 +1991,13 @@
         <v>46.5</v>
       </c>
       <c r="CY5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="CZ5" s="7">
-        <v>46.5</v>
+        <v>0</v>
       </c>
       <c r="DA5" s="7">
-        <v>5.6837945071174545</v>
+        <v>0</v>
       </c>
       <c r="DB5" s="7">
         <v>0</v>
@@ -2032,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="7">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="E6" s="7">
         <v>212</v>
@@ -2107,7 +2107,7 @@
         <v>4</v>
       </c>
       <c r="AE6" s="6">
-        <v>188.19215022999967</v>
+        <v>188.19215023000024</v>
       </c>
       <c r="AF6" s="7">
         <v>212</v>
@@ -2275,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="CK6" s="7">
-        <v>212</v>
+        <v>1E-3</v>
       </c>
       <c r="CL6" s="7">
         <v>212</v>
@@ -2364,10 +2364,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="G7" s="7">
-        <v>464</v>
+        <v>439.2891282063477</v>
       </c>
       <c r="H7" s="7">
         <v>464</v>
@@ -2418,16 +2418,16 @@
         <v>464</v>
       </c>
       <c r="X7" s="7">
-        <v>463.1199952498539</v>
+        <v>414.51945480216932</v>
       </c>
       <c r="Y7" s="7">
-        <v>464</v>
+        <v>347.61374198980587</v>
       </c>
       <c r="Z7" s="7">
-        <v>464</v>
+        <v>262.66120023283236</v>
       </c>
       <c r="AA7" s="8">
-        <v>464</v>
+        <v>178.42378384599022</v>
       </c>
       <c r="AD7">
         <v>5</v>
@@ -2445,10 +2445,10 @@
         <v>0</v>
       </c>
       <c r="AI7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="AJ7" s="7">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="7">
         <v>464</v>
@@ -2490,25 +2490,25 @@
         <v>464</v>
       </c>
       <c r="AX7" s="7">
-        <v>464</v>
+        <v>407.77323581931751</v>
       </c>
       <c r="AY7" s="7">
-        <v>464</v>
+        <v>310.388918644245</v>
       </c>
       <c r="AZ7" s="7">
-        <v>464</v>
+        <v>205.01338665719754</v>
       </c>
       <c r="BA7" s="7">
-        <v>450.40953920636912</v>
+        <v>109.15953920636878</v>
       </c>
       <c r="BB7" s="7">
-        <v>390.34049532887821</v>
+        <v>0</v>
       </c>
       <c r="BC7" s="7">
-        <v>322.31959587866845</v>
+        <v>0</v>
       </c>
       <c r="BD7" s="8">
-        <v>368.8604097178054</v>
+        <v>0</v>
       </c>
       <c r="BF7">
         <v>5</v>
@@ -2520,16 +2520,16 @@
         <v>464</v>
       </c>
       <c r="BI7" s="7">
-        <v>64.341936699998655</v>
+        <v>464</v>
       </c>
       <c r="BJ7" s="7">
-        <v>164.33540916199865</v>
+        <v>164.33540916199851</v>
       </c>
       <c r="BK7" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BL7" s="7">
-        <v>464</v>
+        <v>418.3770497604321</v>
       </c>
       <c r="BM7" s="7">
         <v>464</v>
@@ -2571,25 +2571,25 @@
         <v>464</v>
       </c>
       <c r="BZ7" s="7">
-        <v>464</v>
+        <v>338.94220310946571</v>
       </c>
       <c r="CA7" s="7">
-        <v>464</v>
+        <v>192.88275837832543</v>
       </c>
       <c r="CB7" s="7">
-        <v>464</v>
+        <v>35.274621666756957</v>
       </c>
       <c r="CC7" s="7">
-        <v>378.63396521109075</v>
+        <v>0</v>
       </c>
       <c r="CD7" s="7">
-        <v>285.47723657567963</v>
+        <v>0</v>
       </c>
       <c r="CE7" s="7">
-        <v>180.82116172666497</v>
+        <v>0</v>
       </c>
       <c r="CF7" s="8">
-        <v>120.75299890739029</v>
+        <v>0</v>
       </c>
       <c r="CH7">
         <v>5</v>
@@ -2607,10 +2607,10 @@
         <v>0</v>
       </c>
       <c r="CM7" s="7">
-        <v>290.62982828918558</v>
+        <v>0</v>
       </c>
       <c r="CN7" s="7">
-        <v>464</v>
+        <v>1E-3</v>
       </c>
       <c r="CO7" s="7">
         <v>464</v>
@@ -2643,34 +2643,34 @@
         <v>464</v>
       </c>
       <c r="CY7" s="7">
-        <v>464</v>
+        <v>456.67575200559077</v>
       </c>
       <c r="CZ7" s="7">
-        <v>464</v>
+        <v>370.97482187248545</v>
       </c>
       <c r="DA7" s="7">
-        <v>464</v>
+        <v>294.68379450711768</v>
       </c>
       <c r="DB7" s="7">
-        <v>411.56388865653867</v>
+        <v>148.91534664134758</v>
       </c>
       <c r="DC7" s="7">
-        <v>336.62651257969929</v>
+        <v>0</v>
       </c>
       <c r="DD7" s="7">
-        <v>279.8832696895538</v>
+        <v>0</v>
       </c>
       <c r="DE7" s="7">
-        <v>215.09596025027633</v>
+        <v>0</v>
       </c>
       <c r="DF7" s="7">
-        <v>151.02658553053095</v>
+        <v>0</v>
       </c>
       <c r="DG7" s="7">
-        <v>39.223999034374174</v>
+        <v>0</v>
       </c>
       <c r="DH7" s="8">
-        <v>121.34066526638333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:112" x14ac:dyDescent="0.35">
@@ -3007,10 +3007,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="7">
-        <v>84.6</v>
+        <v>0</v>
       </c>
       <c r="D9" s="7">
-        <v>84.6</v>
+        <v>1E-3</v>
       </c>
       <c r="E9" s="7">
         <v>84.6</v>
@@ -3250,10 +3250,10 @@
         <v>1E-3</v>
       </c>
       <c r="CJ9" s="7">
-        <v>68.972629124942841</v>
+        <v>0</v>
       </c>
       <c r="CK9" s="7">
-        <v>84.6</v>
+        <v>6.1642016999985332</v>
       </c>
       <c r="CL9" s="7">
         <v>84.6</v>
@@ -3665,10 +3665,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="F11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="G11" s="7">
         <v>650</v>
@@ -3746,10 +3746,10 @@
         <v>0</v>
       </c>
       <c r="AH11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="AI11" s="7">
-        <v>650</v>
+        <v>303.83603359117967</v>
       </c>
       <c r="AJ11" s="7">
         <v>650</v>
@@ -3806,10 +3806,10 @@
         <v>650</v>
       </c>
       <c r="BB11" s="7">
-        <v>650</v>
+        <v>640.85686332219518</v>
       </c>
       <c r="BC11" s="7">
-        <v>650</v>
+        <v>408.22003763600441</v>
       </c>
       <c r="BD11" s="8">
         <v>650</v>
@@ -3818,19 +3818,19 @@
         <v>9</v>
       </c>
       <c r="BG11" s="6">
-        <v>55.593150229999651</v>
+        <v>55.593150229999765</v>
       </c>
       <c r="BH11" s="7">
-        <v>152.10430049999832</v>
+        <v>152.10430049999866</v>
       </c>
       <c r="BI11" s="7">
-        <v>650</v>
+        <v>250.34193669999809</v>
       </c>
       <c r="BJ11" s="7">
         <v>650</v>
       </c>
       <c r="BK11" s="7">
-        <v>650</v>
+        <v>616.11456710245147</v>
       </c>
       <c r="BL11" s="7">
         <v>650</v>
@@ -3890,10 +3890,10 @@
         <v>650</v>
       </c>
       <c r="CE11" s="7">
-        <v>650</v>
+        <v>320.67426465833103</v>
       </c>
       <c r="CF11" s="8">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="CH11">
         <v>9</v>
@@ -3908,10 +3908,10 @@
         <v>0</v>
       </c>
       <c r="CL11" s="7">
-        <v>496.63102836740586</v>
+        <v>0</v>
       </c>
       <c r="CM11" s="7">
-        <v>650</v>
+        <v>1E-3</v>
       </c>
       <c r="CN11" s="7">
         <v>650</v>
@@ -3959,22 +3959,22 @@
         <v>650</v>
       </c>
       <c r="DC11" s="7">
-        <v>650</v>
+        <v>615.9469064492489</v>
       </c>
       <c r="DD11" s="7">
-        <v>650</v>
+        <v>417.21379922388599</v>
       </c>
       <c r="DE11" s="7">
-        <v>650</v>
+        <v>237.74552562569124</v>
       </c>
       <c r="DF11" s="7">
-        <v>650</v>
+        <v>42.572088826327331</v>
       </c>
       <c r="DG11" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="DH11" s="8">
-        <v>650</v>
+        <v>218.33228816595874</v>
       </c>
     </row>
     <row r="12" spans="1:112" x14ac:dyDescent="0.35">
@@ -4057,7 +4057,7 @@
         <v>0</v>
       </c>
       <c r="AA12" s="8">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="AD12">
         <v>10</v>
@@ -4084,13 +4084,13 @@
         <v>0</v>
       </c>
       <c r="AL12" s="7">
-        <v>186</v>
+        <v>22.857540059397934</v>
       </c>
       <c r="AM12" s="7">
         <v>186</v>
       </c>
       <c r="AN12" s="7">
-        <v>186</v>
+        <v>182.19090898004583</v>
       </c>
       <c r="AO12" s="7">
         <v>186</v>
@@ -4219,7 +4219,7 @@
         <v>0</v>
       </c>
       <c r="CF12" s="8">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="CH12">
         <v>10</v>
@@ -4246,16 +4246,16 @@
         <v>0</v>
       </c>
       <c r="CP12" s="7">
-        <v>137.77773168219755</v>
+        <v>186</v>
       </c>
       <c r="CQ12" s="7">
+        <v>154.52682637145858</v>
+      </c>
+      <c r="CR12" s="7">
         <v>186</v>
       </c>
-      <c r="CR12" s="7">
-        <v>41.669689448471559</v>
-      </c>
       <c r="CS12" s="7">
-        <v>142.02598075897299</v>
+        <v>114.29698879331659</v>
       </c>
       <c r="CT12" s="7">
         <v>0</v>
@@ -4975,10 +4975,10 @@
         <v>1848</v>
       </c>
       <c r="G15" s="7">
-        <v>1709.7891282063479</v>
+        <v>1848</v>
       </c>
       <c r="H15" s="7">
-        <v>1E-3</v>
+        <v>1848</v>
       </c>
       <c r="I15" s="7">
         <v>0</v>
@@ -4993,46 +4993,46 @@
         <v>0</v>
       </c>
       <c r="M15" s="7">
-        <v>1128.8325853266106</v>
+        <v>1078.8325853266101</v>
       </c>
       <c r="N15" s="7">
-        <v>1043.519642819082</v>
+        <v>956.01964281908215</v>
       </c>
       <c r="O15" s="7">
-        <v>959.37501728620612</v>
+        <v>671.44951748554809</v>
       </c>
       <c r="P15" s="7">
-        <v>876.41857027927108</v>
+        <v>726.41857027927153</v>
       </c>
       <c r="Q15" s="7">
-        <v>704.54859629889552</v>
+        <v>632.17050163321846</v>
       </c>
       <c r="R15" s="7">
-        <v>597.26106520822896</v>
+        <v>526.65135216658325</v>
       </c>
       <c r="S15" s="7">
-        <v>659.88201431901484</v>
+        <v>422.38201431901484</v>
       </c>
       <c r="T15" s="7">
-        <v>581.88373488803688</v>
+        <v>331.88373488803688</v>
       </c>
       <c r="U15" s="7">
-        <v>517.67812266673343</v>
+        <v>192.67812266673343</v>
       </c>
       <c r="V15" s="7">
-        <v>500.83917149429146</v>
+        <v>75.887889885703373</v>
       </c>
       <c r="W15" s="7">
-        <v>452.22000363007646</v>
+        <v>0</v>
       </c>
       <c r="X15" s="7">
-        <v>390.29691910463043</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="7">
-        <v>317.22748397961186</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="7">
-        <v>234.82240046566449</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="8">
         <v>0</v>
@@ -5056,10 +5056,10 @@
         <v>1848</v>
       </c>
       <c r="AJ15" s="7">
-        <v>24.890852503440442</v>
+        <v>1848</v>
       </c>
       <c r="AK15" s="7">
-        <v>0</v>
+        <v>1848</v>
       </c>
       <c r="AL15" s="7">
         <v>0</v>
@@ -5074,37 +5074,37 @@
         <v>0</v>
       </c>
       <c r="AP15" s="7">
-        <v>1246.8712706601282</v>
+        <v>1176.8712706601284</v>
       </c>
       <c r="AQ15" s="7">
-        <v>1050.9313260040872</v>
+        <v>988.3405608032698</v>
       </c>
       <c r="AR15" s="7">
-        <v>935.05058234515684</v>
+        <v>818.63596587612562</v>
       </c>
       <c r="AS15" s="7">
-        <v>842.78002999521914</v>
+        <v>632.78002999521948</v>
       </c>
       <c r="AT15" s="7">
-        <v>728.29568116433654</v>
+        <v>483.29568116433666</v>
       </c>
       <c r="AU15" s="7">
-        <v>615.20623474973024</v>
+        <v>317.70623474973024</v>
       </c>
       <c r="AV15" s="7">
-        <v>486.03540490607475</v>
+        <v>153.53540490607509</v>
       </c>
       <c r="AW15" s="7">
-        <v>451.30730811507817</v>
+        <v>0</v>
       </c>
       <c r="AX15" s="7">
-        <v>334.01315260967453</v>
+        <v>0</v>
       </c>
       <c r="AY15" s="7">
-        <v>200.27783728848988</v>
+        <v>0</v>
       </c>
       <c r="AZ15" s="7">
-        <v>94.526773314394404</v>
+        <v>0</v>
       </c>
       <c r="BA15" s="7">
         <v>0</v>
@@ -5137,55 +5137,55 @@
         <v>1848</v>
       </c>
       <c r="BL15" s="7">
-        <v>1571.5592735724313</v>
+        <v>1848</v>
       </c>
       <c r="BM15" s="7">
-        <v>1145.6518821943591</v>
+        <v>1848</v>
       </c>
       <c r="BN15" s="7">
-        <v>866.97230951446249</v>
+        <v>1041.9723095144623</v>
       </c>
       <c r="BO15" s="7">
-        <v>626.20298064560711</v>
+        <v>726.20298064560757</v>
       </c>
       <c r="BP15" s="7">
-        <v>362.37636953088281</v>
+        <v>412.37636953088236</v>
       </c>
       <c r="BQ15" s="7">
-        <v>150.52450247380705</v>
+        <v>100.52550247380657</v>
       </c>
       <c r="BR15" s="7">
-        <v>1833.6226737786883</v>
+        <v>1670.046234054937</v>
       </c>
       <c r="BS15" s="7">
-        <v>1627.3842377748465</v>
+        <v>1452.3842377748467</v>
       </c>
       <c r="BT15" s="7">
-        <v>1422.8083853562168</v>
+        <v>1197.8083853562173</v>
       </c>
       <c r="BU15" s="7">
-        <v>1219.9233806064715</v>
+        <v>919.92338060647148</v>
       </c>
       <c r="BV15" s="7">
-        <v>1043.7579687359826</v>
+        <v>693.75796873598267</v>
       </c>
       <c r="BW15" s="7">
-        <v>869.34138121009312</v>
+        <v>444.34138121009266</v>
       </c>
       <c r="BX15" s="7">
-        <v>671.70334885626471</v>
+        <v>225.92085999046117</v>
       </c>
       <c r="BY15" s="7">
-        <v>515.8930751396025</v>
+        <v>0</v>
       </c>
       <c r="BZ15" s="7">
-        <v>306.88440621893096</v>
+        <v>0</v>
       </c>
       <c r="CA15" s="7">
-        <v>182.76551675665314</v>
+        <v>0</v>
       </c>
       <c r="CB15" s="7">
-        <v>17.549243333513459</v>
+        <v>0</v>
       </c>
       <c r="CC15" s="7">
         <v>0</v>
@@ -5221,7 +5221,7 @@
         <v>1848</v>
       </c>
       <c r="CO15" s="7">
-        <v>1353.7973705504482</v>
+        <v>1848</v>
       </c>
       <c r="CP15" s="7">
         <v>0</v>
@@ -5236,25 +5236,25 @@
         <v>0</v>
       </c>
       <c r="CT15" s="7">
-        <v>813.03593353943825</v>
+        <v>609.75376040318497</v>
       </c>
       <c r="CU15" s="7">
-        <v>606.5410131857958</v>
+        <v>574.93747955196568</v>
       </c>
       <c r="CV15" s="7">
-        <v>517.80332287971999</v>
+        <v>414.25713849075328</v>
       </c>
       <c r="CW15" s="7">
-        <v>431.52676254429514</v>
+        <v>221.52676254429491</v>
       </c>
       <c r="CX15" s="7">
-        <v>310.05110816674699</v>
+        <v>65.051108166746872</v>
       </c>
       <c r="CY15" s="7">
-        <v>124.51792994448294</v>
+        <v>0</v>
       </c>
       <c r="CZ15" s="7">
-        <v>53.449643744971013</v>
+        <v>0</v>
       </c>
       <c r="DA15" s="7">
         <v>0</v>
@@ -5361,7 +5361,7 @@
         <v>0</v>
       </c>
       <c r="AA16" s="8">
-        <v>37.347567691980771</v>
+        <v>0</v>
       </c>
       <c r="AD16">
         <v>14</v>
@@ -5478,7 +5478,7 @@
         <v>0</v>
       </c>
       <c r="BQ16" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BR16" s="7">
         <v>0</v>
@@ -5523,7 +5523,7 @@
         <v>0</v>
       </c>
       <c r="CF16" s="8">
-        <v>51.859506555655116</v>
+        <v>0</v>
       </c>
       <c r="CH16">
         <v>14</v>
@@ -5849,7 +5849,7 @@
         <v>0</v>
       </c>
       <c r="CF17" s="8">
-        <v>50.3</v>
+        <v>0</v>
       </c>
       <c r="CH17">
         <v>15</v>
@@ -5953,10 +5953,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="H18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="I18" s="7">
         <v>67</v>
@@ -5980,40 +5980,40 @@
         <v>67</v>
       </c>
       <c r="P18" s="7">
-        <v>67</v>
+        <v>25.818460343767015</v>
       </c>
       <c r="Q18" s="7">
         <v>67</v>
       </c>
       <c r="R18" s="7">
+        <v>22.473412038366348</v>
+      </c>
+      <c r="S18" s="7">
+        <v>1.0000000000047748E-3</v>
+      </c>
+      <c r="T18" s="7">
+        <v>45.093743581803778</v>
+      </c>
+      <c r="U18" s="7">
+        <v>1.0000000000047748E-3</v>
+      </c>
+      <c r="V18" s="7">
+        <v>1.0000000000047748E-3</v>
+      </c>
+      <c r="W18" s="7">
+        <v>30.566882403527416</v>
+      </c>
+      <c r="X18" s="7">
         <v>67</v>
       </c>
-      <c r="S18" s="7">
-        <v>0</v>
-      </c>
-      <c r="T18" s="7">
-        <v>0</v>
-      </c>
-      <c r="U18" s="7">
-        <v>0</v>
-      </c>
-      <c r="V18" s="7">
-        <v>0</v>
-      </c>
-      <c r="W18" s="7">
-        <v>0</v>
-      </c>
-      <c r="X18" s="7">
-        <v>0</v>
-      </c>
       <c r="Y18" s="7">
-        <v>1E-3</v>
+        <v>67</v>
       </c>
       <c r="Z18" s="7">
-        <v>0</v>
+        <v>18.761890678388482</v>
       </c>
       <c r="AA18" s="8">
-        <v>67</v>
+        <v>21.082550768985129</v>
       </c>
       <c r="AD18">
         <v>16</v>
@@ -6034,10 +6034,10 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="AK18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="AL18" s="7">
         <v>67</v>
@@ -6061,10 +6061,10 @@
         <v>67</v>
       </c>
       <c r="AS18" s="7">
-        <v>67</v>
+        <v>45.074632498804021</v>
       </c>
       <c r="AT18" s="7">
-        <v>67</v>
+        <v>64.578545291084424</v>
       </c>
       <c r="AU18" s="7">
         <v>67</v>
@@ -6076,25 +6076,25 @@
         <v>67</v>
       </c>
       <c r="AX18" s="7">
+        <v>43.415478728976723</v>
+      </c>
+      <c r="AY18" s="7">
         <v>67</v>
       </c>
-      <c r="AY18" s="7">
-        <v>0</v>
-      </c>
       <c r="AZ18" s="7">
-        <v>0</v>
+        <v>1.0000000000047748E-3</v>
       </c>
       <c r="BA18" s="7">
-        <v>0</v>
+        <v>8.4782227387188414</v>
       </c>
       <c r="BB18" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BC18" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="BD18" s="8">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="BF18">
         <v>16</v>
@@ -6115,10 +6115,10 @@
         <v>0</v>
       </c>
       <c r="BL18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="BM18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="BN18" s="7">
         <v>67</v>
@@ -6157,22 +6157,22 @@
         <v>67</v>
       </c>
       <c r="BZ18" s="7">
+        <v>48.399979580650182</v>
+      </c>
+      <c r="CA18" s="7">
         <v>67</v>
       </c>
-      <c r="CA18" s="7">
-        <v>1E-3</v>
-      </c>
       <c r="CB18" s="7">
-        <v>1E-3</v>
+        <v>67</v>
       </c>
       <c r="CC18" s="7">
-        <v>1E-3</v>
+        <v>67</v>
       </c>
       <c r="CD18" s="7">
-        <v>65.658249775929278</v>
+        <v>49.81948420440807</v>
       </c>
       <c r="CE18" s="7">
-        <v>62.155212378066281</v>
+        <v>67</v>
       </c>
       <c r="CF18" s="8">
         <v>67</v>
@@ -6196,10 +6196,10 @@
         <v>0</v>
       </c>
       <c r="CN18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="CO18" s="7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="CP18" s="7">
         <v>67</v>
@@ -6223,22 +6223,22 @@
         <v>67</v>
       </c>
       <c r="CW18" s="7">
-        <v>33.8189716721281</v>
+        <v>1.0000000000047748E-3</v>
       </c>
       <c r="CX18" s="7">
-        <v>67</v>
+        <v>8.1731874075753694</v>
       </c>
       <c r="CY18" s="7">
-        <v>67</v>
+        <v>1.0000000000047748E-3</v>
       </c>
       <c r="CZ18" s="7">
-        <v>25.892685764889393</v>
+        <v>1.0000000000047748E-3</v>
       </c>
       <c r="DA18" s="7">
-        <v>0</v>
+        <v>1.0000000000047748E-3</v>
       </c>
       <c r="DB18" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="DC18" s="7">
         <v>0</v>
@@ -6256,7 +6256,7 @@
         <v>0</v>
       </c>
       <c r="DH18" s="8">
-        <v>23.891622899575395</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:112" x14ac:dyDescent="0.35">
@@ -6282,13 +6282,13 @@
         <v>257</v>
       </c>
       <c r="H19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="I19" s="7">
         <v>257</v>
       </c>
       <c r="J19" s="7">
-        <v>1E-3</v>
+        <v>257</v>
       </c>
       <c r="K19" s="7">
         <v>257</v>
@@ -6297,46 +6297,46 @@
         <v>257</v>
       </c>
       <c r="M19" s="7">
-        <v>31.280021331652392</v>
+        <v>31.280021331652506</v>
       </c>
       <c r="N19" s="7">
         <v>47.451785704770828</v>
       </c>
       <c r="O19" s="7">
-        <v>63.915629321551705</v>
+        <v>239.34112912220894</v>
       </c>
       <c r="P19" s="7">
-        <v>80.676517569818202</v>
+        <v>121.85805722605073</v>
       </c>
       <c r="Q19" s="7">
-        <v>200.36140574262618</v>
+        <v>97.739500408304593</v>
       </c>
       <c r="R19" s="7">
-        <v>257</v>
+        <v>159.63630100327958</v>
       </c>
       <c r="S19" s="7">
-        <v>199.79237857975363</v>
+        <v>199.79137857975365</v>
       </c>
       <c r="T19" s="7">
-        <v>217.79280872200945</v>
+        <v>172.69906514020556</v>
       </c>
       <c r="U19" s="7">
-        <v>236.11640566668359</v>
+        <v>236.11540566668361</v>
       </c>
       <c r="V19" s="7">
-        <v>219.24265279090469</v>
+        <v>250.46729359519873</v>
       </c>
       <c r="W19" s="7">
-        <v>231.76175124715814</v>
+        <v>220.42145603346728</v>
       </c>
       <c r="X19" s="7">
-        <v>245.70259765093851</v>
+        <v>130.10105720325419</v>
       </c>
       <c r="Y19" s="7">
-        <v>257</v>
+        <v>82.86748798470876</v>
       </c>
       <c r="Z19" s="7">
-        <v>257</v>
+        <v>66.176784670859632</v>
       </c>
       <c r="AA19" s="8">
         <v>0</v>
@@ -6369,7 +6369,7 @@
         <v>257</v>
       </c>
       <c r="AM19" s="7">
-        <v>1E-3</v>
+        <v>257</v>
       </c>
       <c r="AN19" s="7">
         <v>257</v>
@@ -6378,19 +6378,19 @@
         <v>257</v>
       </c>
       <c r="AP19" s="7">
-        <v>178.59844266503217</v>
+        <v>178.59844266503205</v>
       </c>
       <c r="AQ19" s="7">
+        <v>197.09076520081771</v>
+      </c>
+      <c r="AR19" s="7">
+        <v>215.91461646903167</v>
+      </c>
+      <c r="AS19" s="7">
         <v>257</v>
       </c>
-      <c r="AR19" s="7">
+      <c r="AT19" s="7">
         <v>257</v>
-      </c>
-      <c r="AS19" s="7">
-        <v>235.07563249880468</v>
-      </c>
-      <c r="AT19" s="7">
-        <v>254.57854529108442</v>
       </c>
       <c r="AU19" s="7">
         <v>257</v>
@@ -6405,19 +6405,19 @@
         <v>257</v>
       </c>
       <c r="AY19" s="7">
-        <v>257</v>
+        <v>157.33900296636784</v>
       </c>
       <c r="AZ19" s="7">
-        <v>257</v>
+        <v>140.64970498579623</v>
       </c>
       <c r="BA19" s="7">
-        <v>257</v>
+        <v>58.391711070835299</v>
       </c>
       <c r="BB19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="BC19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="BD19" s="8">
         <v>0</v>
@@ -6489,16 +6489,16 @@
         <v>257</v>
       </c>
       <c r="CB19" s="7">
-        <v>257</v>
+        <v>248.41655750013501</v>
       </c>
       <c r="CC19" s="7">
-        <v>257</v>
+        <v>132.20657281663694</v>
       </c>
       <c r="CD19" s="7">
-        <v>257</v>
+        <v>22.151995659111719</v>
       </c>
       <c r="CE19" s="7">
-        <v>257</v>
+        <v>6.4002352608320052</v>
       </c>
       <c r="CF19" s="8">
         <v>0</v>
@@ -6525,13 +6525,13 @@
         <v>257</v>
       </c>
       <c r="CO19" s="7">
-        <v>257</v>
+        <v>150.62814887271884</v>
       </c>
       <c r="CP19" s="7">
         <v>257</v>
       </c>
       <c r="CQ19" s="7">
-        <v>1E-3</v>
+        <v>257</v>
       </c>
       <c r="CR19" s="7">
         <v>257</v>
@@ -6540,43 +6540,43 @@
         <v>257</v>
       </c>
       <c r="CT19" s="7">
-        <v>123.71782686374814</v>
+        <v>257</v>
       </c>
       <c r="CU19" s="7">
-        <v>204.36618869664335</v>
+        <v>113.46972233047245</v>
       </c>
       <c r="CV19" s="7">
-        <v>168.77372523372014</v>
+        <v>114.81990962268776</v>
       </c>
       <c r="CW19" s="7">
-        <v>165.44334396394584</v>
+        <v>199.26131563607385</v>
       </c>
       <c r="CX19" s="7">
-        <v>150.01840204168684</v>
+        <v>208.84521463411147</v>
       </c>
       <c r="CY19" s="7">
-        <v>233.42707506949387</v>
+        <v>181.2682530083863</v>
       </c>
       <c r="CZ19" s="7">
-        <v>227.6003501713534</v>
+        <v>113.96685780872826</v>
       </c>
       <c r="DA19" s="7">
-        <v>231.40631676067642</v>
+        <v>56.405316760676556</v>
       </c>
       <c r="DB19" s="7">
-        <v>192.3504579848086</v>
+        <v>0</v>
       </c>
       <c r="DC19" s="7">
-        <v>136.82039386954898</v>
+        <v>0</v>
       </c>
       <c r="DD19" s="7">
-        <v>99.830529534331617</v>
+        <v>0</v>
       </c>
       <c r="DE19" s="7">
-        <v>55.149565375415477</v>
+        <v>0</v>
       </c>
       <c r="DF19" s="7">
-        <v>11.545503295796834</v>
+        <v>0</v>
       </c>
       <c r="DG19" s="7">
         <v>0</v>
@@ -6593,34 +6593,34 @@
         <v>2007.5531502299996</v>
       </c>
       <c r="C20" s="7">
-        <v>1989.2723004999998</v>
+        <v>2073.8723004999997</v>
       </c>
       <c r="D20" s="7">
-        <v>1451.0559405463616</v>
+        <v>2141.4036726999993</v>
       </c>
       <c r="E20" s="7">
-        <v>597.97089167399861</v>
+        <v>1292.4086869550747</v>
       </c>
       <c r="F20" s="7">
-        <v>367.99093281715614</v>
+        <v>1017.9919328171561</v>
       </c>
       <c r="G20" s="7">
         <v>0</v>
       </c>
       <c r="H20" s="7">
-        <v>1482.3831722620553</v>
+        <v>0</v>
       </c>
       <c r="I20" s="7">
-        <v>1270.2991285133096</v>
+        <v>1357.7991285133098</v>
       </c>
       <c r="J20" s="7">
-        <v>1427.5554355674353</v>
+        <v>1220.5564355674351</v>
       </c>
       <c r="K20" s="7">
-        <v>1059.6789131863811</v>
+        <v>1084.6789131863811</v>
       </c>
       <c r="L20" s="7">
-        <v>975.18976937144953</v>
+        <v>950.18976937144964</v>
       </c>
       <c r="M20" s="7">
         <v>0</v>
@@ -6659,10 +6659,10 @@
         <v>0</v>
       </c>
       <c r="Y20" s="7">
-        <v>9.2527459949030799</v>
+        <v>0</v>
       </c>
       <c r="Z20" s="7">
-        <v>29.277475116416099</v>
+        <v>0</v>
       </c>
       <c r="AA20" s="8">
         <v>0</v>
@@ -6677,31 +6677,31 @@
         <v>2269.6</v>
       </c>
       <c r="AG20" s="7">
-        <v>1733.4865356999983</v>
+        <v>2269.6</v>
       </c>
       <c r="AH20" s="7">
-        <v>1162.2222663449975</v>
+        <v>2269.6000000009999</v>
       </c>
       <c r="AI20" s="7">
-        <v>478.38230085756186</v>
+        <v>1288.5462672663825</v>
       </c>
       <c r="AJ20" s="7">
-        <v>2269.6</v>
+        <v>1023.9908525034407</v>
       </c>
       <c r="AK20" s="7">
-        <v>2077.572545872199</v>
+        <v>296.57254587219916</v>
       </c>
       <c r="AL20" s="7">
-        <v>1836.1524244748257</v>
+        <v>2121.794884415428</v>
       </c>
       <c r="AM20" s="7">
-        <v>1934.2549575602966</v>
+        <v>1747.2559575602968</v>
       </c>
       <c r="AN20" s="7">
-        <v>1502.4090470531219</v>
+        <v>1541.2181380730763</v>
       </c>
       <c r="AO20" s="7">
-        <v>1364.138035513924</v>
+        <v>1329.138035513924</v>
       </c>
       <c r="AP20" s="7">
         <v>0</v>
@@ -6713,37 +6713,37 @@
         <v>0</v>
       </c>
       <c r="AS20" s="7">
-        <v>0</v>
+        <v>1.0000000002037268E-3</v>
       </c>
       <c r="AT20" s="7">
-        <v>1E-3</v>
+        <v>1.0000000002037268E-3</v>
       </c>
       <c r="AU20" s="7">
-        <v>17.432183687432939</v>
+        <v>17.432183687433394</v>
       </c>
       <c r="AV20" s="7">
-        <v>37.639476226518809</v>
+        <v>37.639476226519037</v>
       </c>
       <c r="AW20" s="7">
-        <v>11.707452028769808</v>
+        <v>66.514760143848321</v>
       </c>
       <c r="AX20" s="7">
-        <v>36.908902424139114</v>
+        <v>0</v>
       </c>
       <c r="AY20" s="7">
-        <v>120.95008432212273</v>
+        <v>0</v>
       </c>
       <c r="AZ20" s="7">
-        <v>142.63731832859912</v>
+        <v>0</v>
       </c>
       <c r="BA20" s="7">
-        <v>151.11993380955437</v>
+        <v>0</v>
       </c>
       <c r="BB20" s="7">
-        <v>113.51536799331711</v>
+        <v>0</v>
       </c>
       <c r="BC20" s="7">
-        <v>68.359018818002596</v>
+        <v>0</v>
       </c>
       <c r="BD20" s="8">
         <v>0</v>
@@ -6764,13 +6764,13 @@
         <v>2269.6</v>
       </c>
       <c r="BK20" s="7">
-        <v>2235.7135671024512</v>
+        <v>2269.6</v>
       </c>
       <c r="BL20" s="7">
-        <v>2038.2504937020612</v>
+        <v>1920.9327175140609</v>
       </c>
       <c r="BM20" s="7">
-        <v>2269.6</v>
+        <v>1634.251882194359</v>
       </c>
       <c r="BN20" s="7">
         <v>2269.6</v>
@@ -6785,46 +6785,46 @@
         <v>2269.6</v>
       </c>
       <c r="BR20" s="7">
-        <v>212.66129344467242</v>
+        <v>276.23773316842335</v>
       </c>
       <c r="BS20" s="7">
         <v>236.10168444371209</v>
       </c>
       <c r="BT20" s="7">
-        <v>259.95772133905507</v>
+        <v>259.95772133905461</v>
       </c>
       <c r="BU20" s="7">
         <v>284.23647015161828</v>
       </c>
       <c r="BV20" s="7">
-        <v>308.9451171839961</v>
+        <v>308.94511718399599</v>
       </c>
       <c r="BW20" s="7">
-        <v>334.09097030252406</v>
+        <v>334.09097030252383</v>
       </c>
       <c r="BX20" s="7">
-        <v>359.68146221406664</v>
+        <v>345.07270664696853</v>
       </c>
       <c r="BY20" s="7">
-        <v>365.71466776451416</v>
+        <v>373.66120533431558</v>
       </c>
       <c r="BZ20" s="7">
-        <v>412.2267265547332</v>
+        <v>259.2689500835487</v>
       </c>
       <c r="CA20" s="7">
-        <v>459.69600418916184</v>
+        <v>121.57976256748861</v>
       </c>
       <c r="CB20" s="7">
-        <v>487.14193583337851</v>
+        <v>1.0000000002037268E-3</v>
       </c>
       <c r="CC20" s="7">
-        <v>429.70557281663696</v>
+        <v>0</v>
       </c>
       <c r="CD20" s="7">
-        <v>299.31323008759051</v>
+        <v>0</v>
       </c>
       <c r="CE20" s="7">
-        <v>227.08215521193154</v>
+        <v>0</v>
       </c>
       <c r="CF20" s="8">
         <v>0</v>
@@ -6836,34 +6836,34 @@
         <v>2136.3921502299995</v>
       </c>
       <c r="CJ20" s="7">
-        <v>2136.476671375056</v>
+        <v>2205.449300499999</v>
       </c>
       <c r="CK20" s="7">
-        <v>1313.5652016999986</v>
+        <v>2269.6</v>
       </c>
       <c r="CL20" s="7">
-        <v>888.53124129959269</v>
+        <v>2050.7622696669987</v>
       </c>
       <c r="CM20" s="7">
-        <v>217.43245594685152</v>
+        <v>1158.0612842360374</v>
       </c>
       <c r="CN20" s="7">
-        <v>4.7873955993500203</v>
+        <v>582.28639559934993</v>
       </c>
       <c r="CO20" s="7">
-        <v>274.56275965028999</v>
+        <v>0</v>
       </c>
       <c r="CP20" s="7">
-        <v>1427.5256660547527</v>
+        <v>1501.8033977369505</v>
       </c>
       <c r="CQ20" s="7">
-        <v>1469.639497367878</v>
+        <v>1314.1136709964196</v>
       </c>
       <c r="CR20" s="7">
-        <v>1174.2254345889601</v>
+        <v>1064.8951240374317</v>
       </c>
       <c r="CS20" s="7">
-        <v>927.565395047994</v>
+        <v>920.29438701365052</v>
       </c>
       <c r="CT20" s="7">
         <v>0</v>
@@ -7317,7 +7317,7 @@
         <v>0</v>
       </c>
       <c r="AA22" s="8">
-        <v>286.1587669229948</v>
+        <v>0</v>
       </c>
       <c r="AD22">
         <v>20</v>
@@ -7398,7 +7398,7 @@
         <v>0</v>
       </c>
       <c r="BD22" s="8">
-        <v>328.17123957670856</v>
+        <v>0</v>
       </c>
       <c r="BF22">
         <v>20</v>
@@ -7479,7 +7479,7 @@
         <v>0</v>
       </c>
       <c r="CF22" s="8">
-        <v>398.3</v>
+        <v>157.9041269120662</v>
       </c>
       <c r="CH22">
         <v>20</v>
@@ -9435,7 +9435,7 @@
         <v>2.625</v>
       </c>
       <c r="CF28" s="8">
-        <v>2.625</v>
+        <v>9.9999999999988987E-4</v>
       </c>
       <c r="CH28">
         <v>26</v>
@@ -13999,7 +13999,7 @@
         <v>3.15</v>
       </c>
       <c r="CF42" s="8">
-        <v>3.15</v>
+        <v>2.5252731522641625E-2</v>
       </c>
       <c r="CH42">
         <v>40</v>
@@ -14109,61 +14109,61 @@
         <v>0</v>
       </c>
       <c r="I43" s="7">
-        <v>100</v>
+        <v>12.5</v>
       </c>
       <c r="J43" s="7">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="K43" s="7">
-        <v>462.5</v>
+        <v>437.5</v>
       </c>
       <c r="L43" s="7">
-        <v>625</v>
+        <v>650</v>
       </c>
       <c r="M43" s="7">
-        <v>962.5</v>
+        <v>1012.5</v>
       </c>
       <c r="N43" s="7">
-        <v>1112.5</v>
+        <v>1200</v>
       </c>
       <c r="O43" s="7">
-        <v>1262.5</v>
+        <v>1375</v>
       </c>
       <c r="P43" s="7">
-        <v>1412.5</v>
+        <v>1562.5</v>
       </c>
       <c r="Q43" s="7">
-        <v>1550</v>
+        <v>1725</v>
       </c>
       <c r="R43" s="7">
-        <v>1687.5</v>
+        <v>1900</v>
       </c>
       <c r="S43" s="7">
-        <v>1837.5</v>
+        <v>2075</v>
       </c>
       <c r="T43" s="7">
-        <v>1987.5</v>
+        <v>2237.5</v>
       </c>
       <c r="U43" s="7">
-        <v>2125</v>
+        <v>2450</v>
       </c>
       <c r="V43" s="7">
-        <v>2287.5</v>
+        <v>2650</v>
       </c>
       <c r="W43" s="7">
-        <v>2425</v>
+        <v>2862.5</v>
       </c>
       <c r="X43" s="7">
-        <v>2575</v>
+        <v>3062.5</v>
       </c>
       <c r="Y43" s="7">
-        <v>2725</v>
+        <v>3275</v>
       </c>
       <c r="Z43" s="7">
-        <v>2887.5</v>
+        <v>3525</v>
       </c>
       <c r="AA43" s="8">
-        <v>2887.5</v>
+        <v>3775</v>
       </c>
       <c r="AB43" t="s">
         <v>15</v>
@@ -14193,61 +14193,61 @@
         <v>0</v>
       </c>
       <c r="AL43" s="7">
-        <v>140</v>
+        <v>17.5</v>
       </c>
       <c r="AM43" s="7">
-        <v>385</v>
+        <v>315</v>
       </c>
       <c r="AN43" s="7">
-        <v>647.5</v>
+        <v>612.5</v>
       </c>
       <c r="AO43" s="7">
-        <v>875</v>
+        <v>909.99999999999989</v>
       </c>
       <c r="AP43" s="7">
-        <v>1347.5</v>
+        <v>1417.5</v>
       </c>
       <c r="AQ43" s="7">
-        <v>1557.5</v>
+        <v>1680</v>
       </c>
       <c r="AR43" s="7">
-        <v>1767.5</v>
+        <v>1924.9999999999998</v>
       </c>
       <c r="AS43" s="7">
-        <v>1977.4999999999998</v>
+        <v>2187.5</v>
       </c>
       <c r="AT43" s="7">
-        <v>2170</v>
+        <v>2415</v>
       </c>
       <c r="AU43" s="7">
-        <v>2362.5</v>
+        <v>2660</v>
       </c>
       <c r="AV43" s="7">
-        <v>2572.5</v>
+        <v>2905</v>
       </c>
       <c r="AW43" s="7">
-        <v>2782.5</v>
+        <v>3132.5</v>
       </c>
       <c r="AX43" s="7">
-        <v>2975</v>
+        <v>3430</v>
       </c>
       <c r="AY43" s="7">
-        <v>3202.5</v>
+        <v>3709.9999999999995</v>
       </c>
       <c r="AZ43" s="7">
-        <v>3395</v>
+        <v>4007.4999999999995</v>
       </c>
       <c r="BA43" s="7">
-        <v>3604.9999999999995</v>
+        <v>4287.5</v>
       </c>
       <c r="BB43" s="7">
-        <v>3814.9999999999995</v>
+        <v>4585</v>
       </c>
       <c r="BC43" s="7">
-        <v>4042.4999999999995</v>
+        <v>4935</v>
       </c>
       <c r="BD43" s="8">
-        <v>4042.4999999999995</v>
+        <v>5285</v>
       </c>
       <c r="BF43">
         <v>41</v>
@@ -14274,61 +14274,61 @@
         <v>0</v>
       </c>
       <c r="BN43" s="7">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="BO43" s="7">
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="BP43" s="7">
-        <v>925</v>
+        <v>875</v>
       </c>
       <c r="BQ43" s="7">
-        <v>1250</v>
+        <v>1300</v>
       </c>
       <c r="BR43" s="7">
-        <v>1925</v>
+        <v>2025</v>
       </c>
       <c r="BS43" s="7">
-        <v>2225</v>
+        <v>2400</v>
       </c>
       <c r="BT43" s="7">
-        <v>2525</v>
+        <v>2750</v>
       </c>
       <c r="BU43" s="7">
-        <v>2825</v>
+        <v>3125</v>
       </c>
       <c r="BV43" s="7">
-        <v>3100</v>
+        <v>3450</v>
       </c>
       <c r="BW43" s="7">
-        <v>3375</v>
+        <v>3800</v>
       </c>
       <c r="BX43" s="7">
-        <v>3675</v>
+        <v>4150</v>
       </c>
       <c r="BY43" s="7">
-        <v>3975</v>
+        <v>4475</v>
       </c>
       <c r="BZ43" s="7">
-        <v>4250</v>
+        <v>4900</v>
       </c>
       <c r="CA43" s="7">
-        <v>4575</v>
+        <v>5300</v>
       </c>
       <c r="CB43" s="7">
-        <v>4850</v>
+        <v>5725</v>
       </c>
       <c r="CC43" s="7">
-        <v>5150</v>
+        <v>6125</v>
       </c>
       <c r="CD43" s="7">
-        <v>5450</v>
+        <v>6550</v>
       </c>
       <c r="CE43" s="7">
-        <v>5775</v>
+        <v>7050</v>
       </c>
       <c r="CF43" s="8">
-        <v>5775</v>
+        <v>7550</v>
       </c>
       <c r="CH43">
         <v>41</v>
@@ -14355,61 +14355,61 @@
         <v>0</v>
       </c>
       <c r="CP43" s="7">
-        <v>140</v>
+        <v>17.5</v>
       </c>
       <c r="CQ43" s="7">
-        <v>385</v>
+        <v>315</v>
       </c>
       <c r="CR43" s="7">
-        <v>647.5</v>
+        <v>612.5</v>
       </c>
       <c r="CS43" s="7">
-        <v>875</v>
+        <v>909.99999999999989</v>
       </c>
       <c r="CT43" s="7">
-        <v>1347.5</v>
+        <v>1417.5</v>
       </c>
       <c r="CU43" s="7">
-        <v>1557.5</v>
+        <v>1680</v>
       </c>
       <c r="CV43" s="7">
-        <v>1767.5</v>
+        <v>1924.9999999999998</v>
       </c>
       <c r="CW43" s="7">
-        <v>1977.4999999999998</v>
+        <v>2187.5</v>
       </c>
       <c r="CX43" s="7">
-        <v>2170</v>
+        <v>2415</v>
       </c>
       <c r="CY43" s="7">
-        <v>2362.5</v>
+        <v>2660</v>
       </c>
       <c r="CZ43" s="7">
-        <v>2572.5</v>
+        <v>2905</v>
       </c>
       <c r="DA43" s="7">
-        <v>2782.5</v>
+        <v>3132.5</v>
       </c>
       <c r="DB43" s="7">
-        <v>2975</v>
+        <v>3430</v>
       </c>
       <c r="DC43" s="7">
-        <v>3202.5</v>
+        <v>3709.9999999999995</v>
       </c>
       <c r="DD43" s="7">
-        <v>3395</v>
+        <v>4007.4999999999995</v>
       </c>
       <c r="DE43" s="7">
-        <v>3604.9999999999995</v>
+        <v>4287.5</v>
       </c>
       <c r="DF43" s="7">
-        <v>3814.9999999999995</v>
+        <v>4585</v>
       </c>
       <c r="DG43" s="7">
-        <v>4042.4999999999995</v>
+        <v>4935</v>
       </c>
       <c r="DH43" s="8">
-        <v>4042.4999999999995</v>
+        <v>5285</v>
       </c>
     </row>
     <row r="44" spans="1:112" x14ac:dyDescent="0.35">
@@ -16965,13 +16965,13 @@
         <v>0</v>
       </c>
       <c r="CD53" s="7">
-        <v>24.957580622871205</v>
+        <v>0</v>
       </c>
       <c r="CE53" s="7">
         <v>64.099045520309915</v>
       </c>
       <c r="CF53" s="8">
-        <v>103.93379916725485</v>
+        <v>103.93379916725473</v>
       </c>
       <c r="CH53">
         <v>4</v>
@@ -17617,7 +17617,7 @@
         <v>0</v>
       </c>
       <c r="CD55" s="7">
-        <v>0</v>
+        <v>24.957580622871205</v>
       </c>
       <c r="CE55" s="7">
         <v>0</v>
@@ -19668,10 +19668,10 @@
         <v>13</v>
       </c>
       <c r="B62" s="6">
-        <v>0</v>
+        <v>1848</v>
       </c>
       <c r="C62" s="7">
-        <v>0</v>
+        <v>1848</v>
       </c>
       <c r="D62" s="7">
         <v>0</v>
@@ -19749,7 +19749,7 @@
         <v>13</v>
       </c>
       <c r="AE62" s="6">
-        <v>0</v>
+        <v>1848</v>
       </c>
       <c r="AF62" s="7">
         <v>0</v>
@@ -19830,13 +19830,13 @@
         <v>13</v>
       </c>
       <c r="BG62" s="6">
+        <v>1417.7572042342745</v>
+      </c>
+      <c r="BH62" s="7">
         <v>1848</v>
       </c>
-      <c r="BH62" s="7">
-        <v>0</v>
-      </c>
       <c r="BI62" s="7">
-        <v>0</v>
+        <v>1264.2975279152774</v>
       </c>
       <c r="BJ62" s="7">
         <v>0</v>
@@ -19911,10 +19911,10 @@
         <v>13</v>
       </c>
       <c r="CI62" s="6">
-        <v>125.09026451683894</v>
+        <v>1848</v>
       </c>
       <c r="CJ62" s="7">
-        <v>0</v>
+        <v>357.79074150090446</v>
       </c>
       <c r="CK62" s="7">
         <v>0</v>
@@ -28796,10 +28796,10 @@
         <v>41</v>
       </c>
       <c r="B90" s="6">
-        <v>3720.9531502300001</v>
+        <v>1872.9531502300001</v>
       </c>
       <c r="C90" s="7">
-        <v>3779.2483004999995</v>
+        <v>1931.2483004999992</v>
       </c>
       <c r="D90" s="7">
         <v>3838.6202646999996</v>
@@ -28817,7 +28817,7 @@
         <v>4087.247078180947</v>
       </c>
       <c r="I90" s="7">
-        <v>4152.2840038328241</v>
+        <v>4152.2840038328231</v>
       </c>
       <c r="J90" s="7">
         <v>4218.5123537673817</v>
@@ -28835,7 +28835,7 @@
         <v>4495.7502792986852</v>
       </c>
       <c r="O90" s="7">
-        <v>4568.2465378457628</v>
+        <v>4568.2465378457618</v>
       </c>
       <c r="P90" s="7">
         <v>4642.0610292381407</v>
@@ -28853,7 +28853,7 @@
         <v>4950.9552769364072</v>
       </c>
       <c r="U90" s="7">
-        <v>5031.7048001263265</v>
+        <v>5031.7048001263256</v>
       </c>
       <c r="V90" s="7">
         <v>5101.8911809343444</v>
@@ -28880,7 +28880,7 @@
         <v>41</v>
       </c>
       <c r="AE90" s="6">
-        <v>4044.9531502299992</v>
+        <v>2196.9531502299997</v>
       </c>
       <c r="AF90" s="7">
         <v>4108.7563004999993</v>
@@ -28892,10 +28892,10 @@
         <v>4239.8938485499984</v>
       </c>
       <c r="AI90" s="7">
-        <v>4307.2683799600482</v>
+        <v>4307.2683799600472</v>
       </c>
       <c r="AJ90" s="7">
-        <v>4375.8740749506687</v>
+        <v>4375.8740749506696</v>
       </c>
       <c r="AK90" s="7">
         <v>4445.7318631010303</v>
@@ -28904,7 +28904,7 @@
         <v>4516.8630300965469</v>
       </c>
       <c r="AM90" s="7">
-        <v>4589.2892234775873</v>
+        <v>4589.2892234775863</v>
       </c>
       <c r="AN90" s="7">
         <v>4663.0324584910059</v>
@@ -28916,7 +28916,7 @@
         <v>4814.5599932778377</v>
       </c>
       <c r="AQ90" s="7">
-        <v>4892.3902207159608</v>
+        <v>4892.3902207159617</v>
       </c>
       <c r="AR90" s="7">
         <v>4971.6293582671333</v>
@@ -28925,10 +28925,10 @@
         <v>5052.3013576066742</v>
       </c>
       <c r="AT90" s="7">
-        <v>5115.7406404098656</v>
+        <v>5115.7406404098665</v>
       </c>
       <c r="AU90" s="7">
-        <v>5172.178209160933</v>
+        <v>5172.1782091609321</v>
       </c>
       <c r="AV90" s="7">
         <v>5229.633129184519</v>
@@ -28946,7 +28946,7 @@
         <v>5469.9766624039148</v>
       </c>
       <c r="BA90" s="7">
-        <v>5532.7837191399067</v>
+        <v>5532.7837191399058</v>
       </c>
       <c r="BB90" s="7">
         <v>5596.7164091191589</v>
@@ -28961,28 +28961,28 @@
         <v>41</v>
       </c>
       <c r="BG90" s="6">
-        <v>3155.9531502299992</v>
+        <v>3586.1959459957252</v>
       </c>
       <c r="BH90" s="7">
-        <v>5081.7400278374989</v>
+        <v>3233.7400278374994</v>
       </c>
       <c r="BI90" s="7">
-        <v>5136.788809897499</v>
+        <v>3872.4912819822216</v>
       </c>
       <c r="BJ90" s="7">
-        <v>5192.8313338539729</v>
+        <v>5192.8313338539738</v>
       </c>
       <c r="BK90" s="7">
         <v>5249.8844933191631</v>
       </c>
       <c r="BL90" s="7">
-        <v>5307.9654691642163</v>
+        <v>5307.9654691642154</v>
       </c>
       <c r="BM90" s="7">
-        <v>5367.0917341314434</v>
+        <v>5367.0917341314425</v>
       </c>
       <c r="BN90" s="7">
-        <v>5427.2810582045668</v>
+        <v>5427.2810582045677</v>
       </c>
       <c r="BO90" s="7">
         <v>5488.5515134558891</v>
@@ -29027,7 +29027,7 @@
         <v>6392.2558139807634</v>
       </c>
       <c r="CC90" s="7">
-        <v>6470.7416162935606</v>
+        <v>6470.7416162935597</v>
       </c>
       <c r="CD90" s="7">
         <v>6550.6195905244258</v>
@@ -29042,10 +29042,10 @@
         <v>41</v>
       </c>
       <c r="CI90" s="6">
-        <v>3649.8628857131607</v>
+        <v>1926.9531502299997</v>
       </c>
       <c r="CJ90" s="7">
-        <v>3834.1663005</v>
+        <v>3476.3755589990956</v>
       </c>
       <c r="CK90" s="7">
         <v>3894.4718706999988</v>
@@ -29054,16 +29054,16 @@
         <v>3955.8884320399993</v>
       </c>
       <c r="CM90" s="7">
-        <v>4018.4348713693789</v>
+        <v>4018.4348713693785</v>
       </c>
       <c r="CN90" s="7">
-        <v>4082.1303967139584</v>
+        <v>4082.1303967139575</v>
       </c>
       <c r="CO90" s="7">
-        <v>4146.9945423342942</v>
+        <v>4146.9945423342951</v>
       </c>
       <c r="CP90" s="7">
-        <v>4213.0471748767777</v>
+        <v>4213.0471748767768</v>
       </c>
       <c r="CQ90" s="7">
         <v>4280.3084987190823</v>
@@ -29078,13 +29078,13 @@
         <v>4489.5518472459835</v>
       </c>
       <c r="CU90" s="7">
-        <v>4561.8569362015651</v>
+        <v>4561.8569362015642</v>
       </c>
       <c r="CV90" s="7">
         <v>4635.4770079159916</v>
       </c>
       <c r="CW90" s="7">
-        <v>4710.4344172995634</v>
+        <v>4710.4344172995625</v>
       </c>
       <c r="CX90" s="7">
         <v>4786.751900092655</v>
@@ -29096,7 +29096,7 @@
         <v>4943.559958892175</v>
       </c>
       <c r="DA90" s="7">
-        <v>5024.0979642253405</v>
+        <v>5024.0979642253396</v>
       </c>
       <c r="DB90" s="7">
         <v>5096.611366341941</v>
@@ -30140,55 +30140,55 @@
         <v>1</v>
       </c>
       <c r="B97" s="3">
-        <v>-124.17838247316669</v>
+        <v>-124.17838247316668</v>
       </c>
       <c r="C97" s="4">
-        <v>-88.241148274999986</v>
+        <v>-116.44114827500007</v>
       </c>
       <c r="D97" s="4">
-        <v>121.55387253287903</v>
+        <v>-108.56203818500012</v>
       </c>
       <c r="E97" s="4">
-        <v>3.5270206952999104</v>
+        <v>205.38108893494115</v>
       </c>
       <c r="F97" s="4">
-        <v>111.69647549533488</v>
+        <v>328.36280882866822</v>
       </c>
       <c r="G97" s="4">
-        <v>336.25110555529136</v>
+        <v>266.44385769285651</v>
       </c>
       <c r="H97" s="4">
-        <v>1014.6499034305731</v>
+        <v>384.77829418459146</v>
       </c>
       <c r="I97" s="4">
-        <v>927.94031499321954</v>
+        <v>957.10698165988629</v>
       </c>
       <c r="J97" s="4">
-        <v>878.38700081620084</v>
+        <v>895.05366748286747</v>
       </c>
       <c r="K97" s="4">
-        <v>824.82628987174451</v>
+        <v>833.15962320507776</v>
       </c>
       <c r="L97" s="4">
-        <v>779.76088976000256</v>
+        <v>771.42755642666918</v>
       </c>
       <c r="M97" s="4">
-        <v>362.24935900126059</v>
+        <v>362.2493590012607</v>
       </c>
       <c r="N97" s="4">
         <v>350.12053572142213</v>
       </c>
       <c r="O97" s="4">
-        <v>337.77265300883641</v>
+        <v>396.2478196090558</v>
       </c>
       <c r="P97" s="4">
-        <v>325.20198682263685</v>
+        <v>325.20198682263674</v>
       </c>
       <c r="Q97" s="4">
-        <v>346.61205147187911</v>
+        <v>312.40474969377146</v>
       </c>
       <c r="R97" s="4">
-        <v>346.67385253821703</v>
+        <v>299.3770902187656</v>
       </c>
       <c r="S97" s="4">
         <v>286.11509106518463</v>
@@ -30200,70 +30200,70 @@
         <v>258.87207074998753</v>
       </c>
       <c r="V97" s="4">
-        <v>209.35686781037521</v>
+        <v>240.58250861466922</v>
       </c>
       <c r="W97" s="4">
-        <v>188.64958279421035</v>
+        <v>192.05405615098277</v>
       </c>
       <c r="X97" s="4">
-        <v>168.76916844904054</v>
+        <v>120.16762800135587</v>
       </c>
       <c r="Y97" s="4">
-        <v>154.89406550382273</v>
+        <v>38.507807493628604</v>
       </c>
       <c r="Z97" s="4">
-        <v>139.87626866268783</v>
+        <v>-61.462531104479694</v>
       </c>
       <c r="AA97" s="5">
-        <v>171.09029980775358</v>
+        <v>-160.98591634625609</v>
       </c>
       <c r="AD97" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AE97" s="3">
-        <v>33.960167603499826</v>
+        <v>33.960167603500054</v>
       </c>
       <c r="AF97" s="4">
         <v>68.14133522499958</v>
       </c>
       <c r="AG97" s="4">
-        <v>281.64667916499997</v>
+        <v>102.94219106499918</v>
       </c>
       <c r="AH97" s="4">
-        <v>74.165847740249745</v>
+        <v>138.37326985491586</v>
       </c>
       <c r="AI97" s="4">
-        <v>338.18451843338221</v>
+        <v>298.90584056965577</v>
       </c>
       <c r="AJ97" s="4">
-        <v>970.90856529092127</v>
+        <v>193.03884945873477</v>
       </c>
       <c r="AK97" s="4">
-        <v>1088.8983803517565</v>
+        <v>472.8983803517566</v>
       </c>
       <c r="AL97" s="4">
-        <v>990.09936618872973</v>
+        <v>1085.3135195022639</v>
       </c>
       <c r="AM97" s="4">
-        <v>918.47811171536807</v>
+        <v>941.81144504870144</v>
       </c>
       <c r="AN97" s="4">
-        <v>841.20430548953084</v>
+        <v>854.14066916284901</v>
       </c>
       <c r="AO97" s="4">
-        <v>775.78102080995779</v>
+        <v>764.11435414329117</v>
       </c>
       <c r="AP97" s="4">
         <v>275.25429300122607</v>
       </c>
       <c r="AQ97" s="4">
-        <v>281.35479603244789</v>
+        <v>261.38505109938706</v>
       </c>
       <c r="AR97" s="4">
-        <v>260.96229049188275</v>
+        <v>247.26716264822664</v>
       </c>
       <c r="AS97" s="4">
-        <v>232.89640062589649</v>
+        <v>232.89640062589626</v>
       </c>
       <c r="AT97" s="4">
         <v>218.2684660316869</v>
@@ -30275,28 +30275,28 @@
         <v>188.22351783011106</v>
       </c>
       <c r="AW97" s="4">
-        <v>126.29753597842284</v>
+        <v>175.56663868344884</v>
       </c>
       <c r="AX97" s="4">
-        <v>114.86310233223611</v>
+        <v>54.369678637073548</v>
       </c>
       <c r="AY97" s="4">
-        <v>94.615561758408262</v>
+        <v>-58.995519597346629</v>
       </c>
       <c r="AZ97" s="4">
-        <v>78.350136253551113</v>
+        <v>-180.63647708925134</v>
       </c>
       <c r="BA97" s="4">
-        <v>48.204868253980749</v>
+        <v>-293.04513174601948</v>
       </c>
       <c r="BB97" s="4">
-        <v>-28.713284169451072</v>
+        <v>-412.44573705314212</v>
       </c>
       <c r="BC97" s="4">
-        <v>-113.88259632583231</v>
+        <v>-439.2426151438346</v>
       </c>
       <c r="BD97" s="5">
-        <v>-84.794587676371521</v>
+        <v>-781.40417448413541</v>
       </c>
       <c r="BF97" s="1" t="s">
         <v>1</v>
@@ -30305,22 +30305,22 @@
         <v>540.94806745016672</v>
       </c>
       <c r="BH97" s="4">
-        <v>520.03731822500049</v>
+        <v>520.03731822500026</v>
       </c>
       <c r="BI97" s="4">
-        <v>232.31378818166618</v>
+        <v>498.75249704833379</v>
       </c>
       <c r="BJ97" s="4">
-        <v>277.31085078956613</v>
+        <v>277.31085078956608</v>
       </c>
       <c r="BK97" s="4">
-        <v>334.40694949528597</v>
+        <v>345.70176046113562</v>
       </c>
       <c r="BL97" s="4">
-        <v>608.80629832454724</v>
+        <v>485.95173943550174</v>
       </c>
       <c r="BM97" s="4">
-        <v>863.07700885788893</v>
+        <v>628.96096958934186</v>
       </c>
       <c r="BN97" s="4">
         <v>839.82424960519995</v>
@@ -30329,136 +30329,136 @@
         <v>816.15760419345179</v>
       </c>
       <c r="BP97" s="4">
-        <v>792.07003660164196</v>
+        <v>792.07003660164219</v>
       </c>
       <c r="BQ97" s="4">
-        <v>767.55439113067519</v>
+        <v>767.5543911306753</v>
       </c>
       <c r="BR97" s="4">
-        <v>56.957154916496052</v>
+        <v>78.149301491079768</v>
       </c>
       <c r="BS97" s="4">
         <v>39.376861667216303</v>
       </c>
       <c r="BT97" s="4">
-        <v>21.484833995709437</v>
+        <v>21.484833995709323</v>
       </c>
       <c r="BU97" s="4">
         <v>3.275772386286576</v>
       </c>
       <c r="BV97" s="4">
-        <v>-15.255712887996538</v>
+        <v>-15.255712887996651</v>
       </c>
       <c r="BW97" s="4">
-        <v>-34.115102726892474</v>
+        <v>-34.115102726892246</v>
       </c>
       <c r="BX97" s="4">
-        <v>-53.30797166054947</v>
+        <v>-67.916727227647698</v>
       </c>
       <c r="BY97" s="4">
-        <v>-92.849472847170091</v>
+        <v>-84.90293527736867</v>
       </c>
       <c r="BZ97" s="4">
-        <v>-92.716919916049505</v>
+        <v>-264.27471680658391</v>
       </c>
       <c r="CA97" s="4">
-        <v>-159.44462814187318</v>
+        <v>-430.56186976354638</v>
       </c>
       <c r="CB97" s="4">
-        <v>-180.02907687503364</v>
+        <v>-608.7544552082768</v>
       </c>
       <c r="CC97" s="4">
-        <v>-286.3423654930682</v>
+        <v>-773.84236549306797</v>
       </c>
       <c r="CD97" s="4">
-        <v>-400.81532089020016</v>
+        <v>-950.81532089020016</v>
       </c>
       <c r="CE97" s="4">
-        <v>-527.16286767083443</v>
+        <v>-1000</v>
       </c>
       <c r="CF97" s="5">
-        <v>-609.30412691206607</v>
+        <v>-1100</v>
       </c>
       <c r="CH97" s="1" t="s">
         <v>1</v>
       </c>
       <c r="CI97" s="3">
-        <v>-104.33721580650004</v>
+        <v>-104.33721580650007</v>
       </c>
       <c r="CJ97" s="4">
-        <v>-73.290121900019187</v>
+        <v>-96.280998275000059</v>
       </c>
       <c r="CK97" s="4">
-        <v>232.65585686499998</v>
+        <v>-86.022409235000623</v>
       </c>
       <c r="CL97" s="4">
-        <v>75.465172005347881</v>
+        <v>19.142181461149818</v>
       </c>
       <c r="CM97" s="4">
-        <v>229.72379259059954</v>
+        <v>349.5135164942044</v>
       </c>
       <c r="CN97" s="4">
-        <v>311.6734461532576</v>
+        <v>141.5071128199242</v>
       </c>
       <c r="CO97" s="4">
-        <v>585.22447500660337</v>
+        <v>405.06759229942622</v>
       </c>
       <c r="CP97" s="4">
-        <v>952.87440250857844</v>
+        <v>977.63364640264433</v>
       </c>
       <c r="CQ97" s="4">
-        <v>864.27297469291909</v>
+        <v>898.09736590243301</v>
       </c>
       <c r="CR97" s="4">
-        <v>834.18778465487651</v>
+        <v>797.74434780436707</v>
       </c>
       <c r="CS97" s="4">
-        <v>734.3752502578219</v>
+        <v>731.95158091304074</v>
       </c>
       <c r="CT97" s="4">
-        <v>362.84921086722557</v>
+        <v>407.27660191264329</v>
       </c>
       <c r="CU97" s="4">
-        <v>371.49875249101933</v>
+        <v>341.19993036896267</v>
       </c>
       <c r="CV97" s="4">
-        <v>341.0727979866615</v>
+        <v>323.08819278298381</v>
       </c>
       <c r="CW97" s="4">
         <v>310.00638827294483</v>
       </c>
       <c r="CX97" s="4">
-        <v>296.68932346873498</v>
+        <v>296.6893234687351</v>
       </c>
       <c r="CY97" s="4">
-        <v>304.91085727013638</v>
+        <v>229.30875125349428</v>
       </c>
       <c r="CZ97" s="4">
-        <v>269.33334804781805</v>
+        <v>129.8081699203035</v>
       </c>
       <c r="DA97" s="4">
-        <v>214.47002781694846</v>
+        <v>39.470027816948573</v>
       </c>
       <c r="DB97" s="4">
-        <v>142.05133666033657</v>
+        <v>-97.164844011393598</v>
       </c>
       <c r="DC97" s="4">
-        <v>52.559226612311988</v>
+        <v>-217.46524639733713</v>
       </c>
       <c r="DD97" s="4">
-        <v>-18.999050194028769</v>
+        <v>-238.8647398318418</v>
       </c>
       <c r="DE97" s="4">
-        <v>-98.866118593577085</v>
+        <v>-260.64661388556647</v>
       </c>
       <c r="DF97" s="4">
-        <v>-178.28447779341809</v>
+        <v>-282.8173692457043</v>
       </c>
       <c r="DG97" s="4">
-        <v>-279.23428376786501</v>
+        <v>-440.90095043453198</v>
       </c>
       <c r="DH97" s="5">
-        <v>-239.49442795851019</v>
+        <v>-772.08541243595755</v>
       </c>
     </row>
     <row r="98" spans="1:112" x14ac:dyDescent="0.35">
@@ -30469,52 +30469,52 @@
         <v>-342.12995758816652</v>
       </c>
       <c r="C98" s="7">
-        <v>-339.35229852499987</v>
+        <v>-367.5522985249998</v>
       </c>
       <c r="D98" s="7">
-        <v>-163.32346381712046</v>
+        <v>-393.43937453499962</v>
       </c>
       <c r="E98" s="7">
-        <v>334.26657485830049</v>
+        <v>-113.87935690205813</v>
       </c>
       <c r="F98" s="7">
-        <v>407.42550908675685</v>
+        <v>-25.908157579909773</v>
       </c>
       <c r="G98" s="7">
-        <v>458.1206696584652</v>
+        <v>526.52429358968266</v>
       </c>
       <c r="H98" s="7">
-        <v>-609.56618270045431</v>
+        <v>608.56120805356397</v>
       </c>
       <c r="I98" s="7">
-        <v>-447.23424926343534</v>
+        <v>-505.56758259676872</v>
       </c>
       <c r="J98" s="7">
-        <v>-359.41621696751696</v>
+        <v>-392.74955030085027</v>
       </c>
       <c r="K98" s="7">
-        <v>-263.78816672144615</v>
+        <v>-280.4548333881126</v>
       </c>
       <c r="L98" s="7">
-        <v>-185.3589949257223</v>
+        <v>-168.6923282590557</v>
       </c>
       <c r="M98" s="7">
-        <v>637.75064099873941</v>
+        <v>637.7506409987393</v>
       </c>
       <c r="N98" s="7">
         <v>649.87946427857787</v>
       </c>
       <c r="O98" s="7">
-        <v>662.22734699116359</v>
+        <v>545.27701379072482</v>
       </c>
       <c r="P98" s="7">
-        <v>674.79801317736303</v>
+        <v>674.79801317736337</v>
       </c>
       <c r="Q98" s="7">
-        <v>619.18064675001324</v>
+        <v>687.59525030622854</v>
       </c>
       <c r="R98" s="7">
-        <v>606.02938514233165</v>
+        <v>700.6229097812344</v>
       </c>
       <c r="S98" s="7">
         <v>713.88490893481526</v>
@@ -30526,70 +30526,70 @@
         <v>741.12792925001247</v>
       </c>
       <c r="V98" s="7">
-        <v>790.64313218962479</v>
+        <v>759.41749138533078</v>
       </c>
       <c r="W98" s="7">
-        <v>811.35041720578965</v>
+        <v>800.03488693248528</v>
       </c>
       <c r="X98" s="7">
-        <v>831.23083155095946</v>
+        <v>879.83237199864413</v>
       </c>
       <c r="Y98" s="7">
-        <v>845.10593449617727</v>
+        <v>961.49219250637134</v>
       </c>
       <c r="Z98" s="7">
-        <v>860.12373133731217</v>
+        <v>1061.4625311044797</v>
       </c>
       <c r="AA98" s="8">
-        <v>828.90970019224642</v>
+        <v>1160.9859163462561</v>
       </c>
       <c r="AD98" t="s">
         <v>2</v>
       </c>
       <c r="AE98" s="6">
-        <v>-455.28140751149999</v>
+        <v>-455.28140751150011</v>
       </c>
       <c r="AF98" s="7">
         <v>-459.07931502499991</v>
       </c>
       <c r="AG98" s="7">
-        <v>-284.2415886849995</v>
+        <v>-462.94607678499995</v>
       </c>
       <c r="AH98" s="7">
-        <v>118.9097145677509</v>
+        <v>-466.88286331758331</v>
       </c>
       <c r="AI98" s="7">
-        <v>342.8483680046013</v>
+        <v>-42.594276267945816</v>
       </c>
       <c r="AJ98" s="7">
-        <v>-888.34100845735861</v>
+        <v>156.89842320701433</v>
       </c>
       <c r="AK98" s="7">
-        <v>-836.7828925843429</v>
+        <v>395.21710741565698</v>
       </c>
       <c r="AL98" s="7">
-        <v>-651.87184604868321</v>
+        <v>-842.30015267575163</v>
       </c>
       <c r="AM98" s="7">
-        <v>-521.54486706478042</v>
+        <v>-568.21153373144728</v>
       </c>
       <c r="AN98" s="7">
-        <v>-380.14521803703002</v>
+        <v>-406.0179453836663</v>
       </c>
       <c r="AO98" s="7">
-        <v>-262.68299694700437</v>
+        <v>-239.34966361367105</v>
       </c>
       <c r="AP98" s="7">
         <v>724.74570699877393</v>
       </c>
       <c r="AQ98" s="7">
-        <v>698.67545903449138</v>
+        <v>738.61494890061294</v>
       </c>
       <c r="AR98" s="7">
-        <v>725.34258166446102</v>
+        <v>752.73283735177324</v>
       </c>
       <c r="AS98" s="7">
-        <v>767.1035993741034</v>
+        <v>767.10359937410374</v>
       </c>
       <c r="AT98" s="7">
         <v>781.7315339683131</v>
@@ -30601,109 +30601,109 @@
         <v>811.77648216988905</v>
       </c>
       <c r="AW98" s="7">
-        <v>873.70246402157716</v>
+        <v>821.66425861152493</v>
       </c>
       <c r="AX98" s="7">
-        <v>885.13689766776383</v>
+        <v>945.63032136292645</v>
       </c>
       <c r="AY98" s="7">
-        <v>905.38443824159174</v>
+        <v>1058.9955195973466</v>
       </c>
       <c r="AZ98" s="7">
-        <v>921.64986374644877</v>
+        <v>1180.6364770892515</v>
       </c>
       <c r="BA98" s="7">
-        <v>951.79513174601925</v>
+        <v>1293.0451317460195</v>
       </c>
       <c r="BB98" s="7">
-        <v>1028.7132841694511</v>
+        <v>1405.8376946079552</v>
       </c>
       <c r="BC98" s="7">
-        <v>1113.8825963258323</v>
+        <v>1439.2426151438344</v>
       </c>
       <c r="BD98" s="8">
-        <v>1084.7945876763715</v>
+        <v>1630.6850008686076</v>
       </c>
       <c r="BF98" t="s">
         <v>2</v>
       </c>
       <c r="BG98" s="6">
-        <v>-497.20035743483334</v>
+        <v>-497.20035743483345</v>
       </c>
       <c r="BH98" s="7">
-        <v>-469.85553152500052</v>
+        <v>-469.8555315250004</v>
       </c>
       <c r="BI98" s="7">
-        <v>-308.80218016833334</v>
+        <v>-442.02153460166721</v>
       </c>
       <c r="BJ98" s="7">
         <v>-313.8018537914333</v>
       </c>
       <c r="BK98" s="7">
-        <v>-307.5953340559397</v>
+        <v>-330.18595598763886</v>
       </c>
       <c r="BL98" s="7">
-        <v>-361.43431174026807</v>
+        <v>-207.84814420174496</v>
       </c>
       <c r="BM98" s="7">
-        <v>-585.79205004493156</v>
+        <v>-117.55997150783753</v>
       </c>
       <c r="BN98" s="7">
-        <v>-555.38459563756919</v>
+        <v>-555.3845956375693</v>
       </c>
       <c r="BO98" s="7">
         <v>-524.43590548374459</v>
       </c>
       <c r="BP98" s="7">
-        <v>-492.93677863291634</v>
+        <v>-492.93677863291674</v>
       </c>
       <c r="BQ98" s="7">
-        <v>-460.8778576324213</v>
+        <v>-460.87785763242141</v>
       </c>
       <c r="BR98" s="7">
-        <v>943.04284508350395</v>
+        <v>900.65855193433663</v>
       </c>
       <c r="BS98" s="7">
         <v>960.6231383327837</v>
       </c>
       <c r="BT98" s="7">
-        <v>978.51516600429045</v>
+        <v>978.51516600429068</v>
       </c>
       <c r="BU98" s="7">
         <v>996.72422761371331</v>
       </c>
       <c r="BV98" s="7">
-        <v>1015.2557128879965</v>
+        <v>1015.2557128879967</v>
       </c>
       <c r="BW98" s="7">
-        <v>1034.1151027268925</v>
+        <v>1034.1151027268922</v>
       </c>
       <c r="BX98" s="7">
-        <v>1053.3079716605496</v>
+        <v>1067.9167272276477</v>
       </c>
       <c r="BY98" s="7">
-        <v>1092.8494728471701</v>
+        <v>1084.9029352773687</v>
       </c>
       <c r="BZ98" s="7">
-        <v>1092.7169199160496</v>
+        <v>1264.2747168065839</v>
       </c>
       <c r="CA98" s="7">
-        <v>1159.4446281418732</v>
+        <v>1430.5618697635464</v>
       </c>
       <c r="CB98" s="7">
-        <v>1180.0290768750338</v>
+        <v>1608.7544552082768</v>
       </c>
       <c r="CC98" s="7">
-        <v>1286.3423654930682</v>
+        <v>1773.842365493068</v>
       </c>
       <c r="CD98" s="7">
-        <v>1400.8153208902002</v>
+        <v>1950.8153208902002</v>
       </c>
       <c r="CE98" s="7">
-        <v>1527.1628676708344</v>
+        <v>2000</v>
       </c>
       <c r="CF98" s="8">
-        <v>1609.3041269120661</v>
+        <v>2000</v>
       </c>
       <c r="CH98" t="s">
         <v>2</v>
@@ -30712,43 +30712,43 @@
         <v>-390.57879092149989</v>
       </c>
       <c r="CJ98" s="7">
-        <v>-394.05977215001866</v>
+        <v>-417.05064852499976</v>
       </c>
       <c r="CK98" s="7">
-        <v>-123.27174398499963</v>
+        <v>-441.95001008499992</v>
       </c>
       <c r="CL98" s="7">
-        <v>180.37006553925448</v>
+        <v>-372.58395337234947</v>
       </c>
       <c r="CM98" s="7">
-        <v>451.54765047258098</v>
+        <v>-78.661625623814302</v>
       </c>
       <c r="CN98" s="7">
-        <v>496.38474835358244</v>
+        <v>326.21841502024915</v>
       </c>
       <c r="CO98" s="7">
-        <v>237.94678045668252</v>
+        <v>551.99252719905667</v>
       </c>
       <c r="CP98" s="7">
-        <v>-508.89456467769924</v>
+        <v>-558.4130524658309</v>
       </c>
       <c r="CQ98" s="7">
-        <v>-343.44227399101999</v>
+        <v>-411.09105641004771</v>
       </c>
       <c r="CR98" s="7">
-        <v>-295.23508791536779</v>
+        <v>-222.34821421434879</v>
       </c>
       <c r="CS98" s="7">
-        <v>-107.78945688668887</v>
+        <v>-102.94211819712655</v>
       </c>
       <c r="CT98" s="7">
-        <v>622.86326420507112</v>
+        <v>534.00848211423568</v>
       </c>
       <c r="CU98" s="7">
-        <v>592.94116473559552</v>
+        <v>653.53880897970885</v>
       </c>
       <c r="CV98" s="7">
-        <v>640.94259680966115</v>
+        <v>676.91180721701608</v>
       </c>
       <c r="CW98" s="7">
         <v>689.99361172705517</v>
@@ -30757,34 +30757,34 @@
         <v>703.31067653126502</v>
       </c>
       <c r="CY98" s="7">
-        <v>673.31128470763088</v>
+        <v>770.69124874650572</v>
       </c>
       <c r="CZ98" s="7">
-        <v>730.66665195218195</v>
+        <v>870.1918300796965</v>
       </c>
       <c r="DA98" s="7">
-        <v>785.52997218305154</v>
+        <v>960.52997218305143</v>
       </c>
       <c r="DB98" s="7">
-        <v>857.94866333966343</v>
+        <v>1073.7324826679328</v>
       </c>
       <c r="DC98" s="7">
-        <v>947.44077338768807</v>
+        <v>1150.8632068272871</v>
       </c>
       <c r="DD98" s="7">
-        <v>1018.9990501940288</v>
+        <v>1178.847159780101</v>
       </c>
       <c r="DE98" s="7">
-        <v>1098.8661185935771</v>
+        <v>1207.3311489272794</v>
       </c>
       <c r="DF98" s="7">
-        <v>1178.2844777934181</v>
+        <v>1236.3236751674594</v>
       </c>
       <c r="DG98" s="7">
-        <v>1252.7587167149479</v>
+        <v>1333.5920500482814</v>
       </c>
       <c r="DH98" s="8">
-        <v>1239.4944279585102</v>
+        <v>1517.7357316470216</v>
       </c>
     </row>
     <row r="99" spans="1:112" x14ac:dyDescent="0.35">
@@ -30795,34 +30795,34 @@
         <v>466.30834006133318</v>
       </c>
       <c r="C99" s="10">
-        <v>427.59344679999987</v>
+        <v>483.9934467999999</v>
       </c>
       <c r="D99" s="10">
-        <v>41.769591284241429</v>
+        <v>502.00141271999973</v>
       </c>
       <c r="E99" s="10">
-        <v>-337.79359555360043</v>
+        <v>-91.501732032883012</v>
       </c>
       <c r="F99" s="10">
-        <v>-519.12198458209173</v>
+        <v>-302.45465124875841</v>
       </c>
       <c r="G99" s="10">
-        <v>-794.37177521375656</v>
+        <v>-792.96815128253911</v>
       </c>
       <c r="H99" s="10">
-        <v>-405.08372073011861</v>
+        <v>-993.33950223815532</v>
       </c>
       <c r="I99" s="10">
-        <v>-480.70606572978409</v>
+        <v>-451.53939906311734</v>
       </c>
       <c r="J99" s="10">
-        <v>-518.97078384868394</v>
+        <v>-502.30411718201731</v>
       </c>
       <c r="K99" s="10">
-        <v>-561.03812315029836</v>
+        <v>-552.70478981696499</v>
       </c>
       <c r="L99" s="10">
-        <v>-594.40189483428003</v>
+        <v>-602.7352281676134</v>
       </c>
       <c r="M99" s="10">
         <v>-1000</v>
@@ -30831,16 +30831,16 @@
         <v>-1000</v>
       </c>
       <c r="O99" s="10">
-        <v>-1000</v>
+        <v>-941.52483339978062</v>
       </c>
       <c r="P99" s="10">
         <v>-1000</v>
       </c>
       <c r="Q99" s="10">
-        <v>-965.79269822189235</v>
+        <v>-1000</v>
       </c>
       <c r="R99" s="10">
-        <v>-952.70323768054868</v>
+        <v>-1000</v>
       </c>
       <c r="S99" s="10">
         <v>-1000</v>
@@ -30855,7 +30855,7 @@
         <v>-1000</v>
       </c>
       <c r="W99" s="10">
-        <v>-1000</v>
+        <v>-992.08894308346805</v>
       </c>
       <c r="X99" s="10">
         <v>-1000</v>
@@ -30879,40 +30879,40 @@
         <v>390.93797980000028</v>
       </c>
       <c r="AG99" s="10">
-        <v>2.5949095199995704</v>
+        <v>360.00388572000077</v>
       </c>
       <c r="AH99" s="10">
-        <v>-193.07556230800063</v>
+        <v>328.50959346266745</v>
       </c>
       <c r="AI99" s="10">
-        <v>-681.03288643798351</v>
+        <v>-256.31156430170995</v>
       </c>
       <c r="AJ99" s="10">
-        <v>-82.567556833562605</v>
+        <v>-349.93727266574911</v>
       </c>
       <c r="AK99" s="10">
-        <v>-252.1154877674137</v>
+        <v>-868.11548776741358</v>
       </c>
       <c r="AL99" s="10">
-        <v>-338.22752014004652</v>
+        <v>-243.01336682651231</v>
       </c>
       <c r="AM99" s="10">
-        <v>-396.93324465058765</v>
+        <v>-373.59991131725428</v>
       </c>
       <c r="AN99" s="10">
-        <v>-461.05908745250088</v>
+        <v>-448.12272377918271</v>
       </c>
       <c r="AO99" s="10">
-        <v>-513.09802386295348</v>
+        <v>-524.76469052962011</v>
       </c>
       <c r="AP99" s="10">
         <v>-1000</v>
       </c>
       <c r="AQ99" s="10">
-        <v>-980.03025506693916</v>
+        <v>-1000</v>
       </c>
       <c r="AR99" s="10">
-        <v>-986.30487215634378</v>
+        <v>-1000</v>
       </c>
       <c r="AS99" s="10">
         <v>-1000</v>
@@ -30927,7 +30927,7 @@
         <v>-1000</v>
       </c>
       <c r="AW99" s="10">
-        <v>-1000</v>
+        <v>-997.23089729497372</v>
       </c>
       <c r="AX99" s="10">
         <v>-1000</v>
@@ -30942,13 +30942,13 @@
         <v>-1000</v>
       </c>
       <c r="BB99" s="10">
-        <v>-1000</v>
+        <v>-993.39195755481296</v>
       </c>
       <c r="BC99" s="10">
         <v>-1000</v>
       </c>
       <c r="BD99" s="11">
-        <v>-1000</v>
+        <v>-849.28082638447233</v>
       </c>
       <c r="BF99" t="s">
         <v>3</v>
@@ -30957,37 +30957,37 @@
         <v>-43.747710015333382</v>
       </c>
       <c r="BH99" s="10">
-        <v>-50.18178669999989</v>
+        <v>-50.181786700000032</v>
       </c>
       <c r="BI99" s="10">
-        <v>76.488391986667182</v>
+        <v>-56.730962446666553</v>
       </c>
       <c r="BJ99" s="10">
-        <v>36.491003001867128</v>
+        <v>36.491003001867227</v>
       </c>
       <c r="BK99" s="10">
-        <v>-26.811615439346269</v>
+        <v>-15.515804473496758</v>
       </c>
       <c r="BL99" s="10">
-        <v>-247.37198658427917</v>
+        <v>-278.10359523375678</v>
       </c>
       <c r="BM99" s="10">
-        <v>-277.28495881295737</v>
+        <v>-511.40099808150444</v>
       </c>
       <c r="BN99" s="10">
-        <v>-284.4396539676307</v>
+        <v>-284.43965396763065</v>
       </c>
       <c r="BO99" s="10">
         <v>-291.7216987097072</v>
       </c>
       <c r="BP99" s="10">
-        <v>-299.13325796872567</v>
+        <v>-299.1332579687255</v>
       </c>
       <c r="BQ99" s="10">
-        <v>-306.67653349825395</v>
+        <v>-306.67653349825389</v>
       </c>
       <c r="BR99" s="10">
-        <v>-1000</v>
+        <v>-978.8078534254164</v>
       </c>
       <c r="BS99" s="10">
         <v>-1000</v>
@@ -31029,7 +31029,7 @@
         <v>-1000</v>
       </c>
       <c r="CF99" s="11">
-        <v>-1000</v>
+        <v>-900</v>
       </c>
       <c r="CH99" t="s">
         <v>3</v>
@@ -31038,43 +31038,43 @@
         <v>494.91600672799996</v>
       </c>
       <c r="CJ99" s="10">
-        <v>467.34989405003785</v>
+        <v>513.33164679999982</v>
       </c>
       <c r="CK99" s="10">
-        <v>-109.38411288000037</v>
+        <v>527.97241932000054</v>
       </c>
       <c r="CL99" s="10">
-        <v>-255.83523754460236</v>
+        <v>353.44177191119962</v>
       </c>
       <c r="CM99" s="10">
-        <v>-681.27144306318053</v>
+        <v>-270.85189087039009</v>
       </c>
       <c r="CN99" s="10">
-        <v>-808.05819450683998</v>
+        <v>-467.72552784017336</v>
       </c>
       <c r="CO99" s="10">
-        <v>-823.17125546328589</v>
+        <v>-957.06011949848289</v>
       </c>
       <c r="CP99" s="10">
-        <v>-443.97983783087921</v>
+        <v>-419.22059393681326</v>
       </c>
       <c r="CQ99" s="10">
-        <v>-520.8307007018991</v>
+        <v>-487.0063094923853</v>
       </c>
       <c r="CR99" s="10">
-        <v>-538.95269673950872</v>
+        <v>-575.39613359001817</v>
       </c>
       <c r="CS99" s="10">
-        <v>-626.58579337113304</v>
+        <v>-629.0094627159142</v>
       </c>
       <c r="CT99" s="10">
-        <v>-985.71247507229668</v>
+        <v>-941.28508402687896</v>
       </c>
       <c r="CU99" s="10">
-        <v>-964.43991722661485</v>
+        <v>-994.73873934867152</v>
       </c>
       <c r="CV99" s="10">
-        <v>-982.01539479632265</v>
+        <v>-1000</v>
       </c>
       <c r="CW99" s="10">
         <v>-1000</v>
@@ -31083,7 +31083,7 @@
         <v>-1000</v>
       </c>
       <c r="CY99" s="10">
-        <v>-978.22214197776725</v>
+        <v>-1000</v>
       </c>
       <c r="CZ99" s="10">
         <v>-1000</v>
@@ -31092,25 +31092,25 @@
         <v>-1000</v>
       </c>
       <c r="DB99" s="10">
-        <v>-1000</v>
+        <v>-976.5676386565392</v>
       </c>
       <c r="DC99" s="10">
-        <v>-1000</v>
+        <v>-933.39796042994999</v>
       </c>
       <c r="DD99" s="10">
-        <v>-1000</v>
+        <v>-939.98241994825912</v>
       </c>
       <c r="DE99" s="10">
-        <v>-1000</v>
+        <v>-946.68453504171305</v>
       </c>
       <c r="DF99" s="10">
-        <v>-1000</v>
+        <v>-953.50630592175526</v>
       </c>
       <c r="DG99" s="10">
-        <v>-973.52443294708303</v>
+        <v>-892.69109961374954</v>
       </c>
       <c r="DH99" s="11">
-        <v>-1000</v>
+        <v>-745.65031921106402</v>
       </c>
     </row>
     <row r="101" spans="1:112" x14ac:dyDescent="0.35">
@@ -31146,7 +31146,7 @@
         <v>1</v>
       </c>
       <c r="B103" s="3">
-        <v>-806.20651588316662</v>
+        <v>-806.20651588316673</v>
       </c>
       <c r="C103" s="4">
         <v>-818.83713177499976</v>
@@ -31161,19 +31161,19 @@
         <v>-858.14477009110283</v>
       </c>
       <c r="G103" s="4">
-        <v>-871.73269323110003</v>
+        <v>-871.73269323109992</v>
       </c>
       <c r="H103" s="4">
         <v>-885.5702002725385</v>
       </c>
       <c r="I103" s="4">
-        <v>-899.66153416377847</v>
+        <v>-899.66153416377824</v>
       </c>
       <c r="J103" s="4">
-        <v>-914.01100998293271</v>
+        <v>-914.01100998293259</v>
       </c>
       <c r="K103" s="4">
-        <v>-928.62301609907399</v>
+        <v>-928.62301609907411</v>
       </c>
       <c r="L103" s="4">
         <v>-943.50201554928663</v>
@@ -31182,13 +31182,13 @@
         <v>-958.65254724191584</v>
       </c>
       <c r="N103" s="4">
-        <v>-974.07922718138184</v>
+        <v>-974.07922718138161</v>
       </c>
       <c r="O103" s="4">
         <v>-989.78674986658189</v>
       </c>
       <c r="P103" s="4">
-        <v>-1005.7798896682639</v>
+        <v>-1005.7798896682636</v>
       </c>
       <c r="Q103" s="4">
         <v>-1022.0635022940739</v>
@@ -31203,7 +31203,7 @@
         <v>-1072.7069766695549</v>
       </c>
       <c r="U103" s="4">
-        <v>-1090.2027066940375</v>
+        <v>-1090.2027066940366</v>
       </c>
       <c r="V103" s="4">
         <v>-1100</v>
@@ -31236,7 +31236,7 @@
         <v>-904.30814515166639</v>
       </c>
       <c r="AH103" s="4">
-        <v>-918.64366718583301</v>
+        <v>-918.6436671858329</v>
       </c>
       <c r="AI103" s="4">
         <v>-933.24148232467701</v>
@@ -31248,10 +31248,10 @@
         <v>-963.24190367188987</v>
       </c>
       <c r="AL103" s="4">
-        <v>-978.65365652091862</v>
+        <v>-978.65365652091828</v>
       </c>
       <c r="AM103" s="4">
-        <v>-994.34599842014381</v>
+        <v>-994.3459984201437</v>
       </c>
       <c r="AN103" s="4">
         <v>-1010.3236993397179</v>
@@ -31263,7 +31263,7 @@
         <v>-1043.1546652101981</v>
       </c>
       <c r="AQ103" s="4">
-        <v>-1060.0178811551248</v>
+        <v>-1060.017881155125</v>
       </c>
       <c r="AR103" s="4">
         <v>-1077.1863609578788</v>
@@ -31308,7 +31308,7 @@
         <v>1</v>
       </c>
       <c r="BG103" s="3">
-        <v>-1084.1898492164996</v>
+        <v>-1084.1898492165001</v>
       </c>
       <c r="BH103" s="4">
         <v>-1100</v>
@@ -31398,40 +31398,40 @@
         <v>-843.80223865166636</v>
       </c>
       <c r="CL103" s="4">
-        <v>-857.10916027533324</v>
+        <v>-857.10916027533312</v>
       </c>
       <c r="CM103" s="4">
-        <v>-870.66088879669883</v>
+        <v>-870.6608887966986</v>
       </c>
       <c r="CN103" s="4">
-        <v>-884.46158595469092</v>
+        <v>-884.4615859546908</v>
       </c>
       <c r="CO103" s="4">
         <v>-898.51548417243043</v>
       </c>
       <c r="CP103" s="4">
-        <v>-912.82688788996848</v>
+        <v>-912.82688788996825</v>
       </c>
       <c r="CQ103" s="4">
-        <v>-927.40017472246791</v>
+        <v>-927.40017472246768</v>
       </c>
       <c r="CR103" s="4">
         <v>-942.23979663918112</v>
       </c>
       <c r="CS103" s="4">
-        <v>-957.35028135857578</v>
+        <v>-957.35028135857556</v>
       </c>
       <c r="CT103" s="4">
-        <v>-972.73623356996313</v>
+        <v>-972.73623356996291</v>
       </c>
       <c r="CU103" s="4">
         <v>-988.40233617700562</v>
       </c>
       <c r="CV103" s="4">
-        <v>-1004.3533517151316</v>
+        <v>-1004.3533517151313</v>
       </c>
       <c r="CW103" s="4">
-        <v>-1020.5941237482389</v>
+        <v>-1020.5941237482384</v>
       </c>
       <c r="CX103" s="4">
         <v>-1037.1295783534083</v>
@@ -31440,7 +31440,7 @@
         <v>-1053.9647246973495</v>
       </c>
       <c r="CZ103" s="4">
-        <v>-1071.1046577599711</v>
+        <v>-1071.1046577599714</v>
       </c>
       <c r="DA103" s="4">
         <v>-1088.5545589154904</v>
@@ -31493,7 +31493,7 @@
         <v>1158.0533388179349</v>
       </c>
       <c r="I104" s="7">
-        <v>1176.4804677526336</v>
+        <v>1176.4804677526331</v>
       </c>
       <c r="J104" s="7">
         <v>1195.245166900758</v>
@@ -31508,10 +31508,10 @@
         <v>1253.62256177789</v>
       </c>
       <c r="N104" s="7">
-        <v>1273.7959124679608</v>
+        <v>1273.7959124679605</v>
       </c>
       <c r="O104" s="7">
-        <v>1294.3365190562995</v>
+        <v>1294.336519056299</v>
       </c>
       <c r="P104" s="7">
         <v>1315.2506249508065</v>
@@ -31529,7 +31529,7 @@
         <v>1402.7706617986487</v>
       </c>
       <c r="U104" s="7">
-        <v>1425.6496933691258</v>
+        <v>1425.6496933691255</v>
       </c>
       <c r="V104" s="7">
         <v>1444.9347506126078</v>
@@ -31574,7 +31574,7 @@
         <v>1259.6240278786252</v>
       </c>
       <c r="AL104" s="7">
-        <v>1279.777858527355</v>
+        <v>1279.7778585273547</v>
       </c>
       <c r="AM104" s="7">
         <v>1300.2986133186496</v>
@@ -31589,10 +31589,10 @@
         <v>1364.1253314287205</v>
       </c>
       <c r="AQ104" s="7">
-        <v>1386.1772292028554</v>
+        <v>1386.1772292028556</v>
       </c>
       <c r="AR104" s="7">
-        <v>1408.6283181756876</v>
+        <v>1408.6283181756878</v>
       </c>
       <c r="AS104" s="7">
         <v>1431.4853846552242</v>
@@ -31727,16 +31727,16 @@
         <v>1120.8350557446663</v>
       </c>
       <c r="CM104" s="7">
-        <v>1138.5565468879906</v>
+        <v>1138.5565468879904</v>
       </c>
       <c r="CN104" s="7">
-        <v>1156.603612402288</v>
+        <v>1156.6036124022878</v>
       </c>
       <c r="CO104" s="7">
         <v>1174.9817869947169</v>
       </c>
       <c r="CP104" s="7">
-        <v>1193.6966995484204</v>
+        <v>1193.6966995484202</v>
       </c>
       <c r="CQ104" s="7">
         <v>1212.7540746370732</v>
@@ -31745,10 +31745,10 @@
         <v>1232.1597340666217</v>
       </c>
       <c r="CS104" s="7">
-        <v>1251.9195986996758</v>
+        <v>1251.9195986996756</v>
       </c>
       <c r="CT104" s="7">
-        <v>1272.0396900530286</v>
+        <v>1272.0396900530282</v>
       </c>
       <c r="CU104" s="7">
         <v>1292.5261319237766</v>
@@ -31757,7 +31757,7 @@
         <v>1313.385152242864</v>
       </c>
       <c r="CW104" s="7">
-        <v>1334.6230849015428</v>
+        <v>1334.6230849015426</v>
       </c>
       <c r="CX104" s="7">
         <v>1356.2463716929187</v>
@@ -31798,7 +31798,7 @@
         <v>3</v>
       </c>
       <c r="B105" s="9">
-        <v>-248.06354334866666</v>
+        <v>-248.0635433486666</v>
       </c>
       <c r="C105" s="10">
         <v>-251.94988669999998</v>
@@ -31810,10 +31810,10 @@
         <v>-259.9391565825332</v>
       </c>
       <c r="F105" s="10">
-        <v>-264.04454464341643</v>
+        <v>-264.04454464341632</v>
       </c>
       <c r="G105" s="10">
-        <v>-268.22544407110763</v>
+        <v>-268.22544407110769</v>
       </c>
       <c r="H105" s="10">
         <v>-272.48313854539646</v>
@@ -31825,7 +31825,7 @@
         <v>-281.23415691782543</v>
       </c>
       <c r="K105" s="10">
-        <v>-285.73015879971501</v>
+        <v>-285.73015879971507</v>
       </c>
       <c r="L105" s="10">
         <v>-290.30831247670358</v>
@@ -31834,13 +31834,13 @@
         <v>-294.97001453597414</v>
       </c>
       <c r="N105" s="10">
-        <v>-299.71668528657892</v>
+        <v>-299.71668528657904</v>
       </c>
       <c r="O105" s="10">
-        <v>-304.54976918971761</v>
+        <v>-304.54976918971749</v>
       </c>
       <c r="P105" s="10">
-        <v>-309.47073528254259</v>
+        <v>-309.47073528254271</v>
       </c>
       <c r="Q105" s="10">
         <v>-314.48107762894585</v>
@@ -31855,7 +31855,7 @@
         <v>-330.06368512909376</v>
       </c>
       <c r="U105" s="10">
-        <v>-335.44698667508851</v>
+        <v>-335.44698667508874</v>
       </c>
       <c r="V105" s="10">
         <v>-344.93475061260779</v>
@@ -31888,25 +31888,25 @@
         <v>-278.2486600466666</v>
       </c>
       <c r="AH105" s="10">
-        <v>-282.6595899033332</v>
+        <v>-282.65958990333314</v>
       </c>
       <c r="AI105" s="10">
-        <v>-287.15122533066983</v>
+        <v>-287.15122533066994</v>
       </c>
       <c r="AJ105" s="10">
         <v>-291.72493833004467</v>
       </c>
       <c r="AK105" s="10">
-        <v>-296.3821242067354</v>
+        <v>-296.38212420673534</v>
       </c>
       <c r="AL105" s="10">
-        <v>-301.12420200643624</v>
+        <v>-301.12420200643646</v>
       </c>
       <c r="AM105" s="10">
-        <v>-305.95261489850577</v>
+        <v>-305.95261489850583</v>
       </c>
       <c r="AN105" s="10">
-        <v>-310.86883056606712</v>
+        <v>-310.868830566067</v>
       </c>
       <c r="AO105" s="10">
         <v>-315.87434166308344</v>
@@ -31915,10 +31915,10 @@
         <v>-320.97066621852252</v>
       </c>
       <c r="AQ105" s="10">
-        <v>-326.15934804773076</v>
+        <v>-326.15934804773065</v>
       </c>
       <c r="AR105" s="10">
-        <v>-331.44195721780898</v>
+        <v>-331.44195721780875</v>
       </c>
       <c r="AS105" s="10">
         <v>-336.82009050711122</v>
@@ -31960,7 +31960,7 @@
         <v>3</v>
       </c>
       <c r="BG105" s="9">
-        <v>-333.59687668200002</v>
+        <v>-333.5968766819999</v>
       </c>
       <c r="BH105" s="10">
         <v>-339.71037758749981</v>
@@ -32053,10 +32053,10 @@
         <v>-263.72589546933318</v>
       </c>
       <c r="CM105" s="10">
-        <v>-267.89565809129181</v>
+        <v>-267.89565809129192</v>
       </c>
       <c r="CN105" s="10">
-        <v>-272.14202644759723</v>
+        <v>-272.14202644759729</v>
       </c>
       <c r="CO105" s="10">
         <v>-276.46630282228637</v>
@@ -32065,25 +32065,25 @@
         <v>-280.86981165845191</v>
       </c>
       <c r="CQ105" s="10">
-        <v>-285.35389991460534</v>
+        <v>-285.35389991460545</v>
       </c>
       <c r="CR105" s="10">
         <v>-289.91993742744046</v>
       </c>
       <c r="CS105" s="10">
-        <v>-294.56931734110003</v>
+        <v>-294.56931734110015</v>
       </c>
       <c r="CT105" s="10">
-        <v>-299.30345648306525</v>
+        <v>-299.30345648306559</v>
       </c>
       <c r="CU105" s="10">
-        <v>-304.12379574677095</v>
+        <v>-304.12379574677101</v>
       </c>
       <c r="CV105" s="10">
         <v>-309.03180052773268</v>
       </c>
       <c r="CW105" s="10">
-        <v>-314.02896115330395</v>
+        <v>-314.02896115330418</v>
       </c>
       <c r="CX105" s="10">
         <v>-319.11679333951042</v>
@@ -32092,7 +32092,7 @@
         <v>-324.29683836841537</v>
       </c>
       <c r="CZ105" s="10">
-        <v>-329.5706639261449</v>
+        <v>-329.57066392614479</v>
       </c>
       <c r="DA105" s="10">
         <v>-334.93986428168944</v>
@@ -32207,86 +32207,86 @@
         <v>6</v>
       </c>
       <c r="B108" s="15">
-        <v>882194547.0368638</v>
+        <v>989486080.57346034</v>
       </c>
       <c r="C108" s="16">
-        <v>1027192932.2270336</v>
+        <v>1113841434.2999015</v>
       </c>
       <c r="D108" s="16">
-        <v>740092110.54769337</v>
+        <v>779541553.01127577</v>
       </c>
       <c r="E108" s="16">
-        <v>895741725.70934093</v>
+        <v>908391018.07581735</v>
       </c>
       <c r="F108" s="16">
-        <v>643360549.76442707</v>
+        <v>652779435.79568303</v>
       </c>
       <c r="G108" s="16">
-        <v>610875140.25059938</v>
+        <v>611700610.03888702</v>
       </c>
       <c r="H108" s="16">
-        <v>807393694.8868854</v>
+        <v>596181826.68554759</v>
       </c>
       <c r="I108" s="16">
-        <v>911388930.15661192</v>
+        <v>1003514096.9791226</v>
       </c>
       <c r="J108" s="16">
-        <v>855654976.59322691</v>
+        <v>910908503.93928933</v>
       </c>
       <c r="K108" s="16">
-        <v>732541937.21779132</v>
+        <v>825729046.6302166</v>
       </c>
       <c r="L108" s="16">
-        <v>954986752.14344501</v>
+        <v>993070966.66855288</v>
       </c>
       <c r="M108" s="16">
-        <v>570464081.55472338</v>
+        <v>622260323.62006009</v>
       </c>
       <c r="N108" s="16">
-        <v>523843278.11700046</v>
+        <v>550434509.49703407</v>
       </c>
       <c r="O108" s="16">
-        <v>480866055.10631108</v>
+        <v>519365521.92643291</v>
       </c>
       <c r="P108" s="16">
-        <v>426372390.32923752</v>
+        <v>443641360.96275336</v>
       </c>
       <c r="Q108" s="16">
-        <v>392272870.90558904</v>
+        <v>419897419.0262816</v>
       </c>
       <c r="R108" s="16">
-        <v>373596228.99740398</v>
+        <v>383340924.41647214</v>
       </c>
       <c r="S108" s="16">
-        <v>342660841.99512196</v>
+        <v>338186271.37471366</v>
       </c>
       <c r="T108" s="16">
-        <v>303444350.20832217</v>
+        <v>352807959.2992506</v>
       </c>
       <c r="U108" s="16">
-        <v>299227765.8888917</v>
+        <v>310072982.37741023</v>
       </c>
       <c r="V108" s="16">
-        <v>255330835.24346411</v>
+        <v>291184268.94242656</v>
       </c>
       <c r="W108" s="16">
-        <v>243662473.56028193</v>
+        <v>255783500.28390574</v>
       </c>
       <c r="X108" s="16">
-        <v>223864477.16053623</v>
+        <v>240514754.96915722</v>
       </c>
       <c r="Y108" s="16">
-        <v>213120330.7724058</v>
+        <v>240232542.47137171</v>
       </c>
       <c r="Z108" s="16">
-        <v>107708885.67778352</v>
+        <v>216936427.07525811</v>
       </c>
       <c r="AA108" s="17">
-        <v>108971087.26283523</v>
+        <v>71721495.994884089</v>
       </c>
       <c r="AB108" s="18">
         <f>SUM(TotalCost)</f>
-        <v>13926829249.313826</v>
+        <v>14641524834.935165</v>
       </c>
     </row>
     <row r="110" spans="1:112" x14ac:dyDescent="0.35">
@@ -32380,86 +32380,86 @@
         <v>8</v>
       </c>
       <c r="B111" s="3">
-        <v>56080721.31474176</v>
+        <v>66019542.132053524</v>
       </c>
       <c r="C111" s="4">
-        <v>52122236.529745236</v>
+        <v>60497903.27708631</v>
       </c>
       <c r="D111" s="4">
-        <v>49373483.182217084</v>
+        <v>55214356.882497512</v>
       </c>
       <c r="E111" s="4">
-        <v>46216146.747174747</v>
+        <v>51404129.702921711</v>
       </c>
       <c r="F111" s="4">
-        <v>43561832.338387832</v>
+        <v>47736062.994850621</v>
       </c>
       <c r="G111" s="4">
-        <v>43568858.439155236</v>
+        <v>44010668.088156313</v>
       </c>
       <c r="H111" s="4">
-        <v>36531198.099503912</v>
+        <v>43011696.667752378</v>
       </c>
       <c r="I111" s="4">
-        <v>32595715.086954635</v>
+        <v>33910435.573974378</v>
       </c>
       <c r="J111" s="4">
-        <v>28017365.398364462</v>
+        <v>31595954.281179965</v>
       </c>
       <c r="K111" s="4">
-        <v>28906747.961858839</v>
+        <v>29291798.684541285</v>
       </c>
       <c r="L111" s="4">
-        <v>27377497.553054418</v>
+        <v>26998595.661908001</v>
       </c>
       <c r="M111" s="4">
-        <v>33259205.239409909</v>
+        <v>32164560.172922753</v>
       </c>
       <c r="N111" s="4">
-        <v>31492828.235885065</v>
+        <v>29227786.329085954</v>
       </c>
       <c r="O111" s="4">
-        <v>29454537.231363557</v>
+        <v>26958178.345772751</v>
       </c>
       <c r="P111" s="4">
-        <v>27575838.897670694</v>
+        <v>24572745.514366347</v>
       </c>
       <c r="Q111" s="4">
-        <v>25981432.106680997</v>
+        <v>22068181.531523395</v>
       </c>
       <c r="R111" s="4">
-        <v>24524709.799650617</v>
+        <v>18263768.041157804</v>
       </c>
       <c r="S111" s="4">
-        <v>22860880.313106321</v>
+        <v>15661630.821765177</v>
       </c>
       <c r="T111" s="4">
-        <v>17743422.324856866</v>
+        <v>13527020.140562534</v>
       </c>
       <c r="U111" s="4">
-        <v>16869226.467742521</v>
+        <v>9639309.4927339703</v>
       </c>
       <c r="V111" s="4">
-        <v>12412859.863797221</v>
+        <v>8252920.5455939034</v>
       </c>
       <c r="W111" s="4">
-        <v>10851935.752545834</v>
+        <v>5833105.5875003524</v>
       </c>
       <c r="X111" s="4">
-        <v>9713004.4166006185</v>
+        <v>4209673.8384816227</v>
       </c>
       <c r="Y111" s="4">
-        <v>8971499.7874000669</v>
+        <v>2966129.6147521613</v>
       </c>
       <c r="Z111" s="4">
-        <v>8387922.1251693396</v>
+        <v>2705165.1910867468</v>
       </c>
       <c r="AA111" s="5">
-        <v>8553244.6059758067</v>
+        <v>2760068.0435388321</v>
       </c>
       <c r="AB111" s="12">
         <f>SUM(B111:AA111)</f>
-        <v>733004349.8190136</v>
+        <v>708501387.15776634</v>
       </c>
     </row>
     <row r="112" spans="1:112" x14ac:dyDescent="0.35">
@@ -32467,86 +32467,86 @@
         <v>9</v>
       </c>
       <c r="B112" s="6">
-        <v>13693612.351999726</v>
+        <v>15626966.9124476</v>
       </c>
       <c r="C112" s="7">
-        <v>12910034.955551323</v>
+        <v>14574539.413112208</v>
       </c>
       <c r="D112" s="7">
-        <v>11803031.052291863</v>
+        <v>13574207.705706164</v>
       </c>
       <c r="E112" s="7">
-        <v>10735218.286053972</v>
+        <v>12460955.691577751</v>
       </c>
       <c r="F112" s="7">
-        <v>9825019.9733474664</v>
+        <v>11237954.455891598</v>
       </c>
       <c r="G112" s="7">
-        <v>8699706.2670457829</v>
+        <v>9962459.8232148141</v>
       </c>
       <c r="H112" s="7">
-        <v>7728790.571307431</v>
+        <v>8350464.9660774786</v>
       </c>
       <c r="I112" s="7">
-        <v>6877815.9656397365</v>
+        <v>7275897.8370246533</v>
       </c>
       <c r="J112" s="7">
-        <v>5331580.837738147</v>
+        <v>6619774.3327735644</v>
       </c>
       <c r="K112" s="7">
-        <v>6013121.175167527</v>
+        <v>6026842.5001890566</v>
       </c>
       <c r="L112" s="7">
-        <v>5572376.9896346927</v>
+        <v>5493382.6348428559</v>
       </c>
       <c r="M112" s="7">
-        <v>5350984.7397248773</v>
+        <v>5275972.6827879995</v>
       </c>
       <c r="N112" s="7">
-        <v>5173678.0068704998</v>
+        <v>4594147.9331641337</v>
       </c>
       <c r="O112" s="7">
-        <v>4764542.4772227388</v>
+        <v>4350194.4213034706</v>
       </c>
       <c r="P112" s="7">
-        <v>4399748.7143763676</v>
+        <v>3913282.0105281677</v>
       </c>
       <c r="Q112" s="7">
-        <v>4203913.7553110821</v>
+        <v>3412255.4633895727</v>
       </c>
       <c r="R112" s="7">
-        <v>4060807.9026410091</v>
+        <v>3045568.3090057038</v>
       </c>
       <c r="S112" s="7">
-        <v>3700447.4217935856</v>
+        <v>2627966.4639655915</v>
       </c>
       <c r="T112" s="7">
-        <v>3476909.0214111428</v>
+        <v>2127785.0013942271</v>
       </c>
       <c r="U112" s="7">
-        <v>3173954.1943944762</v>
+        <v>1919907.3698859056</v>
       </c>
       <c r="V112" s="7">
-        <v>2888436.554679858</v>
+        <v>1576751.0605597962</v>
       </c>
       <c r="W112" s="7">
-        <v>2619073.3308371557</v>
+        <v>1332531.7713315303</v>
       </c>
       <c r="X112" s="7">
-        <v>2392734.1153764175</v>
+        <v>756566.98153892858</v>
       </c>
       <c r="Y112" s="7">
-        <v>2177465.1671468522</v>
+        <v>324416.12251611747</v>
       </c>
       <c r="Z112" s="7">
-        <v>2032678.1277358676</v>
+        <v>255578.08344106533</v>
       </c>
       <c r="AA112" s="8">
-        <v>153017.4622869888</v>
+        <v>112939.73302413839</v>
       </c>
       <c r="AB112" s="13">
         <f t="shared" ref="AB112:AB115" si="0">SUM(B112:AA112)</f>
-        <v>149758699.41758659</v>
+        <v>146829309.68069407</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -32554,86 +32554,86 @@
         <v>10</v>
       </c>
       <c r="B113" s="6">
-        <v>65269687549.518211</v>
+        <v>88088931601.740631</v>
       </c>
       <c r="C113" s="7">
-        <v>61748883955.847084</v>
+        <v>83337203217.706909</v>
       </c>
       <c r="D113" s="7">
-        <v>58418000957.947197</v>
+        <v>78841794466.856079</v>
       </c>
       <c r="E113" s="7">
-        <v>55266793783.073227</v>
+        <v>74588878853.007141</v>
       </c>
       <c r="F113" s="7">
-        <v>52285570286.109184</v>
+        <v>70565375714.366684</v>
       </c>
       <c r="G113" s="7">
-        <v>49465161139.507774</v>
+        <v>66758909991.432037</v>
       </c>
       <c r="H113" s="7">
-        <v>46796891631.255989</v>
+        <v>63157774165.110214</v>
       </c>
       <c r="I113" s="7">
-        <v>44272554984.126129</v>
+        <v>59750892247.986176</v>
       </c>
       <c r="J113" s="7">
-        <v>41884387114.150406</v>
+        <v>56527785717.988411</v>
       </c>
       <c r="K113" s="7">
-        <v>39625042750.684059</v>
+        <v>53478541289.674393</v>
       </c>
       <c r="L113" s="7">
-        <v>37487572844.609558</v>
+        <v>50593780424.010269</v>
       </c>
       <c r="M113" s="7">
-        <v>35465403195.196495</v>
+        <v>47864630482.866142</v>
       </c>
       <c r="N113" s="7">
-        <v>33552314229.879929</v>
+        <v>45282697439.507187</v>
       </c>
       <c r="O113" s="7">
-        <v>31742421874.766056</v>
+        <v>42840040061.146317</v>
       </c>
       <c r="P113" s="7">
-        <v>30030159457.028679</v>
+        <v>40529145484.151939</v>
       </c>
       <c r="Q113" s="7">
-        <v>28410260583.533855</v>
+        <v>38342906106.787621</v>
       </c>
       <c r="R113" s="7">
-        <v>26877742943.032642</v>
+        <v>36274597728.412842</v>
       </c>
       <c r="S113" s="7">
-        <v>25427892982.102398</v>
+        <v>34317858867.907711</v>
       </c>
       <c r="T113" s="7">
-        <v>24056251407.704639</v>
+        <v>32466671197.711487</v>
       </c>
       <c r="U113" s="7">
-        <v>22758599471.769672</v>
+        <v>30715341033.296055</v>
       </c>
       <c r="V113" s="7">
-        <v>21530945995.623684</v>
+        <v>29058481821.141586</v>
       </c>
       <c r="W113" s="7">
-        <v>20369515094.349354</v>
+        <v>27490997571.35284</v>
       </c>
       <c r="X113" s="7">
-        <v>19270734563.323925</v>
+        <v>26008067183.9599</v>
       </c>
       <c r="Y113" s="7">
-        <v>18231224891.215282</v>
+        <v>24605129620.695862</v>
       </c>
       <c r="Z113" s="7">
-        <v>17247788865.643391</v>
+        <v>23277869876.64444</v>
       </c>
       <c r="AA113" s="8">
-        <v>16300903735.875515</v>
+        <v>22022205708.610542</v>
       </c>
       <c r="AB113" s="13">
         <f t="shared" si="0"/>
-        <v>923792706287.87439</v>
+        <v>1246786507874.0715</v>
       </c>
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.35">
@@ -32641,86 +32641,86 @@
         <v>11</v>
       </c>
       <c r="B114" s="6">
-        <v>6606342.4784868807</v>
+        <v>7600224.5602180585</v>
       </c>
       <c r="C114" s="7">
-        <v>6213123.4120814856</v>
+        <v>7066525.7230596915</v>
       </c>
       <c r="D114" s="7">
-        <v>5656070.9531539548</v>
+        <v>6559978.2190679964</v>
       </c>
       <c r="E114" s="7">
-        <v>5113302.4717280017</v>
+        <v>6002964.8411675831</v>
       </c>
       <c r="F114" s="7">
-        <v>4649926.2565279137</v>
+        <v>5379900.8056758111</v>
       </c>
       <c r="G114" s="7">
-        <v>4123696.1745990287</v>
+        <v>4728202.0434844792</v>
       </c>
       <c r="H114" s="7">
-        <v>3692313.8671914116</v>
+        <v>4147984.7589948531</v>
       </c>
       <c r="I114" s="7">
-        <v>3290786.8852165756</v>
+        <v>3502596.8215158079</v>
       </c>
       <c r="J114" s="7">
-        <v>3012600.634946811</v>
+        <v>3153101.7511834726</v>
       </c>
       <c r="K114" s="7">
-        <v>2825868.9320089985</v>
+        <v>2835741.6440682458</v>
       </c>
       <c r="L114" s="7">
-        <v>2591559.7939695362</v>
+        <v>2548635.3171840515</v>
       </c>
       <c r="M114" s="7">
-        <v>2623260.3317634696</v>
+        <v>2497362.8973091128</v>
       </c>
       <c r="N114" s="7">
-        <v>2417046.2567987777</v>
+        <v>2219187.2229077425</v>
       </c>
       <c r="O114" s="7">
-        <v>2220620.1173502416</v>
+        <v>1956291.1677324316</v>
       </c>
       <c r="P114" s="7">
-        <v>2039058.9125348767</v>
+        <v>1723112.4697841131</v>
       </c>
       <c r="Q114" s="7">
-        <v>1859791.6089713401</v>
+        <v>1477624.097399974</v>
       </c>
       <c r="R114" s="7">
-        <v>1694002.770603453</v>
+        <v>1267484.7433943497</v>
       </c>
       <c r="S114" s="7">
-        <v>1549631.9927355277</v>
+        <v>1070837.3284140327</v>
       </c>
       <c r="T114" s="7">
-        <v>1419426.1447825434</v>
+        <v>871294.75426194526</v>
       </c>
       <c r="U114" s="7">
-        <v>1279426.8517870007</v>
+        <v>748488.32699015108</v>
       </c>
       <c r="V114" s="7">
-        <v>1180213.4304401167</v>
+        <v>619026.6547870771</v>
       </c>
       <c r="W114" s="7">
-        <v>1059974.8759382542</v>
+        <v>517958.05564630253</v>
       </c>
       <c r="X114" s="7">
-        <v>961624.53677715315</v>
+        <v>405086.66185941268</v>
       </c>
       <c r="Y114" s="7">
-        <v>867777.30963733129</v>
+        <v>315272.44532089843</v>
       </c>
       <c r="Z114" s="7">
-        <v>794756.61880210228</v>
+        <v>281749.53123739792</v>
       </c>
       <c r="AA114" s="8">
-        <v>384124.63297383673</v>
+        <v>240017.55020063929</v>
       </c>
       <c r="AB114" s="13">
         <f t="shared" si="0"/>
-        <v>70126328.251806632</v>
+        <v>69736650.392865643</v>
       </c>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.35">
@@ -32728,86 +32728,86 @@
         <v>12</v>
       </c>
       <c r="B115" s="9">
-        <v>955595.9216688897</v>
+        <v>1100688.1963741709</v>
       </c>
       <c r="C115" s="10">
-        <v>897884.89886747301</v>
+        <v>1022522.9778893453</v>
       </c>
       <c r="D115" s="10">
-        <v>816491.5310087346</v>
+        <v>948316.78249005205</v>
       </c>
       <c r="E115" s="10">
-        <v>736908.00105995941</v>
+        <v>866602.09543490061</v>
       </c>
       <c r="F115" s="10">
-        <v>668732.58585753199</v>
+        <v>775235.1850442756</v>
       </c>
       <c r="G115" s="10">
-        <v>590098.75073441374</v>
+        <v>679907.01630599273</v>
       </c>
       <c r="H115" s="10">
-        <v>524274.35039086896</v>
+        <v>594652.14647394256</v>
       </c>
       <c r="I115" s="10">
-        <v>464551.89448695438</v>
+        <v>495195.66952553601</v>
       </c>
       <c r="J115" s="10">
-        <v>424041.79825055395</v>
+        <v>444626.33161440911</v>
       </c>
       <c r="K115" s="10">
-        <v>397361.71086526359</v>
+        <v>398736.73362766643</v>
       </c>
       <c r="L115" s="10">
-        <v>363444.28848854068</v>
+        <v>357252.67816157057</v>
       </c>
       <c r="M115" s="10">
-        <v>373108.91934383818</v>
+        <v>354609.07775422488</v>
       </c>
       <c r="N115" s="10">
-        <v>342877.23941183393</v>
+        <v>314070.14918926836</v>
       </c>
       <c r="O115" s="10">
-        <v>314173.58159605711</v>
+        <v>275545.69205720752</v>
       </c>
       <c r="P115" s="10">
-        <v>287657.23042405397</v>
+        <v>241552.18802064902</v>
       </c>
       <c r="Q115" s="10">
-        <v>261350.35163565871</v>
+        <v>205623.08982092029</v>
       </c>
       <c r="R115" s="10">
-        <v>237004.51382745529</v>
+        <v>174960.10397104808</v>
       </c>
       <c r="S115" s="10">
-        <v>215962.48213829487</v>
+        <v>146283.0529369709</v>
       </c>
       <c r="T115" s="10">
-        <v>197085.34469663331</v>
+        <v>117115.48148601741</v>
       </c>
       <c r="U115" s="10">
-        <v>176557.71513180475</v>
+        <v>99619.868329876976</v>
       </c>
       <c r="V115" s="10">
-        <v>162190.7350648967</v>
+        <v>81016.177239515731</v>
       </c>
       <c r="W115" s="10">
-        <v>144576.40080419567</v>
+        <v>66713.040295107552</v>
       </c>
       <c r="X115" s="10">
-        <v>130290.02709576955</v>
+        <v>50587.599830930398</v>
       </c>
       <c r="Y115" s="10">
-        <v>116722.78001623673</v>
+        <v>37877.271892806995</v>
       </c>
       <c r="Z115" s="10">
-        <v>106216.39368047542</v>
+        <v>33664.925437655249</v>
       </c>
       <c r="AA115" s="11">
-        <v>44806.457940911219</v>
+        <v>27776.162287365001</v>
       </c>
       <c r="AB115" s="14">
         <f t="shared" si="0"/>
-        <v>9949965.9044873007</v>
+        <v>9910749.6934914235</v>
       </c>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
spinning reserves tweaks (runs)
</commit_message>
<xml_diff>
--- a/717A11_output.xlsx
+++ b/717A11_output.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jawessel\opl\ENV717A11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfi\Google Drive\School\College\Semester 6 (Spring 2020)\ENV 717\Assignments\Assignment 11 (group project)\ENV717A11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="BuildNGCC">Sheet2!$B$121:$AA$121</definedName>
     <definedName name="BuildSolar">Sheet2!$B$119:$AA$119</definedName>
+    <definedName name="BuildStorage">Sheet2!$B$120:$AA$120</definedName>
     <definedName name="BuildWind">Sheet2!$B$118:$AA$118</definedName>
     <definedName name="CH4_total">Sheet2!$B$114:$AA$114</definedName>
     <definedName name="CO2_total">Sheet2!$B$113:$AA$113</definedName>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="39">
   <si>
     <t>Line</t>
   </si>
@@ -161,6 +163,12 @@
   </si>
   <si>
     <t>*New NGCC</t>
+  </si>
+  <si>
+    <t>BuildNGCC</t>
+  </si>
+  <si>
+    <t>BuildStorage</t>
   </si>
 </sst>
 </file>
@@ -680,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DH119"/>
+  <dimension ref="A1:DH121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="Q114" sqref="Q114"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AB110" sqref="AB110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1377,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>0</v>
+        <v>429.71772768133212</v>
       </c>
       <c r="D4" s="7">
         <v>665.6</v>
@@ -1455,10 +1463,10 @@
         <v>2</v>
       </c>
       <c r="AE4" s="6">
-        <v>1E-3</v>
+        <v>8.8581981387899873</v>
       </c>
       <c r="AF4" s="7">
-        <v>144.34685534967628</v>
+        <v>52.151300499999024</v>
       </c>
       <c r="AG4" s="7">
         <v>665.6</v>
@@ -2107,7 +2115,7 @@
         <v>4</v>
       </c>
       <c r="AE6" s="6">
-        <v>198.41517248122545</v>
+        <v>212</v>
       </c>
       <c r="AF6" s="7">
         <v>212</v>
@@ -2278,7 +2286,7 @@
         <v>212</v>
       </c>
       <c r="CL6" s="7">
-        <v>132.42057623405913</v>
+        <v>132.42156536450631</v>
       </c>
       <c r="CM6" s="7">
         <v>0</v>
@@ -2520,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="BI7" s="7">
-        <v>64.341936699998627</v>
+        <v>64.341936699998655</v>
       </c>
       <c r="BJ7" s="7">
         <v>0</v>
@@ -3085,7 +3093,7 @@
         <v>7</v>
       </c>
       <c r="AE9" s="6">
-        <v>74.376977748774266</v>
+        <v>51.934952091209652</v>
       </c>
       <c r="AF9" s="7">
         <v>84.6</v>
@@ -3662,7 +3670,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="7">
-        <v>422.69481875332951</v>
+        <v>650</v>
       </c>
       <c r="E11" s="7">
         <v>0</v>
@@ -3677,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="7">
-        <v>0</v>
+        <v>639.44939469696737</v>
       </c>
       <c r="J11" s="7">
         <v>650</v>
@@ -3692,13 +3700,13 @@
         <v>640.83130332913174</v>
       </c>
       <c r="N11" s="7">
-        <v>650</v>
+        <v>639.17047026398018</v>
       </c>
       <c r="O11" s="7">
         <v>650</v>
       </c>
       <c r="P11" s="7">
-        <v>650</v>
+        <v>631.21378756871422</v>
       </c>
       <c r="Q11" s="7">
         <v>650</v>
@@ -3719,10 +3727,10 @@
         <v>650</v>
       </c>
       <c r="W11" s="7">
-        <v>431.74350612439457</v>
+        <v>431.74350612439321</v>
       </c>
       <c r="X11" s="7">
-        <v>347.70211440650985</v>
+        <v>347.70211440650849</v>
       </c>
       <c r="Y11" s="7">
         <v>220.73497596941766</v>
@@ -3776,7 +3784,7 @@
         <v>650</v>
       </c>
       <c r="AR11" s="7">
-        <v>650</v>
+        <v>636.9141548044613</v>
       </c>
       <c r="AS11" s="7">
         <v>650</v>
@@ -3788,19 +3796,19 @@
         <v>650</v>
       </c>
       <c r="AV11" s="7">
-        <v>597.24761976880757</v>
+        <v>597.24756816910747</v>
       </c>
       <c r="AW11" s="7">
-        <v>611.71450967903604</v>
+        <v>650</v>
       </c>
       <c r="AX11" s="7">
         <v>521.83095745795401</v>
       </c>
       <c r="AY11" s="7">
-        <v>439.67800593273824</v>
+        <v>422.17800593273631</v>
       </c>
       <c r="AZ11" s="7">
-        <v>9.8014099715944436</v>
+        <v>9.801409971592534</v>
       </c>
       <c r="BA11" s="7">
         <v>0</v>
@@ -3818,7 +3826,7 @@
         <v>9</v>
       </c>
       <c r="BG11" s="6">
-        <v>0</v>
+        <v>55.593150229999651</v>
       </c>
       <c r="BH11" s="7">
         <v>616.10430049999832</v>
@@ -3836,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="BM11" s="7">
-        <v>30.261663085972486</v>
+        <v>30.261663085972373</v>
       </c>
       <c r="BN11" s="7">
         <v>250.18115475723152</v>
@@ -3857,7 +3865,7 @@
         <v>650</v>
       </c>
       <c r="BT11" s="7">
-        <v>637.05639225222285</v>
+        <v>650</v>
       </c>
       <c r="BU11" s="7">
         <v>650</v>
@@ -3866,7 +3874,7 @@
         <v>650</v>
       </c>
       <c r="BW11" s="7">
-        <v>650</v>
+        <v>624.06395056645249</v>
       </c>
       <c r="BX11" s="7">
         <v>650</v>
@@ -3878,10 +3886,10 @@
         <v>650</v>
       </c>
       <c r="CA11" s="7">
-        <v>650</v>
+        <v>632.159525134977</v>
       </c>
       <c r="CB11" s="7">
-        <v>21.835115000273618</v>
+        <v>21.835115000270889</v>
       </c>
       <c r="CC11" s="7">
         <v>0</v>
@@ -3920,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="CP11" s="7">
-        <v>632.61453829050447</v>
+        <v>1E-3</v>
       </c>
       <c r="CQ11" s="7">
         <v>650</v>
@@ -3935,25 +3943,25 @@
         <v>475.52188020159247</v>
       </c>
       <c r="CU11" s="7">
-        <v>626.01551610340414</v>
+        <v>650</v>
       </c>
       <c r="CV11" s="7">
         <v>650</v>
       </c>
       <c r="CW11" s="7">
-        <v>631.62218349112743</v>
+        <v>650</v>
       </c>
       <c r="CX11" s="7">
-        <v>547.84409202646123</v>
+        <v>650</v>
       </c>
       <c r="CY11" s="7">
-        <v>637.67626926528021</v>
+        <v>650</v>
       </c>
       <c r="CZ11" s="7">
         <v>428.93571561745659</v>
       </c>
       <c r="DA11" s="7">
-        <v>1E-3</v>
+        <v>138.81263352135349</v>
       </c>
       <c r="DB11" s="7">
         <v>0</v>
@@ -4144,7 +4152,7 @@
         <v>10</v>
       </c>
       <c r="BG12" s="6">
-        <v>55.593150229999651</v>
+        <v>0</v>
       </c>
       <c r="BH12" s="7">
         <v>0</v>
@@ -4171,10 +4179,10 @@
         <v>0</v>
       </c>
       <c r="BP12" s="7">
-        <v>170.86471700224638</v>
+        <v>170.86471700225184</v>
       </c>
       <c r="BQ12" s="7">
-        <v>170.69335138729204</v>
+        <v>170.69335138729056</v>
       </c>
       <c r="BR12" s="7">
         <v>0</v>
@@ -4981,10 +4989,10 @@
         <v>1074.2170861310274</v>
       </c>
       <c r="I15" s="7">
-        <v>1111.1745642566548</v>
+        <v>471.7251695596874</v>
       </c>
       <c r="J15" s="7">
-        <v>498.80321778371763</v>
+        <v>498.80321778371786</v>
       </c>
       <c r="K15" s="7">
         <v>263.61445659319065</v>
@@ -5149,10 +5157,10 @@
         <v>1502.7964903228039</v>
       </c>
       <c r="BP15" s="7">
-        <v>1212.5184677631951</v>
+        <v>1212.5184677631896</v>
       </c>
       <c r="BQ15" s="7">
-        <v>844.26439984961166</v>
+        <v>844.26439984961314</v>
       </c>
       <c r="BR15" s="7">
         <v>422.53698361168017</v>
@@ -5224,7 +5232,7 @@
         <v>1151.0750651003696</v>
       </c>
       <c r="CP15" s="7">
-        <v>556.93216057797122</v>
+        <v>1189.5456988684757</v>
       </c>
       <c r="CQ15" s="7">
         <v>578.71524868393908</v>
@@ -6124,7 +6132,7 @@
         <v>0</v>
       </c>
       <c r="BO18" s="7">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="BP18" s="7">
         <v>67</v>
@@ -6133,7 +6141,7 @@
         <v>67</v>
       </c>
       <c r="BR18" s="7">
-        <v>62.900856435897367</v>
+        <v>67</v>
       </c>
       <c r="BS18" s="7">
         <v>67</v>
@@ -6214,7 +6222,7 @@
         <v>67</v>
       </c>
       <c r="CT18" s="7">
-        <v>67</v>
+        <v>62.900856435907372</v>
       </c>
       <c r="CU18" s="7">
         <v>67</v>
@@ -6309,7 +6317,7 @@
         <v>257</v>
       </c>
       <c r="Q19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="R19" s="7">
         <v>0</v>
@@ -6318,7 +6326,7 @@
         <v>231.48338573926094</v>
       </c>
       <c r="T19" s="7">
-        <v>135.48467616602784</v>
+        <v>141.73467616602784</v>
       </c>
       <c r="U19" s="7">
         <v>0</v>
@@ -6390,16 +6398,16 @@
         <v>257</v>
       </c>
       <c r="AT19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="AU19" s="7">
         <v>0</v>
       </c>
       <c r="AV19" s="7">
-        <v>240.28336879515291</v>
+        <v>240.28239459500298</v>
       </c>
       <c r="AW19" s="7">
-        <v>84.753851246791527</v>
+        <v>74.361106086309519</v>
       </c>
       <c r="AX19" s="7">
         <v>0</v>
@@ -6471,16 +6479,16 @@
         <v>257</v>
       </c>
       <c r="BV19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="BW19" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="BX19" s="7">
         <v>257</v>
       </c>
       <c r="BY19" s="7">
-        <v>257</v>
+        <v>186.10786328440736</v>
       </c>
       <c r="BZ19" s="7">
         <v>0</v>
@@ -6552,7 +6560,7 @@
         <v>257</v>
       </c>
       <c r="CX19" s="7">
-        <v>233.62191011182972</v>
+        <v>0</v>
       </c>
       <c r="CY19" s="7">
         <v>0</v>
@@ -6561,7 +6569,7 @@
         <v>0</v>
       </c>
       <c r="DA19" s="7">
-        <v>60.655816760676771</v>
+        <v>0</v>
       </c>
       <c r="DB19" s="7">
         <v>0</v>
@@ -6593,16 +6601,16 @@
         <v>2087.9521502299995</v>
       </c>
       <c r="C20" s="7">
-        <v>1777.2723004999998</v>
+        <v>1347.5545728186678</v>
       </c>
       <c r="D20" s="7">
-        <v>756.50985394666941</v>
+        <v>529.20467269999926</v>
       </c>
       <c r="E20" s="7">
-        <v>625.5708916739984</v>
+        <v>625.57089167399852</v>
       </c>
       <c r="F20" s="7">
-        <v>95.591932817154884</v>
+        <v>95.591932817156135</v>
       </c>
       <c r="G20" s="7">
         <v>14.452226923808666</v>
@@ -6626,19 +6634,19 @@
         <v>512.03066233039181</v>
       </c>
       <c r="N20" s="7">
-        <v>462.21160711431196</v>
+        <v>467.62637198232187</v>
       </c>
       <c r="O20" s="7">
         <v>355.35313796465476</v>
       </c>
       <c r="P20" s="7">
-        <v>255.63580270945369</v>
+        <v>265.02890892509663</v>
       </c>
       <c r="Q20" s="7">
-        <v>156.82475122491383</v>
+        <v>420.07475122491383</v>
       </c>
       <c r="R20" s="7">
-        <v>328.4353891249375</v>
+        <v>328.43538912493756</v>
       </c>
       <c r="S20" s="7">
         <v>0</v>
@@ -6650,7 +6658,7 @@
         <v>52.955467000050248</v>
       </c>
       <c r="V20" s="7">
-        <v>33.912238538051042</v>
+        <v>27.66223853805036</v>
       </c>
       <c r="W20" s="7">
         <v>0</v>
@@ -6674,10 +6682,10 @@
         <v>2269.6</v>
       </c>
       <c r="AF20" s="7">
-        <v>2177.4044451503228</v>
+        <v>2269.6</v>
       </c>
       <c r="AG20" s="7">
-        <v>1733.4865356999981</v>
+        <v>1733.4865356999983</v>
       </c>
       <c r="AH20" s="7">
         <v>1189.8222663449976</v>
@@ -6710,19 +6718,19 @@
         <v>705.51104560245244</v>
       </c>
       <c r="AR20" s="7">
-        <v>543.23259940709409</v>
+        <v>549.77552200486343</v>
       </c>
       <c r="AS20" s="7">
-        <v>390.71564749641425</v>
+        <v>390.71564749641419</v>
       </c>
       <c r="AT20" s="7">
-        <v>239.22738587325262</v>
+        <v>504.97738587325273</v>
       </c>
       <c r="AU20" s="7">
         <v>363.28530106229846</v>
       </c>
       <c r="AV20" s="7">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="AW20" s="7">
         <v>0</v>
@@ -6761,10 +6769,10 @@
         <v>2269.6</v>
       </c>
       <c r="BJ20" s="7">
-        <v>2249.5354091619988</v>
+        <v>2249.5354091619984</v>
       </c>
       <c r="BK20" s="7">
-        <v>1963.3145671024511</v>
+        <v>2269.6</v>
       </c>
       <c r="BL20" s="7">
         <v>1466.9097672744924</v>
@@ -6776,7 +6784,7 @@
         <v>1165.6550583300618</v>
       </c>
       <c r="BO20" s="7">
-        <v>1203.885793225963</v>
+        <v>1203.884793225963</v>
       </c>
       <c r="BP20" s="7">
         <v>1175.7964793358092</v>
@@ -6785,31 +6793,31 @@
         <v>1215.3986758658325</v>
       </c>
       <c r="BR20" s="7">
-        <v>1259.803282092279</v>
+        <v>1255.7041385281764</v>
       </c>
       <c r="BS20" s="7">
         <v>1296.7248227764958</v>
       </c>
       <c r="BT20" s="7">
-        <v>1115.3337178910519</v>
+        <v>1108.8619140171634</v>
       </c>
       <c r="BU20" s="7">
         <v>881.69816045485391</v>
       </c>
       <c r="BV20" s="7">
-        <v>655.82410155198727</v>
+        <v>925.32410155198727</v>
       </c>
       <c r="BW20" s="7">
-        <v>456.26166090757056</v>
+        <v>726.22968562434437</v>
       </c>
       <c r="BX20" s="7">
         <v>233.033136642199</v>
       </c>
       <c r="BY20" s="7">
-        <v>11.161205334315355</v>
+        <v>94.553342049907997</v>
       </c>
       <c r="BZ20" s="7">
-        <v>72.668929664198913</v>
+        <v>72.668929664198686</v>
       </c>
       <c r="CA20" s="7">
         <v>0</v>
@@ -6842,10 +6850,10 @@
         <v>1313.5652016999986</v>
       </c>
       <c r="CL20" s="7">
-        <v>630.34169343293956</v>
+        <v>630.34070430249255</v>
       </c>
       <c r="CM20" s="7">
-        <v>235.66228423603752</v>
+        <v>308.5757220284122</v>
       </c>
       <c r="CN20" s="7">
         <v>108.87468735961011</v>
@@ -6866,22 +6874,22 @@
         <v>546.36173153243817</v>
       </c>
       <c r="CT20" s="7">
-        <v>575.29356614111475</v>
+        <v>579.39270970520738</v>
       </c>
       <c r="CU20" s="7">
-        <v>419.28881307776135</v>
+        <v>407.29657112946353</v>
       </c>
       <c r="CV20" s="7">
-        <v>239.94847886806411</v>
+        <v>239.94847886806406</v>
       </c>
       <c r="CW20" s="7">
-        <v>91.46460516265779</v>
+        <v>82.275696908221562</v>
       </c>
       <c r="CX20" s="7">
-        <v>0</v>
+        <v>191.29395612506028</v>
       </c>
       <c r="CY20" s="7">
-        <v>50.431118375746109</v>
+        <v>44.269253008386158</v>
       </c>
       <c r="CZ20" s="7">
         <v>0</v>
@@ -7464,7 +7472,7 @@
         <v>0</v>
       </c>
       <c r="CA22" s="7">
-        <v>3.5797625674899791</v>
+        <v>0</v>
       </c>
       <c r="CB22" s="7">
         <v>0</v>
@@ -7927,7 +7935,7 @@
         <v>4.6875</v>
       </c>
       <c r="M24" s="7">
-        <v>4.6875000000000009</v>
+        <v>4.6875</v>
       </c>
       <c r="N24" s="7">
         <v>4.6875</v>
@@ -14133,7 +14141,7 @@
         <v>1425</v>
       </c>
       <c r="Q43" s="7">
-        <v>1725</v>
+        <v>1712.5</v>
       </c>
       <c r="R43" s="7">
         <v>2000</v>
@@ -14142,19 +14150,19 @@
         <v>2300</v>
       </c>
       <c r="T43" s="7">
-        <v>2600</v>
+        <v>2587.5</v>
       </c>
       <c r="U43" s="7">
         <v>2875</v>
       </c>
       <c r="V43" s="7">
-        <v>3024.9999999999986</v>
+        <v>3037.5</v>
       </c>
       <c r="W43" s="7">
-        <v>3424.9999999999986</v>
+        <v>3425</v>
       </c>
       <c r="X43" s="7">
-        <v>3624.9999999999986</v>
+        <v>3625</v>
       </c>
       <c r="Y43" s="7">
         <v>3700</v>
@@ -14217,7 +14225,7 @@
         <v>1994.9999999999998</v>
       </c>
       <c r="AT43" s="7">
-        <v>2415</v>
+        <v>2397.5</v>
       </c>
       <c r="AU43" s="7">
         <v>2800</v>
@@ -14226,19 +14234,19 @@
         <v>3220</v>
       </c>
       <c r="AW43" s="7">
-        <v>3639.9999999999995</v>
+        <v>3622.4999999999995</v>
       </c>
       <c r="AX43" s="7">
         <v>4024.9999999999995</v>
       </c>
       <c r="AY43" s="7">
-        <v>4234.9999999999982</v>
+        <v>4252.5</v>
       </c>
       <c r="AZ43" s="7">
-        <v>4794.9999999999982</v>
+        <v>4795</v>
       </c>
       <c r="BA43" s="7">
-        <v>5074.9999999999982</v>
+        <v>5075</v>
       </c>
       <c r="BB43" s="7">
         <v>5180</v>
@@ -14298,7 +14306,7 @@
         <v>2850</v>
       </c>
       <c r="BV43" s="7">
-        <v>3450</v>
+        <v>3425</v>
       </c>
       <c r="BW43" s="7">
         <v>4000</v>
@@ -14307,19 +14315,19 @@
         <v>4600</v>
       </c>
       <c r="BY43" s="7">
-        <v>5200</v>
+        <v>5175</v>
       </c>
       <c r="BZ43" s="7">
         <v>5750</v>
       </c>
       <c r="CA43" s="7">
-        <v>6049.9999999999973</v>
+        <v>6075</v>
       </c>
       <c r="CB43" s="7">
-        <v>6849.9999999999973</v>
+        <v>6850</v>
       </c>
       <c r="CC43" s="7">
-        <v>7249.9999999999973</v>
+        <v>7250</v>
       </c>
       <c r="CD43" s="7">
         <v>7400</v>
@@ -14379,7 +14387,7 @@
         <v>1994.9999999999998</v>
       </c>
       <c r="CX43" s="7">
-        <v>2415</v>
+        <v>2397.5</v>
       </c>
       <c r="CY43" s="7">
         <v>2800</v>
@@ -14388,19 +14396,19 @@
         <v>3220</v>
       </c>
       <c r="DA43" s="7">
-        <v>3639.9999999999995</v>
+        <v>3622.4999999999995</v>
       </c>
       <c r="DB43" s="7">
         <v>4024.9999999999995</v>
       </c>
       <c r="DC43" s="7">
-        <v>4234.9999999999982</v>
+        <v>4252.5</v>
       </c>
       <c r="DD43" s="7">
-        <v>4794.9999999999982</v>
+        <v>4795</v>
       </c>
       <c r="DE43" s="7">
-        <v>5074.9999999999982</v>
+        <v>5075</v>
       </c>
       <c r="DF43" s="7">
         <v>5180</v>
@@ -15111,16 +15119,16 @@
         <v>2725.8506409987394</v>
       </c>
       <c r="N46" s="10">
-        <v>2659.8598214095409</v>
+        <v>2665.274586277551</v>
       </c>
       <c r="O46" s="10">
         <v>2536.5375086431031</v>
       </c>
       <c r="P46" s="10">
-        <v>2420.0592851396359</v>
+        <v>2429.4523913552785</v>
       </c>
       <c r="Q46" s="10">
-        <v>2304.1852508166094</v>
+        <v>2310.4352508166094</v>
       </c>
       <c r="R46" s="10">
         <v>2201.4256760832914</v>
@@ -15129,13 +15137,13 @@
         <v>2086.7910071595074</v>
       </c>
       <c r="T46" s="10">
-        <v>1972.7918674440184</v>
+        <v>1979.0418674440184</v>
       </c>
       <c r="U46" s="10">
         <v>1871.9390613333667</v>
       </c>
       <c r="V46" s="10">
-        <v>1834.243575692034</v>
+        <v>1827.9935756920333</v>
       </c>
       <c r="W46" s="10">
         <v>1781.3448323126013</v>
@@ -15180,10 +15188,10 @@
         <v>2700</v>
       </c>
       <c r="AL46" s="10">
-        <v>2759.7731136712237</v>
+        <v>2759.7731136712232</v>
       </c>
       <c r="AM46" s="10">
-        <v>2772.6886436340433</v>
+        <v>2772.6886436340446</v>
       </c>
       <c r="AN46" s="10">
         <v>2785.8366070579682</v>
@@ -15198,22 +15206,22 @@
         <v>2753.5202804016344</v>
       </c>
       <c r="AR46" s="10">
-        <v>2572.4179829380628</v>
+        <v>2578.9609055358319</v>
       </c>
       <c r="AS46" s="10">
         <v>2400.7400149976097</v>
       </c>
       <c r="AT46" s="10">
-        <v>2229.7478405821685</v>
+        <v>2238.4978405821685</v>
       </c>
       <c r="AU46" s="10">
         <v>2076.9531173748651</v>
       </c>
       <c r="AV46" s="10">
-        <v>1933.7438925686338</v>
+        <v>1933.7439183684837</v>
       </c>
       <c r="AW46" s="10">
-        <v>1757.6463992180213</v>
+        <v>1747.2536540575393</v>
       </c>
       <c r="AX46" s="10">
         <v>1651.9577570903407</v>
@@ -15225,7 +15233,7 @@
         <v>1608.9626816714008</v>
       </c>
       <c r="BA46" s="10">
-        <v>1516.1294730159248</v>
+        <v>1516.1294730159227</v>
       </c>
       <c r="BB46" s="10">
         <v>1438.4568633221947</v>
@@ -15252,7 +15260,7 @@
         <v>1500</v>
       </c>
       <c r="BK46" s="10">
-        <v>2100</v>
+        <v>1793.7145671024514</v>
       </c>
       <c r="BL46" s="10">
         <v>2700</v>
@@ -15279,34 +15287,34 @@
         <v>3000</v>
       </c>
       <c r="BT46" s="10">
-        <v>2843.475996551997</v>
+        <v>2837.0041926781087</v>
       </c>
       <c r="BU46" s="10">
         <v>2585.561690303236</v>
       </c>
       <c r="BV46" s="10">
-        <v>2334.9789843679914</v>
+        <v>2347.478984367991</v>
       </c>
       <c r="BW46" s="10">
-        <v>2110.2706906050466</v>
+        <v>2123.2387153218201</v>
       </c>
       <c r="BX46" s="10">
         <v>1861.4516744281325</v>
       </c>
       <c r="BY46" s="10">
-        <v>1613.5370535562099</v>
+        <v>1626.0370535562099</v>
       </c>
       <c r="BZ46" s="10">
-        <v>1391.5422031094658</v>
+        <v>1391.5422031094656</v>
       </c>
       <c r="CA46" s="10">
-        <v>1295.4827583783267</v>
+        <v>1291.902995810837</v>
       </c>
       <c r="CB46" s="10">
         <v>1264.4570641666219</v>
       </c>
       <c r="CC46" s="10">
-        <v>1092.9405380277312</v>
+        <v>1092.9405380277285</v>
       </c>
       <c r="CD46" s="10">
         <v>963.89255746587992</v>
@@ -15315,7 +15323,7 @@
         <v>934.65852931666359</v>
       </c>
       <c r="CF46" s="11">
-        <v>869.31250546304568</v>
+        <v>869.31250546304545</v>
       </c>
       <c r="CH46">
         <v>44</v>
@@ -15333,19 +15341,19 @@
         <v>1500</v>
       </c>
       <c r="CM46" s="10">
-        <v>2100</v>
+        <v>2027.0865622076253</v>
       </c>
       <c r="CN46" s="10">
         <v>2301.0127082397403</v>
       </c>
       <c r="CO46" s="10">
-        <v>2679.7042695301107</v>
+        <v>2679.7042695301097</v>
       </c>
       <c r="CP46" s="10">
         <v>2691.2457596605427</v>
       </c>
       <c r="CQ46" s="10">
-        <v>2702.9963246051816</v>
+        <v>2702.996324605183</v>
       </c>
       <c r="CR46" s="10">
         <v>2714.9595186056149</v>
@@ -15357,37 +15365,37 @@
         <v>2739.5383140604777</v>
       </c>
       <c r="CU46" s="10">
-        <v>2566.7028727012735</v>
+        <v>2554.7106307529757</v>
       </c>
       <c r="CV46" s="10">
         <v>2370.2285692453761</v>
       </c>
       <c r="CW46" s="10">
-        <v>2204.302289526584</v>
+        <v>2195.1133812721478</v>
       </c>
       <c r="CX46" s="10">
-        <v>2071.7035080701426</v>
+        <v>2029.3755540833733</v>
       </c>
       <c r="CY46" s="10">
-        <v>1870.4376173729506</v>
+        <v>1864.2757520055907</v>
       </c>
       <c r="CZ46" s="10">
         <v>1801.6069640637572</v>
       </c>
       <c r="DA46" s="10">
-        <v>1843.5332945071179</v>
+        <v>1782.8774777464412</v>
       </c>
       <c r="DB46" s="10">
-        <v>1681.5153466413476</v>
+        <v>1681.5153466413474</v>
       </c>
       <c r="DC46" s="10">
-        <v>1568.5469064492499</v>
+        <v>1551.0469064492481</v>
       </c>
       <c r="DD46" s="10">
-        <v>1107.3137992238876</v>
+        <v>1107.3137992238856</v>
       </c>
       <c r="DE46" s="10">
-        <v>927.84552562569343</v>
+        <v>927.84552562569138</v>
       </c>
       <c r="DF46" s="10">
         <v>840.17208882632758</v>
@@ -16166,7 +16174,7 @@
         <v>0</v>
       </c>
       <c r="AF51" s="7">
-        <v>665.6</v>
+        <v>0</v>
       </c>
       <c r="AG51" s="7">
         <v>665.6</v>
@@ -16316,7 +16324,7 @@
         <v>0</v>
       </c>
       <c r="CE51" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="CF51" s="8">
         <v>0</v>
@@ -16743,7 +16751,7 @@
         <v>212</v>
       </c>
       <c r="E53" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F53" s="7">
         <v>0</v>
@@ -16968,7 +16976,7 @@
         <v>104.42657567209426</v>
       </c>
       <c r="CE53" s="7">
-        <v>122.49086716321972</v>
+        <v>122.49186716321992</v>
       </c>
       <c r="CF53" s="8">
         <v>0</v>
@@ -16986,7 +16994,7 @@
         <v>212</v>
       </c>
       <c r="CL53" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="CM53" s="7">
         <v>0</v>
@@ -18370,7 +18378,7 @@
         <v>0</v>
       </c>
       <c r="D58" s="7">
-        <v>650</v>
+        <v>195.38963750666881</v>
       </c>
       <c r="E58" s="7">
         <v>0</v>
@@ -18385,7 +18393,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="J58" s="7">
         <v>650</v>
@@ -18532,7 +18540,7 @@
         <v>0</v>
       </c>
       <c r="BI58" s="7">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="BJ58" s="7">
         <v>0</v>
@@ -18613,7 +18621,7 @@
         <v>0</v>
       </c>
       <c r="CK58" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="CL58" s="7">
         <v>0</v>
@@ -18628,7 +18636,7 @@
         <v>0</v>
       </c>
       <c r="CP58" s="7">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="CQ58" s="7">
         <v>650</v>
@@ -19414,7 +19422,7 @@
         <v>0</v>
       </c>
       <c r="Z61" s="7">
-        <v>36.81637794793366</v>
+        <v>36.816377947933688</v>
       </c>
       <c r="AA61" s="8">
         <v>118.95676867291331</v>
@@ -19657,7 +19665,7 @@
         <v>32.456580825592482</v>
       </c>
       <c r="DG61" s="7">
-        <v>84.927308397533579</v>
+        <v>84.926611429303648</v>
       </c>
       <c r="DH61" s="8">
         <v>150</v>
@@ -19683,13 +19691,13 @@
         <v>1848</v>
       </c>
       <c r="G62" s="7">
-        <v>1507.8334695934477</v>
+        <v>1507.8334695934523</v>
       </c>
       <c r="H62" s="7">
         <v>843.62353909047397</v>
       </c>
       <c r="I62" s="7">
-        <v>226.14200191641203</v>
+        <v>876.14200191641203</v>
       </c>
       <c r="J62" s="7">
         <v>259.25617688369084</v>
@@ -19731,7 +19739,7 @@
         <v>0</v>
       </c>
       <c r="W62" s="7">
-        <v>562.80212731970596</v>
+        <v>0</v>
       </c>
       <c r="X62" s="7">
         <v>0</v>
@@ -19806,13 +19814,13 @@
         <v>658.90570033500353</v>
       </c>
       <c r="AX62" s="7">
-        <v>630.00327112130526</v>
+        <v>703.01073898169852</v>
       </c>
       <c r="AY62" s="7">
-        <v>602.57618465871178</v>
+        <v>723.08859441316645</v>
       </c>
       <c r="AZ62" s="7">
-        <v>137.51234252141876</v>
+        <v>403.4297728181939</v>
       </c>
       <c r="BA62" s="7">
         <v>0</v>
@@ -19875,7 +19883,7 @@
         <v>1097.2810413117072</v>
       </c>
       <c r="BV62" s="7">
-        <v>1148.6668678635051</v>
+        <v>1146.7612737379552</v>
       </c>
       <c r="BW62" s="7">
         <v>1200.9691511831847</v>
@@ -19932,7 +19940,7 @@
         <v>873.49727116714757</v>
       </c>
       <c r="CP62" s="7">
-        <v>906.52358743838886</v>
+        <v>256.52358743838886</v>
       </c>
       <c r="CQ62" s="7">
         <v>290.15424935954115</v>
@@ -19968,13 +19976,13 @@
         <v>476.04898211267027</v>
       </c>
       <c r="DB62" s="7">
-        <v>517.04545654958565</v>
+        <v>444.83154812245971</v>
       </c>
       <c r="DC62" s="7">
         <v>0</v>
       </c>
       <c r="DD62" s="7">
-        <v>313.73022150077236</v>
+        <v>601.27049651999141</v>
       </c>
       <c r="DE62" s="7">
         <v>0</v>
@@ -20057,7 +20065,7 @@
         <v>520.95643032173666</v>
       </c>
       <c r="W63" s="7">
-        <v>0</v>
+        <v>562.80212731970596</v>
       </c>
       <c r="X63" s="7">
         <v>605.40209939164106</v>
@@ -20132,13 +20140,13 @@
         <v>0</v>
       </c>
       <c r="AX63" s="7">
-        <v>73.007467860393263</v>
+        <v>0</v>
       </c>
       <c r="AY63" s="7">
-        <v>145.33227634317495</v>
+        <v>24.819866588720288</v>
       </c>
       <c r="AZ63" s="7">
-        <v>656.1</v>
+        <v>390.18256970322477</v>
       </c>
       <c r="BA63" s="7">
         <v>656.1</v>
@@ -20201,7 +20209,7 @@
         <v>0</v>
       </c>
       <c r="BV63" s="7">
-        <v>0</v>
+        <v>1.9055941255498965</v>
       </c>
       <c r="BW63" s="7">
         <v>0</v>
@@ -20294,13 +20302,13 @@
         <v>0</v>
       </c>
       <c r="DB63" s="7">
-        <v>0</v>
+        <v>72.213908427125943</v>
       </c>
       <c r="DC63" s="7">
         <v>558.78176876842826</v>
       </c>
       <c r="DD63" s="7">
-        <v>287.54027501921905</v>
+        <v>0</v>
       </c>
       <c r="DE63" s="7">
         <v>644.52443086833136</v>
@@ -20551,7 +20559,7 @@
         <v>0</v>
       </c>
       <c r="CD64" s="7">
-        <v>37.205249857870967</v>
+        <v>37.205249857864601</v>
       </c>
       <c r="CE64" s="7">
         <v>50.3</v>
@@ -20913,7 +20921,7 @@
         <v>0</v>
       </c>
       <c r="CQ65" s="7">
-        <v>12.31919338234502</v>
+        <v>12.31719338238122</v>
       </c>
       <c r="CR65" s="7">
         <v>67</v>
@@ -20987,7 +20995,7 @@
         <v>257</v>
       </c>
       <c r="G66" s="7">
-        <v>160.11226184324525</v>
+        <v>160.11226184324315</v>
       </c>
       <c r="H66" s="7">
         <v>257</v>
@@ -21008,7 +21016,7 @@
         <v>257</v>
       </c>
       <c r="N66" s="7">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="O66" s="7">
         <v>257</v>
@@ -21017,7 +21025,7 @@
         <v>0</v>
       </c>
       <c r="Q66" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="R66" s="7">
         <v>0</v>
@@ -21089,7 +21097,7 @@
         <v>257</v>
       </c>
       <c r="AQ66" s="7">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="AR66" s="7">
         <v>257</v>
@@ -21098,7 +21106,7 @@
         <v>0</v>
       </c>
       <c r="AT66" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="AU66" s="7">
         <v>0</v>
@@ -21179,7 +21187,7 @@
         <v>257</v>
       </c>
       <c r="BV66" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="BW66" s="7">
         <v>0</v>
@@ -21260,7 +21268,7 @@
         <v>0</v>
       </c>
       <c r="CX66" s="7">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="CY66" s="7">
         <v>0</v>
@@ -21304,10 +21312,10 @@
         <v>712.04830049999941</v>
       </c>
       <c r="D67" s="7">
-        <v>121.42026469999939</v>
+        <v>576.03062719333059</v>
       </c>
       <c r="E67" s="7">
-        <v>209.48634873799847</v>
+        <v>209.48734873799833</v>
       </c>
       <c r="F67" s="7">
         <v>0</v>
@@ -21334,7 +21342,7 @@
         <v>324.59257631386413</v>
       </c>
       <c r="N67" s="7">
-        <v>606.51259775453968</v>
+        <v>349.51259775453968</v>
       </c>
       <c r="O67" s="7">
         <v>374.88628824601665</v>
@@ -21343,7 +21351,7 @@
         <v>657.72136023334906</v>
       </c>
       <c r="Q67" s="7">
-        <v>427.02565755196565</v>
+        <v>684.02565755196565</v>
       </c>
       <c r="R67" s="7">
         <v>710.80715632654938</v>
@@ -21364,13 +21372,13 @@
         <v>852.16148912379413</v>
       </c>
       <c r="X67" s="7">
-        <v>823.15366359381142</v>
+        <v>881.98146957414883</v>
       </c>
       <c r="Y67" s="7">
         <v>378.73841879965858</v>
       </c>
       <c r="Z67" s="7">
-        <v>199.64146456355232</v>
+        <v>199.64146456355229</v>
       </c>
       <c r="AA67" s="8">
         <v>0</v>
@@ -21382,7 +21390,7 @@
         <v>1939.9531502299997</v>
       </c>
       <c r="AF67" s="7">
-        <v>1041.5563004999992</v>
+        <v>1707.1563004999991</v>
       </c>
       <c r="AG67" s="7">
         <v>456.52990069999908</v>
@@ -21415,7 +21423,7 @@
         <v>461.09599764724317</v>
       </c>
       <c r="AQ67" s="7">
-        <v>745.33657725058629</v>
+        <v>488.33657725058629</v>
       </c>
       <c r="AR67" s="7">
         <v>516.07027539349656</v>
@@ -21424,7 +21432,7 @@
         <v>801.30547516233537</v>
       </c>
       <c r="AT67" s="7">
-        <v>573.05070243474529</v>
+        <v>830.05070243474529</v>
       </c>
       <c r="AU67" s="7">
         <v>859.31462697233565</v>
@@ -21466,13 +21474,13 @@
         <v>2269.6</v>
       </c>
       <c r="BI67" s="7">
-        <v>1448.4130516999981</v>
+        <v>2098.4130516999981</v>
       </c>
       <c r="BJ67" s="7">
         <v>1559.039013116997</v>
       </c>
       <c r="BK67" s="7">
-        <v>1043.5622123246862</v>
+        <v>1043.5622123246858</v>
       </c>
       <c r="BL67" s="7">
         <v>570.52486147930335</v>
@@ -21505,7 +21513,7 @@
         <v>969.29672891819473</v>
       </c>
       <c r="BV67" s="7">
-        <v>1005.2668075044535</v>
+        <v>1262.2668075044535</v>
       </c>
       <c r="BW67" s="7">
         <v>1298.8784058282295</v>
@@ -21526,10 +21534,10 @@
         <v>1491.9474591011362</v>
       </c>
       <c r="CC67" s="7">
-        <v>1532.6438010411057</v>
+        <v>1475.0948604081846</v>
       </c>
       <c r="CD67" s="7">
-        <v>1053.5567600436825</v>
+        <v>1053.5567600436889</v>
       </c>
       <c r="CE67" s="7">
         <v>872.61435671417939</v>
@@ -21547,13 +21555,13 @@
         <v>1432.5663004999997</v>
       </c>
       <c r="CK67" s="7">
-        <v>827.27187069999889</v>
+        <v>177.271870699999</v>
       </c>
       <c r="CL67" s="7">
-        <v>266.28743203999909</v>
+        <v>266.28843203999907</v>
       </c>
       <c r="CM67" s="7">
-        <v>758.39774137984477</v>
+        <v>0</v>
       </c>
       <c r="CN67" s="7">
         <v>0</v>
@@ -21565,7 +21573,7 @@
         <v>317.56651120687206</v>
       </c>
       <c r="CQ67" s="7">
-        <v>328.78878116933356</v>
+        <v>328.79078116929736</v>
       </c>
       <c r="CR67" s="7">
         <v>298.07967149406204</v>
@@ -21586,7 +21594,7 @@
         <v>681.65204605484678</v>
       </c>
       <c r="CX67" s="7">
-        <v>451.36316503242915</v>
+        <v>708.36316503242915</v>
       </c>
       <c r="CY67" s="7">
         <v>735.55840143418027</v>
@@ -21613,7 +21621,7 @@
         <v>406.58960657791476</v>
       </c>
       <c r="DG67" s="7">
-        <v>224.14255585958608</v>
+        <v>224.14290434370105</v>
       </c>
       <c r="DH67" s="8">
         <v>33.860402318144679</v>
@@ -22016,7 +22024,7 @@
         <v>0</v>
       </c>
       <c r="X69" s="7">
-        <v>58.827805980337416</v>
+        <v>0</v>
       </c>
       <c r="Y69" s="7">
         <v>398.3</v>
@@ -22178,7 +22186,7 @@
         <v>0</v>
       </c>
       <c r="CC69" s="7">
-        <v>0</v>
+        <v>57.548940632921131</v>
       </c>
       <c r="CD69" s="7">
         <v>398.3</v>
@@ -29798,7 +29806,7 @@
         <v>1771.068169651244</v>
       </c>
       <c r="G93" s="10">
-        <v>2270.8359296299222</v>
+        <v>2270.83592962992</v>
       </c>
       <c r="H93" s="10">
         <v>2628.4870617271422</v>
@@ -29930,7 +29938,7 @@
         <v>2850.5725383005661</v>
       </c>
       <c r="AZ93" s="10">
-        <v>2864.2837027564251</v>
+        <v>2864.2837027564256</v>
       </c>
       <c r="BA93" s="10">
         <v>2878.2408264755345</v>
@@ -30041,7 +30049,7 @@
         <v>1500</v>
       </c>
       <c r="CM93" s="10">
-        <v>1070.437129989534</v>
+        <v>1828.834871369379</v>
       </c>
       <c r="CN93" s="10">
         <v>2124.2521586855833</v>
@@ -30056,7 +30064,7 @@
         <v>2657.4462748078622</v>
       </c>
       <c r="CR93" s="10">
-        <v>2667.7198592117406</v>
+        <v>2667.7198592117411</v>
       </c>
       <c r="CS93" s="10">
         <v>2678.1809640174752</v>
@@ -30101,7 +30109,7 @@
         <v>2832.7669742476778</v>
       </c>
       <c r="DG93" s="10">
-        <v>2842.3904858401352</v>
+        <v>2842.3908343242501</v>
       </c>
       <c r="DH93" s="11">
         <v>2846.3569348787632</v>
@@ -30143,16 +30151,16 @@
         <v>-126.82179913983335</v>
       </c>
       <c r="C97" s="4">
-        <v>-17.574481608333329</v>
+        <v>125.6647609521107</v>
       </c>
       <c r="D97" s="4">
-        <v>71.272688897223404</v>
+        <v>-4.4957048516666589</v>
       </c>
       <c r="E97" s="4">
         <v>427.66035402863315</v>
       </c>
       <c r="F97" s="4">
-        <v>635.8294754953348</v>
+        <v>635.82947549533469</v>
       </c>
       <c r="G97" s="4">
         <v>694.9597820515869</v>
@@ -30176,16 +30184,16 @@
         <v>1100</v>
       </c>
       <c r="N97" s="4">
-        <v>1021.8803571309633</v>
+        <v>1027.2951219989732</v>
       </c>
       <c r="O97" s="4">
         <v>886.21016165193942</v>
       </c>
       <c r="P97" s="4">
-        <v>757.16127196227239</v>
+        <v>766.5543781779154</v>
       </c>
       <c r="Q97" s="4">
-        <v>628.4900005103807</v>
+        <v>634.7400005103807</v>
       </c>
       <c r="R97" s="4">
         <v>512.70276630205717</v>
@@ -30194,13 +30202,13 @@
         <v>384.80609822469205</v>
       </c>
       <c r="T97" s="4">
-        <v>257.30663590251152</v>
+        <v>263.55663590251152</v>
       </c>
       <c r="U97" s="4">
         <v>142.71113208335419</v>
       </c>
       <c r="V97" s="4">
-        <v>91.02645355752162</v>
+        <v>84.776453557520938</v>
       </c>
       <c r="W97" s="4">
         <v>23.887831547051945</v>
@@ -30224,10 +30232,10 @@
         <v>33.960167603499826</v>
       </c>
       <c r="AF97" s="4">
-        <v>98.873186841558663</v>
+        <v>68.14133522499958</v>
       </c>
       <c r="AG97" s="4">
-        <v>281.64667916499991</v>
+        <v>281.64667916499997</v>
       </c>
       <c r="AH97" s="4">
         <v>498.29918107358316</v>
@@ -30260,22 +30268,22 @@
         <v>1026.8053315010218</v>
       </c>
       <c r="AR97" s="4">
-        <v>831.58514558628917</v>
+        <v>838.12806818405852</v>
       </c>
       <c r="AS97" s="4">
         <v>645.53641562350617</v>
       </c>
       <c r="AT97" s="4">
-        <v>459.91630661385517</v>
+        <v>468.66630661385523</v>
       </c>
       <c r="AU97" s="4">
         <v>292.23210460929073</v>
       </c>
       <c r="AV97" s="4">
-        <v>133.8674103987446</v>
+        <v>133.86743619859465</v>
       </c>
       <c r="AW97" s="4">
-        <v>-57.656064803555864</v>
+        <v>-68.0488099640379</v>
       </c>
       <c r="AX97" s="4">
         <v>-179.0458000919034</v>
@@ -30287,7 +30295,7 @@
         <v>-254.28718207504801</v>
       </c>
       <c r="BA97" s="4">
-        <v>-362.42182047616683</v>
+        <v>-362.42182047616825</v>
       </c>
       <c r="BB97" s="4">
         <v>-410.20782817167901</v>
@@ -30311,10 +30319,10 @@
         <v>232.31378818166618</v>
       </c>
       <c r="BJ97" s="4">
-        <v>717.33238106889996</v>
+        <v>717.33238106889985</v>
       </c>
       <c r="BK97" s="4">
-        <v>858.53994949528601</v>
+        <v>756.44480519610318</v>
       </c>
       <c r="BL97" s="4">
         <v>1070.6260561820245</v>
@@ -30341,34 +30349,34 @@
         <v>1100</v>
       </c>
       <c r="BT97" s="4">
-        <v>876.86083054770643</v>
+        <v>870.38902667381785</v>
       </c>
       <c r="BU97" s="4">
         <v>600.73746268952232</v>
       </c>
       <c r="BV97" s="4">
-        <v>331.62327147999468</v>
+        <v>344.12327147999463</v>
       </c>
       <c r="BW97" s="4">
-        <v>88.055587878154086</v>
+        <v>101.02361259492784</v>
       </c>
       <c r="BX97" s="4">
         <v>-179.95629723241723</v>
       </c>
       <c r="BY97" s="4">
-        <v>-447.4029352773689</v>
+        <v>-434.9029352773689</v>
       </c>
       <c r="BZ97" s="4">
-        <v>-689.27471680658391</v>
+        <v>-689.27471680658414</v>
       </c>
       <c r="CA97" s="4">
-        <v>-805.56186976354502</v>
+        <v>-809.14163233103523</v>
       </c>
       <c r="CB97" s="4">
         <v>-857.17201270841224</v>
       </c>
       <c r="CC97" s="4">
-        <v>-1024.1068412208538</v>
+        <v>-1024.1068412208556</v>
       </c>
       <c r="CD97" s="4">
         <v>-1100</v>
@@ -30392,10 +30400,10 @@
         <v>232.65585686499998</v>
       </c>
       <c r="CL97" s="4">
-        <v>492.61570687250298</v>
+        <v>492.61603658265204</v>
       </c>
       <c r="CM97" s="4">
-        <v>656.98051649420449</v>
+        <v>632.6760372300796</v>
       </c>
       <c r="CN97" s="4">
         <v>732.64434889983772</v>
@@ -30419,37 +30427,37 @@
         <v>1100</v>
       </c>
       <c r="CU97" s="4">
-        <v>914.54154241890762</v>
+        <v>902.54930047060975</v>
       </c>
       <c r="CV97" s="4">
         <v>705.21676202836011</v>
       </c>
       <c r="CW97" s="4">
-        <v>526.20867779952869</v>
+        <v>517.01976954509246</v>
       </c>
       <c r="CX97" s="4">
-        <v>380.29283153887786</v>
+        <v>337.96487755210842</v>
       </c>
       <c r="CY97" s="4">
-        <v>165.47061662085412</v>
+        <v>159.30875125349417</v>
       </c>
       <c r="CZ97" s="4">
         <v>82.840312111575258</v>
       </c>
       <c r="DA97" s="4">
-        <v>110.71952781694881</v>
+        <v>50.063711056271956</v>
       </c>
       <c r="DB97" s="4">
-        <v>-60.498177344726926</v>
+        <v>-60.498177344727083</v>
       </c>
       <c r="DC97" s="4">
-        <v>-156.83397543117044</v>
+        <v>-168.50064209783841</v>
       </c>
       <c r="DD97" s="4">
-        <v>-485.72220701591698</v>
+        <v>-485.72220701591823</v>
       </c>
       <c r="DE97" s="4">
-        <v>-627.14959680177094</v>
+        <v>-627.14959680177208</v>
       </c>
       <c r="DF97" s="4">
         <v>-679.43597669481937</v>
@@ -30469,16 +30477,16 @@
         <v>-375.29837425483316</v>
       </c>
       <c r="C98" s="7">
-        <v>-268.68563185833318</v>
+        <v>-125.44638929788917</v>
       </c>
       <c r="D98" s="7">
-        <v>209.09017130055344</v>
+        <v>360.62695879833359</v>
       </c>
       <c r="E98" s="7">
         <v>108.39990819163393</v>
       </c>
       <c r="F98" s="7">
-        <v>281.55850908675694</v>
+        <v>281.55850908675689</v>
       </c>
       <c r="G98" s="7">
         <v>305.0402179484131</v>
@@ -30502,31 +30510,31 @@
         <v>-100</v>
       </c>
       <c r="N98" s="7">
-        <v>-21.880357130963262</v>
+        <v>-27.295121998973173</v>
       </c>
       <c r="O98" s="7">
         <v>113.78983834806053</v>
       </c>
       <c r="P98" s="7">
-        <v>242.83872803772755</v>
+        <v>233.4456218220846</v>
       </c>
       <c r="Q98" s="7">
-        <v>371.5099994896193</v>
+        <v>365.2599994896193</v>
       </c>
       <c r="R98" s="7">
-        <v>487.29723369794283</v>
+        <v>487.29723369794277</v>
       </c>
       <c r="S98" s="7">
         <v>615.19390177530795</v>
       </c>
       <c r="T98" s="7">
-        <v>742.69336409748848</v>
+        <v>736.44336409748848</v>
       </c>
       <c r="U98" s="7">
         <v>857.28886791664581</v>
       </c>
       <c r="V98" s="7">
-        <v>908.97354644247844</v>
+        <v>915.22354644247912</v>
       </c>
       <c r="W98" s="7">
         <v>976.11216845294803</v>
@@ -30550,7 +30558,7 @@
         <v>-455.28140751149999</v>
       </c>
       <c r="AF98" s="7">
-        <v>-428.34746340844083</v>
+        <v>-459.07931502499991</v>
       </c>
       <c r="AG98" s="7">
         <v>-284.2415886849995</v>
@@ -30586,22 +30594,22 @@
         <v>-26.805331501021783</v>
       </c>
       <c r="AR98" s="7">
-        <v>168.41485441371077</v>
+        <v>161.87193181594148</v>
       </c>
       <c r="AS98" s="7">
-        <v>354.46358437649383</v>
+        <v>354.46358437649388</v>
       </c>
       <c r="AT98" s="7">
-        <v>540.08369338614489</v>
+        <v>531.33369338614477</v>
       </c>
       <c r="AU98" s="7">
         <v>707.76789539070933</v>
       </c>
       <c r="AV98" s="7">
-        <v>866.1325896012554</v>
+        <v>866.13256380140535</v>
       </c>
       <c r="AW98" s="7">
-        <v>1057.6560648035559</v>
+        <v>1068.0488099640379</v>
       </c>
       <c r="AX98" s="7">
         <v>1179.0458000919034</v>
@@ -30613,7 +30621,7 @@
         <v>1254.2871820750479</v>
       </c>
       <c r="BA98" s="7">
-        <v>1361.1684430158703</v>
+        <v>1361.1684430158707</v>
       </c>
       <c r="BB98" s="7">
         <v>1362.2187401672236</v>
@@ -30637,16 +30645,16 @@
         <v>-308.80218016833334</v>
       </c>
       <c r="BJ98" s="7">
-        <v>-523.78032351209959</v>
+        <v>-523.78032351209936</v>
       </c>
       <c r="BK98" s="7">
-        <v>-433.46233405593978</v>
+        <v>-535.55747835512273</v>
       </c>
       <c r="BL98" s="7">
         <v>-273.17382745522224</v>
       </c>
       <c r="BM98" s="7">
-        <v>-266.25927801120724</v>
+        <v>-266.25927801120736</v>
       </c>
       <c r="BN98" s="7">
         <v>-100</v>
@@ -30667,34 +30675,34 @@
         <v>-100</v>
       </c>
       <c r="BT98" s="7">
-        <v>123.13916945229357</v>
+        <v>129.61097332618209</v>
       </c>
       <c r="BU98" s="7">
-        <v>399.26253731047768</v>
+        <v>399.26253731047763</v>
       </c>
       <c r="BV98" s="7">
-        <v>668.37672852000537</v>
+        <v>655.87672852000537</v>
       </c>
       <c r="BW98" s="7">
-        <v>911.94441212184597</v>
+        <v>898.97638740507216</v>
       </c>
       <c r="BX98" s="7">
         <v>1179.9562972324172</v>
       </c>
       <c r="BY98" s="7">
-        <v>1447.4029352773689</v>
+        <v>1434.9029352773689</v>
       </c>
       <c r="BZ98" s="7">
-        <v>1689.2747168065839</v>
+        <v>1689.2747168065841</v>
       </c>
       <c r="CA98" s="7">
-        <v>1805.561869763545</v>
+        <v>1809.141632331035</v>
       </c>
       <c r="CB98" s="7">
         <v>1857.1720127084122</v>
       </c>
       <c r="CC98" s="7">
-        <v>1998.5778897652795</v>
+        <v>1998.5778897652804</v>
       </c>
       <c r="CD98" s="7">
         <v>2000</v>
@@ -30703,7 +30711,7 @@
         <v>1935.9086568675002</v>
       </c>
       <c r="CF98" s="8">
-        <v>1857.7176247268478</v>
+        <v>1857.7176247268476</v>
       </c>
       <c r="CH98" t="s">
         <v>2</v>
@@ -30715,13 +30723,13 @@
         <v>-96.317315191666239</v>
       </c>
       <c r="CK98" s="7">
-        <v>-123.27174398499963</v>
+        <v>-123.27174398499966</v>
       </c>
       <c r="CL98" s="7">
-        <v>100.88957203900338</v>
+        <v>100.88990174915244</v>
       </c>
       <c r="CM98" s="7">
-        <v>228.80437437618548</v>
+        <v>204.49989511206059</v>
       </c>
       <c r="CN98" s="7">
         <v>267.35565110016228</v>
@@ -30745,37 +30753,37 @@
         <v>-100</v>
       </c>
       <c r="CU98" s="7">
-        <v>85.458457581092375</v>
+        <v>97.450699529390192</v>
       </c>
       <c r="CV98" s="7">
-        <v>294.78323797163983</v>
+        <v>294.78323797163989</v>
       </c>
       <c r="CW98" s="7">
-        <v>473.79132220047131</v>
+        <v>482.98023045490754</v>
       </c>
       <c r="CX98" s="7">
-        <v>619.70716846112214</v>
+        <v>662.03512244789158</v>
       </c>
       <c r="CY98" s="7">
-        <v>834.52938337914588</v>
+        <v>840.69124874650583</v>
       </c>
       <c r="CZ98" s="7">
         <v>917.15968788842474</v>
       </c>
       <c r="DA98" s="7">
-        <v>889.28047218305119</v>
+        <v>949.93628894372796</v>
       </c>
       <c r="DB98" s="7">
-        <v>1055.3991493345995</v>
+        <v>1055.3991493345993</v>
       </c>
       <c r="DC98" s="7">
-        <v>1120.5475713442038</v>
+        <v>1126.3809046775377</v>
       </c>
       <c r="DD98" s="7">
-        <v>1302.2758933721386</v>
+        <v>1302.2758933721393</v>
       </c>
       <c r="DE98" s="7">
-        <v>1390.5826403853816</v>
+        <v>1390.5826403853825</v>
       </c>
       <c r="DF98" s="7">
         <v>1392.132978892017</v>
@@ -30795,10 +30803,10 @@
         <v>502.12017339466655</v>
       </c>
       <c r="C99" s="10">
-        <v>286.26011346666655</v>
+        <v>-0.21837165422152793</v>
       </c>
       <c r="D99" s="10">
-        <v>-280.36286019777685</v>
+        <v>-356.13125394666696</v>
       </c>
       <c r="E99" s="10">
         <v>-536.06026222026708</v>
@@ -30873,13 +30881,13 @@
         <v>3</v>
       </c>
       <c r="AE99" s="9">
-        <v>421.32123990800005</v>
+        <v>421.32123990800011</v>
       </c>
       <c r="AF99" s="10">
-        <v>329.47427656688217</v>
+        <v>390.93797980000033</v>
       </c>
       <c r="AG99" s="10">
-        <v>2.5949095199995327</v>
+        <v>2.5949095199995704</v>
       </c>
       <c r="AH99" s="10">
         <v>-391.34222897466719</v>
@@ -30939,7 +30947,7 @@
         <v>-1000</v>
       </c>
       <c r="BA99" s="10">
-        <v>-998.74662253970337</v>
+        <v>-998.74662253970268</v>
       </c>
       <c r="BB99" s="10">
         <v>-952.01091199554457</v>
@@ -30954,7 +30962,7 @@
         <v>3</v>
       </c>
       <c r="BG99" s="9">
-        <v>-43.747710015333439</v>
+        <v>-43.747710015333382</v>
       </c>
       <c r="BH99" s="10">
         <v>104.4848799666668</v>
@@ -30963,16 +30971,16 @@
         <v>76.488391986667182</v>
       </c>
       <c r="BJ99" s="10">
-        <v>-193.55205755680032</v>
+        <v>-193.55205755680049</v>
       </c>
       <c r="BK99" s="10">
-        <v>-425.07761543934635</v>
+        <v>-220.88732684098045</v>
       </c>
       <c r="BL99" s="10">
         <v>-797.45222872680188</v>
       </c>
       <c r="BM99" s="10">
-        <v>-833.74072198879276</v>
+        <v>-833.74072198879264</v>
       </c>
       <c r="BN99" s="10">
         <v>-1000</v>
@@ -31020,7 +31028,7 @@
         <v>-1000</v>
       </c>
       <c r="CC99" s="10">
-        <v>-974.47104854442568</v>
+        <v>-974.47104854442478</v>
       </c>
       <c r="CD99" s="10">
         <v>-900</v>
@@ -31041,13 +31049,13 @@
         <v>-128.13501986666699</v>
       </c>
       <c r="CK99" s="10">
-        <v>-109.38411288000037</v>
+        <v>-109.38411288000034</v>
       </c>
       <c r="CL99" s="10">
-        <v>-593.50527891150637</v>
+        <v>-593.50593833180449</v>
       </c>
       <c r="CM99" s="10">
-        <v>-885.78489087038997</v>
+        <v>-837.17593234214019</v>
       </c>
       <c r="CN99" s="10">
         <v>-1000</v>
@@ -31095,13 +31103,13 @@
         <v>-994.90097198987246</v>
       </c>
       <c r="DC99" s="10">
-        <v>-963.71359591303326</v>
+        <v>-957.88026257969932</v>
       </c>
       <c r="DD99" s="10">
-        <v>-816.55368635622176</v>
+        <v>-816.55368635622108</v>
       </c>
       <c r="DE99" s="10">
-        <v>-763.43304358361092</v>
+        <v>-763.43304358361002</v>
       </c>
       <c r="DF99" s="10">
         <v>-712.69700219719789</v>
@@ -31152,16 +31160,16 @@
         <v>145.64563505833328</v>
       </c>
       <c r="D103" s="4">
-        <v>-64.094302451666692</v>
+        <v>87.442485046110392</v>
       </c>
       <c r="E103" s="4">
-        <v>367.09385735276658</v>
+        <v>367.09352401943323</v>
       </c>
       <c r="F103" s="4">
         <v>464.63400967639319</v>
       </c>
       <c r="G103" s="4">
-        <v>751.92868046992999</v>
+        <v>751.92868046992783</v>
       </c>
       <c r="H103" s="4">
         <v>1100</v>
@@ -31230,7 +31238,7 @@
         <v>-144.08879913983333</v>
       </c>
       <c r="AF103" s="4">
-        <v>184.08823505833331</v>
+        <v>-37.778431608333378</v>
       </c>
       <c r="AG103" s="4">
         <v>-24.998178251666701</v>
@@ -31314,13 +31322,13 @@
         <v>213.62668522499956</v>
       </c>
       <c r="BI103" s="4">
-        <v>90.721522698333189</v>
+        <v>307.38818936499985</v>
       </c>
       <c r="BJ103" s="4">
         <v>524.54121819698298</v>
       </c>
       <c r="BK103" s="4">
-        <v>734.40225810454683</v>
+        <v>734.4022581045466</v>
       </c>
       <c r="BL103" s="4">
         <v>930.80202561637657</v>
@@ -31395,13 +31403,13 @@
         <v>-69.813931608333291</v>
       </c>
       <c r="CK103" s="4">
-        <v>159.08838491499998</v>
+        <v>-57.578281751666708</v>
       </c>
       <c r="CL103" s="4">
-        <v>373.72065040466657</v>
+        <v>373.72031707133328</v>
       </c>
       <c r="CM103" s="4">
-        <v>237.82977832293889</v>
+        <v>490.62902544955392</v>
       </c>
       <c r="CN103" s="4">
         <v>596.53259917848959</v>
@@ -31461,7 +31469,7 @@
         <v>1100</v>
       </c>
       <c r="DG103" s="4">
-        <v>1096.1764333255469</v>
+        <v>1096.1767818096619</v>
       </c>
       <c r="DH103" s="5">
         <v>1086.454334299227</v>
@@ -31478,16 +31486,16 @@
         <v>104.02148480833355</v>
       </c>
       <c r="D104" s="7">
-        <v>514.59556519833359</v>
+        <v>211.52199020277942</v>
       </c>
       <c r="E104" s="7">
-        <v>265.55018298376723</v>
+        <v>265.54984965043388</v>
       </c>
       <c r="F104" s="7">
         <v>332.29992485077111</v>
       </c>
       <c r="G104" s="7">
-        <v>248.07131953007004</v>
+        <v>248.07131953007215</v>
       </c>
       <c r="H104" s="7">
         <v>-100</v>
@@ -31544,7 +31552,7 @@
         <v>-100</v>
       </c>
       <c r="Z104" s="7">
-        <v>-99.999999999999574</v>
+        <v>-99.999999999999545</v>
       </c>
       <c r="AA104" s="8">
         <v>-81.40010913706692</v>
@@ -31556,7 +31564,7 @@
         <v>-318.56537425483327</v>
       </c>
       <c r="AF104" s="7">
-        <v>-22.289915191666324</v>
+        <v>-244.156581858333</v>
       </c>
       <c r="AG104" s="7">
         <v>386.13687139833365</v>
@@ -31640,19 +31648,19 @@
         <v>-480.40296502499996</v>
       </c>
       <c r="BI104" s="7">
-        <v>5.9149968483340274</v>
+        <v>-427.41833648499926</v>
       </c>
       <c r="BJ104" s="7">
         <v>-251.77828836151565</v>
       </c>
       <c r="BK104" s="7">
-        <v>-84.178848057796273</v>
+        <v>-84.178848057796131</v>
       </c>
       <c r="BL104" s="7">
         <v>69.197974383623432</v>
       </c>
       <c r="BM104" s="7">
-        <v>41.420385362542618</v>
+        <v>41.420385362542675</v>
       </c>
       <c r="BN104" s="7">
         <v>-100</v>
@@ -31721,13 +31729,13 @@
         <v>-138.89708185833331</v>
       </c>
       <c r="CK104" s="7">
-        <v>59.852449565000342</v>
+        <v>493.18578289833363</v>
       </c>
       <c r="CL104" s="7">
-        <v>243.77643438466691</v>
+        <v>243.77610105133363</v>
       </c>
       <c r="CM104" s="7">
-        <v>76.61234263824943</v>
+        <v>329.41158976486429</v>
       </c>
       <c r="CN104" s="7">
         <v>403.46740082151041</v>
@@ -31787,7 +31795,7 @@
         <v>-100</v>
       </c>
       <c r="DG104" s="7">
-        <v>-96.176433325546896</v>
+        <v>-96.176781809661861</v>
       </c>
       <c r="DH104" s="8">
         <v>-86.454334299226957</v>
@@ -31804,10 +31812,10 @@
         <v>-249.66711986666684</v>
       </c>
       <c r="D105" s="10">
-        <v>-450.50126274666684</v>
+        <v>-298.96447524888981</v>
       </c>
       <c r="E105" s="10">
-        <v>-632.64404033653364</v>
+        <v>-632.64337366986706</v>
       </c>
       <c r="F105" s="10">
         <v>-796.9339345271643</v>
@@ -31882,7 +31890,7 @@
         <v>462.6541733946666</v>
       </c>
       <c r="AF105" s="10">
-        <v>-161.79831986666696</v>
+        <v>281.93501346666636</v>
       </c>
       <c r="AG105" s="10">
         <v>-361.13869314666692</v>
@@ -31966,13 +31974,13 @@
         <v>266.77627980000034</v>
       </c>
       <c r="BI105" s="10">
-        <v>-96.636519546667216</v>
+        <v>120.03014711999944</v>
       </c>
       <c r="BJ105" s="10">
         <v>-272.76292983546739</v>
       </c>
       <c r="BK105" s="10">
-        <v>-650.22341004675025</v>
+        <v>-650.22341004675036</v>
       </c>
       <c r="BL105" s="10">
         <v>-1000</v>
@@ -32047,13 +32055,13 @@
         <v>208.7110134666666</v>
       </c>
       <c r="CK105" s="10">
-        <v>-218.94083448000029</v>
+        <v>-435.60750114666695</v>
       </c>
       <c r="CL105" s="10">
-        <v>-617.49708478933348</v>
+        <v>-617.4964181226668</v>
       </c>
       <c r="CM105" s="10">
-        <v>-314.44212096118832</v>
+        <v>-820.04061521441815</v>
       </c>
       <c r="CN105" s="10">
         <v>-1000</v>
@@ -32207,19 +32215,19 @@
         <v>6</v>
       </c>
       <c r="B108" s="15">
-        <v>1213169599.756042</v>
+        <v>1213175944.1526644</v>
       </c>
       <c r="C108" s="16">
         <v>1117412343.1119051</v>
       </c>
       <c r="D108" s="16">
-        <v>1047326684.3117517</v>
+        <v>1047326684.3117518</v>
       </c>
       <c r="E108" s="16">
-        <v>909134746.0640763</v>
+        <v>909134746.06407619</v>
       </c>
       <c r="F108" s="16">
-        <v>833461140.92699659</v>
+        <v>833461140.92699671</v>
       </c>
       <c r="G108" s="16">
         <v>766839504.33914042</v>
@@ -32228,10 +32236,10 @@
         <v>713297195.62222552</v>
       </c>
       <c r="I108" s="16">
-        <v>673110474.5765729</v>
+        <v>673110474.57657301</v>
       </c>
       <c r="J108" s="16">
-        <v>808696822.63076174</v>
+        <v>808696822.63076186</v>
       </c>
       <c r="K108" s="16">
         <v>982580055.12718165</v>
@@ -32243,50 +32251,50 @@
         <v>771279471.60926163</v>
       </c>
       <c r="N108" s="16">
-        <v>888165439.01926208</v>
+        <v>888157276.78748119</v>
       </c>
       <c r="O108" s="16">
         <v>794857414.13648987</v>
       </c>
       <c r="P108" s="16">
-        <v>726937727.68298936</v>
+        <v>712014866.8050288</v>
       </c>
       <c r="Q108" s="16">
-        <v>636804790.32176328</v>
+        <v>651653564.1653862</v>
       </c>
       <c r="R108" s="16">
-        <v>608750670.6536727</v>
+        <v>608757000.78996181</v>
       </c>
       <c r="S108" s="16">
-        <v>555656775.40989709</v>
+        <v>543899227.50121486</v>
       </c>
       <c r="T108" s="16">
-        <v>485181300.99563813</v>
+        <v>496879683.91329432</v>
       </c>
       <c r="U108" s="16">
-        <v>343623205.49908417</v>
+        <v>353645839.31095994</v>
       </c>
       <c r="V108" s="16">
-        <v>601473002.47824812</v>
+        <v>591445506.46392012</v>
       </c>
       <c r="W108" s="16">
-        <v>538005010.11586976</v>
+        <v>538005010.11586964</v>
       </c>
       <c r="X108" s="16">
-        <v>423060634.14244336</v>
+        <v>423060634.14244241</v>
       </c>
       <c r="Y108" s="16">
         <v>166332886.56645423</v>
       </c>
       <c r="Z108" s="16">
-        <v>155898700.25842091</v>
+        <v>155898698.57836688</v>
       </c>
       <c r="AA108" s="17">
-        <v>147213869.41091657</v>
+        <v>147213869.41091654</v>
       </c>
       <c r="AB108" s="18">
         <f>SUM(TotalCost)</f>
-        <v>17989996940.800991</v>
+        <v>17989863337.194248</v>
       </c>
     </row>
     <row r="110" spans="1:112" x14ac:dyDescent="0.35">
@@ -32380,16 +32388,16 @@
         <v>8</v>
       </c>
       <c r="B111" s="3">
-        <v>77326696.472296745</v>
+        <v>77247790.401512206</v>
       </c>
       <c r="C111" s="4">
-        <v>73993066.167501688</v>
+        <v>73993066.167501703</v>
       </c>
       <c r="D111" s="4">
         <v>69325338.847167581</v>
       </c>
       <c r="E111" s="4">
-        <v>66241962.903168276</v>
+        <v>66241962.903168269</v>
       </c>
       <c r="F111" s="4">
         <v>62350169.305988468</v>
@@ -32401,65 +32409,65 @@
         <v>50148129.12422248</v>
       </c>
       <c r="I111" s="4">
-        <v>43612849.648524821</v>
+        <v>43612849.648524784</v>
       </c>
       <c r="J111" s="4">
-        <v>37029377.54958161</v>
+        <v>37029377.549581587</v>
       </c>
       <c r="K111" s="4">
-        <v>33520145.796386212</v>
+        <v>33520145.796386197</v>
       </c>
       <c r="L111" s="4">
         <v>29980693.625015594</v>
       </c>
       <c r="M111" s="4">
-        <v>26882874.9316517</v>
+        <v>26882874.931651689</v>
       </c>
       <c r="N111" s="4">
-        <v>23418970.842420299</v>
+        <v>24343475.691097654</v>
       </c>
       <c r="O111" s="4">
-        <v>23218976.99221117</v>
+        <v>23218976.992211156</v>
       </c>
       <c r="P111" s="4">
-        <v>20935917.725577474</v>
+        <v>20935917.725577466</v>
       </c>
       <c r="Q111" s="4">
-        <v>21479149.166130401</v>
+        <v>15877237.304760041</v>
       </c>
       <c r="R111" s="4">
-        <v>16075542.500197833</v>
+        <v>15135714.366735756</v>
       </c>
       <c r="S111" s="4">
-        <v>19096926.354174819</v>
+        <v>19096922.830327563</v>
       </c>
       <c r="T111" s="4">
-        <v>17982757.019836895</v>
+        <v>17393590.91759995</v>
       </c>
       <c r="U111" s="4">
-        <v>13542139.658573288</v>
+        <v>13542139.658573292</v>
       </c>
       <c r="V111" s="4">
-        <v>10718389.998944059</v>
+        <v>10892746.491084132</v>
       </c>
       <c r="W111" s="4">
-        <v>11375061.214811446</v>
+        <v>11375061.214811467</v>
       </c>
       <c r="X111" s="4">
-        <v>9640152.2023706958</v>
+        <v>9640152.2023706809</v>
       </c>
       <c r="Y111" s="4">
-        <v>10970222.520621492</v>
+        <v>10970222.52062148</v>
       </c>
       <c r="Z111" s="4">
-        <v>10532234.387018345</v>
+        <v>10532235.275392339</v>
       </c>
       <c r="AA111" s="5">
         <v>9958107.0371292606</v>
       </c>
       <c r="AB111" s="12">
         <f>SUM(B111:AA111)</f>
-        <v>847410558.65288389</v>
+        <v>841299605.19037378</v>
       </c>
     </row>
     <row r="112" spans="1:112" x14ac:dyDescent="0.35">
@@ -32467,16 +32475,16 @@
         <v>9</v>
       </c>
       <c r="B112" s="6">
-        <v>19141647.951826602</v>
+        <v>19141343.696437359</v>
       </c>
       <c r="C112" s="7">
-        <v>17723521.699126001</v>
+        <v>17723521.699126005</v>
       </c>
       <c r="D112" s="7">
-        <v>16161919.77151829</v>
+        <v>16161919.771518286</v>
       </c>
       <c r="E112" s="7">
-        <v>15516432.996562738</v>
+        <v>15516432.996562731</v>
       </c>
       <c r="F112" s="7">
         <v>14364626.364027293</v>
@@ -32488,65 +32496,65 @@
         <v>11927782.388539556</v>
       </c>
       <c r="I112" s="7">
-        <v>10638450.016255572</v>
+        <v>10638450.016255567</v>
       </c>
       <c r="J112" s="7">
-        <v>9362510.1759077944</v>
+        <v>9362510.1759077832</v>
       </c>
       <c r="K112" s="7">
-        <v>8200197.1783657372</v>
+        <v>8200197.1783657335</v>
       </c>
       <c r="L112" s="7">
-        <v>7548432.3371936418</v>
+        <v>7548432.3371936427</v>
       </c>
       <c r="M112" s="7">
-        <v>7378692.8066161117</v>
+        <v>7378692.806616107</v>
       </c>
       <c r="N112" s="7">
-        <v>6316633.0832906347</v>
+        <v>6670545.0045672785</v>
       </c>
       <c r="O112" s="7">
-        <v>6378561.6204540748</v>
+        <v>6378561.6204540702</v>
       </c>
       <c r="P112" s="7">
-        <v>5541488.9899401646</v>
+        <v>5541488.9899401627</v>
       </c>
       <c r="Q112" s="7">
-        <v>5779445.154024574</v>
+        <v>3637389.310110162</v>
       </c>
       <c r="R112" s="7">
-        <v>3738266.6217706329</v>
+        <v>3378488.7570474111</v>
       </c>
       <c r="S112" s="7">
-        <v>4911377.7222420853</v>
+        <v>4911376.3732696567</v>
       </c>
       <c r="T112" s="7">
-        <v>4491642.9862143882</v>
+        <v>4268086.9674924603</v>
       </c>
       <c r="U112" s="7">
-        <v>2824600.2343795197</v>
+        <v>2824600.2343795206</v>
       </c>
       <c r="V112" s="7">
-        <v>2176315.8153821677</v>
+        <v>2217688.7736536404</v>
       </c>
       <c r="W112" s="7">
-        <v>2348366.9656352107</v>
+        <v>2348366.9656352154</v>
       </c>
       <c r="X112" s="7">
-        <v>1873907.1310892375</v>
+        <v>1873907.1310892422</v>
       </c>
       <c r="Y112" s="7">
-        <v>1336879.9519540735</v>
+        <v>1336879.9519540751</v>
       </c>
       <c r="Z112" s="7">
-        <v>1146081.9181854059</v>
+        <v>1146082.0248890703</v>
       </c>
       <c r="AA112" s="8">
         <v>954594.67431902024</v>
       </c>
       <c r="AB112" s="13">
         <f t="shared" ref="AB112:AB115" si="0">SUM(B112:AA112)</f>
-        <v>200748966.98486531</v>
+        <v>198418556.6393958</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -32554,7 +32562,7 @@
         <v>10</v>
       </c>
       <c r="B113" s="6">
-        <v>90373390585.434616</v>
+        <v>90373390585.434586</v>
       </c>
       <c r="C113" s="7">
         <v>85498433001.118835</v>
@@ -32578,16 +32586,16 @@
         <v>61300445183.839294</v>
       </c>
       <c r="J113" s="7">
-        <v>57993752049.554565</v>
+        <v>57993752049.554558</v>
       </c>
       <c r="K113" s="7">
-        <v>54865429878.996674</v>
+        <v>54865429878.996666</v>
       </c>
       <c r="L113" s="7">
-        <v>51905856914.291885</v>
+        <v>51905856914.291878</v>
       </c>
       <c r="M113" s="7">
-        <v>49105930418.278389</v>
+        <v>49105930418.278381</v>
       </c>
       <c r="N113" s="7">
         <v>46457038677.283447</v>
@@ -32641,86 +32649,86 @@
         <v>11</v>
       </c>
       <c r="B114" s="6">
-        <v>9167688.2344861161</v>
+        <v>9167068.2749783825</v>
       </c>
       <c r="C114" s="7">
-        <v>8456952.3715645336</v>
+        <v>8456952.3715645373</v>
       </c>
       <c r="D114" s="7">
-        <v>7661395.0828903355</v>
+        <v>7661395.0828903336</v>
       </c>
       <c r="E114" s="7">
-        <v>7325412.8845815146</v>
+        <v>7325412.8845815118</v>
       </c>
       <c r="F114" s="7">
-        <v>6736606.8558932543</v>
+        <v>6736606.8558932561</v>
       </c>
       <c r="G114" s="7">
-        <v>6161432.0598707376</v>
+        <v>6161432.0598707385</v>
       </c>
       <c r="H114" s="7">
         <v>5577206.5059953146</v>
       </c>
       <c r="I114" s="7">
-        <v>4961434.7315524323</v>
+        <v>4961434.7315524295</v>
       </c>
       <c r="J114" s="7">
-        <v>4357066.4201968256</v>
+        <v>4357066.4201968201</v>
       </c>
       <c r="K114" s="7">
-        <v>3794822.8811413711</v>
+        <v>3794822.8811413688</v>
       </c>
       <c r="L114" s="7">
-        <v>3465818.4466309776</v>
+        <v>3465818.446630978</v>
       </c>
       <c r="M114" s="7">
-        <v>3350302.6355046649</v>
+        <v>3350302.6355046621</v>
       </c>
       <c r="N114" s="7">
-        <v>2986607.5398146883</v>
+        <v>2994183.8929235027</v>
       </c>
       <c r="O114" s="7">
-        <v>2812469.7726880098</v>
+        <v>2812469.772688007</v>
       </c>
       <c r="P114" s="7">
-        <v>2616521.7187062586</v>
+        <v>2616521.7187062576</v>
       </c>
       <c r="Q114" s="7">
-        <v>2463563.7316814987</v>
+        <v>2402763.5162719549</v>
       </c>
       <c r="R114" s="7">
-        <v>2250747.7910444024</v>
+        <v>2243045.8630221803</v>
       </c>
       <c r="S114" s="7">
-        <v>2154091.4145042673</v>
+        <v>2154091.3856262024</v>
       </c>
       <c r="T114" s="7">
-        <v>2039637.6291575988</v>
+        <v>2019947.6546863541</v>
       </c>
       <c r="U114" s="7">
-        <v>1879674.4333351851</v>
+        <v>1879674.4333351855</v>
       </c>
       <c r="V114" s="7">
-        <v>1568460.1441300286</v>
+        <v>1586096.5566582475</v>
       </c>
       <c r="W114" s="7">
-        <v>1612402.4978738185</v>
+        <v>1612402.4978738206</v>
       </c>
       <c r="X114" s="7">
-        <v>1379322.6612578339</v>
+        <v>1379322.6612578363</v>
       </c>
       <c r="Y114" s="7">
-        <v>1104057.3170182602</v>
+        <v>1104057.3170182612</v>
       </c>
       <c r="Z114" s="7">
-        <v>992517.81841826835</v>
+        <v>992517.87630567711</v>
       </c>
       <c r="AA114" s="8">
         <v>879643.18101986451</v>
       </c>
       <c r="AB114" s="13">
         <f t="shared" si="0"/>
-        <v>97755856.760958046</v>
+        <v>97692257.478193685</v>
       </c>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.35">
@@ -32728,86 +32736,86 @@
         <v>12</v>
       </c>
       <c r="B115" s="9">
-        <v>1325812.7999590654</v>
+        <v>1325718.0707614366</v>
       </c>
       <c r="C115" s="10">
-        <v>1221748.5744893658</v>
+        <v>1221748.5744893663</v>
       </c>
       <c r="D115" s="10">
-        <v>1105640.0308994877</v>
+        <v>1105640.0308994874</v>
       </c>
       <c r="E115" s="10">
-        <v>1052303.5098022474</v>
+        <v>1052303.5098022469</v>
       </c>
       <c r="F115" s="10">
-        <v>965066.90106988023</v>
+        <v>965066.90106988035</v>
       </c>
       <c r="G115" s="10">
-        <v>879657.74630202504</v>
+        <v>879657.74630202516</v>
       </c>
       <c r="H115" s="10">
         <v>790917.80793941848</v>
       </c>
       <c r="I115" s="10">
-        <v>698965.15968370065</v>
+        <v>698965.1596837003</v>
       </c>
       <c r="J115" s="10">
-        <v>608641.62087170547</v>
+        <v>608641.62087170465</v>
       </c>
       <c r="K115" s="10">
-        <v>525563.15854071174</v>
+        <v>525563.15854071139</v>
       </c>
       <c r="L115" s="10">
-        <v>477297.37650254538</v>
+        <v>477297.37650254549</v>
       </c>
       <c r="M115" s="10">
-        <v>461171.79014386388</v>
+        <v>461171.79014386341</v>
       </c>
       <c r="N115" s="10">
-        <v>407922.2449780993</v>
+        <v>409105.27409722254</v>
       </c>
       <c r="O115" s="10">
-        <v>383903.45445980015</v>
+        <v>383903.45445979974</v>
       </c>
       <c r="P115" s="10">
-        <v>356456.12373206241</v>
+        <v>356456.12373206229</v>
       </c>
       <c r="Q115" s="10">
-        <v>335493.67241677293</v>
+        <v>326099.06027448329</v>
       </c>
       <c r="R115" s="10">
-        <v>305170.20518533373</v>
+        <v>303967.56784876616</v>
       </c>
       <c r="S115" s="10">
-        <v>292583.56940753449</v>
+        <v>292583.56489829486</v>
       </c>
       <c r="T115" s="10">
-        <v>277030.36271254218</v>
+        <v>274055.82783867256</v>
       </c>
       <c r="U115" s="10">
-        <v>254399.95424059284</v>
+        <v>254399.9542405929</v>
       </c>
       <c r="V115" s="10">
-        <v>208288.62572638484</v>
+        <v>211007.3691745321</v>
       </c>
       <c r="W115" s="10">
-        <v>216644.19006568057</v>
+        <v>216644.19006568089</v>
       </c>
       <c r="X115" s="10">
-        <v>182373.86048529739</v>
+        <v>182373.86048529774</v>
       </c>
       <c r="Y115" s="10">
-        <v>142020.16457023652</v>
+        <v>142020.16457023664</v>
       </c>
       <c r="Z115" s="10">
-        <v>126243.15594488282</v>
+        <v>126243.16411892779</v>
       </c>
       <c r="AA115" s="11">
         <v>110367.50268686251</v>
       </c>
       <c r="AB115" s="14">
         <f t="shared" si="0"/>
-        <v>13711683.562816096</v>
+        <v>13701918.825497817</v>
       </c>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.35">
@@ -32955,13 +32963,13 @@
         <v>0</v>
       </c>
       <c r="V118" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W118" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X118" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y118" s="16">
         <v>0</v>
@@ -32987,22 +32995,22 @@
         <v>0</v>
       </c>
       <c r="E119" s="16">
+        <v>0</v>
+      </c>
+      <c r="F119" s="16">
+        <v>0</v>
+      </c>
+      <c r="G119" s="16">
+        <v>0</v>
+      </c>
+      <c r="H119" s="16">
+        <v>0</v>
+      </c>
+      <c r="I119" s="16">
+        <v>0</v>
+      </c>
+      <c r="J119" s="16">
         <v>1</v>
-      </c>
-      <c r="F119" s="16">
-        <v>1</v>
-      </c>
-      <c r="G119" s="16">
-        <v>1</v>
-      </c>
-      <c r="H119" s="16">
-        <v>1</v>
-      </c>
-      <c r="I119" s="16">
-        <v>1</v>
-      </c>
-      <c r="J119" s="16">
-        <v>0</v>
       </c>
       <c r="K119" s="16">
         <v>1</v>
@@ -33011,40 +33019,40 @@
         <v>1</v>
       </c>
       <c r="M119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X119" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y119" s="16">
         <v>0</v>
@@ -33053,6 +33061,172 @@
         <v>0</v>
       </c>
       <c r="AA119" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B120" s="15">
+        <v>0</v>
+      </c>
+      <c r="C120" s="16">
+        <v>0</v>
+      </c>
+      <c r="D120" s="16">
+        <v>0</v>
+      </c>
+      <c r="E120" s="16">
+        <v>0</v>
+      </c>
+      <c r="F120" s="16">
+        <v>0</v>
+      </c>
+      <c r="G120" s="16">
+        <v>0</v>
+      </c>
+      <c r="H120" s="16">
+        <v>0</v>
+      </c>
+      <c r="I120" s="16">
+        <v>0</v>
+      </c>
+      <c r="J120" s="16">
+        <v>0</v>
+      </c>
+      <c r="K120" s="16">
+        <v>0</v>
+      </c>
+      <c r="L120" s="16">
+        <v>0</v>
+      </c>
+      <c r="M120" s="16">
+        <v>0</v>
+      </c>
+      <c r="N120" s="16">
+        <v>0</v>
+      </c>
+      <c r="O120" s="16">
+        <v>0</v>
+      </c>
+      <c r="P120" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="16">
+        <v>0</v>
+      </c>
+      <c r="R120" s="16">
+        <v>0</v>
+      </c>
+      <c r="S120" s="16">
+        <v>0</v>
+      </c>
+      <c r="T120" s="16">
+        <v>0</v>
+      </c>
+      <c r="U120" s="16">
+        <v>0</v>
+      </c>
+      <c r="V120" s="16">
+        <v>0</v>
+      </c>
+      <c r="W120" s="16">
+        <v>0</v>
+      </c>
+      <c r="X120" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y120" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z120" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA120" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A121" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B121" s="15">
+        <v>1</v>
+      </c>
+      <c r="C121" s="16">
+        <v>1</v>
+      </c>
+      <c r="D121" s="16">
+        <v>1</v>
+      </c>
+      <c r="E121" s="16">
+        <v>0</v>
+      </c>
+      <c r="F121" s="16">
+        <v>1</v>
+      </c>
+      <c r="G121" s="16">
+        <v>0</v>
+      </c>
+      <c r="H121" s="16">
+        <v>0</v>
+      </c>
+      <c r="I121" s="16">
+        <v>0</v>
+      </c>
+      <c r="J121" s="16">
+        <v>0</v>
+      </c>
+      <c r="K121" s="16">
+        <v>0</v>
+      </c>
+      <c r="L121" s="16">
+        <v>0</v>
+      </c>
+      <c r="M121" s="16">
+        <v>0</v>
+      </c>
+      <c r="N121" s="16">
+        <v>0</v>
+      </c>
+      <c r="O121" s="16">
+        <v>0</v>
+      </c>
+      <c r="P121" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q121" s="16">
+        <v>0</v>
+      </c>
+      <c r="R121" s="16">
+        <v>0</v>
+      </c>
+      <c r="S121" s="16">
+        <v>0</v>
+      </c>
+      <c r="T121" s="16">
+        <v>0</v>
+      </c>
+      <c r="U121" s="16">
+        <v>0</v>
+      </c>
+      <c r="V121" s="16">
+        <v>0</v>
+      </c>
+      <c r="W121" s="16">
+        <v>0</v>
+      </c>
+      <c r="X121" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y121" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z121" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA121" s="17">
         <v>0</v>
       </c>
     </row>

</xml_diff>